<commit_message>
Update combine_dataset.py & Upload changed dataset
</commit_message>
<xml_diff>
--- a/datasets/hyundai/hyundai_cleaned_combined_dataset.xlsx
+++ b/datasets/hyundai/hyundai_cleaned_combined_dataset.xlsx
@@ -4024,265 +4024,265 @@
     <t>20220610</t>
   </si>
   <si>
-    <t>현대차-Valuation Trap 탈출이 시작되다,17년도 하반기 순이익, 증가율 25.2%전년 대비 증감율예상,투자포인트 1, 상품전략의 변화</t>
-  </si>
-  <si>
-    <t>현대차-수익성과 성장성 갖춘 경쟁력 10위 업체,2017 Global Auto Insight 평점 2.3점/5.0점,현대차그룹 기준 글로벌 5위 한국 자동차 업체,2017년 브랜드가치 개선 원년, 현대차-하반기 업황 개선 보다 신차 효과 기대,2017년도 판매 0%, 생산 1.5% 증가 전망,이익 증가폭 미미</t>
-  </si>
-  <si>
-    <t>현대차-SUV 봉인해제가 장기성장을 이끈다,SUV 인기 지속에 세단 고집 꺾은 현대차,코나 출시는 SUV 확장 전략의 신호탄, Hyundai Motor-Renewed SUV push to fuel long-term growth,SUV 인기 지속에 세단 고집 꺾은 현대차,코나 출시는 SUV 확장 전략의 신호탄</t>
-  </si>
-  <si>
-    <t>현대차-SUV 봉인해제가 장기성장을 이끈다 (요약),SUV 인기 지속에 세단 고집 꺾은 현대차,코나 출시는 SUV 확장 전략의 신호탄</t>
-  </si>
-  <si>
-    <t>현대차-현대차, SUV 차종의 확대에 주목하자,높은 성장률의 SUV-B 세그먼트, 마침내 진출하다,2017년: 판매대수의 변화보다는 ASP의 변화를 주목</t>
-  </si>
-  <si>
-    <t>현대차-북미/중국사업 안정화 필요,2분기 Preview: 영업이익 양호, 세전이익 부진</t>
-  </si>
-  <si>
-    <t>현대차-년도년도 1분기 2분기 Preview, 내수/수출 호조로 시장 기대치 상회,년도년도 1분기 2분기 Preview: 내수/수출 호조로 시장 기대치 상회할 전망,발목 잡는 미국, 개선되는 이머징</t>
-  </si>
-  <si>
-    <t>현대차-년도년도 하반기 하반기 전년 대비 증감율 실적개선, 신차효과는 2018년,년도년도 하반기 2분기 영업이익은 1.54조원으로 전년 대비 증감율 13% 감소 예상,년도년도 하반기 하반기 전년 대비 증감율 영업이익 증가 전환. 신차효과 반영은 2018년 기대, 현대차-신흥시장 회복과 상품성 강화,러시아, 브라질 등 신흥시장 회복,차세대 파워트레인과 SUV 모델 강화, Hyundai Motor-전년 대비 증감율 earnings growth in 년도년도 하반기 하반기 ; new model effects in 2018,년도년도 하반기 2분기 영업이익은 1.54조원으로 전년 대비 증감율 13% 감소 예상,년도년도 하반기 하반기 전년 대비 증감율 영업이익 증가 전환. 신차효과 반영은 2018년 기대</t>
-  </si>
-  <si>
-    <t>현대차-인도 크레타 돌풍, G70까지,인도 시장 투자 포인트 : SUV 비중 확대,2분기 실적 전망</t>
-  </si>
-  <si>
-    <t>현대차-탐방노트: 북미 우려 심화,미국 시장 경쟁 격화,낮아진 신흥시장 기저 효과</t>
-  </si>
-  <si>
-    <t>Hyundai Motor-2Q expectations to be missed due to weak retail and added incentives,2Q 영업이익, 소매판매 부진과 인센티브 증가로 기대치 하회 예상, 현대차-소매 판매 부진과 인센티브 증가로 기대치 하회 예상,2Q 영업이익, 소매판매 부진과 인센티브 증가로 기대치 하회 예상</t>
-  </si>
-  <si>
-    <t>현대차-2분기 실적은 기존 추정치 수준,2Q는 기존 추정치와 유사. 3Q 이후 점진적 회복 전망,17년도 2분기 Preview: 영업이익률 6.1% 전망</t>
-  </si>
-  <si>
-    <t>Hyundai Motor Company-Weak US sales weigh on 2Q results,2분기 실적은 기존 추정치와 컨센서스 하회할 전망,2분기 중국제외 글로벌 출고는 1.4% 전년 대비 증감율 증가했지만 리테일판매(중국제외)는 3.7% 감소, 현대차-미국영향으로 2분기 실적 부진 예상,2분기 실적은 기존 추정치와 컨센서스 하회할 전망,2분기 중국제외 글로벌 출고는 1.4% 전년 대비 증감율 증가했지만 리테일판매(중국제외)는 3.7% 감소</t>
-  </si>
-  <si>
-    <t>현대차-하반기 P와 Q 모두에서 성장 기대,17년도 2분기 Preview - 매출액 25.4 조원, 영업이익 1 조 5,446 억원(OPM 6.1%),P - 신차효과와 믹스개선, Q ? 국내공장과 기타시장 회복 기대</t>
-  </si>
-  <si>
-    <t>현대차-미국 부진 심화로 시각 조정 불가피,미국 부진 심화,다시 쌓이기 시작한 재고</t>
-  </si>
-  <si>
-    <t>현대차-모델 진부화의 끝자락에서,반등하던 주가가 판매부진에 기인한 Earnings shock 우려로 다시 하락,2분기 실적 예상치의 매출액을 25.6조, 영업이익을 1.47조로 하향하여 전망</t>
-  </si>
-  <si>
-    <t>현대차-한걸음 더 늦어졌지만 여전히 업황 개선추세 유효,17년도 2분기 Preview: 미국, 중국에 의한 부진한 분기실적 연출,신흥국 업황개선 추세는 지속적으로 이어지고 있음</t>
-  </si>
-  <si>
-    <t>현대차-하반기 실적은 국내공장 생산실적이 관건,주력 모델의 노후화와 맞물린 경쟁업체의 볼륨모델 신차,역대급 기저효과로 인해 하반기 증익은 가능 할 것,당장의 실적보다 새로운 전략적 변화를 기대</t>
-  </si>
-  <si>
-    <t>현대차- 제품의 힘, 그랜저,제품의 힘: 그랜(다이)저, 현대차를 구하다,년도년도 1분기 2분기 Preview: 매출 및 영업이익은 양호하나 순이익 감소 전망, 현대차-여전히 업종내 방어주,업황 부진에도 부진은 상대적으로 미미,17년도 2분기 영업이익 1.46조원 전망</t>
-  </si>
-  <si>
-    <t>현대차-내수 호조 북미 부진이 상쇄,17년도 2분기 영업이익 1조 5,109억원 (-14.2%전년 대비 증감율)으로 시장기대치 하회 전망,하반기 내수 외에 미국 및 주요 지역 판매 둔화 지속 전망</t>
-  </si>
-  <si>
-    <t>현대차-하반기 회복 기조 전망되나 파업, 사드 영향 등 변수 확인 필요,2분기 연결기준 공장판매(+), ASP 및 믹스(+), 환율(-) 영향 추정,2분기 영업이익은 컨센서스 및 전년동기비 부진 전망</t>
-  </si>
-  <si>
-    <t>현대차-년도년도 1분기 2분기 Review ? 발목 잡는 G2시장의 부진,년도년도 1분기 2분기 영업이익, 추정치 11.0%하회,G2시장의 실적부진 장기화 우려</t>
-  </si>
-  <si>
-    <t>Hyundai Motor-Poor G2 performance weighs on 2Q results,17년도 2분기 영업이익, 추정치 11.0%하회,G2시장의 실적부진 장기화 우려, 현대차-년도년도 하반기 하반기 북미우려 지속,년도년도 하반기 2분기 , Shock,년도년도 하반기 하반기 어려운 영업환경 지속, 현대차-아쉬운 실적, 나아질 하반기,2분기 영업이익 1.34조원(-23.7% 전년 대비 증감율) 으로 컨센서스(1.53조원) 12.0% 하회,2분기 실적을 바닥으로 점진적인 개선, 3분기 영업이익 1.36조원(+27.2%) 전망, 현대차-마침표,17년도 2분기 은 12년 이후 6년간 지속됐던 Earnings Downtrend의 종점,시장: Hard Data (소득지표) 개선이 판매로 연결되기 시작할 17년도 하반기, 현대차-17년도 2분기 Review: 낮아진 기대치를 하회,영업이익 기준 컨센서스와 당사 추정치를 각각 10.4%, 11.8% 하회하였으며, 지배이익은 일회성 비용과 지분법이익 감소로 기대치를 대폭 하회함,특히, 2분기 판매보증충당금(5,884억원)은 세타 엔진 리콜 비용이 발생했던 지난 1분기 대비 1,750억원이나 증가해 예상 밖의 영업이익 감소를 불러왔음, 현대차-하반기 실적은 8월 임금협상이 관건,매출액 24,308십억원(전년 대비 증감율-1.5%), 영업이익 1,344십억원(전년 대비 증감율-23.7%), OPM 5.5%,차량, 금융, 기타사업부 동반 부진이 초래한 역대 최저수준의 2분기 영업이익, Hyundai Motor-Product competitiveness to drive gradual earnings improvement,17년도 2분기 영업이익 전년 대비 증감율 23.7% 감소, 부진 지속,핵심시장 수익부진 불구 17년도 하반기 전년 대비 증감율 영업이익 증가 전환 가능, 현대차-제품경쟁력 제고로 점진적 실적개선 (요약),17년도 2분기 영업이익 전년 대비 증감율 23.7% 감소, 부진 지속,핵심시장 수익부진 불구 17년도 하반기 전년 대비 증감율 영업이익 증가 전환 가능, Hyundai Motor-Getting past the worst,What’s new: 미국과 중국으로 부진한 2분기 실적,Positives: 신흥국 호조 지속 및 신차 출시,Negatives: 기대에 못 미친 국내 공장 가동률 상승효과와 단기 모멘텀 부재, 현대차-보릿고개를 넘기자,What’s new: 미국과 중국으로 부진한 2분기 실적,Positives: 신흥국 호조 지속 및 신차 출시,Negatives: 기대에 못 미친 국내 공장 가동률 상승효과와 단기 모멘텀 부재, 현대차-Top-line과 Bottom-line의 온도차가 극심한 실적,17년도 2분기 Review - Top-line과 Bottom-line의 온도차가 극심한 실적, Hyundai Motor-Disappointing results, brighter prospects for 2H,2분기 영업이익 1.34조원(-23.7% 전년 대비 증감율) 으로 컨센서스(1.53조원) 12.0% 하회,2분기 실적을 바닥으로 점진적인 개선, 3분기 영업이익 1.36조원(+27.2%) 전망, Hyundai Motor-Disappointing results, brighter prospects for 2H,2분기 영업이익 1.34조원(-23.7% 전년 대비 증감율) 으로 컨센서스(1.53조원) 12.0% 하회,2분기 실적을 바닥으로 점진적인 개선, 3분기 영업이익 1.36조원(+27.2%) 전망, 현대차-제품경쟁력 제고로 점진적 실적개선,17년도 2분기 영업이익 전년 대비 증감율 23.7% 감소, 부진 지속,핵심시장 수익부진 불구 17년도 하반기 전년 대비 증감율 영업이익 증가 전환 가능, Hyundai Motor-Getting past the worst,What’s new: 미국과 중국으로 부진한 2분기 실적,Positives: 신흥국 호조 지속 및 신차 출시,Negatives: 기대에 못 미친 국내 공장 가동률 상승효과와 단기 모멘텀 부재, 현대차-제품경쟁력 제고로 점진적 실적개선,17년도 2분기 영업이익 전년 대비 증감율 23.7% 감소, 부진 지속,핵심시장 수익부진 불구 17년도 하반기 전년 대비 증감율 영업이익 증가 전환 가능, 현대차-제품경쟁력 제고로 점진적 실적개선 (요약),17년도 2분기 영업이익 전년 대비 증감율 23.7% 감소, 부진 지속,핵심시장 수익부진 불구 17년도 하반기 전년 대비 증감율 영업이익 증가 전환 가능, Hyundai Motor-Product competitiveness to drive gradual earnings improvement,17년도 2분기 영업이익 전년 대비 증감율 23.7% 감소, 부진 지속,핵심시장 수익부진 불구 17년도 하반기 전년 대비 증감율 영업이익 증가 전환 가능, 현대차-하반기 실적은 8월 임금협상이 관건,매출액 24,308십억원(전년 대비 증감율-1.5%), 영업이익 1,344십억원(전년 대비 증감율-23.7%), OPM 5.5%,차량, 금융, 기타사업부 동반 부진이 초래한 역대 최저수준의 2분기 영업이익, 현대차-17년도 2분기 Review: 낮아진 기대치를 하회,영업이익 기준 컨센서스와 당사 추정치를 각각 10.4%, 11.8% 하회하였으며, 지배이익은 일회성 비용과 지분법이익 감소로 기대치를 대폭 하회함,특히, 2분기 판매보증충당금(5,884억원)은 세타 엔진 리콜 비용이 발생했던 지난 1분기 대비 1,750억원이나 증가해 예상 밖의 영업이익 감소를 불러왔음, 현대차-부담을 덜고 맞이하는 하반기,17년도 2분기 Review ? 비용반영으로 시장 기대치 하회,하지만 2011 년 이후 가장 높은 판매 보증관련 비용(5,890 억원, 2.4%) 반영, 매도가능증권 손상차손 처리를 감안할 필요, 현대차-마침표,17년도 2분기 은 12년 이후 6년간 지속됐던 Earnings Downtrend의 종점,시장: Hard Data (소득지표) 개선이 판매로 연결되기 시작할 17년도 하반기, 현대차-주가 추세전환을 위한 조건 (요약),북미/중국사업 안정화 필요,2분기 Review-컨센서스 하회, 현대차-주가 추세전환을 위한 조건,북미/중국사업 안정화 필요,2분기 Review-컨센서스 하회, HMC-What is needed for shares to break out of range?,북미/중국사업 안정화 필요,2분기 Review-컨센서스 하회, 현대차-2분기 기대치 하회, 판매 및 품질 비용은 지속적인 부담 요인,현대차의 2017년 2분기 매출액은 전년 동기 대비 1.5% 감소한 24.3조원을 기록,3분기 실적은 기저효과로 지난해와 유사, 현대차-G2에서의 부진으로 2Q 실적 예상 하회,2분기 실적은 당사 추정치와 컨센서스를 하회,미국시장 수요가 6개월 연속으로 전년 대비 증감율 감소, 현대차-보릿고개를 넘기자,What’s new: 미국과 중국으로 부진한 2분기 실적,Positives: 신흥국 호조 지속 및 신차 출시,Negatives: 기대에 못 미친 국내 공장 가동률 상승효과와 단기 모멘텀 부재</t>
-  </si>
-  <si>
-    <t>현대차-다양함이 나쁘지 않다,상반기 친환경차 판매 양호,하이브리드부터 수소차까지 친환경차 전 라인업 확보</t>
-  </si>
-  <si>
-    <t>현대차- 픽업트럭 출시 고려 중,2000년대부터 시장이 요청하던 픽업트럭, 마침내 ‘고려’단계 진입,출시될 경우 미국에서 30년만에 첫 전륜구동 소형픽업트럭이 될 전망</t>
-  </si>
-  <si>
-    <t>현대차-별도손익의 개선 vs 미, 중 부진의 심화,17년 반기보고서에서 검토해봐야 할 것들,투자전략-3분기, 마지막 고비</t>
-  </si>
-  <si>
-    <t>현대차-FCEV, 외부와의 소통 카드,현대차, 2세대 FCEV 출시,FCEV 조기상용화, 브랜드 재정립을 위한 노력</t>
-  </si>
-  <si>
-    <t>현대차-공포 국면, 현대차가 답할 차례,중국파트너사와의 갈등, 중국사업 불확실성 확대,공정거래위원장, 현대차그룹의 사업구조 재편 필요성 강조</t>
+    <t>Valuation Trap 탈출이 시작되다,17년도 하반기 순이익, 증가율 25.2%전년 대비 증감율예상,투자포인트 1, 상품전략의 변화</t>
+  </si>
+  <si>
+    <t>수익성과 성장성 갖춘 경쟁력 10위 업체,2017 Global Auto Insight 평점 2.3점/5.0점,현대차그룹 기준 글로벌 5위 한국 자동차 업체,2017년 브랜드가치 개선 원년, 하반기 업황 개선 보다 신차 효과 기대,2017년도 판매 0%, 생산 1.5% 증가 전망,이익 증가폭 미미</t>
+  </si>
+  <si>
+    <t>SUV 봉인해제가 장기성장을 이끈다,SUV 인기 지속에 세단 고집 꺾은 현대차,코나 출시는 SUV 확장 전략의 신호탄, Hyundai Motor-Renewed SUV push to fuel long-term growth,SUV 인기 지속에 세단 고집 꺾은 현대차,코나 출시는 SUV 확장 전략의 신호탄</t>
+  </si>
+  <si>
+    <t>SUV 봉인해제가 장기성장을 이끈다 (요약),SUV 인기 지속에 세단 고집 꺾은 현대차,코나 출시는 SUV 확장 전략의 신호탄</t>
+  </si>
+  <si>
+    <t>현대차, SUV 차종의 확대에 주목하자,높은 성장률의 SUV-B 세그먼트, 마침내 진출하다,2017년: 판매대수의 변화보다는 ASP의 변화를 주목</t>
+  </si>
+  <si>
+    <t>북미/중국사업 안정화 필요,2분기 Preview: 영업이익 양호, 세전이익 부진</t>
+  </si>
+  <si>
+    <t>년도년도 1분기 2분기 Preview, 내수/수출 호조로 시장 기대치 상회,년도년도 1분기 2분기 Preview: 내수/수출 호조로 시장 기대치 상회할 전망,발목 잡는 미국, 개선되는 이머징</t>
+  </si>
+  <si>
+    <t>년도년도 하반기 하반기 전년 대비 증감율 실적개선, 신차효과는 2018년,년도년도 하반기 2분기 영업이익은 1.54조원으로 전년 대비 증감율 13% 감소 예상,년도년도 하반기 하반기 전년 대비 증감율 영업이익 증가 전환. 신차효과 반영은 2018년 기대, 신흥시장 회복과 상품성 강화,러시아, 브라질 등 신흥시장 회복,차세대 파워트레인과 SUV 모델 강화, Hyundai Motor-전년 대비 증감율 earnings growth in 년도년도 하반기 하반기 ; new model effects in 2018,년도년도 하반기 2분기 영업이익은 1.54조원으로 전년 대비 증감율 13% 감소 예상,년도년도 하반기 하반기 전년 대비 증감율 영업이익 증가 전환. 신차효과 반영은 2018년 기대</t>
+  </si>
+  <si>
+    <t>인도 크레타 돌풍, G70까지,인도 시장 투자 포인트 : SUV 비중 확대,2분기 실적 전망</t>
+  </si>
+  <si>
+    <t>탐방노트: 북미 우려 심화,미국 시장 경쟁 격화,낮아진 신흥시장 기저 효과</t>
+  </si>
+  <si>
+    <t>Hyundai Motor-2Q expectations to be missed due to weak retail and added incentives,2Q 영업이익, 소매판매 부진과 인센티브 증가로 기대치 하회 예상, 소매 판매 부진과 인센티브 증가로 기대치 하회 예상,2Q 영업이익, 소매판매 부진과 인센티브 증가로 기대치 하회 예상</t>
+  </si>
+  <si>
+    <t>2분기 실적은 기존 추정치 수준,2Q는 기존 추정치와 유사. 3Q 이후 점진적 회복 전망,17년도 2분기 Preview: 영업이익률 6.1% 전망</t>
+  </si>
+  <si>
+    <t>Hyundai Motor Company-Weak US sales weigh on 2Q results,2분기 실적은 기존 추정치와 컨센서스 하회할 전망,2분기 중국제외 글로벌 출고는 1.4% 전년 대비 증감율 증가했지만 리테일판매(중국제외)는 3.7% 감소, 미국영향으로 2분기 실적 부진 예상,2분기 실적은 기존 추정치와 컨센서스 하회할 전망,2분기 중국제외 글로벌 출고는 1.4% 전년 대비 증감율 증가했지만 리테일판매(중국제외)는 3.7% 감소</t>
+  </si>
+  <si>
+    <t>하반기 P와 Q 모두에서 성장 기대,17년도 2분기 Preview - 매출액 25.4 조원, 영업이익 1 조 5,446 억원(OPM 6.1%),P - 신차효과와 믹스개선, Q ? 국내공장과 기타시장 회복 기대</t>
+  </si>
+  <si>
+    <t>미국 부진 심화로 시각 조정 불가피,미국 부진 심화,다시 쌓이기 시작한 재고</t>
+  </si>
+  <si>
+    <t>모델 진부화의 끝자락에서,반등하던 주가가 판매부진에 기인한 Earnings shock 우려로 다시 하락,2분기 실적 예상치의 매출액을 25.6조, 영업이익을 1.47조로 하향하여 전망</t>
+  </si>
+  <si>
+    <t>한걸음 더 늦어졌지만 여전히 업황 개선추세 유효,17년도 2분기 Preview: 미국, 중국에 의한 부진한 분기실적 연출,신흥국 업황개선 추세는 지속적으로 이어지고 있음</t>
+  </si>
+  <si>
+    <t>하반기 실적은 국내공장 생산실적이 관건,주력 모델의 노후화와 맞물린 경쟁업체의 볼륨모델 신차,역대급 기저효과로 인해 하반기 증익은 가능 할 것,당장의 실적보다 새로운 전략적 변화를 기대</t>
+  </si>
+  <si>
+    <t>제품의 힘, 그랜저,제품의 힘: 그랜(다이)저, 현대차를 구하다,년도년도 1분기 2분기 Preview: 매출 및 영업이익은 양호하나 순이익 감소 전망, 여전히 업종내 방어주,업황 부진에도 부진은 상대적으로 미미,17년도 2분기 영업이익 1.46조원 전망</t>
+  </si>
+  <si>
+    <t>내수 호조 북미 부진이 상쇄,17년도 2분기 영업이익 1조 5,109억원 (-14.2%전년 대비 증감율)으로 시장기대치 하회 전망,하반기 내수 외에 미국 및 주요 지역 판매 둔화 지속 전망</t>
+  </si>
+  <si>
+    <t>하반기 회복 기조 전망되나 파업, 사드 영향 등 변수 확인 필요,2분기 연결기준 공장판매(+), ASP 및 믹스(+), 환율(-) 영향 추정,2분기 영업이익은 컨센서스 및 전년동기비 부진 전망</t>
+  </si>
+  <si>
+    <t>년도년도 1분기 2분기 Review ? 발목 잡는 G2시장의 부진,년도년도 1분기 2분기 영업이익, 추정치 11.0%하회,G2시장의 실적부진 장기화 우려</t>
+  </si>
+  <si>
+    <t>Hyundai Motor-Poor G2 performance weighs on 2Q results,17년도 2분기 영업이익, 추정치 11.0%하회,G2시장의 실적부진 장기화 우려, 년도년도 하반기 하반기 북미우려 지속,년도년도 하반기 2분기 , Shock,년도년도 하반기 하반기 어려운 영업환경 지속, 아쉬운 실적, 나아질 하반기,2분기 영업이익 1.34조원(-23.7% 전년 대비 증감율) 으로 컨센서스(1.53조원) 12.0% 하회,2분기 실적을 바닥으로 점진적인 개선, 3분기 영업이익 1.36조원(+27.2%) 전망, 마침표,17년도 2분기 은 12년 이후 6년간 지속됐던 Earnings Downtrend의 종점,시장: Hard Data (소득지표) 개선이 판매로 연결되기 시작할 17년도 하반기, 17년도 2분기 Review: 낮아진 기대치를 하회,영업이익 기준 컨센서스와 당사 추정치를 각각 10.4%, 11.8% 하회하였으며, 지배이익은 일회성 비용과 지분법이익 감소로 기대치를 대폭 하회함,특히, 2분기 판매보증충당금(5,884억원)은 세타 엔진 리콜 비용이 발생했던 지난 1분기 대비 1,750억원이나 증가해 예상 밖의 영업이익 감소를 불러왔음, 하반기 실적은 8월 임금협상이 관건,매출액 24,308십억원(전년 대비 증감율-1.5%), 영업이익 1,344십억원(전년 대비 증감율-23.7%), OPM 5.5%,차량, 금융, 기타사업부 동반 부진이 초래한 역대 최저수준의 2분기 영업이익, Hyundai Motor-Product competitiveness to drive gradual earnings improvement,17년도 2분기 영업이익 전년 대비 증감율 23.7% 감소, 부진 지속,핵심시장 수익부진 불구 17년도 하반기 전년 대비 증감율 영업이익 증가 전환 가능, 제품경쟁력 제고로 점진적 실적개선 (요약),17년도 2분기 영업이익 전년 대비 증감율 23.7% 감소, 부진 지속,핵심시장 수익부진 불구 17년도 하반기 전년 대비 증감율 영업이익 증가 전환 가능, Hyundai Motor-Getting past the worst,What’s new: 미국과 중국으로 부진한 2분기 실적,Positives: 신흥국 호조 지속 및 신차 출시,Negatives: 기대에 못 미친 국내 공장 가동률 상승효과와 단기 모멘텀 부재, 보릿고개를 넘기자,What’s new: 미국과 중국으로 부진한 2분기 실적,Positives: 신흥국 호조 지속 및 신차 출시,Negatives: 기대에 못 미친 국내 공장 가동률 상승효과와 단기 모멘텀 부재, Top-line과 Bottom-line의 온도차가 극심한 실적,17년도 2분기 Review - Top-line과 Bottom-line의 온도차가 극심한 실적, Hyundai Motor-Disappointing results, brighter prospects for 2H,2분기 영업이익 1.34조원(-23.7% 전년 대비 증감율) 으로 컨센서스(1.53조원) 12.0% 하회,2분기 실적을 바닥으로 점진적인 개선, 3분기 영업이익 1.36조원(+27.2%) 전망, Hyundai Motor-Disappointing results, brighter prospects for 2H,2분기 영업이익 1.34조원(-23.7% 전년 대비 증감율) 으로 컨센서스(1.53조원) 12.0% 하회,2분기 실적을 바닥으로 점진적인 개선, 3분기 영업이익 1.36조원(+27.2%) 전망, 제품경쟁력 제고로 점진적 실적개선,17년도 2분기 영업이익 전년 대비 증감율 23.7% 감소, 부진 지속,핵심시장 수익부진 불구 17년도 하반기 전년 대비 증감율 영업이익 증가 전환 가능, Hyundai Motor-Getting past the worst,What’s new: 미국과 중국으로 부진한 2분기 실적,Positives: 신흥국 호조 지속 및 신차 출시,Negatives: 기대에 못 미친 국내 공장 가동률 상승효과와 단기 모멘텀 부재, 제품경쟁력 제고로 점진적 실적개선,17년도 2분기 영업이익 전년 대비 증감율 23.7% 감소, 부진 지속,핵심시장 수익부진 불구 17년도 하반기 전년 대비 증감율 영업이익 증가 전환 가능, 제품경쟁력 제고로 점진적 실적개선 (요약),17년도 2분기 영업이익 전년 대비 증감율 23.7% 감소, 부진 지속,핵심시장 수익부진 불구 17년도 하반기 전년 대비 증감율 영업이익 증가 전환 가능, Hyundai Motor-Product competitiveness to drive gradual earnings improvement,17년도 2분기 영업이익 전년 대비 증감율 23.7% 감소, 부진 지속,핵심시장 수익부진 불구 17년도 하반기 전년 대비 증감율 영업이익 증가 전환 가능, 하반기 실적은 8월 임금협상이 관건,매출액 24,308십억원(전년 대비 증감율-1.5%), 영업이익 1,344십억원(전년 대비 증감율-23.7%), OPM 5.5%,차량, 금융, 기타사업부 동반 부진이 초래한 역대 최저수준의 2분기 영업이익, 17년도 2분기 Review: 낮아진 기대치를 하회,영업이익 기준 컨센서스와 당사 추정치를 각각 10.4%, 11.8% 하회하였으며, 지배이익은 일회성 비용과 지분법이익 감소로 기대치를 대폭 하회함,특히, 2분기 판매보증충당금(5,884억원)은 세타 엔진 리콜 비용이 발생했던 지난 1분기 대비 1,750억원이나 증가해 예상 밖의 영업이익 감소를 불러왔음, 부담을 덜고 맞이하는 하반기,17년도 2분기 Review ? 비용반영으로 시장 기대치 하회,하지만 2011 년 이후 가장 높은 판매 보증관련 비용(5,890 억원, 2.4%) 반영, 매도가능증권 손상차손 처리를 감안할 필요, 마침표,17년도 2분기 은 12년 이후 6년간 지속됐던 Earnings Downtrend의 종점,시장: Hard Data (소득지표) 개선이 판매로 연결되기 시작할 17년도 하반기, 주가 추세전환을 위한 조건 (요약),북미/중국사업 안정화 필요,2분기 Review-컨센서스 하회, 주가 추세전환을 위한 조건,북미/중국사업 안정화 필요,2분기 Review-컨센서스 하회, HMC-What is needed for shares to break out of range?,북미/중국사업 안정화 필요,2분기 Review-컨센서스 하회, 2분기 기대치 하회, 판매 및 품질 비용은 지속적인 부담 요인,현대차의 2017년 2분기 매출액은 전년 동기 대비 1.5% 감소한 24.3조원을 기록,3분기 실적은 기저효과로 지난해와 유사, G2에서의 부진으로 2Q 실적 예상 하회,2분기 실적은 당사 추정치와 컨센서스를 하회,미국시장 수요가 6개월 연속으로 전년 대비 증감율 감소, 보릿고개를 넘기자,What’s new: 미국과 중국으로 부진한 2분기 실적,Positives: 신흥국 호조 지속 및 신차 출시,Negatives: 기대에 못 미친 국내 공장 가동률 상승효과와 단기 모멘텀 부재</t>
+  </si>
+  <si>
+    <t>다양함이 나쁘지 않다,상반기 친환경차 판매 양호,하이브리드부터 수소차까지 친환경차 전 라인업 확보</t>
+  </si>
+  <si>
+    <t>픽업트럭 출시 고려 중,2000년대부터 시장이 요청하던 픽업트럭, 마침내 ‘고려’단계 진입,출시될 경우 미국에서 30년만에 첫 전륜구동 소형픽업트럭이 될 전망</t>
+  </si>
+  <si>
+    <t>별도손익의 개선 vs 미, 중 부진의 심화,17년 반기보고서에서 검토해봐야 할 것들,투자전략-3분기, 마지막 고비</t>
+  </si>
+  <si>
+    <t>FCEV, 외부와의 소통 카드,현대차, 2세대 FCEV 출시,FCEV 조기상용화, 브랜드 재정립을 위한 노력</t>
+  </si>
+  <si>
+    <t>공포 국면, 현대차가 답할 차례,중국파트너사와의 갈등, 중국사업 불확실성 확대,공정거래위원장, 현대차그룹의 사업구조 재편 필요성 강조</t>
   </si>
   <si>
     <t>Hyundai Motor-Needs to take action to spark recovery,중국파트너사와의 갈등, 중국사업 불확실성 확대,공정거래위원장, 현대차그룹의 사업구조 재편 필요성 강조</t>
   </si>
   <si>
-    <t>현대차- 악천후를 뚫고,중국 발 정치 리스크: 노이즈를 제거하면 희망이 보인다,신차 효과를 통한 판매 증대 및 내수 시장 방어로 하반기 마무리 전망, 현대차-비교적 조용한 역할 예상,지배구조 변화 국면에 적극 개입하지 않을 듯,지금은 펀더멘털 개선에 집중해야하는 시기</t>
-  </si>
-  <si>
-    <t>현대차-기저효과 이상의 영업실적 회복 필요 (요약),박스권 내에서의 주가등락,3분기 Preview: 기저효과로 영업이익 성장세 전환, HMC-Needs to get earnings back on track,박스권 내에서의 주가등락,3분기 Preview: 기저효과로 영업이익 성장세 전환, 현대차-기저효과 이상의 영업실적 회복 필요,박스권 내에서의 주가등락,3분기 Preview: 기저효과로 영업이익 성장세 전환</t>
-  </si>
-  <si>
-    <t>현대차-기다림의 시간은 필요,낮은 P/B, 배당수익률, 그리고 펀더멘털 점진 개선,17년도 3분기 Preview: 영업이익률 5.2% 전망</t>
-  </si>
-  <si>
-    <t>현대차-FCEV 핵심기술 독자개발,현대자동차 친환경차 라인업 계획,현대자동차 MEA와 금속분리판(Plate) 기술 독자 개발</t>
-  </si>
-  <si>
-    <t>현대차-수소연료전지차에 몇 안 되는 준비된 기업,차세대 양산형 수소연료전지차 FE 출시 예정,3분기 매출액은 1.2%(전년 대비 증감율) 증가한 22.3조 원으로 추정함</t>
-  </si>
-  <si>
-    <t>현대차-년도년도 1분기 3분기 Preview, 내수가 살린 실적,년도년도 1분기 3분기 Preview: 내수 판매 호조로 영업이익 13% 증가,지분법 이익의 감익 불가피</t>
-  </si>
-  <si>
-    <t>현대차-확인된 중국의 회복, 이제 남은 우려는 미국 뿐,중국.미국 외 지역에서의 고무적 판매성과 지속 중,중국, 9월 이후 본격적인 판매회복 시작, 현대차-년도년도 1분기 3분기 Preview: G2의 마지막 부진,년도년도 1분기 3분기 Preview: 美/中 G2 지역이 부진한 실적을 주도,년도년도 1분기 4분기 부터 신차 효과에 따른 점진적 실적개선을 기대</t>
-  </si>
-  <si>
-    <t>현대차-내수 호조를 미국 부진이 상쇄한 3분기,3분기 실적은 기존 추정치와 컨센서스 하회할 전망,내수판매와 국내공장 수출이 신차효과와 기저효과가 더해지며 전년 대비 증감율 크게 증가</t>
-  </si>
-  <si>
-    <t>현대차-투자심리 개선 진행중,신차효과로 미국은 2018년 하반기 판매량 회복을 기대,GM 등 글로벌 완성차 업체에 대한 투심 개선이 진행중, 현대차-최악의 실적이지만 바닥으로 기록될 것,17년도 3분기 Preview-최악의 실적이지만 바닥으로 기록될 것</t>
-  </si>
-  <si>
-    <t>현대차-주가 회복에 필요한 3가지,정책, 북미, 국내 불확실성 해소 필요,17년도 3분기 영업이익 1.18조원 전망</t>
-  </si>
-  <si>
-    <t>현대차- 반환점을 돌고 있는 주자,관찰 요소들: 중국과 미국 시장, 그리고 제품의 ‘인내력’,년도년도 1분기 3분기 : 영업이익 1.1조원 전망</t>
-  </si>
-  <si>
-    <t>Hyundai Motor-New model effects to support modest earnings recovery,17년도 3분기 영업이익 전년 대비 증감율 2% 증가에 그쳐 기대 하회 전망,향후 신차효과와 이머징 마켓 호전에 따라 완만한 실적회복 전망, 현대차-신차 통해 완만한 실적회복 전망 (요약),17년도 3분기 영업이익 전년 대비 증감율 2% 증가에 그쳐 기대 하회 전망,향후 신차효과와 이머징 마켓 호전에 따라 완만한 실적회복 전망, 현대차-신차 통해 완만한 실적회복 전망,17년도 3분기 영업이익 전년 대비 증감율 2% 증가에 그쳐 기대 하회 전망,향후 신차효과와 이머징 마켓 호전에 따라 완만한 실적회복 전망, 현대차-기대보다는 낮지만, 회복은 시작,17년도 3분기 Preview-매출액 23.2 조원, 영업이익 1 조 1,505 억원(OPM 5.0%),17년도 4분기 및 2018 년 사업계획에 관심</t>
-  </si>
-  <si>
-    <t>현대차-기저와 신차의 힘으로 판매 반등,2018년 영업이익 5.7조원(+14.5% 전년 대비 증감율)으로 대폭 개선될 전망,신차 모멘텀으로 판매 개선 극대화</t>
-  </si>
-  <si>
-    <t>현대차-년도년도 1분기 3분기 Review: Kospi가는길, 더 이상 방해하지 않겠어요,년도년도 1분기 3분기 영업이익, 추정치 1.2% 상회,미국 부진만 남았다</t>
-  </si>
-  <si>
-    <t>현대차-우려에 비해 양호한 3분기 실적,3분기 실적은 당사 추정치와 시장 컨센서스를 상회하며 우려에 비해 양호한 실적 시현, 유럽/미국 등 해외판매법인의 판매실적이 예상보다 좋았던 것으로 보이며 판매보증충당금 전입액도 예상보다 적게 반영,3분기 연결 매출액은 24.2조원(+9.6% 전년 대비 증감율)으로 당사 추정치와 컨센서스를 각각 5.4%, 4.4% 상회, 공장별 매출액은 예상치에 대체로 부합했으나 미국/유럽 등 주요 판매법인의 매출액이 당사 추정보다 양호했던 것으로 판단, 현대차-실로 오랜만에 맛본 영업이익 증가,17년도 3분기 Review - 실로 오랜만에 맛본 영업이익 증가,17년도 4분기 Preview - 강성노조라는 변수에도 긍정적 기대감 커, 현대차-회복을 이어가기 위한 합리적 계획 필요,17년도 3분기 Review ? 낮아진 시장전망치를 상회,회복을 이어가기 위해서, Hyundai Motor-Profits rise for first time in 3.5 years,17년도 3분기 영업이익, 추정치 1.2% 상회,미국 부진만 남았다, 현대차-여전히 불확실한 18년 전망,17년도 3분기 , 내수의 힘,18년, 주요 지역 판매 둔화 지속 전망, 현대차-낮아진 시장 예상 부합, 년도년도 1분기 4분기 는?년도 이분기 ,3Q17 국내 기저효과로 낮아진 시장 예상 부합,년도년도 1분기 4분기 이후 기저효과 기대를 낮추는 3가지 요인, 현대차-주가 박스권 상향,2018년 실적 방향성 개선으로 순자산가치대비 주가 할인요인 축소 예상,3분기 Review - 컨센서스 상회, 현대차-3분기 컨센서스 부합, 4분기도 개선세 전망,3분기 실적은 컨센서스에 부합,4분기에도 실적 개선세 전망, 현대차-단기 저점을 통과,17년도 3분기 영업이익 1조 2,042억원(전년 대비 증감율 +12.7%) 기록,지배순이익은 8,524억원(전년 대비 증감율 -19.7%) 기록하며 낮았던 시장기대치를 상회, 현대차-반가운 이익 회복. 최악의 국면을 지나는 중,17년도 3분기 Review: 오랜만에 찾아온 분기 영업이익 성장,신차 &amp; 믹스 개선 효과 지속, 점진적인 실적 개선 전망, 현대차-년도년도 1분기 3분기 Review: 판매호조가 빚어낸 우수한 결과,년도년도 1분기 3분기 Review: 영업이익 1.2조원 기록으로 시장 기대치 상회,년도년도 1분기 4분기 은 완만한 개선, 2018년부터 기대요인 크게 강화, 현대차-3분기 기대치 상회, 강력한 신차효과 지속 가능할까?,3분기 실적 리뷰 : 강한 신차 효과,4분기 실적은 지난해와 비슷, 현대차-미국 외 글로벌에서 회복 중,3Q 양호. 4Q 중국/신흥국 회복과 배당 수익,17년도 3분기 Review: 영업이익률 5.0% 기록, HMC-Share price set to break free of range,2018년 실적 방향성 개선으로 순자산가치대비 주가 할인요인 축소 예상,3분기 Review - 컨센서스 상회, 현대차-주가 박스권 상향(요약),2018년 실적 방향성 개선으로 순자산가치대비 주가 할인요인 축소 예상,3분기 Review ? 컨센서스 상회, 현대차-리스크 해소 중,3분기 영업이익 1.20조원(+12.7%)으로 컨센서스(1.16조원) 부합,중국 판매 반등 효과가 예상보다 빠르게 손익에 반영, 현대차-바닥을 통과한 실적,What’s new: 영업이익 컨센서스 3.7% 상회,Positives: 중국 가동률 회복, Hyundai Motor-Earnings bottoming out,What’s new: 영업이익 컨센서스 3.7% 상회,Positives: 중국 가동률 회복, 현대차-년도년도 1분기 3분기 기대부합, 신차 통해 실적개선 예상,년도년도 1분기 3분기 영업이익 1.2조원(전년 대비 증감율 12.7% 증가)으로 기대에 부합,신차효과와 이머징 마켓 호전에 따라 완만한 실적회복 예상, 현대차-년도년도 1분기 3분기 기대부합, 신차 통해 실적개선 예상 (요약),년도년도 1분기 3분기 영업이익 1.2조원(전년 대비 증감율 12.7% 증가)으로 기대에 부합,신차효과와 이머징 마켓 호전에 따라 완만한 실적회복 예상, 현대차-년도년도 1분기 3분기 Review: 기대치 상회, 2018년 본격적인 개선 기대,년도년도 1분기 3분기 Review: 자동차 부문의 호조로 시장 기대치를 상회,년도년도 1분기 4분기 Preview: 기저 효과로 인한 증익 추세 유지, 현대차-년도년도 1분기 3분기 기대부합, 신차 통해 실적개선 예상(요약),년도년도 1분기 3분기 영업이익 1.2조원(전년 대비 증감율 12.7% 증가)으로 기대에 부합,신차효과와 이머징 마켓 호전에 따라 완만한 실적회복 예상, 현대차-년도년도 1분기 3분기 기대부합, 신차 통해 실적개선 예상 (요약),년도년도 1분기 3분기 영업이익 1.2조원(전년 대비 증감율 12.7% 증가)으로 기대에 부합,신차효과와 이머징 마켓 호전에 따라 완만한 실적회복 예상, 현대차-년도년도 1분기 3분기 기대부합, 신차 통해 실적개선 예상,년도년도 1분기 3분기 영업이익 1.2조원(전년 대비 증감율 12.7% 증가)으로 기대에 부합,신차효과와 이머징 마켓 호전에 따라 완만한 실적회복 예상, 현대차-마침표, 펀더멘탈 반등의 시작,17년도 3분기 Review: Cycle 교체시점에서 발현된 유의미한 실적개선,핵심은 cycle 이 본격화될 18 년 이익방향성 (EPS +42.2% 전년 대비 증감율 전망), Hyundai Motor-Earnings bottoming out,What’s new: 영업이익 컨센서스 3.7% 상회,Positives: 중국 가동률 회복, 현대차-바닥을 통과한 실적,What’s new: 영업이익 컨센서스 3.7% 상회,Positives: 중국 가동률 회복</t>
-  </si>
-  <si>
-    <t>현대차-바닥을 통과한 실적 (요약),What’s new: 영업이익 컨센서스 3.7% 상회,Positives: 중국 가동률 회복</t>
-  </si>
-  <si>
-    <t>현대차-년도년도 1분기 3분기 Review: 판매호조가 빚어낸 우수한 결과,년도년도 1분기 3분기 Review: 영업이익 1.2조원 기록으로 시장 기대치 상회,년도년도 1분기 4분기 은 완만한 개선, 2018년부터 기대요인 크게 강화</t>
-  </si>
-  <si>
-    <t>현대차-2018년 출하/이익 회복과 EV 대응력 강화,출하 회복과 EV 대응력 강화,영업이익과 지분법이익 동반 증가로 순이익 27% 증가</t>
-  </si>
-  <si>
-    <t>현대차-2018년 판매/실적 모두 턴어라운드,2018년 리테일 판매 전년 대비 증감율 +12.4%,2018년 역대급 신차 라인업, 현대차-2018년은 판매는 회복, 실적은 정체,2018년 판매 8%, 생산 6.2% 증가,매출액, 영업이익 성장 없을 듯, 순이익은 개선</t>
-  </si>
-  <si>
-    <t>현대차-현대차 년도년도 1분기 3분기 실적 리뷰,년도년도 1분기 3분기 Review: 영업이익률 5.0% 기록,실적발표 IR의 주요 내용: 시장 변화에 적극 대응</t>
-  </si>
-  <si>
-    <t>현대차-신차 경쟁력 회복이 관건,17년도 3분기 , 시장기대치 상회,18년, 주요 지역 판매 둔화 지속 전망,신차 경쟁력 회복 18년도 하반기 확인 가능</t>
-  </si>
-  <si>
-    <t>현대차-BIG2 시장 회복을 기대해 보자,기저 속 신차 모맨텀을 통한 회복세 기대,‘18년 글로벌 8.8% 성장한 498만대 전망, 현대차-기저효과, 18년도 하반기 가시화,정책, 북미, 국내 불확실성 해소 필요,투자 포인트와 리스크 요인</t>
-  </si>
-  <si>
-    <t>현대차-중국 회복과 함께 단기 주가는 양호. 2018년 상반기까지 보면 아직은 보수적,중국 공장 가동 회복과 함께 주가는 2017년 12월까지 양호한 흐름 예상,다만, 2018년 상반기까지 투자 기간을 늘릴 경우, 보수적 의견 제시</t>
-  </si>
-  <si>
-    <t>현대차-5년간의 실적하락세에서 벗어날 전망,차세대 파워트레인과 SUV 모델 강화,2018년은 5년간 실적 하락세에서 벗어날 전망, 현대차-2018년 전망: 길었던 침묵을 깨고 추격을 시작,2020년까지 실적회복,미국과 아중동 시장만 남았다</t>
-  </si>
-  <si>
-    <t>현대차-명백한 이익개선 Cycle의 시작,18년 EPS +39% 전년 대비 증감율 전망,지배구조 개편 시 최대 수혜 가능</t>
+    <t>악천후를 뚫고,중국 발 정치 리스크: 노이즈를 제거하면 희망이 보인다,신차 효과를 통한 판매 증대 및 내수 시장 방어로 하반기 마무리 전망, 비교적 조용한 역할 예상,지배구조 변화 국면에 적극 개입하지 않을 듯,지금은 펀더멘털 개선에 집중해야하는 시기</t>
+  </si>
+  <si>
+    <t>기저효과 이상의 영업실적 회복 필요 (요약),박스권 내에서의 주가등락,3분기 Preview: 기저효과로 영업이익 성장세 전환, HMC-Needs to get earnings back on track,박스권 내에서의 주가등락,3분기 Preview: 기저효과로 영업이익 성장세 전환, 기저효과 이상의 영업실적 회복 필요,박스권 내에서의 주가등락,3분기 Preview: 기저효과로 영업이익 성장세 전환</t>
+  </si>
+  <si>
+    <t>기다림의 시간은 필요,낮은 P/B, 배당수익률, 그리고 펀더멘털 점진 개선,17년도 3분기 Preview: 영업이익률 5.2% 전망</t>
+  </si>
+  <si>
+    <t>FCEV 핵심기술 독자개발,현대자동차 친환경차 라인업 계획,현대자동차 MEA와 금속분리판(Plate) 기술 독자 개발</t>
+  </si>
+  <si>
+    <t>수소연료전지차에 몇 안 되는 준비된 기업,차세대 양산형 수소연료전지차 FE 출시 예정,3분기 매출액은 1.2%(전년 대비 증감율) 증가한 22.3조 원으로 추정함</t>
+  </si>
+  <si>
+    <t>년도년도 1분기 3분기 Preview, 내수가 살린 실적,년도년도 1분기 3분기 Preview: 내수 판매 호조로 영업이익 13% 증가,지분법 이익의 감익 불가피</t>
+  </si>
+  <si>
+    <t>확인된 중국의 회복, 이제 남은 우려는 미국 뿐,중국.미국 외 지역에서의 고무적 판매성과 지속 중,중국, 9월 이후 본격적인 판매회복 시작, 년도년도 1분기 3분기 Preview: G2의 마지막 부진,년도년도 1분기 3분기 Preview: 美/中 G2 지역이 부진한 실적을 주도,년도년도 1분기 4분기 부터 신차 효과에 따른 점진적 실적개선을 기대</t>
+  </si>
+  <si>
+    <t>내수 호조를 미국 부진이 상쇄한 3분기,3분기 실적은 기존 추정치와 컨센서스 하회할 전망,내수판매와 국내공장 수출이 신차효과와 기저효과가 더해지며 전년 대비 증감율 크게 증가</t>
+  </si>
+  <si>
+    <t>투자심리 개선 진행중,신차효과로 미국은 2018년 하반기 판매량 회복을 기대,GM 등 글로벌 완성차 업체에 대한 투심 개선이 진행중, 최악의 실적이지만 바닥으로 기록될 것,17년도 3분기 Preview-최악의 실적이지만 바닥으로 기록될 것</t>
+  </si>
+  <si>
+    <t>주가 회복에 필요한 3가지,정책, 북미, 국내 불확실성 해소 필요,17년도 3분기 영업이익 1.18조원 전망</t>
+  </si>
+  <si>
+    <t>반환점을 돌고 있는 주자,관찰 요소들: 중국과 미국 시장, 그리고 제품의 ‘인내력’,년도년도 1분기 3분기 : 영업이익 1.1조원 전망</t>
+  </si>
+  <si>
+    <t>Hyundai Motor-New model effects to support modest earnings recovery,17년도 3분기 영업이익 전년 대비 증감율 2% 증가에 그쳐 기대 하회 전망,향후 신차효과와 이머징 마켓 호전에 따라 완만한 실적회복 전망, 신차 통해 완만한 실적회복 전망 (요약),17년도 3분기 영업이익 전년 대비 증감율 2% 증가에 그쳐 기대 하회 전망,향후 신차효과와 이머징 마켓 호전에 따라 완만한 실적회복 전망, 신차 통해 완만한 실적회복 전망,17년도 3분기 영업이익 전년 대비 증감율 2% 증가에 그쳐 기대 하회 전망,향후 신차효과와 이머징 마켓 호전에 따라 완만한 실적회복 전망, 기대보다는 낮지만, 회복은 시작,17년도 3분기 Preview-매출액 23.2 조원, 영업이익 1 조 1,505 억원(OPM 5.0%),17년도 4분기 및 2018 년 사업계획에 관심</t>
+  </si>
+  <si>
+    <t>기저와 신차의 힘으로 판매 반등,2018년 영업이익 5.7조원(+14.5% 전년 대비 증감율)으로 대폭 개선될 전망,신차 모멘텀으로 판매 개선 극대화</t>
+  </si>
+  <si>
+    <t>년도년도 1분기 3분기 Review: Kospi가는길, 더 이상 방해하지 않겠어요,년도년도 1분기 3분기 영업이익, 추정치 1.2% 상회,미국 부진만 남았다</t>
+  </si>
+  <si>
+    <t>우려에 비해 양호한 3분기 실적,3분기 실적은 당사 추정치와 시장 컨센서스를 상회하며 우려에 비해 양호한 실적 시현, 유럽/미국 등 해외판매법인의 판매실적이 예상보다 좋았던 것으로 보이며 판매보증충당금 전입액도 예상보다 적게 반영,3분기 연결 매출액은 24.2조원(+9.6% 전년 대비 증감율)으로 당사 추정치와 컨센서스를 각각 5.4%, 4.4% 상회, 공장별 매출액은 예상치에 대체로 부합했으나 미국/유럽 등 주요 판매법인의 매출액이 당사 추정보다 양호했던 것으로 판단, 실로 오랜만에 맛본 영업이익 증가,17년도 3분기 Review - 실로 오랜만에 맛본 영업이익 증가,17년도 4분기 Preview - 강성노조라는 변수에도 긍정적 기대감 커, 회복을 이어가기 위한 합리적 계획 필요,17년도 3분기 Review ? 낮아진 시장전망치를 상회,회복을 이어가기 위해서, Hyundai Motor-Profits rise for first time in 3.5 years,17년도 3분기 영업이익, 추정치 1.2% 상회,미국 부진만 남았다, 여전히 불확실한 18년 전망,17년도 3분기 , 내수의 힘,18년, 주요 지역 판매 둔화 지속 전망, 낮아진 시장 예상 부합, 년도년도 1분기 4분기 는?년도 이분기 ,3Q17 국내 기저효과로 낮아진 시장 예상 부합,년도년도 1분기 4분기 이후 기저효과 기대를 낮추는 3가지 요인, 주가 박스권 상향,2018년 실적 방향성 개선으로 순자산가치대비 주가 할인요인 축소 예상,3분기 Review - 컨센서스 상회, 3분기 컨센서스 부합, 4분기도 개선세 전망,3분기 실적은 컨센서스에 부합,4분기에도 실적 개선세 전망, 단기 저점을 통과,17년도 3분기 영업이익 1조 2,042억원(전년 대비 증감율 +12.7%) 기록,지배순이익은 8,524억원(전년 대비 증감율 -19.7%) 기록하며 낮았던 시장기대치를 상회, 반가운 이익 회복. 최악의 국면을 지나는 중,17년도 3분기 Review: 오랜만에 찾아온 분기 영업이익 성장,신차 &amp; 믹스 개선 효과 지속, 점진적인 실적 개선 전망, 년도년도 1분기 3분기 Review: 판매호조가 빚어낸 우수한 결과,년도년도 1분기 3분기 Review: 영업이익 1.2조원 기록으로 시장 기대치 상회,년도년도 1분기 4분기 은 완만한 개선, 2018년부터 기대요인 크게 강화, 3분기 기대치 상회, 강력한 신차효과 지속 가능할까?,3분기 실적 리뷰 : 강한 신차 효과,4분기 실적은 지난해와 비슷, 미국 외 글로벌에서 회복 중,3Q 양호. 4Q 중국/신흥국 회복과 배당 수익,17년도 3분기 Review: 영업이익률 5.0% 기록, HMC-Share price set to break free of range,2018년 실적 방향성 개선으로 순자산가치대비 주가 할인요인 축소 예상,3분기 Review - 컨센서스 상회, 주가 박스권 상향(요약),2018년 실적 방향성 개선으로 순자산가치대비 주가 할인요인 축소 예상,3분기 Review ? 컨센서스 상회, 리스크 해소 중,3분기 영업이익 1.20조원(+12.7%)으로 컨센서스(1.16조원) 부합,중국 판매 반등 효과가 예상보다 빠르게 손익에 반영, 바닥을 통과한 실적,What’s new: 영업이익 컨센서스 3.7% 상회,Positives: 중국 가동률 회복, Hyundai Motor-Earnings bottoming out,What’s new: 영업이익 컨센서스 3.7% 상회,Positives: 중국 가동률 회복, 년도년도 1분기 3분기 기대부합, 신차 통해 실적개선 예상,년도년도 1분기 3분기 영업이익 1.2조원(전년 대비 증감율 12.7% 증가)으로 기대에 부합,신차효과와 이머징 마켓 호전에 따라 완만한 실적회복 예상, 년도년도 1분기 3분기 기대부합, 신차 통해 실적개선 예상 (요약),년도년도 1분기 3분기 영업이익 1.2조원(전년 대비 증감율 12.7% 증가)으로 기대에 부합,신차효과와 이머징 마켓 호전에 따라 완만한 실적회복 예상, 년도년도 1분기 3분기 Review: 기대치 상회, 2018년 본격적인 개선 기대,년도년도 1분기 3분기 Review: 자동차 부문의 호조로 시장 기대치를 상회,년도년도 1분기 4분기 Preview: 기저 효과로 인한 증익 추세 유지, 년도년도 1분기 3분기 기대부합, 신차 통해 실적개선 예상(요약),년도년도 1분기 3분기 영업이익 1.2조원(전년 대비 증감율 12.7% 증가)으로 기대에 부합,신차효과와 이머징 마켓 호전에 따라 완만한 실적회복 예상, 년도년도 1분기 3분기 기대부합, 신차 통해 실적개선 예상 (요약),년도년도 1분기 3분기 영업이익 1.2조원(전년 대비 증감율 12.7% 증가)으로 기대에 부합,신차효과와 이머징 마켓 호전에 따라 완만한 실적회복 예상, 년도년도 1분기 3분기 기대부합, 신차 통해 실적개선 예상,년도년도 1분기 3분기 영업이익 1.2조원(전년 대비 증감율 12.7% 증가)으로 기대에 부합,신차효과와 이머징 마켓 호전에 따라 완만한 실적회복 예상, 마침표, 펀더멘탈 반등의 시작,17년도 3분기 Review: Cycle 교체시점에서 발현된 유의미한 실적개선,핵심은 cycle 이 본격화될 18 년 이익방향성 (EPS +42.2% 전년 대비 증감율 전망), Hyundai Motor-Earnings bottoming out,What’s new: 영업이익 컨센서스 3.7% 상회,Positives: 중국 가동률 회복, 바닥을 통과한 실적,What’s new: 영업이익 컨센서스 3.7% 상회,Positives: 중국 가동률 회복</t>
+  </si>
+  <si>
+    <t>바닥을 통과한 실적 (요약),What’s new: 영업이익 컨센서스 3.7% 상회,Positives: 중국 가동률 회복</t>
+  </si>
+  <si>
+    <t>년도년도 1분기 3분기 Review: 판매호조가 빚어낸 우수한 결과,년도년도 1분기 3분기 Review: 영업이익 1.2조원 기록으로 시장 기대치 상회,년도년도 1분기 4분기 은 완만한 개선, 2018년부터 기대요인 크게 강화</t>
+  </si>
+  <si>
+    <t>2018년 출하/이익 회복과 EV 대응력 강화,출하 회복과 EV 대응력 강화,영업이익과 지분법이익 동반 증가로 순이익 27% 증가</t>
+  </si>
+  <si>
+    <t>2018년 판매/실적 모두 턴어라운드,2018년 리테일 판매 전년 대비 증감율 +12.4%,2018년 역대급 신차 라인업, 2018년은 판매는 회복, 실적은 정체,2018년 판매 8%, 생산 6.2% 증가,매출액, 영업이익 성장 없을 듯, 순이익은 개선</t>
+  </si>
+  <si>
+    <t>현대차 년도년도 1분기 3분기 실적 리뷰,년도년도 1분기 3분기 Review: 영업이익률 5.0% 기록,실적발표 IR의 주요 내용: 시장 변화에 적극 대응</t>
+  </si>
+  <si>
+    <t>신차 경쟁력 회복이 관건,17년도 3분기 , 시장기대치 상회,18년, 주요 지역 판매 둔화 지속 전망,신차 경쟁력 회복 18년도 하반기 확인 가능</t>
+  </si>
+  <si>
+    <t>BIG2 시장 회복을 기대해 보자,기저 속 신차 모맨텀을 통한 회복세 기대,‘18년 글로벌 8.8% 성장한 498만대 전망, 기저효과, 18년도 하반기 가시화,정책, 북미, 국내 불확실성 해소 필요,투자 포인트와 리스크 요인</t>
+  </si>
+  <si>
+    <t>중국 회복과 함께 단기 주가는 양호. 2018년 상반기까지 보면 아직은 보수적,중국 공장 가동 회복과 함께 주가는 2017년 12월까지 양호한 흐름 예상,다만, 2018년 상반기까지 투자 기간을 늘릴 경우, 보수적 의견 제시</t>
+  </si>
+  <si>
+    <t>5년간의 실적하락세에서 벗어날 전망,차세대 파워트레인과 SUV 모델 강화,2018년은 5년간 실적 하락세에서 벗어날 전망, 2018년 전망: 길었던 침묵을 깨고 추격을 시작,2020년까지 실적회복,미국과 아중동 시장만 남았다</t>
+  </si>
+  <si>
+    <t>명백한 이익개선 Cycle의 시작,18년 EPS +39% 전년 대비 증감율 전망,지배구조 개편 시 최대 수혜 가능</t>
   </si>
   <si>
     <t>현대차,중국의 신차출시로 판매량 회복이 이어지는 가운데, 미국의 SUV 확대로 재고 및 인센티브 하락이 나타날 전망,10년 만에 출시되는 신형 엔진은 가성비 매력을 되찾아 점유율을 회복하기 위한 필수 조건</t>
   </si>
   <si>
-    <t>Hyundai Motor-Spring finally comes after a long winter,코나를 중심으로 한 SUV 신차 효과, 2018년 글로벌 판매량 8.8% 증가,5년간 지속된 이익 감소, 전환점을 맞이하다: 2018 EPS Growth +35.0 %, 현대차-겨울이 깊어지면 봄이 온다,코나를 중심으로 한 SUV 신차 효과, 2018년 글로벌 판매량 8.8% 증가,5년간 지속된 이익 감소, 전환점을 맞이하다: 2018 EPS Growth +35.0 %</t>
-  </si>
-  <si>
-    <t>현대차-2018년 경쟁력 개선 싸이클,2018년 미국 시장 제외 글로벌 주요 시장 전반적으로 판매실적 및 공장가동 호전 전망,코나, 싼타페 후속, 대형 SUV 등 SUV 라인업 점진적 강화, 중국 현지전략형 모델투입 강화</t>
-  </si>
-  <si>
-    <t>현대차-부진을 벗어나 회복 진행 중,부진을 벗어나 회복 진행 중</t>
-  </si>
-  <si>
-    <t>현대차-디스카운트 요인이 점점 사라지고 있다,이익 감소의 전환점, 경쟁력 있는 제품으로 성장한다,현기차의 친환경차 기술력은 글로벌 Top 급, 현대차-중국 회복, 신흥국 성장 수혜,중국 회복, 신흥국 성장 수혜,하방경직성 강화, 제한적 반등 예상</t>
-  </si>
-  <si>
-    <t>현대차-12 월 글로벌 판매실적 업데이트,현대차 12월 도매판매, 국내 및 중국 판매감소로 전년동기 대비 -17% 하락,중국의 전월 대비 증감율 판매회복세 지속 중</t>
-  </si>
-  <si>
-    <t>현대차-2019년을 준비,박스권 주가흐름에서 벗어나려면..,4분기 Preview: 기말환율 하락에 따른 판매보증충당금 환입효과, 현대차-혼재된 우려에 대한 해석,17년도 4분기 영업이익, 1.12 조원 (+9% 전년 대비 증감율) 전망,18 년 연간판매, 보수적 사업계획을 상회하는 491 만대 (+7% 전년 대비 증감율) 전망</t>
-  </si>
-  <si>
-    <t>현대차-환율 하락이 부정적으로 반영,17년도 4분기 Preview: 영업이익률 4.4% 전망,2018년 도매판매 목표는 4% 증가한 467.5만대</t>
-  </si>
-  <si>
-    <t>현대차-새로운 생각, 새로운 가능성,현대차그룹: 세계 BEV 판매 6위 기록,그룹 친환경차 전략의 선두주자, 현대차-디스카운트 해소가 기대되는 한해,신차 출시효과, SUV라인업 확대 등 제품믹스 개선과 친환경차 비중 증가,17년도 4분기 실적은 파업, 조업일수 감소, 원화강세 영향으로 시장 기대치 하회 전망</t>
+    <t>Hyundai Motor-Spring finally comes after a long winter,코나를 중심으로 한 SUV 신차 효과, 2018년 글로벌 판매량 8.8% 증가,5년간 지속된 이익 감소, 전환점을 맞이하다: 2018 EPS Growth +35.0 %, 겨울이 깊어지면 봄이 온다,코나를 중심으로 한 SUV 신차 효과, 2018년 글로벌 판매량 8.8% 증가,5년간 지속된 이익 감소, 전환점을 맞이하다: 2018 EPS Growth +35.0 %</t>
+  </si>
+  <si>
+    <t>2018년 경쟁력 개선 싸이클,2018년 미국 시장 제외 글로벌 주요 시장 전반적으로 판매실적 및 공장가동 호전 전망,코나, 싼타페 후속, 대형 SUV 등 SUV 라인업 점진적 강화, 중국 현지전략형 모델투입 강화</t>
+  </si>
+  <si>
+    <t>부진을 벗어나 회복 진행 중,부진을 벗어나 회복 진행 중</t>
+  </si>
+  <si>
+    <t>디스카운트 요인이 점점 사라지고 있다,이익 감소의 전환점, 경쟁력 있는 제품으로 성장한다,현기차의 친환경차 기술력은 글로벌 Top 급, 중국 회복, 신흥국 성장 수혜,중국 회복, 신흥국 성장 수혜,하방경직성 강화, 제한적 반등 예상</t>
+  </si>
+  <si>
+    <t>12 월 글로벌 판매실적 업데이트,현대차 12월 도매판매, 국내 및 중국 판매감소로 전년동기 대비 -17% 하락,중국의 전월 대비 증감율 판매회복세 지속 중</t>
+  </si>
+  <si>
+    <t>2019년을 준비,박스권 주가흐름에서 벗어나려면..,4분기 Preview: 기말환율 하락에 따른 판매보증충당금 환입효과, 혼재된 우려에 대한 해석,17년도 4분기 영업이익, 1.12 조원 (+9% 전년 대비 증감율) 전망,18 년 연간판매, 보수적 사업계획을 상회하는 491 만대 (+7% 전년 대비 증감율) 전망</t>
+  </si>
+  <si>
+    <t>환율 하락이 부정적으로 반영,17년도 4분기 Preview: 영업이익률 4.4% 전망,2018년 도매판매 목표는 4% 증가한 467.5만대</t>
+  </si>
+  <si>
+    <t>새로운 생각, 새로운 가능성,현대차그룹: 세계 BEV 판매 6위 기록,그룹 친환경차 전략의 선두주자, 디스카운트 해소가 기대되는 한해,신차 출시효과, SUV라인업 확대 등 제품믹스 개선과 친환경차 비중 증가,17년도 4분기 실적은 파업, 조업일수 감소, 원화강세 영향으로 시장 기대치 하회 전망</t>
   </si>
   <si>
     <t>현대차,2018년 리테일 판매 505만대(전년 대비 증감율 +12.4%)를 기록할 전망. 기저 효과가 큰 중국 시장, 고성장세에 접어든 이머징 시장, 점유율 확대되고 있는 내수 시장이 성장을 견인,신형 싼타페, 투싼 F/L 등 SUV 신차 라인업 강화로 판매 부진에서 벗어날 전망</t>
   </si>
   <si>
-    <t>현대차-4Q 실적 저조 예상, 환율부담 가중,4분기 실적은 기존 추정치와 시장 컨센서스를 하회할 것으로 예상,미국시장 부진을 타개할 방법은 SUV 중심의 신차투입</t>
-  </si>
-  <si>
-    <t>Hyundai Motor-Earnings growth to be modest in 2018,17년도 4분기 영업이익 9,586억원으로 크게 부진할 것으로 추정,기대에는 못 미치지만 2018년 실적 우상향 전망 유효, 현대차-협력을 통한 기술개발 강화,현대차, 자율주행기술 개발을 위한 Aurora Project 발표,자율주행을 양분한 Intel Mobileye 연맹 및 NVIDIA 연맹과도 제휴, 현대차-Future Mobility 전략 및 이익 개선 방향성의 구체화,CES 기간 중 발표된 6가지 Future Mobility 전략:자동차 업체를 넘어 ICT 업체로 진화 포부,18년 지배주주 순이익 +38% 전년 대비 증감율, 지난 5년 간 이어졌던 이익 축소 방향성 해제될 전망, 현대차-또 한번의 실망감과 점진적 우상향,17년도 4분기 영업이익 9,586억원으로 크게 부진할 것으로 추정,기대에는 못 미치지만 2018년 실적 우상향 전망 유효</t>
-  </si>
-  <si>
-    <t>현대차-년도년도 1분기 4분기 Preview: 길어진진,년도 분기 1Q18부터는 개선,년도년도 1분기 4분기 Preview: 영업이익 1.05조원 기록으로 시장 기대치 하회 예상,美시장 M/S 회복 가능성으로 하방 경직성 강화, 현대차-외부 협력을 통한 체질 개선,CES 2018 관전 포인트: 1) 오로라(자율주행), 2) AI 비서,CES 2018 관전 포인트: 3) 넥쏘(수소차)</t>
-  </si>
-  <si>
-    <t>현대차-부진한 현실에 안주할건가,전통적 산업 영역 내 안주,17년도 4분기 영업이익 1.03조원 전망</t>
-  </si>
-  <si>
-    <t>현대차-년도년도 1분기 4분기 실적 업데이트,년도년도 1분기 4분기 Review: 매출 기대치 1.6% 상회, 영업이익 기대치 33.2% 하회</t>
-  </si>
-  <si>
-    <t>Hyundai Motor-A disappointing end to the year,4분기 영업이익 0.78조원(-24.1%)으로 컨센서스(1.12조원) 하회,1회성 이슈가 다수 발생, 18년도 1분기 정상화 예상, 현대차-바닥의 깊이보다 방향성을 보자,Facts: 부진한 4분기 실적,Pros &amp; cons: 이익 감소에도 배당금액 유지, SUV 확대 본격화, Hyundai Motor-More emphasis on road to recovery,Facts: 부진한 4분기 실적,Pros &amp; cons: 이익 감소에도 배당금액 유지, SUV 확대 본격화, 현대차-예상보다 더 부진했지만 지난 실적,17년도 4분기 영업이익 7,752억원 기록(전년 대비 증감율 24.1% 감소)해 크게 부진,2018년 실적 우상향 전망 유효, Hyundai Motor-Weaker than feared, but the worst is over,17년도 4분기 영업이익 7,752억원 기록(전년 대비 증감율 24.1% 감소)해 크게 부진,2018년 실적 우상향 전망 유효, 현대차-구원투수(신차) 등판이 필요한 실적,매출액 24조원(전년 대비 증감율-0.2%), 영업이익 7,752억원(전년 대비 증감율-24.1%), OPM 3.2%,국내, 미국 동반 부진이 초래한 역대 최저수준의 차량사업부 수익성, 현대차-년도년도 1분기 4분기 Review: 실적은 쇼크였지만 긍정적인 부분을 찾는다면,년도년도 1분기 4분기 Review: 파업, 환율, 판매 비용 증가로 기대치를 큰 폭으로 하회,18년도 1분기 Preview: 파업 영향권이나 신차 효과 본격화 시기, 현대차-바닥의 깊이보다 방향성을 보자,Facts: 부진한 4분기 실적,Pros &amp; cons: 이익 감소에도 배당금액 유지, SUV 확대 본격화, 현대차-Cycle의 전환점,실패한 13 년 Cycle 의 마무리 17년도 4분기 ,3 월, 기저효과와 함께할 새로운 신차 Cycle 의 본격적인 시작, 현대차-2018년도 어려운 환경,주가 박스권 상향을 위한 필요조건,4분기 Review ? 실적 부진 지속, Hyundai Motor-More emphasis on road to recovery,Facts: 부진한 4분기 실적,Pros &amp; cons: 이익 감소에도 배당금액 유지, SUV 확대 본격화, 현대차-예상보다 더 부진했지만 지난 실적,17년도 4분기 영업이익 7,752억원 기록(전년 대비 증감율 24.1% 감소)해 크게 부진,2018년 실적 우상향 전망 유효, Hyundai Motor-Weaker than feared, but the worst is over,17년도 4분기 영업이익 7,752억원 기록(전년 대비 증감율 24.1% 감소)해 크게 부진,2018년 실적 우상향 전망 유효, 현대차-구원투수(신차) 등판이 필요한 실적,매출액 24조원(전년 대비 증감율-0.2%), 영업이익 7,752억원(전년 대비 증감율-24.1%), OPM 3.2%,국내, 미국 동반 부진이 초래한 역대 최저수준의 차량사업부 수익성, 현대차-아픈마무리,4분기 영업이익 0.78조원(-24.1%)으로 컨센서스(1.12조원) 하회,1회성 이슈가 다수 발생, 18년도 1분기 정상화 예상, Hyundai Motor-A disappointing end to the year,4분기 영업이익 0.78조원(-24.1%)으로 컨센서스(1.12조원) 하회,1회성 이슈가 다수 발생, 18년도 1분기 정상화 예상, 현대차-2018년도 어려운 환경(요약),주가 박스권 상향을 위한 필요조건,4분기 Review ? 실적 부진 지속, 현대차-문제는 세단,17년도 4분기 , Shock,세단 판매 부진 부담 지속,신차 경쟁력 회복 18년도 하반기 확인 가능, 현대차-우려의 해소와 선순환 전환까지 시간이 필요,17년도 4분기 Review ? 환율과 고정비 부담, 그리고 각종 비용반영,우려의 해소와 선순환 전환까지 시간이 필요, Hyundai Motor-년도년도 1분기 4분기 review: weak, as expected,년도년도 1분기 4분기 영업이익 7,750억원으로 시장기대치를 크게 하회,2018년 글로벌 판매 480만대 전망, 낮아진 기대감은 기회 요인, 현대차-년도년도 1분기 4분기 Review: 예상되었던 실적 부진,년도년도 1분기 4분기 영업이익 7,750억원으로 시장기대치를 크게 하회,2018년 글로벌 판매 480만대 전망, 낮아진 기대감은 기회 요인, 현대차-그래도 나아질 미래, 4분기 실적은 당사 추정치와 시장 컨센서스를 하회하며 부진, 현대차-4분기 기대치 크게 하회, 올해도 수익성 악화 국면 지속,4분기 실적 리뷰 : 고정비 부담이 예상 보다 컸다,2018년 1분기 전망 : 개선되지만 역성장 지속, HMC-Business environment to remain unfavorable in 2018,주가 박스권 상향을 위한 필요조건,4분기 Review ? 실적 부진 지속, 현대차-년도년도 1분기 4분기 Review : Level Down,년도년도 1분기 4분기 영업이익, 당사추정치 26.8% 하회,자동차부문, 영업이익률 0.4% 기록, 현대차-예상보다 더 큰 Earnings Shock,17년도 4분기 Review ? 예상보다 더 큰 Earnings Shock</t>
+    <t>4Q 실적 저조 예상, 환율부담 가중,4분기 실적은 기존 추정치와 시장 컨센서스를 하회할 것으로 예상,미국시장 부진을 타개할 방법은 SUV 중심의 신차투입</t>
+  </si>
+  <si>
+    <t>Hyundai Motor-Earnings growth to be modest in 2018,17년도 4분기 영업이익 9,586억원으로 크게 부진할 것으로 추정,기대에는 못 미치지만 2018년 실적 우상향 전망 유효, 협력을 통한 기술개발 강화,현대차, 자율주행기술 개발을 위한 Aurora Project 발표,자율주행을 양분한 Intel Mobileye 연맹 및 NVIDIA 연맹과도 제휴, Future Mobility 전략 및 이익 개선 방향성의 구체화,CES 기간 중 발표된 6가지 Future Mobility 전략:자동차 업체를 넘어 ICT 업체로 진화 포부,18년 지배주주 순이익 +38% 전년 대비 증감율, 지난 5년 간 이어졌던 이익 축소 방향성 해제될 전망, 또 한번의 실망감과 점진적 우상향,17년도 4분기 영업이익 9,586억원으로 크게 부진할 것으로 추정,기대에는 못 미치지만 2018년 실적 우상향 전망 유효</t>
+  </si>
+  <si>
+    <t>년도년도 1분기 4분기 Preview: 길어진진,년도 분기 1Q18부터는 개선,년도년도 1분기 4분기 Preview: 영업이익 1.05조원 기록으로 시장 기대치 하회 예상,美시장 M/S 회복 가능성으로 하방 경직성 강화, 외부 협력을 통한 체질 개선,CES 2018 관전 포인트: 1) 오로라(자율주행), 2) AI 비서,CES 2018 관전 포인트: 3) 넥쏘(수소차)</t>
+  </si>
+  <si>
+    <t>부진한 현실에 안주할건가,전통적 산업 영역 내 안주,17년도 4분기 영업이익 1.03조원 전망</t>
+  </si>
+  <si>
+    <t>년도년도 1분기 4분기 실적 업데이트,년도년도 1분기 4분기 Review: 매출 기대치 1.6% 상회, 영업이익 기대치 33.2% 하회</t>
+  </si>
+  <si>
+    <t>Hyundai Motor-A disappointing end to the year,4분기 영업이익 0.78조원(-24.1%)으로 컨센서스(1.12조원) 하회,1회성 이슈가 다수 발생, 18년도 1분기 정상화 예상, 바닥의 깊이보다 방향성을 보자,Facts: 부진한 4분기 실적,Pros &amp; cons: 이익 감소에도 배당금액 유지, SUV 확대 본격화, Hyundai Motor-More emphasis on road to recovery,Facts: 부진한 4분기 실적,Pros &amp; cons: 이익 감소에도 배당금액 유지, SUV 확대 본격화, 예상보다 더 부진했지만 지난 실적,17년도 4분기 영업이익 7,752억원 기록(전년 대비 증감율 24.1% 감소)해 크게 부진,2018년 실적 우상향 전망 유효, Hyundai Motor-Weaker than feared, but the worst is over,17년도 4분기 영업이익 7,752억원 기록(전년 대비 증감율 24.1% 감소)해 크게 부진,2018년 실적 우상향 전망 유효, 구원투수(신차) 등판이 필요한 실적,매출액 24조원(전년 대비 증감율-0.2%), 영업이익 7,752억원(전년 대비 증감율-24.1%), OPM 3.2%,국내, 미국 동반 부진이 초래한 역대 최저수준의 차량사업부 수익성, 년도년도 1분기 4분기 Review: 실적은 쇼크였지만 긍정적인 부분을 찾는다면,년도년도 1분기 4분기 Review: 파업, 환율, 판매 비용 증가로 기대치를 큰 폭으로 하회,18년도 1분기 Preview: 파업 영향권이나 신차 효과 본격화 시기, 바닥의 깊이보다 방향성을 보자,Facts: 부진한 4분기 실적,Pros &amp; cons: 이익 감소에도 배당금액 유지, SUV 확대 본격화, Cycle의 전환점,실패한 13 년 Cycle 의 마무리 17년도 4분기 ,3 월, 기저효과와 함께할 새로운 신차 Cycle 의 본격적인 시작, 2018년도 어려운 환경,주가 박스권 상향을 위한 필요조건,4분기 Review ? 실적 부진 지속, Hyundai Motor-More emphasis on road to recovery,Facts: 부진한 4분기 실적,Pros &amp; cons: 이익 감소에도 배당금액 유지, SUV 확대 본격화, 예상보다 더 부진했지만 지난 실적,17년도 4분기 영업이익 7,752억원 기록(전년 대비 증감율 24.1% 감소)해 크게 부진,2018년 실적 우상향 전망 유효, Hyundai Motor-Weaker than feared, but the worst is over,17년도 4분기 영업이익 7,752억원 기록(전년 대비 증감율 24.1% 감소)해 크게 부진,2018년 실적 우상향 전망 유효, 구원투수(신차) 등판이 필요한 실적,매출액 24조원(전년 대비 증감율-0.2%), 영업이익 7,752억원(전년 대비 증감율-24.1%), OPM 3.2%,국내, 미국 동반 부진이 초래한 역대 최저수준의 차량사업부 수익성, 아픈마무리,4분기 영업이익 0.78조원(-24.1%)으로 컨센서스(1.12조원) 하회,1회성 이슈가 다수 발생, 18년도 1분기 정상화 예상, Hyundai Motor-A disappointing end to the year,4분기 영업이익 0.78조원(-24.1%)으로 컨센서스(1.12조원) 하회,1회성 이슈가 다수 발생, 18년도 1분기 정상화 예상, 2018년도 어려운 환경(요약),주가 박스권 상향을 위한 필요조건,4분기 Review ? 실적 부진 지속, 문제는 세단,17년도 4분기 , Shock,세단 판매 부진 부담 지속,신차 경쟁력 회복 18년도 하반기 확인 가능, 우려의 해소와 선순환 전환까지 시간이 필요,17년도 4분기 Review ? 환율과 고정비 부담, 그리고 각종 비용반영,우려의 해소와 선순환 전환까지 시간이 필요, Hyundai Motor-년도년도 1분기 4분기 review: weak, as expected,년도년도 1분기 4분기 영업이익 7,750억원으로 시장기대치를 크게 하회,2018년 글로벌 판매 480만대 전망, 낮아진 기대감은 기회 요인, 년도년도 1분기 4분기 Review: 예상되었던 실적 부진,년도년도 1분기 4분기 영업이익 7,750억원으로 시장기대치를 크게 하회,2018년 글로벌 판매 480만대 전망, 낮아진 기대감은 기회 요인, 그래도 나아질 미래, 4분기 실적은 당사 추정치와 시장 컨센서스를 하회하며 부진, 4분기 기대치 크게 하회, 올해도 수익성 악화 국면 지속,4분기 실적 리뷰 : 고정비 부담이 예상 보다 컸다,2018년 1분기 전망 : 개선되지만 역성장 지속, HMC-Business environment to remain unfavorable in 2018,주가 박스권 상향을 위한 필요조건,4분기 Review ? 실적 부진 지속, 년도년도 1분기 4분기 Review : Level Down,년도년도 1분기 4분기 영업이익, 당사추정치 26.8% 하회,자동차부문, 영업이익률 0.4% 기록, 예상보다 더 큰 Earnings Shock,17년도 4분기 Review ? 예상보다 더 큰 Earnings Shock</t>
   </si>
   <si>
     <t>Hyundai Motor-4Q results weak-lower 2018 expectations,17년도 4분기 영업이익, 당사추정치 26.8% 하회,자동차부문, 영업이익률 0.4% 기록</t>
   </si>
   <si>
-    <t>현대차-중국을 살릴 수 있다면야,중국, 가격인하를 통한 턴어라운드,신형 SUV과 신형 엔진이 온다</t>
-  </si>
-  <si>
-    <t>Hyundai Motor-NDR takeaways-Striving for change,신차 출시,중국시장 실적회복, 18년도 2분기 이후 전망, 현대차-NDR key takeaways: 방향 전환,신차 출시,중국시장 실적회복, 18년도 2분기 이후 전망</t>
-  </si>
-  <si>
-    <t>현대차-신차 효과와 엔화 강세로 박스권 탈출,현대차에게 가장 중요한 신차는 싼타페,힘을 받고 있는 엔화 강세론</t>
-  </si>
-  <si>
-    <t>현대차-현대차 년도년도 1분기 4분기 실적 리뷰,년도년도 1분기 4분기 Review: 영업이익률 3.2% 기록,실적발표 컨퍼런스 콜의 주요 내용: SUV 투입 확대</t>
-  </si>
-  <si>
-    <t>현대차-수소차 'NEXO' 출시와 그 시사점,보조금 규모를 무색하게 만든 733대의 수소차 'NEXO'의 사전계약,태동하고 있는 전세계 수소차 시장, 현대차 입지 강화</t>
-  </si>
-  <si>
-    <t>현대차-수소차 돌풍으로 존재감 부각,2세대 수소차 ‘NEXO’ 출시로 미래사업 방향성 수면위로 부각,현대차가 수소차에 베팅하는 이유</t>
-  </si>
-  <si>
-    <t>현대차-1Q 부진. 하지만, 중국 3월, 미국 6월부터 개선,다수의 주가 모멘텀 발생 중,18년도 1분기 Preview: 영업이익률 4.2% 전망</t>
-  </si>
-  <si>
-    <t>현대차-1분기, 가장 힘든 터널의 끝,18년도 1분기 Preview - 손익에서 큰 기대는 어려운 분기, 현대차-18년도 1분기 Preview, 원화 강세와 판매 감소로 부진한 실적 전망,신차 효과 vs. 원화 강세,단기 보수적인 대응을 추천</t>
-  </si>
-  <si>
-    <t>현대차-2분기에나 이익 감소 폭 축소 기대,18년도 1분기 실적 전망: 기존 예상치 하회,2분기 들어서야 감익 폭 줄어 들 듯, 현대차-18년도 1분기 Preview-신차와 기저효과는 다음 분기부터,1 분기 실적 매출액 22.2 조원, 영업이익 9,235 억원, 당기순이익 9,385 억원 전망, 현대차-끝이 보이는 긴 부진의 터널,18년도 1분기 매출 23,018십억원(전년 대비 증감율-1.5%), 영업이익 944십억원(전년 대비 증감율-24.6%, OPM 4 1%) 전망,18년도 하반기 부터 BIG2(중국, 미국) 동반 회복세 기대</t>
-  </si>
-  <si>
-    <t>현대차-판매 방향성 전환 시작,판매개선을 위한 Cycle 전환기 시작, 18년 EPS +26% 전년 대비 증감율 전망,지배구조 개편 과정에서 주주 친화적 배당정책 제시 가능성 증가</t>
-  </si>
-  <si>
-    <t>현대차-북미 회복이 관건,18년도 1분기 영업이익 8,958억원 (-28.4%전년 대비 증감율) 시장기대치 하회 전망,싼타페 신차의 북미 시장 성공이 절실, 현대차-우선주, 고 배당과 Capital Gain매력을 겸비,엘리엇 등 행동주의 펀드, 적극적인 의사표명,현대차그룹, 예상되는 주주 환원 정책들</t>
-  </si>
-  <si>
-    <t>현대차-주주환원정책 확대 기대 (요약),영업실적 회복은 점진적으로 진행될 전망,1분기 Preview: 원화강세, 글로벌 재고조정 여파로 부진, 현대차-주주환원정책 확대 기대,영업실적 회복은 점진적으로 진행될 전망,1분기 Preview: 원화강세, 글로벌 재고조정 여파로 부진, HMC-Shareholder return policy to grow friendlier,영업실적 회복은 점진적으로 진행될 전망,1분기 Preview: 원화강세, 글로벌 재고조정 여파로 부진, Hyundai Motor-Preferred shares attractive,엘리엇 등 행동주의 펀드, 적극적인 의사표명,현대차그룹, 예상되는 주주 환원 정책들, 현대차-경쟁력 시험 무대,내년까지 본질적인 판매 경쟁력이 판가름 날 중요한 시점,연간 영업이익 4.48조원(-2% 전년 대비 증감율) 전망</t>
-  </si>
-  <si>
-    <t>'현대차 3인방'은 강세… 글로비스는 하락, 현대차 지배구조 개편 헛짚은 엘리엇… 무리한 요구로 발목잡기 나서, 현대차 “엘리엇 요구 현실성 없어… 원안대로 간다”, 엘리엇, 현대차·모비스 합병 요구 ‘의도’는 보유 주가 띄우기?, 코스피 코스닥 동반하락, 반도체 수요 약화 불안감에 발목 잡혀, 현대차 정몽구-정의선, 더 이상 '애국심마케팅' 안 통한다, 현대차-18년도 1분기 Preview - 부진한 실적에도 주가 방향은 긍정적,환율 변동과 판매 부진에 따른 영업이익 감소 예상,현지화 모델 중심의 중국 판매 회복, 부진한 미국 판매, 마케팅 비용 증가 감안해야, `엘리엇` 와중에…외인 勢결집 돕는 정부, 엘리엇 "현대 가속화에 대한 제안"vs재계 "주가 띄우기", 행동 돌입한 엘리엇…다시 시험대 오른 국민연금</t>
+    <t>중국을 살릴 수 있다면야,중국, 가격인하를 통한 턴어라운드,신형 SUV과 신형 엔진이 온다</t>
+  </si>
+  <si>
+    <t>Hyundai Motor-NDR takeaways-Striving for change,신차 출시,중국시장 실적회복, 18년도 2분기 이후 전망, NDR key takeaways: 방향 전환,신차 출시,중국시장 실적회복, 18년도 2분기 이후 전망</t>
+  </si>
+  <si>
+    <t>신차 효과와 엔화 강세로 박스권 탈출,현대차에게 가장 중요한 신차는 싼타페,힘을 받고 있는 엔화 강세론</t>
+  </si>
+  <si>
+    <t>현대차 년도년도 1분기 4분기 실적 리뷰,년도년도 1분기 4분기 Review: 영업이익률 3.2% 기록,실적발표 컨퍼런스 콜의 주요 내용: SUV 투입 확대</t>
+  </si>
+  <si>
+    <t>수소차 'NEXO' 출시와 그 시사점,보조금 규모를 무색하게 만든 733대의 수소차 'NEXO'의 사전계약,태동하고 있는 전세계 수소차 시장, 현대차 입지 강화</t>
+  </si>
+  <si>
+    <t>수소차 돌풍으로 존재감 부각,2세대 수소차 ‘NEXO’ 출시로 미래사업 방향성 수면위로 부각,현대차가 수소차에 베팅하는 이유</t>
+  </si>
+  <si>
+    <t>1Q 부진. 하지만, 중국 3월, 미국 6월부터 개선,다수의 주가 모멘텀 발생 중,18년도 1분기 Preview: 영업이익률 4.2% 전망</t>
+  </si>
+  <si>
+    <t>1분기, 가장 힘든 터널의 끝,18년도 1분기 Preview - 손익에서 큰 기대는 어려운 분기, 18년도 1분기 Preview, 원화 강세와 판매 감소로 부진한 실적 전망,신차 효과 vs. 원화 강세,단기 보수적인 대응을 추천</t>
+  </si>
+  <si>
+    <t>2분기에나 이익 감소 폭 축소 기대,18년도 1분기 실적 전망: 기존 예상치 하회,2분기 들어서야 감익 폭 줄어 들 듯, 18년도 1분기 Preview-신차와 기저효과는 다음 분기부터,1 분기 실적 매출액 22.2 조원, 영업이익 9,235 억원, 당기순이익 9,385 억원 전망, 끝이 보이는 긴 부진의 터널,18년도 1분기 매출 23,018십억원(전년 대비 증감율-1.5%), 영업이익 944십억원(전년 대비 증감율-24.6%, OPM 4 1%) 전망,18년도 하반기 부터 BIG2(중국, 미국) 동반 회복세 기대</t>
+  </si>
+  <si>
+    <t>판매 방향성 전환 시작,판매개선을 위한 Cycle 전환기 시작, 18년 EPS +26% 전년 대비 증감율 전망,지배구조 개편 과정에서 주주 친화적 배당정책 제시 가능성 증가</t>
+  </si>
+  <si>
+    <t>북미 회복이 관건,18년도 1분기 영업이익 8,958억원 (-28.4%전년 대비 증감율) 시장기대치 하회 전망,싼타페 신차의 북미 시장 성공이 절실, 우선주, 고 배당과 Capital Gain매력을 겸비,엘리엇 등 행동주의 펀드, 적극적인 의사표명,현대차그룹, 예상되는 주주 환원 정책들</t>
+  </si>
+  <si>
+    <t>주주환원정책 확대 기대 (요약),영업실적 회복은 점진적으로 진행될 전망,1분기 Preview: 원화강세, 글로벌 재고조정 여파로 부진, 주주환원정책 확대 기대,영업실적 회복은 점진적으로 진행될 전망,1분기 Preview: 원화강세, 글로벌 재고조정 여파로 부진, HMC-Shareholder return policy to grow friendlier,영업실적 회복은 점진적으로 진행될 전망,1분기 Preview: 원화강세, 글로벌 재고조정 여파로 부진, Hyundai Motor-Preferred shares attractive,엘리엇 등 행동주의 펀드, 적극적인 의사표명,현대차그룹, 예상되는 주주 환원 정책들, 경쟁력 시험 무대,내년까지 본질적인 판매 경쟁력이 판가름 날 중요한 시점,연간 영업이익 4.48조원(-2% 전년 대비 증감율) 전망</t>
+  </si>
+  <si>
+    <t>'현대차 3인방'은 강세… 글로비스는 하락, 현대차 지배구조 개편 헛짚은 엘리엇… 무리한 요구로 발목잡기 나서, 현대차 “엘리엇 요구 현실성 없어… 원안대로 간다”, 엘리엇, 현대차·모비스 합병 요구 ‘의도’는 보유 주가 띄우기?, 코스피 코스닥 동반하락, 반도체 수요 약화 불안감에 발목 잡혀, 현대차 정몽구-정의선, 더 이상 '애국심마케팅' 안 통한다, 18년도 1분기 Preview - 부진한 실적에도 주가 방향은 긍정적,환율 변동과 판매 부진에 따른 영업이익 감소 예상,현지화 모델 중심의 중국 판매 회복, 부진한 미국 판매, 마케팅 비용 증가 감안해야, `엘리엇` 와중에…외인 勢결집 돕는 정부, 엘리엇 "현대 가속화에 대한 제안"vs재계 "주가 띄우기", 행동 돌입한 엘리엇…다시 시험대 오른 국민연금</t>
   </si>
   <si>
     <t>현대車까지 ‘탐욕 엘리엇’ 먹잇감, 경영권보호法 시급하다, 한국기업 노리는 해외 투기자본… 주가 흔든뒤 이익만 챙겨 ‘먹튀’, "배당 2배로 늘려라" 주주 공략..1% 지분 지렛대로 제몫 늘리기 시도, 잔꾀 밝은 엘리엇, 주가 부양 위한 엘리엇의 흔들기…현대차, 남은 과제는?, 외신도 "엘리엇 현대차 공세 현실성 없다", 엘리엇매니지먼트 제안 뒤 현대차 주식 살까 현대모비스 주식 살까, 본색 드러낸 엘리엇, 현대차그룹 "주주 설득 이어갈 듯", 코스피 코스닥 동반하락, 미국 국채금리 상승에 외국인 매도세 강해, 한국 증시 덮친 '美 국채금리 쇼크'… 외국인, 4년10개월 만에 최대 순매도, 지분 미미하지만…엘리엇 입김에 출렁이는 그룹株</t>
   </si>
   <si>
-    <t>현대차-년도년도 1분기 1분기 Review: 실적쇼크와 쓸쓸한 빈손,년도년도 1분기 1분기 실적은 G2시장 판매둔화, 인센티브 증가, 원화강세로 컨센서스를 큰 폭 하회,영업이익 개선은 미국시장 싼타페 출시가 예정된 년도년도 1분기 3분기 예상, '법보다 빡빡하네' 금융 통합감독에 미래·삼성 '속앓이', 김상조 “엘리엇, 현대차 지주사요구는 법 위반”, 집중투표하면 현대차·삼성전자, 외국인에 넘어간다</t>
-  </si>
-  <si>
-    <t>현대차-1Q 부진. 2Q도 부정적. 하지만, 판매개선과 주주환원 기대,낮은 기저와 신차투입으로 판매회복 시작,18년도 1분기 Review: 영업이익률 3.0% 기록, 현대차-1분기, 가동률 저하가 만든 또 한 번의 어닝쇼크,18년도 1분기 Review-가동률 하락, 큰 폭의 어닝쇼크,18년도 2분기 Preview-2분기도 회복이 어렵다, 현대차-주식소각 발표로 목표주가 상향,기다리던 소식,자기주식 소각 발표, 현대차-1분기 부진, 2분기부터 지배순이익 개선 기대,18년 1분기 실적은 크게 부진,18년 2분기부터 지배순이익 개선 전망, 현대차-약해지는 증익 기대감,18년도 1분기 영업이익 6,813억원(전년 대비 증감율 -45.5%, OPM 3.0%)으로 어닝쇼크 재현,순이익 역시 7,316억원(전년 대비 증감율 -48.0%)을 기록하며 시장 기대치 하회, 현대차-년도년도 1분기 1분기 Review: 한번 더 쉬어가실적년도 는분기 ,년도년도 1분기 1분기 Review: 영업이익 6,813억원 기록, 시장 기대치 하회,년도년도 1분기 1분기 의 부진요인, 년도년도 1분기 2분기 에는 개선요인으로 작용할 것, 증시 전문가들 “현대차 1분기 실적 부진했지만 중장기 반등 가능성”, 현대차-기대보다 부진한 실적,1분기 영업이익 0.68조원(-45.5%)으로 시장 기대치(0.97조원) 크게 하회,2분기 개선 요인: 글로벌 싼타페 출시, 중국 개선 본격화, 현대차 자사주 1조 규모 소각 결정, “주주가치 높이기 계속”, 현대차, 14년만에 자사주 소각…854만주·1조원 규모(종합2보), 현대차-낮아진 기초 체력,18년도 1분기 , Shock,실적 부진 원인: 1) 원화 강세, 2) 파업, 3) 미주 도매 판매 부진, 4) 미국 공장 가동률 하락, 현대차 854만주 자사주 소각…"주주가치 제고 노력", 현대차-년도년도 1분기 1분기 Review-기대에 못 미친 실적과 주주환원정책,년도년도 1분기 1분기 잠정 영업이익 6,813억원(-45.5% 전년 대비 증감율) - 시장 컨센서스 하회,영업이익 부진의 원인은 인센티브 강화, 환율 상승 등으로 추정, Hyundai Motor-1Q operating profit falls well short of forecasts,18년도 1분기 실적은 G2시장 판매둔화, 인센티브 증가, 원화강세로 컨센서스를 큰 폭 하회,영업이익 개선은 미국시장 싼타페 출시가 예정된 18년도 3분기 예상, 현대차-물량과 가격 동반 하락이 초래한 실적,매출액 22,437십억원(전년 대비 증감율-4.0%), 영업이익 681십억원(전년 대비 증감율-45.5%), OPM 3.0%,국내, 미국 동반 부진이 초래한 차량사업부 부진 지속, Hyundai Motor-18년도 1분기 review: time to revisit Hyundai Motor,1Q 18 실적 시장기대치를 크게 하회: 환율·리콜 증가·타부문 부진 3중고,원화강세 등 경영환경 악화에도 실적개선은 18년도 2분기 부터 가능, 현대차-18년도 1분기 Review: 현대차를 보아야할 때,1Q 18 실적 시장기대치를 크게 하회: 환율·리콜 증가·타부문 부진 3중고,원화강세 등 경영환경 악화에도 실적개선은 18년도 2분기 부터 가능, 현대차-기대치 크게 하회, 2분기 기저 효과 반감,1분기 실적 리뷰: 미국 부진이 예상보다 커,2018년 2분기 전망: 기대했던 강력한 기저 효과 반감, 현대차-2019년으로 가는 징검다리,상반기까지는 의미있는 실적 모멘텀 회복 어려울 전망,1분기 Review-실적 감소추세 지속, 현대차-뒤가 아닌 앞을 보자,18년도 1분기 실적, 모델 노후화 및 신차 투입 전 가동률 하락으로 부진,18년도 2분기 신차효과 및 기저효과에 근거한 양적 질적 판매개선 반영 시작, 현대차-년도년도 1분기 1분기 Review:1분기 실적 기대치 대폭 하회,년도년도 1분기 1분기 Review:1분기 실적 기대치 대폭 하회,년도년도 1분기 2분기 Review: 점진적 회복 국면에 돌입, 하지만 외부 변수가 많아, 현대차, 1조 규모 자사주 소각… 엘리엇 제안 영향(?), 현대차-체력이 약해지면 감기도 병이 된다,1분기 실적은 파업과 환율로 부진,국내 이익 기여도 상승과 가동률 하락으로 파업과 환율에 취약해진 기초체력, Hyundai Motor-Earnings worse than expected,1분기 영업이익 0.68조원(-45.5%)으로 시장 기대치(0.97조원) 크게 하회,2분기 개선 요인: 글로벌 싼타페 출시, 중국 개선 본격화, 현대차, 14년만 자사주 소각 결정…엘리엇 압박 있었나?, 현대차, 자사주 소각 발표에 반등…현대모비스 2%↑, 현대차, 9600억 규모 자사주 소각··· “주주가치 제고 일환”(종합), 현대차 자사주 854만주 소각, “다각적인 주주환원 확대 방안 마련과 적정 주가 평가를 위한 노력을 이어갈 것”, 현대차-년도년도 1분기 1분기 Review - 기대와 실현 사이의 시차,년도년도 1분기 1분기 Review - 하향된 시장기대치를 하회,기대와 실현 사이의 시차, 우려의 해소와 선순환 전환까지 시간이 필요, 현대차, 주주가치 제고 노력… 854만주 자사주 소각, 현대차, 주주가치 제고 위해 854만주 자사주 소각, 현대차 자사주 854만주 소각 “주주가치 제고 노력 일환”, 시장심리 톱5, 삼성전자·SK하이닉스·현대모비스·기아차·두산인프라코어, 현대차, 14년만에 자사주 소각.."주주가치 제고"(종합), 현대차, 14년 만에 자사주 소각..."854만주·9600억 규모", 현대차 “주주가치 제고” 자사주 854만주 소각, 현대차, 자사주 854만주 소각…“주주가치 제고 위해 결정”, 현대차, 854만주(1조원 규모) 자사주 소각…“주주가치 제고 노력 일환”, 노무라 "현대자동차 앞날은 밝아보인다", 현대차, 1조 규모 자사주 소각…주주가치 제고 확대, 현대차 1분기 영업이익 반토막…원화강세·G2 판매부진 영향, 현대차, 주주가치 제고 위해 854만주 자사주 소각, 현대차, 주가부양 나서…주식총수 3% 자사주 소각, 현대차 14년만에 자사주 854만주 소각..9600억 규모, 현대차, 9천600억원 자사주 소각…14년래 처음(상보), 현대차, 자사주 854만주, 1조원 규모 소각, 현대차 854만주 자사주 소각···주주가치 제고 일환, 현대차, 주주가치 제고 위해 자사주 854만주 소각, 현대차, 9600억 규모 자사주 854만주 소각 추진… 주주가치 제고 차원, 현대차, 14년 만에 자사주 소각…854만 주·1조 원 규모, 현대차 "285만주 매입 등 자사주 854만주 소각" (상보), 현대차, 14년 만에 자사주 소각…"주주가치 제고", 현대차, 1조 규모 자사주 소각 "주주가치 제고", 현대차, 14년 만에 자사주 소각…854만 주·1조 원 규모, 현대차, 14년 만에 자사주 854만주 소각…“엘리엇 영향? 주주가치 제고?”, 현대차, 9600억원 규모 자사주 소각…"주주가치 제고 일환", 현대차, 자사주 1조 규모 소각…'14년 만', 현대차, 자사주 소각에 반등…현대모비스 1%↑, 현대차, 자사주 854만주 이익소각…“주주가치 제고”, 현대차 14년만에 자사주 소각…“주주가치 제고 일환”, 현대차, 14년만에 자사주 소각…854만주·1조원 규모(종합), 현대차 자사주 854만주 소각…1조 규모, 현대차 "엘리엇과 무관" 자사주 소각시점 기존 보유 7월 27일 예정, 현대차, 14년 만에 자사주 '854만주' 소각…"주주가치 제고", 현대차 14년만에 자사주 854만주 소각… 1조원 규모, 현대차, 1조 규모 자사주 소각…14년만에 결정 이유는?, 현대차, 14년만에 자사주 소각…854만주·1조원 규모, 현대차, 정의선 승계 앞두고 자사주 소각 발표...'자의반, 타의반'?, 854만주 자사주 소각, 영업이익 반토막 난 현대차, 향후 주가 신차에 달렸다, 현대차, 자사주 854만 주 소각 처리…총 발행주식의 3% 수준, 현대차 자사주 소각, 엘리엇 의식했나, 현대차 "1兆 자사주 소각해 주주가치 제고", 현대차, 엘리엇 공세 정면돌파…14년만에 자사주 1조 소각, 현대차 자사주 소각 결정에 강세…증권사 목표주가 '상향', 현대차 1조 규모 자사주 소각, AG시스템 “한 눈에 보는 경제”, 현대차, 14년 만에 자사주 소각…“주주가치 제고”, 현대차 854만주 자사주 소각 "주주가치 제고 노력 일환", 현대차, 1조원 자사주 소각…“전부터 검토, 엘리엣 무관”, 현대차, 14년만에 자사주 소각, 현대차, 14년만에 자사주 854만주 소각, 현대차, 자사주 854만주 소각… 주주가치 제고, 현대차, 1조원 규모 자사주 소각.."주주가치 제고 목적", 현대차, 자사주 854만주 소각…주주가치 제고, 현대차, 자사주 854만 주 소각 결정…총 발행주식의 3% 수준, 현대차 "자사주 소각, 엘리엇 요구와 무관", 현대차 자사주 845만주 소각…주주가치 높인다, 현대차, 14년 만에 1兆 자사주 소각 추진…“주주가치 제고 노력 일환”, 현대차 854만주 자사주 소각 "주주가치 제고", 현대차 14년 만에 자사주 854만주 소각… "주주가치 제고 위해", 현대차 노조 "자사주 소각은 경영잘못 객관적으로 입증한 것", 현대차 자사주 854만주 소각, 엘리엇과 무관 "적정 주가 평가 위해 노력"</t>
+    <t>년도년도 1분기 1분기 Review: 실적쇼크와 쓸쓸한 빈손,년도년도 1분기 1분기 실적은 G2시장 판매둔화, 인센티브 증가, 원화강세로 컨센서스를 큰 폭 하회,영업이익 개선은 미국시장 싼타페 출시가 예정된 년도년도 1분기 3분기 예상, '법보다 빡빡하네' 금융 통합감독에 미래·삼성 '속앓이', 김상조 “엘리엇, 현대차 지주사요구는 법 위반”, 집중투표하면 현대차·삼성전자, 외국인에 넘어간다</t>
+  </si>
+  <si>
+    <t>1Q 부진. 2Q도 부정적. 하지만, 판매개선과 주주환원 기대,낮은 기저와 신차투입으로 판매회복 시작,18년도 1분기 Review: 영업이익률 3.0% 기록, 1분기, 가동률 저하가 만든 또 한 번의 어닝쇼크,18년도 1분기 Review-가동률 하락, 큰 폭의 어닝쇼크,18년도 2분기 Preview-2분기도 회복이 어렵다, 주식소각 발표로 목표주가 상향,기다리던 소식,자기주식 소각 발표, 1분기 부진, 2분기부터 지배순이익 개선 기대,18년 1분기 실적은 크게 부진,18년 2분기부터 지배순이익 개선 전망, 약해지는 증익 기대감,18년도 1분기 영업이익 6,813억원(전년 대비 증감율 -45.5%, OPM 3.0%)으로 어닝쇼크 재현,순이익 역시 7,316억원(전년 대비 증감율 -48.0%)을 기록하며 시장 기대치 하회, 년도년도 1분기 1분기 Review: 한번 더 쉬어가실적년도 는분기 ,년도년도 1분기 1분기 Review: 영업이익 6,813억원 기록, 시장 기대치 하회,년도년도 1분기 1분기 의 부진요인, 년도년도 1분기 2분기 에는 개선요인으로 작용할 것, 증시 전문가들 “현대차 1분기 실적 부진했지만 중장기 반등 가능성”, 기대보다 부진한 실적,1분기 영업이익 0.68조원(-45.5%)으로 시장 기대치(0.97조원) 크게 하회,2분기 개선 요인: 글로벌 싼타페 출시, 중국 개선 본격화, 현대차 자사주 1조 규모 소각 결정, “주주가치 높이기 계속”, 현대차, 14년만에 자사주 소각…854만주·1조원 규모(종합2보), 낮아진 기초 체력,18년도 1분기 , Shock,실적 부진 원인: 1) 원화 강세, 2) 파업, 3) 미주 도매 판매 부진, 4) 미국 공장 가동률 하락, 현대차 854만주 자사주 소각…"주주가치 제고 노력", 년도년도 1분기 1분기 Review-기대에 못 미친 실적과 주주환원정책,년도년도 1분기 1분기 잠정 영업이익 6,813억원(-45.5% 전년 대비 증감율) - 시장 컨센서스 하회,영업이익 부진의 원인은 인센티브 강화, 환율 상승 등으로 추정, Hyundai Motor-1Q operating profit falls well short of forecasts,18년도 1분기 실적은 G2시장 판매둔화, 인센티브 증가, 원화강세로 컨센서스를 큰 폭 하회,영업이익 개선은 미국시장 싼타페 출시가 예정된 18년도 3분기 예상, 물량과 가격 동반 하락이 초래한 실적,매출액 22,437십억원(전년 대비 증감율-4.0%), 영업이익 681십억원(전년 대비 증감율-45.5%), OPM 3.0%,국내, 미국 동반 부진이 초래한 차량사업부 부진 지속, Hyundai Motor-18년도 1분기 review: time to revisit Hyundai Motor,1Q 18 실적 시장기대치를 크게 하회: 환율·리콜 증가·타부문 부진 3중고,원화강세 등 경영환경 악화에도 실적개선은 18년도 2분기 부터 가능, 18년도 1분기 Review: 현대차를 보아야할 때,1Q 18 실적 시장기대치를 크게 하회: 환율·리콜 증가·타부문 부진 3중고,원화강세 등 경영환경 악화에도 실적개선은 18년도 2분기 부터 가능, 기대치 크게 하회, 2분기 기저 효과 반감,1분기 실적 리뷰: 미국 부진이 예상보다 커,2018년 2분기 전망: 기대했던 강력한 기저 효과 반감, 2019년으로 가는 징검다리,상반기까지는 의미있는 실적 모멘텀 회복 어려울 전망,1분기 Review-실적 감소추세 지속, 뒤가 아닌 앞을 보자,18년도 1분기 실적, 모델 노후화 및 신차 투입 전 가동률 하락으로 부진,18년도 2분기 신차효과 및 기저효과에 근거한 양적 질적 판매개선 반영 시작, 년도년도 1분기 1분기 Review:1분기 실적 기대치 대폭 하회,년도년도 1분기 1분기 Review:1분기 실적 기대치 대폭 하회,년도년도 1분기 2분기 Review: 점진적 회복 국면에 돌입, 하지만 외부 변수가 많아, 현대차, 1조 규모 자사주 소각… 엘리엇 제안 영향(?), 체력이 약해지면 감기도 병이 된다,1분기 실적은 파업과 환율로 부진,국내 이익 기여도 상승과 가동률 하락으로 파업과 환율에 취약해진 기초체력, Hyundai Motor-Earnings worse than expected,1분기 영업이익 0.68조원(-45.5%)으로 시장 기대치(0.97조원) 크게 하회,2분기 개선 요인: 글로벌 싼타페 출시, 중국 개선 본격화, 현대차, 14년만 자사주 소각 결정…엘리엇 압박 있었나?, 현대차, 자사주 소각 발표에 반등…현대모비스 2%↑, 현대차, 9600억 규모 자사주 소각··· “주주가치 제고 일환”(종합), 현대차 자사주 854만주 소각, “다각적인 주주환원 확대 방안 마련과 적정 주가 평가를 위한 노력을 이어갈 것”, 년도년도 1분기 1분기 Review - 기대와 실현 사이의 시차,년도년도 1분기 1분기 Review - 하향된 시장기대치를 하회,기대와 실현 사이의 시차, 우려의 해소와 선순환 전환까지 시간이 필요, 현대차, 주주가치 제고 노력… 854만주 자사주 소각, 현대차, 주주가치 제고 위해 854만주 자사주 소각, 현대차 자사주 854만주 소각 “주주가치 제고 노력 일환”, 시장심리 톱5, 삼성전자·SK하이닉스·현대모비스·기아차·두산인프라코어, 현대차, 14년만에 자사주 소각.."주주가치 제고"(종합), 현대차, 14년 만에 자사주 소각..."854만주·9600억 규모", 현대차 “주주가치 제고” 자사주 854만주 소각, 현대차, 자사주 854만주 소각…“주주가치 제고 위해 결정”, 현대차, 854만주(1조원 규모) 자사주 소각…“주주가치 제고 노력 일환”, 노무라 "현대자동차 앞날은 밝아보인다", 현대차, 1조 규모 자사주 소각…주주가치 제고 확대, 현대차 1분기 영업이익 반토막…원화강세·G2 판매부진 영향, 현대차, 주주가치 제고 위해 854만주 자사주 소각, 현대차, 주가부양 나서…주식총수 3% 자사주 소각, 현대차 14년만에 자사주 854만주 소각..9600억 규모, 현대차, 9천600억원 자사주 소각…14년래 처음(상보), 현대차, 자사주 854만주, 1조원 규모 소각, 현대차 854만주 자사주 소각···주주가치 제고 일환, 현대차, 주주가치 제고 위해 자사주 854만주 소각, 현대차, 9600억 규모 자사주 854만주 소각 추진… 주주가치 제고 차원, 현대차, 14년 만에 자사주 소각…854만 주·1조 원 규모, 현대차 "285만주 매입 등 자사주 854만주 소각" (상보), 현대차, 14년 만에 자사주 소각…"주주가치 제고", 현대차, 1조 규모 자사주 소각 "주주가치 제고", 현대차, 14년 만에 자사주 소각…854만 주·1조 원 규모, 현대차, 14년 만에 자사주 854만주 소각…“엘리엇 영향? 주주가치 제고?”, 현대차, 9600억원 규모 자사주 소각…"주주가치 제고 일환", 현대차, 자사주 1조 규모 소각…'14년 만', 현대차, 자사주 소각에 반등…현대모비스 1%↑, 현대차, 자사주 854만주 이익소각…“주주가치 제고”, 현대차 14년만에 자사주 소각…“주주가치 제고 일환”, 현대차, 14년만에 자사주 소각…854만주·1조원 규모(종합), 현대차 자사주 854만주 소각…1조 규모, 현대차 "엘리엇과 무관" 자사주 소각시점 기존 보유 7월 27일 예정, 현대차, 14년 만에 자사주 '854만주' 소각…"주주가치 제고", 현대차 14년만에 자사주 854만주 소각… 1조원 규모, 현대차, 1조 규모 자사주 소각…14년만에 결정 이유는?, 현대차, 14년만에 자사주 소각…854만주·1조원 규모, 현대차, 정의선 승계 앞두고 자사주 소각 발표...'자의반, 타의반'?, 854만주 자사주 소각, 영업이익 반토막 난 현대차, 향후 주가 신차에 달렸다, 현대차, 자사주 854만 주 소각 처리…총 발행주식의 3% 수준, 현대차 자사주 소각, 엘리엇 의식했나, 현대차 "1兆 자사주 소각해 주주가치 제고", 현대차, 엘리엇 공세 정면돌파…14년만에 자사주 1조 소각, 현대차 자사주 소각 결정에 강세…증권사 목표주가 '상향', 현대차 1조 규모 자사주 소각, AG시스템 “한 눈에 보는 경제”, 현대차, 14년 만에 자사주 소각…“주주가치 제고”, 현대차 854만주 자사주 소각 "주주가치 제고 노력 일환", 현대차, 1조원 자사주 소각…“전부터 검토, 엘리엣 무관”, 현대차, 14년만에 자사주 소각, 현대차, 14년만에 자사주 854만주 소각, 현대차, 자사주 854만주 소각… 주주가치 제고, 현대차, 1조원 규모 자사주 소각.."주주가치 제고 목적", 현대차, 자사주 854만주 소각…주주가치 제고, 현대차, 자사주 854만 주 소각 결정…총 발행주식의 3% 수준, 현대차 "자사주 소각, 엘리엇 요구와 무관", 현대차 자사주 845만주 소각…주주가치 높인다, 현대차, 14년 만에 1兆 자사주 소각 추진…“주주가치 제고 노력 일환”, 현대차 854만주 자사주 소각 "주주가치 제고", 현대차 14년 만에 자사주 854만주 소각… "주주가치 제고 위해", 현대차 노조 "자사주 소각은 경영잘못 객관적으로 입증한 것", 현대차 자사주 854만주 소각, 엘리엇과 무관 "적정 주가 평가 위해 노력"</t>
   </si>
   <si>
     <t>현대모비스 가치평가 논란, 현대차, 주주가치제고 본격화에 증권사 목표주가도 ‘UP’, 엘리엇·어닝쇼크·자사주소각…현대차의 한주, 현대글로비스 “물류 넘어 미래차… 2025년 매출 40조”, 현대차 1조원 규모 자사주 소각</t>
@@ -4291,7 +4291,7 @@
     <t>쏟아지는 ‘주주친화 정책’…대형주 주가부양 박차, 현대차그룹, 중장기 전략ㆍ주주환원책 쏟아내는 이유는, 현대차그룹,친환경車 라인업 확대...질적성장 노린다, 자사주 소각 현대차, 배당성향 확대 기대감↑, 현대자동차, 1조원 규모 자사주 소각</t>
   </si>
   <si>
-    <t>'준비 안된 대박'은 '달콤한 독', 엘리엇의 몽니 "현대차 자사주소각 미흡", 현대차 vs 엘리엇, 본격 공방 개막… 1라운드는 현대차 판정승?, "현대차 자사주 소각 등 주주 환원정책으로 주가 오를 가능성", 현대차에게 엘리엇매니지먼트는 얼마나 위협적일까, 엘리엇 "현대차 자사주 소각 계획 고무적이나 기대에 못미쳐", 엘리엇 "현대차 '자사주 소각' 기대에 못미친다", 지배구조 개편, 엘리엇 개입, 자사주 매입...현대차그룹 주가 향방은?, 엘리엇 “현대차, ‘자사주 소각’ 만족스럽지 않다”, 현대차-끝이 보이는 긴 부진의 터널,18년도 1분기 매출액 22,437십억원(전년 대비 증감율-4.0%), 영업이익 681십억원(전년 대비 증감율-45.5%), OPM 3.0% 기록,18년도 하반기 부터 BIG2(중국, 미국) 동반 회복세 기대, 현대차-약 1 조원 규모 자기주식 소각,현대차 주식소각 결정,발행주식수 감소에 따른 EPS 3% 증가효과</t>
+    <t>'준비 안된 대박'은 '달콤한 독', 엘리엇의 몽니 "현대차 자사주소각 미흡", 현대차 vs 엘리엇, 본격 공방 개막… 1라운드는 현대차 판정승?, "현대차 자사주 소각 등 주주 환원정책으로 주가 오를 가능성", 현대차에게 엘리엇매니지먼트는 얼마나 위협적일까, 엘리엇 "현대차 자사주 소각 계획 고무적이나 기대에 못미쳐", 엘리엇 "현대차 '자사주 소각' 기대에 못미친다", 지배구조 개편, 엘리엇 개입, 자사주 매입...현대차그룹 주가 향방은?, 엘리엇 “현대차, ‘자사주 소각’ 만족스럽지 않다”, 끝이 보이는 긴 부진의 터널,18년도 1분기 매출액 22,437십억원(전년 대비 증감율-4.0%), 영업이익 681십억원(전년 대비 증감율-45.5%), OPM 3.0% 기록,18년도 하반기 부터 BIG2(중국, 미국) 동반 회복세 기대, 약 1 조원 규모 자기주식 소각,현대차 주식소각 결정,발행주식수 감소에 따른 EPS 3% 증가효과</t>
   </si>
   <si>
     <t>현대엔지니어링 SK건설, 지배구조 개편 압박에 상장으로 방향 정해, 현대글로비스 주가 하락세..지배구조개편에 '적신호', 남북경협·주주친화…정부-대기업, 증시살리기 '한방향' 주목</t>
@@ -4318,19 +4318,19 @@
     <t>②현대차그룹 - 지배구조 개편서 만난 엘리엇 암초, TheCapitalGroupCompanies,Inc. 외</t>
   </si>
   <si>
-    <t>현대차-18년도 1분기 NDR 후기: 바닥을 다진다,‘18년 2분기: 현재 모든 지표는 위를 가리키고 있다, 식인상어 엘리엇은 남을 배려하지 않는다, 차 부품사 '우수AMS', 에이알에스텍에 매각, 자신이 쓴 보고서가 '지배구조 정답'이라며 삼성 몰아친 김상조, 코스피 코스닥 동반상승, 북미 정상회담 기대 커져, 현대모비스 ‘현대차그룹 구글’로 바뀐다</t>
-  </si>
-  <si>
-    <t>엘리엇 "현대차 지배구조 개편안에 반대표 던질 것", 정의선 부회장 "현대차그룹 지배구조 개편 흔들리지 않을 것", 현대차그룹, '엘리엇 공세'에도 순환출자 고리 끊어야, 엘리엇, 현대자동차그룹 개편안에 반대투표 결정, 엘리엇 "현대차 개편 반대표" vs 정의선 "흔들리지 않는다", '행동' 나선 엘리엇...현대차그룹 지배구조 개편 훼방놓나, 엘리엇매니지먼트 “현대차그룹 지배구조 개편안에 반대표 던진다”, 모비스의 운명…`단기이익이냐, 미래가치냐` 국민연금 딜레마, 경협주 팔고 실적주 사들인 외국인…SK하이닉스·호텔신라 매수, 현대모비스 키우기 위한 정의선 부회장의 ‘글로벌스탠더드’ 행보, 엘리엇, 현대차그룹 지배구조 개편안에 반대투표 결정, 현대차-엘리엇, 지배구조 개편안 놓고 결국 표 대결…판세는?, 정의선과 엘리엇매니지먼트, 현대모비스 주주 표심 붙잡기 공방</t>
+    <t>18년도 1분기 NDR 후기: 바닥을 다진다,‘18년 2분기: 현재 모든 지표는 위를 가리키고 있다, 식인상어 엘리엇은 남을 배려하지 않는다, 차 부품사 '우수AMS', 에이알에스텍에 매각, 자신이 쓴 보고서가 '지배구조 정답'이라며 삼성 몰아친 김상조, 코스피 코스닥 동반상승, 북미 정상회담 기대 커져, 현대모비스 ‘현대차그룹 구글’로 바뀐다</t>
+  </si>
+  <si>
+    <t>엘리엇 "현대차 지배구조 개편안에 반대표 던질 것", 정의선 부회장 "현대차그룹 지배구조 개편 흔들리지 않을 것", 현대차그룹, '엘리엇 공세'에도 순환출자 고리 끊어야, 엘리엇, 현대자동차그룹 개편안에 반대투표 결정, 엘리엇 "현대차 개편 반대표" vs 정의선 "흔들리지 않는다", '행동' 나선 엘리엇...현대차그룹 지배구조 개편 훼방놓나, 엘리엇매니지먼트 “현대차그룹 지배구조 개편안에 반대표 던진다”, 모비스의 운명…`단기이익이냐, 미래가치냐` 국민연금 딜레마, 경협주 팔고 실적주 사들인 외국인…SK하이닉스·호텔신라 매수, 현대모비스 키우기 위한 정의선 부회장의 ‘글로벌스탠더드’ 행보, 엘리엇, 현대차그룹 지배구조 개편안에 반대투표 결정, 엘리엇, 지배구조 개편안 놓고 결국 표 대결…판세는?, 정의선과 엘리엇매니지먼트, 현대모비스 주주 표심 붙잡기 공방</t>
   </si>
   <si>
     <t>현대차그룹에 선전포고 엘리엇....지배구조 개편, 정의선 승계에 영향?</t>
   </si>
   <si>
-    <t>50전 49승…하이에나 엘리엇, 한국 노린다, 29일 현대차 주총...엘리엇 '반대표 여론몰이'vs현대차 '시장·주주 신뢰 얻겠다', 현대차-엘리엇, 정면 승부 벌인다, 모비스 주가·외국인·국민연금… 현대車 지배구조 개편 命運 가른다</t>
-  </si>
-  <si>
-    <t>한온시스템 주가 상승 가능, 자동차부품 수주회복 기대 유효, 운명의 날 앞둔 현대모비스, 주가·국민연금에 달렸다, 개미들의 행동대장 자처하는 엘리엇…쟁점 핵심은 ‘현대모비스’, 현대모비스 분할합병 주총 3대 변수…미래가치·주가·국민연금, “현대모비스 분할안 주총 통과에 의결권 자문사 의견이 변수”, 현대차·엘리엇 주총 전쟁… 국민연금·모비스 주가 ‘관건’, 현대차-재고문제가 먼저 풀려야 한다,줄지 않는 재고,2018년이후 10년간 한국공장 은퇴자 2.1만명 예상</t>
+    <t>50전 49승…하이에나 엘리엇, 한국 노린다, 29일 현대차 주총...엘리엇 '반대표 여론몰이'vs현대차 '시장·주주 신뢰 얻겠다', 엘리엇, 정면 승부 벌인다, 모비스 주가·외국인·국민연금… 현대車 지배구조 개편 命運 가른다</t>
+  </si>
+  <si>
+    <t>한온시스템 주가 상승 가능, 자동차부품 수주회복 기대 유효, 운명의 날 앞둔 현대모비스, 주가·국민연금에 달렸다, 개미들의 행동대장 자처하는 엘리엇…쟁점 핵심은 ‘현대모비스’, 현대모비스 분할합병 주총 3대 변수…미래가치·주가·국민연금, “현대모비스 분할안 주총 통과에 의결권 자문사 의견이 변수”, 현대차·엘리엇 주총 전쟁… 국민연금·모비스 주가 ‘관건’, 재고문제가 먼저 풀려야 한다,줄지 않는 재고,2018년이후 10년간 한국공장 은퇴자 2.1만명 예상</t>
   </si>
   <si>
     <t>ISS, 현대모비스 분할·합병에 반대 의견, 엘리엇 공격에 방어 나선 현대車… 국민연금 선택은, "해외 투기자본 꼼짝마!"… 엘리엇 방지法 발의, 현대모비스 분할에 반대의견 늘어, 주주 환원정책 더 내놓을까, 현대차 지배구조개편 주총 2주앞…혼전!, 현대차그룹, 지배구조개편 ‘찬성 위임장’ 확보 총력, 현대글로비스 주가 급락, 현대차그룹 지배구조 반대 권고 여파, 정의선, 등기이사 15년 만에 후계구도 밑그림 그렸다, ISS·글래스루이스, 현대모비스 분할·합병에 잇단 '반대'(종합), ISS 반대 의견에, 현대차그룹 "모비스 주주에 유리" 반박, ISS '합병 반대'... 현대차 "국내법 이해 못한 의견일 뿐", ISS "현대차 지배구조 개편안 반대"…현대차 "모비스 주주 이익", ISS도 개편안 '반대'…현대차그룹 "국내법 이해 못한 결정", 이번엔 현대기아차…모비스-글로비스 합병 '빨간불'</t>
@@ -4342,7 +4342,7 @@
     <t>남북경협 기대주 현대로템, 2017년 법인세 납부액은 '0'원, '셀빠'는 있는데, '삼바빠', '현대차빠'는 왜 없나?, 현대車 “지배구조 개편, 기존주주에 유리… ISS가 시장 호도”, ‘합병’ 비상 걸린 현대차그룹, 주주 만족 시킬 개편안 내나, 현대차 “ISS 반대는 국내 법규 이해 못한 심각한 오류”, 한진家 전횡에 힘실린 ‘상법 개정’… “갑질 견제” vs “경영권 위협”, '엘리엇 어깃장'에 뿔난 상장사들 "현대車그룹 지지", ISS, "모비스 분할합병은 결국 '정 패밀리' 위한 거래", 여론전 총대멘 사장들..'릴레이 호소문' 통할까, 현대차그룹 지배구조 개편안 주총 앞두고 '예측불허', “지배구조 개편안 지지 호소”…현대차그룹 CEO들 주주 설득 총력, 현대車 지배구조개편안 논란…‘경영승계 작업’ vs ‘투명성 강화’, 현대차 미래가 걸린 '지배구조 개편' …단기 vs 장기 투자자 표대결, 의결권자문사 vs 현대차그룹, 의견 엇갈리는 이유는?, 현대모비스 주총 카운트다운, 기업지배구조원 주목 이유가</t>
   </si>
   <si>
-    <t>Hyundai Motor Company-Effects of higher ASP and reduced costs to materialize,점진적으로 가격 개선과 비용 절감 효과가 가시화 되며 완만한 이익 회복 기대,‘가격-원가 경쟁력’ 회복 확인이 탄력적 주가 상승을 위한 관전포인트, 현대차 개편안, '강대강' 대결…투표따른 득과 실은, “현대모비스 분할합병 온도차는 이해와 설득, 소통 부족이 원인”, 현대차-가격-비용 개선 효과, 점진 가시화,점진적으로 가격 개선과 비용 절감 효과가 가시화 되며 완만한 이익 회복 기대,‘가격-원가 경쟁력’ 회복 확인이 탄력적 주가 상승을 위한 관전포인트, 국민연금 자문사도 반대 권고… 현대차 구조개편 난항, 전문가들 “분할합병 ‘온도차’, 이해와 소통 부족 때문”</t>
+    <t>Hyundai Motor Company-Effects of higher ASP and reduced costs to materialize,점진적으로 가격 개선과 비용 절감 효과가 가시화 되며 완만한 이익 회복 기대,‘가격-원가 경쟁력’ 회복 확인이 탄력적 주가 상승을 위한 관전포인트, 현대차 개편안, '강대강' 대결…투표따른 득과 실은, “현대모비스 분할합병 온도차는 이해와 설득, 소통 부족이 원인”, 가격-비용 개선 효과, 점진 가시화,점진적으로 가격 개선과 비용 절감 효과가 가시화 되며 완만한 이익 회복 기대,‘가격-원가 경쟁력’ 회복 확인이 탄력적 주가 상승을 위한 관전포인트, 국민연금 자문사도 반대 권고… 현대차 구조개편 난항, 전문가들 “분할합병 ‘온도차’, 이해와 소통 부족 때문”</t>
   </si>
   <si>
     <t>삼성 이재용, 전자와 생명 중 하나만 선택해야 한다면?, 남북경협주 ‘두 얼굴’…외국인 팔고 개미들 사고 “왜”</t>
@@ -4351,7 +4351,7 @@
     <t>'모비스 합병' 헤지펀드 여론전에도···국민연금 '중립' 지키나, 지배구조 개편 '표대결' 불리해진 현대차그룹, 대안 검토 나서나, 지배구조 개편 리스크, 증시 반등에 '걸림돌'</t>
   </si>
   <si>
-    <t>현대차그룹 지배구조 개편 불발에도…‘지금이 적기’, 개편안 부결시 당위성·공정성 타격… 백기 든 현대차그룹, "모비스 중심 지배구조안 고수"'…합병비율 등은 재조정, 부결시 타격 우려…결국 지배구조 개편 접은 현대차그룹(종합), 코스피 코스닥 동반상승, 미국과 중국 무역협상 합의 반겨, 현대차 지배구조 개편 무산…"높아진 주주 눈높이 못 맞췄다", 현대차 지배구조 개편 전격 연기, 분할 모비스 가치 재산정 방안 유력..지주사 전환 가능성도, 김상조도 호응했지만... 헤지펀드 흔들기에 현대차 '속도조절', 현대글로비스, 현대차 지배구조 개편 불투명에 시장심리 급락, 중간배당 평균 4.4%수익, 배당재테크 놀랍네, 현대차-하반기 G2(미국, 중국)시장 점진적인 회복 기대,4월 현대차 도매판매 전년대비 11% 증가,18년도 2분기 실적 개선 지연 예상되나 중국시장 기저효과 기대, 현대차그룹 지배구조 개편 ‘운명의 1주일’, 현대차 지배구조 개편, 이번에도 국민연금이 '열쇠 가졌다, 시장심리 톱5, LG·현대차·LG유플러스·삼성전자·아모레퍼시픽, 현대차그룹, 국민연금·주주 설득에 총력…외국인 '입김'에 운명 달렸다, 국민연금, 현대차 단기차익? 미래가치?… 지배구조 금주 판가름, 구본무 회장, 한 때 '좌파 재벌'이라고 불린 이유, 현대차그룹, '운명의 일주일'…전면 나선 정의선 부회장, 현대차, 캐스팅보트 쥔 국민연금마저 미온적… 결국 스톱, 지분 1%에 흔들리는 쉬운 나라…엘리엇에 막힌 모비스, 현대차, 지배구조 개편안 철회...모비스 비율 조정? 글로비스 CKD 매각?, 현대차그룹 "지배구조 개편안 보완하고 개선하겠다"…반대여론 부담됐나(종합), 현대차그룹, 지배구조 개편안 전격 포기 배경은?, 현대차그룹 지배구조개편안 ‘무산’…플랜B는</t>
+    <t>현대차그룹 지배구조 개편 불발에도…‘지금이 적기’, 개편안 부결시 당위성·공정성 타격… 백기 든 현대차그룹, "모비스 중심 지배구조안 고수"'…합병비율 등은 재조정, 부결시 타격 우려…결국 지배구조 개편 접은 현대차그룹(종합), 코스피 코스닥 동반상승, 미국과 중국 무역협상 합의 반겨, 현대차 지배구조 개편 무산…"높아진 주주 눈높이 못 맞췄다", 현대차 지배구조 개편 전격 연기, 분할 모비스 가치 재산정 방안 유력..지주사 전환 가능성도, 김상조도 호응했지만... 헤지펀드 흔들기에 현대차 '속도조절', 현대글로비스, 현대차 지배구조 개편 불투명에 시장심리 급락, 중간배당 평균 4.4%수익, 배당재테크 놀랍네, 하반기 G2(미국, 중국)시장 점진적인 회복 기대,4월 현대차 도매판매 전년대비 11% 증가,18년도 2분기 실적 개선 지연 예상되나 중국시장 기저효과 기대, 현대차그룹 지배구조 개편 ‘운명의 1주일’, 현대차 지배구조 개편, 이번에도 국민연금이 '열쇠 가졌다, 시장심리 톱5, LG·현대차·LG유플러스·삼성전자·아모레퍼시픽, 현대차그룹, 국민연금·주주 설득에 총력…외국인 '입김'에 운명 달렸다, 국민연금, 현대차 단기차익? 미래가치?… 지배구조 금주 판가름, 구본무 회장, 한 때 '좌파 재벌'이라고 불린 이유, 현대차그룹, '운명의 일주일'…전면 나선 정의선 부회장, 현대차, 캐스팅보트 쥔 국민연금마저 미온적… 결국 스톱, 지분 1%에 흔들리는 쉬운 나라…엘리엇에 막힌 모비스, 현대차, 지배구조 개편안 철회...모비스 비율 조정? 글로비스 CKD 매각?, 현대차그룹 "지배구조 개편안 보완하고 개선하겠다"…반대여론 부담됐나(종합), 현대차그룹, 지배구조 개편안 전격 포기 배경은?, 현대차그룹 지배구조개편안 ‘무산’…플랜B는</t>
   </si>
   <si>
     <t>현대차그룹 지배구조개편 연기에 주가는? "우려는 이미 반영", "주주·시장과 소통 부족 절감" 일단 후진 현대차그룹, KB증권 "분할합병안 철회로 현대글로비스 단기조정 가능성", 주가 상승 기대했던 개미들 혼란, "현대차, 주주환원 정책 강화할 것…불확실성은 부담", #행동주의 헤지펀드, 공정위도 찬성한 개편안 제동에…셈법 복잡해진 현대차그룹, "승자는 없었다" 지주회사로 갈까. 현대차그룹의 다음 선택은?, 현대자동차그룹 지배구조 개편 중단…모비스글로비스 주가 어쩌나, 엘리엇, 현대차 현금 12조 '눈독'···특별배당 요구 등 총공세 나서나</t>
@@ -4360,16 +4360,16 @@
     <t>현대차 지배구조 개편 철회 …“모비스 뜨고, 글로비스 지고”, 삼성-현대-LG, 경영권 승계 논란에 '휘청', '실패' 낙인 찍힌 자문업체들 "...", AG시스템 “한 눈에 보는 경제”, “현대글로비스 가치 높인 뒤 현대차그룹 지배구조 개편 나설 수도”, 현대차그룹 지배구조 수정안, 모비스 ‘유리’, 글로비스 ‘불리’, “현대차그룹 지배구조 재편 개선안, 기존 틀 크게 벗어나지 않을 것”, ‘기세등등’ 엘리엇…현대차 압박 거세지나, 이재용, 삼성전자 포기할 수 있다?, 현대차 지배구조 개편 철회… 증권가 “모비스 뜨고, 글로비스 지고”, 현대차, 극한 표대결 승리보다 시장신뢰 택했다, 현대차 ‘지배회사’ 골격 유지… 모비스는 先 분할·상장?, 현대차 지배구조 철회...증권가 "이미 예상했던 일...신뢰 상실", '현대차그룹 개편안 철회' 엇갈린 현대모비스‧글로비스 주가 향방은?, 현대글로비스와 닮은꼴 삼성SDS, 이재용 부회장 자금줄 역할 '부각', "현대모비스, 분할·합병 중단 단기간 주가에 긍정적"-하나, 금감원, 우후죽순 투자자문사 난립에 철퇴, "현대모비스 주식 사도 된다", 분할합병 재추진하면 주가에 긍정적</t>
   </si>
   <si>
-    <t>현대차-가동률과 인센티브 개선 지속 전망,신차 Cycle이 시작된 지난 3월 이후 전년 대비 증감율 가동률 증가와 인센티브 감소 추이 지속 중,주주친화정책의 확대 개선 기대감 여전히 유효, '차등의결권ㆍ포이즌필ㆍ황금의결권'…경영권방어제도 도입, 어려운 이유, '기업사냥꾼' 엘리엇 실체 해부, 현대차그룹 향후 개편안은? 기존 개편안 수정 VS 신규 개편안 ‘팽팽’, 시장심리 톱5, SK하이닉스·삼성전자·현대모비스·롯데푸드·LS산전, 합병 실패한 현대차그룹, '뒷북 주주관리' 도마에, 골드만삭스 등, 체면 구긴 현대차 자문사들, 재계는 지금 '지뢰밭'…SK만 조용한 '딥체인지', 현대차 공격한 `행동주의 헤지펀드`</t>
-  </si>
-  <si>
-    <t>삼성 지배구조 개선 ‘김상조식 해법’ 현실성 논란, ‘LG 후계자’ 구광모, 상속세 납부 어떻게?, '지배구조개편 중단' 현대차-모비스, 자사주 소각 어쩌나, AG시스템 “한 눈에 보는 경제”, 현대차-2018 하반기 전망: 미국 회복의 시작,미국 회복의 시작: 신형 싼타페 현지생산, 확대되는 SUV 비중,연초 계획대로 재고 3.0개월 이하로 떨어질 것을 기대, 현대차-M/S 반등, Mix 개선 모두 필요,싼타페만으로는 부족,실적 개선에 의한 배당 증가 필요</t>
+    <t>가동률과 인센티브 개선 지속 전망,신차 Cycle이 시작된 지난 3월 이후 전년 대비 증감율 가동률 증가와 인센티브 감소 추이 지속 중,주주친화정책의 확대 개선 기대감 여전히 유효, '차등의결권ㆍ포이즌필ㆍ황금의결권'…경영권방어제도 도입, 어려운 이유, '기업사냥꾼' 엘리엇 실체 해부, 현대차그룹 향후 개편안은? 기존 개편안 수정 VS 신규 개편안 ‘팽팽’, 시장심리 톱5, SK하이닉스·삼성전자·현대모비스·롯데푸드·LS산전, 합병 실패한 현대차그룹, '뒷북 주주관리' 도마에, 골드만삭스 등, 체면 구긴 현대차 자문사들, 재계는 지금 '지뢰밭'…SK만 조용한 '딥체인지', 현대차 공격한 `행동주의 헤지펀드`</t>
+  </si>
+  <si>
+    <t>삼성 지배구조 개선 ‘김상조식 해법’ 현실성 논란, ‘LG 후계자’ 구광모, 상속세 납부 어떻게?, '지배구조개편 중단' 현대차-모비스, 자사주 소각 어쩌나, AG시스템 “한 눈에 보는 경제”, 2018 하반기 전망: 미국 회복의 시작,미국 회복의 시작: 신형 싼타페 현지생산, 확대되는 SUV 비중,연초 계획대로 재고 3.0개월 이하로 떨어질 것을 기대, M/S 반등, Mix 개선 모두 필요,싼타페만으로는 부족,실적 개선에 의한 배당 증가 필요</t>
   </si>
   <si>
     <t>기업공시, ‘젊은 총수’ 시대 맞은 재계, 풀어야 할 과제, “현대차 기아차 주식 저점매수 기회”, 미국 관세폭탄 가능성 낮아, 스튜어드십 코드 현명한 해법 찾아야</t>
   </si>
   <si>
-    <t>"현대차 주식 매수 신중해야", 미국 판매 부진하고 중국은 회복 더뎌, 신동빈 항소심 치열한 공방 ‘PT만 4시간’...3대 쟁점은(종합), 개인도 공매도 가능? '대주거래' 활성화 안 되는 이유, 엘리엇의 진짜 노림수는?···현대차의 대응 방안은 뭘까, 현대차-G2 시장 부진과 미래차 기술 비용 증가,하반기에도 미국 시장 부진 지속 전망,중국 시장 예상보다 더딘 점진적 회복 전망</t>
+    <t>"현대차 주식 매수 신중해야", 미국 판매 부진하고 중국은 회복 더뎌, 신동빈 항소심 치열한 공방 ‘PT만 4시간’...3대 쟁점은(종합), 개인도 공매도 가능? '대주거래' 활성화 안 되는 이유, 엘리엇의 진짜 노림수는?···현대차의 대응 방안은 뭘까, G2 시장 부진과 미래차 기술 비용 증가,하반기에도 미국 시장 부진 지속 전망,중국 시장 예상보다 더딘 점진적 회복 전망</t>
   </si>
   <si>
     <t>손 안대고 재벌개혁?…국민연금 앞세운 정부 '팝콘각', 기업 경영권 방어수단 도입, "글로비스, 저평가 심해..경협 확대땐 수혜", ‘여름 보너스’(중간배당금)많이 주는 회사 어디?, A주 MSCI EM 편입 임박, 한국·대만 사례를 통해 보는 A주 투자 기회</t>
@@ -4387,7 +4387,7 @@
     <t>현대엔지니어링, 현대건설 주가 급등에 합병 가능성 '뚝', “해외배당 역대 최대” 삼성전자·현대차 흔든 엘리엇은 얼마 벌었나</t>
   </si>
   <si>
-    <t>현대차-신형 싼타페 성공적 론칭과 중국회복 필요,신차사이클 Vs 비우호적인 외부환경,2분기 Preview: 영업이익 감소추세 지속, "이노션 주식 사도 된다", 월드컵 특수와 현대차 신차 출시효과 기대, 현대모비스 목표주가 낮아져, 현대차 중국 판매회복 더딘 여파, "급등한 현대건설 주가, 고민되네"…복잡해진 현대차그룹 승계 셈법, 현대차그룹 지배구조 개편안의 교훈, 현대차그룹주 구조개편 불발·美 관세폭탄 우려에 휘청</t>
+    <t>신형 싼타페 성공적 론칭과 중국회복 필요,신차사이클 Vs 비우호적인 외부환경,2분기 Preview: 영업이익 감소추세 지속, "이노션 주식 사도 된다", 월드컵 특수와 현대차 신차 출시효과 기대, 현대모비스 목표주가 낮아져, 현대차 중국 판매회복 더딘 여파, "급등한 현대건설 주가, 고민되네"…복잡해진 현대차그룹 승계 셈법, 현대차그룹 지배구조 개편안의 교훈, 현대차그룹주 구조개편 불발·美 관세폭탄 우려에 휘청</t>
   </si>
   <si>
     <t>채형석 애경그룹 부회장, 10대그룹사 1/4 자본잠식···롯데·신세계는 1/3</t>
@@ -4396,7 +4396,7 @@
     <t>"하반기 유로존 경기 살아난다… 건설·조선 등 경기 민감株 담아라", 6월 중간배당 받아 '여름 보너스' 챙겨볼까</t>
   </si>
   <si>
-    <t>글로벌 배터리 1위 CATL 상장 첫날 44% 급등, 글로벌 배터리 1위 CATL 창업판 대장주될까, “현대차 기아차 현대모비스 주식 살 때", 새 지배구조 기대 높아, 현대차-기나긴 BIG2 시장 판매부진에서 탈출,기저 속 신차 모맨텀을 통한 회복세 기대,18년도 2분기 매출 24.8조, 영업이익 940십억원(OPM 3.8%) 전망</t>
+    <t>글로벌 배터리 1위 CATL 상장 첫날 44% 급등, 글로벌 배터리 1위 CATL 창업판 대장주될까, “현대차 기아차 현대모비스 주식 살 때", 새 지배구조 기대 높아, 기나긴 BIG2 시장 판매부진에서 탈출,기저 속 신차 모맨텀을 통한 회복세 기대,18년도 2분기 매출 24.8조, 영업이익 940십억원(OPM 3.8%) 전망</t>
   </si>
   <si>
     <t>코스피 코스닥 동반하락, 북미 정상회담 열리자 차익매물 쏟아져</t>
@@ -4414,7 +4414,7 @@
     <t>삼성·LG그룹 지고 현대그룹 '비상'..그룹주펀드 세대교체하나</t>
   </si>
   <si>
-    <t>美·中 무역전쟁 우려 ‘털썩’...외인 5일째 '팔자', 현대차-상반기, 긴 터널의 끝,상반기로 어두운 터널은 벗어날 것,하반기 투자포인트 - 생산량과 판매량의 동시 회복, 기업 사냥꾼과 싸우려면, 현대차, 하반기 터닝포인트 기대… 美 무역확장법 232조 시행 변수도, 현대차 회복세 확실..폭풍 할인 약발 언제까지, 코스피 코스닥 동반하락, 미국과 중국 무역분쟁에 '움찔'</t>
+    <t>美·中 무역전쟁 우려 ‘털썩’...외인 5일째 '팔자', 상반기, 긴 터널의 끝,상반기로 어두운 터널은 벗어날 것,하반기 투자포인트 - 생산량과 판매량의 동시 회복, 기업 사냥꾼과 싸우려면, 현대차, 하반기 터닝포인트 기대… 美 무역확장법 232조 시행 변수도, 현대차 회복세 확실..폭풍 할인 약발 언제까지, 코스피 코스닥 동반하락, 미국과 중국 무역분쟁에 '움찔'</t>
   </si>
   <si>
     <t>코스피 코스닥 동반하락, 미국과 중국 무역분쟁에 발목 잡혀, 스웨덴전 패배가 뼈아픈 월드컵 수혜주, 김상조 한마디에 기업 주가 급락…"책임져라" 청원 봇물, “김상조 발언에 주가폭락… 책임져라” 뿔난 삼성SDS 소액주주들 靑 청원</t>
@@ -4426,13 +4426,13 @@
     <t>코스피 코스닥 동반하락, 외국인 매도세 강해, 경영의 족쇄냐, 승계 면죄부냐…합병비율 규제의 두 얼굴, 불만 달래기용 '땜질 전략'…기업 가치만 떨어뜨린다, 현대차, 아우디와 수소차 협력 밸류에이션 할인 완화 기대 - NH투자증권, 김상조 “순환출자, 역사의 뒤안길로 사라졌다”, 정몽구-정의선 경영승계 현대차그룹, 정부당국 '협공'에 주름살</t>
   </si>
   <si>
-    <t>삼성바이오로직스 주가 급등해 시총 순위 뛰어, 셀트리온도 올라, "현대차 주식에 보수적 대응해야", 하반기 실적도 밝지 않아, 현대차-18년도 2분기 Preview, 영업이익 감익 추세 지속,하반기 부정적인 대외 변수 강화,단기 보수적인 대응을 추천</t>
+    <t>삼성바이오로직스 주가 급등해 시총 순위 뛰어, 셀트리온도 올라, "현대차 주식에 보수적 대응해야", 하반기 실적도 밝지 않아, 18년도 2분기 Preview, 영업이익 감익 추세 지속,하반기 부정적인 대외 변수 강화,단기 보수적인 대응을 추천</t>
   </si>
   <si>
     <t>행동주의 펀드 엘리엇 현대차 손익계산서는</t>
   </si>
   <si>
-    <t>현대차, 영업익 감익 추세…시장심리↓, 차세대 2차전지 전고체 선점 경쟁…치솟는 씨아이에스 몸값, "등락 심하고 운용범위 제한"… 그룹주 펀드 외면하는 투자자들, 현대차-상반기보다 개선된 하반기 기대,18년도 2분기 예측값 매출액 24.0조원(-1.3% 전년 대비 증감율), 영업이익 9,085억원(-32.4% 전년 대비 증감율),하반기 미국 Top 5 판매 차종 중 3개 차종 상품성 개선 모델 출시</t>
+    <t>현대차, 영업익 감익 추세…시장심리↓, 차세대 2차전지 전고체 선점 경쟁…치솟는 씨아이에스 몸값, "등락 심하고 운용범위 제한"… 그룹주 펀드 외면하는 투자자들, 상반기보다 개선된 하반기 기대,18년도 2분기 예측값 매출액 24.0조원(-1.3% 전년 대비 증감율), 영업이익 9,085억원(-32.4% 전년 대비 증감율),하반기 미국 Top 5 판매 차종 중 3개 차종 상품성 개선 모델 출시</t>
   </si>
   <si>
     <t>공정위발 SI 일감 몰아주기 논란…비상장사 현대오토에버 주목</t>
@@ -4459,25 +4459,25 @@
     <t>현대차 `FCA 인수설`, 끝날 때까지 끝난 게 아니다?, 4일 주가에 영향을 미칠 만한 전일 주요 공시, "현대차 부인에도 'FCA 인수' 가능성 여전" 해외 언론 주목</t>
   </si>
   <si>
-    <t>현대차-끝이 보이는 긴 부진의 터널,18년도 2분기 매출액 23,697십억원(전년 대비 증감율-2.5%), 영업이익 922십억원(전년 대비 증감율-31.4%), OPM 3.0% 전망,18년도 하반기 부터 미국 판매, 생산 동반 회복세 기대, 대기업 오너家의 희비, 재상장 앞둔 '왕년 PC왕' 델, 기업사냥꾼 난관 넘을까, 현대車그룹 시가총액 한달새 16조 증발, 8년 전 주가로 후진한 현대車, 다시 전진할까</t>
-  </si>
-  <si>
-    <t>시장심리 톱5, 카카오·SK·LG이노텍·GS리테일·네이버, 현대차-경쟁 심화, 무역분쟁 불확실성으로 기저효과 반감,하반기 긍정적 요인 4가지,하반기 부정적 요인 4가지,2분기 실적 프리뷰, 현대차-2Q 실적 하회. 미국 개선. 중국 지연,18년도 2분기 Preview: 영업이익률 3.8% 예상,미국의 개선 vs. 중국의 부진, 현대차-중국과 미국 엇갈린 방향성,2분기 매출 23.5조원, 영업이익 9,520억원 예상,중국 회복은 예상보다 느리나 미국은 기대 수준으로 회복 중. 하반기 실적 개선</t>
+    <t>끝이 보이는 긴 부진의 터널,18년도 2분기 매출액 23,697십억원(전년 대비 증감율-2.5%), 영업이익 922십억원(전년 대비 증감율-31.4%), OPM 3.0% 전망,18년도 하반기 부터 미국 판매, 생산 동반 회복세 기대, 대기업 오너家의 희비, 재상장 앞둔 '왕년 PC왕' 델, 기업사냥꾼 난관 넘을까, 현대車그룹 시가총액 한달새 16조 증발, 8년 전 주가로 후진한 현대車, 다시 전진할까</t>
+  </si>
+  <si>
+    <t>시장심리 톱5, 카카오·SK·LG이노텍·GS리테일·네이버, 경쟁 심화, 무역분쟁 불확실성으로 기저효과 반감,하반기 긍정적 요인 4가지,하반기 부정적 요인 4가지,2분기 실적 프리뷰, 2Q 실적 하회. 미국 개선. 중국 지연,18년도 2분기 Preview: 영업이익률 3.8% 예상,미국의 개선 vs. 중국의 부진, 중국과 미국 엇갈린 방향성,2분기 매출 23.5조원, 영업이익 9,520억원 예상,중국 회복은 예상보다 느리나 미국은 기대 수준으로 회복 중. 하반기 실적 개선</t>
   </si>
   <si>
     <t>현대차그룹 지배구조 개편 무산 50일···‘발로 뛴’ 정의선 해법 찾았나</t>
   </si>
   <si>
-    <t>Hyundai Motor-China recovery slow; US meets expectations,2분기 매출 23.5조원, 영업이익 9,520억원 예상,중국 회복은 예상보다 느리나 미국은 기대 수준으로 회복 중. 하반기 실적 개선, 현대차-년도년도 1분기 2분기 Preview: 반등전의 마지막 실적,년도년도 1분기 2분기 Preview: 영업이익 9,581억원 예상, 컨센서스 소폭 하회,전년동기 시차로는 아직 부진한 실적, "KCC, 부동산 정책과 코스피 약세 부담…목표가↓"-SK, KCC, 크게 기대할 것 없는 하반기-SK, KCC 목표주가 낮아져, 강력한 부동산대책에 건설경기 위축, 코스피 소폭 오르고 코스닥은 하락, 해외투자자 매도세 강해, KCC, "부동산 정책과 KO…" 매수(유지)-SK증권</t>
-  </si>
-  <si>
-    <t>국민연금, 상반기 국내 주식서 9兆 평가손, 현대차-판매 경쟁력 회복이 우선,내년까지 본질적인 판매 경쟁력이 판가름 날 중요한 시점, 환율 부담. 신차 중심 판매 믹스 개선은 하반기부터, 현대차-18년도 2분기 실적은 기대치 소폭 하회 전망,2분기 컨센서스 소폭 하회 전망,미국 7월 싼타페 투입, 소매판매 미흡한 중국은 9월이후 프로모션 강화, KAI 지분 모두 판 한화에어로스페이스..."주가 최저가 수준인데 왜"에 "재원 마련", TheCapitalGroupCompanies,Inc. 외</t>
-  </si>
-  <si>
-    <t>"13억 인구·포스트차이나"… 인도의 재발견, 한국항공우주산업의 미국 고등훈련기 수주에 난기류 흐르나, 현대차-멀리 보면 회복이 보인다,북미 손익 악화, 중국 회복 지연으로 낮아진 실적 반영해 주가는 역사적, 상대적 저점 수준까지 하락,손익 회복시 Bottom fishing 타이밍에 대한 고민 필요, 뉴욕 외국인 투자자가 보는 한국, 한국 주식</t>
-  </si>
-  <si>
-    <t>시장심리 톱5, 카카오·LG디스플레이·쌍용차·빙그레·한섬, 현대차, 파업 돌입·무역 전쟁 직격타…시장심리↓, 현대차-18년도 2분기 Preview-하반기에 대한 확신이 필요,2 분기 실적보다 중요한 하반기 전망, 현대차-무역전쟁의 위협,개선 및 회복 국면을 실현 중인 현대차 주요 시장 판매 실적,무역전쟁 위협으로 MSCI Global Auto Index 6 월 이후 하락세 심화, 현대차그룹 '지배구조 개편' 재시동說에...주가 꿈틀</t>
+    <t>Hyundai Motor-China recovery slow; US meets expectations,2분기 매출 23.5조원, 영업이익 9,520억원 예상,중국 회복은 예상보다 느리나 미국은 기대 수준으로 회복 중. 하반기 실적 개선, 년도년도 1분기 2분기 Preview: 반등전의 마지막 실적,년도년도 1분기 2분기 Preview: 영업이익 9,581억원 예상, 컨센서스 소폭 하회,전년동기 시차로는 아직 부진한 실적, "KCC, 부동산 정책과 코스피 약세 부담…목표가↓"-SK, KCC, 크게 기대할 것 없는 하반기-SK, KCC 목표주가 낮아져, 강력한 부동산대책에 건설경기 위축, 코스피 소폭 오르고 코스닥은 하락, 해외투자자 매도세 강해, KCC, "부동산 정책과 KO…" 매수(유지)-SK증권</t>
+  </si>
+  <si>
+    <t>국민연금, 상반기 국내 주식서 9兆 평가손, 판매 경쟁력 회복이 우선,내년까지 본질적인 판매 경쟁력이 판가름 날 중요한 시점, 환율 부담. 신차 중심 판매 믹스 개선은 하반기부터, 18년도 2분기 실적은 기대치 소폭 하회 전망,2분기 컨센서스 소폭 하회 전망,미국 7월 싼타페 투입, 소매판매 미흡한 중국은 9월이후 프로모션 강화, KAI 지분 모두 판 한화에어로스페이스..."주가 최저가 수준인데 왜"에 "재원 마련", TheCapitalGroupCompanies,Inc. 외</t>
+  </si>
+  <si>
+    <t>"13억 인구·포스트차이나"… 인도의 재발견, 한국항공우주산업의 미국 고등훈련기 수주에 난기류 흐르나, 멀리 보면 회복이 보인다,북미 손익 악화, 중국 회복 지연으로 낮아진 실적 반영해 주가는 역사적, 상대적 저점 수준까지 하락,손익 회복시 Bottom fishing 타이밍에 대한 고민 필요, 뉴욕 외국인 투자자가 보는 한국, 한국 주식</t>
+  </si>
+  <si>
+    <t>시장심리 톱5, 카카오·LG디스플레이·쌍용차·빙그레·한섬, 현대차, 파업 돌입·무역 전쟁 직격타…시장심리↓, 18년도 2분기 Preview-하반기에 대한 확신이 필요,2 분기 실적보다 중요한 하반기 전망, 무역전쟁의 위협,개선 및 회복 국면을 실현 중인 현대차 주요 시장 판매 실적,무역전쟁 위협으로 MSCI Global Auto Index 6 월 이후 하락세 심화, 현대차그룹 '지배구조 개편' 재시동說에...주가 꿈틀</t>
   </si>
   <si>
     <t>현대차 지배구조 개편 무산됐지만 나머지 기업은…, 코스피 코스닥 동반상승, 외국인 사자에 투자심리 좋아져</t>
@@ -4486,7 +4486,7 @@
     <t>다른 가문의 ‘황태자’들과는 달랐던···총수로 선택된 구광모의 과제, 김상조 말에 화들짝?···현대차그룹 新 지배구조 개편안 윤곽 나오나</t>
   </si>
   <si>
-    <t>"이노션 주식은 저가매수 기회", 일감몰아주기 규제 영향은 제한적, '미·중 무역전쟁' 한국 수출 악화일로…수출주 반등 언제쯤?, "현대차 주식 사도 된다", 넥쏘로 수소전기차의 대중화 가능성 보여, 현대차-수소전기차 이니셔티브 주도,수소전기차 대중화 가능성 높인 넥쏘,2020년경 수소전기차 시장 본격화 전망, 아우디폭스바겐과의 제휴는 긍정적</t>
+    <t>"이노션 주식은 저가매수 기회", 일감몰아주기 규제 영향은 제한적, '미·중 무역전쟁' 한국 수출 악화일로…수출주 반등 언제쯤?, "현대차 주식 사도 된다", 넥쏘로 수소전기차의 대중화 가능성 보여, 수소전기차 이니셔티브 주도,수소전기차 대중화 가능성 높인 넥쏘,2020년경 수소전기차 시장 본격화 전망, 아우디폭스바겐과의 제휴는 긍정적</t>
   </si>
   <si>
     <t>LG 구광모가 직면할 3가지 숙제, 삼성바이오로직스 주가 올라 시총순위 뛰어, 셀트리온은 떨어져</t>
@@ -4498,7 +4498,7 @@
     <t>코스피 중국 증시 상승에 소폭 올라, 코스닥은 하락, 현대차그룹 지배구조 개편 재추진하나?...중심축 모비스서 글로비스로 이동</t>
   </si>
   <si>
-    <t>헤지펀드 알아야 돈 번다, 코스피 코스닥 하락, 미중 환율전쟁 조짐과 중국 바이오주 급락 영향, 현대차-공포가 걷히면 숫자가 보인다,무파업의 경제적 효과, 연간 영업이익 4,356 억원,미국 관세부과 우려 이미 주가에 충분히 반영, 이제 Upside 를 고민할 때, 유비벨록스, 창업주 지분율 낮지만 든든한 우군 확보</t>
+    <t>헤지펀드 알아야 돈 번다, 코스피 코스닥 하락, 미중 환율전쟁 조짐과 중국 바이오주 급락 영향, 공포가 걷히면 숫자가 보인다,무파업의 경제적 효과, 연간 영업이익 4,356 억원,미국 관세부과 우려 이미 주가에 충분히 반영, 이제 Upside 를 고민할 때, 유비벨록스, 창업주 지분율 낮지만 든든한 우군 확보</t>
   </si>
   <si>
     <t>"진영 논리에 집착하니 대화가 안 된다" - 장하준 교수 인터뷰, 코스피 코스닥 동반상승, 중국 재정정책 확대에 증시 밝아져</t>
@@ -4507,10 +4507,10 @@
     <t>현대차 지배구조 중심축, 모비스에서 글로비스로 이동하나</t>
   </si>
   <si>
-    <t>현대차-현대차 18년도 2분기 Review-주력 모델 교체 시기에 대한 기대,2분기 영업이익 9,508억원 (-29.3% 전년 대비 증감율), 시장 컨센서스 부합,차량 판매 마진 축소. 판매보증비 등의 감소를 감안하면 더욱 부진했던 실적, 현대차-년도년도 1분기 2분기 Review: 경계선, 더 이상의 현금유출은 위험하다,년도년도 1분기 2분기 영업이익, 부진,자동차 부문 부진을 금융부분 개선이 일부 상쇄, 코스피 코스닥 상승, 미국과 유럽 무역갈등 완화에 투자심리 좋아져</t>
-  </si>
-  <si>
-    <t>Hyundai Motor-Taking small steps to make big strides,2분기 영업이익 0.95조원(-29.3%)으로 시장 기대치에 부합,대외변수에서 실적의 방향성으로 무게추의 이동을 기대, 현대차-오랜만에 보는 군더더기 없는 실적,2분기 실적은 컨센서스와 추정치에 부합,내수판매와 금융부문 호조가 비우호적 환율과 미국 가동률 하락을 방어,하반기 미국 가동률 상승과 인센티브 축소에 주목, 현대차-하반기 판매 경쟁력 회복 여부가 관건,18년도 2분기 Review-자동차부문 기대 이하 vs. 금융부문 기대 이상,하반기 판매 경쟁력 회복 여부가 관건, Hyundai Motor-Regaining sales competitiveness in 18년도 하반기 will be key,18년도 2분기 Review-자동차부문 기대 이하 vs. 금융부문 기대 이상,하반기 판매 경쟁력 회복 여부가 관건, 현대차-3개 분기 연속 영업이익 1조 하회,24,712십억원, OP 951십억원, 순익 701십억원 기록,국내, 미국 동반 부진이 초래한 차량사업부 부진 지속, 현대차-금융 부분 선전으로 시장 기대치에 부합,2분기 실적 리뷰: 금융 부분 선전,2018년 3분기 전망: 소폭 개선되나 감익 추세 지속, 현대차-년도년도 1분기 2분기 Review: 시장 기대치에는 부합하였으나...,년도년도 1분기 2분기 Review: 시장 기대치에 부합한 실적,년도년도 1분기 3분기 Preview: 환율 상승, 개별소비세 인하 긍정적, 현대차-우보천리의 시작,2분기 영업이익 0.95조원(-29.3%)으로 시장 기대치에 부합,대외변수에서 실적의 방향성으로 무게추의 이동을 기대, 코스피 '외국인 매수세' 덕에 올라, 코스닥도 이틀째 상승, 27일 주가에 영향을 미칠 만한 전일 주요 공시, 바이오 간판만 달아도 대박났는데… 6개월새 반토막 속출, Hyundai Motor-Taking small steps to make big strides,2분기 영업이익 0.95조원(-29.3%)으로 시장 기대치에 부합,대외변수에서 실적의 방향성으로 무게추의 이동을 기대, 현대차-하반기 판매 경쟁력 회복 여부가 관건,18년도 2분기 Review-자동차부문 기대 이하 vs. 금융부문 기대 이상,하반기 판매 경쟁력 회복 여부가 관건, Hyundai Motor-Regaining sales competitiveness in 18년도 하반기 will be key,18년도 2분기 Review-자동차부문 기대 이하 vs. 금융부문 기대 이상,하반기 판매 경쟁력 회복 여부가 관건, 현대차-3개 분기 연속 영업이익 1조 하회,24,712십억원, OP 951십억원, 순익 701십억원 기록,국내, 미국 동반 부진이 초래한 차량사업부 부진 지속, 현대차-오랜만에 보는 군더더기 없는 실적,2분기 실적은 컨센서스와 추정치에 부합,내수판매와 금융부문 호조가 비우호적 환율과 미국 가동률 하락을 방어,하반기 미국 가동률 상승과 인센티브 축소에 주목, 현대차-계산이 서는 실적 흐름의 시작,시장기대치에 부합한 18년도 2분기 실적 기록,더 나아질 18년도 하반기 실적 방향성, 현대차-하반기 관전 포인트는? (요약),신형 싼타페와 중국시장 M/S 회복 여부,2분기 Review-영업실적 감소추세 지속, 현대차-하반기 관전 포인트는?,신형 싼타페와 중국시장 M/S 회복 여부,2분기 Review-영업실적 감소추세 지속, HMC-What are the key factors for 18년도 하반기 ?,신형 싼타페와 중국시장 M/S 회복 여부,2분기 Review-영업실적 감소추세 지속, 현대차-계산이 서는 실적 흐름의 시작,시장기대치에 부합한 18년도 2분기 실적 기록,더 나아질 18년도 하반기 실적 방향성, 현대차-소확회, 작지만 확실한 회복의 단서,영업이익은 9,508억원 기록,주요 부진지역 북미 손익개선 예상보다 빠를 전망, 현대차-운용의 묘가 중요해질 하반기,18 년 2 분기 매출액 24.7 조, 영업이익 9,508 억원, 당기순이익 8,107 억원 기록,막연한 기대감보다는 현실화될 가능성이 높은 리스크 요인을 점검할 필요, 현대차-년도년도 1분기 2분기 Review: 시장 기대치에는 부합하였으나...,년도년도 1분기 2분기 Review: 시장 기대치에 부합한 실적,년도년도 1분기 3분기 Preview: 환율 상승, 개별소비세 인하 긍정적</t>
+    <t>현대차 18년도 2분기 Review-주력 모델 교체 시기에 대한 기대,2분기 영업이익 9,508억원 (-29.3% 전년 대비 증감율), 시장 컨센서스 부합,차량 판매 마진 축소. 판매보증비 등의 감소를 감안하면 더욱 부진했던 실적, 년도년도 1분기 2분기 Review: 경계선, 더 이상의 현금유출은 위험하다,년도년도 1분기 2분기 영업이익, 부진,자동차 부문 부진을 금융부분 개선이 일부 상쇄, 코스피 코스닥 상승, 미국과 유럽 무역갈등 완화에 투자심리 좋아져</t>
+  </si>
+  <si>
+    <t>Hyundai Motor-Taking small steps to make big strides,2분기 영업이익 0.95조원(-29.3%)으로 시장 기대치에 부합,대외변수에서 실적의 방향성으로 무게추의 이동을 기대, 오랜만에 보는 군더더기 없는 실적,2분기 실적은 컨센서스와 추정치에 부합,내수판매와 금융부문 호조가 비우호적 환율과 미국 가동률 하락을 방어,하반기 미국 가동률 상승과 인센티브 축소에 주목, 하반기 판매 경쟁력 회복 여부가 관건,18년도 2분기 Review-자동차부문 기대 이하 vs. 금융부문 기대 이상,하반기 판매 경쟁력 회복 여부가 관건, Hyundai Motor-Regaining sales competitiveness in 18년도 하반기 will be key,18년도 2분기 Review-자동차부문 기대 이하 vs. 금융부문 기대 이상,하반기 판매 경쟁력 회복 여부가 관건, 3개 분기 연속 영업이익 1조 하회,24,712십억원, OP 951십억원, 순익 701십억원 기록,국내, 미국 동반 부진이 초래한 차량사업부 부진 지속, 금융 부분 선전으로 시장 기대치에 부합,2분기 실적 리뷰: 금융 부분 선전,2018년 3분기 전망: 소폭 개선되나 감익 추세 지속, 년도년도 1분기 2분기 Review: 시장 기대치에는 부합하였으나...,년도년도 1분기 2분기 Review: 시장 기대치에 부합한 실적,년도년도 1분기 3분기 Preview: 환율 상승, 개별소비세 인하 긍정적, 우보천리의 시작,2분기 영업이익 0.95조원(-29.3%)으로 시장 기대치에 부합,대외변수에서 실적의 방향성으로 무게추의 이동을 기대, 코스피 '외국인 매수세' 덕에 올라, 코스닥도 이틀째 상승, 27일 주가에 영향을 미칠 만한 전일 주요 공시, 바이오 간판만 달아도 대박났는데… 6개월새 반토막 속출, Hyundai Motor-Taking small steps to make big strides,2분기 영업이익 0.95조원(-29.3%)으로 시장 기대치에 부합,대외변수에서 실적의 방향성으로 무게추의 이동을 기대, 하반기 판매 경쟁력 회복 여부가 관건,18년도 2분기 Review-자동차부문 기대 이하 vs. 금융부문 기대 이상,하반기 판매 경쟁력 회복 여부가 관건, Hyundai Motor-Regaining sales competitiveness in 18년도 하반기 will be key,18년도 2분기 Review-자동차부문 기대 이하 vs. 금융부문 기대 이상,하반기 판매 경쟁력 회복 여부가 관건, 3개 분기 연속 영업이익 1조 하회,24,712십억원, OP 951십억원, 순익 701십억원 기록,국내, 미국 동반 부진이 초래한 차량사업부 부진 지속, 오랜만에 보는 군더더기 없는 실적,2분기 실적은 컨센서스와 추정치에 부합,내수판매와 금융부문 호조가 비우호적 환율과 미국 가동률 하락을 방어,하반기 미국 가동률 상승과 인센티브 축소에 주목, 계산이 서는 실적 흐름의 시작,시장기대치에 부합한 18년도 2분기 실적 기록,더 나아질 18년도 하반기 실적 방향성, 하반기 관전 포인트는? (요약),신형 싼타페와 중국시장 M/S 회복 여부,2분기 Review-영업실적 감소추세 지속, 하반기 관전 포인트는?,신형 싼타페와 중국시장 M/S 회복 여부,2분기 Review-영업실적 감소추세 지속, HMC-What are the key factors for 18년도 하반기 ?,신형 싼타페와 중국시장 M/S 회복 여부,2분기 Review-영업실적 감소추세 지속, 계산이 서는 실적 흐름의 시작,시장기대치에 부합한 18년도 2분기 실적 기록,더 나아질 18년도 하반기 실적 방향성, 소확회, 작지만 확실한 회복의 단서,영업이익은 9,508억원 기록,주요 부진지역 북미 손익개선 예상보다 빠를 전망, 운용의 묘가 중요해질 하반기,18 년 2 분기 매출액 24.7 조, 영업이익 9,508 억원, 당기순이익 8,107 억원 기록,막연한 기대감보다는 현실화될 가능성이 높은 리스크 요인을 점검할 필요, 년도년도 1분기 2분기 Review: 시장 기대치에는 부합하였으나...,년도년도 1분기 2분기 Review: 시장 기대치에 부합한 실적,년도년도 1분기 3분기 Preview: 환율 상승, 개별소비세 인하 긍정적</t>
   </si>
   <si>
     <t>호황의 끝에 가까워졌다-포춘의 경고, 신사업 발굴 나선 재계 2·3위, 투자은행(IB) 전문가 찾는 까닭은?, 코스피 코스닥 동반하락, 코스피 거래대금 연중 가장 적어</t>
@@ -4519,7 +4519,7 @@
     <t>바이오주 거품 논란·미중 무역전쟁…추락하는 증시 기댈 언덕은?, 코스피 코스닥 동반상승, 저가매수세 활발히 유입</t>
   </si>
   <si>
-    <t>현대차-18년도 2분기 NDR Review: Step by Step,환율 영향에도 이머징 수익성 방어, 북미 인센티브 하향으로 손익 회복,우호적 환율, 유가상승, 신차 출시가 중국 회복 지연 영향 극복하며 분기별 이익 회복 기대, 1일 장 마감 후 주요 종목뉴스</t>
+    <t>18년도 2분기 NDR Review: Step by Step,환율 영향에도 이머징 수익성 방어, 북미 인센티브 하향으로 손익 회복,우호적 환율, 유가상승, 신차 출시가 중국 회복 지연 영향 극복하며 분기별 이익 회복 기대, 1일 장 마감 후 주요 종목뉴스</t>
   </si>
   <si>
     <t>현대글로비스, ‘2차 개편’ 기대감에 주가 쑥쑥, 삼성전자SK하이닉스현대차…‘시총 빅5’의 8월은 ‘살얼음판 건너기’, 1일 장 마감 후 주요 종목뉴스</t>
@@ -4591,7 +4591,7 @@
     <t>시장 설득 가능한 '플랜B' 올해 안 발표...모비스 중심 틀은 변하지 않아</t>
   </si>
   <si>
-    <t>'가치투자 펀드' 美 캐피털그룹, SK하이닉스 지분 5% 확보, 美 캐피털그룹, SK하이닉스 주식 더 샀다, 현대차-금융마저 좋아진다,금융부문의 개선, 일회성이 아니다,미국 내 리스 손익 회복이 이어진다</t>
+    <t>'가치투자 펀드' 美 캐피털그룹, SK하이닉스 지분 5% 확보, 美 캐피털그룹, SK하이닉스 주식 더 샀다, 금융마저 좋아진다,금융부문의 개선, 일회성이 아니다,미국 내 리스 손익 회복이 이어진다</t>
   </si>
   <si>
     <t>엘리엇 지배구조 개편요구에 현대모비스와 현대차 주가 희비, 엘리엇매니지먼트, 현대차 지분 3% 들고 주가 상승을 노리다, 엘리엇, 지배구조 개편 재압박...희비 엇갈린 현대차그룹株, 엘리엇 지배구조 개편안 재압박...현대차그룹 계열사 주가 엇갈려, 막나가는 엘리엇…1차공격때 손해보자 주가띄우기 `무리수`, ‘자사주 매입의 힘’..엔씨소프트, 신작 부재에도 주가 쑥</t>
@@ -4651,22 +4651,22 @@
     <t>주식 부호 35인, 올해 지분 가치 8.5조↓…30대 이하, 지분 증여 혜택 '다이아몬드수저' 위력 발휘, 스튜어드십 코드에 따른 의결권 연대 행사 막아야</t>
   </si>
   <si>
-    <t>현대차-이종통화 약세로 지연된 실적 회복,18년도 3분기 영업이익은 9,880억원(-18.0% 전년 대비 증감율, OPM 4.0%)으로 컨센서스 5.6% 하회할 전망,中 부진 지속, 영업일수 감소에도 볼륨 선방했으나 이종통화 약세로 실적예상 하회, Hyundai Motor Company-Unfavorable FX slows down earnings recovery,18년도 3분기 영업이익은 9,880억원(-18.0% 전년 대비 증감율, OPM 4.0%)으로 컨센서스 5.6% 하회할 전망,中 부진 지속, 영업일수 감소에도 볼륨 선방했으나 이종통화 약세로 실적예상 하회, 현대차-신흥국 통화 약세로 3Q 하회할 듯,3Q 실적보다는 미국/중국 점유율 회복이 중요,18년도 3분기 Preview: 영업이익률 3.4% 전망, 시장심리 톱5, 삼성전자·현대차·삼성엔지니어링·KT·이마트</t>
-  </si>
-  <si>
-    <t>현대차-점차 중요해질 중국 대응전략,18년도 3분기 Preview - 신흥국 환율과 리콜 비용,점차 중요해질 중국 대응전략, 현대차-18년도 3분기 Preview: 부진한 실적 흐름 지속,이머징 통화 약세와 판매보증충당비용 증가,단기 대외 변수 비우호적, 부진한 주가 흐름 지속될 전망, “현대차 주식 매수 신중해야”, 하반기 실적전망 밝지 않아, '북미정상회담 지연'에 경협주 ‘추풍낙엽’...코스피 연중 최저치</t>
-  </si>
-  <si>
-    <t>현대차-년도년도 1분기 3분기 Preview: 단기부진,년도년도 1분기 3분기 Preview: 영업이익 9,180억원 (전년 대비 증감율 -23.8%) 예상,신흥국 노이즈 우려 지속불구, 미국/한국 판매증가로 년도년도 1분기 4분기 실적 개선, 현대차-현대차 Corporate Day Q&amp;A,내수시장 SUV (코나, 싼타페, 투싼 F/L) 중심 신차효과로 점유율 개선 지속 중,19년 쏘나타, G80, G90 F/L 출시를 통해 판매성장 전환 가능, 외국인 8일새 2.3조 팔아치워…"반등 장담못해", 뉴로스, 수소차 핵심 부품 공급 업체 부각-미래에셋대우</t>
-  </si>
-  <si>
-    <t>사흘만에 빗나간 코스피 10월 예상밴드...'내년 전망 어쩌지', 현대차-실적 가시성 회복 필요 (요약),글로벌 수요둔화 및 자동차산업 패러다임 변화에 따른 Valuation trap,3분기 Preview: 신흥국 통화약세 및 리콜비용 반영 영향으로 부진, 현대차-선전하는 곳에서 통화 약세, 전망 악화,3분기 실적 프리뷰: 이익 전망 악화,3분기 이후 실적 전망: 신흥국 통화 약세, 신차 효과 약화, HMC-Earnings visibility required,글로벌 수요둔화 및 자동차산업 패러다임 변화에 따른 Valuation trap,3분기 Preview: 신흥국 통화약세 및 리콜비용 반영 영향으로 부진, 현대차-실적 가시성 회복 필요,글로벌 수요둔화 및 자동차산업 패러다임 변화에 따른 Valuation trap,3분기 Preview: 신흥국 통화약세 및 리콜비용 반영 영향으로 부진</t>
+    <t>이종통화 약세로 지연된 실적 회복,18년도 3분기 영업이익은 9,880억원(-18.0% 전년 대비 증감율, OPM 4.0%)으로 컨센서스 5.6% 하회할 전망,中 부진 지속, 영업일수 감소에도 볼륨 선방했으나 이종통화 약세로 실적예상 하회, Hyundai Motor Company-Unfavorable FX slows down earnings recovery,18년도 3분기 영업이익은 9,880억원(-18.0% 전년 대비 증감율, OPM 4.0%)으로 컨센서스 5.6% 하회할 전망,中 부진 지속, 영업일수 감소에도 볼륨 선방했으나 이종통화 약세로 실적예상 하회, 신흥국 통화 약세로 3Q 하회할 듯,3Q 실적보다는 미국/중국 점유율 회복이 중요,18년도 3분기 Preview: 영업이익률 3.4% 전망, 시장심리 톱5, 삼성전자·현대차·삼성엔지니어링·KT·이마트</t>
+  </si>
+  <si>
+    <t>점차 중요해질 중국 대응전략,18년도 3분기 Preview - 신흥국 환율과 리콜 비용,점차 중요해질 중국 대응전략, 18년도 3분기 Preview: 부진한 실적 흐름 지속,이머징 통화 약세와 판매보증충당비용 증가,단기 대외 변수 비우호적, 부진한 주가 흐름 지속될 전망, “현대차 주식 매수 신중해야”, 하반기 실적전망 밝지 않아, '북미정상회담 지연'에 경협주 ‘추풍낙엽’...코스피 연중 최저치</t>
+  </si>
+  <si>
+    <t>년도년도 1분기 3분기 Preview: 단기부진,년도년도 1분기 3분기 Preview: 영업이익 9,180억원 (전년 대비 증감율 -23.8%) 예상,신흥국 노이즈 우려 지속불구, 미국/한국 판매증가로 년도년도 1분기 4분기 실적 개선, 현대차 Corporate Day Q&amp;A,내수시장 SUV (코나, 싼타페, 투싼 F/L) 중심 신차효과로 점유율 개선 지속 중,19년 쏘나타, G80, G90 F/L 출시를 통해 판매성장 전환 가능, 외국인 8일새 2.3조 팔아치워…"반등 장담못해", 뉴로스, 수소차 핵심 부품 공급 업체 부각-미래에셋대우</t>
+  </si>
+  <si>
+    <t>사흘만에 빗나간 코스피 10월 예상밴드...'내년 전망 어쩌지', 실적 가시성 회복 필요 (요약),글로벌 수요둔화 및 자동차산업 패러다임 변화에 따른 Valuation trap,3분기 Preview: 신흥국 통화약세 및 리콜비용 반영 영향으로 부진, 선전하는 곳에서 통화 약세, 전망 악화,3분기 실적 프리뷰: 이익 전망 악화,3분기 이후 실적 전망: 신흥국 통화 약세, 신차 효과 약화, HMC-Earnings visibility required,글로벌 수요둔화 및 자동차산업 패러다임 변화에 따른 Valuation trap,3분기 Preview: 신흥국 통화약세 및 리콜비용 반영 영향으로 부진, 실적 가시성 회복 필요,글로벌 수요둔화 및 자동차산업 패러다임 변화에 따른 Valuation trap,3분기 Preview: 신흥국 통화약세 및 리콜비용 반영 영향으로 부진</t>
   </si>
   <si>
     <t>10대 그룹 상장사 시총 10월에만 65조원 감소</t>
   </si>
   <si>
-    <t>국민연금 ‘공매도 작전’ 미스터리, 현대차-하반기 미국중심 점진적인 수익성 개선,9월 현대차 도매판매 영업일수 감소로 전년대비 -6.6% 감소,18년도 3분기 영업이익 시장 컨센서스 하회 예상</t>
+    <t>국민연금 ‘공매도 작전’ 미스터리, 하반기 미국중심 점진적인 수익성 개선,9월 현대차 도매판매 영업일수 감소로 전년대비 -6.6% 감소,18년도 3분기 영업이익 시장 컨센서스 하회 예상</t>
   </si>
   <si>
     <t>현대차·하이닉스 '맑음' LG화학·네이버 '흐림', "현대차 · 기아차 · 현대모비스 안심할 상황 아냐"...노무라, 시장심리 톱5, LG디스플레이·GS리테일·현대상선·LG이노텍·삼성중공업</t>
@@ -4687,16 +4687,16 @@
     <t>현대-11 왕자의 난과 현대그룹 분해, '시총 1.2조' 상장폐지…'꾼'은 웃었다, 맥빠진 코스피…상승 돌파구 찾을까</t>
   </si>
   <si>
-    <t>국민연금이 현대엘리베이터 선택한 이유, 국감서 화제된 미성년자 주식부자 “쌀 때 주면 세금 줄인다”…너도나도 증여 바람, 현대차-18년도 3분기 Preview - ASP 하락과 품질보증 관련 비용,투자의견 Buy 유지. 목표주가 140,000원으로 17.6% 하향,영업이익 8,183억원 (-32.0% 전년 대비 증감율) 예상. 시장 컨센서스 12.9% 하회 전망</t>
+    <t>국민연금이 현대엘리베이터 선택한 이유, 국감서 화제된 미성년자 주식부자 “쌀 때 주면 세금 줄인다”…너도나도 증여 바람, 18년도 3분기 Preview - ASP 하락과 품질보증 관련 비용,투자의견 Buy 유지. 목표주가 140,000원으로 17.6% 하향,영업이익 8,183억원 (-32.0% 전년 대비 증감율) 예상. 시장 컨센서스 12.9% 하회 전망</t>
   </si>
   <si>
     <t>수소차株 주가 널뛰기…`투자 주의보`</t>
   </si>
   <si>
-    <t>현대차그룹 시총 하루 새 3.6兆 증발, 어닝쇼크, 어떤 뜻일까? 예상보다 저조한 실적에 충격… 반댓말은 '어닝 서프라이즈', 현대차 3분기 영업이익 사상 처음 3천억 밑돌아…시장전망치 절반에도 못 미쳐 '어닝쇼크?', 현대자동차 2시의 악몽, 코스피·코스닥 날개없는 추락 中…투자자, 배당주로 옮겨가나, 최종식 대표 체제 쌍용자동차, 부채비율 55.4%p↑, 현대차-18년도 3분기 Review - 예상을 초과했던 품질비용,영업이익 2,889억원 (-76.0% 전년 대비 증감율) 시장 컨센서스 68.8% 하회,예상을 초과한 품질비용으로 영업이익 크게 감소, 현대차 지배구조 개편에도 악영향, 현대車 실적쇼크…영업익 8년새 최악, 10월 25일 주요공시, 현대차 3분기 실적부진 충격, 체력 약화 탓인가 기술 투자 때문인가, 현대차, 최악의 '실적 쇼크'…반도체도 "파티는 끝?", 성장 둔화, 증시급락...한국경제 먹구름 짙어졌다, 현대차 실적쇼크에 '망연자실', 분기 영업익 3000억원 붕괴(종합), '어닝쇼크'? 현대차 3분기 영업이익 3천억 밑돌아…사상처음 시장전망치 절반도 못 미쳐, 현대차 어닝쇼크…3분기 영업이익 76% 감소, 추락하는 것은 날개가 있다는데...코스피·코스닥 시장 하락 어쩌나</t>
-  </si>
-  <si>
-    <t>현대차-환율 영향에 더한 품질비용 증가로 어닝쇼크,18년도 3분기 영업이익 2,889억원을 기록하며 예상을 크게 하회,이머징 통화 약세에 따른 실적 부진에 더해 대규모 품질비용 발생까지 겹쳤음, Hyundai Motor-All negatives reflected in the earnings shock,3분기 영업이익 2,889억원(-76.0%)으로 시장 기대치 대폭 하회 ？,일회성 비용과 업황 둔화의 이중고, 현대차-불신이 키운 비용,대규모 품질비용과 환율 영향으로 어닝쇼크,품질비용이 커진 이유는 뿌리깊은 불신,환율 감안 TP 5% 하향, 단 미국 회복 지속, 4Q 실적 정상화, 현대차-품질비용이 초래한 실적 쇼크,매출 24,434십억원(전년 대비 증감율+1.0%), OP 289십억원(전년 대비 증감율-76.0%, OPM 1.2%) 지배순익 269십억원(전년 대비 증감율-68.4%, NIM 1.1%) 기록하며 어닝 쇼크 기록,非우호적 환율과 품질관련 비용이 차량 사업부 적자전환 배경, 현대차-년도년도 1분기 3분기 Review: 반복되는 리콜 비용의 늪,년도년도 1분기 3분기 Review: 일회성 리콜 비용으로 시장 기대치 대폭 하회,반복되는 리콜 비용의 늪, 일회성 이슈?, 현대차-어닝쇼크, 그 이후의 과제,대규모 대외변수 비용 발생으로 18년도 3분기 Earning Shock 기록,앞으로의 관건, 1) 품질 이슈 지속 여부, 2) 판매실적 개선 여부, 3) 배당, 현대차-실적 쇼크 요인 해소에 시간이 필요,3분기 실적 리뷰 : 어닝쇼크,3분기 이후 실적 전망 : 신흥국 위기, 품질비용 부담 지속, 현대차-리콜확산 선제대응으로 실적부진하나 배당정책 유지,18년도 3분기 영업이익은 2,889억원(-76.0% 전년 대비 증감율, OPM 1.2%) 기록, 컨센서스 68.8% 하회,품질관련 일회성비용(5,000억원), 이종통화 약세(2,500억원), 영업일수 감소 영향, 현대차-어닝쇼크, 판매보증비용과 신흥국 통화 약세 영향,3Q 18 Review: 예상치 못한 2017년 엔진리콜 비용 추가 반영,4분기 북미지역 개선 여부가 중요한 시점, 현대차-품질강화비용으로 실적 쇼크,3분기 어닝 쇼크요인 두가지, 품질강화비용과 신흥국 통화불안 영향, Hyundai Motor-Earnings shock on sales guarantees and weak emerging currencies,3Q 18 Review: 예상치 못한 2017년 엔진리콜 비용 추가 반영,4분기 북미지역 개선 여부가 중요한 시점, 현대차-년도년도 1분기 3분기 Review: 체력저하와 방향성 부재,년도년도 1분기 3분기 실적은 신흥시장환율 상승 및 품질비용 확대로 쇼크 기록,연간 배당 4천원 유지는 긍정적이나, 2012년 이후 지속된 품질비용 증가, 높은 글로벌 재고, 중국실적 부진을 감안할 때 영업현금흐름 개선은 지연될 전망, 저성장의 늪 깊어지는데… 정부 위기의식이 없다, 미국發 리스크…공포의 ‘블랙 데이' 이달만 세 번째, 이건희·홍라희 부부와 세 자녀. 이달들어 지분가치 3조4200억 증발, 현대차-방향성 확인 필요,18년도 3분기 , Shock,18년도 4분기 실적은 반등,배당은 바닥 근거 일뿐, 방향성 확인 필요, 현대차-예상치 못했던 큰 충격,18년도 3분기 Review-예상치 못했던 큰 충격,18년도 4분기 Preview-증익은 가능하다, 현대차-모든 악재를 반영한 쇼크,3분기 영업이익 2,889억원(-76.0%)으로 시장 기대치 대폭 하회 ？,일회성 비용과 업황 둔화의 이중고, 현대차-품질 비용과 신흥국 통화 약세가 원인,3Q 하회. 4Q 개선. 향후 미국/중국 신차 성과가 중요,18년도 3분기 Review: 영업이익률 1.2% 기록, 현대차-년도년도 1분기 3분기 Review: 어쨌든 부진한 실적,년도년도 1분기 3분기 Review: 영업이익 2,889억원 (전년 대비 증감율 -76%)으로 컨센 대폭 하회,미국과 신흥국은 개선세를 띄기 시작하나 추가 리콜우려 여전히 존재, 현대차-기대감의 선반영보다 확인이 필요한 시기,18년도 3분기 Review ? 예상을 넘어선 일회성비용,기대감의 선반영보다 확인 이후 대응을 권고, 현대차-18년도 3분기 리뷰: 예상외 일회성 비용 반영,털고 갈 것은 털고 가야지만 품질비용은 지속 증가 중</t>
+    <t>현대차그룹 시총 하루 새 3.6兆 증발, 어닝쇼크, 어떤 뜻일까? 예상보다 저조한 실적에 충격… 반댓말은 '어닝 서프라이즈', 현대차 3분기 영업이익 사상 처음 3천억 밑돌아…시장전망치 절반에도 못 미쳐 '어닝쇼크?', 현대자동차 2시의 악몽, 코스피·코스닥 날개없는 추락 中…투자자, 배당주로 옮겨가나, 최종식 대표 체제 쌍용자동차, 부채비율 55.4%p↑, 18년도 3분기 Review - 예상을 초과했던 품질비용,영업이익 2,889억원 (-76.0% 전년 대비 증감율) 시장 컨센서스 68.8% 하회,예상을 초과한 품질비용으로 영업이익 크게 감소, 현대차 지배구조 개편에도 악영향, 현대車 실적쇼크…영업익 8년새 최악, 10월 25일 주요공시, 현대차 3분기 실적부진 충격, 체력 약화 탓인가 기술 투자 때문인가, 현대차, 최악의 '실적 쇼크'…반도체도 "파티는 끝?", 성장 둔화, 증시급락...한국경제 먹구름 짙어졌다, 현대차 실적쇼크에 '망연자실', 분기 영업익 3000억원 붕괴(종합), '어닝쇼크'? 현대차 3분기 영업이익 3천억 밑돌아…사상처음 시장전망치 절반도 못 미쳐, 현대차 어닝쇼크…3분기 영업이익 76% 감소, 추락하는 것은 날개가 있다는데...코스피·코스닥 시장 하락 어쩌나</t>
+  </si>
+  <si>
+    <t>환율 영향에 더한 품질비용 증가로 어닝쇼크,18년도 3분기 영업이익 2,889억원을 기록하며 예상을 크게 하회,이머징 통화 약세에 따른 실적 부진에 더해 대규모 품질비용 발생까지 겹쳤음, Hyundai Motor-All negatives reflected in the earnings shock,3분기 영업이익 2,889억원(-76.0%)으로 시장 기대치 대폭 하회 ？,일회성 비용과 업황 둔화의 이중고, 불신이 키운 비용,대규모 품질비용과 환율 영향으로 어닝쇼크,품질비용이 커진 이유는 뿌리깊은 불신,환율 감안 TP 5% 하향, 단 미국 회복 지속, 4Q 실적 정상화, 품질비용이 초래한 실적 쇼크,매출 24,434십억원(전년 대비 증감율+1.0%), OP 289십억원(전년 대비 증감율-76.0%, OPM 1.2%) 지배순익 269십억원(전년 대비 증감율-68.4%, NIM 1.1%) 기록하며 어닝 쇼크 기록,非우호적 환율과 품질관련 비용이 차량 사업부 적자전환 배경, 년도년도 1분기 3분기 Review: 반복되는 리콜 비용의 늪,년도년도 1분기 3분기 Review: 일회성 리콜 비용으로 시장 기대치 대폭 하회,반복되는 리콜 비용의 늪, 일회성 이슈?, 어닝쇼크, 그 이후의 과제,대규모 대외변수 비용 발생으로 18년도 3분기 Earning Shock 기록,앞으로의 관건, 1) 품질 이슈 지속 여부, 2) 판매실적 개선 여부, 3) 배당, 실적 쇼크 요인 해소에 시간이 필요,3분기 실적 리뷰 : 어닝쇼크,3분기 이후 실적 전망 : 신흥국 위기, 품질비용 부담 지속, 리콜확산 선제대응으로 실적부진하나 배당정책 유지,18년도 3분기 영업이익은 2,889억원(-76.0% 전년 대비 증감율, OPM 1.2%) 기록, 컨센서스 68.8% 하회,품질관련 일회성비용(5,000억원), 이종통화 약세(2,500억원), 영업일수 감소 영향, 어닝쇼크, 판매보증비용과 신흥국 통화 약세 영향,3Q 18 Review: 예상치 못한 2017년 엔진리콜 비용 추가 반영,4분기 북미지역 개선 여부가 중요한 시점, 품질강화비용으로 실적 쇼크,3분기 어닝 쇼크요인 두가지, 품질강화비용과 신흥국 통화불안 영향, Hyundai Motor-Earnings shock on sales guarantees and weak emerging currencies,3Q 18 Review: 예상치 못한 2017년 엔진리콜 비용 추가 반영,4분기 북미지역 개선 여부가 중요한 시점, 년도년도 1분기 3분기 Review: 체력저하와 방향성 부재,년도년도 1분기 3분기 실적은 신흥시장환율 상승 및 품질비용 확대로 쇼크 기록,연간 배당 4천원 유지는 긍정적이나, 2012년 이후 지속된 품질비용 증가, 높은 글로벌 재고, 중국실적 부진을 감안할 때 영업현금흐름 개선은 지연될 전망, 저성장의 늪 깊어지는데… 정부 위기의식이 없다, 미국發 리스크…공포의 ‘블랙 데이' 이달만 세 번째, 이건희·홍라희 부부와 세 자녀. 이달들어 지분가치 3조4200억 증발, 방향성 확인 필요,18년도 3분기 , Shock,18년도 4분기 실적은 반등,배당은 바닥 근거 일뿐, 방향성 확인 필요, 예상치 못했던 큰 충격,18년도 3분기 Review-예상치 못했던 큰 충격,18년도 4분기 Preview-증익은 가능하다, 모든 악재를 반영한 쇼크,3분기 영업이익 2,889억원(-76.0%)으로 시장 기대치 대폭 하회 ？,일회성 비용과 업황 둔화의 이중고, 품질 비용과 신흥국 통화 약세가 원인,3Q 하회. 4Q 개선. 향후 미국/중국 신차 성과가 중요,18년도 3분기 Review: 영업이익률 1.2% 기록, 년도년도 1분기 3분기 Review: 어쨌든 부진한 실적,년도년도 1분기 3분기 Review: 영업이익 2,889억원 (전년 대비 증감율 -76%)으로 컨센 대폭 하회,미국과 신흥국은 개선세를 띄기 시작하나 추가 리콜우려 여전히 존재, 기대감의 선반영보다 확인이 필요한 시기,18년도 3분기 Review ? 예상을 넘어선 일회성비용,기대감의 선반영보다 확인 이후 대응을 권고, 18년도 3분기 리뷰: 예상외 일회성 비용 반영,털고 갈 것은 털고 가야지만 품질비용은 지속 증가 중</t>
   </si>
   <si>
     <t>현대자동차 3분기 ‘어닝 쇼크’ 어떻게 봐야 할까요?, 요동치는 금융시장...한국 경제 적신호, 주가는 폭락하고, 기름값은 치솟고…우울한 지표만 가득했던 한주</t>
@@ -4705,7 +4705,7 @@
     <t>행동주의 헤지펀드에 멍드는 한국기업들, 비관론 고개드는 韓 증시…투자심리가 변수</t>
   </si>
   <si>
-    <t>‘검은 10월’ 시총 261조 증발…코스피 2000 깨지나, 대외 악재에 기업 실적부진까지 겹친 韓증시, ‘어닝 쇼크’ 현대차, 눈높이 낮추는 증권가, 증선위의 삼성바이오로직스 회계처리 현명한 판단이 기대되는 이유, 현대차-실적 신뢰도 회복에 시간이 필요 (요약),2019년 자동차 업황 불확실성 지속,3분기 Review - 품질비용 증가와 신흥국 통화약세 영향, HMC-Time needed to regain earnings visibility,2019년 자동차 업황 불확실성 지속,3분기 Review - 품질비용 증가와 신흥국 통화약세 영향, 현대차-실적 신뢰도 회복에 시간이 필요,2019년 자동차 업황 불확실성 지속,3분기 Review - 품질비용 증가와 신흥국 통화약세 영향, 금춘수 한화그룹 부회장</t>
+    <t>‘검은 10월’ 시총 261조 증발…코스피 2000 깨지나, 대외 악재에 기업 실적부진까지 겹친 韓증시, ‘어닝 쇼크’ 현대차, 눈높이 낮추는 증권가, 증선위의 삼성바이오로직스 회계처리 현명한 판단이 기대되는 이유, 실적 신뢰도 회복에 시간이 필요 (요약),2019년 자동차 업황 불확실성 지속,3분기 Review - 품질비용 증가와 신흥국 통화약세 영향, HMC-Time needed to regain earnings visibility,2019년 자동차 업황 불확실성 지속,3분기 Review - 품질비용 증가와 신흥국 통화약세 영향, 실적 신뢰도 회복에 시간이 필요,2019년 자동차 업황 불확실성 지속,3분기 Review - 품질비용 증가와 신흥국 통화약세 영향, 금춘수 한화그룹 부회장</t>
   </si>
   <si>
     <t>증권사, 현대글로비스 3분기 실적 '긍정적'…4분기 '안정' 전망, 文대통령, 북한보다 경제 챙기란 신호, &lt;사설&gt;證市 추락 더 부추기는 경제정책 헛발질, 어닝쇼크 뜻은 무엇? 일명 '실적 충격'…예상보다 저조한 실적 발표, 반댓말은 '어닝 서프라이즈', 코스피 2000선 붕괴…‘컨틴전시 플랜’ 가동되나</t>
@@ -4729,7 +4729,7 @@
     <t>현대차_거래비중 기관 37.07%, 외국인 46.94%, "한때 투톱이었는데" 현대차 시총 10위권도 위태, TheCapitalGroupCompanies,Inc. 외, 현대차 지배구조 훼방놨던 엘리엇, 최대 3천억 손실...손절매할까</t>
   </si>
   <si>
-    <t>더캐피탈그룹, 현대차 줄이고 SK하이닉스 늘리고, 현대차-Downside보다는 Upside를 고민할 시기, 저성장·경쟁심화 환경 속 신차효과 만을 통한 과거 수준으로의 높은 이익 개선은 불가능, 그럼에도 불구하고 이제 Downside보다는 Upside를 논할 시기, 19년 국내 및 미국공장의 가동률 개선과 인센티브 감소를 통해 17년 수준의 이익 회복은 가능할 전망</t>
+    <t>더캐피탈그룹, 현대차 줄이고 SK하이닉스 늘리고, Downside보다는 Upside를 고민할 시기, 저성장·경쟁심화 환경 속 신차효과 만을 통한 과거 수준으로의 높은 이익 개선은 불가능, 그럼에도 불구하고 이제 Downside보다는 Upside를 논할 시기, 19년 국내 및 미국공장의 가동률 개선과 인센티브 감소를 통해 17년 수준의 이익 회복은 가능할 전망</t>
   </si>
   <si>
     <t>"현대제철 주식 사도 된다", 투자회수 통해 주주친화정책 강화 기대, 지배구조 개편의 히든카드 현대엔지니어링, 되레 정의선 부회장 발목 잡나?, 상장사 3분기 실적 ‘뚝’… 목표주가 하향 쏟아져</t>
@@ -4741,7 +4741,7 @@
     <t>文 대통령 신남방 행보…이번주(12~16일) 주요일정</t>
   </si>
   <si>
-    <t>현대차-현대차 글로벌 판매 점검, 매출 24.4조(전년 대비 증감율 +1.0%), 영업이익률 1.2%, 당사 컨센서스 OPM 3.7% 하회, 북미 1)세타 엔진, 2)엔진 센서, 3)에어백 관련 리콜 비용 5천억 반영, 일회성 비용 제외 시 정상 영업이익은 8천억 추정, OPM 3.5%, 현대차-실적에 대한 가시성 축소, 미국 싼타페 신차모멘텀은 기대치를 하회, 중국 역시 지속적인 걸림돌이 될 것, 낮아진 어닝 모멘텀으로 눈높이를 낮출 수 밖에 없는 국면, 투자의견 BUY 유지하나, 목표주가 130,000원으로 하향, 문 대통령, 이번주 아세안·APEC 참석…‘新남방정책’ 가속</t>
+    <t>현대차 글로벌 판매 점검, 매출 24.4조(전년 대비 증감율 +1.0%), 영업이익률 1.2%, 당사 컨센서스 OPM 3.7% 하회, 북미 1)세타 엔진, 2)엔진 센서, 3)에어백 관련 리콜 비용 5천억 반영, 일회성 비용 제외 시 정상 영업이익은 8천억 추정, OPM 3.5%, 실적에 대한 가시성 축소, 미국 싼타페 신차모멘텀은 기대치를 하회, 중국 역시 지속적인 걸림돌이 될 것, 낮아진 어닝 모멘텀으로 눈높이를 낮출 수 밖에 없는 국면, 투자의견 BUY 유지하나, 목표주가 130,000원으로 하향, 문 대통령, 이번주 아세안·APEC 참석…‘新남방정책’ 가속</t>
   </si>
   <si>
     <t>현대차, 장 중 10만원 붕괴…위기의 끝이 안 보인다, "현대차 과도한 자본 보유"...엘리엇, 자사주 매입 요구</t>
@@ -4762,10 +4762,10 @@
     <t>삼성바이오로직스와 경영권…총수일가 기업의 사유화</t>
   </si>
   <si>
-    <t>현대차-쉬어 가는 타이밍, 기대에 미치지 못했던 2018년, 2019년, 쉬어 가는 타이밍, 제네시스 회복을 기다리며, 한진칼, ‘한국형 엘리엇’ 첫 사례 될까, 막 내린 미국 중간선거…한국 증시 미칠 영향은</t>
-  </si>
-  <si>
-    <t>'트럭·버스 위기' 현대차, 3년 만에 수출 반토막, ②행동주의 펀드, 약탈자와 천사 사이, "현대차 주식 사도 돤다", 미국과 중국에서 내년 판매 개선 가능, 현대차, 9년만에 10만원선 아래로 떨어져, 현대차 주가, 9년 만에 '10만원선 붕괴'...실적 부진 탓, 현대차-미워도 다시 한번, 2019년 어려운 경영환경, 일정부분 회복기조 전망, 최근 품질강화비용은 고육지책이지만 나름 현명한 대처, 투자의견 매수와 목표주가 14만원 유지</t>
+    <t>쉬어 가는 타이밍, 기대에 미치지 못했던 2018년, 2019년, 쉬어 가는 타이밍, 제네시스 회복을 기다리며, 한진칼, ‘한국형 엘리엇’ 첫 사례 될까, 막 내린 미국 중간선거…한국 증시 미칠 영향은</t>
+  </si>
+  <si>
+    <t>'트럭·버스 위기' 현대차, 3년 만에 수출 반토막, ②행동주의 펀드, 약탈자와 천사 사이, "현대차 주식 사도 돤다", 미국과 중국에서 내년 판매 개선 가능, 현대차, 9년만에 10만원선 아래로 떨어져, 현대차 주가, 9년 만에 '10만원선 붕괴'...실적 부진 탓, 미워도 다시 한번, 2019년 어려운 경영환경, 일정부분 회복기조 전망, 최근 품질강화비용은 고육지책이지만 나름 현명한 대처, 투자의견 매수와 목표주가 14만원 유지</t>
   </si>
   <si>
     <t>“000은 누구 겁니까”…트위터· 다스· 비자금·스위스 계좌까지, 갈팡질팡 코스피…'마라톤주'로 달려라</t>
@@ -4780,13 +4780,13 @@
     <t>10대 그룹 상장사, 올해 시총 195조원 증발… 현대차그룹 29.4%↓, 정의선 수석부회장 ‘현대엔지니어링 카드’ 꺼내나, 10대그룹 상장사 시가총액이 1년만에 190조원↓, 10대 그룹 상장사, 올해 시총 195조 '증발'…주식시장 300조↓ 패닉, 현대차_거래비중 기관 28.66%, 외국인 41.33%, 10대 그룹 상장사 시가총액 '195조' 증발…증시도 300조 감소</t>
   </si>
   <si>
-    <t>'방탄소년단 테마주' 대부분 올라, 지엠피 급등하고 디피씨 급락, 현대차-제품의 힘을 믿는다, SUV 차종 보강: 소형 및 대형고급 SUV 추가로 라인업 완전 구비, 19년도 하반기 : 리콜과 지배구조개편이라는 Noise 영향, 투자의견: BUY, 목표주가 13만원 유지, 대기업 SI업체 상장 러시…왜 이제서야?, IT서비스기업, '음지'서 '양지'로…재계 성장동력 될까, 현대차_거래비중 기관 28.38%, 외국인 41.27%, 현대차 주가 쌍끌이 매수로 6%대 급등, 기아차 현대모비스도 강세, 모처럼…외국인, 코스피에 2000억 쐈다</t>
-  </si>
-  <si>
-    <t>대기업 SI계열사, 잇단 IPO 추진 ‘왜?’, ‘행동주의 투자자’ 입김 세진다, 트럼프發 '자동차 관세폭탄' 결국 터지나, “우리나라 기업가치 안 오르는 이유? 지배주주가 돈 빼돌리기 때문”, 현대차-2019년 전망: 반전의 열쇠는 현대차에게 있다, 글로벌 수요 정체 상황에서, 국내 중소부품사의 유동성위기 및 최저임금 상승 영향으로 재료비 증가 불가피. C.A.S.E로 대변되는 산업패러다임 변화는 가속화되고 있음, 생산능력 및 세단라인업의 Downsizing과 그룹의 사업구조 재편이 동시에 진행되어야 하며, 그룹 내에서 결정권한을 가지고 있는 회사는 현대차, Value Chain의 유동성위기와 최저임금 인상에 따른 재료비 상승 가능성을 반영하여 수익추정을 하향하고 목표주가를 125,000원으로 7.4%하향, 주진형 “오르지 않는 기업가치? 재벌총수가 돈 빼돌리기 때문”, 車→인터넷→화장품株…연말 '순환매 장세'</t>
-  </si>
-  <si>
-    <t>車부품주 줄줄이 하락…증권가에 부는 현대·기아괴담, 현대차-미 법무부의 쎄타 엔진 리콜 조사로 품질 비용에 대한 불확실성이 극대화되며 주가 전 저점 아래로, 단 펀더멘털 관점에서 미국 내 재고조정 마무리 되며 공장 가동률 상승, 이에 따라 손익이 개선되는 점은 긍정적, 글로벌 자동차 수요가 둔화되나 SUV 비중 확대와 신형 엔진 탑재 확산도 본격화 되면서 점유율은 회복, 정의선 부회장의 수석부회장 승진에 따라 리더십 공백도 정상화될 전망</t>
+    <t>'방탄소년단 테마주' 대부분 올라, 지엠피 급등하고 디피씨 급락, 제품의 힘을 믿는다, SUV 차종 보강: 소형 및 대형고급 SUV 추가로 라인업 완전 구비, 19년도 하반기 : 리콜과 지배구조개편이라는 Noise 영향, 투자의견: BUY, 목표주가 13만원 유지, 대기업 SI업체 상장 러시…왜 이제서야?, IT서비스기업, '음지'서 '양지'로…재계 성장동력 될까, 현대차_거래비중 기관 28.38%, 외국인 41.27%, 현대차 주가 쌍끌이 매수로 6%대 급등, 기아차 현대모비스도 강세, 모처럼…외국인, 코스피에 2000억 쐈다</t>
+  </si>
+  <si>
+    <t>대기업 SI계열사, 잇단 IPO 추진 ‘왜?’, ‘행동주의 투자자’ 입김 세진다, 트럼프發 '자동차 관세폭탄' 결국 터지나, “우리나라 기업가치 안 오르는 이유? 지배주주가 돈 빼돌리기 때문”, 2019년 전망: 반전의 열쇠는 현대차에게 있다, 글로벌 수요 정체 상황에서, 국내 중소부품사의 유동성위기 및 최저임금 상승 영향으로 재료비 증가 불가피. C.A.S.E로 대변되는 산업패러다임 변화는 가속화되고 있음, 생산능력 및 세단라인업의 Downsizing과 그룹의 사업구조 재편이 동시에 진행되어야 하며, 그룹 내에서 결정권한을 가지고 있는 회사는 현대차, Value Chain의 유동성위기와 최저임금 인상에 따른 재료비 상승 가능성을 반영하여 수익추정을 하향하고 목표주가를 125,000원으로 7.4%하향, 주진형 “오르지 않는 기업가치? 재벌총수가 돈 빼돌리기 때문”, 車→인터넷→화장품株…연말 '순환매 장세'</t>
+  </si>
+  <si>
+    <t>車부품주 줄줄이 하락…증권가에 부는 현대·기아괴담, 미 법무부의 쎄타 엔진 리콜 조사로 품질 비용에 대한 불확실성이 극대화되며 주가 전 저점 아래로, 단 펀더멘털 관점에서 미국 내 재고조정 마무리 되며 공장 가동률 상승, 이에 따라 손익이 개선되는 점은 긍정적, 글로벌 자동차 수요가 둔화되나 SUV 비중 확대와 신형 엔진 탑재 확산도 본격화 되면서 점유율은 회복, 정의선 부회장의 수석부회장 승진에 따라 리더십 공백도 정상화될 전망</t>
   </si>
   <si>
     <t>현대차 자사주 277만 주 매입 추진, 재계 '투톱' 삼성·현대차, 자사주 매입·소각…왜?(종합), 삼성전자 자사주 소각하고 현대차는 매입한다, 현대차, 자사주 277만주 매입한다…2500억원 규모, 현대차, 자사주 매입으로 ‘주주가치 제고’, '주주가치 제고' 현대차, 2547억원 규모 277만주 자사주 매입 추진, 현대자동차, 자사주 277만주 매입 추진…"주가 안정화 의지 표명", 현대차, 277만주 자사주 매입… "주주가치 제고 노력 일환", 삼성전자·현대차 각각 자사주 소각·매입…“주주가치 제고”, 현대차, 2547억원 규모 277만주 자사주 매입, 현대차 277만주 자사주 매입 "주가 안정화 의지", 현대차 "주주환원 정책 강화" 자사주 277만주 매입…주가 상승, 주주가치 높인다…삼성전자는 자사주 소각·현대차는 매입, 삼성·현대차, 자사주 소각하고 매입하고…주주가치 제고 나서, 현대차, “2500억원 상당” 자사주 277만주 매입, 현대차, 2547억 규모 자사주 매입…"주주가치 제고 목적", 현대자동차, 자사주 277만주 매입…주주가치 제고, 현대차, 277만주 자사주 매입…“주주가치 제고 차원”, 현대차, 팰리세이드 사전계약·자사주 매입에 급등...주가 반등 시그널?, 현대차, 2500억원 규모 자사주 매입 소식에 주가 10만원대 '회복', 현대차, 자사주 ‘277만주’ 매입···“주주가치 제고 일환”, 10~11월 증시 폭락장 개미들 이렇게 망했다, 현대차, 2500억 규모 자사주 277만주 대거 매입…"주가안정화 의지", 현대차, ‘2500억원’ 투입해 자사주 매입 추진… 주주가치 제고 조치, 현대車는 자사주 매입에 주가 급등, 주가 부양 나선 삼성전자·현대車…악재 털어낼까?, 현대차 주가부양 나섰지만 효과 내기 위해 갈 길은 '험난', 현대차, 277만주 사들여 주가 안정 노린다, 삼성전자·현대차 자사주 소각·매입·…“주주가치 제고위한 것”, 현대차, 자사주 277만주 매입한다..총 2547억원 규모, 삼성전자 현대차 일제히 자사주 소각 매입..."주주가치 제고", 주주가치 제고나선 재계 1, 2위…삼성전자는 자사주 ‘태우고’ 현대차는 ‘사들이고’, 현대차 "277만주 자사주 매입, 주주가치 제고 노력 일환", 현대차 자사주 227만주 매입 '주주가치 제고·주주환원 정책 강화', 현대자동차, 2500억원 자사주 277만주 매입 추진, "자사주 사고, 소각하고"…삼성·현대차 주가부양 나선 이유, '팰리세이드·제네시스 G90' 업은 현대차 자사주 277만주 매입, 현대차, 2500억 규모 자사주 매입 추진…"주주가치 제고할 것", 현대차 자사주 277만주 매입 "주주가치 제고 노력 일환", 삼성전자 자사주 5억3000만 소각, 경고장 보내는 주주들…고민 커지는 상장사, 삼성전자는 자사주 소각, 현대차는 매입...주주가치 높이기, 현대차, 자사주 277만주 취득…'주가 안정화 의지'(상보), 현대차, 자사주 277만주 매입…"주가 안정화 의지 표현", 현대차, 주주가치 제고 위해 자사주 277만주 매입, 현대차, 자사주 277만주 매입 "주주가치 제고 노력 일환", 현대차 자사주 277만주 매입 "주주가치 제고 일환", 현대차, 277만주 자사주 매입 “주주가치 높이기 노력”, 현대차, 2500억원 규모 자사주 취득 결정, 현대車, 자사주 277만株 산다…"주주가치 높일 것", 현대차 2547억원 자사주 매입 "주주가치 제고할 것", 현대차, 주가 안정 위해 자사주 2500억어치 매입 결정, 현대차, 자사주 277만주 대거 매입 "투자자들에 주가안정화 의지 강조", 현대차, 자사주 277만주 취득…'주주가치 제고', 현대자동차, 2547억원 규모 자사주 취득 결정, 현대차 277만주 자사주 매입… “주주가치 제고 노력 일환”, 현대차, 2500억원 규모 자사주 취득 결정에 강세, 현대자동차, 자사주 취득 결정, 현대차, 자사주 277만주 취득 결정, 현대차 277만주 자사주 매입…“주주가치 제고 일환”, 현대차, “주주 가치 제고” 자사주 277만주 약 2,500억원에 매입, 현대차, 자사주 277만주 매입…"주주가치 제고 노력 일환", 현대차, 자사주 276만주 매입…"주가 안정화·주주가치 제고", 현대차, 자사주 277만주 매입..."주주가치 제고 노력", “주주가치 제고” 현대차는 자사주 매입ㆍ삼성전자는 소각, 현대차, 2500억원 규모 자사주 매입…"주주 가치 제고", '277만주 자사주 매입' 현대차 "주주가치 제고 노력 일환", 현대차, 자사주 277만주 매입 "주주가치 높이겠다", 현대차, 277만주 자사주 매입…"주주가치 제고", 현대차, 2500억원 규모 자사주 매입 추진, 현대차, 자사주 277만주 취득결정, 현대차, 277만주 자사주 매입…"주주가치 제고 노력 일환", 현대차, 2500억 규모 자사주 277만주 매입 추진... "주주가치 제고", 삼성전자 ‘소각’·현대차 ‘매입’…“주주가치 제고”, 현대차 자사주 277만주 매입...주주환원정책 강화, 현대차, 2500억원 규모 자사주 276만주 매입…"주가 안정화·주주가치 제고", 현대차 277만주 자사주 매입…“주주가치 제고 노력 일환”, 현대차, 자사주 277만주 매입 나선다… “주주가치 제고”, 현대차, '주주가치 제고' 자사주 277만주 매입 "2500억 규모", 현대차 자사주 277만주 매입 “주주가치 제고 일환”, 현대차, 자사주 277만주 매입 추진..."주주가치 제고"</t>
@@ -4801,7 +4801,7 @@
     <t>현대차의 선별적 협력사 지원, 못 받는 부품사가 수두룩, 현대자동차 자사주 매입 또 발표...효과는?, 12월 3일 주요공시, 기업들의 현금과 배당에 주목할 때, 외국인 현대차 매집에 “리콜 영향 제한적”, 최단기간 부자되려면 나이키 커브를 찾아라</t>
   </si>
   <si>
-    <t>현대차-해외에서도 ASP는 올릴 수 있어야 한다, 무엇으로 인해 수익성이 하락했나, 어떻게 해야 수익성이 회복할까, 2019년 세단과 SUV에서 플래그쉽 모델이 본격적으로 출시, '단기 미봉책'에 그칠 수도, 삼성·현대차 자사주 매입 괜찮나, 대기업 오너 일가 ‘가족경영’의 명과 암, 잇단 재벌 IT업체 IPO에 "흥행은 글쎄"</t>
+    <t>해외에서도 ASP는 올릴 수 있어야 한다, 무엇으로 인해 수익성이 하락했나, 어떻게 해야 수익성이 회복할까, 2019년 세단과 SUV에서 플래그쉽 모델이 본격적으로 출시, '단기 미봉책'에 그칠 수도, 삼성·현대차 자사주 매입 괜찮나, 대기업 오너 일가 ‘가족경영’의 명과 암, 잇단 재벌 IT업체 IPO에 "흥행은 글쎄"</t>
   </si>
   <si>
     <t>현대차, 주가부양 나섰지만···'노조 총파업' 악재에 골머리, 잇단 재벌 IT업체 IPO에 "흥행은 글쎄"</t>
@@ -4882,16 +4882,16 @@
     <t>정부 수소차 육성계획에 도내 수소차 관련주 급등, CES 개막 D-2…증권가, 첨단 신기술 관심 '고조'</t>
   </si>
   <si>
-    <t>이재용·최태원·서경배…주가폭락에 체면구긴 회장님들, 현대차-18년도 4분기 Preview, Buy 유지, TP 145,000원으로 상향</t>
+    <t>이재용·최태원·서경배…주가폭락에 체면구긴 회장님들, 18년도 4분기 Preview, Buy 유지, TP 145,000원으로 상향</t>
   </si>
   <si>
     <t>한일 CEO 절반, 양국관계 부정적 전망, 'GBC 승인'·실적상승 현대차, 'V'자 반등 '시동'</t>
   </si>
   <si>
-    <t>반도체 호황 꺾였는데… 美 3대 자산운용사 '더캐피탈', SK하이닉스 주식 또 샀다, 휘청이는 재계, 정치 공세까지 이중고 빠져, 현대차-신차 투입으로 원가율 상승, 수익성 개선 부담, 18년도 4분기 영업이익은 6,778억원(-12.6% 전년 대비 증감율, OPM 2.6%) 기록, 컨센서스 23.0% 하회, 자동차 RV 믹스 개선에도 美 인센티브 하락 효과 이연, 이종통화 약세, 신차 투입으로 원가율 상승 부담, 현대차-년도년도 1분기 4분기 Preview: 3분기 쇼크를 딛고 회복세로 전환, 년도년도 1분기 4분기 Preview: 3분기 쇼크를 딛고 회복세로 전환, SUV 신차 판매 호조, 이머징 시장 통화 약세</t>
-  </si>
-  <si>
-    <t>현대차-4Q 하회 예상. 상반기 신차 사이클 기대, 일시적 실적 하회는 1분기부터 해소 가능, 18년도 4분기 Preview: 영업이익률 2.7% 예상, 상반기 강화되는 신차 사이클 주목</t>
+    <t>반도체 호황 꺾였는데… 美 3대 자산운용사 '더캐피탈', SK하이닉스 주식 또 샀다, 휘청이는 재계, 정치 공세까지 이중고 빠져, 신차 투입으로 원가율 상승, 수익성 개선 부담, 18년도 4분기 영업이익은 6,778억원(-12.6% 전년 대비 증감율, OPM 2.6%) 기록, 컨센서스 23.0% 하회, 자동차 RV 믹스 개선에도 美 인센티브 하락 효과 이연, 이종통화 약세, 신차 투입으로 원가율 상승 부담, 년도년도 1분기 4분기 Preview: 3분기 쇼크를 딛고 회복세로 전환, 년도년도 1분기 4분기 Preview: 3분기 쇼크를 딛고 회복세로 전환, SUV 신차 판매 호조, 이머징 시장 통화 약세</t>
+  </si>
+  <si>
+    <t>4Q 하회 예상. 상반기 신차 사이클 기대, 일시적 실적 하회는 1분기부터 해소 가능, 18년도 4분기 Preview: 영업이익률 2.7% 예상, 상반기 강화되는 신차 사이클 주목</t>
   </si>
   <si>
     <t>대한민국 경제의 미래를 책임질 4人4色 | “공격적·글로벌·변화 추구형 CEO, 소탈함과 孝心이 공통점”</t>
@@ -4903,13 +4903,13 @@
     <t>한국의 자동차산업 : 베드 뉴스와 굿 뉴스, "시장 뒤흔들 대형 악재 가능성 당분간 없어…낙폭 컸던 철강·화학·금융株 눈여겨볼 만"</t>
   </si>
   <si>
-    <t>어닝쇼크, 현대차-수소차 돌풍의 주역, 수소차와 전기차 Two-Track 전략, 2019년부터 본격화, 현대차가 수소차에 베팅하는 이유: 결국은 공유경제의 패권, 2019년 실적은 상저하고 패턴, 그리고 증익, 투자의견 BUY 유지, 목표주가 145,000원 유지, 현대차-CES 2019: 모빌리티 혁신 고도화 전략 발표, 커넥티드, 전동화, 오픈이노베이션 중심의 전략 구체화, 전략에서 언급된 향후 주요 변화/기대 요인, 파격적인 전략은 아니지만, 그래도 반가운 변화, 현대차-영업 레버리지의 발현을 기다리며, 본격적인 RV 중심 신차 Cycle 개시로 가동률 · 재고 · 인센티브 정상화 진행 중, 19년도 1분기 이후 본격적인 영업 레버리지 효과 발현 전망, 적정주가 140,000원 유지</t>
-  </si>
-  <si>
-    <t>현대차-단기실적보다 중요한 19 년 실적방향성, 18년도 4분기 Preview-비용반영으로 기대치 하회 전망, 단기실적보다 중요한 19 년 수익성 전망, "현대 · 기아차, 올해 신차출시로 실적 모멘텀 개선 기대", 정몽구 회장, 주가 하락에도 상장사 주식부호 5위 유지, 코웨이 품에 안자 靑초청도...웅진그룹 위상 강화, '운전기사 갑질 논란' 대림 이해욱, 회장 승진과 청와대 모임 제외의 남다른 의미</t>
-  </si>
-  <si>
-    <t>그들은 왜 행동주의 투자자들의 타깃이 됐나, 현대차-년도년도 1분기 4분기 프리뷰: 기나긴 밤의 끝, 년도년도 1분기 4분기 Preview: 시장 기대치 하회 전망, 2019년 전망: SUV 라인업 보강 및 제네시스 반격 시작</t>
+    <t>어닝쇼크, 수소차 돌풍의 주역, 수소차와 전기차 Two-Track 전략, 2019년부터 본격화, 현대차가 수소차에 베팅하는 이유: 결국은 공유경제의 패권, 2019년 실적은 상저하고 패턴, 그리고 증익, 투자의견 BUY 유지, 목표주가 145,000원 유지, CES 2019: 모빌리티 혁신 고도화 전략 발표, 커넥티드, 전동화, 오픈이노베이션 중심의 전략 구체화, 전략에서 언급된 향후 주요 변화/기대 요인, 파격적인 전략은 아니지만, 그래도 반가운 변화, 영업 레버리지의 발현을 기다리며, 본격적인 RV 중심 신차 Cycle 개시로 가동률 · 재고 · 인센티브 정상화 진행 중, 19년도 1분기 이후 본격적인 영업 레버리지 효과 발현 전망, 적정주가 140,000원 유지</t>
+  </si>
+  <si>
+    <t>단기실적보다 중요한 19 년 실적방향성, 18년도 4분기 Preview-비용반영으로 기대치 하회 전망, 단기실적보다 중요한 19 년 수익성 전망, "현대 · 기아차, 올해 신차출시로 실적 모멘텀 개선 기대", 정몽구 회장, 주가 하락에도 상장사 주식부호 5위 유지, 코웨이 품에 안자 靑초청도...웅진그룹 위상 강화, '운전기사 갑질 논란' 대림 이해욱, 회장 승진과 청와대 모임 제외의 남다른 의미</t>
+  </si>
+  <si>
+    <t>그들은 왜 행동주의 투자자들의 타깃이 됐나, 년도년도 1분기 4분기 프리뷰: 기나긴 밤의 끝, 년도년도 1분기 4분기 Preview: 시장 기대치 하회 전망, 2019년 전망: SUV 라인업 보강 및 제네시스 반격 시작</t>
   </si>
   <si>
     <t>IBK투자 “하림지주, 사업확장…종합식품회사로 발돋움 할 것 ”, ④본게임 들어가기 전에 체력방전, "현대차, 올해 턴어라운드 여부 주목"...CS, &lt;포럼&gt;국민연금 주주권 유일 기준은 수익률, "하림지주, 한국판 카길이 되기 위한 담금질", 국민연금, 총수 일가 견제 현실화… 경영 개입 ‘관치’ 부작용도</t>
@@ -4933,10 +4933,10 @@
     <t>IT 다음은 車·유통…덜 오른 실적개선주 '찜', 주식시장 부진 우려…IPO 공모기업, 스스로 '몸값' 하향 조정, 지코, 수소 전기차용 연료펌프 개발 완료..현대차 납품대기중, 하림지주 - 사업 확장 시너지 효과 기대·매수 목표가 16000원</t>
   </si>
   <si>
-    <t>현대차-년도년도 1분기 4분기 Revie-판매 믹스 개선에도 마진은 축소, 현대차 년도년도 1분기 4분기 잠정 영업이익 5,011억원 (-35.4% 전년 대비 증감율) ? 시장 컨센서스 하회, 기타사업부문 적자 전환이 영업이익 감소의 주된 원인, 판매 증가와 믹스 개선에도 자동차 부문 영업이익은 감소, 현대차-년도년도 1분기 4분기 Review: 국내공장 영업적자의 의미, 년도년도 1분기 4분기 실적은 분기 사상최대 매출에도 로템의 2천억원 적자, 금융부분 부진으로 쇼크. 순이익은 개발비 조기상각, 지분법 대상법인 손상차손 반영, 법인세 추징 등으로 적자전환. 실적부진에도 연간 배당 4천원 유지는 긍정적, 한편, 국내공장은 가동률 117%에도 영업적자 900억원을 기록, 2개분기 연속 적자. 이는 가동률과 수익성의 상관관계가 깨졌음을 의미, 현대차 주가 롤러코스터, 실적 발표에 급락했다가 상승 반전, "실적 최악인데"…현대차놓고 고민에 빠진 펀드매니저들</t>
-  </si>
-  <si>
-    <t>새해 활기 띠는 IPO시장…올해 눈여겨 볼 공모주는?, 현대차-4Q 실적 바닥. 신차 사이클과 지배구조 개선, 상반기에 집중된 모멘텀, 18년도 4분기 Review: 영업이익률 2.0% 기록, 컨퍼런스 콜의 주요 내용: 2019년 도매판매 +2% 목표, 현대차-주가는 기대감을 선반영, 관건은 무역확장법, 18년도 4분기 매출 25,670십억원(전년 대비 증감율+4.8%), OP 501십억원(전년 대비 증감율-35.4%, OPM%) 지배순익, 실적 개선세는 기대 요인이나 이미 주가에 선반영 된 상황, 현대차-결국 신차, 18년도 4분기 , 시장기대치 하회, 여전히 어려운 영업 환경, 결국 신차, 현대차-일회성의 향연, 일회성 비용 집중으로 영업이익 컨센서스 38% 하회, 비정상의 정상화 지속, 실적회복 이어질 전망, 상반기까지의 실적회복 미국이 주도, 이후의 회복은 원가절감을 중심으로, 현대차-실적보다 방향성, 4분기 영업이익 5,011억원(-35.4%)으로 시장 기대치를 36.8% 하회, 관건은 자동차 부문의 회복 지속과 일회성 비용의 소멸, 목표주가 165,000원(+10.0%)으로 상향, 투자의견 매수 유지, 현대차-주가는 기대감을 선반영, 관건은 무역확장법, 18년도 4분기 매출 25,670십억원(전년 대비 증감율+4.8%), OP 501십억원(전년 대비 증감율-35.4%, OPM%) 지배순익, 실적 개선세는 기대 요인이나 이미 주가에 선반영 된 상황, 현대차-년도년도 1분기 4분기 Review: 자세히 보면 나쁘지 않은 실적, 년도년도 1분기 4분기 Review: 금융/기타 부문 부진과 일회성 비용 발생으로 당기순이익 적자 전환, 자세히 보면 나쁘지 않은 실적, 2019년 실적 개선 전망 유효, 상승 추세 유지할 전망, 현대차-다사다난했던 18년을 넘어, 다양한 비용 이슈로 점철됐던 18 년, 4 분기 실적 또한 같은 흐름 속에서 부진. 다만, 자동차 부문 실적 회복 시작됐으며, 비자동차 비용들을 배제한 손익은 기대치 근접, 최근 주가 흐름 부정적 이슈에 둔감해지고 긍정적 이슈에 민감, 이는 그 무엇보다 가동률, 재고, 인센티브와 같은 핵심 영업지표가 빠르게 회복세로 전환됐기 때문, 향후 이들 영업지표의 지속적인 개선 추이를 전망하며, 기업가치는 이에 동행할 예정. 19 년 이익 추정치를 +5.5% 조정하며, 적정주가를 15 만원으로 상향, 현대차-일회성의 향연, 일회성 비용 집중으로 영업이익 컨센서스 38% 하회, 비정상의 정상화 지속, 실적회복 이어질 전망, 상반기까지의 실적회복 미국이 주도, 이후의 회복은 원가절감을 중심으로, 현대차-낮아진 기저 뒤 회복될 2019년, 18년도 4분기 영업이익은 5,011억원(-35.4% 전년 대비 증감율, OPM 2.0%) 기록, 컨센서스 36.8% 하회, 자동차부문 영업이익 4,630억원(OPM 2.3%) 회복세애도 연결자회사 현대로템 2,129억 - 자동차부문 영업이익 4,630억원(OPM 2.3%) 회복세애도 연결자회사 현대로템 2,129억원 영업손실, 금융 일회성 급여비용(300억원) 등 비자동차부문 실적 악화로 하회, 현대차-기타부문 실적부진으로 컨센서스 하회, 4Q 18 Review: 기타부문의 실적쇼크와 자동차금융부문 수익성 악화, 2019년 글로벌 판매량 468만대(전년 대비 증감율+2.0%), 질적 성장 기대, 목표주가 15만원 및 투자의견 매수 유지, 현대차-Misses consensus on weak “other” results, 18년도 4분기 review: “other” earnings shock and worse auto and finance profitability, 2019E global sales volume 4.68mn (+2.0% 전년 대비 증감율); qualitative growth likely, 현대차-긍정과 부담의 혼재, 18년도 4분기 Review - 자동차부문 회복 vs 금융/기타부문의 부진, 긍정과 부담의 혼재, 현대차-2019년, 쏘나타가 Key Model, 장기실적 전망 신뢰도 상승이 주가 상승의 필요조건, 4분기 Review - 일회성 요인과 구조적 요인 혼재</t>
+    <t>년도년도 1분기 4분기 Revie-판매 믹스 개선에도 마진은 축소, 현대차 년도년도 1분기 4분기 잠정 영업이익 5,011억원 (-35.4% 전년 대비 증감율) ? 시장 컨센서스 하회, 기타사업부문 적자 전환이 영업이익 감소의 주된 원인, 판매 증가와 믹스 개선에도 자동차 부문 영업이익은 감소, 년도년도 1분기 4분기 Review: 국내공장 영업적자의 의미, 년도년도 1분기 4분기 실적은 분기 사상최대 매출에도 로템의 2천억원 적자, 금융부분 부진으로 쇼크. 순이익은 개발비 조기상각, 지분법 대상법인 손상차손 반영, 법인세 추징 등으로 적자전환. 실적부진에도 연간 배당 4천원 유지는 긍정적, 한편, 국내공장은 가동률 117%에도 영업적자 900억원을 기록, 2개분기 연속 적자. 이는 가동률과 수익성의 상관관계가 깨졌음을 의미, 현대차 주가 롤러코스터, 실적 발표에 급락했다가 상승 반전, "실적 최악인데"…현대차놓고 고민에 빠진 펀드매니저들</t>
+  </si>
+  <si>
+    <t>새해 활기 띠는 IPO시장…올해 눈여겨 볼 공모주는?, 4Q 실적 바닥. 신차 사이클과 지배구조 개선, 상반기에 집중된 모멘텀, 18년도 4분기 Review: 영업이익률 2.0% 기록, 컨퍼런스 콜의 주요 내용: 2019년 도매판매 +2% 목표, 주가는 기대감을 선반영, 관건은 무역확장법, 18년도 4분기 매출 25,670십억원(전년 대비 증감율+4.8%), OP 501십억원(전년 대비 증감율-35.4%, OPM%) 지배순익, 실적 개선세는 기대 요인이나 이미 주가에 선반영 된 상황, 결국 신차, 18년도 4분기 , 시장기대치 하회, 여전히 어려운 영업 환경, 결국 신차, 일회성의 향연, 일회성 비용 집중으로 영업이익 컨센서스 38% 하회, 비정상의 정상화 지속, 실적회복 이어질 전망, 상반기까지의 실적회복 미국이 주도, 이후의 회복은 원가절감을 중심으로, 실적보다 방향성, 4분기 영업이익 5,011억원(-35.4%)으로 시장 기대치를 36.8% 하회, 관건은 자동차 부문의 회복 지속과 일회성 비용의 소멸, 목표주가 165,000원(+10.0%)으로 상향, 투자의견 매수 유지, 주가는 기대감을 선반영, 관건은 무역확장법, 18년도 4분기 매출 25,670십억원(전년 대비 증감율+4.8%), OP 501십억원(전년 대비 증감율-35.4%, OPM%) 지배순익, 실적 개선세는 기대 요인이나 이미 주가에 선반영 된 상황, 년도년도 1분기 4분기 Review: 자세히 보면 나쁘지 않은 실적, 년도년도 1분기 4분기 Review: 금융/기타 부문 부진과 일회성 비용 발생으로 당기순이익 적자 전환, 자세히 보면 나쁘지 않은 실적, 2019년 실적 개선 전망 유효, 상승 추세 유지할 전망, 다사다난했던 18년을 넘어, 다양한 비용 이슈로 점철됐던 18 년, 4 분기 실적 또한 같은 흐름 속에서 부진. 다만, 자동차 부문 실적 회복 시작됐으며, 비자동차 비용들을 배제한 손익은 기대치 근접, 최근 주가 흐름 부정적 이슈에 둔감해지고 긍정적 이슈에 민감, 이는 그 무엇보다 가동률, 재고, 인센티브와 같은 핵심 영업지표가 빠르게 회복세로 전환됐기 때문, 향후 이들 영업지표의 지속적인 개선 추이를 전망하며, 기업가치는 이에 동행할 예정. 19 년 이익 추정치를 +5.5% 조정하며, 적정주가를 15 만원으로 상향, 일회성의 향연, 일회성 비용 집중으로 영업이익 컨센서스 38% 하회, 비정상의 정상화 지속, 실적회복 이어질 전망, 상반기까지의 실적회복 미국이 주도, 이후의 회복은 원가절감을 중심으로, 낮아진 기저 뒤 회복될 2019년, 18년도 4분기 영업이익은 5,011억원(-35.4% 전년 대비 증감율, OPM 2.0%) 기록, 컨센서스 36.8% 하회, 자동차부문 영업이익 4,630억원(OPM 2.3%) 회복세애도 연결자회사 현대로템 2,129억 - 자동차부문 영업이익 4,630억원(OPM 2.3%) 회복세애도 연결자회사 현대로템 2,129억원 영업손실, 금융 일회성 급여비용(300억원) 등 비자동차부문 실적 악화로 하회, 기타부문 실적부진으로 컨센서스 하회, 4Q 18 Review: 기타부문의 실적쇼크와 자동차금융부문 수익성 악화, 2019년 글로벌 판매량 468만대(전년 대비 증감율+2.0%), 질적 성장 기대, 목표주가 15만원 및 투자의견 매수 유지, Misses consensus on weak “other” results, 18년도 4분기 review: “other” earnings shock and worse auto and finance profitability, 2019E global sales volume 4.68mn (+2.0% 전년 대비 증감율); qualitative growth likely, 긍정과 부담의 혼재, 18년도 4분기 Review - 자동차부문 회복 vs 금융/기타부문의 부진, 긍정과 부담의 혼재, 2019년, 쏘나타가 Key Model, 장기실적 전망 신뢰도 상승이 주가 상승의 필요조건, 4분기 Review - 일회성 요인과 구조적 요인 혼재</t>
   </si>
   <si>
     <t>10대 그룹 총수 성장주식 가치 8.3% 오른 30조원, 현대차, 영업익 악화에도 주가 '꿋꿋'…정의선 체제 효과, 총수 상장주식 가치 2위 정몽구 4300억 증가, 1위는?, 현대차, 작년 실적 급감...영업익 2조4222억, 올해 10대 그룹 총수 상장사 주식자산 2조원 증가, 총수 상장사 주식자산 증가 정몽구·이건희·김승연 순, 중국 의존도 높은 한국 증시의 한계</t>
@@ -4945,7 +4945,7 @@
     <t>"현대모비스 주식 사도 된다", 현대차 신차 출시의 수혜, 오토에버 상장승인…현대차 `일석이조`, 기업가치 제고로 포장된 먹튀…선진국형 지배구조가 해법&lt;上&gt;, "고배당을 원한다면 ㅇㅇㅇ주식을 사라"…5대그룹 계열사 주식배당 현황 살펴보니</t>
   </si>
   <si>
-    <t>“현대차 주식 매수 신중해야”, 수소차 투자로 장기적 부담 안아, “현대모비스 주식 매수 신중해야”, 수소전기차 투자 부담 커, 시끌벅적 물류산업, 증권가 주요 이슈는…, 하림지주_상장주식수 대비 거래량은 0.18%로 적정수준, 현대차-수소전기차 선도적 투자, 난제 많아 부담, 수소전기차 중장기 로드맵 발표, 일본보다 앞서가는 투자, 수소전기차 대규모 투자는 부담 요인</t>
+    <t>“현대차 주식 매수 신중해야”, 수소차 투자로 장기적 부담 안아, “현대모비스 주식 매수 신중해야”, 수소전기차 투자 부담 커, 시끌벅적 물류산업, 증권가 주요 이슈는…, 하림지주_상장주식수 대비 거래량은 0.18%로 적정수준, 수소전기차 선도적 투자, 난제 많아 부담, 수소전기차 중장기 로드맵 발표, 일본보다 앞서가는 투자, 수소전기차 대규모 투자는 부담 요인</t>
   </si>
   <si>
     <t>현대오토에버, 지배구조 개편 신호탄, 현대오토에버 상장 시동…현대차 지배구조 개편 2막 돌입?, "수소차 멀었다"...개미 향한 한화證 일침</t>
@@ -4969,10 +4969,10 @@
     <t>수소차 테마주 ‘쑥쑥’...엇갈리는 증권가 전망, 정재훈 플랫폼파트너스자산운용 대표</t>
   </si>
   <si>
-    <t>현대차-정부와 업계 선투자로 수소차 대중화 가능성 상승, 2018년 품질비용 등으로 실적 악화, 2019년 가동률과 믹스 개선으로 실적 턴어라운드 기대, 투자의견 매수와 목표주가 16만원 유지, "신차 들어온다"…이노션 주가 '훨훨', 디스플레이 장비주 中 저평가 1위는 디아이티. 왜?</t>
-  </si>
-  <si>
-    <t>현대자동차, 특별관계자 지분변동, “현대모비스 주식 사도 된다”, 친환경차 핵심부품 올해 높은 성장, TheCapitalGroupCompanies,Inc. 외, 효성중공업 SK가스 주가 급등, 수소충전소 규제 샌드박스 효과, 현대차-미래기술 선도 업체로 도약, 수소차 투자 확대, 미래기술 선도 업체로 도약, 친환경차 포트폴리오 강화 = 수익성 개선</t>
+    <t>정부와 업계 선투자로 수소차 대중화 가능성 상승, 2018년 품질비용 등으로 실적 악화, 2019년 가동률과 믹스 개선으로 실적 턴어라운드 기대, 투자의견 매수와 목표주가 16만원 유지, "신차 들어온다"…이노션 주가 '훨훨', 디스플레이 장비주 中 저평가 1위는 디아이티. 왜?</t>
+  </si>
+  <si>
+    <t>현대자동차, 특별관계자 지분변동, “현대모비스 주식 사도 된다”, 친환경차 핵심부품 올해 높은 성장, TheCapitalGroupCompanies,Inc. 외, 효성중공업 SK가스 주가 급등, 수소충전소 규제 샌드박스 효과, 미래기술 선도 업체로 도약, 수소차 투자 확대, 미래기술 선도 업체로 도약, 친환경차 포트폴리오 강화 = 수익성 개선</t>
   </si>
   <si>
     <t>현대글로비스, 주당 3300원 배당 결정…정의선 부회장 288억원, 규제 샌드박스 선정에 수혜주 ‘주목’...투자 유의 지적도</t>
@@ -4987,7 +4987,7 @@
     <t>자화전자 - 2019년 턴어라운드·목표가 18000원 유지, 올해 증시 지루한 박스권…스튜어드십코드·행동주의 업고 가치주 뜬다</t>
   </si>
   <si>
-    <t>엠에스오토텍, 왜 '헤지펀드'로 자금조달하나, 현대오토에버 증권신고서 제출, 자금 1500억 조달 예상, 현대차-19년도 1분기 실적보다 8세대 Sonata 상품성에 주목, 투자의견 Buy 유지. 목표주가 150,000원으로 7.1% 상향, 년도년도 1분기 4분기 영업이익 5,011억원 (-35.4% 전년 대비 증감율) - 시장 컨센서스 36.8% 하회, 년도년도 1분기 4분기 자동차 부문 영업이익 전년동기대비 10.8% 감소, 3월 출시 8세대 Sonata의 상품성이 19년도 2분기 및 2019년 영업이익에 큰 영향 미칠 것</t>
+    <t>엠에스오토텍, 왜 '헤지펀드'로 자금조달하나, 현대오토에버 증권신고서 제출, 자금 1500억 조달 예상, 19년도 1분기 실적보다 8세대 Sonata 상품성에 주목, 투자의견 Buy 유지. 목표주가 150,000원으로 7.1% 상향, 년도년도 1분기 4분기 영업이익 5,011억원 (-35.4% 전년 대비 증감율) - 시장 컨센서스 36.8% 하회, 년도년도 1분기 4분기 자동차 부문 영업이익 전년동기대비 10.8% 감소, 3월 출시 8세대 Sonata의 상품성이 19년도 2분기 및 2019년 영업이익에 큰 영향 미칠 것</t>
   </si>
   <si>
     <t>현대오토에버 상장 잰걸음…현대차그룹 계열사 교통정리 '속도', "주식 투자 타이밍?…공포와 혐오가 겹칠 때", 현대오토에버 상장 성공해도…정의선 선택 따라 주가 방향 달라질 듯</t>
@@ -5005,7 +5005,7 @@
     <t>탤런트 박순애씨, 수소차 덕에 연예인 주식부자 5위, 수소차 테마주 급등…배우 박순애 연예인 부호 5위, 오너 재선임·경영권 분쟁…기업들 '주총 속앓이', '수소차 대박' 연예인 주식부자 5위에 탤런트 박순자씨</t>
   </si>
   <si>
-    <t>① 구광모 웃고 이재용·정의선 울었다, 현대차-Top Pick 으로 변경. 볼륨 cycle 의 최대 수혜주, 18년도 4분기 Review: 영업이익 5,021 억원 (전년 대비 증감율 -35%)으로 컨센서스 하회, 2019 년 전반적인 그림의 변화: 증익, 신차, 지배구조, 제네시스 브랜드 효과 본격화, 미국판매량 2020 년에는 4 만대 넘어설 것, 업종내 최선호주. 최근의 주가조정은 밸류에이션 메리트 제공</t>
+    <t>① 구광모 웃고 이재용·정의선 울었다, Top Pick 으로 변경. 볼륨 cycle 의 최대 수혜주, 18년도 4분기 Review: 영업이익 5,021 억원 (전년 대비 증감율 -35%)으로 컨센서스 하회, 2019 년 전반적인 그림의 변화: 증익, 신차, 지배구조, 제네시스 브랜드 효과 본격화, 미국판매량 2020 년에는 4 만대 넘어설 것, 업종내 최선호주. 최근의 주가조정은 밸류에이션 메리트 제공</t>
   </si>
   <si>
     <t>현대차, 이사회 전문성·다양성·투명성 강화, 현대차, 1조1천억 배당 통해 주주가치 제고…배당성향 70.7% 육박, 손실 본 엘리엇의 무리수, "현대차·모비스 8조 배당하라", 정의선 부회장, 3월 주총서 현대차 신임 대표이사 취임…혁신 리더십 강화, '명실상부'한 정의선 시대 열린다, 엘리엇매니지먼트, 현대차 주식 손실을 고배당으로 만회 시도, 엘리엇, 이번엔 8.3조 배당 요구…현대차그룹 '정면돌파', 현대차, 정의선 대표이사 선임…'정의선 시대' 날개단다, '본색'드러낸 엘리엇, 수조원 배당 요구 '논란', 엘리엇, 현대차그룹에 7조 배당 요구... 현대차 "받아들일 수 없는 요구", 현대차·모비스 주주에 '毒 사과' 제안한 엘리엇, '엘리엇의 무리수'..현대차에 작년 순익 353% 배당 요구, 엘리엇, 현대차 고배당·사외이사 압박··· 주가하락에 '생떼부리기' 제안, 현대차, 총 ‘1兆’ 배당 책정···주주가치 제고 방침, 현대차, 실적부진에도 1.1조 배당…배당성향 70.7% 육박, 국민연금 칼바람에 알아서 배당 늘리는 재계, 현대차, 보통주 1주당 기말배당 3000원 추진…주주가치↑, 정의선 수석부회장, 현대차 대표이사 선임된다, 정의선, 기아차 사내이사 이어 현대차 대표이사 맡는다, 현대차, 정의선 수석부회장 신규 대표이사 선임 추진, 현대차,이사회 전문성·다양성·투명성 강화…주주 및 시장 친화적 배당 지속, 현대차, 이사회 전문성·다양성·투명성 강화…'선진 경영' 구축, 현대차, 영업실적 부진 불구 1조 원 배당, '책임경영 '정의선 부회장, 모비스 이어 현대차 대표이사 선임, 현대차, ‘책임 경영’ 강화..정의선 수석부회장 대표이사 선임 추진, 현대차, 정의선 대표이사·외국인 사내이사 첫 선임 등 이사회 선진화, 현대차 이사회, 정의선 수석부회장 신규 '대표이사' 선임 추진, 현대차, 정의선 수석부회장 대표이사 선임 추진, 정의선 "현대차 대표이사 된다"…주주가치 제고안 발표, 현대자동차, 정의선 수석부회장 신규 대표이사 선임 추진…이사회 전문성·다양성·투명성 강화, 현대차_주가와 투자심리는 약세, 거래량은 침체</t>
@@ -5014,7 +5014,7 @@
     <t>'정의선 효과'…현대차·모비스 동반 상승, 현대차그룹주, 추가 주주환원 정책에 강세, 엘리엇, 현대차에 5조8000억 배당 '무리수' 요구, 정의선, 현대차 '대관식'의 불청객 엘리엇매니지먼트 어떻게 할까, 표집결 나선 엘리엇, 현대모비스 주주에 공개서신, 엘리엇의 반격 “현대차그룹, 초과 자본금 환원해라”…주주제안 서신공개, 엘리엇매니지먼트, 현대차 현대모비스 일반주주 결집할 수 있나, 엘리엇의 요구, 탐욕은 선한 것인가?, 현대차그룹 압박나선 엘리엇...증권가 “지배구조 개편 시급해”, 현대차그룹株, 대규모 주주친화 정책 발표에 장 초반 강세, 현대차 등골 뽑겠다는 엘리엇, 멍석 깔아주려는 정부·여당, 엘리엇 투기본색…“현대차, 작년 순익 3.5배 배당하라”, 현대차 무리한 배당소식에 총수일가 '배불리기' 비난 고조, 엘리엇 투기 본색…“현대차, 작년 순익 3.5배 배당하라”, 하나금융투자 “현대모비스, 주주가치 제고 방안 긍정적”, 현대차그룹주, '정의선 체제'로 그룹 개편 추진에 강세, 투기자본의 도 넘은 기업 흔들기… 현대차 “미래 투자 발목 잡아”, “현대모비스 주식은 업종 최선호주”, 선진적 경영체계 도입 긍정적, 현대차 경영 주도하는 정의선부회장, '실질 투명경영 체제' 확보, 롯데정보통신 약진에 정의선 부회장 미소짓는 까닭, '원톱' 정의선, 입사 20년 만에 현대차 대표 맡는다, 현대차, 이사회 중심 '주주가치 경영시스템' 구축, 엘리엇, 현대차·모비스에 과도한 배당 요구한 이유는?</t>
   </si>
   <si>
-    <t>현대차, 주주환원 기대에도 하락…주총 표 대결 '주목', 현대차-CEO 컨퍼런스 후기, 현대차 CEO 간담회를 통한 중장기 비전과 목표 제시, 주주환원 정책은 기존 계획 지속, 지속경영 가능한 유동성 유지가 중요, 수익성 개선의 필수조건은 브랜드 회복, 주력 모델의 흥행 여부에 주목, 현대차-CEO Investor Day: 천리길도 한걸음, 1시간 반 이상 진행된 본 행사에서 이원희 대표이사는 투자가들에게 현대차의 중장기 수익목표 및 투자계획을 발표, 영업이익은 ‘19년 4%을 시작으로 ‘2022년 7%까지 매년 1% 포인트씩 올리고 ROE는 ‘22년 9% 수준의 목표를 제시, 현대차-CEO Investor Day, 향후 5개년 중장기 투자 로드맵 제시, 경영진 목표: 수익성 개선, 주주환원정책 제시, 현대차-중장기 수익성 목표 제시 긍정적, 중장기 경영전략과 경영 목표 제시, 달라진 점, 현대차-중장기 경영전략과 경영진 목표를 발표, 경쟁력 강화의 핵심은 SUV와 고급차, 그리고 미래기술 확대, 경영진 목표로 2022년 자동차 부문 OPM 7%, ROE 9% 제시, 비전 제시를 통해 주주 동의를 구하려는 의지, 현대차-중장기 수익성 및 경영전략 발표. 시장과의 소통강화 시작, 현대차 CEO Investor Day 진행, 중장기 수익성 및 경영전략 발표하며 시장과의 소통강화 시작, SUV및 고급차 확대, 상품성 강화 신차, 미래대응력 강화 계획, 22년까지 7%OPM, 9% ROE, R&amp;D와 미래기술 45조 투자, 수익성 개선을 기반으로 한 주주환원 정책 지속 예정, 미래 제시, 현대차 vs 주총서 '목줄' 쥐려는 엘리엇…주주 판단은, 현대차-본업 회복과 미래 대응의지 확인, 현대차는 2월 27일 CEO Investor Day를 통해 중장기 재무 목표와 R&amp;D/투자 계획, 기술 로드맵 공유, 중장기 경영전략(사업 경쟁력 고도화, 미래 대응력 강화, 경영 조직 혁신)과 경영 목표(수익성 개선, 주주 환원 강화, 유동성 등 재무구조 가이던스)가 주요 내용. 정의선 수석부회장 책임경영 하의 주주 요구에 맞춘 유휴 현금의 활용(주주친화정책, 투자 로드맵)과 방향성(경영 전략)을 제시했다는 점 긍정적, 현대차-OPM 7% 회복의 관건은 GENESIS와 친환경차, 현대자동차, CEO Investor Day 개최, 현대차-중장기 경영전략: 22년 영업이익률 7% 목표, 수익성 개선 전략 추진을 통해 ‘22년 영업이익률 7%, ROE 9% 달성 목표, 원가절감과 판매비용 개선, (현장에서)기업을 흔드는 외국 투기자본, 현대차-이제 말이 통한다, 처음으로 열린 CEO Investor Day 주요 내용, 질의응답 주요 내용, 달라진 현대차의 소통방법 및 내용에 주목, 엘리엇, 현대자동차 주주들에 신임 이사 선임·특별 배당 제안 서신 발송, 국내 증시 '결렬' 쇼크…남북 경협주 20% 안팎 급락, 엘리엇, 모비스 이어 현대차 주주에도 지지호소 서신, 엘리엇 어깃장에 떠밀리듯 진화 나선 현대차, 현대차-모비스와 달리 ‘정공법’을 선택, CEO 간담회에서 제시된 Elliott 주주제안에 대한 현대차의 대응 방안은 새로운 주주환원 정책이 아닌 실적개선이라는 정공법 (당사 추정 및 시장 기대를 상회하는 가이던스 제시), 한전부지 매입과 장기화된 실적악화로 신뢰상실의 문제를 겪고 있는 현대차, 단기 배당에 높은 가중치를 두는 기조가 주류가 된다면 주총을 앞두고 주가 급등락 가능, 그러나 주주제안 충돌을 넘어 주총을 마친다면, 향후 기업가치 방향성은 결국 실적개선이라는 본질과 동행할 예정. 19년 실적은 중장기 실적 가이던스의 바로미터</t>
+    <t>현대차, 주주환원 기대에도 하락…주총 표 대결 '주목', CEO 컨퍼런스 후기, 현대차 CEO 간담회를 통한 중장기 비전과 목표 제시, 주주환원 정책은 기존 계획 지속, 지속경영 가능한 유동성 유지가 중요, 수익성 개선의 필수조건은 브랜드 회복, 주력 모델의 흥행 여부에 주목, CEO Investor Day: 천리길도 한걸음, 1시간 반 이상 진행된 본 행사에서 이원희 대표이사는 투자가들에게 현대차의 중장기 수익목표 및 투자계획을 발표, 영업이익은 ‘19년 4%을 시작으로 ‘2022년 7%까지 매년 1% 포인트씩 올리고 ROE는 ‘22년 9% 수준의 목표를 제시, CEO Investor Day, 향후 5개년 중장기 투자 로드맵 제시, 경영진 목표: 수익성 개선, 주주환원정책 제시, 중장기 수익성 목표 제시 긍정적, 중장기 경영전략과 경영 목표 제시, 달라진 점, 중장기 경영전략과 경영진 목표를 발표, 경쟁력 강화의 핵심은 SUV와 고급차, 그리고 미래기술 확대, 경영진 목표로 2022년 자동차 부문 OPM 7%, ROE 9% 제시, 비전 제시를 통해 주주 동의를 구하려는 의지, 중장기 수익성 및 경영전략 발표. 시장과의 소통강화 시작, 현대차 CEO Investor Day 진행, 중장기 수익성 및 경영전략 발표하며 시장과의 소통강화 시작, SUV및 고급차 확대, 상품성 강화 신차, 미래대응력 강화 계획, 22년까지 7%OPM, 9% ROE, R&amp;D와 미래기술 45조 투자, 수익성 개선을 기반으로 한 주주환원 정책 지속 예정, 미래 제시, 현대차 vs 주총서 '목줄' 쥐려는 엘리엇…주주 판단은, 본업 회복과 미래 대응의지 확인, 현대차는 2월 27일 CEO Investor Day를 통해 중장기 재무 목표와 R&amp;D/투자 계획, 기술 로드맵 공유, 중장기 경영전략(사업 경쟁력 고도화, 미래 대응력 강화, 경영 조직 혁신)과 경영 목표(수익성 개선, 주주 환원 강화, 유동성 등 재무구조 가이던스)가 주요 내용. 정의선 수석부회장 책임경영 하의 주주 요구에 맞춘 유휴 현금의 활용(주주친화정책, 투자 로드맵)과 방향성(경영 전략)을 제시했다는 점 긍정적, OPM 7% 회복의 관건은 GENESIS와 친환경차, 현대자동차, CEO Investor Day 개최, 중장기 경영전략: 22년 영업이익률 7% 목표, 수익성 개선 전략 추진을 통해 ‘22년 영업이익률 7%, ROE 9% 달성 목표, 원가절감과 판매비용 개선, (현장에서)기업을 흔드는 외국 투기자본, 이제 말이 통한다, 처음으로 열린 CEO Investor Day 주요 내용, 질의응답 주요 내용, 달라진 현대차의 소통방법 및 내용에 주목, 엘리엇, 현대자동차 주주들에 신임 이사 선임·특별 배당 제안 서신 발송, 국내 증시 '결렬' 쇼크…남북 경협주 20% 안팎 급락, 엘리엇, 모비스 이어 현대차 주주에도 지지호소 서신, 엘리엇 어깃장에 떠밀리듯 진화 나선 현대차, 모비스와 달리 ‘정공법’을 선택, CEO 간담회에서 제시된 Elliott 주주제안에 대한 현대차의 대응 방안은 새로운 주주환원 정책이 아닌 실적개선이라는 정공법 (당사 추정 및 시장 기대를 상회하는 가이던스 제시), 한전부지 매입과 장기화된 실적악화로 신뢰상실의 문제를 겪고 있는 현대차, 단기 배당에 높은 가중치를 두는 기조가 주류가 된다면 주총을 앞두고 주가 급등락 가능, 그러나 주주제안 충돌을 넘어 주총을 마친다면, 향후 기업가치 방향성은 결국 실적개선이라는 본질과 동행할 예정. 19년 실적은 중장기 실적 가이던스의 바로미터</t>
   </si>
   <si>
     <t>현대차 자사주 매입효과 '톡톡'…3개월간 시총 4.3조원↑, 증시도 '회담 결렬' 쇼크…남북 경협주 20% 안팎 급락, 현대차 주식 샀다가 4550억 날린 엘리엇, 고배당 요구하며 분풀이</t>
@@ -5029,10 +5029,10 @@
     <t>中A주 MSCI 편입 확대 "악재지만 매도 우려만큼 크지 않을듯", 막 오른 '현대차 vs 엘리엇' 공방전…배당·이사선임 두고 확연한 이견, 시장심리 톱5, 대한항공·두산·NH투자증권·한국가스공사·두산인프라코어, '넥스트 한진칼'은 어디?, 기업-투자자 '윈윈게임'으로, “재벌총수 일가 95명, 사익편취로 자산가치 35조 이상 불렸다”</t>
   </si>
   <si>
-    <t>경제개혁연구소 “대기업 총수 일가가 사익편취로 35조 얻어”, 달튼, 현대홈쇼핑에 "3억6500만달러 주주환원하라" 압력, 팰리세이드 효과…가속페달 밟는 에스텍, 현대차-Better late than never, 18년도 4분기 Review: 2019년을 위한 기저, 2019년 전망: 드디어 차세대자동차 기업이 된다, 투자의견 매수, 목표주가 160,000원으로 커버리지 개시, 3월에 핫한 우선주, '스튜어드십 코드'가 할인율 축소, 달튼, 현대홈쇼핑에 "3억6500만달러 주주환원하라" 압력, '소떼 1000마리'로 시작한 대북 사업, 현대그룹 20년 아픔과 좌절, 美투자회사, "현대홈쇼핑, 주주 손실에도 경영진 보상은 증가"…현대차는 엘리엇과 전쟁 중</t>
-  </si>
-  <si>
-    <t>법조인은 옛말, 대세는 '사회공헌가'... 사외이사가 바뀐다, 현대차-기대감을 가질 수 있는 이유, 4개의 이슈에 대한 기대감, 이슈들에 대한 해석, 명확해지는 방향성, 목표주가 165,000원, 투자의견 매수 유지, 행동주의 펀드 놀이터 된 주총...초조한 재계, 보유 현금 218억인데...“주주에 240억 풀어라” 요구, 현대차-신형 쏘나타에서 챙겨봐야 할 숫자들, 8세대 쏘나타 디자인 및 주요 제원 공개, 가격정책은 중립적, 연비는 긍정적, 향후 신차들에 대한 기대감 향상, 쏘나타 세대별 가격 및 연비 비교, 현대차-신형 쏘나타 공개, 세단 시장 부진에도 주목해야 하는 이유, 8세대 신형 쏘나타 전일 공개, 신형 쏘나타 출시에 주목해야 하는 이유, 현대차-8세대 Sonata (DN8) 첫 공개, 시장 기대 만족시킬 듯, 현대차, 8세대 Sonata (DN8) 최초 공개. 아직 최종 판단은 이르지만 시장 기대 만족시킬 가능성, 스포티한 이미지, 연비개선, 다수의 최신 기술 사양 적용. 가격은 2,346~3,289만원, 현대차-베이징 제1공장 가동 중단 관련 언론 보도 코멘트, 국내외 다수 언론, 베이징현대 1공장 가동 중단 보도, 언론에 보도된 가동 중단 이유는 판매부진과 환경문제, 출하대수 회복전망에도 불구하고 실적 개선을 위해 베이징현대가 설비를 감축해야 할 것으로 판단</t>
+    <t>경제개혁연구소 “대기업 총수 일가가 사익편취로 35조 얻어”, 달튼, 현대홈쇼핑에 "3억6500만달러 주주환원하라" 압력, 팰리세이드 효과…가속페달 밟는 에스텍, Better late than never, 18년도 4분기 Review: 2019년을 위한 기저, 2019년 전망: 드디어 차세대자동차 기업이 된다, 투자의견 매수, 목표주가 160,000원으로 커버리지 개시, 3월에 핫한 우선주, '스튜어드십 코드'가 할인율 축소, 달튼, 현대홈쇼핑에 "3억6500만달러 주주환원하라" 압력, '소떼 1000마리'로 시작한 대북 사업, 현대그룹 20년 아픔과 좌절, 美투자회사, "현대홈쇼핑, 주주 손실에도 경영진 보상은 증가"…현대차는 엘리엇과 전쟁 중</t>
+  </si>
+  <si>
+    <t>법조인은 옛말, 대세는 '사회공헌가'... 사외이사가 바뀐다, 기대감을 가질 수 있는 이유, 4개의 이슈에 대한 기대감, 이슈들에 대한 해석, 명확해지는 방향성, 목표주가 165,000원, 투자의견 매수 유지, 행동주의 펀드 놀이터 된 주총...초조한 재계, 보유 현금 218억인데...“주주에 240억 풀어라” 요구, 신형 쏘나타에서 챙겨봐야 할 숫자들, 8세대 쏘나타 디자인 및 주요 제원 공개, 가격정책은 중립적, 연비는 긍정적, 향후 신차들에 대한 기대감 향상, 쏘나타 세대별 가격 및 연비 비교, 신형 쏘나타 공개, 세단 시장 부진에도 주목해야 하는 이유, 8세대 신형 쏘나타 전일 공개, 신형 쏘나타 출시에 주목해야 하는 이유, 8세대 Sonata (DN8) 첫 공개, 시장 기대 만족시킬 듯, 현대차, 8세대 Sonata (DN8) 최초 공개. 아직 최종 판단은 이르지만 시장 기대 만족시킬 가능성, 스포티한 이미지, 연비개선, 다수의 최신 기술 사양 적용. 가격은 2,346~3,289만원, 베이징 제1공장 가동 중단 관련 언론 보도 코멘트, 국내외 다수 언론, 베이징현대 1공장 가동 중단 보도, 언론에 보도된 가동 중단 이유는 판매부진과 환경문제, 출하대수 회복전망에도 불구하고 실적 개선을 위해 베이징현대가 설비를 감축해야 할 것으로 판단</t>
   </si>
   <si>
     <t>볼턴 "트럼프, 대화 의지 있어...동창리 사실이면 유감", 석탄발전소 ‘464기’ 추가로 짓는 중국, 공정위 칼날 이번엔 '중견그룹' 겨눠, 미세먼지=국가 재난? 여야 "13일 본회의 처리 방침", 침, "기업 주식 배당 늘려라? 정부 개입할 여지 없어", 오너일가 늘어난 배당금 만큼 소득세도 '껑충', 한국 증시 하노이 쇼크 북한 테마주 동반 폭락</t>
@@ -5050,7 +5050,7 @@
     <t>TheCapitalGroupCompanies,Inc. 외, 해외 자문사들 이어 대신지배硏도 "엘리엇 고배당 요구 반대", 주주친화 따르는 주가…`착한투자` SRI 펀드 투자해볼까, 대신지배구조硏 "엘리엇, 현대차 배당요구 지나쳐"</t>
   </si>
   <si>
-    <t>현대차-2/27 CEO Investor Day와 CASE, 강점: C(커넥티드카)와 E(전동화), 약점: A(자율주행차) 및 S(차량공유), “인재 뺏길라…” 네이버, 임직원 스톡옵션 1500억 베팅, 구글 인재 영입 나서자… 네이버 ‘1500억 스톡옵션’ 꺼냈다, 네이버 "구글에 핵심인재 뺏길라"...스톡옵션 1500억어치 푼다, ‘인재 잡아라’···임직원 스톡옵션 1,500억 푸는 네이버, 네이버, 임직원 스톡옵션에 5년간 1500억원 투입…"떠나는 인재 잡아라", “인재 유출 막자”…네이버, 임직원에 1500억원 스톡옵션 쏜다, 김상조 공정거래위원회 위원장, 시장심리 톱5, CJ·삼성전자·현대차·KT·롯데칠성, 네이버, "5년간 스톡옵션 1500억원 쏜다”, 네이버, 임직원에 5년간 '1,500억원' 스톡옵션 쏘는 까닭은, '인재유출 비상' 네이버, 임직원 스톡옵션에 1천500억 쓴다, "외국인 투자자, 한국 주식 관심 줄었다", 네이버, '인재 쟁탈전' 맞서 스톡옵션 1500억원 쓴다</t>
+    <t>2/27 CEO Investor Day와 CASE, 강점: C(커넥티드카)와 E(전동화), 약점: A(자율주행차) 및 S(차량공유), “인재 뺏길라…” 네이버, 임직원 스톡옵션 1500억 베팅, 구글 인재 영입 나서자… 네이버 ‘1500억 스톡옵션’ 꺼냈다, 네이버 "구글에 핵심인재 뺏길라"...스톡옵션 1500억어치 푼다, ‘인재 잡아라’···임직원 스톡옵션 1,500억 푸는 네이버, 네이버, 임직원 스톡옵션에 5년간 1500억원 투입…"떠나는 인재 잡아라", “인재 유출 막자”…네이버, 임직원에 1500억원 스톡옵션 쏜다, 김상조 공정거래위원회 위원장, 시장심리 톱5, CJ·삼성전자·현대차·KT·롯데칠성, 네이버, "5년간 스톡옵션 1500억원 쏜다”, 네이버, 임직원에 5년간 '1,500억원' 스톡옵션 쏘는 까닭은, '인재유출 비상' 네이버, 임직원 스톡옵션에 1천500억 쓴다, "외국인 투자자, 한국 주식 관심 줄었다", 네이버, '인재 쟁탈전' 맞서 스톡옵션 1500억원 쓴다</t>
   </si>
   <si>
     <t>규제 폐지에 LPG 관련주 훨훨⋯진짜 수혜주 바로 '나', 주총 시즌…"배당주펀드 관심 가질 만"</t>
@@ -5062,7 +5062,7 @@
     <t>더캐피털그룹 현대차 지분 매각 왜, 주총과는 무관</t>
   </si>
   <si>
-    <t>카카오, 신형 쏘나타에 AI 플랫폼 '카카오 i' 탑재, 현대차 방향 좌우할 3월22일 주주총회, 최대의 관심사 ‘삼성전자·현대차’...관전 포인트는?, 삼성전자·현대차, 이변은 없다...이번주 471개사 '슈퍼주총 데이', 현대차-부진했던 Segment의 판매회복 시작, 판매 기저효과가 높은 SUV 신차 투입과 상품성 개선 Sedan 신차 확대를 통해, 18년도 하반기 이후 내수/미국/중국시장 판매 증가 및 점유율 상승 기록 중, B/E/F-SUV 신차 출시와 Sedan 부진요인 마무리를 통해, 14년 이후 5년 만의 사업계획 및 시장기대치를 상회하는 19년 판매실적 및 영업실적 전망, 기존 투자의견 Buy와 적정주가 150,000원을 유지, 현대차 기아차 현대모비스 주가 올라, 실적반등 가능성 부각, 제2, 제3의 '주주 행동주의' 떼들이 몰려오고 있다</t>
+    <t>카카오, 신형 쏘나타에 AI 플랫폼 '카카오 i' 탑재, 현대차 방향 좌우할 3월22일 주주총회, 최대의 관심사 ‘삼성전자·현대차’...관전 포인트는?, 삼성전자·현대차, 이변은 없다...이번주 471개사 '슈퍼주총 데이', 부진했던 Segment의 판매회복 시작, 판매 기저효과가 높은 SUV 신차 투입과 상품성 개선 Sedan 신차 확대를 통해, 18년도 하반기 이후 내수/미국/중국시장 판매 증가 및 점유율 상승 기록 중, B/E/F-SUV 신차 출시와 Sedan 부진요인 마무리를 통해, 14년 이후 5년 만의 사업계획 및 시장기대치를 상회하는 19년 판매실적 및 영업실적 전망, 기존 투자의견 Buy와 적정주가 150,000원을 유지, 현대차 기아차 현대모비스 주가 올라, 실적반등 가능성 부각, 제2, 제3의 '주주 행동주의' 떼들이 몰려오고 있다</t>
   </si>
   <si>
     <t>다가온 슈퍼주총데이 '스튜어드십코드' 안착 시험대, 기업의 미래가 국가 백년대계 출발점이다, 기회의 땅에서 무덤으로, 글로벌 자동차 기업 중국 경영 휘청, 현대 기아도 앞날도 먹구름, 끝나지 않은 론스타의 ‘저주’ | 외환은행 인수 자금으로 쓰인 정체불명의 뭉칫돈 ‘6349억원’의 실제 주인은 한국인?</t>
@@ -5083,13 +5083,13 @@
     <t>한숨 돌린 현대차, 한진칼도 웃을 수 있나</t>
   </si>
   <si>
-    <t>‘용두사미’로 끝나버린 행동주의 펀드의 꿈, 2019 슈퍼 주총데이 관전 포인트!, 현대차-수소전기차 개발 및 생산능력은 세계 선도 수준, 투자의견 Buy, 목표주가 150,000원 유지, 수소차 기술 선도 업체. 2018년 출시된 Nexo는 상용 수소차 중 가장 긴 주행 기록 보유, 현대차그룹, 2030년 FCEV 비전 발표, 2019 슈퍼 주총데이 관전 포인트!</t>
-  </si>
-  <si>
-    <t>(주)현대성우쏠라이트 ‘쏠라이트 배터리’, 브랜드스타 자동차배터리 부문 수상, 현대성우쏠라이트, 2019 브랜드스타 수상, 현대성우쏠라이트, 2019 브랜드스타 자동차 배터리 부문 최우수 브랜드 수상, 주가 4천원 탈출법…'글로벌 스탠다드에 답 있다', 현대차-19년도 1분기 Preview: 이머징 통화 약세로 기대치 다소 하회, 내수 시장과 미국 시장의 판매 회복, 이머징 통화 약세와 해외 공장 가동률 하락, 속도의 문제일 뿐 개선의 흐름은 변화 없어</t>
-  </si>
-  <si>
-    <t>현대차-트로이의 목마, 8세대 쏘나타, 8세대 쏘나타: 한국보다 미국 판매량이 중요하다, 트로이의 목마: 현대차의 모빌리티 서비스 시발점, 대한항공 주가 급등…최종구 위원장 "스튜어드십코드 긍정적인 면", 제법 어려운 질문, 삼성생명 종합검사는 '보복'인가</t>
+    <t>‘용두사미’로 끝나버린 행동주의 펀드의 꿈, 2019 슈퍼 주총데이 관전 포인트!, 수소전기차 개발 및 생산능력은 세계 선도 수준, 투자의견 Buy, 목표주가 150,000원 유지, 수소차 기술 선도 업체. 2018년 출시된 Nexo는 상용 수소차 중 가장 긴 주행 기록 보유, 현대차그룹, 2030년 FCEV 비전 발표, 2019 슈퍼 주총데이 관전 포인트!</t>
+  </si>
+  <si>
+    <t>(주)현대성우쏠라이트 ‘쏠라이트 배터리’, 브랜드스타 자동차배터리 부문 수상, 현대성우쏠라이트, 2019 브랜드스타 수상, 현대성우쏠라이트, 2019 브랜드스타 자동차 배터리 부문 최우수 브랜드 수상, 주가 4천원 탈출법…'글로벌 스탠다드에 답 있다', 19년도 1분기 Preview: 이머징 통화 약세로 기대치 다소 하회, 내수 시장과 미국 시장의 판매 회복, 이머징 통화 약세와 해외 공장 가동률 하락, 속도의 문제일 뿐 개선의 흐름은 변화 없어</t>
+  </si>
+  <si>
+    <t>트로이의 목마, 8세대 쏘나타, 8세대 쏘나타: 한국보다 미국 판매량이 중요하다, 트로이의 목마: 현대차의 모빌리티 서비스 시발점, 대한항공 주가 급등…최종구 위원장 "스튜어드십코드 긍정적인 면", 제법 어려운 질문, 삼성생명 종합검사는 '보복'인가</t>
   </si>
   <si>
     <t>조양호 회장, 대한항공 경영 퇴진... 연금 사회주의인가, 주주 자본주의인가, 조양호 회장, 대한항공 경영 퇴진... 연금 사회주의인가, 주주 자본주의인가?, 상장 첫날 현대오토에버 초강세, 현대오토에버, 상장 첫 날 '급등'…단숨에 9만원선까지, 현대오토에버, 증시 '화려한 데뷔'</t>
@@ -5110,7 +5110,7 @@
     <t>디에스자산운용, 美 리프트 투자로 대박난 사연</t>
   </si>
   <si>
-    <t>현대차-득과 실, 19년도 1분기 영업이익은 7,408억원(+8.7% 전년 대비 증감율, OPM 3.2%) 기록, 컨센서스 9.5% 하회, 단 xEV 비중 증가, 쏘나타 출고 지연 속 초기 런칭비, 신규 플랫폼 및 엔진 적용에 따른 원가비 증가로 수익성 회복은 기대보다 지연, 현대차-실적 개선 진행, 장기 성장가능성에 초점, 19년도 1분기 Preview - 영업이익 7,467억원(전년 대비 증감율 +9.6%, OPM 3.2%) 전망, 실적 개선 진행, 장기 성장가능성에 초점, 아시아 몰려드는 행동주의 펀드, 기회인가 위기인가, 1분기 주식부자 정유경·김창수 웃고 문은상·조양호 울었다</t>
+    <t>득과 실, 19년도 1분기 영업이익은 7,408억원(+8.7% 전년 대비 증감율, OPM 3.2%) 기록, 컨센서스 9.5% 하회, 단 xEV 비중 증가, 쏘나타 출고 지연 속 초기 런칭비, 신규 플랫폼 및 엔진 적용에 따른 원가비 증가로 수익성 회복은 기대보다 지연, 실적 개선 진행, 장기 성장가능성에 초점, 19년도 1분기 Preview - 영업이익 7,467억원(전년 대비 증감율 +9.6%, OPM 3.2%) 전망, 실적 개선 진행, 장기 성장가능성에 초점, 아시아 몰려드는 행동주의 펀드, 기회인가 위기인가, 1분기 주식부자 정유경·김창수 웃고 문은상·조양호 울었다</t>
   </si>
   <si>
     <t>현대글로비스 - 18년도 1분기 매출 4 조 1624 억원, 영업익 1862 억원 전망·실적 안정성 부각</t>
@@ -5119,7 +5119,7 @@
     <t>1분기 반등장에도 개미 '쓴잔'…순매수 상위 10개 중 8개 하락</t>
   </si>
   <si>
-    <t>지난해 순이익 증가율 1위 자동차주는 기아차. 왜?, 현대차-신차 출시를 통한 점유율 상승 스토리, 하반기 실적 개선폭이 클 것, 19년도 1분기 Preview: 영업이익률 3.2% 전망, 신차 출시로 점유율 상승 목표, 현대차-기대감 선반영으로 높아져 있는 valuation, 중장기 주가 향방에 대한 고민, 전년 기저효과에 더해 새로운 신차싸이클 시작으로 실적 회복에 대한 기대감이 높아져 있음, 이익의 회복이 가시적인 반면, 향후 5년간 동사 ROIC는 4~5%의 낮은 수준에 머무를 것., 결국 주가는 현 수준에서 크게 상승하기보다는 실적 회복의 기대감을 좌우할 수 있는 단기 지표들이 현재의 높은 valuation을 지탱하는 흐름이 지속될 것으로 예상함</t>
+    <t>지난해 순이익 증가율 1위 자동차주는 기아차. 왜?, 신차 출시를 통한 점유율 상승 스토리, 하반기 실적 개선폭이 클 것, 19년도 1분기 Preview: 영업이익률 3.2% 전망, 신차 출시로 점유율 상승 목표, 기대감 선반영으로 높아져 있는 valuation, 중장기 주가 향방에 대한 고민, 전년 기저효과에 더해 새로운 신차싸이클 시작으로 실적 회복에 대한 기대감이 높아져 있음, 이익의 회복이 가시적인 반면, 향후 5년간 동사 ROIC는 4~5%의 낮은 수준에 머무를 것., 결국 주가는 현 수준에서 크게 상승하기보다는 실적 회복의 기대감을 좌우할 수 있는 단기 지표들이 현재의 높은 valuation을 지탱하는 흐름이 지속될 것으로 예상함</t>
   </si>
   <si>
     <t>제15차 한중일 FTA 협상 도쿄서 개최…4개월 만에 재협상 外</t>
@@ -5137,10 +5137,10 @@
     <t>미세먼지·산불·쓰레기의 '역습', 코엔텍·인선이엔티·와이엔텍…폐기물 처리株 눈여겨 볼 만</t>
   </si>
   <si>
-    <t>"현대모비스 주식 비중 늘려도 된다", 중국에서 사업 점차 정상화, 현대차-SUV 상승 Cycle을 이끈다, 펠리세이드 증산 결정, 하반기 마진회복을 담보, 하반기 이어지는 제네시스 볼륨 모멘텀, 가동률 회복으로 실적의 가시성 강화, 투자의견 BUY 유지, 목표주가 170,000원으로 상향. Top Pick!, 현대건설 - 1Q실적 시장 예상치부합 예상·2분기 이후 양호한 해외수주 성과 기대</t>
-  </si>
-  <si>
-    <t>“중국 경기 좋아져", 현대차 LS LG생활건강 주식 볼 때, 현대위아 - 엔진사업부 호조세·19년도 1분기 영업익 242억원으로 흑자전환, 현대차-기업별 19년도 1분기 Preview, 컨센서스 소폭 하회 전망, TP 15만원(M), 투자의견 BUY(M)</t>
+    <t>"현대모비스 주식 비중 늘려도 된다", 중국에서 사업 점차 정상화, SUV 상승 Cycle을 이끈다, 펠리세이드 증산 결정, 하반기 마진회복을 담보, 하반기 이어지는 제네시스 볼륨 모멘텀, 가동률 회복으로 실적의 가시성 강화, 투자의견 BUY 유지, 목표주가 170,000원으로 상향. Top Pick!, 현대건설 - 1Q실적 시장 예상치부합 예상·2분기 이후 양호한 해외수주 성과 기대</t>
+  </si>
+  <si>
+    <t>“중국 경기 좋아져", 현대차 LS LG생활건강 주식 볼 때, 현대위아 - 엔진사업부 호조세·19년도 1분기 영업익 242억원으로 흑자전환, 기업별 19년도 1분기 Preview, 컨센서스 소폭 하회 전망, TP 15만원(M), 투자의견 BUY(M)</t>
   </si>
   <si>
     <t>LG화학·한화케미칼 등 235곳 미세먼지 배출조작…공정위, 하도급법위반 GS건설 공공공사 입찰 제한 등</t>
@@ -5152,19 +5152,19 @@
     <t>지난해 ROE 증가율 1위 광고주는 오리콤. 비결은?</t>
   </si>
   <si>
-    <t>현대차-3세대 플랫폼 확대 시 원가 절감 기대, 최근 현대차의 전략적 방향성은 1) 믹스 개선, 판매 회복, 비용 절감, 신규 플랫폼을 통한 수익성 개선과, 2) 전기차, 자율주행차, 모빌리티를 지향하는 구체적 비전 공유 및 투자, 협업 모델을 지향하며 시장 요구에 수렴, 도요타의 플랫폼 개발, 선행기술 개발과 전동화, 자율주행 양산, 이관 등 원가 절감을 위한 움직임은 현대차그룹 원가절감 전략과 미래 전략에 시사하는 바가 큼, 주가 하락? 공매도 종목의 대반전-삼성전기 만도 셀트리온 두산인프라 ‘훨훨’, 현대오토에버, 현대차 지배구조 개편 '핵'으로 떠오르나</t>
+    <t>3세대 플랫폼 확대 시 원가 절감 기대, 최근 현대차의 전략적 방향성은 1) 믹스 개선, 판매 회복, 비용 절감, 신규 플랫폼을 통한 수익성 개선과, 2) 전기차, 자율주행차, 모빌리티를 지향하는 구체적 비전 공유 및 투자, 협업 모델을 지향하며 시장 요구에 수렴, 도요타의 플랫폼 개발, 선행기술 개발과 전동화, 자율주행 양산, 이관 등 원가 절감을 위한 움직임은 현대차그룹 원가절감 전략과 미래 전략에 시사하는 바가 큼, 주가 하락? 공매도 종목의 대반전-삼성전기 만도 셀트리온 두산인프라 ‘훨훨’, 현대오토에버, 현대차 지배구조 개편 '핵'으로 떠오르나</t>
   </si>
   <si>
     <t>시장심리 톱5, 한화·현대차·미래에셋대우·대우조선해양·두산</t>
   </si>
   <si>
-    <t>현대차-년도년도 1분기 1분기 Review: 악순환 탈출 성공, 확인해야 할 지,년도 두분기 년도년도 1분기 1분기 실적은 당사 기대치를 상회. ASP상승, 한국공장 흑자전환, 금융이익 증가가 견인, 한편 2012년 이후 처음으로 매출원가율이 -0.8%p전년 대비 증감율감소. 금융부분 제외 순현금 16.2조원 (+1.8조원전분기 대비 증감율) 신차출시 효과라면 부품사 실적도 동반회복 예상. 그 외 신차효과 지속을 위해서는 글로벌 수요회복이 필요, 년도년도 1분기 1분기 실적호조와 현금증가를 반영하여 목표주가를 155,000원으로 14.8%상향. ‘BUY’의견 유지. 향후 완성차와 부품사의 실적방향성 동행여부에 주목, 후진하던 현대차, 다시 발진? 신차 SUV가 살렸다, 현대차-확인된 방향, 다음 과제는 속도와 강도, 19년도 1분기 매출/ 영업이익 각각 +7% 전년 대비 증감율, +21% 전년 대비 증감율 증가했으며, 시장 기대치를 상회, 신차 Cycle 개시를 통한 영업지표 호전이 실적 개선으로 연결, 주요 시장 가동률 상승/인센티브 감소 기조 지속 중이며, 이를 통한 제조분야 원가율 회복과 금융분야 손익 정상화 실현될 전망, 19 년 영업이익, 시장 기대치를 +16% 상회하는 4.14 조원 (+71% 전년 대비 증감율)을 전망, 투자의견 Buy 유지, 적정주가 165,000원으로 상향, 현대차 주가 이틀째 올라, 1분기 실적 기대이상, 현대차-상하이 모터쇼에 4개의 신차 공개, 상하이 모터쇼에서 4개의 신차 공개, 2011년 이후 감소한 판매보증충당부채가 우려 요인, 주가는 실적 개선 기대를 선 반영, 실제 실적 개선은 더딜 것, 현대차-년도년도 1분기 1분기 Review-드러나기 시작하는 믹스 개선 효과, 년도년도 1분기 1분기 영업이익 8,249억원 (+21.1% 전년 대비 증감율) 기록. 시장 컨센서스 상회, 신차 중심의 내수 시장 믹스 개선에 힘입은 영업이익 증가, 내수 Palisade에서 시작한 수익성 개선은 신형 Sonata, Genesis 브랜드, 해외 시장으로 확대될 것</t>
-  </si>
-  <si>
-    <t>현대차-차량믹스와 금융부문 동반 개선, 금융 사업부 이익 개선에 힘입어 최근 낮아진 시장 기대치 영업이익 8% 상회, 매출 증감 요인(전년 대비 증감율+1,217십억원): SUV 확대에 따른 Mix개선이 매출 견인, 영업이익 증감 요인(전년 대비 증감율+144십억원): 물량 &amp; 믹스개선 효과와 금융부분이 견인, KB자산운용,‘KB스타베트남VN30인덱스펀드’ 출시, 현대차, 팰리세이드 덕봤다…남은 과제는 ‘차이나 리스크’, 현대차 - 상하이 모터쇼에서 신형 싼타페·쏘나타 등 공개·이익개선은 제한적, 자동차 '어닝쇼크'에 약세…스톡스 0.1%↓, 현대차-이젠 실적도 말이 통한다, 1분기 영업이익은 신차 판매가 늘고 믹스가 개선되며 컨센서스 7% 상회, 2분기부터는 쏘나타 효과 본격화, 팰리세이드 증산으로 실적 더욱 강하게 반등, 신차들의 가격 대비 성능이 좋아지면서 글로벌 점유율 회복으로 이어질 전망, 현대차-구조적 변화의 시작, 19년도 1분기 Review: 중국 우려를 떨치고 이뤄낸 실적, 상품성과 수요는 입증, 앞으로는 비용이 관건, 투자의견 매수 유지, 목표주가 166,000원으로 3.8% 상향, 현대차-수익성 개선 시작, 신차라인업 강화로 장기 실적전망 신뢰도 상승, 1분기 Review - 영업이익, 컨센서스 상회, 현대차-19년도 1분기 Review: SUV 신차 효과로 기대치 상회한 호실적, 믹스개선 효과에 대한 우려 해소, 원/달러 환율 연중 최고치, 하반기로 갈수록 기대, 목표주가 상향, 현대차-구조적 변화의 시작, 19년도 1분기 Review: 중국 우려를 떨치고 이뤄낸 실적, 상품성과 수요는 입증, 앞으로는 비용이 관건, 투자의견 매수 유지, 목표주가 166,000원으로 3.8% 상향, 현대차-차량믹스와 금융부문 동반 개선, 금융 사업부 이익 개선에 힘입어 최근 낮아진 시장 기대치 영업이익 8% 상회, 매출 증감 요인(전년 대비 증감율+1,217십억원): SUV 확대에 따른 Mix개선이 매출 견인, 영업이익 증감 요인(전년 대비 증감율+144십억원): 물량 &amp; 믹스개선 효과와 금융부분이 견인, 현대차-전사적 실적 개선의 시작, 1분기 영업이익은 8,249억원(+21.1%)으로 시장 기대치 +7.1% 상회, 2분기 영업이익도 1.02조원(+7.3%)으로 양호할 전망, 목표주가 170,000원(+6.3%)으로 상향, 투자의견 매수 유지, 현대차-이젠 실적도 말이 통한다, 1분기 영업이익은 신차 판매가 늘고 믹스가 개선되며 컨센서스 7% 상회, 2분기부터는 쏘나타 효과 본격화, 팰리세이드 증산으로 실적 더욱 강하게 반등, 신차들의 가격 대비 성능이 좋아지면서 글로벌 점유율 회복으로 이어질 전망, 현대차-수익성 개선 달성을 위한 엔드 게임, 19년도 1분기 영업이익은 8,249억원(+21.1% 전년 대비 증감율, OPM 3.4%) 기록, 컨센서스 7.1% 상회. 팰리세이드, G90 등 신차 효과로 인한 믹스 개선이 비용 증가 요인을 상쇄, 19년도 하반기 이후 낮아진 기저와 주요 신차 글로벌 확대로 인한 믹스 개선 효과, 플랫폼 확대 적용에 따른 원가율 개선 효과 맞물리며 이익 개선 속도 높일 전망, 투자의견 BUY 유지, 목표주가 기존 150,000원에서 170,000원으로 13.3% 상향. 예상보다 빨라진 수익성 회복 속도를 반영한 추정치 변경에 기인, 현대차-판매믹스 개선의 효과, 1Q 19 Review: 시장 기대치를 상회하는 실적 시현!, 신차 빅 싸이클 진입 단계판매믹스 개선이 이익으로 연결되는 신뢰감 회복 중, 현대차-수익성 개선 시작, 신차라인업 강화로 장기 실적전망 신뢰도 상승, 1분기 Review - 영업이익, 컨센서스 상회, 현대차-19년도 1분기 Review: SUV 신차 효과로 기대치 상회한 호실적, 믹스개선 효과에 대한 우려 해소, 원/달러 환율 연중 최고치, 하반기로 갈수록 기대, 목표주가 상향</t>
-  </si>
-  <si>
-    <t>현대차-패러다임 변화에 적극 대응, 미래 성장 동력 확보, 신차 효과와 미래형 자동차 개발 진행, 실적 개선 본격적 진행 예상</t>
+    <t>년도년도 1분기 1분기 Review: 악순환 탈출 성공, 확인해야 할 지,년도 두분기 년도년도 1분기 1분기 실적은 당사 기대치를 상회. ASP상승, 한국공장 흑자전환, 금융이익 증가가 견인, 한편 2012년 이후 처음으로 매출원가율이 -0.8%p전년 대비 증감율감소. 금융부분 제외 순현금 16.2조원 (+1.8조원전분기 대비 증감율) 신차출시 효과라면 부품사 실적도 동반회복 예상. 그 외 신차효과 지속을 위해서는 글로벌 수요회복이 필요, 년도년도 1분기 1분기 실적호조와 현금증가를 반영하여 목표주가를 155,000원으로 14.8%상향. ‘BUY’의견 유지. 향후 완성차와 부품사의 실적방향성 동행여부에 주목, 후진하던 현대차, 다시 발진? 신차 SUV가 살렸다, 확인된 방향, 다음 과제는 속도와 강도, 19년도 1분기 매출/ 영업이익 각각 +7% 전년 대비 증감율, +21% 전년 대비 증감율 증가했으며, 시장 기대치를 상회, 신차 Cycle 개시를 통한 영업지표 호전이 실적 개선으로 연결, 주요 시장 가동률 상승/인센티브 감소 기조 지속 중이며, 이를 통한 제조분야 원가율 회복과 금융분야 손익 정상화 실현될 전망, 19 년 영업이익, 시장 기대치를 +16% 상회하는 4.14 조원 (+71% 전년 대비 증감율)을 전망, 투자의견 Buy 유지, 적정주가 165,000원으로 상향, 현대차 주가 이틀째 올라, 1분기 실적 기대이상, 상하이 모터쇼에 4개의 신차 공개, 상하이 모터쇼에서 4개의 신차 공개, 2011년 이후 감소한 판매보증충당부채가 우려 요인, 주가는 실적 개선 기대를 선 반영, 실제 실적 개선은 더딜 것, 년도년도 1분기 1분기 Review-드러나기 시작하는 믹스 개선 효과, 년도년도 1분기 1분기 영업이익 8,249억원 (+21.1% 전년 대비 증감율) 기록. 시장 컨센서스 상회, 신차 중심의 내수 시장 믹스 개선에 힘입은 영업이익 증가, 내수 Palisade에서 시작한 수익성 개선은 신형 Sonata, Genesis 브랜드, 해외 시장으로 확대될 것</t>
+  </si>
+  <si>
+    <t>차량믹스와 금융부문 동반 개선, 금융 사업부 이익 개선에 힘입어 최근 낮아진 시장 기대치 영업이익 8% 상회, 매출 증감 요인(전년 대비 증감율+1,217십억원): SUV 확대에 따른 Mix개선이 매출 견인, 영업이익 증감 요인(전년 대비 증감율+144십억원): 물량 &amp; 믹스개선 효과와 금융부분이 견인, KB자산운용,‘KB스타베트남VN30인덱스펀드’ 출시, 현대차, 팰리세이드 덕봤다…남은 과제는 ‘차이나 리스크’, 현대차 - 상하이 모터쇼에서 신형 싼타페·쏘나타 등 공개·이익개선은 제한적, 자동차 '어닝쇼크'에 약세…스톡스 0.1%↓, 이젠 실적도 말이 통한다, 1분기 영업이익은 신차 판매가 늘고 믹스가 개선되며 컨센서스 7% 상회, 2분기부터는 쏘나타 효과 본격화, 팰리세이드 증산으로 실적 더욱 강하게 반등, 신차들의 가격 대비 성능이 좋아지면서 글로벌 점유율 회복으로 이어질 전망, 구조적 변화의 시작, 19년도 1분기 Review: 중국 우려를 떨치고 이뤄낸 실적, 상품성과 수요는 입증, 앞으로는 비용이 관건, 투자의견 매수 유지, 목표주가 166,000원으로 3.8% 상향, 수익성 개선 시작, 신차라인업 강화로 장기 실적전망 신뢰도 상승, 1분기 Review - 영업이익, 컨센서스 상회, 19년도 1분기 Review: SUV 신차 효과로 기대치 상회한 호실적, 믹스개선 효과에 대한 우려 해소, 원/달러 환율 연중 최고치, 하반기로 갈수록 기대, 목표주가 상향, 구조적 변화의 시작, 19년도 1분기 Review: 중국 우려를 떨치고 이뤄낸 실적, 상품성과 수요는 입증, 앞으로는 비용이 관건, 투자의견 매수 유지, 목표주가 166,000원으로 3.8% 상향, 차량믹스와 금융부문 동반 개선, 금융 사업부 이익 개선에 힘입어 최근 낮아진 시장 기대치 영업이익 8% 상회, 매출 증감 요인(전년 대비 증감율+1,217십억원): SUV 확대에 따른 Mix개선이 매출 견인, 영업이익 증감 요인(전년 대비 증감율+144십억원): 물량 &amp; 믹스개선 효과와 금융부분이 견인, 전사적 실적 개선의 시작, 1분기 영업이익은 8,249억원(+21.1%)으로 시장 기대치 +7.1% 상회, 2분기 영업이익도 1.02조원(+7.3%)으로 양호할 전망, 목표주가 170,000원(+6.3%)으로 상향, 투자의견 매수 유지, 이젠 실적도 말이 통한다, 1분기 영업이익은 신차 판매가 늘고 믹스가 개선되며 컨센서스 7% 상회, 2분기부터는 쏘나타 효과 본격화, 팰리세이드 증산으로 실적 더욱 강하게 반등, 신차들의 가격 대비 성능이 좋아지면서 글로벌 점유율 회복으로 이어질 전망, 수익성 개선 달성을 위한 엔드 게임, 19년도 1분기 영업이익은 8,249억원(+21.1% 전년 대비 증감율, OPM 3.4%) 기록, 컨센서스 7.1% 상회. 팰리세이드, G90 등 신차 효과로 인한 믹스 개선이 비용 증가 요인을 상쇄, 19년도 하반기 이후 낮아진 기저와 주요 신차 글로벌 확대로 인한 믹스 개선 효과, 플랫폼 확대 적용에 따른 원가율 개선 효과 맞물리며 이익 개선 속도 높일 전망, 투자의견 BUY 유지, 목표주가 기존 150,000원에서 170,000원으로 13.3% 상향. 예상보다 빨라진 수익성 회복 속도를 반영한 추정치 변경에 기인, 판매믹스 개선의 효과, 1Q 19 Review: 시장 기대치를 상회하는 실적 시현!, 신차 빅 싸이클 진입 단계판매믹스 개선이 이익으로 연결되는 신뢰감 회복 중, 수익성 개선 시작, 신차라인업 강화로 장기 실적전망 신뢰도 상승, 1분기 Review - 영업이익, 컨센서스 상회, 19년도 1분기 Review: SUV 신차 효과로 기대치 상회한 호실적, 믹스개선 효과에 대한 우려 해소, 원/달러 환율 연중 최고치, 하반기로 갈수록 기대, 목표주가 상향</t>
+  </si>
+  <si>
+    <t>패러다임 변화에 적극 대응, 미래 성장 동력 확보, 신차 효과와 미래형 자동차 개발 진행, 실적 개선 본격적 진행 예상</t>
   </si>
   <si>
     <t>'순환출자 고리 열쇠' 현대모비스…중간지주사 전환 추진 중인 SKT 관심</t>
@@ -5173,7 +5173,7 @@
     <t>글로벌 적대적 M&amp;A 다시 고개...작년 19년 만의 최대치, "깜짝 실적" 현대글로비스 · 현대위아 주가, 29일 장초반 '급등'</t>
   </si>
   <si>
-    <t>현대차-월드클래스 수소차 생산업체, 글로벌 수준의 기술력 보유, 따라서 수요 확보는 기술력이 아니라 인프라가 관건, 시장 전망과 점유율 전망, 단기 실적에 영향을 미치긴 어려우나, 밸류에이션을 타당하게 만드는 요인, 현대차-이익 증가 방향성 확인, 19년도 1분기 현대차 실적 개선 주요인이 1) 제한된 판매 개선 속 2) 팰리세이드, G90에만 의존한 믹스 개선인 점을 감안 시 19년도 2분기 쏘나타(볼륨/믹스), 년도년도 1분기 3분기 베뉴(),년도 볼분기 4Q19 G80, GV80(믹스) 신차 라인업은 수익성 개선을 지속 견인할 것으로 판단, 금융 부분의 경우 현대카드 코스트코 고객 모집에 따른 2Q~년도년도 1분기 3분기 비용 증가 전망되나 국내 신차출시로 판매/믹스 개선(현대캐피탈), 미국 금리인상 압력 완화, 중고차 잔존가치 개선, 신차 확대(HCA)로 수익성 개선은 지속될 것으로 판단</t>
+    <t>월드클래스 수소차 생산업체, 글로벌 수준의 기술력 보유, 따라서 수요 확보는 기술력이 아니라 인프라가 관건, 시장 전망과 점유율 전망, 단기 실적에 영향을 미치긴 어려우나, 밸류에이션을 타당하게 만드는 요인, 이익 증가 방향성 확인, 19년도 1분기 현대차 실적 개선 주요인이 1) 제한된 판매 개선 속 2) 팰리세이드, G90에만 의존한 믹스 개선인 점을 감안 시 19년도 2분기 쏘나타(볼륨/믹스), 년도년도 1분기 3분기 베뉴(),년도 볼분기 4Q19 G80, GV80(믹스) 신차 라인업은 수익성 개선을 지속 견인할 것으로 판단, 금융 부분의 경우 현대카드 코스트코 고객 모집에 따른 2Q~년도년도 1분기 3분기 비용 증가 전망되나 국내 신차출시로 판매/믹스 개선(현대캐피탈), 미국 금리인상 압력 완화, 중고차 잔존가치 개선, 신차 확대(HCA)로 수익성 개선은 지속될 것으로 판단</t>
   </si>
   <si>
     <t>"작년과 다르다"…현대차그룹, 시총 증가율 1위, 쌍용차 - 신차 출격개시·코란도 판매 본격화에 따른 실적반전 기대</t>
@@ -5194,19 +5194,19 @@
     <t>1Q 영업이익 증가율 1위 자동차주는 기아차. 비결은?</t>
   </si>
   <si>
-    <t>美 자동차 관세 연기에 국내 완성차 이해득실 분주, 현대차-상품성 회복에 대한 신뢰 구축, 그랜져, 싼타페, 팰리세이드의 흥행 열풍, 하반기 출시될 신차에 대한 기대감도 유효</t>
+    <t>美 자동차 관세 연기에 국내 완성차 이해득실 분주, 상품성 회복에 대한 신뢰 구축, 그랜져, 싼타페, 팰리세이드의 흥행 열풍, 하반기 출시될 신차에 대한 기대감도 유효</t>
   </si>
   <si>
     <t>포춘 500 기업 중 여성 CEO 33명 - 사상 최고, 美 관세 부과 연기 방침에 한숨 돌린 현대차</t>
   </si>
   <si>
-    <t>현대차-수익성 결정변수의 개선, 2019년 매출액 최초로 100조원 상회 전망, 제품 경쟁력 강화 구간: 3세대 플랫폼 적용된 신차출시 사이클 본격화, 2Q 예상 순이익 1위 물류 기업은 현대글로비스. 비결은?</t>
+    <t>수익성 결정변수의 개선, 2019년 매출액 최초로 100조원 상회 전망, 제품 경쟁력 강화 구간: 3세대 플랫폼 적용된 신차출시 사이클 본격화, 2Q 예상 순이익 1위 물류 기업은 현대글로비스. 비결은?</t>
   </si>
   <si>
     <t>하락장에 외국인 삼바 대차거래 급증, ‘삼바’ 팔자…외인 대차거래 급증, 美 화웨이 제재에 삼성전자 강세, LG유플러스 약세</t>
   </si>
   <si>
-    <t>“강단과 인내가 큰 열매 맺는 법… 시장 나빠도 전략 고수”, 文대통령 "바이오·헬스 韓경제 이끌 것", OECD "올해 한국 성장률 2.6%→2.4% 하향" 전망, 베트남 간 대형 증권사 성적표 외, 현대차 주가 오를 힘 다져, 신차효과로 하반기 실적 개선폭 커져, 현대차-하반기 신차 라인업 우수, P/B 0.5배 초반. 배당수익률도 3% 이상, SUV와 럭셔리 부문의 강화, 수익성 확보를 위한 전략 실행 중, 현대차-제네시스, 서울을 대표하는 브랜드가 된다, 한국시장과 미국시장에서 제네시스는 Flagship 모델로서 트래픽 증가 역할과 수익원이 될 전망. 제네시스GV80, G80은 한국공장 수출 모델로 원화약세와 맞물려 신차효과가 극대화 될 전망, 19년도 3분기 에 소형SUV 베뉴, 그랜져F/L, 19년도 4분기 에 GV80, 20년도 1분기 에 G80으로 이어지는 신차출시의 특징은 디자인 혁신과 Connectivity, 3분기에 한국공장 노조파업이 단기리스크가 될 수 있으나, 퇴직자 증가로 노사갈등 이슈는 Peak-out 한 것으로 판단되며, 산업트렌드에 맞는 유연한 생산구조를 갖출 수 있게 될 전망. 목표주가 산정기준을 2019년에서 2019년, 2020년 평균을 적용, Target Valuation은 유지하여 목표주가를 160,000원으로 3.2%상향. 19년도 하반기 에 업종 Top-pick으로 제시</t>
+    <t>“강단과 인내가 큰 열매 맺는 법… 시장 나빠도 전략 고수”, 文대통령 "바이오·헬스 韓경제 이끌 것", OECD "올해 한국 성장률 2.6%→2.4% 하향" 전망, 베트남 간 대형 증권사 성적표 외, 현대차 주가 오를 힘 다져, 신차효과로 하반기 실적 개선폭 커져, 하반기 신차 라인업 우수, P/B 0.5배 초반. 배당수익률도 3% 이상, SUV와 럭셔리 부문의 강화, 수익성 확보를 위한 전략 실행 중, 제네시스, 서울을 대표하는 브랜드가 된다, 한국시장과 미국시장에서 제네시스는 Flagship 모델로서 트래픽 증가 역할과 수익원이 될 전망. 제네시스GV80, G80은 한국공장 수출 모델로 원화약세와 맞물려 신차효과가 극대화 될 전망, 19년도 3분기 에 소형SUV 베뉴, 그랜져F/L, 19년도 4분기 에 GV80, 20년도 1분기 에 G80으로 이어지는 신차출시의 특징은 디자인 혁신과 Connectivity, 3분기에 한국공장 노조파업이 단기리스크가 될 수 있으나, 퇴직자 증가로 노사갈등 이슈는 Peak-out 한 것으로 판단되며, 산업트렌드에 맞는 유연한 생산구조를 갖출 수 있게 될 전망. 목표주가 산정기준을 2019년에서 2019년, 2020년 평균을 적용, Target Valuation은 유지하여 목표주가를 160,000원으로 3.2%상향. 19년도 하반기 에 업종 Top-pick으로 제시</t>
   </si>
   <si>
     <t>상장은 했지만… 리프트와 우버의 고민, '닷컴버블 붕괴'와 함께 무너진 신뢰…코스닥 '20년 침체' 불렀다</t>
@@ -5215,7 +5215,7 @@
     <t>미중 무역분쟁 여파…100대 주식부호 지분가치 7.9조원↓</t>
   </si>
   <si>
-    <t>현대차-제네시스, 서울을 대표하는 브랜드가 된다, 한국시장과 미국시장에서 제네시스는 Flagship 모델로서 트래픽 증가 역할과 수익원이 될 전망. 제네시스GV80, G80은 한국공장 수출 모델로 원화약세와 맞물려 신차효과가 극대화 될 전망, 19년도 3분기 에 소형SUV 베뉴, 그랜져F/L, 19년도 4분기 에 GV80, 20년도 1분기 에 G80으로 이어지는 신차출시의 특징은 디자인 혁신과 Connectivity, 3분기에 한국공장 노조파업이 단기리스크가 될 수 있으나, 퇴직자 증가로 노사갈등 이슈는 Peak-out 한 것으로 판단되며, 산업트렌드에 맞는 유연한 생산구조를 갖출 수 있게 될 전망. 목표주가 산정기준을 2019년에서 2019년, 2020년 평균을 적용, Target Valuation은 유지하여 목표주가를 160,000원으로 3.2%상향. 19년도 하반기 에 업종 Top-pick으로 제시, 현대차-친환경차 No.2 를 향해, E-GMP 공개, 게임 체인저를 향해, 미국시장 HEV 도입으로 유럽 OEM들과의 격차 본격화, 펠리세이드의 미국시장 landing 이후부터 주가 재평가 기대, 투자의견 BUY유지, 목표주가 170,000원 유지, 현대차-시장기대치 상회 실적 지속될 전망, 인센티브 방향성 전환 = 이익 방향성 전환, 19년 영업이익, 시장 기대치 +16% 상회 전망 → 기업가치 회복 지속 전망, 현대차 지배구조 개편 언제쯤…합병비율 산 넘을까, '좀비기업' 된 우버... '공유경제'는 사기다, "카카오 주식 매수 의견 유지", 카카오톡 기반 광고매출 본격화, "현대차 주가 상승 예상", SUV 팰리세이드 수출 실적에 반영, "현대모비스 주식 매수 의견 유지", 전기차 부품 공급 대폭 늘어나</t>
+    <t>제네시스, 서울을 대표하는 브랜드가 된다, 한국시장과 미국시장에서 제네시스는 Flagship 모델로서 트래픽 증가 역할과 수익원이 될 전망. 제네시스GV80, G80은 한국공장 수출 모델로 원화약세와 맞물려 신차효과가 극대화 될 전망, 19년도 3분기 에 소형SUV 베뉴, 그랜져F/L, 19년도 4분기 에 GV80, 20년도 1분기 에 G80으로 이어지는 신차출시의 특징은 디자인 혁신과 Connectivity, 3분기에 한국공장 노조파업이 단기리스크가 될 수 있으나, 퇴직자 증가로 노사갈등 이슈는 Peak-out 한 것으로 판단되며, 산업트렌드에 맞는 유연한 생산구조를 갖출 수 있게 될 전망. 목표주가 산정기준을 2019년에서 2019년, 2020년 평균을 적용, Target Valuation은 유지하여 목표주가를 160,000원으로 3.2%상향. 19년도 하반기 에 업종 Top-pick으로 제시, 친환경차 No.2 를 향해, E-GMP 공개, 게임 체인저를 향해, 미국시장 HEV 도입으로 유럽 OEM들과의 격차 본격화, 펠리세이드의 미국시장 landing 이후부터 주가 재평가 기대, 투자의견 BUY유지, 목표주가 170,000원 유지, 시장기대치 상회 실적 지속될 전망, 인센티브 방향성 전환 = 이익 방향성 전환, 19년 영업이익, 시장 기대치 +16% 상회 전망 → 기업가치 회복 지속 전망, 현대차 지배구조 개편 언제쯤…합병비율 산 넘을까, '좀비기업' 된 우버... '공유경제'는 사기다, "카카오 주식 매수 의견 유지", 카카오톡 기반 광고매출 본격화, "현대차 주가 상승 예상", SUV 팰리세이드 수출 실적에 반영, "현대모비스 주식 매수 의견 유지", 전기차 부품 공급 대폭 늘어나</t>
   </si>
   <si>
     <t>이철영 현대해상 대표이사 부회장</t>
@@ -5224,7 +5224,7 @@
     <t>글로벌 업체, 사활 건 전기차 전쟁</t>
   </si>
   <si>
-    <t>현대차-별도 부문과 북미 법인의 수익성 회복, 별도 부문 손익 2018년 상반기 수준 회복, 북미 법인의 수익성 회복, 원/달러 환율 상승, 하반기 북미 지역 신차 회복 투입 본격화, "현대차 주식 오를 힘 다져", 국내 이어 하반기 미국에서 신차효과, 위즈도메인 “하반기 특허공유플랫폼 출시할것”</t>
+    <t>별도 부문과 북미 법인의 수익성 회복, 별도 부문 손익 2018년 상반기 수준 회복, 북미 법인의 수익성 회복, 원/달러 환율 상승, 하반기 북미 지역 신차 회복 투입 본격화, "현대차 주식 오를 힘 다져", 국내 이어 하반기 미국에서 신차효과, 위즈도메인 “하반기 특허공유플랫폼 출시할것”</t>
   </si>
   <si>
     <t>美트럼프 "멕시코에 최대 25% 관세" 발표…기아차 긴장</t>
@@ -5233,13 +5233,13 @@
     <t>‘우파 실물경제학자’ 김정호 전 자유기업원 원장, 6월 3일 주요공시, 주식 1주도 없이 기업을 지배하는 방법</t>
   </si>
   <si>
-    <t>“현대차 주식은 하반기 자동차업종 최선호주", 신차효과 미국으로 확대, 이노션 - 미주지역 고성장 및 M&amp;A의 기대 유효, 현대차-신차 모멘텀, 국내에서 북미 시장으로, 상반기, 신차 효과로 국내 시장 석권, 하반기 신차 효과, 북미 시장으로 확대, 2019년 하반기 Top Pick</t>
+    <t>“현대차 주식은 하반기 자동차업종 최선호주", 신차효과 미국으로 확대, 이노션 - 미주지역 고성장 및 M&amp;A의 기대 유효, 신차 모멘텀, 국내에서 북미 시장으로, 상반기, 신차 효과로 국내 시장 석권, 하반기 신차 효과, 북미 시장으로 확대, 2019년 하반기 Top Pick</t>
   </si>
   <si>
     <t>현대차 - 국내별도부문·북미법인 수익성회복으로 국내와 미국시장 쌍끌이 실적개선 예상</t>
   </si>
   <si>
-    <t>현대차-업황 부진 지속과 SUV의 하드캐리, 2019년 5월 판매 현황 및 하반기 판매 전망, 투자의견 매수 유지, 목표주가 178,000원으로 상향, 국민연금, 5%이상 지분 100개사 주식투자 재미 못 봐...삼성물산·SK㈜가 악영향, "이노션 주가 오를 힘 키워", 현대차 신차 출시 따른 광고 늘어, 행동주의 펀드, 국내 증시에서 목소리 높인다</t>
+    <t>업황 부진 지속과 SUV의 하드캐리, 2019년 5월 판매 현황 및 하반기 판매 전망, 투자의견 매수 유지, 목표주가 178,000원으로 상향, 국민연금, 5%이상 지분 100개사 주식투자 재미 못 봐...삼성물산·SK㈜가 악영향, "이노션 주가 오를 힘 키워", 현대차 신차 출시 따른 광고 늘어, 행동주의 펀드, 국내 증시에서 목소리 높인다</t>
   </si>
   <si>
     <t>신라젠 시가총액 7317억↓…지난달 부울경 상위 상장사 고전</t>
@@ -5248,13 +5248,13 @@
     <t>KB운용, 지배구조 개편+주가 상승 '두마리 토끼' 잡았다</t>
   </si>
   <si>
-    <t>현대차-GENESIS가 이끄는 질적 성장, GENESIS 브랜드 독립 출시 4년, 서서히 보이는 가능성, GENESIS가 이끄는 ASP 인상 효과가 2022년 기대, ASP 상승을 통한 원재료 부담 완화, 수익성 개선 기대, 박한우 기아자동차 대표이사 사장, 현대차-년도년도 하반기 하반기 : 판매 차종의 변화 수혜, 차종 비중 변경에 따른 수익성 개선 전망, 년도년도 하반기 하반기 : 무역전쟁, 지배구조 개편 및 리콜이라는 3가지 요소, 투자의견: BUY, 목표주가 18만원 유지, 현대중공업 사태, 스웨덴과 독일에서 배울 것: 복지국가</t>
+    <t>GENESIS가 이끄는 질적 성장, GENESIS 브랜드 독립 출시 4년, 서서히 보이는 가능성, GENESIS가 이끄는 ASP 인상 효과가 2022년 기대, ASP 상승을 통한 원재료 부담 완화, 수익성 개선 기대, 박한우 기아자동차 대표이사 사장, 년도년도 하반기 하반기 : 판매 차종의 변화 수혜, 차종 비중 변경에 따른 수익성 개선 전망, 년도년도 하반기 하반기 : 무역전쟁, 지배구조 개편 및 리콜이라는 3가지 요소, 투자의견: BUY, 목표주가 18만원 유지, 현대중공업 사태, 스웨덴과 독일에서 배울 것: 복지국가</t>
   </si>
   <si>
     <t>정교선, 1년 만에 현대그린푸드 주식 쇼핑 재개...왜?</t>
   </si>
   <si>
-    <t>현대차-2020년 영업이익이 5조원을 넘어선다면, 4월 이후 원/달러 환율 급상승 및 원/유로 전년동기비 상승 전환, 이종통화 환율 약세 개선 등 환율 여건 개선. 최근 팰리세이드, 쏘나타 등 신차 수출 확대로 수익성 개선을 감안 시 선적 이후 도매판매로 이어지는 19년도 하반기 이후 손익 개선 기대, 현대차는 국내 수출 매출액이 연결 매출액의 22.5%이며 평균환율 1% 변동 시, 2,431억원의 영업이익 변동. 19년도 1분기 말 이후 5% 급상승한 환율(1,190원 가정) 시 2020년 영업이익 5조원 상회 가능할 전망, 투자의견 BUY 유지, 목표주가 기존 170,000원에서 185,000원 8.8% 상향, 우호적 환율 여건을 반영한 이익 추정치 상향에 근거</t>
+    <t>2020년 영업이익이 5조원을 넘어선다면, 4월 이후 원/달러 환율 급상승 및 원/유로 전년동기비 상승 전환, 이종통화 환율 약세 개선 등 환율 여건 개선. 최근 팰리세이드, 쏘나타 등 신차 수출 확대로 수익성 개선을 감안 시 선적 이후 도매판매로 이어지는 19년도 하반기 이후 손익 개선 기대, 현대차는 국내 수출 매출액이 연결 매출액의 22.5%이며 평균환율 1% 변동 시, 2,431억원의 영업이익 변동. 19년도 1분기 말 이후 5% 급상승한 환율(1,190원 가정) 시 2020년 영업이익 5조원 상회 가능할 전망, 투자의견 BUY 유지, 목표주가 기존 170,000원에서 185,000원 8.8% 상향, 우호적 환율 여건을 반영한 이익 추정치 상향에 근거</t>
   </si>
   <si>
     <t>이재웅 쏘카 대표이사</t>
@@ -5266,7 +5266,7 @@
     <t>정의선 부회장, 현대차그룹 ‘지배구조 개편’ 카드 언제 꺼내나, 日, 美·EU와 수소동맹 추진…한국만 쏙 뺀 이유는?</t>
   </si>
   <si>
-    <t>19일 장 마감 후 주요 종목 뉴스, 일등 브라질펀드 '0%대 경제성장률'에도 괜찮을까, 현대차-미국시장: RV라는 밀물이 들어온다, 예상보다 더 좋은 미국, 미국: 국내과 더불어 2H 실적의 견인차 역할, 미국 판매 순항 중이나 몇 가지 변수 대기 중</t>
+    <t>19일 장 마감 후 주요 종목 뉴스, 일등 브라질펀드 '0%대 경제성장률'에도 괜찮을까, 미국시장: RV라는 밀물이 들어온다, 예상보다 더 좋은 미국, 미국: 국내과 더불어 2H 실적의 견인차 역할, 미국 판매 순항 중이나 몇 가지 변수 대기 중</t>
   </si>
   <si>
     <t>사모펀드, 적인가 동지인가?, 19일 장 마감 후 주요 종목 뉴스, 잘나가는 새내기주 담는 공모주펀드 살까</t>
@@ -5281,7 +5281,7 @@
     <t>美증시 혼조…이란 갈등에 무역협상 불확실성, "현대차, 중국 판매 부진 속 2분기 실적 주목"</t>
   </si>
   <si>
-    <t>"현대차 등 완성차 영업이익 개선 추세", '무자본 M&amp;A'로 상장사 망친 기업사냥꾼, 현대차-수익성 개선 시작, 2019년 매출액 100조원, 영업이익 4조원 상회 전망, 2분기 Preview: 큰 폭의 영업이익 개선</t>
+    <t>"현대차 등 완성차 영업이익 개선 추세", '무자본 M&amp;A'로 상장사 망친 기업사냥꾼, 수익성 개선 시작, 2019년 매출액 100조원, 영업이익 4조원 상회 전망, 2분기 Preview: 큰 폭의 영업이익 개선</t>
   </si>
   <si>
     <t>'3세 경영' 돌입 정의선호…현대차그룹 지배구조 개편 시나리오는?, 수소차株, 현대차-사우디 아람코와 동맹 소식에 '급등', 수소차株, 현대차-사우디 동맹 소식에 강세, 현대차, 사우디 아람코와 맞손…투자자들, 수소차株 관심↑, 현대차, 사우디 아람코와 맞손…투자자들, 수소차株 관심↑</t>
@@ -5296,7 +5296,7 @@
     <t>무역休戰에도 코스피 부진…外人이 구세주?</t>
   </si>
   <si>
-    <t>현대차-GV80이 기대되는 이유, 19년도 2분기 , Preview: 현대차의 내수 판매 강세가 계속되고 있음, 하반기 제네시스 SUV 신차 기대, 방향성 확인 필요, 北·美·中·日 영향권에 놓인 한국 증시 하반기 전망은?</t>
+    <t>GV80이 기대되는 이유, 19년도 2분기 , Preview: 현대차의 내수 판매 강세가 계속되고 있음, 하반기 제네시스 SUV 신차 기대, 방향성 확인 필요, 北·美·中·日 영향권에 놓인 한국 증시 하반기 전망은?</t>
   </si>
   <si>
     <t>국민연금공단 외 1명 1.03%p 증가, 9.05% 보유, 대한민국 전자정보통신 산업발전사 프리뷰 &lt;2권 1990~2005년&gt;</t>
@@ -5305,22 +5305,22 @@
     <t>현대차_상장주식수 대비 거래량은 0.18%로 적정수준</t>
   </si>
   <si>
-    <t>손정의 회장의 제안은 항상 기간 인프라였다...문 대통령, 받을까?, 현대차-예상보다 좋았던 환율. 기대보다 좋을 신차 라인업, 2Q 기대치 부합. 3Q 적극적 매수 접근, 기대보다 좋을 신차 라인업, "현대차 주식 매수의견 유지", 베뉴 GV80 그랜저 G80 신차효과기대, "현대차 실적, 향후 출시 신차 라인업 주목"</t>
-  </si>
-  <si>
-    <t>차남규 한화생명 대표이사 부회장, 경동나비엔, 손연호 회장 일가 회사 '경동원'에 일감 몰빵…시민사회 "사익편취" 비판, 정유·자동차 실적개선 `훈풍`…반도체·헬스케어는 `안갯속`, 현대차-년도년도 1분기 2분기 Preview: 시장 기대치 상회, 연결 조정으로 일부 수익 3분기 이전, 년도년도 1분기 2분기 Preview: 시장 기대치 상회하는 호실적 전망, 내수 시장과 미국 시장 판매 호조, 연결 조정과 현대카드 마케팅 비용, 상반기보다 좋을 하반기, 현대차-년도년도 1분기 2분기 Preview: 예상 부합 후 하반기 신차 기대감 지속될 전망, 년도년도 1분기 2분기 연결 매출액 26.8조원(전년 대비 증감율 +8.6%), 영업이익 1.1조원(전년 대비 증감율 +15.6%) 전망, 자동차 부문 매출액 전년 대비 증감율 +10.4%, OPM 3.5% 예상, BHMC로부터의 지분법손실 100억원 예상, 현대차-높아진 기대, 넘치지도 부족하지도 않은, 년도년도 1분기 2분기 영업이익은 1.13조원 기록, 언/달러 환율이 당초 기대보다 낮아졌으나 년도년도 1분기 2분기 판매보증충당금 증가에는 제한적인 영향 준것으로 판단</t>
-  </si>
-  <si>
-    <t>현대차-해외에서 신차 효과를 기대할 때, 19년도 2분기 내수 신차효과와 우호적 환 효과가 실적 견인할 전망, 19년도 하반기 에는 신차효과가 해외에서도 기대, “현대글로비스 주식 매수의견 유지”, 2분기부터 이익 안정화 국면, 올 들어 대차잔고 `최대`…韓日 경제전쟁 틈타 공매도 기승 우려, 공매도 증가에 … 올 대차잔고 55兆 `최대`, 두올산업, BK 지분 57% 산다…빗썸, 우회상장하나?</t>
+    <t>손정의 회장의 제안은 항상 기간 인프라였다...문 대통령, 받을까?, 예상보다 좋았던 환율. 기대보다 좋을 신차 라인업, 2Q 기대치 부합. 3Q 적극적 매수 접근, 기대보다 좋을 신차 라인업, "현대차 주식 매수의견 유지", 베뉴 GV80 그랜저 G80 신차효과기대, "현대차 실적, 향후 출시 신차 라인업 주목"</t>
+  </si>
+  <si>
+    <t>차남규 한화생명 대표이사 부회장, 경동나비엔, 손연호 회장 일가 회사 '경동원'에 일감 몰빵…시민사회 "사익편취" 비판, 정유·자동차 실적개선 `훈풍`…반도체·헬스케어는 `안갯속`, 년도년도 1분기 2분기 Preview: 시장 기대치 상회, 연결 조정으로 일부 수익 3분기 이전, 년도년도 1분기 2분기 Preview: 시장 기대치 상회하는 호실적 전망, 내수 시장과 미국 시장 판매 호조, 연결 조정과 현대카드 마케팅 비용, 상반기보다 좋을 하반기, 년도년도 1분기 2분기 Preview: 예상 부합 후 하반기 신차 기대감 지속될 전망, 년도년도 1분기 2분기 연결 매출액 26.8조원(전년 대비 증감율 +8.6%), 영업이익 1.1조원(전년 대비 증감율 +15.6%) 전망, 자동차 부문 매출액 전년 대비 증감율 +10.4%, OPM 3.5% 예상, BHMC로부터의 지분법손실 100억원 예상, 높아진 기대, 넘치지도 부족하지도 않은, 년도년도 1분기 2분기 영업이익은 1.13조원 기록, 언/달러 환율이 당초 기대보다 낮아졌으나 년도년도 1분기 2분기 판매보증충당금 증가에는 제한적인 영향 준것으로 판단</t>
+  </si>
+  <si>
+    <t>해외에서 신차 효과를 기대할 때, 19년도 2분기 내수 신차효과와 우호적 환 효과가 실적 견인할 전망, 19년도 하반기 에는 신차효과가 해외에서도 기대, “현대글로비스 주식 매수의견 유지”, 2분기부터 이익 안정화 국면, 올 들어 대차잔고 `최대`…韓日 경제전쟁 틈타 공매도 기승 우려, 공매도 증가에 … 올 대차잔고 55兆 `최대`, 두올산업, BK 지분 57% 산다…빗썸, 우회상장하나?</t>
   </si>
   <si>
     <t>현대위아 - 기아차 향 매출 뚜렷한 증가에 따른 이익개선 기대, TheCapitalGroupCompanies,Inc. 외, (9일) 현대자동차 등</t>
   </si>
   <si>
-    <t>현대차-가시화되는 구조적 실적개선, 19년도 2분기 Preview-영업이익 1.1조원(전년 대비 증감율 +14.2%, OPM 4.1%) 전망, 선순환에 대한 기대, 실적 개선 가시성 확보</t>
-  </si>
-  <si>
-    <t>국내 애플 앱스토어, ‘카카오페이’로 결제 가능해진다, 2Q 예상 순이익증가율 1위 운송물류주는 현대글로비스. 왜?, 현대차-19년도 2분기 Preview, 높아진 컨센서스 부합 전망 / TP 17 만원 (M), 투자의견 BUY(M)</t>
+    <t>가시화되는 구조적 실적개선, 19년도 2분기 Preview-영업이익 1.1조원(전년 대비 증감율 +14.2%, OPM 4.1%) 전망, 선순환에 대한 기대, 실적 개선 가시성 확보</t>
+  </si>
+  <si>
+    <t>국내 애플 앱스토어, ‘카카오페이’로 결제 가능해진다, 2Q 예상 순이익증가율 1위 운송물류주는 현대글로비스. 왜?, 19년도 2분기 Preview, 높아진 컨센서스 부합 전망 / TP 17 만원 (M), 투자의견 BUY(M)</t>
   </si>
   <si>
     <t>곳곳 암초…10대그룹 초라한 ‘주가 성적표’, 두올산업 이창현 대표 "빗썸 직접 인수 아냐…BTHMB 지분투자 제안한 상태"</t>
@@ -5329,10 +5329,10 @@
     <t>대우조선 등 조선株 수주 기대↑…실적 개선 영원무역·한세실업 관심, 대외악재에 휩쓸린 증시…"현대·기아차·아모레 등 저평가株 주목", 국민연금, 10대그룹 지분가치 7.7兆 늘어, 美中 무역전쟁·日 수출 규제…신중한 자세로 시장 접근</t>
   </si>
   <si>
-    <t>현대차-2분기 예상실적 및 투자포인트, 신차 효과와 환율 효과로 2분기 영업이익은 전년동기대비 27.0% 증가한 1.2조원(OPM 4.6%)을 기록할 전망, 2019년 연간 영업이익은 전년대비 80.5% 증가한 4.3조원을 전망함. 기저 효과에 의한 반등 이상의 실적 개선 보여줄 것, 신형 팰리세이드, 쏘나타의 글로벌 신차 효과가 하반기부터 본격화 됨. 신형 GV80 출시로 기대하던 제네시스의 SUV 라인업이 확충됨, 신규 파워트레인(스마트 스트림) 싸이클 돌입함에 따라 연비 및 상품성 개선이 확연이 나타남, 메트라이프, 변액보험 상위권 독식 비결은</t>
-  </si>
-  <si>
-    <t>빌 게이츠, 아르노 루이비통 회장에 밀려 세계 부자 3위로, 현대차-싸우지 마세요, 노사분규로 인한 3분기 실적 우려가 부각되며 주가 약세, 파업을 미리 걱정하는 시장, 전운 너머로 보이는 무지개를 보자</t>
+    <t>2분기 예상실적 및 투자포인트, 신차 효과와 환율 효과로 2분기 영업이익은 전년동기대비 27.0% 증가한 1.2조원(OPM 4.6%)을 기록할 전망, 2019년 연간 영업이익은 전년대비 80.5% 증가한 4.3조원을 전망함. 기저 효과에 의한 반등 이상의 실적 개선 보여줄 것, 신형 팰리세이드, 쏘나타의 글로벌 신차 효과가 하반기부터 본격화 됨. 신형 GV80 출시로 기대하던 제네시스의 SUV 라인업이 확충됨, 신규 파워트레인(스마트 스트림) 싸이클 돌입함에 따라 연비 및 상품성 개선이 확연이 나타남, 메트라이프, 변액보험 상위권 독식 비결은</t>
+  </si>
+  <si>
+    <t>빌 게이츠, 아르노 루이비통 회장에 밀려 세계 부자 3위로, 싸우지 마세요, 노사분규로 인한 3분기 실적 우려가 부각되며 주가 약세, 파업을 미리 걱정하는 시장, 전운 너머로 보이는 무지개를 보자</t>
   </si>
   <si>
     <t>경기 방어주로 주목받는 현대차그룹…"1년만에 달라졌다"</t>
@@ -5344,10 +5344,10 @@
     <t>"오너물량 안나온다"…외국인 오토에버 `찜`</t>
   </si>
   <si>
-    <t>현대차-믹스 개선 효과 시작, 19년도 2분기 영업이익 1조 2,377억원(전년 대비 증감율 +30.2%)을 기록하며 시장 예상을 상회. 자동차 부문의 수익성이 예상을 크게 상회했음. 지분법손익 부진으로 순이익은 예상 부합, 호실적에 양호한 주가 흐름 예상. 3분기는 영업일수도 감소하고 하투(夏鬪)가 확대될 시 전분기 대비 증감율 감익이 불가피하겠으나 신차효과에 따른 믹스개선은 하반기 들어서며 강해질 전망. 하반기 미국 팰리세이드 판매 본격화, 내수 GV80 등 출시 예정, 상기 신차에 대한 반응 호조 시 믹스 개선에 따른 실적 회복 기대감이 지속되며 주가는 지지될 수 있을 전망. 당사는 재고소진이 마무리 된 중국 시장 수요가 하반기 중 회복될 것으로 기대하는데, 현실화 될 경우 추가 상승 동력이 될 수 있을 것으로 전망, 정의선 현대자동차그룹 총괄 수석부회장, 日연기금, 코스피에 6조원 투자…韓 흔들면 자국민 노후 `휘청`, 현대차-년도년도 1분기 2분기 Review: 또 다시 어려운 시소타기로, 년도년도 1분기 2분기 실적은 매출액 및 영업이익은 당사 기대치 부합. 중국 지분법 손익 악화로 순이익은 당사 추정치 하회. 중국지분법이익은 -1500억원 이상으로 추정되며, 재고처분을 위한 인센티브 증가와 부품사 단가보전 영향으로 추정, 글로벌 수요감소폭 확대로 업종 실적회복에 대한 확신이 낮아지고 있음. 수요일 발표되는 모비스 실적이 견조할 경우, 단기간에 업종 내에서 부품사로 수급이 이동할 가능성 높음, 현대차의 Turnaround는 미국 및 한국판매에 의존. 년도년도 1분기 3분기 에 파업 시 타격이 클 수 있어 노사협상이 마무리되는 년도년도 1분기 3분기 말까지 업종 전반의 주가는 횡보 예상</t>
-  </si>
-  <si>
-    <t>시장심리 톱5, 현대차·신한지주·삼성카드·아모레퍼시픽·셀트리온, 현대차-파업 너머 보이는 무지개, 2분기 실적은 우호적 환율 속 신차 판매가 늘고 믹스가 개선되며 컨센 7% 상회, 신차 상품성 회복을 통한 글로벌 점유율 상승에 주목할 시점, 최근 파업 우려로 인한 조정은 비중을 늘릴 기회, 현대차-궤도에 오른 사이클을 확인, 19년도 2분기 Review: 높아진 컨센서스를 상회, 부진한 업황 속 경쟁력 강화, 다만 비용은 우려 요인, 투자의견 매수, 목표주가 178,000원 유지, 현대차-년도년도 1분기 2분기 Review: 실적 기대치 상회, 하반기 전망도 긍정적, 년도년도 1분기 2분기 Review: 환율 신차 효과로 기대치 상회, 2분기 보수적인 비용 수익 인식은 하반기 실적의 완충 역할 해줄 것, 하반기에도 실적 개선 추세 유지될 것, 현대차-영업지표 개선 선순환 Cycle 진입, 두 분기 연속 시장기대치 상회 실적 실현, 19년도 1분기 , 19년도 2분기 모두 높아진 실적 눈높이를 다시금 상회, 우려요인인 파업이 경상적 수준에 머문다면 19년도 3분기 또한 기대치 상회실적 가능, 현대차-On track, 제품 경쟁력 강화로 중장기 실적 개선 기대, 2분기 Review-판매믹스개선, 원화약세 효과, 현대차-기대했던 수준의 호실적 시현, 2Q 19 Review: 높아진 시장 기대치에 부합하는 실적 시현!, SUV 비중 40%, 판매믹스 개선은 지속 중, 현대차-Company Comment, 19년도 2분기 는 시장기대치 상회하는 실적 기록, 미국시장 턴어라운드 기대, 세원정공, 日 탄소섬유 수출 규제 확산에 '급등', 현대차-자동차 개선 지속, 높아진 기대 상회, 19년도 2분기 영업이익은 1.24조원 기록, 컨센서스 7.0% 상회, 북미 19년도 하반기 SUV 신차 텔루라이드, 베뉴 출시로 점유율 상승, 플릿 축소, 인센티브 하락 등 체질 개선을 통한 손익 가시화 전망, 최태원 SK그룹 회장, 현대차-자동차 부문의 마진 개선 확인, 2분기 영업이익 1.24조원(+30.2%)으로 시장 기대치 +7.0% 상회, 계절성을 제외하면 꾸준한 성장 곡선의 지속, 현대차-On track, 제품 경쟁력 강화로 중장기 실적 개선 기대, 2분기 Review-판매믹스개선, 원화약세 효과, 현대차-영업지표 개선 선순환 Cycle 진입, 두 분기 연속 시장기대치 상회 실적 실현, 19년도 1분기 , 19년도 2분기 모두 높아진 실적 눈높이를 다시금 상회, 우려요인인 파업이 경상적 수준에 머문다면 19년도 3분기 또한 기대치 상회실적 가능, 현대차-년도년도 1분기 2분기 Review: 실적 기대치 상회, 하반기 전망도 긍정적, 년도년도 1분기 2분기 Review: 환율 신차 효과로 기대치 상회, 2분기 보수적인 비용 수익 인식은 하반기 실적의 완충 역할 해줄 것, 하반기에도 실적 개선 추세 유지될 것, 현대차-궤도에 오른 사이클을 확인, 19년도 2분기 Review: 높아진 컨센서스를 상회, 부진한 업황 속 경쟁력 강화, 다만 비용은 우려 요인, 투자의견 매수, 목표주가 178,000원 유지, 현대차-파업 너머 보이는 무지개, 2분기 실적은 우호적 환율 속 신차 판매가 늘고 믹스가 개선되며 컨센 7% 상회, 신차 상품성 회복을 통한 글로벌 점유율 상승에 주목할 시점, 최근 파업 우려로 인한 조정은 비중을 늘릴 기회, 김상조 청와대 정책실장</t>
+    <t>믹스 개선 효과 시작, 19년도 2분기 영업이익 1조 2,377억원(전년 대비 증감율 +30.2%)을 기록하며 시장 예상을 상회. 자동차 부문의 수익성이 예상을 크게 상회했음. 지분법손익 부진으로 순이익은 예상 부합, 호실적에 양호한 주가 흐름 예상. 3분기는 영업일수도 감소하고 하투(夏鬪)가 확대될 시 전분기 대비 증감율 감익이 불가피하겠으나 신차효과에 따른 믹스개선은 하반기 들어서며 강해질 전망. 하반기 미국 팰리세이드 판매 본격화, 내수 GV80 등 출시 예정, 상기 신차에 대한 반응 호조 시 믹스 개선에 따른 실적 회복 기대감이 지속되며 주가는 지지될 수 있을 전망. 당사는 재고소진이 마무리 된 중국 시장 수요가 하반기 중 회복될 것으로 기대하는데, 현실화 될 경우 추가 상승 동력이 될 수 있을 것으로 전망, 정의선 현대자동차그룹 총괄 수석부회장, 日연기금, 코스피에 6조원 투자…韓 흔들면 자국민 노후 `휘청`, 년도년도 1분기 2분기 Review: 또 다시 어려운 시소타기로, 년도년도 1분기 2분기 실적은 매출액 및 영업이익은 당사 기대치 부합. 중국 지분법 손익 악화로 순이익은 당사 추정치 하회. 중국지분법이익은 -1500억원 이상으로 추정되며, 재고처분을 위한 인센티브 증가와 부품사 단가보전 영향으로 추정, 글로벌 수요감소폭 확대로 업종 실적회복에 대한 확신이 낮아지고 있음. 수요일 발표되는 모비스 실적이 견조할 경우, 단기간에 업종 내에서 부품사로 수급이 이동할 가능성 높음, 현대차의 Turnaround는 미국 및 한국판매에 의존. 년도년도 1분기 3분기 에 파업 시 타격이 클 수 있어 노사협상이 마무리되는 년도년도 1분기 3분기 말까지 업종 전반의 주가는 횡보 예상</t>
+  </si>
+  <si>
+    <t>시장심리 톱5, 현대차·신한지주·삼성카드·아모레퍼시픽·셀트리온, 파업 너머 보이는 무지개, 2분기 실적은 우호적 환율 속 신차 판매가 늘고 믹스가 개선되며 컨센 7% 상회, 신차 상품성 회복을 통한 글로벌 점유율 상승에 주목할 시점, 최근 파업 우려로 인한 조정은 비중을 늘릴 기회, 궤도에 오른 사이클을 확인, 19년도 2분기 Review: 높아진 컨센서스를 상회, 부진한 업황 속 경쟁력 강화, 다만 비용은 우려 요인, 투자의견 매수, 목표주가 178,000원 유지, 년도년도 1분기 2분기 Review: 실적 기대치 상회, 하반기 전망도 긍정적, 년도년도 1분기 2분기 Review: 환율 신차 효과로 기대치 상회, 2분기 보수적인 비용 수익 인식은 하반기 실적의 완충 역할 해줄 것, 하반기에도 실적 개선 추세 유지될 것, 영업지표 개선 선순환 Cycle 진입, 두 분기 연속 시장기대치 상회 실적 실현, 19년도 1분기 , 19년도 2분기 모두 높아진 실적 눈높이를 다시금 상회, 우려요인인 파업이 경상적 수준에 머문다면 19년도 3분기 또한 기대치 상회실적 가능, On track, 제품 경쟁력 강화로 중장기 실적 개선 기대, 2분기 Review-판매믹스개선, 원화약세 효과, 기대했던 수준의 호실적 시현, 2Q 19 Review: 높아진 시장 기대치에 부합하는 실적 시현!, SUV 비중 40%, 판매믹스 개선은 지속 중, Company Comment, 19년도 2분기 는 시장기대치 상회하는 실적 기록, 미국시장 턴어라운드 기대, 세원정공, 日 탄소섬유 수출 규제 확산에 '급등', 자동차 개선 지속, 높아진 기대 상회, 19년도 2분기 영업이익은 1.24조원 기록, 컨센서스 7.0% 상회, 북미 19년도 하반기 SUV 신차 텔루라이드, 베뉴 출시로 점유율 상승, 플릿 축소, 인센티브 하락 등 체질 개선을 통한 손익 가시화 전망, 최태원 SK그룹 회장, 자동차 부문의 마진 개선 확인, 2분기 영업이익 1.24조원(+30.2%)으로 시장 기대치 +7.0% 상회, 계절성을 제외하면 꾸준한 성장 곡선의 지속, On track, 제품 경쟁력 강화로 중장기 실적 개선 기대, 2분기 Review-판매믹스개선, 원화약세 효과, 영업지표 개선 선순환 Cycle 진입, 두 분기 연속 시장기대치 상회 실적 실현, 19년도 1분기 , 19년도 2분기 모두 높아진 실적 눈높이를 다시금 상회, 우려요인인 파업이 경상적 수준에 머문다면 19년도 3분기 또한 기대치 상회실적 가능, 년도년도 1분기 2분기 Review: 실적 기대치 상회, 하반기 전망도 긍정적, 년도년도 1분기 2분기 Review: 환율 신차 효과로 기대치 상회, 2분기 보수적인 비용 수익 인식은 하반기 실적의 완충 역할 해줄 것, 하반기에도 실적 개선 추세 유지될 것, 궤도에 오른 사이클을 확인, 19년도 2분기 Review: 높아진 컨센서스를 상회, 부진한 업황 속 경쟁력 강화, 다만 비용은 우려 요인, 투자의견 매수, 목표주가 178,000원 유지, 파업 너머 보이는 무지개, 2분기 실적은 우호적 환율 속 신차 판매가 늘고 믹스가 개선되며 컨센 7% 상회, 신차 상품성 회복을 통한 글로벌 점유율 상승에 주목할 시점, 최근 파업 우려로 인한 조정은 비중을 늘릴 기회, 김상조 청와대 정책실장</t>
   </si>
   <si>
     <t>3Q 예상 순이익증가율 1위 자동차주는 현대차. 왜?, 주식시장으로 본 車업계…“신차 사이클로 점유율 회복”, 실적으로 보여준 정의선의 자신감, 미뤘던 지배구조개편 판 벌일까(?)</t>
@@ -5362,7 +5362,7 @@
     <t>KCC 정몽익 독립의 발판 '1000억 자금줄' 코리아오토글라스, 증시 뉴페이스 대해부-웹케시(경리 SW)·플리토(AI 번역)·천보(디스플레이 소재)·에이스토리(드라마 제작) 전도유망, 독립경영 나서는 KCC 삼형제…신설·존속 법인 경쟁력과 전망은</t>
   </si>
   <si>
-    <t>현대차-국내외 Kona EV 화재 사고, 주가에 큰 영향 미칠 요인 아닐 것, 국내와 캐나다에서 현대 Kona EV와 관련된 화재 발생했지만 주가에 미치는 영향은 약할 것, 화재가 EV만의 문제는 아님. 캐나다 사고의 경우 일반적인 EV 사고와는 다른 양상 보임, 현대차 주가에 미칠 영향은 낮다는 판단</t>
+    <t>국내외 Kona EV 화재 사고, 주가에 큰 영향 미칠 요인 아닐 것, 국내와 캐나다에서 현대 Kona EV와 관련된 화재 발생했지만 주가에 미치는 영향은 약할 것, 화재가 EV만의 문제는 아님. 캐나다 사고의 경우 일반적인 EV 사고와는 다른 양상 보임, 현대차 주가에 미칠 영향은 낮다는 판단</t>
   </si>
   <si>
     <t>미국, 기준금리 0.25p 인하…보유자산 축소 프로그램 종료 예정, 트럼프 “파월이 실망시켜…연준 도움 안 된다”, 한국일본 갈등 변곡점 맞나, 6월 제조업 생산소비 모두 하락, 삼성전자 “반도체 인위적</t>
@@ -5407,28 +5407,28 @@
     <t>연기금, 이달 들어 2兆 풀었지만…삼성전자·현대車 등 대형주만 편식, 대형주만 편식하는 연기금</t>
   </si>
   <si>
-    <t>현대차-노이즈를 제품으로 극복한다, 10년만의 대형 신차 교체주기 진행 중, BEV: ‘21년 대거 출시에 따른 수익성 방어는 RV가 담당</t>
-  </si>
-  <si>
-    <t>현대자동차 노사합의 경제적 가치는.."최대 6000억원대 영업이익 효과", 완성차 '형님' 덕에…자금조달 숨통 트인 車 부품사들, 현대차-현대차 노사, 8년 만의 무분규 임단협 잠정협의, 현대차 노조, 8년 만의 무분규 임단협 잠정합의, 전년대비 완화된 임금 인상. 통상임금 관련해서는 노사의 안이 절충을 이룬 것으로 보임, 우선주 포함 시가총액 대비 1.2~2.0% 수준의 영업이익 개선 예상, 현대차 "무분규 임단협 합의"...장초반 주가 '껑충', 한국경제 반등 어려운 3가지 이유, 현대차그룹株 일제 상승···'무분규 임단협'에 주가도 '훈풍', 코스피, 미국發 경기둔화 우려에도 상승출발…외국인 '사자'</t>
-  </si>
-  <si>
-    <t>현대글로비스 - 3분기 사상최대 영업이익 달성 가시화·원/달러 환율 상승 수혜 예상, 현대차-노사관계도 비정상의 정상화, 8년 만에 무분규 임금협상 합의, 3분기 컨센서스 상승 이어질 것, 강성노조 문제도 완화될 전망, 현대차-우선주에도 관심을 가질 시기, 현대차 보통주의 주가상승 기대. 우선주도 배당 관점에서 매력적, 현대차는 3종의 우선주를 발행, 5% 대 배당수익률 기록. 보통주와의 괴리율도 2015년 이후 최대, “현대차, 5% 대 배당수익률 기록. 보통주와의 괴리율도 2015년 이후 최대”, 홀로서기 나선 어펄마캐피탈, 기분좋은 새출발, "현대차 주식 매수의견 유지", 판매호조에 노사관계 비정상의 정상화</t>
+    <t>노이즈를 제품으로 극복한다, 10년만의 대형 신차 교체주기 진행 중, BEV: ‘21년 대거 출시에 따른 수익성 방어는 RV가 담당</t>
+  </si>
+  <si>
+    <t>현대자동차 노사합의 경제적 가치는.."최대 6000억원대 영업이익 효과", 완성차 '형님' 덕에…자금조달 숨통 트인 車 부품사들, 현대차 노사, 8년 만의 무분규 임단협 잠정협의, 현대차 노조, 8년 만의 무분규 임단협 잠정합의, 전년대비 완화된 임금 인상. 통상임금 관련해서는 노사의 안이 절충을 이룬 것으로 보임, 우선주 포함 시가총액 대비 1.2~2.0% 수준의 영업이익 개선 예상, 현대차 "무분규 임단협 합의"...장초반 주가 '껑충', 한국경제 반등 어려운 3가지 이유, 현대차그룹株 일제 상승···'무분규 임단협'에 주가도 '훈풍', 코스피, 미국發 경기둔화 우려에도 상승출발…외국인 '사자'</t>
+  </si>
+  <si>
+    <t>현대글로비스 - 3분기 사상최대 영업이익 달성 가시화·원/달러 환율 상승 수혜 예상, 노사관계도 비정상의 정상화, 8년 만에 무분규 임금협상 합의, 3분기 컨센서스 상승 이어질 것, 강성노조 문제도 완화될 전망, 우선주에도 관심을 가질 시기, 현대차 보통주의 주가상승 기대. 우선주도 배당 관점에서 매력적, 현대차는 3종의 우선주를 발행, 5% 대 배당수익률 기록. 보통주와의 괴리율도 2015년 이후 최대, “현대차, 5% 대 배당수익률 기록. 보통주와의 괴리율도 2015년 이후 최대”, 홀로서기 나선 어펄마캐피탈, 기분좋은 새출발, "현대차 주식 매수의견 유지", 판매호조에 노사관계 비정상의 정상화</t>
   </si>
   <si>
     <t>외국인 8월 한국 주식 2조6천억어치 순매도, 삼성전자가 절반</t>
   </si>
   <si>
-    <t>두올 - 제네시스 GV80 수혜주로 주목, 윤석열號 첫 검찰 인사에 담긴 ‘메시지’, 현대차-본격 비중확대 시점, 19년도 2분기 Review: 영업이익 1.24조원(전년 대비 증감율 +30.2%) 기록, 2개분기 연속 상회, 매출 상승 Cycle에 본격 진입하다! 19년도 3분기 도 기대, 친환경차 출시 본격화, 유럽 현지생산으로 M/S 확대 기대, 목표주가 180,000원, 투자의견 BUY 유지</t>
-  </si>
-  <si>
-    <t>심상찮은 '기업 위기론'··· 투기자본 경영권 공격 가능성 고조, 해외 투기자본에 무방비로 노출된 기업들…재계 "포이즌필 등 경영권 방어수단 법제화해야", 현대차-전기차 언더독에서 주류로, 과소평가된 친환경차 경쟁력, 출시 전략 가속화, 글로벌 친환경차 점유율 상승, 경쟁사 대비 돈을 버는 시기가 빨라진다</t>
+    <t>두올 - 제네시스 GV80 수혜주로 주목, 윤석열號 첫 검찰 인사에 담긴 ‘메시지’, 본격 비중확대 시점, 19년도 2분기 Review: 영업이익 1.24조원(전년 대비 증감율 +30.2%) 기록, 2개분기 연속 상회, 매출 상승 Cycle에 본격 진입하다! 19년도 3분기 도 기대, 친환경차 출시 본격화, 유럽 현지생산으로 M/S 확대 기대, 목표주가 180,000원, 투자의견 BUY 유지</t>
+  </si>
+  <si>
+    <t>심상찮은 '기업 위기론'··· 투기자본 경영권 공격 가능성 고조, 해외 투기자본에 무방비로 노출된 기업들…재계 "포이즌필 등 경영권 방어수단 법제화해야", 전기차 언더독에서 주류로, 과소평가된 친환경차 경쟁력, 출시 전략 가속화, 글로벌 친환경차 점유율 상승, 경쟁사 대비 돈을 버는 시기가 빨라진다</t>
   </si>
   <si>
     <t>상승중인 주가에 영향 얼마나 미칠까?... 현대글로비스 운반선 '골든레이' 전도</t>
   </si>
   <si>
-    <t>현대차-전기차도, 수소차도 가능한 업체, 수소차 판매 초기 시장 진입, 2020년 유럽을 중심으로 친환경차 시장 확대, 삼성 이건희 지분가치 14조8천억…병상서도 주식부호 1위, 이건희 삼성전자 회장, 주식가치 15조원으로 1위 자리 '사수', 이재용 '주식감소액 1위' 이건희는 증가액 최다...삼성물산-삼성전자 가치에 엇갈려, 이건희 회장 보유주식 가치 15조....이중근 부영 회장도 10위권</t>
+    <t>전기차도, 수소차도 가능한 업체, 수소차 판매 초기 시장 진입, 2020년 유럽을 중심으로 친환경차 시장 확대, 삼성 이건희 지분가치 14조8천억…병상서도 주식부호 1위, 이건희 삼성전자 회장, 주식가치 15조원으로 1위 자리 '사수', 이재용 '주식감소액 1위' 이건희는 증가액 최다...삼성물산-삼성전자 가치에 엇갈려, 이건희 회장 보유주식 가치 15조....이중근 부영 회장도 10위권</t>
   </si>
   <si>
     <t>주식부자들 사이에서도 통한 ‘부익부 빈익빈’, 지엠비코리아 현대기아자동차 주식회사와 538억원 계약체결, 지엠비코리아 수주공시 - ITM(냉각수 유량 조절장치) 공급계약 538.9억원 (매출액대비 11.79%), 정몽구 정의선 현대차 계열사 주식가치 급감, 현대글로비스 하락 탓</t>
@@ -5443,7 +5443,7 @@
     <t>강남 좌파와 뉴욕증시 코리아 디스카운트, 국제 유가 급등 기로에 선 증시.. .SK텔레콤, KT, LG유플러스 등 '가치주' vs 삼성전자, 현대자동차, 현대중공업지주 등 '성장주', 어, 벌써 찬바람이…슬슬 배당주 사볼까, 유가 폭등 기로에 선 증시..'가치주' vs '성장주'</t>
   </si>
   <si>
-    <t>터지지 않는 거래량…현대오토에버, 개인 매수세에도 불안, 찬바람 불면 각광받는 '배당주'…증권가 추천 종목은, 개미 몰린 현대오토에버…터지지 않는 거래량 ‘고민’, 현대차-여전히 청산가치에 거래되고 있는 턴어라운드 기업, 존속 불가 기업 프레임을 겨우 벗어난 주가, 여전히 실적개선에 대한 기업가치 반영은 미진, 유럽 탄소배출 규제에 따른 과징금 부과 가능성 제한적, 경쟁우위의 EV 모델 출시와 플랫폼 상용화에 주목, [EBN 오늘(18일) 이슈 종합] 은성수 금융위원장 '소부장 펀드' 조성, LG전자·디스플레이, OLED 시장 선도 사활 등</t>
+    <t>터지지 않는 거래량…현대오토에버, 개인 매수세에도 불안, 찬바람 불면 각광받는 '배당주'…증권가 추천 종목은, 개미 몰린 현대오토에버…터지지 않는 거래량 ‘고민’, 여전히 청산가치에 거래되고 있는 턴어라운드 기업, 존속 불가 기업 프레임을 겨우 벗어난 주가, 여전히 실적개선에 대한 기업가치 반영은 미진, 유럽 탄소배출 규제에 따른 과징금 부과 가능성 제한적, 경쟁우위의 EV 모델 출시와 플랫폼 상용화에 주목, [EBN 오늘(18일) 이슈 종합] 은성수 금융위원장 '소부장 펀드' 조성, LG전자·디스플레이, OLED 시장 선도 사활 등</t>
   </si>
   <si>
     <t>미디어젠, IPO 주관 보수 '두둑'…신주인수권까지, 대형주만 쇼핑하는 연기금, "현대글로비스 주식 매수 신중해야", 지배구조 개편 불확실성 안아</t>
@@ -5461,16 +5461,16 @@
     <t>"현대차 자율주행 합작법인 설립은 긍정적 요인", 현대모비스 주가 '자율주행 투자'에 3%대 올라, 현대차 기아차는 보합, 현대차그룹株, 자율주행 합작사 설립에 일제히 '상승세', 현대차 자율주행법인 설립 소식에...만도 주가 '장중 급락', 현대모비스 창사이래 최대 자사주 매입...정의선 승계작업 재개 신호탄?, 현대모비스, "주주가치 높이려 자사주 130만주 취득", 대우부품·대한제당3우B·대성엘텍·코리아에프티·진바이오텍 上...차부품·돼지열병주 강세</t>
   </si>
   <si>
-    <t>트럼프 대통령 탄핵 조사 착수 여파는?…자율주행 수혜주 ‘주목’, 中 자동차 공장 가동률 추락…일부 업체 20%대, 현대차-년도년도 1분기 3분기 preview - 비용 기저효과, 세그먼트 대형화, 환율, 투자의견 Buy 유지, 목표주가 170,000원으로 13.3% 상향, 년도년도 1분기 3분기 영업이익 1.2조원으로 시장 컨센서스 6.6% 상회 예상, 판매보증비 축소, 세그먼트 대형화, 우호적 환율 등으로 영업이익 증가 예상, 유리한 환율, 신차 판매 기여, 무역 및 환경규제에 대한 적정한 대응이 투자의견의 핵심 가정, 필승코리아 펀드가 보여준 자산운용업계의 우울한 단면</t>
-  </si>
-  <si>
-    <t>현대차-CO2 감축 규제에 따른 완성차 영향 분석, 2020년 유럽내 평균 CO2 배출량 96gCO2/km으로 예상되어 규제 기준을 크게 벗어나지 않을 것으로 전망, 내연기관차 대비 원가율이 높은 친환경차 판매량 확대에 따른 수익성 일부 감소할 수 있으나, 볼륨 증가에 따른 친환경차 마진 개선도 함께 진행</t>
+    <t>트럼프 대통령 탄핵 조사 착수 여파는?…자율주행 수혜주 ‘주목’, 中 자동차 공장 가동률 추락…일부 업체 20%대, 년도년도 1분기 3분기 preview - 비용 기저효과, 세그먼트 대형화, 환율, 투자의견 Buy 유지, 목표주가 170,000원으로 13.3% 상향, 년도년도 1분기 3분기 영업이익 1.2조원으로 시장 컨센서스 6.6% 상회 예상, 판매보증비 축소, 세그먼트 대형화, 우호적 환율 등으로 영업이익 증가 예상, 유리한 환율, 신차 판매 기여, 무역 및 환경규제에 대한 적정한 대응이 투자의견의 핵심 가정, 필승코리아 펀드가 보여준 자산운용업계의 우울한 단면</t>
+  </si>
+  <si>
+    <t>CO2 감축 규제에 따른 완성차 영향 분석, 2020년 유럽내 평균 CO2 배출량 96gCO2/km으로 예상되어 규제 기준을 크게 벗어나지 않을 것으로 전망, 내연기관차 대비 원가율이 높은 친환경차 판매량 확대에 따른 수익성 일부 감소할 수 있으나, 볼륨 증가에 따른 친환경차 마진 개선도 함께 진행</t>
   </si>
   <si>
     <t>박윤식 한화손해보험 대표이사 사장, 정의선, 보호예수기간 끝난 현대오토에버 지분 9.6% 매각할까</t>
   </si>
   <si>
-    <t>"日 불매운동 여파에"… 유니클로, 브랜드가치 27계단↓, 日 불매운동 여파…유니클로 대한민국 100대 브랜드 가치 99위로 추락, 한국 무시한 유니클로의 최후 '브랜드 가치' 99위, 현대차-년도년도 1분기 3분기 Preview: 3분기 실적은 기대 이상!, 년도년도 1분기 3분기 Preview: 환율, 신차 효과로 호실적 기대, 환율 상승과 수출 판매 호조, 건비 관련 일회성 비용은 변수</t>
+    <t>"日 불매운동 여파에"… 유니클로, 브랜드가치 27계단↓, 日 불매운동 여파…유니클로 대한민국 100대 브랜드 가치 99위로 추락, 한국 무시한 유니클로의 최후 '브랜드 가치' 99위, 년도년도 1분기 3분기 Preview: 3분기 실적은 기대 이상!, 년도년도 1분기 3분기 Preview: 환율, 신차 효과로 호실적 기대, 환율 상승과 수출 판매 호조, 건비 관련 일회성 비용은 변수</t>
   </si>
   <si>
     <t>S&amp;T모티브, 최대 498억원어치 자사주 매각</t>
@@ -5479,7 +5479,7 @@
     <t>이 주식들 요즘 어때?, ‘현명한 투자자의 지표 분석법’ 사례분석, IR 조직 손질···현대차 지배구조 개편 신호?, 정의선 체제 ‘저울질’…모비스·글로비스 활용안 관심</t>
   </si>
   <si>
-    <t>금춘수 한화 대표이사 부회장, “현대차 주식 매수의견 유지”, SUV 차종 라인업 모두 갖춰 신차효과 봐, 포트폴리오 물갈이…국민연금 "바이오 묻고 대형株 더블로 가!", 현대위아 주가 7%대 급락, 현대차 기아차 현대글로비스도 약세, “한온시스템 주식 매수의견 유지”, 전기차부품 수주 늘려 중장기 성장, 현대차-쏘나타와 GV80 출시 기대, 쏘나타는 미국 공장 수익성 개선을 위한 마지막 퍼즐, 3분기 Preview: 영업이익 개선 추세 지속, 현대차-년도년도 1분기 3분기 Preview: 잠깐의 내수 공백, 3분기 연결 매출액 26.1조원(전년 대비 증감율 +6.7%), 영업이익 1조175억원(전년 대비 증감율 +252%) 전망, 자동차 부문 매출액 19.7조원(전년 대비 증감율 +5.7%), 영업이익 6,889억원(OPM 3.5%) 예상. 중국을 제외한 연결대상 지역의 년도년도 1분기 3분기 도매판매는 93.4만대로 전년 대비 증감율 -0.7%를 기록. 내 수 도매판매가 -4.7%로 부진했지만 북미 +7.2% 호조가 이를 만회. 판매볼륨이 전년 과 유사하지만, RV믹스의 상승, 인센티브 감소, 원달러 평균 환율이 1,193원으로 전년 대비 증감율 6.4% 상승하며 ASP 상승요인으로 작용했을 전망</t>
+    <t>금춘수 한화 대표이사 부회장, “현대차 주식 매수의견 유지”, SUV 차종 라인업 모두 갖춰 신차효과 봐, 포트폴리오 물갈이…국민연금 "바이오 묻고 대형株 더블로 가!", 현대위아 주가 7%대 급락, 현대차 기아차 현대글로비스도 약세, “한온시스템 주식 매수의견 유지”, 전기차부품 수주 늘려 중장기 성장, 쏘나타와 GV80 출시 기대, 쏘나타는 미국 공장 수익성 개선을 위한 마지막 퍼즐, 3분기 Preview: 영업이익 개선 추세 지속, 년도년도 1분기 3분기 Preview: 잠깐의 내수 공백, 3분기 연결 매출액 26.1조원(전년 대비 증감율 +6.7%), 영업이익 1조175억원(전년 대비 증감율 +252%) 전망, 자동차 부문 매출액 19.7조원(전년 대비 증감율 +5.7%), 영업이익 6,889억원(OPM 3.5%) 예상. 중국을 제외한 연결대상 지역의 년도년도 1분기 3분기 도매판매는 93.4만대로 전년 대비 증감율 -0.7%를 기록. 내 수 도매판매가 -4.7%로 부진했지만 북미 +7.2% 호조가 이를 만회. 판매볼륨이 전년 과 유사하지만, RV믹스의 상승, 인센티브 감소, 원달러 평균 환율이 1,193원으로 전년 대비 증감율 6.4% 상승하며 ASP 상승요인으로 작용했을 전망</t>
   </si>
   <si>
     <t>조국 부부 ‘모르쇠’ 일관해도 연결고리 밝혀내면 소추 가능</t>
@@ -5488,10 +5488,10 @@
     <t>주식 시총 상위 10위 중 절반 바뀌어</t>
   </si>
   <si>
-    <t>20년 만에 25일 연속 순매수한 연기금, 왜?...시장왜곡 우려도, 현대차-모멘텀을 맞이할 준비를 하자, 19년도 3분기 영업이익은 1.13조원(+291% 전년 대비 증감율, OPM 4.3%) 기록, 컨센서스 9.0% 상회 전망. 환율, 美 팰리세이드 매출실현 긍정적이나 임단협합의금(2,500억원 추정), 전년수준 도매판매(중국외 -0.7% 전년 대비 증감율), 내수감소(-4.7% 전년 대비 증감율), 기말환율상승(+3.8% 전분기 대비 증감율), 현대카드 코스트코 모객비용 증가 부정적, 19년도 4분기 집중되는 모멘텀에 주목. GV80, 그랜저 F/L, G80 판매로 내수 회복, 쏘나타 북미 판매 본격화(11월~) 기대. 부진한 볼륨모델 수요 회복과 함께 추가 믹스 개선에 따른 매출 증가 전망, 투자의견 BUY, 목표주가 185,000원 유지, “현대차 주식 매수의견 유지”, 내수와 북미에서 4분기 차량 판매증가, 7일 장 마감 후 주요 종목 뉴스</t>
-  </si>
-  <si>
-    <t>현대차-3분기 부합 전망. 환율과 신차 효과가 큰 4분기 주목, 4분기 이후 모멘텀 강화, 19년도 3분기 Preview: 영업이익률 4.0% 전망, 신차 라인업 점검. 제네시스 라인업 강화에 주목, 임상 결과에 울고 웃는 바이오株···"신중한 투자 필요", 7일 장 마감 후 주요 종목 뉴스, 현대차 3社 시총 68兆…올들어 12兆 늘어, 현대카드, 상장 추진…재무적 투자자 달래기 성공할까</t>
+    <t>20년 만에 25일 연속 순매수한 연기금, 왜?...시장왜곡 우려도, 모멘텀을 맞이할 준비를 하자, 19년도 3분기 영업이익은 1.13조원(+291% 전년 대비 증감율, OPM 4.3%) 기록, 컨센서스 9.0% 상회 전망. 환율, 美 팰리세이드 매출실현 긍정적이나 임단협합의금(2,500억원 추정), 전년수준 도매판매(중국외 -0.7% 전년 대비 증감율), 내수감소(-4.7% 전년 대비 증감율), 기말환율상승(+3.8% 전분기 대비 증감율), 현대카드 코스트코 모객비용 증가 부정적, 19년도 4분기 집중되는 모멘텀에 주목. GV80, 그랜저 F/L, G80 판매로 내수 회복, 쏘나타 북미 판매 본격화(11월~) 기대. 부진한 볼륨모델 수요 회복과 함께 추가 믹스 개선에 따른 매출 증가 전망, 투자의견 BUY, 목표주가 185,000원 유지, “현대차 주식 매수의견 유지”, 내수와 북미에서 4분기 차량 판매증가, 7일 장 마감 후 주요 종목 뉴스</t>
+  </si>
+  <si>
+    <t>3분기 부합 전망. 환율과 신차 효과가 큰 4분기 주목, 4분기 이후 모멘텀 강화, 19년도 3분기 Preview: 영업이익률 4.0% 전망, 신차 라인업 점검. 제네시스 라인업 강화에 주목, 임상 결과에 울고 웃는 바이오株···"신중한 투자 필요", 7일 장 마감 후 주요 종목 뉴스, 현대차 3社 시총 68兆…올들어 12兆 늘어, 현대카드, 상장 추진…재무적 투자자 달래기 성공할까</t>
   </si>
   <si>
     <t>현대차 기아차 주가 대폭 하락, 기관과 외인 팔고 개인은 사들여, 현대카드, FI 경영개입 여지...교보생명 데자뷔?, 상장 박차 '현대카드', 떨어지는 기업가치 어쩌나, 현대자동차, 특별관계자 지분변동</t>
@@ -5500,7 +5500,7 @@
     <t>FI 엑시트 위한 현대카드 IPO, 업계2위 삼성카드보다 높은 PBR 가능?, 상장 신호탄 올린 현대카드, 기업가치 평가가 관건</t>
   </si>
   <si>
-    <t>현대차-년도년도 1분기 3분기 Preview - 해소되지 않은 불성,년도 확분기 3Q18에 이어 년도년도 1분기 3분기 에도 엔진 결함비용 발생, 美 검찰조사, MY2015-2019 차량에 대한 불확실성 지속, 현대차-컨센서스 하회 전망, 19년도 3분기 현대차 매출 및 영업이익은 26조 558억원, 5,705억원으로 전년동기 대비 6.6%, 97.4% 증가 할 것으로 전망, 컨센서스 하회 전망, TP 17만원(M), 투자의견 BUY(M), 현대차-본업 개선 vs 비용반영, 19년도 3분기 Preview ? 본업 개선 vs 비용반영, 단기 비용반영은 부담되나 불확실성 해소에 초점을 맞출 필요, 현대차-브랜드 가치 회복 과정, 19년도 3분기 Preview: 6,000억원 규모의 충당금 설정, 단기 실적 악화 불가피, 신차 효과가 더 높은 궤도에 오를 2020년, 투자의견 매수 및 목표주가 178,000원 유지, "현대차 주식 매수의견 유지", 내년 신차 출시주기로 실적 계속 좋아져, 현대차-19년도 3분기 Preview: 리콜 비용 반영, 세타2 직분사(GDi) 엔진 집단소송 고객과 화해안 합의, 3Q Preview: 일회성 비용 제외시 우수한 실적, 향후 전망: 신차 출시에 따른 매출 및 수익성 개선 지속</t>
+    <t>년도년도 1분기 3분기 Preview - 해소되지 않은 불성,년도 확분기 3Q18에 이어 년도년도 1분기 3분기 에도 엔진 결함비용 발생, 美 검찰조사, MY2015-2019 차량에 대한 불확실성 지속, 컨센서스 하회 전망, 19년도 3분기 현대차 매출 및 영업이익은 26조 558억원, 5,705억원으로 전년동기 대비 6.6%, 97.4% 증가 할 것으로 전망, 컨센서스 하회 전망, TP 17만원(M), 투자의견 BUY(M), 본업 개선 vs 비용반영, 19년도 3분기 Preview ? 본업 개선 vs 비용반영, 단기 비용반영은 부담되나 불확실성 해소에 초점을 맞출 필요, 브랜드 가치 회복 과정, 19년도 3분기 Preview: 6,000억원 규모의 충당금 설정, 단기 실적 악화 불가피, 신차 효과가 더 높은 궤도에 오를 2020년, 투자의견 매수 및 목표주가 178,000원 유지, "현대차 주식 매수의견 유지", 내년 신차 출시주기로 실적 계속 좋아져, 19년도 3분기 Preview: 리콜 비용 반영, 세타2 직분사(GDi) 엔진 집단소송 고객과 화해안 합의, 3Q Preview: 일회성 비용 제외시 우수한 실적, 향후 전망: 신차 출시에 따른 매출 및 수익성 개선 지속</t>
   </si>
   <si>
     <t>코스피 '기준금리 관망'으로 강보합, 코스닥은 '외국인 매수'로 올라, 올해 국민연금 보유 10대 그룹 주식가치 10.7조원 증가</t>
@@ -5512,16 +5512,16 @@
     <t>"수소충전소 설치 확대 및 일반인 사용 허가"...관련주 강세, "현대차, 신사업 투자 앞서 내년 지배구조 개편 나설것", SK. 주가상승 여력 얻었지만 지배구조 개편은 “아직…”</t>
   </si>
   <si>
-    <t>현대차 직원 “회사 주가 때문에 고민이 많습니다”…정의선의 답은?, '소통행보' 정의선..“정체된 현대차, 과감한 변화 필요”, 현대차-제네시스 라인업 강화에 주목, SUV 비중 높아지며 수익구조 턴어라운드, 제네시스 라인업 강화에 주목, 투자의견 매수와 목표주가 170,000원 유지</t>
-  </si>
-  <si>
-    <t>"현대차 주식 매수의견 유지" 내년 신차 출시와 원가 개선해 실적 밝아, 정의선호(號) 실적호조에 현대모비스-국민연금 ‘휘파람’, 현대차-혹평탈출 - 반격의 서막, 2020년 자동차 수요 부진이 지속됨에도 1)노후화된 신차 출시로 볼륨과 믹스가 동시 개선되고, 2) 가동률 상승과 플랫폼 통합으로 원가 개선되며 매출액 증가와 수익성 개선이 기대보다 가파를 전망, 경쟁사의 유럽, 미국 볼륨 감소와 친환경차 확대에도 원가 절감 전략이 체감함에 따라 수익성 악화 부담 예상, 유럽/일본 완성차 대비 높은 투자 매력 기대. 투자의견 BUY, 목표주가 185,000원 유지</t>
-  </si>
-  <si>
-    <t>애국소비 불 붙은 중국...주식회사 미국 “나 떨고 있니?”, 상장 후 5연상 간 두산솔루스, 기아차, 올해 3Q 매출액 15조895억(+7.2%) 영업이익 2915억(+149%) (연결), 2만원대 회복앞둔 '신라젠'주가…MSCI코리아 리밸런싱에 발목?, 현대차증권, 1000억 유상증자로 자기자본 1조 대열, 현대카드 상장, 교보생명과 다른 3가지 이유, 현대차-년도년도 1분기 3분기 Review: 보수적인 외국인 vs GV80기대감, 년도년도 1분기 3분기 영업이익은 당사 기대치 및 컨센서스 하회로 부진. 쎄타GDI엔진 리콜비용 6천억원 감안 시 영업이익 1조원 하회. EV전략에 대해서는 배터리 수급계획 부재 및 경쟁사 판매전망에 대해 보수적인 관점이 아쉬움, 10/23일기준 현대차에 대한 외국인 보유비율이 42.92%로 3년내 최저치 기록. 엔진 관련 미국검찰조사 우려로 주가가 92,500원으로 저점을 기록했던 2018년 11월 22일 대비로도 3.2%p낮음. 현대차는 신차출시로 실적회복, 미래차에 대한 활발한 투자, 무 파업 등 긍정적인 이벤트가 이어졌지만 외국인 지분율은 지속 축소. 이는 현대차에 대한 우려보다는 산업패러다임 변화로 비용증가, 경쟁심화에 대한 우려가 주 요인으로 판단됨, 산업에 대한 우려가 지속되고 있어 단기로는 GV80과 그랜져F/L의 성공이, 중장기적으로는 회사의 사업구조 변화가 중요</t>
-  </si>
-  <si>
-    <t>현대차-문제는 비용 증가, 년도년도 1분기 3분기 , 낮아진 기대감도회:년도 분기 년도년도 1분기 3분기 실적은 매출액 26조 9,689원(+10%전년 대비 증감율, +0%전분기 대비 증감율), 영업이익 3,785억원(+31%전년 대비 증감율, -69%전분기 대비 증감율)으로 일회비용년도 성분기 에 대한 우려로 낮아진 시장 컨센서스를 하회했음., 본업의 개선이 절실: 일회비용년도 성분기 을 제외한 3Q18 및 년도년도 1분기 3분기 에 영업이익은 각각 7,800억원과 1조 620억원임., 녹록치 않은 환경: 미국 등 주요 지역의 수요 부진이 지속되고 있는 가운데 경쟁사들의 SUV 신차 출시 확대로 경쟁 강도가 상승 중임. 투자의견을 HOLD로 유지함., 현대차-년도년도 1분기 3분기 Review - 일회성 비용과 판관비 증가의 영향, 투자의견 Buy 유지, 목표주가 160,000원으로 5.9% 하향, 2020년 및 2021년 영업이익 전망치 13.7%, 7.1% 하향. 환율 가정 변동이 주된 이유, 년도년도 1분기 3분기 영업이익 3,785억원. 일회성 요인 제거하면 1.06조원, 준고정비의 불규칙한 변동이 없었다면 영업이익은 1.45조원에 달했을 것, 현대차-일회성 빼면 무난한 실적, 19년도 3분기 Review: 영업이익 3,790억원으로 시장 기대치 하회, 실적이 본격적으로 증가하는 시점은 20년도 하반기 부터, 목표주가 165,000원 유지 , 불확실성은 마무리 되었다, 현대차-일시적 내수 부진과 일회성 비용, 19년도 3분기 영업이익 3,785억원(전년 대비 증감율 +31%)을 기록하며 시장 예상을 소폭 하회. 일회성 비용 약 6,900억원을 감안하면 1.06조원에 해당하는 영업이익을 기록, 일회성을 감안하더라도 기대에 소폭 미치지 못하는 실적인데, 내수 판매 부진에서 이유를 찾을 수 있음. 그러나 이는 주요 차종 출시 직전의 수요공백이 발생한 사이 경쟁차종이 출시된 효과로 분석하므로 상품성 문제라고 보기 어려움, 기대를 모으고 있는 그랜져 F/L와 GV80는 11월 출시 예정이므로 4Q에도 내수 부진은 일정부분 이어질 가능성이 있지만, 사전예약 대수 등 신차에 대한 긍정적인 반응이 있다면 20년도 1분기 호실적을 기대하며 우려를 지울 수 있을 전망, 현대차-3분기는 하회. 이제는 GV80에 주목할 때, 강화되는 신차 사이클로 관심 이동, 19년도 3분기 Review: 영업이익률 1.4% 기록, 실적발표 컨퍼런스 콜의 주요 내용: 규제 대응과 시장재편 목표로 친환경차 적극 출시, 현대차-단기보다는 중장기 개선에 포인트, 19년도 3분기 Review - 일회성 비용을 제외하면 본업 개선흐름 지속, 단기보다는 중장기 개선에 포인트, 현대차-년도년도 1분기 3분기 Review: 일회성 비용 아쉽지만 미래 전망에 초점, 년도년도 1분기 3분기 Review: 대규모 일회성 비용 반영으로 부진한 실적 시현, 4분기 기대 신차 출시를 통해 회복 기대, 현대차-아쉬운 실적, 그러나 변하고 있는 현대차, 19년도 3분기 Review: 품질비용 증가에 따른 시장 기대치 하회, 달라지는 현대차 , 체질 개선과 미래 성장 동력 확보 중, 현대차-방향성이 확실한 점이 매력, 3분기 영업이익 0.38조원(+31.0%)에서 일회성 비용 제거시 양호, SUV 및 전기차, 확실한 전략적 방향성 확인, 목표주가 170,000원, 투자의견 매수 유지, 현대차-묻고 가는 실적, 실적은 SUV 등 믹스개선과 인센티브 축소에도 불구하고 일회성 비용으로 부진, 일회성 비용 6,830억원을 조정한 영업이익은 1조 620억원(영업이익률 3.9%), 턴어라운드 지속, 11월을 기점으로 투자심리 개선 전망, 현대차-옅어지는 불확실성과 짙어지는 펀더멘털, 19년도 3분기 Review: 구조적 개선이 불식시킨 충당금 우려, 차세대 자동차 분야의 글로벌 선도 기업, 투자의견 매수 유지, 목표주가 178,000원 유지, SK하이닉스, '깜짝 실적'에 외국인 '리턴'…실적 향방은, "현대차 주식 매수의견 유지", 그랜저 투싼 GV80 등 신차 라인업 강화, 현대차-품질비용 발현으로 부진한 년도년도 1분기 3분기 기년도 실분기 록, 영업지표 개선을 통해 우상향 실적 흐름을 이어왔던 현대 그년도 차분기 러나 지난 년도년도 1분기 3분기 실적은 쎄타엔진 리콜 발생과 노조 통상임금 합의금 지급으로 부진한 기년도 실분기 록, 지난 1Q19 (+6.9% 전년비 년도 분기 증감율), 2Q19 (+9.1% 전년비 년도 분기 증감율)에 이어 년도년도 1분기 3분기 에도 +10.4% 전년비 년도 분기 증감율의 높은 매출성장을 기록한 점은 영업지표 호전이 확대되고 있음을 의미, 그러나 품질비용 이슈 지속으로 경상적 판매보증 충당부채 전입 규모가 확대된 점은 실적 추정 하향요인. 20년 실적추정 조정 반영해, 적정주가 165,000원으로 하향, 현대차-다소 높아 보이는 19년도 4분기 기대치, 엔진 품질 관련 &amp; 임급협상 타결 격려금 비용으로 빛바래버린 믹스 개선 효과, 차량사업부 매출 26,969십억원(전년 대비 증감율+10.4%), OP 379십억원(전년 대비 증감율+31%, OPM 1.4%), 믹스 개선 효과를 견인해줄 신차는 기대요인이지만, 본격적인 효과는 20년도 1분기 부터, 현대차-악재는 묻고 모멘텀은 더블로 가, 19년도 3분기 영업이익은 3,785억원(+31.0% 전년 대비 증감율, OPM 1.4%) 기록, 컨센서스 29.0% 하회. 품질 비용(6,030억원)과 통상임금 합의금(800억원) 제거 시 1.06조원으로 시장 기대 소폭 하회, 판매 믹스 및 신차 효과로 인한 이익증가는 19년도 2분기 보다 강화. 비우호적 경영 환경에도 개선되는 신차 모멘텀을 감안 시 이익 개선 속도는 더욱 빨라질 전망, 투자의견 BUY, 목표주가 185,000원, Top-pick 유지, 현대차-신차효과 누적에 따른 영업이익 회복과정, 11월 쏘나타 미국생산 시작. GV80 출시, 3분기 Review: 일회성 제거 시 예상범위</t>
+    <t>현대차 직원 “회사 주가 때문에 고민이 많습니다”…정의선의 답은?, '소통행보' 정의선..“정체된 현대차, 과감한 변화 필요”, 제네시스 라인업 강화에 주목, SUV 비중 높아지며 수익구조 턴어라운드, 제네시스 라인업 강화에 주목, 투자의견 매수와 목표주가 170,000원 유지</t>
+  </si>
+  <si>
+    <t>"현대차 주식 매수의견 유지" 내년 신차 출시와 원가 개선해 실적 밝아, 정의선호(號) 실적호조에 현대모비스-국민연금 ‘휘파람’, 혹평탈출 - 반격의 서막, 2020년 자동차 수요 부진이 지속됨에도 1)노후화된 신차 출시로 볼륨과 믹스가 동시 개선되고, 2) 가동률 상승과 플랫폼 통합으로 원가 개선되며 매출액 증가와 수익성 개선이 기대보다 가파를 전망, 경쟁사의 유럽, 미국 볼륨 감소와 친환경차 확대에도 원가 절감 전략이 체감함에 따라 수익성 악화 부담 예상, 유럽/일본 완성차 대비 높은 투자 매력 기대. 투자의견 BUY, 목표주가 185,000원 유지</t>
+  </si>
+  <si>
+    <t>애국소비 불 붙은 중국...주식회사 미국 “나 떨고 있니?”, 상장 후 5연상 간 두산솔루스, 기아차, 올해 3Q 매출액 15조895억(+7.2%) 영업이익 2915억(+149%) (연결), 2만원대 회복앞둔 '신라젠'주가…MSCI코리아 리밸런싱에 발목?, 현대차증권, 1000억 유상증자로 자기자본 1조 대열, 현대카드 상장, 교보생명과 다른 3가지 이유, 년도년도 1분기 3분기 Review: 보수적인 외국인 vs GV80기대감, 년도년도 1분기 3분기 영업이익은 당사 기대치 및 컨센서스 하회로 부진. 쎄타GDI엔진 리콜비용 6천억원 감안 시 영업이익 1조원 하회. EV전략에 대해서는 배터리 수급계획 부재 및 경쟁사 판매전망에 대해 보수적인 관점이 아쉬움, 10/23일기준 현대차에 대한 외국인 보유비율이 42.92%로 3년내 최저치 기록. 엔진 관련 미국검찰조사 우려로 주가가 92,500원으로 저점을 기록했던 2018년 11월 22일 대비로도 3.2%p낮음. 현대차는 신차출시로 실적회복, 미래차에 대한 활발한 투자, 무 파업 등 긍정적인 이벤트가 이어졌지만 외국인 지분율은 지속 축소. 이는 현대차에 대한 우려보다는 산업패러다임 변화로 비용증가, 경쟁심화에 대한 우려가 주 요인으로 판단됨, 산업에 대한 우려가 지속되고 있어 단기로는 GV80과 그랜져F/L의 성공이, 중장기적으로는 회사의 사업구조 변화가 중요</t>
+  </si>
+  <si>
+    <t>문제는 비용 증가, 년도년도 1분기 3분기 , 낮아진 기대감도회:년도 분기 년도년도 1분기 3분기 실적은 매출액 26조 9,689원(+10%전년 대비 증감율, +0%전분기 대비 증감율), 영업이익 3,785억원(+31%전년 대비 증감율, -69%전분기 대비 증감율)으로 일회비용년도 성분기 에 대한 우려로 낮아진 시장 컨센서스를 하회했음., 본업의 개선이 절실: 일회비용년도 성분기 을 제외한 3Q18 및 년도년도 1분기 3분기 에 영업이익은 각각 7,800억원과 1조 620억원임., 녹록치 않은 환경: 미국 등 주요 지역의 수요 부진이 지속되고 있는 가운데 경쟁사들의 SUV 신차 출시 확대로 경쟁 강도가 상승 중임. 투자의견을 HOLD로 유지함., 년도년도 1분기 3분기 Review - 일회성 비용과 판관비 증가의 영향, 투자의견 Buy 유지, 목표주가 160,000원으로 5.9% 하향, 2020년 및 2021년 영업이익 전망치 13.7%, 7.1% 하향. 환율 가정 변동이 주된 이유, 년도년도 1분기 3분기 영업이익 3,785억원. 일회성 요인 제거하면 1.06조원, 준고정비의 불규칙한 변동이 없었다면 영업이익은 1.45조원에 달했을 것, 일회성 빼면 무난한 실적, 19년도 3분기 Review: 영업이익 3,790억원으로 시장 기대치 하회, 실적이 본격적으로 증가하는 시점은 20년도 하반기 부터, 목표주가 165,000원 유지 , 불확실성은 마무리 되었다, 일시적 내수 부진과 일회성 비용, 19년도 3분기 영업이익 3,785억원(전년 대비 증감율 +31%)을 기록하며 시장 예상을 소폭 하회. 일회성 비용 약 6,900억원을 감안하면 1.06조원에 해당하는 영업이익을 기록, 일회성을 감안하더라도 기대에 소폭 미치지 못하는 실적인데, 내수 판매 부진에서 이유를 찾을 수 있음. 그러나 이는 주요 차종 출시 직전의 수요공백이 발생한 사이 경쟁차종이 출시된 효과로 분석하므로 상품성 문제라고 보기 어려움, 기대를 모으고 있는 그랜져 F/L와 GV80는 11월 출시 예정이므로 4Q에도 내수 부진은 일정부분 이어질 가능성이 있지만, 사전예약 대수 등 신차에 대한 긍정적인 반응이 있다면 20년도 1분기 호실적을 기대하며 우려를 지울 수 있을 전망, 3분기는 하회. 이제는 GV80에 주목할 때, 강화되는 신차 사이클로 관심 이동, 19년도 3분기 Review: 영업이익률 1.4% 기록, 실적발표 컨퍼런스 콜의 주요 내용: 규제 대응과 시장재편 목표로 친환경차 적극 출시, 단기보다는 중장기 개선에 포인트, 19년도 3분기 Review - 일회성 비용을 제외하면 본업 개선흐름 지속, 단기보다는 중장기 개선에 포인트, 년도년도 1분기 3분기 Review: 일회성 비용 아쉽지만 미래 전망에 초점, 년도년도 1분기 3분기 Review: 대규모 일회성 비용 반영으로 부진한 실적 시현, 4분기 기대 신차 출시를 통해 회복 기대, 아쉬운 실적, 그러나 변하고 있는 현대차, 19년도 3분기 Review: 품질비용 증가에 따른 시장 기대치 하회, 달라지는 현대차 , 체질 개선과 미래 성장 동력 확보 중, 방향성이 확실한 점이 매력, 3분기 영업이익 0.38조원(+31.0%)에서 일회성 비용 제거시 양호, SUV 및 전기차, 확실한 전략적 방향성 확인, 목표주가 170,000원, 투자의견 매수 유지, 묻고 가는 실적, 실적은 SUV 등 믹스개선과 인센티브 축소에도 불구하고 일회성 비용으로 부진, 일회성 비용 6,830억원을 조정한 영업이익은 1조 620억원(영업이익률 3.9%), 턴어라운드 지속, 11월을 기점으로 투자심리 개선 전망, 옅어지는 불확실성과 짙어지는 펀더멘털, 19년도 3분기 Review: 구조적 개선이 불식시킨 충당금 우려, 차세대 자동차 분야의 글로벌 선도 기업, 투자의견 매수 유지, 목표주가 178,000원 유지, SK하이닉스, '깜짝 실적'에 외국인 '리턴'…실적 향방은, "현대차 주식 매수의견 유지", 그랜저 투싼 GV80 등 신차 라인업 강화, 품질비용 발현으로 부진한 년도년도 1분기 3분기 기년도 실분기 록, 영업지표 개선을 통해 우상향 실적 흐름을 이어왔던 현대 그년도 차분기 러나 지난 년도년도 1분기 3분기 실적은 쎄타엔진 리콜 발생과 노조 통상임금 합의금 지급으로 부진한 기년도 실분기 록, 지난 1Q19 (+6.9% 전년비 년도 분기 증감율), 2Q19 (+9.1% 전년비 년도 분기 증감율)에 이어 년도년도 1분기 3분기 에도 +10.4% 전년비 년도 분기 증감율의 높은 매출성장을 기록한 점은 영업지표 호전이 확대되고 있음을 의미, 그러나 품질비용 이슈 지속으로 경상적 판매보증 충당부채 전입 규모가 확대된 점은 실적 추정 하향요인. 20년 실적추정 조정 반영해, 적정주가 165,000원으로 하향, 다소 높아 보이는 19년도 4분기 기대치, 엔진 품질 관련 &amp; 임급협상 타결 격려금 비용으로 빛바래버린 믹스 개선 효과, 차량사업부 매출 26,969십억원(전년 대비 증감율+10.4%), OP 379십억원(전년 대비 증감율+31%, OPM 1.4%), 믹스 개선 효과를 견인해줄 신차는 기대요인이지만, 본격적인 효과는 20년도 1분기 부터, 악재는 묻고 모멘텀은 더블로 가, 19년도 3분기 영업이익은 3,785억원(+31.0% 전년 대비 증감율, OPM 1.4%) 기록, 컨센서스 29.0% 하회. 품질 비용(6,030억원)과 통상임금 합의금(800억원) 제거 시 1.06조원으로 시장 기대 소폭 하회, 판매 믹스 및 신차 효과로 인한 이익증가는 19년도 2분기 보다 강화. 비우호적 경영 환경에도 개선되는 신차 모멘텀을 감안 시 이익 개선 속도는 더욱 빨라질 전망, 투자의견 BUY, 목표주가 185,000원, Top-pick 유지, 신차효과 누적에 따른 영업이익 회복과정, 11월 쏘나타 미국생산 시작. GV80 출시, 3분기 Review: 일회성 제거 시 예상범위</t>
   </si>
   <si>
     <t>제이엔케이히터, 수소차 시대 앞두고 기대 커져, "기아차 내년 매출 60兆"에 반기 든 외국계證</t>
@@ -5533,10 +5533,10 @@
     <t>`깜짝` 실적에 웃은 車부품주…주가도 `활짝`</t>
   </si>
   <si>
-    <t>"현대차 주가 상승 전망", 새 그랜저와 제네시스 SUV로 이익회복 기대, 현대차-4분기 반등 모색, 19년도 3분기 현대차 실적 부진 요인은 1) 일회성 품질비용(6,000억원), 2) 임단협 합의금(800억원), 3) 기말환율 상승으로 인한 판매보증충당금 증분(1,000억원), 4) 일시 약화된 신차효과로 내수 부진, 5) 로템 적자로 인한 기타손익 부진 요인으로 일회성 비용과 기타 부진 감안 시 예상 수준 실적 기록했다고 판단, 19년도 4분기 잔여 임단협 합의금(1,200억원) 지급에도 국내 그랜져 F/L(11월 중순), GV80(11월 말) 출시로 내수 회복, 미국 쏘나타 양산(11월 초 생산), 팰리세이드 증산(글로비스 화재로 재고 부족, 11월 판매 정상화)으로 미국 볼륨과 믹스(인센티브) 개선되며 이익은 회복세 전망. 투자의견 BUY, 목표주가 185,000원 유지</t>
-  </si>
-  <si>
-    <t>현대차-제네시스 2장 1절, GV80으로 부활하는 제네시스, 제네시스 이익기여도 상승 전망, 수혜주는 현대차 및 ADAS 관련업체 등, 현대차-빠른 변화 속도에 적응 필요, 3분기 실적 기대치 하회, 향후 고군분투 전망, 신차 효과 가시화, 미래형 자동차 개발 진행, 급변하는 자동차 시장 환경 변화에 대응 필요, APEC 취소로 미중협상 차질, P2P금융법 국회 통과, 허창수 GS 회장 美에 벤처캐피탈 설립, 하이트 진로 시총 2조원 돌파, 국고보조금 부정수급 1년간 21억원 적발, 삼성 전자 3분기 영업익 3조</t>
+    <t>"현대차 주가 상승 전망", 새 그랜저와 제네시스 SUV로 이익회복 기대, 4분기 반등 모색, 19년도 3분기 현대차 실적 부진 요인은 1) 일회성 품질비용(6,000억원), 2) 임단협 합의금(800억원), 3) 기말환율 상승으로 인한 판매보증충당금 증분(1,000억원), 4) 일시 약화된 신차효과로 내수 부진, 5) 로템 적자로 인한 기타손익 부진 요인으로 일회성 비용과 기타 부진 감안 시 예상 수준 실적 기록했다고 판단, 19년도 4분기 잔여 임단협 합의금(1,200억원) 지급에도 국내 그랜져 F/L(11월 중순), GV80(11월 말) 출시로 내수 회복, 미국 쏘나타 양산(11월 초 생산), 팰리세이드 증산(글로비스 화재로 재고 부족, 11월 판매 정상화)으로 미국 볼륨과 믹스(인센티브) 개선되며 이익은 회복세 전망. 투자의견 BUY, 목표주가 185,000원 유지</t>
+  </si>
+  <si>
+    <t>제네시스 2장 1절, GV80으로 부활하는 제네시스, 제네시스 이익기여도 상승 전망, 수혜주는 현대차 및 ADAS 관련업체 등, 빠른 변화 속도에 적응 필요, 3분기 실적 기대치 하회, 향후 고군분투 전망, 신차 효과 가시화, 미래형 자동차 개발 진행, 급변하는 자동차 시장 환경 변화에 대응 필요, APEC 취소로 미중협상 차질, P2P금융법 국회 통과, 허창수 GS 회장 美에 벤처캐피탈 설립, 하이트 진로 시총 2조원 돌파, 국고보조금 부정수급 1년간 21억원 적발, 삼성 전자 3분기 영업익 3조</t>
   </si>
   <si>
     <t>"익성으로 대박 노렸다" 검찰 '조국 펀드' 너머 조국 직접 겨냥, 반도체, 상승사이클 기대…철강은 수요둔화 부담</t>
@@ -5554,13 +5554,13 @@
     <t>코스닥벤처펀드 자금 '썰물'… 순자산 4000억원 붕괴되나, 지배구조 개편 신호탄 쏜 SK···주가 레벨업 구간 진입, 하반기, 우수한 성적표 받은 외국인투자자…개미는 '저조', 개미는 또 ‘쪽박’ 외국인은 여전히 ‘대박’, 미중 무역전쟁 2년… 쪼그라든 주식시장, 덩치 커진 채권시장, 유통업계 다시 볕드나…'3가지 위기탈출 신호'에 주가 일제히 급등, 유준원의 '상상인', 금융그룹 야심 제동 걸리나</t>
   </si>
   <si>
-    <t>상장사 임원 10명 중 2명 “회사 성과 줄어도 보수는 더 챙겨”, 한온시스템 주식 매수의견 유지, "전동화부품부문 꾸준히 성장", 현대차-제네시스 브랜드가 커진다, 제네시스 비중 상승으로 믹스 개선을 기대, GV80과 G80을 통해 영업이익 5% 증가할 전망, Valuation 재평가의 계기로 작용할 것</t>
+    <t>상장사 임원 10명 중 2명 “회사 성과 줄어도 보수는 더 챙겨”, 한온시스템 주식 매수의견 유지, "전동화부품부문 꾸준히 성장", 제네시스 브랜드가 커진다, 제네시스 비중 상승으로 믹스 개선을 기대, GV80과 G80을 통해 영업이익 5% 증가할 전망, Valuation 재평가의 계기로 작용할 것</t>
   </si>
   <si>
     <t>외국인 코스피 3주 연속 매수세, 3738억 원 사들여</t>
   </si>
   <si>
-    <t>정몽규 '2.5兆 승부수'…항공날개 달다, "현대모비스 주식 매수의견", 전기차시장 확대로 전동화사업 전망 밝아, 현대차-2년 차는 더 좋다, 2년 차에 진입하는 신차싸이클, 가동률 개선 통한 인센티브 추가 하락 및 금융 손익 회복에 주목, 20년 본격적인 ROE 회복 국면에 진입하는 현대차의 기업가치 정상화 발현 전망</t>
+    <t>정몽규 '2.5兆 승부수'…항공날개 달다, "현대모비스 주식 매수의견", 전기차시장 확대로 전동화사업 전망 밝아, 2년 차는 더 좋다, 2년 차에 진입하는 신차싸이클, 가동률 개선 통한 인센티브 추가 하락 및 금융 손익 회복에 주목, 20년 본격적인 ROE 회복 국면에 진입하는 현대차의 기업가치 정상화 발현 전망</t>
   </si>
   <si>
     <t>외국인, 올해 반도체·바이오株 사고 車·통신·정유株 팔았다</t>
@@ -5578,10 +5578,10 @@
     <t>'아시아나 인수전' 재계 평가 '냉혹'…정몽규-채형석 '반전 희비', 현대건설, 2800억 규모 채무 조건부 인수 결정</t>
   </si>
   <si>
-    <t>현대차-동텄다, 투자의견 Buy, 목표주가 16만원으로 커버리지 개시, 내년 신차 사이클과 제네시스 모멘텀 기대, 수익성 개선을 통해 큰 폭의 이익 성장 전망</t>
-  </si>
-  <si>
-    <t>현대차, 연이은 신차 효과에 4Q 실적·주가 '방긋', 현대차-문제는 비용 증가문제는 비용 증가, 본업의 개선이 절실, 녹록치 않은 환경</t>
+    <t>동텄다, 투자의견 Buy, 목표주가 16만원으로 커버리지 개시, 내년 신차 사이클과 제네시스 모멘텀 기대, 수익성 개선을 통해 큰 폭의 이익 성장 전망</t>
+  </si>
+  <si>
+    <t>현대차, 연이은 신차 효과에 4Q 실적·주가 '방긋', 문제는 비용 증가문제는 비용 증가, 본업의 개선이 절실, 녹록치 않은 환경</t>
   </si>
   <si>
     <t>11개월 동안 38배 오른 주가가 하루 98% '폭삭'....어느 중국 기업의 몰락, '수천억' 역대급 재벌가 상속세 TOP7</t>
@@ -5596,28 +5596,28 @@
     <t>'셀 코리아'도 빗겨가는 삼바·카카오·삼성전기, 중국 대리석업체 아트고 주가 천당에서 지옥으로</t>
   </si>
   <si>
-    <t>현대차 주식 매수의견 유지, "내년부터 신차 출시효과 본격화", 현대차-내수 판매 개선과 함께 주가 상승 재개 전망, 그랜져 f/l, GV80 연말 출시로 20년도 1분기 화려한 신차 효과 대기. 19년도 3분기 이후 하락세 전환했던 내수 판매량은 재차 증가세 전환 가능할 전망이며, ASP 개선 효과도 수반. 이어서 G80 풀체인지, 아반떼 풀체인지, 투싼 풀체인지 등 신차가 2020년 내내 이어질 전망, 미국은 팰리세이드 수출이 2019년 하반기부터이므로 RV믹스 상승세 상반기 내내 지속되며, 원달러 환율 전년 대비 증감율 상승 효과도 유지되므로 P, Q 개선 유효, 현대차-세그먼트 대형화에서 판매 대수 증가로 초점 이동, 투자의견 Buy 유지, 목표주가 150,000원으로 6.3% 하향, 2020년 영업이익 전년동기대비 25.1% 증가 예상, 도매 판매 대수 증가, 세그먼트 대형화 예상, 환율 변화, 세타2 엔진 관련 추가 비용 발생 여부가 투자의견 리스크 요인, 현대모비스 주식 매수의견 유지, "주력 모듈부문 안정적 성장 가능"</t>
-  </si>
-  <si>
-    <t>현대차-인도네시아 공장 설립을 위한 MOU 체결, 동남아 시장을 겨냥해 연산 25만대 공장을 건설, 인도네시아 내수 시장은 연간 115만대 규모, 2022년 이후 현대차의 성장동력으로 작동할 것, 현대차-미리 가본 인도네시아 공장, 인도네시아 공장 건설을 위한 MOU 체결, 현지 탐방을 통해 파악한 인도네시아 자동차 시장 특징, 중국을 부분적으로 대체할 중장기 성장동력이 될 전망, 外人 투매 불구...SK계열 · 효성계열 급등하며 코스피 '견인'</t>
-  </si>
-  <si>
-    <t>국민연금, ‘연금 사회주의’로 민간기업 손아귀에?, 현대차-임중도원(任重道遠), 갈 길은 멀고 책임은 무겁다, 원가 절감: 차세대 플랫폼 사용, 부품 공용화율 상승 등으로 제조 원가의 구조적 절감, 신차 사이클: 2년 사이 4개의 신규 차종 출시, 볼륨 모델들의 연이은 완전변경 모델 출시, 브랜드 가치 제고: 글로벌 친환경차 선두 메이커, 제네시스 미국 성공시 리레이팅 가능, 현대차-2020년 전망 : 자사주 정책발표를 기대하며, 마이너스 금리 확산에 따라 주식시장에서 투자자의 관심도 초 고성장 주와 배당성장주로 양극화. 이는 자동차 산업에서도 테슬라와 도요타의 신고가 기록으로 입증, 전통적인 자동차업체인 도요타는 엔고에도 강력한 주주친화정책으로 역사적 신고가를 기록하였고, 이는 한국자동차업체에도 많은 시사점을 줌. 현대차는 주주친화정책 강화 가능성이 높으며 현재 자사주 5.1% 및 그룹 지분 29.1%를 감안할 때 자사주 취득 정책에 따라 약 35%~40% 물량이 유통주식수에서 사실상 제외되는 효과, 영업적으로는 GV80의 성공여부 및 유럽시장에서 전기차 M/S 추이가 Valuation multiple을 자극할 수 있음</t>
+    <t>현대차 주식 매수의견 유지, "내년부터 신차 출시효과 본격화", 내수 판매 개선과 함께 주가 상승 재개 전망, 그랜져 f/l, GV80 연말 출시로 20년도 1분기 화려한 신차 효과 대기. 19년도 3분기 이후 하락세 전환했던 내수 판매량은 재차 증가세 전환 가능할 전망이며, ASP 개선 효과도 수반. 이어서 G80 풀체인지, 아반떼 풀체인지, 투싼 풀체인지 등 신차가 2020년 내내 이어질 전망, 미국은 팰리세이드 수출이 2019년 하반기부터이므로 RV믹스 상승세 상반기 내내 지속되며, 원달러 환율 전년 대비 증감율 상승 효과도 유지되므로 P, Q 개선 유효, 세그먼트 대형화에서 판매 대수 증가로 초점 이동, 투자의견 Buy 유지, 목표주가 150,000원으로 6.3% 하향, 2020년 영업이익 전년동기대비 25.1% 증가 예상, 도매 판매 대수 증가, 세그먼트 대형화 예상, 환율 변화, 세타2 엔진 관련 추가 비용 발생 여부가 투자의견 리스크 요인, 현대모비스 주식 매수의견 유지, "주력 모듈부문 안정적 성장 가능"</t>
+  </si>
+  <si>
+    <t>인도네시아 공장 설립을 위한 MOU 체결, 동남아 시장을 겨냥해 연산 25만대 공장을 건설, 인도네시아 내수 시장은 연간 115만대 규모, 2022년 이후 현대차의 성장동력으로 작동할 것, 미리 가본 인도네시아 공장, 인도네시아 공장 건설을 위한 MOU 체결, 현지 탐방을 통해 파악한 인도네시아 자동차 시장 특징, 중국을 부분적으로 대체할 중장기 성장동력이 될 전망, 外人 투매 불구...SK계열 · 효성계열 급등하며 코스피 '견인'</t>
+  </si>
+  <si>
+    <t>국민연금, ‘연금 사회주의’로 민간기업 손아귀에?, 임중도원(任重道遠), 갈 길은 멀고 책임은 무겁다, 원가 절감: 차세대 플랫폼 사용, 부품 공용화율 상승 등으로 제조 원가의 구조적 절감, 신차 사이클: 2년 사이 4개의 신규 차종 출시, 볼륨 모델들의 연이은 완전변경 모델 출시, 브랜드 가치 제고: 글로벌 친환경차 선두 메이커, 제네시스 미국 성공시 리레이팅 가능, 2020년 전망 : 자사주 정책발표를 기대하며, 마이너스 금리 확산에 따라 주식시장에서 투자자의 관심도 초 고성장 주와 배당성장주로 양극화. 이는 자동차 산업에서도 테슬라와 도요타의 신고가 기록으로 입증, 전통적인 자동차업체인 도요타는 엔고에도 강력한 주주친화정책으로 역사적 신고가를 기록하였고, 이는 한국자동차업체에도 많은 시사점을 줌. 현대차는 주주친화정책 강화 가능성이 높으며 현재 자사주 5.1% 및 그룹 지분 29.1%를 감안할 때 자사주 취득 정책에 따라 약 35%~40% 물량이 유통주식수에서 사실상 제외되는 효과, 영업적으로는 GV80의 성공여부 및 유럽시장에서 전기차 M/S 추이가 Valuation multiple을 자극할 수 있음</t>
   </si>
   <si>
     <t>이노션 주식 매수의견 유지, "호주 웰컴그룹 인수해 이익 늘어", 배당주의 계절 투자법 A to Z| 배당수익률 높다고 무조건 유리한 것 아냐, 종목 고를 자신 없다면 펀드 가입이 무난, '코스닥 이전상장' 미디어젠...FI 잇단 회수 수순</t>
   </si>
   <si>
-    <t>현대차 주식 매수의견 유지, "내년 판매단가 높아져 실적개선 전망", 현대차-판매믹스 개선의 효과, SUV Genesis Sedan 믹스 개선의 3박자, 2020년 영업 이익은 32.3% 증가 전망, 체질개선 확인 후 밸류에이션 재평가 전망</t>
+    <t>현대차 주식 매수의견 유지, "내년 판매단가 높아져 실적개선 전망", 판매믹스 개선의 효과, SUV Genesis Sedan 믹스 개선의 3박자, 2020년 영업 이익은 32.3% 증가 전망, 체질개선 확인 후 밸류에이션 재평가 전망</t>
   </si>
   <si>
     <t>국민경제 위협 사회주의 굿판 벌이는 공정위·국민연금, 미중협상 불확실성 확대·경제지표 하락에 美증시 상승세 주춤, 이원컴포텍, 투자위험 경고 나몰라라 '두달새 7배 급등'</t>
   </si>
   <si>
-    <t>현대차-중장기 비전이 판매 대수 및 주주환원 정책에 미칠 영향, 현대차, 2025 비전 제시 - Smart Mobility Solution Provider, 비용절감을 중심으로 디바이스 사업의 수익성 개선하며, 이를 토대로 세계 3대 EV 메이커 지향, 플랫폼 기반 모빌리티 서비스 사업 전개해 수익 창출 기회 만들 것, 현대차-차트로 보는 2020년 전망, 점차 소멸되는 SUV 효과를 제네시스가 보완. 라인업 확대로 이익기여도 상승 전망, 신형 엔진과 신형 플랫폼 효과 본격화. 원가절감으로 수익성 상승 전망, 현대차 3,000억 규모 자사주 매입···61조 투자계획으로 장기 투심도 공략, 최중경 한국공인회계사회 회장, 기업 경영전략까지 손 뻗은 곳, '엘리엇' 만이 아니다, 조국사태 논란 '익성' 매물로 나온다</t>
-  </si>
-  <si>
-    <t>"현대차 주가 상승 가능", 중장기 청사진과 자사주 취득 긍정적, 현대차-근거 있는 자신감, 과거 물량 중심 문화. 전략은 물량의 달성 수단. 이젠 전략 중심으로 방향 설정, Smart Mobility Solution Provider를 새로운 전략적 지향점으로 설정, 이는 Smart Mobility Device와 Smart Mobility Service의 사업구조로 나뉨, 현대차-2025 전략 발표, 스마트 모빌리티 솔루션 기업으로 변화, 3대 핵심 재무 목표달성을 통한 주주가치 제고 지속, 현대차-확신의 근거를 찾아서, 사업 부문 개편 이동성의 모든 부분, 재무 목표 재확인 2020년 5% 2025년 8%, 현대차-2025 전략 발표, 스마트 모빌리티 솔루션 기업으로 변화, 3대 핵심 재무 목표달성을 통한 주주가치 제고 지속, 현대차-확신의 근거를 찾아서, 사업 부문 개편 이동성의 모든 부분, 재무 목표 재확인 2020년 5% 2025년 8%, 현대차-미래 중장기 전략 - 2025년 수익성 8%, 현대차 2025 중장기 전략 : Smart Mobility Solution Provider, 중장기 재무목표 제시 : 20E 5%-&gt; 22E 7%-&gt; 25E 8%, 현대차-CEO Investor day: Transformation을 위한 투자의 시기, Vision 2025 발표를 통해 제조중심에서 제조와 서비스를 하는 회사로 변화 방향 제시, 제네시스 강화 및 원가절감 (5년간 34.5조원 절감)을 통한 수익성강화 의지표명, 현대차의 투자금액 증가 계획은 산업트렌드 변화 및 마이너스 금리환경을 감안할 때 올바른 방향으로 판단, 현대차-2025 성공에 대하여, 2025년 중장기 전략을 통해 스마트 모빌리티 솔루션 사업 확장에 대한 의지와 구체적 전략, 원가 절감을 통한 기존 사업 수익성 강화의 가능성과 의지를 재차 확인, 2020년 현대차는 상대적 유리한 파냄 포트폴리오, 신차 출시로 시장 상회하는 판매 증가, 3세대 모듈러 플랫폼 확산으로 비용절감 효과 확대되며 시장 기대치 보다 높은 5% 영업이익 달성 가능성 높을 전망</t>
+    <t>중장기 비전이 판매 대수 및 주주환원 정책에 미칠 영향, 현대차, 2025 비전 제시 - Smart Mobility Solution Provider, 비용절감을 중심으로 디바이스 사업의 수익성 개선하며, 이를 토대로 세계 3대 EV 메이커 지향, 플랫폼 기반 모빌리티 서비스 사업 전개해 수익 창출 기회 만들 것, 차트로 보는 2020년 전망, 점차 소멸되는 SUV 효과를 제네시스가 보완. 라인업 확대로 이익기여도 상승 전망, 신형 엔진과 신형 플랫폼 효과 본격화. 원가절감으로 수익성 상승 전망, 현대차 3,000억 규모 자사주 매입···61조 투자계획으로 장기 투심도 공략, 최중경 한국공인회계사회 회장, 기업 경영전략까지 손 뻗은 곳, '엘리엇' 만이 아니다, 조국사태 논란 '익성' 매물로 나온다</t>
+  </si>
+  <si>
+    <t>"현대차 주가 상승 가능", 중장기 청사진과 자사주 취득 긍정적, 근거 있는 자신감, 과거 물량 중심 문화. 전략은 물량의 달성 수단. 이젠 전략 중심으로 방향 설정, Smart Mobility Solution Provider를 새로운 전략적 지향점으로 설정, 이는 Smart Mobility Device와 Smart Mobility Service의 사업구조로 나뉨, 2025 전략 발표, 스마트 모빌리티 솔루션 기업으로 변화, 3대 핵심 재무 목표달성을 통한 주주가치 제고 지속, 확신의 근거를 찾아서, 사업 부문 개편 이동성의 모든 부분, 재무 목표 재확인 2020년 5% 2025년 8%, 2025 전략 발표, 스마트 모빌리티 솔루션 기업으로 변화, 3대 핵심 재무 목표달성을 통한 주주가치 제고 지속, 확신의 근거를 찾아서, 사업 부문 개편 이동성의 모든 부분, 재무 목표 재확인 2020년 5% 2025년 8%, 미래 중장기 전략 - 2025년 수익성 8%, 현대차 2025 중장기 전략 : Smart Mobility Solution Provider, 중장기 재무목표 제시 : 20E 5%-&gt; 22E 7%-&gt; 25E 8%, CEO Investor day: Transformation을 위한 투자의 시기, Vision 2025 발표를 통해 제조중심에서 제조와 서비스를 하는 회사로 변화 방향 제시, 제네시스 강화 및 원가절감 (5년간 34.5조원 절감)을 통한 수익성강화 의지표명, 현대차의 투자금액 증가 계획은 산업트렌드 변화 및 마이너스 금리환경을 감안할 때 올바른 방향으로 판단, 2025 성공에 대하여, 2025년 중장기 전략을 통해 스마트 모빌리티 솔루션 사업 확장에 대한 의지와 구체적 전략, 원가 절감을 통한 기존 사업 수익성 강화의 가능성과 의지를 재차 확인, 2020년 현대차는 상대적 유리한 파냄 포트폴리오, 신차 출시로 시장 상회하는 판매 증가, 3세대 모듈러 플랫폼 확산으로 비용절감 효과 확대되며 시장 기대치 보다 높은 5% 영업이익 달성 가능성 높을 전망</t>
   </si>
   <si>
     <t>G2협상 또 벼랑끝…글로벌증시 불확실성 커져</t>
@@ -5635,16 +5635,16 @@
     <t>하나금투, "자동차업종 배당투자 현대차우·현대차2우B·한라홀딩스 유망", 현대차우 현대차2우B, 자동차업종에서 배당매력 높은 주식으로 꼽혀</t>
   </si>
   <si>
-    <t>'소버린 사태' 재현 가능성은, 현대차-어느 때보다 균형 잡힌 세단과 SUV 라인업, 2020년 선진 시장 ASP 상승, 신흥 시장 물량 증가 기대, 20년도 하반기 대규모 추가 충당금 설정 가능성 제한 적</t>
+    <t>'소버린 사태' 재현 가능성은, 어느 때보다 균형 잡힌 세단과 SUV 라인업, 2020년 선진 시장 ASP 상승, 신흥 시장 물량 증가 기대, 20년도 하반기 대규모 추가 충당금 설정 가능성 제한 적</t>
   </si>
   <si>
     <t>아시아나항공 매각, 크리스마스 시점으로 연기 등, SK·LG, 대표이사-이사회 의장 분리...독립성 강화 포석</t>
   </si>
   <si>
-    <t>현대차-해외 NDR Key Takeaways: 투자시기 진입, 12/9~12/13일에 미국지역 NDR실시, 변화를 위한 투자시기 진입, 중국에 대해서는 2020년 초에 중장기 계획 발표 예정</t>
-  </si>
-  <si>
-    <t>현대차 주식 매수의견 유지, "신차효과 내년에도 주가에 계속 반영", 현대차-성장 곡선양호, 주춤했던 모멘텀과 주가, 20 년도 성장에 대한 방향성은 확실</t>
+    <t>해외 NDR Key Takeaways: 투자시기 진입, 12/9~12/13일에 미국지역 NDR실시, 변화를 위한 투자시기 진입, 중국에 대해서는 2020년 초에 중장기 계획 발표 예정</t>
+  </si>
+  <si>
+    <t>현대차 주식 매수의견 유지, "신차효과 내년에도 주가에 계속 반영", 성장 곡선양호, 주춤했던 모멘텀과 주가, 20 년도 성장에 대한 방향성은 확실</t>
   </si>
   <si>
     <t>2020년 유망주는 ‘삼성전자·카카오’…리서치센터장 6명 ‘강추’</t>
@@ -5689,10 +5689,10 @@
     <t>"CES 2020 수혜주 잡아라"....주요 종목들 한달간 5%↑</t>
   </si>
   <si>
-    <t>"CES 2020 수혜주 잡아라"....주요 종목들 한달간 5%↑, 최태원 SK그룹 회장, 코스닥 현재 하안가 출발 12.60포인트 하락..코스피는?, 세계 최대 기술전시회 CES 2020 개막 D-2...국내 수혜주는?, 현대차-채워지는 회복의 단추, 19년도 4분기 영업이익은 1.01조원(+100.6% 전년 대비 증감율, OPM 3.7%) 기록, 컨센서스 8.2% 하회 전망, 예정된 임단협합의금(1,200억원 추정), 계절적 비용 증가와 GV80 출시 지연으로 선지급된 홍보/마케팅비용 부담으로 당초 기대에 소폭 못미친 실적 기록 전망, 20년도 2분기 까지 신차 출시 확대에 주목. 기 출시된 쏘나타, 그랜저 F/L 외에 팰리세이드 증산과 GV80, G80, 아반떼, 싼타페 F/L 출시로 믹스 개선(ASP 상승, 인센티브 하락), 볼륨 증가(가동률 회복, 원가율 하락) 기대, 20년도 하반기 주요 신차 출시로 매출 기대치 상향, 20년도 하반기 원가율 개선으로 수익성 기대치 상향 전망. 투자의견 BUY, 목표주가 185,000원 유지, 현대차-할인의 추억, 년도년도 1분기 4분기 , 비용의 역습 : 년도년도 1분기 4분기 현대차의 중국을 제외한 주요 공장의 가동률은 90%를 상회했지만, 연결 기준 전체 도매 판매는 전년 동기 대비 1% 감소했다, 2020년 SUV 전쟁 : 글로벌 수요 둔화와 경쟁사들의 SUV 신차 출시 강화로 판매 경쟁은 날이 갈수 록 심화되고 있다, 험난한 구간 지속: 미국 등 주요 지역의 수요 부진이 지속되고 있는 가운데 경쟁사들의 SUV 신차 출시 확대로 경쟁 강도가 상승 중이다, 정몽구·정의선 父子, 보유주식가치 8천억 원 증가…주식부호 1계단씩 ‘up’</t>
-  </si>
-  <si>
-    <t>[그랜드 CEO in KOREA(11)] 현대家 3세경영 선두주자 정지선 현대백화점그룹 회장, 현대차-년도년도 1분기 4분기 Preview: 할인매수구간 진입, 년도년도 1분기 4분기 Preview: 영업이익 1조 700억원 예상, 시장 기대치 부합, Mix 및 ASP의 대대적 개선이 진행: 실제 발생 이익은 약 1.3조원, 목표주가 165,000원 유지, 저가매수기회로 판단, 현대차-계획 짤 때가 제일 신난다, CES에서 도심형 항공기 제조업 진출 구체화, 새로운 모빌리티 컨셉도 제시</t>
+    <t>"CES 2020 수혜주 잡아라"....주요 종목들 한달간 5%↑, 최태원 SK그룹 회장, 코스닥 현재 하안가 출발 12.60포인트 하락..코스피는?, 세계 최대 기술전시회 CES 2020 개막 D-2...국내 수혜주는?, 채워지는 회복의 단추, 19년도 4분기 영업이익은 1.01조원(+100.6% 전년 대비 증감율, OPM 3.7%) 기록, 컨센서스 8.2% 하회 전망, 예정된 임단협합의금(1,200억원 추정), 계절적 비용 증가와 GV80 출시 지연으로 선지급된 홍보/마케팅비용 부담으로 당초 기대에 소폭 못미친 실적 기록 전망, 20년도 2분기 까지 신차 출시 확대에 주목. 기 출시된 쏘나타, 그랜저 F/L 외에 팰리세이드 증산과 GV80, G80, 아반떼, 싼타페 F/L 출시로 믹스 개선(ASP 상승, 인센티브 하락), 볼륨 증가(가동률 회복, 원가율 하락) 기대, 20년도 하반기 주요 신차 출시로 매출 기대치 상향, 20년도 하반기 원가율 개선으로 수익성 기대치 상향 전망. 투자의견 BUY, 목표주가 185,000원 유지, 할인의 추억, 년도년도 1분기 4분기 , 비용의 역습 : 년도년도 1분기 4분기 현대차의 중국을 제외한 주요 공장의 가동률은 90%를 상회했지만, 연결 기준 전체 도매 판매는 전년 동기 대비 1% 감소했다, 2020년 SUV 전쟁 : 글로벌 수요 둔화와 경쟁사들의 SUV 신차 출시 강화로 판매 경쟁은 날이 갈수 록 심화되고 있다, 험난한 구간 지속: 미국 등 주요 지역의 수요 부진이 지속되고 있는 가운데 경쟁사들의 SUV 신차 출시 확대로 경쟁 강도가 상승 중이다, 정몽구·정의선 父子, 보유주식가치 8천억 원 증가…주식부호 1계단씩 ‘up’</t>
+  </si>
+  <si>
+    <t>[그랜드 CEO in KOREA(11)] 현대家 3세경영 선두주자 정지선 현대백화점그룹 회장, 년도년도 1분기 4분기 Preview: 할인매수구간 진입, 년도년도 1분기 4분기 Preview: 영업이익 1조 700억원 예상, 시장 기대치 부합, Mix 및 ASP의 대대적 개선이 진행: 실제 발생 이익은 약 1.3조원, 목표주가 165,000원 유지, 저가매수기회로 판단, 계획 짤 때가 제일 신난다, CES에서 도심형 항공기 제조업 진출 구체화, 새로운 모빌리티 컨셉도 제시</t>
   </si>
   <si>
     <t>미국과 이란 갈등 속 외국인 자금 유입 韓 증시에 ‘위장된 축복’ 될까?</t>
@@ -5701,7 +5701,7 @@
     <t>CES가 점찍은 ‘마·폴’···IT주 반등 신호탄 될까, '디지털·주가부양' 일석이조 노린 윤종규 KB 회장</t>
   </si>
   <si>
-    <t>현대차-4분기는 하회. 2020년 럭셔리 사이클이 모멘텀, P/B 0.4배 초반으로 글로벌 Peers 중 가장 낮은 수준, 19년도 4분기 Preview: 영업이익률 4.0% 전망, 2020년 도매판매 목표는 458만대(+4%), 칼자루 쥔 국민연금 ‘예상 타깃 리스트’에 대한항공은 없다?</t>
+    <t>4분기는 하회. 2020년 럭셔리 사이클이 모멘텀, P/B 0.4배 초반으로 글로벌 Peers 중 가장 낮은 수준, 19년도 4분기 Preview: 영업이익률 4.0% 전망, 2020년 도매판매 목표는 458만대(+4%), 칼자루 쥔 국민연금 ‘예상 타깃 리스트’에 대한항공은 없다?</t>
   </si>
   <si>
     <t>‘국민연금 지분율’ 따라 기업도 롤러코스터</t>
@@ -5710,16 +5710,16 @@
     <t>현기차에 배팅하는 개미들, 주가는 언제 상승 할까</t>
   </si>
   <si>
-    <t>현대차-수익성 개선의 포인트는 원가, 19년도 4분기 Preview - 영업이익 1조 589억원(OPM 3.9%) 전망, 수익성 개선의 포인트는 원가, "스타트업 생태계에 독 풀었다"…손정의의 민낯?, 현대모비스 주식 매수의견 유지, “전동화부문 하반기 실적개선”, 현대로템 갑작스런 주가상승중 왜?, 현대차-Smart Mobility Provider로 변화 추진, 2020년 선진 시장 ASP 상승, 신흥 시장 물량 증가 기대, UBER와 개인 비행체 분야에서 글로벌 제휴 체결, 현대차-완전 자율주행과 같은 정밀한 Path-finding이 필요한 시기, 현재에 대한 개선과 미래에 대한 준비에 긍정적 결과값을 보이기 시작한 현대차, 그러나 공격적 투자 이후의 Return에 대한 시장의 신중론 확산이 밸류에이션 부담 요인으로 작용 중</t>
+    <t>수익성 개선의 포인트는 원가, 19년도 4분기 Preview - 영업이익 1조 589억원(OPM 3.9%) 전망, 수익성 개선의 포인트는 원가, "스타트업 생태계에 독 풀었다"…손정의의 민낯?, 현대모비스 주식 매수의견 유지, “전동화부문 하반기 실적개선”, 현대로템 갑작스런 주가상승중 왜?, Smart Mobility Provider로 변화 추진, 2020년 선진 시장 ASP 상승, 신흥 시장 물량 증가 기대, UBER와 개인 비행체 분야에서 글로벌 제휴 체결, 완전 자율주행과 같은 정밀한 Path-finding이 필요한 시기, 현재에 대한 개선과 미래에 대한 준비에 긍정적 결과값을 보이기 시작한 현대차, 그러나 공격적 투자 이후의 Return에 대한 시장의 신중론 확산이 밸류에이션 부담 요인으로 작용 중</t>
   </si>
   <si>
     <t>"현대모비스 주가 상승 가능", 친환경차 수요 늘어 전동화부품도 성장, 한온시스템, 폴크스바겐 전기차 생산 확대 덕에 매출 증가 가능</t>
   </si>
   <si>
-    <t>현대차-년도년도 1분기 4분기 Preview, 년도년도 1분기 4분기 현대차 매출 및 영업이익은 27조 1,207억원, 1조 166억원으로 전년동기 대비 7.5%, 102.9 % 증가할 것으로 전망한다., 2020년 연간 매출 107.8조원(전년 대비 증감율+ 2.6%), 영업이익 4.7조원(전년 대비 증감율+35.9%)을 전망한다., 美 투자사도 현대차 '매도'···지분율 대폭율 대폭 축소, 한온시스템 주식 매수의견 유지, “전기차부품 공급 올해부터 본격화”, 캐롯손해보험 출격…디지털 보험 시장 선점 경쟁 막 올랐다</t>
-  </si>
-  <si>
-    <t>현대차 주식 매수의견 유지, "제네시스 GV80 판매로 이익 증가 예상", 현대차-뒤늦게 찾아온 부활절, 제네시스 GV80 출시, 제네시스 브랜드 부활로 현대차 이익 증가 전망</t>
+    <t>년도년도 1분기 4분기 Preview, 년도년도 1분기 4분기 현대차 매출 및 영업이익은 27조 1,207억원, 1조 166억원으로 전년동기 대비 7.5%, 102.9 % 증가할 것으로 전망한다., 2020년 연간 매출 107.8조원(전년 대비 증감율+ 2.6%), 영업이익 4.7조원(전년 대비 증감율+35.9%)을 전망한다., 美 투자사도 현대차 '매도'···지분율 대폭율 대폭 축소, 한온시스템 주식 매수의견 유지, “전기차부품 공급 올해부터 본격화”, 캐롯손해보험 출격…디지털 보험 시장 선점 경쟁 막 올랐다</t>
+  </si>
+  <si>
+    <t>현대차 주식 매수의견 유지, "제네시스 GV80 판매로 이익 증가 예상", 뒤늦게 찾아온 부활절, 제네시스 GV80 출시, 제네시스 브랜드 부활로 현대차 이익 증가 전망</t>
   </si>
   <si>
     <t>삼성전자 올해 시가총액 27조 늘어..이재용 공판 결과에 영향 받을까?</t>
@@ -5728,13 +5728,13 @@
     <t>MS·블랙록도 콕 찍었다…월가 달구는 'ESG펀드 투자 열풍', 꿈을 먹고 사는 주식 투자자들</t>
   </si>
   <si>
-    <t>현대차-제네시스SUV 라인업 강화 및 수익구조 턴어라운드, 제네시스 라인업 강화에 주목, SUV 비중 높아지며 수익구조 턴어라운드, 투자의견 매수와 목표주가 170 000 원 유지, 현대차-믹스 개선과 우호적 환율 효과 지속, 내수와 북미 믹스개선과 우호적 원달러 환율흐름이 지속되며 컨센서스 수준의 양호한 실적 전망, 믹스개선과 환율 상승에 따른 자연스러운 전년 대비 증감율 실적개선 기대감은 2020년 하반기로 갈수록 옅어지지만, 구형 모델 소진에 따른 후행적인 원가율 개선이 확인된다면 증익 기대감은 지속될 수 있을 전망, 이노션 주식 매수의견 유지, "제네시스 GV80 출시로 광고물량 증가", LG화학, 현대차와 배터리부문 제휴?...장중 주가 '급등'</t>
-  </si>
-  <si>
-    <t>현대차 지배구조 개편 발목잡던 엘리엇, 모든 지분 팔았다, 엘리엇, 현대차그룹 지분 모두 처분, 엘리엇, 현대차그룹 지분 모두 처분…지배구조 개편 속도높이나, 현대차 지배구조개편 훼방 놓던 엘리엇, 계열사 지분 모두 매각, 현대차그룹에 반기들던 엘리엇, 지분 팔고 빠져나가, 엘리엇, 현대차그룹 계열사 지분 전략 매각, 현대차-19년도 4분기 Review: 어려운 산업에서 좋은 주식이 되다, 발표실적 vs 컨센서스: 4분기 영업이익은 1.2조원으로 시장 기대치 1조원을 크게 (+15.7%)상회. 이는 일회성비용인 통상임금 합의금 2천억원 포함 이익. 대수 감소에도 신차 믹스개선과 환율효과, 원가절감으로 매출액과 수익성 모두 개선 ., 이익전망 변경: 신차효과가 환율효과를 넘어서기 시작하면서 2020년 5%OPM달성에 대한 신뢰도 상승. 2020년 EPS를 15.2%상향. 실적가시성이 높아지면서 당분간 주가는 강세를 기록할 전망, 현대차-년도년도 1분기 4분기 Review - 호실적의 이유와 2020년에 달라질 점, 기대를 상회한 영업이익 발표. 2020년에는 새로운 이익 증가 요인 나타날 것, 년도년도 1분기 4분기 영업이익 1.2조원 (+148.2% 전년 대비 증감율), 시장 컨센서스 15.5% 상회. 세그먼트 대형화가 핵심, 2020년에는 세그먼트 대형화 이외의 영업이익 증가 요소를 보여줄 것으로 예상, 현대차 공격하던 엘리엇, 지분 다 팔고 떠났다, 美 헤지펀드 엘리엇, 현대車 지분 다 팔았다</t>
-  </si>
-  <si>
-    <t>ESG는 새로운 펀드팔이 방법일까, 일감몰아주기, 재벌총수일가 이외 모두 피해자, 韓 경제, 10년 만 최악 2.0% 성장으로 `성장 쇼크` 빠져, 현대차 주식 매수의견 유지, "고가 자동차 판매비중 늘어 긍정적", 엘리엇, 현대차 계열사 지분 모두 '매각', 현대차 공격 엘리엇 참패철수, 투기자본 막을 차등의결 허용해야, 엘리엇 떠난 현대차, 지배구조 개편 시동 거나, 美 행동주의 헤지펀드 엘리엇, 현대차그룹 지분 모두 매각, 100조 클럽 가입한 현대차, 엘리엇 리스크도 털었다, 엘리엇, 현대차 지분 매각…전쟁선포 20개월만에 ‘백기’, 엘리엇, 현대차그룹 지분 모두 처분, 현대차 ‘시총 30조클럽’ 가입 성큼, 현대차 경영 참여 요구한 '엘리엇매니지먼트' 지분 팔고 떠났다, 100조클럽 가입·엘리엇 퇴치…현대차그룹 '겹경사', 현대차, ‘시총 30조 클럽’ 가입 눈앞…글로벌 완성차들과 격차는 여전, 증권계 "현대차, 올해 실적도 기대"...장중 주가 또 '급등', 현대차그룹 지배구조개편 제동 건 ‘엘리엇’ 지분 모두 팔았다, 현대차-기대치 상회, 주가 반전 시작된다, 19년도 4분기 Review: 영업이익 기준 기대치 상회하는 호실적, 제네시스 SUV 출시 효과, 주가 반전 시작된다, 엘리엇 철수… 현대차 지배구조 개편 탄력, 현대차-주문하신 서프라이즈 나왔습니다, 컨센서스 16% 상회, 일회성 비용 2천억원 감안 시 34% 상회, 우호적 환율과 믹스개선, 원가절감 덕분. 이는 2020년에도 이어질 전망, 수익성 가이던스 달성 가시성 상승, 보수적인 컨센서스 높아질 전망, 현대차-믹스 개선이 견인한 서프라이즈, 19년도 4분기 연결 매출 27,868 십억원 (전년 대비 증감율+10.5%), OP 1,244 십억원 (전년 대비 증감율%+ 2 %, OPM 4.5%) 기록, 19년도 2분기 에 이어 다시 한번 연결 영업이익 1.2 조원을 수성 (OPM Y oY+2.5% pt), 현대차-기대치 상회, 주가 반전 시작된다, 19년도 4분기 Review: 영업이익 기준 기대치 상회하는 호실적, 제네시스 SUV 출시 효과, 주가 반전 시작된다, 현대차-실적 방향성에 대한 시장의 신뢰 상승, 년도년도 1분기 4분기 시장기대치를 큰 폭으로 상회하는 분기 실적 달성, 년도년도 1분기 4분기 일회성 비용을 제외한 영업이익률은 5.1%로 20년 목표 영업이익률 5.0% 실현 가능성에 대한 시장의 신뢰 큰 폭으로 상승 (시장기대치 우상향 지속 전망), 20년도 하반기 신차효과 통한 지속적인 실적개선과 유럽 EV 판매점유율 확대를 통한 과징금 규제 회피로 기업가치 개선 지속될 수 있다고 판단, 현대차-무엇보다 반가운 설 선물, 19년도 4분기 Review, 어닝 서프라이즈 실현, 20년 실적에 대한 시장 기대치 우상향 지속 전망, 유럽 탄소배출 규제 넘어설 EV 판매 실현으로 기업가치 개선 가속 예정, 현대차-2019년 4분기 실적 Review, 19년도 4분기 실적 Review, 올해 글로벌 도매 판매 목표, 올해 수익성 개선 기대, 현대차-무엇보다 반가운 설 선물, 19년도 4분기 Review: 예상을 뛰어넘은 실적 기록, 2020년 이익과 주가의 눈높이는 더욱 상향될 전망, 현대차-숫자로 확인한 믹스개선 효과, 4Q 19 Review: 시장 컨센서스 상회, 2020년에도 믹스 개선 지속, 현대차-상반기 반등을 즐기자, 19년도 4분기 , Surprise, 상반기 반등을 즐기자, 투자의견 상향, 현대차-덜 팔아도 성장하는 방법을 알다, 고가차를 많이 팔면 된다, 19년도 4분기 Review: 영업이익률 4.5% 기록, 컨퍼런스 콜의 주요 내용: 자동차 영업이익률 5.0% 재확인, 현대차-믿음직한 맏형, 4분기 영업이익 1.24조원(+148.2%)으로 시장 기대치 상회, 펀더멘탈 정상화에 대한 신뢰를 회복할 시점, 목표주가 170,000원, 투자의견 매수 유지, '앓던 이' 엘리엇 퇴장…현대차 '정의선 리더십' 날개 단다, 엘리엇, 현대차 지분 모두 팔아… 정의선 체제 완성 박차, 엘리엇, 현대차에 ‘백기’… 정의선 미래 구상 탄력, 글로비스 첫 회사채…엘리엇 부담덜고 몸값높이기 수순, 현대차-믹스 개선이 견인한 서프라이즈, 19년도 4분기 연결 매출 27,868 십억원 (전년 대비 증감율+10.5%), OP 1,244 십억원 (전년 대비 증감율%+ 2 %, OPM 4.5%) 기록, 19년도 2분기 에 이어 다시 한번 연결 영업이익 1.2 조원을 수성 (OPM Y oY+2.5% pt), 현대차-주문하신 서프라이즈 나왔습니다, 컨센서스 16% 상회, 일회성 비용 2천억원 감안 시 34% 상회, 우호적 환율과 믹스개선, 원가절감 덕분. 이는 2020년에도 이어질 전망, 수익성 가이던스 달성 가시성 상승, 보수적인 컨센서스 높아질 전망</t>
+    <t>제네시스SUV 라인업 강화 및 수익구조 턴어라운드, 제네시스 라인업 강화에 주목, SUV 비중 높아지며 수익구조 턴어라운드, 투자의견 매수와 목표주가 170 000 원 유지, 믹스 개선과 우호적 환율 효과 지속, 내수와 북미 믹스개선과 우호적 원달러 환율흐름이 지속되며 컨센서스 수준의 양호한 실적 전망, 믹스개선과 환율 상승에 따른 자연스러운 전년 대비 증감율 실적개선 기대감은 2020년 하반기로 갈수록 옅어지지만, 구형 모델 소진에 따른 후행적인 원가율 개선이 확인된다면 증익 기대감은 지속될 수 있을 전망, 이노션 주식 매수의견 유지, "제네시스 GV80 출시로 광고물량 증가", LG화학, 현대차와 배터리부문 제휴?...장중 주가 '급등'</t>
+  </si>
+  <si>
+    <t>현대차 지배구조 개편 발목잡던 엘리엇, 모든 지분 팔았다, 엘리엇, 현대차그룹 지분 모두 처분, 엘리엇, 현대차그룹 지분 모두 처분…지배구조 개편 속도높이나, 현대차 지배구조개편 훼방 놓던 엘리엇, 계열사 지분 모두 매각, 현대차그룹에 반기들던 엘리엇, 지분 팔고 빠져나가, 엘리엇, 현대차그룹 계열사 지분 전략 매각, 19년도 4분기 Review: 어려운 산업에서 좋은 주식이 되다, 발표실적 vs 컨센서스: 4분기 영업이익은 1.2조원으로 시장 기대치 1조원을 크게 (+15.7%)상회. 이는 일회성비용인 통상임금 합의금 2천억원 포함 이익. 대수 감소에도 신차 믹스개선과 환율효과, 원가절감으로 매출액과 수익성 모두 개선 ., 이익전망 변경: 신차효과가 환율효과를 넘어서기 시작하면서 2020년 5%OPM달성에 대한 신뢰도 상승. 2020년 EPS를 15.2%상향. 실적가시성이 높아지면서 당분간 주가는 강세를 기록할 전망, 년도년도 1분기 4분기 Review - 호실적의 이유와 2020년에 달라질 점, 기대를 상회한 영업이익 발표. 2020년에는 새로운 이익 증가 요인 나타날 것, 년도년도 1분기 4분기 영업이익 1.2조원 (+148.2% 전년 대비 증감율), 시장 컨센서스 15.5% 상회. 세그먼트 대형화가 핵심, 2020년에는 세그먼트 대형화 이외의 영업이익 증가 요소를 보여줄 것으로 예상, 현대차 공격하던 엘리엇, 지분 다 팔고 떠났다, 美 헤지펀드 엘리엇, 현대車 지분 다 팔았다</t>
+  </si>
+  <si>
+    <t>ESG는 새로운 펀드팔이 방법일까, 일감몰아주기, 재벌총수일가 이외 모두 피해자, 韓 경제, 10년 만 최악 2.0% 성장으로 `성장 쇼크` 빠져, 현대차 주식 매수의견 유지, "고가 자동차 판매비중 늘어 긍정적", 엘리엇, 현대차 계열사 지분 모두 '매각', 현대차 공격 엘리엇 참패철수, 투기자본 막을 차등의결 허용해야, 엘리엇 떠난 현대차, 지배구조 개편 시동 거나, 美 행동주의 헤지펀드 엘리엇, 현대차그룹 지분 모두 매각, 100조 클럽 가입한 현대차, 엘리엇 리스크도 털었다, 엘리엇, 현대차 지분 매각…전쟁선포 20개월만에 ‘백기’, 엘리엇, 현대차그룹 지분 모두 처분, 현대차 ‘시총 30조클럽’ 가입 성큼, 현대차 경영 참여 요구한 '엘리엇매니지먼트' 지분 팔고 떠났다, 100조클럽 가입·엘리엇 퇴치…현대차그룹 '겹경사', 현대차, ‘시총 30조 클럽’ 가입 눈앞…글로벌 완성차들과 격차는 여전, 증권계 "현대차, 올해 실적도 기대"...장중 주가 또 '급등', 현대차그룹 지배구조개편 제동 건 ‘엘리엇’ 지분 모두 팔았다, 기대치 상회, 주가 반전 시작된다, 19년도 4분기 Review: 영업이익 기준 기대치 상회하는 호실적, 제네시스 SUV 출시 효과, 주가 반전 시작된다, 엘리엇 철수… 현대차 지배구조 개편 탄력, 주문하신 서프라이즈 나왔습니다, 컨센서스 16% 상회, 일회성 비용 2천억원 감안 시 34% 상회, 우호적 환율과 믹스개선, 원가절감 덕분. 이는 2020년에도 이어질 전망, 수익성 가이던스 달성 가시성 상승, 보수적인 컨센서스 높아질 전망, 믹스 개선이 견인한 서프라이즈, 19년도 4분기 연결 매출 27,868 십억원 (전년 대비 증감율+10.5%), OP 1,244 십억원 (전년 대비 증감율%+ 2 %, OPM 4.5%) 기록, 19년도 2분기 에 이어 다시 한번 연결 영업이익 1.2 조원을 수성 (OPM Y oY+2.5% pt), 기대치 상회, 주가 반전 시작된다, 19년도 4분기 Review: 영업이익 기준 기대치 상회하는 호실적, 제네시스 SUV 출시 효과, 주가 반전 시작된다, 실적 방향성에 대한 시장의 신뢰 상승, 년도년도 1분기 4분기 시장기대치를 큰 폭으로 상회하는 분기 실적 달성, 년도년도 1분기 4분기 일회성 비용을 제외한 영업이익률은 5.1%로 20년 목표 영업이익률 5.0% 실현 가능성에 대한 시장의 신뢰 큰 폭으로 상승 (시장기대치 우상향 지속 전망), 20년도 하반기 신차효과 통한 지속적인 실적개선과 유럽 EV 판매점유율 확대를 통한 과징금 규제 회피로 기업가치 개선 지속될 수 있다고 판단, 무엇보다 반가운 설 선물, 19년도 4분기 Review, 어닝 서프라이즈 실현, 20년 실적에 대한 시장 기대치 우상향 지속 전망, 유럽 탄소배출 규제 넘어설 EV 판매 실현으로 기업가치 개선 가속 예정, 2019년 4분기 실적 Review, 19년도 4분기 실적 Review, 올해 글로벌 도매 판매 목표, 올해 수익성 개선 기대, 무엇보다 반가운 설 선물, 19년도 4분기 Review: 예상을 뛰어넘은 실적 기록, 2020년 이익과 주가의 눈높이는 더욱 상향될 전망, 숫자로 확인한 믹스개선 효과, 4Q 19 Review: 시장 컨센서스 상회, 2020년에도 믹스 개선 지속, 상반기 반등을 즐기자, 19년도 4분기 , Surprise, 상반기 반등을 즐기자, 투자의견 상향, 덜 팔아도 성장하는 방법을 알다, 고가차를 많이 팔면 된다, 19년도 4분기 Review: 영업이익률 4.5% 기록, 컨퍼런스 콜의 주요 내용: 자동차 영업이익률 5.0% 재확인, 믿음직한 맏형, 4분기 영업이익 1.24조원(+148.2%)으로 시장 기대치 상회, 펀더멘탈 정상화에 대한 신뢰를 회복할 시점, 목표주가 170,000원, 투자의견 매수 유지, '앓던 이' 엘리엇 퇴장…현대차 '정의선 리더십' 날개 단다, 엘리엇, 현대차 지분 모두 팔아… 정의선 체제 완성 박차, 엘리엇, 현대차에 ‘백기’… 정의선 미래 구상 탄력, 글로비스 첫 회사채…엘리엇 부담덜고 몸값높이기 수순, 믹스 개선이 견인한 서프라이즈, 19년도 4분기 연결 매출 27,868 십억원 (전년 대비 증감율+10.5%), OP 1,244 십억원 (전년 대비 증감율%+ 2 %, OPM 4.5%) 기록, 19년도 2분기 에 이어 다시 한번 연결 영업이익 1.2 조원을 수성 (OPM Y oY+2.5% pt), 주문하신 서프라이즈 나왔습니다, 컨센서스 16% 상회, 일회성 비용 2천억원 감안 시 34% 상회, 우호적 환율과 믹스개선, 원가절감 덕분. 이는 2020년에도 이어질 전망, 수익성 가이던스 달성 가시성 상승, 보수적인 컨센서스 높아질 전망</t>
   </si>
   <si>
     <t>'엘리엇의 현대차 공격 실패와 대조적'…日 행동주의펀드 활동 2배 늘어</t>
@@ -5743,7 +5743,7 @@
     <t>‘엘리엇·실적 리스크’ 걷어낸 현대차, 지배구조 개편 밑그림 나오나, 이코노미스트가 권하는 ‘2030세대’ 재테크 전략</t>
   </si>
   <si>
-    <t>'우한 폐렴' 공포 고조… 산업계 드리우는 먹구름, 우한 폐렴에 글로벌 車들 고민 커지는데...현대차는 장중 주가 '강세', 무슨 일?, 현대차-가시성이 높아진 수익성 개선, 19년도 4분기 Review-신차효과와 믹스개선의 반영, 가시성이 높아진 수익성 개선</t>
+    <t>'우한 폐렴' 공포 고조… 산업계 드리우는 먹구름, 우한 폐렴에 글로벌 車들 고민 커지는데...현대차는 장중 주가 '강세', 무슨 일?, 가시성이 높아진 수익성 개선, 19년도 4분기 Review-신차효과와 믹스개선의 반영, 가시성이 높아진 수익성 개선</t>
   </si>
   <si>
     <t>현대건설 국내외 수주 다 잡았다, 박동욱 주가는 아쉬워</t>
@@ -5758,7 +5758,7 @@
     <t>'미래 유망 산업' 연료전지 투자자가 알아야 할 5가지, 영원한 아군도 적도 없는 재계, 지배구조 재편 ‘서막’</t>
   </si>
   <si>
-    <t>현대차-년도년도 1분기 4분기 NDR Review: 흔들리지 않는 편안함, 년도년도 1분기 4분기 현대차 실적은 1) 2,000억원 임단협 합의금 일회성 지급과 볼륨 감소라는 부정적 요인에도, 2) 환율 효과와 예상 이상의 믹스 개선효과가 지속되며 실적 견인, 20년도 1분기 국내 개소세인하 종료, 중국 코로나바이러스 수요 부진, 인도 BS6(4월) 전 수요 감소 영향으로 볼륨은 부진하나 원/달러 상승, 신차 출시(그랜져 F/L, 팰리세이드 증산, 쏘나타 미국, GV80 내수 출시)로 믹스 개선과 인센티브(플릿축소) 개선되며 실적 개선 견인할 전망, 매도 폭탄 외국인, 그래도 사들인 종목은</t>
+    <t>년도년도 1분기 4분기 NDR Review: 흔들리지 않는 편안함, 년도년도 1분기 4분기 현대차 실적은 1) 2,000억원 임단협 합의금 일회성 지급과 볼륨 감소라는 부정적 요인에도, 2) 환율 효과와 예상 이상의 믹스 개선효과가 지속되며 실적 견인, 20년도 1분기 국내 개소세인하 종료, 중국 코로나바이러스 수요 부진, 인도 BS6(4월) 전 수요 감소 영향으로 볼륨은 부진하나 원/달러 상승, 신차 출시(그랜져 F/L, 팰리세이드 증산, 쏘나타 미국, GV80 내수 출시)로 믹스 개선과 인센티브(플릿축소) 개선되며 실적 개선 견인할 전망, 매도 폭탄 외국인, 그래도 사들인 종목은</t>
   </si>
   <si>
     <t>마스크·손 소독제 사재기 '엄벌'…최대 징역 2년</t>
@@ -5797,7 +5797,7 @@
     <t>코스피 코스닥 1%대 동반하락, 코로나19로 경기둔화 우려에 눌려, 코스피 코스닥 동반하락 출발, 한신기계 피씨디렉트 에너토크 급등, 윤석열 부인 의혹 '물타기 제목'에 뉴스타파 기자 "그런식 안돼", 코스피 코스닥 중반 1%대 동반하락, 신풍제약 씨젠 피씨디렉트 급등</t>
   </si>
   <si>
-    <t>"현대차, 독일 렌터카회사 인수 땐 모빌리티 전략 구현에 도움", 코스피 초반 '상승' 코스닥 '하락', 국보 KR모터스 구영테크 급등, 황각규 롯데지주 대표이사 부회장, 현대차-구체화되는 스마트 모빌리티, 현대캐피탈 주도로 독일 렌터카 회사 인수설, 현실화 될 경우 스마트 모빌리티 구현에 더 가까워질 전망, 현대차 주식 매수의견 유지, "독일 렌터카회사 사면 모빌리티 강화"</t>
+    <t>"현대차, 독일 렌터카회사 인수 땐 모빌리티 전략 구현에 도움", 코스피 초반 '상승' 코스닥 '하락', 국보 KR모터스 구영테크 급등, 황각규 롯데지주 대표이사 부회장, 구체화되는 스마트 모빌리티, 현대캐피탈 주도로 독일 렌터카 회사 인수설, 현실화 될 경우 스마트 모빌리티 구현에 더 가까워질 전망, 현대차 주식 매수의견 유지, "독일 렌터카회사 사면 모빌리티 강화"</t>
   </si>
   <si>
     <t>골라보는 재미…한국 기업 주총 드라마, 코스피 코스닥 동반상승 출발, 랩지노믹스 누리플랜 피씨엘 급등, 코스피 코스닥 장중 동반하락, 모나리자 창해에탄올 웰크론 승일 급등, 코스피 코스닥 동반하락, 코로나19 지역감역 확산에 짓눌려</t>
@@ -5842,13 +5842,13 @@
     <t>코스피 코스닥 동반하락 출발, 쌍방울 컨버즈 씨젠 모나미 급등, 삼성전자 현대차 주가 초반 2%대 하락, 코스피 시총 상위 10종목 약세</t>
   </si>
   <si>
-    <t>현대차-전기차와 프리미엄 시장 모두 진입한다, Top Pick으로 전환: 밸류에이션 프리미엄 적용 시점, 코로나 생산차질은 잊어라. 핵심 라인 재가동의 시작을 보자, 유럽 전기차 시장의 강자로 급부상. 코나EV 증산효과 기대, 적극매수 타이밍: 목표주가 175,000원 유지, 정몽규 HDC그룹 회장, '혁신과 파격의 아이콘' 아시아나항공 품다, 현대모비스 주식 매수의견 유지, “현대기아차 친환경차 확대의 수혜”, 코스피 코스닥 동반급락 출발, 청호컴넷 레몬 수젠텍 씨젠 급등, 코스피 시총 상위 10종목 초반 약세, 삼성전자 SK하이닉스 급락, 코스피 코스닥 장중 동반 하락폭 커져, 모나미 랩지노믹스 피씨엘 급등</t>
-  </si>
-  <si>
-    <t>현대차-초점은 차에서 에너지로, 투자의견 BUY, 목표주가 185,000원, Top-pick 유지, 원가 경쟁력 확보되는 2030년 이후 대중화 수혜 기대, 코스피 '뉴욕증시 폭락' 이겨내고 반등, 코스닥도 3거래일 만에 올라, 코스피 시총 상위 10종목 초반 혼조, 삼성전자 SK하이닉스 올라, 코스피 코스닥 동반하락 출발, JW중외제약 코센 수젠텍 급등, 코스피 코스닥 장중 하락 반전, 일양약품 지노믹트리 한국알콜 급등, 현대차 주식 매수의견 유지, "수소연료전지차와 에너지사업에서 기회"</t>
-  </si>
-  <si>
-    <t>코스피 2%대 급락해 1900선 겨우 지켜, 코스닥도 3%대 폭락, 현대차 주가 계속 떨어져 10만 원 겨우 지켜, 현대위아 3%대 하락, 현대차-실적 업데이트 및 목표주가 변경, 현대차, 1분기 영업이익 8,730억원 전망, 이익 전망치 8% 하향, 목표주가 16만원으로 하향, 투자의견 매수 유지, 삼성전자 외국인 대차거래 집중, 코스피 코스닥 동반하락 출발, 이에스브이 한프 마크로젠 급등, ‘외국계 큰손’ 현대차·현대해상 담았다, 外人 삼성전자 대차거래 급증…시총 31조 증발, 2월 ‘외국계 큰손’, 헬릭스미스·현대차·현대해상 담았다</t>
+    <t>전기차와 프리미엄 시장 모두 진입한다, Top Pick으로 전환: 밸류에이션 프리미엄 적용 시점, 코로나 생산차질은 잊어라. 핵심 라인 재가동의 시작을 보자, 유럽 전기차 시장의 강자로 급부상. 코나EV 증산효과 기대, 적극매수 타이밍: 목표주가 175,000원 유지, 정몽규 HDC그룹 회장, '혁신과 파격의 아이콘' 아시아나항공 품다, 현대모비스 주식 매수의견 유지, “현대기아차 친환경차 확대의 수혜”, 코스피 코스닥 동반급락 출발, 청호컴넷 레몬 수젠텍 씨젠 급등, 코스피 시총 상위 10종목 초반 약세, 삼성전자 SK하이닉스 급락, 코스피 코스닥 장중 동반 하락폭 커져, 모나미 랩지노믹스 피씨엘 급등</t>
+  </si>
+  <si>
+    <t>초점은 차에서 에너지로, 투자의견 BUY, 목표주가 185,000원, Top-pick 유지, 원가 경쟁력 확보되는 2030년 이후 대중화 수혜 기대, 코스피 '뉴욕증시 폭락' 이겨내고 반등, 코스닥도 3거래일 만에 올라, 코스피 시총 상위 10종목 초반 혼조, 삼성전자 SK하이닉스 올라, 코스피 코스닥 동반하락 출발, JW중외제약 코센 수젠텍 급등, 코스피 코스닥 장중 하락 반전, 일양약품 지노믹트리 한국알콜 급등, 현대차 주식 매수의견 유지, "수소연료전지차와 에너지사업에서 기회"</t>
+  </si>
+  <si>
+    <t>코스피 2%대 급락해 1900선 겨우 지켜, 코스닥도 3%대 폭락, 현대차 주가 계속 떨어져 10만 원 겨우 지켜, 현대위아 3%대 하락, 실적 업데이트 및 목표주가 변경, 현대차, 1분기 영업이익 8,730억원 전망, 이익 전망치 8% 하향, 목표주가 16만원으로 하향, 투자의견 매수 유지, 삼성전자 외국인 대차거래 집중, 코스피 코스닥 동반하락 출발, 이에스브이 한프 마크로젠 급등, ‘외국계 큰손’ 현대차·현대해상 담았다, 外人 삼성전자 대차거래 급증…시총 31조 증발, 2월 ‘외국계 큰손’, 헬릭스미스·현대차·현대해상 담았다</t>
   </si>
   <si>
     <t>12일 장 마감 후 주요 종목 뉴스, 코스피 코스닥 장중 4%대로 낙폭 커져, 진원생명과학 휴마시스 급등, 코스피 코스닥 1%대 동반하락 출발, 부광약품 한프 휴마시스 급등, 심상찮게 움직이는 주식시장…SK·현대차 CEO 잇단 ‘주주 달래기’</t>
@@ -5857,7 +5857,7 @@
     <t>12일 장 마감 후 주요 종목 뉴스, 매각설 나도는 이베이코리아, 코스피 코스닥 동반폭락 출발, 신풍제약 화일약품 한프 급등, 팬데믹 공포에… 현대차 하루 만에 8만원대 ‘신저가’, 코스피 코스닥 장중 급락 지속, 흥아해운 이노인스트루먼트는 급등, '코로나패닉' 한국경제, 콘트롤타워가 안보인다(종합), 삼성전자 SK하이닉스 현대차 주식 외국인 매도공세는 언제 끝날까, HDC현대산업개발, 3450억 채무보증 결정外</t>
   </si>
   <si>
-    <t>현대차-공포의 정량화에 근거한 기업가치 정상화 기대, 피해갈 수 없는 C19, 20년 판매 -7%, EPS -11%, 12개월 TP -12% 조정, 그러나 PBR 0.29배는 존속 가능성 우려가 팽배했던 18년말보다 낮은 가치평가, C19 전 확인됐던 판매 경쟁력 여전히 유효, 이제 공포 이후를 바라볼 시기, 16일 장 마감 이후 주요 종목뉴스, 현대차 주가 5% 급락해 계속 빠져, 기아차 6% 하락 계열사 약세 지속, 코스피 코스닥 3%대 동반급락, 미국 금리 전격 인하에 경기침체 우려 커져, 현대차 정몽구·정의선 주식가치, 한달새 1.3兆 증발, 윤석열 검찰총장 처갓집의 비밀</t>
+    <t>공포의 정량화에 근거한 기업가치 정상화 기대, 피해갈 수 없는 C19, 20년 판매 -7%, EPS -11%, 12개월 TP -12% 조정, 그러나 PBR 0.29배는 존속 가능성 우려가 팽배했던 18년말보다 낮은 가치평가, C19 전 확인됐던 판매 경쟁력 여전히 유효, 이제 공포 이후를 바라볼 시기, 16일 장 마감 이후 주요 종목뉴스, 현대차 주가 5% 급락해 계속 빠져, 기아차 6% 하락 계열사 약세 지속, 코스피 코스닥 3%대 동반급락, 미국 금리 전격 인하에 경기침체 우려 커져, 현대차 정몽구·정의선 주식가치, 한달새 1.3兆 증발, 윤석열 검찰총장 처갓집의 비밀</t>
   </si>
   <si>
     <t>코로나19에 시장 급락… 코스닥株 전환가액 조정 공시 봇물, 16일 장 마감 이후 주요 종목뉴스, 은성수 금융위원회 위원장, 현대차 주가 떨어져 8만 원 겨우 지켜, 현대차그룹주 계속 빠져</t>
@@ -5875,13 +5875,13 @@
     <t>국내 기업 1분기 실적 전망치 17%나 내려 잡았다, 하나銀 인니지점 폐쇄·'삼성·SK 반도체장비 공급' 램리서치 셧다운(3월3주차)</t>
   </si>
   <si>
-    <t>현대·기아차 해외생산 30% 마비되자 '보폭 넓히는' 정의선, 코스피 3천포인트 간다는 말 믿고 아내 몰래 대출 받아 '주식 5억' 샀다가 깡통 된 남편, (Today 공시)칩스앤미디어, 주당 0.3주 무상증자 결정, 정의선, 190억원어치 자사주 매입, 정의선의 현대차그룹 '공포' 뚫고 하이킥 선언, '성장의 봄'을 화두로 제안, 정의선, 현대차‧모비스 주식 190억 어치 매입, 정의선의 '책임경영·자신감'···현대차·현대모비스 주식 190억 매입, 정의선, 현대차ㆍ현대모비스 주식 190억원치 매입…“책임경영ㆍ지배력 강화”, 코스피 코스닥 5%대 동반급락, 외국인과 기관 '쌍끌이 매도' 거세, 정의선, 현대車·현대모비스 주식 샀다, '코로나발 주가폭락' 증여 타이밍일까, 정의선, 현대차·모비스 주식 샀다…"주주가치 지킬 것", 삼성전자·LG전자·현대자동차 인도공장 일시 가동 중단, 정의선 수석부회장, 현대차·현대모비수 주식 매수, 정의선 현대차 부회장, 현대차·현대모비스 주식 190억원 매입..책임경영 의지 강조, 정의선, 주주가치 제고 위해 현대차·모비스 주식 매입, 현대차-배당수익률 9%를 상회하는 우선주, P/B 0.2배 중반의 Valuation과 9% 상회하는 우선주 배당수익률, 주당 배당금의 축소 가능성은 낮은 편, 여전히 양호한 신차 사이클, 현대차-코로나 극복과 함께 정상화될 주가, 연간 생산 판매 지연은 불가피하나, 코로나 완화되며 정상화될 것으로 판단한다, (코로나 제외한) 현대차 실적의 핵심은 ‘신차 출시에 따른 믹스개선’이다, 정의선 “책임경영”...현대차·모비스 자사주 190억 매입, 정의선, 190억어치 현대車·모비스株 샀다, 정의선 현대車 부회장, 책임경영 일환 현대차·모비스 주식 190억 매입, 정의선 현대차그룹 수석부회장, 현대차·현대모비스 주식 190억원어치 매수, 코스피 코스닥 6%대 급락 출발, 신풍제약 한진칼 비씨월드제약 급등, 정기선 부사장 경영 능력 도마...노조 "세습경영에 올인", 코스피 코스닥 장중 하락폭 줄어, 한진칼 금호전기 셀트리온제약 급등, 정의선, 현대차 13만9000주·모비스 7만2552주 매입(3보), 정의선, '코로나19 패닉' 속 주주가치 제고…현대차·모비스 주식 매입, 정의선, 현대차·모비스 주식 190억원어치 매수…"책임경영 차원"(종합), 정의선, 현대차·모비스 190억원 규모 주식 매입 "비상시기 책임경영 차원"(종합), 정의선, 현대차·모비스 주식 사들여..책임경영 강화(상보), '책임경영' 정의선 수석부회장, 190억 규모 현대차?현대모비스 주식 매입, 정의선 '무한 책임경영' 핸들 잡고…'주가 방어운전' 시동 걸었다, 정의선 수석부회장, 현대차·모비스 주식 190억원어치 매수(종합2보), 현대차·모비스 주식 매수, 정의선 수석부회장, 190억어치, 정의선 수석부회장, 사재 털어 자사주 매입…190억 규모, 현대차 주식 매수의견 유지, “코로나19로 부진하지만 배당매력 여전”, 정의선, 현대모비스·현대차 주식 매입…지배구조 개편 적기?, 현대차그룹서 역할 커진 정의선 수석부회장, ‘책임경영’으로 답했다, "현대차는 굳건하다"…정의선 수석부회장 이하 임원진 주식매입 '책임경영', 정의선 수석부회장, 현대차·현대모비스 주식 190억원 매입, 정의선의 '책임경영' 시동, 정의선의 자신감…현대차·현대모비스 주식 190억원 매입, 정의선 수석부회장, 현대차·모비스 주식 190억원 매입···"책임경영 강화", 정의선 수석부회장 ‘책임경영’ 190억원 규모 현대차·현대모비스 주식 매입, 정의선 수석부회장, '190억 규모' 현대차·모비스 주식 매입 "책임경영 의지", 정의선, 코로나19 '책임경영'으로 돌파...자사주 190억원 규모 매입, 정의선 부회장, 190억원 규모 현대차·현대모비스 주식 매수…"책임경영 의지", 정의선 수석부회장, `책임경영`으로 코로나19 위기 돌파, 정의선, 현대차·모비스 주식 190억원 매입...'책임경영 차원'</t>
+    <t>현대·기아차 해외생산 30% 마비되자 '보폭 넓히는' 정의선, 코스피 3천포인트 간다는 말 믿고 아내 몰래 대출 받아 '주식 5억' 샀다가 깡통 된 남편, (Today 공시)칩스앤미디어, 주당 0.3주 무상증자 결정, 정의선, 190억원어치 자사주 매입, 정의선의 현대차그룹 '공포' 뚫고 하이킥 선언, '성장의 봄'을 화두로 제안, 정의선, 현대차‧모비스 주식 190억 어치 매입, 정의선의 '책임경영·자신감'···현대차·현대모비스 주식 190억 매입, 정의선, 현대차ㆍ현대모비스 주식 190억원치 매입…“책임경영ㆍ지배력 강화”, 코스피 코스닥 5%대 동반급락, 외국인과 기관 '쌍끌이 매도' 거세, 정의선, 현대車·현대모비스 주식 샀다, '코로나발 주가폭락' 증여 타이밍일까, 정의선, 현대차·모비스 주식 샀다…"주주가치 지킬 것", 삼성전자·LG전자·현대자동차 인도공장 일시 가동 중단, 정의선 수석부회장, 현대차·현대모비수 주식 매수, 정의선 현대차 부회장, 현대차·현대모비스 주식 190억원 매입..책임경영 의지 강조, 정의선, 주주가치 제고 위해 현대차·모비스 주식 매입, 배당수익률 9%를 상회하는 우선주, P/B 0.2배 중반의 Valuation과 9% 상회하는 우선주 배당수익률, 주당 배당금의 축소 가능성은 낮은 편, 여전히 양호한 신차 사이클, 코로나 극복과 함께 정상화될 주가, 연간 생산 판매 지연은 불가피하나, 코로나 완화되며 정상화될 것으로 판단한다, (코로나 제외한) 현대차 실적의 핵심은 ‘신차 출시에 따른 믹스개선’이다, 정의선 “책임경영”...현대차·모비스 자사주 190억 매입, 정의선, 190억어치 현대車·모비스株 샀다, 정의선 현대車 부회장, 책임경영 일환 현대차·모비스 주식 190억 매입, 정의선 현대차그룹 수석부회장, 현대차·현대모비스 주식 190억원어치 매수, 코스피 코스닥 6%대 급락 출발, 신풍제약 한진칼 비씨월드제약 급등, 정기선 부사장 경영 능력 도마...노조 "세습경영에 올인", 코스피 코스닥 장중 하락폭 줄어, 한진칼 금호전기 셀트리온제약 급등, 정의선, 현대차 13만9000주·모비스 7만2552주 매입(3보), 정의선, '코로나19 패닉' 속 주주가치 제고…현대차·모비스 주식 매입, 정의선, 현대차·모비스 주식 190억원어치 매수…"책임경영 차원"(종합), 정의선, 현대차·모비스 190억원 규모 주식 매입 "비상시기 책임경영 차원"(종합), 정의선, 현대차·모비스 주식 사들여..책임경영 강화(상보), '책임경영' 정의선 수석부회장, 190억 규모 현대차?현대모비스 주식 매입, 정의선 '무한 책임경영' 핸들 잡고…'주가 방어운전' 시동 걸었다, 정의선 수석부회장, 현대차·모비스 주식 190억원어치 매수(종합2보), 현대차·모비스 주식 매수, 정의선 수석부회장, 190억어치, 정의선 수석부회장, 사재 털어 자사주 매입…190억 규모, 현대차 주식 매수의견 유지, “코로나19로 부진하지만 배당매력 여전”, 정의선, 현대모비스·현대차 주식 매입…지배구조 개편 적기?, 현대차그룹서 역할 커진 정의선 수석부회장, ‘책임경영’으로 답했다, "현대차는 굳건하다"…정의선 수석부회장 이하 임원진 주식매입 '책임경영', 정의선 수석부회장, 현대차·현대모비스 주식 190억원 매입, 정의선의 '책임경영' 시동, 정의선의 자신감…현대차·현대모비스 주식 190억원 매입, 정의선 수석부회장, 현대차·모비스 주식 190억원 매입···"책임경영 강화", 정의선 수석부회장 ‘책임경영’ 190억원 규모 현대차·현대모비스 주식 매입, 정의선 수석부회장, '190억 규모' 현대차·모비스 주식 매입 "책임경영 의지", 정의선, 코로나19 '책임경영'으로 돌파...자사주 190억원 규모 매입, 정의선 부회장, 190억원 규모 현대차·현대모비스 주식 매수…"책임경영 의지", 정의선 수석부회장, `책임경영`으로 코로나19 위기 돌파, 정의선, 현대차·모비스 주식 190억원 매입...'책임경영 차원'</t>
   </si>
   <si>
     <t>재계 총수·경영진들 자사주 매입하는 까닭은?…주가보호·시세차익 일거양득, 정의선 수석부회장, 현대차·모비스주식 추가 매입...이틀간 280억 규모, 이틀연속 자사주 매입하는 현대기아차 정의선, 현대차 주가 8%대 올라 7만 원선 회복, 현대차 계열사 주가 다 상승, 정의선 수석부회장, 이틀간 현대차·모비스 주식 280억 원 매입, 정의선의 자사주 통큰 베팅…현대차·모비스 주식 이틀간 280억 쇼핑, 정의선 수석부회장, 현대차·현대모비스 주식 또 매입, 정의선·최정우·신동빈 등 책임경영 실천…자사주 매입으로 주가방어, 정의선, 현대차·모비스 주식 또 샀다, 정의선 수석부회장, 이틀째 자사주 매집 나서, 정의선 수석부회장 현대차·모비스 주식 매수...190억원 규모, 정의선 수석부회장, 이틀간 현대차·모비스 주식 280억원 매입, 정의선, 시장불안 상황서 자사주 280억원어치 매입, 현대차그룹 정의선, '경영권 강화' 자사주 취득 잰걸음, 감봉·휴직·급전·방어…대기업들, 코로나19 비상경영 돌입, 현대차 현대모비스 주가 저점, 정의선은 계속 사들일까, 정의선 수석부회장, 이틀간 현대차·모비스 주식 280억원어치 매수, 정의선, 이틀간 현대차·모비스주식 280억원 매입 "책임경영 강화", 책임경영 의지 확고한 정의선 부회장, 90억원 규모 현대차·현대모비스 주식 추가 매수, “펀더멘털 자신” 자사주 매입 나선 정의선, 정의선, 자사주 190억어치 매입… 주가폭락 막는다, 현대차 주가 끝없는 하락세... "외국인 매도공세 멈춰설때가 매수 시점", 정몽구 회장, 하락장서 주식평가손실 1조7810억원 달해, 낮은 주가가 오히려 최고의 호재, 현대차 정의선, 한국금융 김남구 등 코로나 급락장 속 과감한 주식매입 나선 경영인들, "정의선 자사주 매입, 주가 저평가·사업개선 의지 확인"-하나금융투자, 정의선, 현대차·모비스 주식매수…코로나19 위기 속 책임경영 의지, 정의선, 현대차 주식 190억원 매입 '효과봤나, 24일 반등', 포스코그룹 임원들, 회사 주식 매입…“책임 경영 의지”, 코스피 코스닥 2%대 상승 출발, 콤텍시스템 동양파일 화일약품 급등, "주주를 위해" 자기주 사들이는 재계…경영권 강화까지 노린다, 현대차·현대모비스, 오너 자사주 190억 매입에 상승, 코로나19發 재계 '자사주 쇼핑' 열풍, 재벌家 3·4세들, 요즘 시국에 주식 사들이는 ‘속내’, 정의선 현대차그룹 수석부회장, 190억 규모 자사주 매입, 정의선, 자사주 190억 어치 매입…주가폭락 방지 나서, 코로나로 폭락 '자사주 쇼핑' 열풍...'책임경영' 이유 뿐일까, 정의선 이어 최정우도 자사주 매입…재계 책임경영 강화, 정의선, ‘주가 반토막’ 현대차·모비스 자사주 190억 매입, 너무 떨어졌나…자사주 사들이는 제약사와 경영진들, 재계, 자사주 매입으로 어려움 극복…"책임경영 강화", 자사주 매입한 정의선, 190억 매입 '현대차·모비스', 정의선, 현대차·모비스 주식 또 샀다…이틀간 280억 투입, 정의선, 이틀간 현대차그룹 주식 280억 매입···"책임경영 강화", 정의선, 현대車·현대모비스 190억원어치 자사주 매입, 주가폭락 방어나선 정의선, 현대차·모비스 주식 190억어치 매입</t>
   </si>
   <si>
-    <t>현대차-펀더멘털 대비 과매도 국면, 불확실성 감안해도 과매도 국면, 1분기 Preview: 글로벌 판매 감소, 환율 변동성 확대, 정의선, 사흘간 현대차·현대모비스 주식 680억어치 집중매입, "주가 급락 막자"…코로나發 폭락장에 기업들 자사주 매입 행진(종합), 2008 금융위기땐…반년후 `대장주` 40% 올라, 정의선 수석부회장, 자사주 매입 '책임경영'...주주가치 제고 총력, 개인의 힘···2%대 강세 이어가는 코스피, 이재용·최태원·신동빈 "코로나19 잘 버텨보자"독려, 정의선, 사흘 연속 현대차·현대모비스 주식 매입, '책임 경영' 정의선, 사흘 연속 현대차·모비스 주식 매수, 현장찾고 머리맞댄 재계 총수…코로나 위기극복 총력전, 운송장비 업종 강세…정의선 현대차·모비스 자사주 매입 영향, 정의선 수석부회장, 주식 소량매입 ‘랠리’ 언제까지, 정의선 수석부회장, 사흘간 현대차·모비스 680억어치 사들여, 정의선, 현대차·현대모비스 주식 사흘 연속 매수, 정의선, 현대차·모비스 지분 추가 매입, 코스피 1700선 회복, 이틀째 급등…글로벌 부양책 기대, 사흘간 675억원 쏟아부은 정의선… 현대차·모비스 주가 올렸네, 전경련 "대기업들 각종 규제 한시적 유예 절실", 재계 총수 리더십, 코로나 위기에 빛난다, 정의선 수석부회장의 `책임 경영`… 사흘 연속 현대차·모비스 담았다, 정부의 금융시장 안정화 방안…코스피·코스닥 5% 넘게 상승 마감, 정의선 수석부회장, 사흘 연속 현대차·모비스 주식 매입, 정의선, 현대차·모비스 주식 사흘째 매입, "자사주 매입 · 신차 효과"...현대차 · 기아차, 장중 주가 '껑충', 코로나發 폭락장에…재계 총수·임원들 자사주 매입 확산, 현대차 현대모비스 주가 초반 대폭 올라, 정의선 주식 매입효과, SK, 삼성, 현대차 "코로나19 넘어서자"...위기극복 분주한 재계 총수들, "포스트 코로나 대비"...분주해진 재계 총수, 현대차·포스코 등 총수·CEO 자사주 잇단 매입, 코로나19에 재계 '자사주 매입' 열풍···정의선, 이틀새 280억원, 재계 총수들 “믿어 달라”... 자사주 매입으로 ‘극복 의지’, 현대차 주가 12%대 올라 8만 원대 회복, 현대모비스 현대위아 급등, 코스피 코스닥 3%대 상승 출발, 롯데푸드 GH신소재 동양파일 급등, 현대모비스(+9.34%) 주가 급등...이유가 뭐길래?, 코로나發 위기 속, 대규모 서울 개발사업 순항할수 있을까?, 정의선 효과? 현대차·현대모비스 강세</t>
+    <t>펀더멘털 대비 과매도 국면, 불확실성 감안해도 과매도 국면, 1분기 Preview: 글로벌 판매 감소, 환율 변동성 확대, 정의선, 사흘간 현대차·현대모비스 주식 680억어치 집중매입, "주가 급락 막자"…코로나發 폭락장에 기업들 자사주 매입 행진(종합), 2008 금융위기땐…반년후 `대장주` 40% 올라, 정의선 수석부회장, 자사주 매입 '책임경영'...주주가치 제고 총력, 개인의 힘···2%대 강세 이어가는 코스피, 이재용·최태원·신동빈 "코로나19 잘 버텨보자"독려, 정의선, 사흘 연속 현대차·현대모비스 주식 매입, '책임 경영' 정의선, 사흘 연속 현대차·모비스 주식 매수, 현장찾고 머리맞댄 재계 총수…코로나 위기극복 총력전, 운송장비 업종 강세…정의선 현대차·모비스 자사주 매입 영향, 정의선 수석부회장, 주식 소량매입 ‘랠리’ 언제까지, 정의선 수석부회장, 사흘간 현대차·모비스 680억어치 사들여, 정의선, 현대차·현대모비스 주식 사흘 연속 매수, 정의선, 현대차·모비스 지분 추가 매입, 코스피 1700선 회복, 이틀째 급등…글로벌 부양책 기대, 사흘간 675억원 쏟아부은 정의선… 현대차·모비스 주가 올렸네, 전경련 "대기업들 각종 규제 한시적 유예 절실", 재계 총수 리더십, 코로나 위기에 빛난다, 정의선 수석부회장의 `책임 경영`… 사흘 연속 현대차·모비스 담았다, 정부의 금융시장 안정화 방안…코스피·코스닥 5% 넘게 상승 마감, 정의선 수석부회장, 사흘 연속 현대차·모비스 주식 매입, 정의선, 현대차·모비스 주식 사흘째 매입, "자사주 매입 · 신차 효과"...현대차 · 기아차, 장중 주가 '껑충', 코로나發 폭락장에…재계 총수·임원들 자사주 매입 확산, 현대차 현대모비스 주가 초반 대폭 올라, 정의선 주식 매입효과, SK, 삼성, 현대차 "코로나19 넘어서자"...위기극복 분주한 재계 총수들, "포스트 코로나 대비"...분주해진 재계 총수, 현대차·포스코 등 총수·CEO 자사주 잇단 매입, 코로나19에 재계 '자사주 매입' 열풍···정의선, 이틀새 280억원, 재계 총수들 “믿어 달라”... 자사주 매입으로 ‘극복 의지’, 현대차 주가 12%대 올라 8만 원대 회복, 현대모비스 현대위아 급등, 코스피 코스닥 3%대 상승 출발, 롯데푸드 GH신소재 동양파일 급등, 현대모비스(+9.34%) 주가 급등...이유가 뭐길래?, 코로나發 위기 속, 대규모 서울 개발사업 순항할수 있을까?, 정의선 효과? 현대차·현대모비스 강세</t>
   </si>
   <si>
     <t>"주가폭락 막아라" 자사주 매입 나선 재계…정의선 817억원어치 사들여, 유례 없는 시총 증발에 '초비상'...상장사들, 주가 방어 '총력', 정의선 부회장 현대차·모비스 지분 추가 매입, “정의선 수석부회장 주식 매수, 책임 경영 의지 표명”, 정의선, 현대차·현대모비스 주식 또 샀다…5일새 817억원 투자, 코스피 코스닥 동반상승 출발, 체시스 진에어 우노앤컴퍼니 씨젠 급등, 정의선, 현대차·모비스 397억 추가 매입…사흘간 총 677억, 닻 올린 최병철 號, 당면과제는?, 삼성공조, 오너 3세 이사회 진입…후계 승계 '잰걸음', 현대차 정의선의 3가지 뚝심경영 행보, 4월초에 분수령 넘는다, 대규모 시총 증발, 주가 방어 비상깜빡이 킨 상장사, 현대자동차, 특별관계자 지분변동, 정의선, 현대차·모비스 397억원 추가 매입…사흘간 총 677억, 정의선, 현대차·모비스 주식 5일간 817억원 매수, "정의선 수석부회장 또 자사주 매입"...현대차-기아차, 장중 '연일 강세', "책임경영 일환"...자사주 매입 나선 재계, 정의선, 817억 규모 현대차·모비스 지분 매입, 정의선 수석부회장, 5일간 주식 800억원 담았다, 얼어 붙은 조달 시장···현대로템, 창사이래 첫 CB 발행, 정의선, 현대차·모비스 주식 추매 '총 800억원'..."왜", 정의선 수석부회장, 5일간 현대차·모비스 817억어치 사들여, 정의선, 817억 투입 현대차·현대모비스 주식 5일 연속 매집, 정의선, 현대차·모비스 주식 또샀다…닷새간 817억 쏟아 부어, 정의선, 닷새간 현대차·모비스 주식 817억원어치 매입, 정의선, 5일간 현대차·모비스 817억원어치 주식 매입, 정의선 부회장 '신드롬'… 현대차 주가 24.5% 폭등, 정의선, 현대차·현대모비스 주식 5일간 817억원어치 매입, 현대차 정의선, 자사주 '쇼핑 삼매경' 왜?, 정의선, 현대차·모비스 주식 5일간 817억원 매입, 정의선 현대차 현대모비스 주식 집중매입, 5거래일간 817억 규모, ‘위기가 기회’…정의선, 주가 방어하고 ICT전환 속도, "책임경영으로 위기 돌파" 정의선, 현대차·현대모비스 주식 5일간 817억원 매입</t>
@@ -5893,34 +5893,34 @@
     <t>“힘내라, 아반떼·쏘렌토·G80”…‘신차’로 코로나19 위기 돌파, '정의선 매직' 가속 페달 밟는 현대차 주가, 삼성전자 이어 국민주 예약, 정의선 수석부회장, 현대차·현대모비스 800억 매입…책임경영으로 위기 돌파, 재계 총수들, 자사주 매입하고 현장 찾고…코로나19 극복 총력전, 오너 자사주 매입 봇물...'누이 좋고 매부 좋고'</t>
   </si>
   <si>
-    <t>현대차-제네시스를 사야 할 시간, 신차 Big Cycle의 시작, 하반기 외형성장 재개에 투자하자, 제네시스 판매 급증: 환호하는 소비자, 강화된 양산능력, 동학개미운동, 코스피 코스닥 동반하락 출발, 비상교육 한진칼 경남제약 급등, 코로나19 사태 속 부동산·주식시장 '큰손' 된 30·40세대, '위기를 기회로'...주가 방어로 '두마리 토끼' 잡은 정의선, 한국 산업 지도 바꾸는 코로나19의 역설, 블룸버그 "떨어진 주식 대거 사들인 현대차 정의선 · 신세계 정유경", "韓 S&amp;P500 검색 세계 1위"...바닥은 어디일까?, 코스피 '중국 유동성 공급'에 낙폭 줄어 약보합, 코스닥은 3%대 급등</t>
-  </si>
-  <si>
-    <t>현대차-년도년도 2분기 1분기 Preview - 코로나19에 의한 타격 불가피, 투자의견 Buy 유지. 목표주가 26.7% 하향, 년도년도 2분기 1분기 영업이익 6,029억원 (-26.9% 전년 대비 증감율 예상, 기존 전망치 및 시장 컨센서스 각각 34.9%, 37.7% 하회하는 것), 2020년 영업이익 3.7조원 (+0.9% 전년 대비 증감율)전망, 이는 기존 전망치 및 시장 컨센서스 각각 22.1%, 16.2% 하회하는 것), 영업손익 전망치 조정에 비해 주가 하락은 과도, 현대차-년도년도 2분기 1분기 Preview - 코로나19에 의한 타격 불가피, 투자의견 Buy 유지. 목표주가 26.7% 하향, 년도년도 2분기 1분기 영업이익 6,029억원 (-26.9% 전년 대비 증감율 예상, 기존 전망치 및 시장 컨센서스 각각 34.9%, 37.7% 하회하는 것), 2020년 영업이익 3.7조원 (+0.9% 전년 대비 증감율)전망, 이는 기존 전망치 및 시장 컨센서스 각각 22.1%, 16.2% 하회하는 것), 영업손익 전망치 조정에 비해 주가 하락은 과도, 긴급재난지원금,소득하위70% 기준 네티즌 초미 관심, 현대차 주가 외국인 순매수로 3%대 올라, 현대로템은 15%대 급등, 코스피 코스닥 동반상승 출발, 진원생명과학 부광약품 알서포트 급등, 주주제안 119개 쏟아졌지만…통과된 안건은 3개 불과, 에스엘, 현대차와 627억 규모 배터리 매니지먼트 시스템 공급계약 체결外, ‘자사주 매입’ 정의선 부회장, 기아차 외면한 이유는, 배형근 현대모비스 부사장, 쌈짓돈 털어 주식매집 동참</t>
-  </si>
-  <si>
-    <t>1일 장 마감 후 주요 종목 뉴스, 코스피 코스닥 3%대 동반급락, 외국인과 기관 쌍끌이 매도에 밀려, 코스피 코스닥 동반상승 출발, 해태제과식품 모베이스전자 급등, 현대차-G80 글로벌 히트 예감, 90년대 일본차의 데자뷰, 제네시스 신형 G80 공개, 90년대 일본차의 데자뷰</t>
+    <t>제네시스를 사야 할 시간, 신차 Big Cycle의 시작, 하반기 외형성장 재개에 투자하자, 제네시스 판매 급증: 환호하는 소비자, 강화된 양산능력, 동학개미운동, 코스피 코스닥 동반하락 출발, 비상교육 한진칼 경남제약 급등, 코로나19 사태 속 부동산·주식시장 '큰손' 된 30·40세대, '위기를 기회로'...주가 방어로 '두마리 토끼' 잡은 정의선, 한국 산업 지도 바꾸는 코로나19의 역설, 블룸버그 "떨어진 주식 대거 사들인 현대차 정의선 · 신세계 정유경", "韓 S&amp;P500 검색 세계 1위"...바닥은 어디일까?, 코스피 '중국 유동성 공급'에 낙폭 줄어 약보합, 코스닥은 3%대 급등</t>
+  </si>
+  <si>
+    <t>년도년도 2분기 1분기 Preview - 코로나19에 의한 타격 불가피, 투자의견 Buy 유지. 목표주가 26.7% 하향, 년도년도 2분기 1분기 영업이익 6,029억원 (-26.9% 전년 대비 증감율 예상, 기존 전망치 및 시장 컨센서스 각각 34.9%, 37.7% 하회하는 것), 2020년 영업이익 3.7조원 (+0.9% 전년 대비 증감율)전망, 이는 기존 전망치 및 시장 컨센서스 각각 22.1%, 16.2% 하회하는 것), 영업손익 전망치 조정에 비해 주가 하락은 과도, 년도년도 2분기 1분기 Preview - 코로나19에 의한 타격 불가피, 투자의견 Buy 유지. 목표주가 26.7% 하향, 년도년도 2분기 1분기 영업이익 6,029억원 (-26.9% 전년 대비 증감율 예상, 기존 전망치 및 시장 컨센서스 각각 34.9%, 37.7% 하회하는 것), 2020년 영업이익 3.7조원 (+0.9% 전년 대비 증감율)전망, 이는 기존 전망치 및 시장 컨센서스 각각 22.1%, 16.2% 하회하는 것), 영업손익 전망치 조정에 비해 주가 하락은 과도, 긴급재난지원금,소득하위70% 기준 네티즌 초미 관심, 현대차 주가 외국인 순매수로 3%대 올라, 현대로템은 15%대 급등, 코스피 코스닥 동반상승 출발, 진원생명과학 부광약품 알서포트 급등, 주주제안 119개 쏟아졌지만…통과된 안건은 3개 불과, 에스엘, 현대차와 627억 규모 배터리 매니지먼트 시스템 공급계약 체결外, ‘자사주 매입’ 정의선 부회장, 기아차 외면한 이유는, 배형근 현대모비스 부사장, 쌈짓돈 털어 주식매집 동참</t>
+  </si>
+  <si>
+    <t>1일 장 마감 후 주요 종목 뉴스, 코스피 코스닥 3%대 동반급락, 외국인과 기관 쌍끌이 매도에 밀려, 코스피 코스닥 동반상승 출발, 해태제과식품 모베이스전자 급등, G80 글로벌 히트 예감, 90년대 일본차의 데자뷰, 제네시스 신형 G80 공개, 90년대 일본차의 데자뷰</t>
   </si>
   <si>
     <t>현대차 주가 외국인 매도에도 상승, 현대차 계열사 대체로 올라, 리먼 사태 닮은 증시, 지금은 과감한 결정 내릴 때, 1일 장 마감 후 주요 종목 뉴스, 삼성전자 부진에 지난해 코스피 상장사 전체 영업이익 40% 감소, 코스피 코스닥 동반 약보합 출발, 나노엔텍 레몬 엔에스쇼핑 급등</t>
   </si>
   <si>
-    <t>증권업계, 위기냐 기회냐 ‘갈림길’에 서다, 주가 연계 콜옵션 단 현대로템, CB 투심 잡을까, 현대차-제네시스 20년도 2분기 본격화, 판매 감소로 20년도 1분기 실적 컨센서스 하회 전망, 코로나바이러스로 연간 실적 역시 컨센서스 하회 전망, 5월 이후 수요 회복에 주목 필요, 코스피 코스닥 강보합 출발, 태평양물산 코오롱머티리얼 명문제약 급등</t>
+    <t>증권업계, 위기냐 기회냐 ‘갈림길’에 서다, 주가 연계 콜옵션 단 현대로템, CB 투심 잡을까, 제네시스 20년도 2분기 본격화, 판매 감소로 20년도 1분기 실적 컨센서스 하회 전망, 코로나바이러스로 연간 실적 역시 컨센서스 하회 전망, 5월 이후 수요 회복에 주목 필요, 코스피 코스닥 강보합 출발, 태평양물산 코오롱머티리얼 명문제약 급등</t>
   </si>
   <si>
     <t>강성부의 KCGI 펀드, 한진칼과 싸울 때 아냐</t>
   </si>
   <si>
-    <t>코스피 코스닥 장중 상승폭 커져, 우성사료 남선알미늄 크루셜텍 급등, 현대차-경쟁우위의 EV/자율주행 기술 역량 확보한 글로벌 OEM, COVID-19에 의한 업종 전반의 20년도 하반기 실적 부진 불가피하나, 회복기 차별화된 판매 및 실적 개선 실현 전망, 비즈니스 모델 전환기 시작 → 기존 비즈니스에서의 영업 호전과 더불어 EV ? AV 역량에 대한 재평가 기대</t>
-  </si>
-  <si>
-    <t>현대차 주식 매수의견 유지, “제네시스와 친환경차 성장 긍정적”, 외국인, 한국 증시 이탈에도 셀트리온은 샀다, 재계 코로나19 비상경영, 자사주 매입 봇물, LG상사·미래에셋대우·효성, 자사주 매입 앞세워 '高高', 코스피 '기관 매수' 힘입어 1820선 회복, 코스닥도 1%대 상승, 현대차-1분기 실적 프리뷰, 1분기 연결 매출액과 영업이익은 각각 22조 5,420억원(-6.0전년 대비 증감율), 6,540억원(-20.7%전년 대비 증감율, OPM 2.9%)을 전망함, 내수 판매 양호한 가운데 GV80, G80 등 제네시스 신차의 국내 사전 판매 실적이 기대치를 상회함, EPS 추정치 하향을 반영해 목표주가를 기존 160,000원에서 120,000원으로 25% 하향 조정함, 현대차-강력한 라인업이 있는 만큼 폭풍이 지나가길 기다리자, 20년도 1분기 매출 23,251십억원(전년 대비 증감율-3.1%), 영익 738(-10.6%) 예상, 어려운 업황이지만 어느때 보다 강력한 신차 라인업, 현대차-한국 신차효과, 중국 개선, 북미/유럽은 시장수요 급감, 부정적 산업환경을 신차 사이클로 만회, 컨콜 주요 내용: 한국 견조, 중국 회복, 기타 불확실, 유동성 관리 집중. 주주환원정책은 불변, 현대차-1분기 실적 프리뷰, 1분기 연결 매출액과 영업이익은 각각 22조 5,420억원(-6.0전년 대비 증감율), 6,540억원(-20.7%전년 대비 증감율, OPM 2.9%)을 전망함, 내수 판매 양호한 가운데 GV80, G80 등 제네시스 신차의 국내 사전 판매 실적이 기대치를 상회함, EPS 추정치 하향을 반영해 목표주가를 기존 160,000원에서 120,000원으로 25% 하향 조정함</t>
-  </si>
-  <si>
-    <t>현대차-코로나 영향을 넘어서, 20년도 1분기 Preview: 코로나19로 시장 예상치 하회. 20년도 2분기 까지 부진 전망, 코로나19 회복 시 경쟁사 대비 탄력 회복 기대, 투자의견 BUY 유지, 목표주가 추정치 변경으로 140,000원으로 하향, 코로나 사태와 ‘동학개미운동’, 電·車에 올라탔던 동학개미, 바이오·정치테마주로 '환승'</t>
-  </si>
-  <si>
-    <t>"25만원대 매수 아직도 보유 너무 힘들다"... 현대차, 기관 개인 대량 매수 눈길, "반등했지만 아직 싸다" vs "올라도 1900대가 한계", "사회를 지키자" 코로나19 악재 속 빛 발하는 총수 리더십, 현대오토에버, 오일석 대표 등 경영진 자사주 매입, 현대차-기회요인과 위기요인이 공존, 코로나 19확산 및 유가급락 영향으로 2020년 현대차 영업이익은 32% 추가 하향 조정, 선진시장 M/S 확대기회를 적극 활용해야</t>
+    <t>코스피 코스닥 장중 상승폭 커져, 우성사료 남선알미늄 크루셜텍 급등, 경쟁우위의 EV/자율주행 기술 역량 확보한 글로벌 OEM, COVID-19에 의한 업종 전반의 20년도 하반기 실적 부진 불가피하나, 회복기 차별화된 판매 및 실적 개선 실현 전망, 비즈니스 모델 전환기 시작 → 기존 비즈니스에서의 영업 호전과 더불어 EV ? AV 역량에 대한 재평가 기대</t>
+  </si>
+  <si>
+    <t>현대차 주식 매수의견 유지, “제네시스와 친환경차 성장 긍정적”, 외국인, 한국 증시 이탈에도 셀트리온은 샀다, 재계 코로나19 비상경영, 자사주 매입 봇물, LG상사·미래에셋대우·효성, 자사주 매입 앞세워 '高高', 코스피 '기관 매수' 힘입어 1820선 회복, 코스닥도 1%대 상승, 1분기 실적 프리뷰, 1분기 연결 매출액과 영업이익은 각각 22조 5,420억원(-6.0전년 대비 증감율), 6,540억원(-20.7%전년 대비 증감율, OPM 2.9%)을 전망함, 내수 판매 양호한 가운데 GV80, G80 등 제네시스 신차의 국내 사전 판매 실적이 기대치를 상회함, EPS 추정치 하향을 반영해 목표주가를 기존 160,000원에서 120,000원으로 25% 하향 조정함, 강력한 라인업이 있는 만큼 폭풍이 지나가길 기다리자, 20년도 1분기 매출 23,251십억원(전년 대비 증감율-3.1%), 영익 738(-10.6%) 예상, 어려운 업황이지만 어느때 보다 강력한 신차 라인업, 한국 신차효과, 중국 개선, 북미/유럽은 시장수요 급감, 부정적 산업환경을 신차 사이클로 만회, 컨콜 주요 내용: 한국 견조, 중국 회복, 기타 불확실, 유동성 관리 집중. 주주환원정책은 불변, 1분기 실적 프리뷰, 1분기 연결 매출액과 영업이익은 각각 22조 5,420억원(-6.0전년 대비 증감율), 6,540억원(-20.7%전년 대비 증감율, OPM 2.9%)을 전망함, 내수 판매 양호한 가운데 GV80, G80 등 제네시스 신차의 국내 사전 판매 실적이 기대치를 상회함, EPS 추정치 하향을 반영해 목표주가를 기존 160,000원에서 120,000원으로 25% 하향 조정함</t>
+  </si>
+  <si>
+    <t>코로나 영향을 넘어서, 20년도 1분기 Preview: 코로나19로 시장 예상치 하회. 20년도 2분기 까지 부진 전망, 코로나19 회복 시 경쟁사 대비 탄력 회복 기대, 투자의견 BUY 유지, 목표주가 추정치 변경으로 140,000원으로 하향, 코로나 사태와 ‘동학개미운동’, 電·車에 올라탔던 동학개미, 바이오·정치테마주로 '환승'</t>
+  </si>
+  <si>
+    <t>"25만원대 매수 아직도 보유 너무 힘들다"... 현대차, 기관 개인 대량 매수 눈길, "반등했지만 아직 싸다" vs "올라도 1900대가 한계", "사회를 지키자" 코로나19 악재 속 빛 발하는 총수 리더십, 현대오토에버, 오일석 대표 등 경영진 자사주 매입, 기회요인과 위기요인이 공존, 코로나 19확산 및 유가급락 영향으로 2020년 현대차 영업이익은 32% 추가 하향 조정, 선진시장 M/S 확대기회를 적극 활용해야</t>
   </si>
   <si>
     <t>'동학개미', 삼성전자·현대차·삼성SDI 등 쓸어 담았지만…, 안철수 국민의당 대표, 호감 이미지로 변하고 있다?, 현대모비스 목표주가 낮아져, "코로나19 자동차부품업종 전망 나빠", "체코공장 생산재개 임박"...현대차 · 기아차, 장중 주가 '연일 급등', 코스피 '개인 매수'에 1%대 올라, 코스닥은 7거래일 만에 하락, 코스피 장중 약보합 코스닥 2% 하락, 테라젠이텍스 이에스브이 급등, '책임경영+신차효과'… 현대차 주가 가속페달</t>
@@ -5929,13 +5929,13 @@
     <t>현대차 주가 급등과 `정의선 효과`</t>
   </si>
   <si>
-    <t>현대차증권, 증시 악재 속 조용한 순항 가능할까, 코오롱 ‘인보사’, 美 FDA 임상 재개 승인…회생하나?, 쫄지 말고 `숨은 진株` 싸게…역발상 투자로 기회 잡아라, 가치하락 막는다…'자사주 매입'으로 시장 방어 나서는 기업들, 역송금 수요에 한때 두자릿수 급등…9.70원↑, 코로나에도 28곳 주가 2배 이상 증가…셀트리온 서정진, 주식재산 1조↑ 등, 권영수 LG그룹 부회장, 화훼농가 위해 릴레이 캠페인 참여 外, 자사주 통 크게 사들이는 기업들…주가 약발 받을까, 현대차-20년도 1분기 Preview: 다음 분기가 더 걱정되지만, 1분기 연결 매출액 23.2조원(전년 대비 증감율 -3.3%), 영업이익 6,535억원(전년 대비 증감율 -21%) 전망, 목표주가를 2020E PBR 0.5x 적용한 14만원으로 하향</t>
-  </si>
-  <si>
-    <t>현대차-운용의 묘가 중요해지는 시점, 20년도 1분기 Preview - 믹스개선에도 피해갈 수 없는 부진한 업황, 운용의 묘가 중요해지는 시점, SKT, 간편결제로 요금 자동납부 확대 등, 코스피 '기관 매수' 코스닥 '외국인 개인 매수' 힘입어 나란히 반등, 코로나19로 생긴 '동학개미운동' 주식 모아 되찾는 주권, 코스피 코스닥 동반상승 출발, 코오롱머티리얼 두산퓨얼셀 코센 급등</t>
-  </si>
-  <si>
-    <t>현대모비스, 현대차 의존…실적 회복 가능성은, 현대차-상품성 개선을 믿고 참는 구간, 1Q 실적 Preview: 예상된 부진, 2Q에도 해외 發 실적 부진 예상, Covid19 확산 완화 시 하반기 이익 모멘텀 발생 기대, 투자의견 Buy, 목표주가 120,000원 제시, 반등場서 2조 쏜 연기금은 뭘 담았지?, 현대차그룹株, '정의선 효과'로 반등…현대·기아차 돌파구는, '코로나19' 한국 경제 여진 지속…기업들 실탄확보·주주친화 정책 가속화, 코스피 코스닥 동반하락 출발, 세우글로벌 코오롱 아이즈비전 급등</t>
+    <t>현대차증권, 증시 악재 속 조용한 순항 가능할까, 코오롱 ‘인보사’, 美 FDA 임상 재개 승인…회생하나?, 쫄지 말고 `숨은 진株` 싸게…역발상 투자로 기회 잡아라, 가치하락 막는다…'자사주 매입'으로 시장 방어 나서는 기업들, 역송금 수요에 한때 두자릿수 급등…9.70원↑, 코로나에도 28곳 주가 2배 이상 증가…셀트리온 서정진, 주식재산 1조↑ 등, 권영수 LG그룹 부회장, 화훼농가 위해 릴레이 캠페인 참여 外, 자사주 통 크게 사들이는 기업들…주가 약발 받을까, 20년도 1분기 Preview: 다음 분기가 더 걱정되지만, 1분기 연결 매출액 23.2조원(전년 대비 증감율 -3.3%), 영업이익 6,535억원(전년 대비 증감율 -21%) 전망, 목표주가를 2020E PBR 0.5x 적용한 14만원으로 하향</t>
+  </si>
+  <si>
+    <t>운용의 묘가 중요해지는 시점, 20년도 1분기 Preview - 믹스개선에도 피해갈 수 없는 부진한 업황, 운용의 묘가 중요해지는 시점, SKT, 간편결제로 요금 자동납부 확대 등, 코스피 '기관 매수' 코스닥 '외국인 개인 매수' 힘입어 나란히 반등, 코로나19로 생긴 '동학개미운동' 주식 모아 되찾는 주권, 코스피 코스닥 동반상승 출발, 코오롱머티리얼 두산퓨얼셀 코센 급등</t>
+  </si>
+  <si>
+    <t>현대모비스, 현대차 의존…실적 회복 가능성은, 상품성 개선을 믿고 참는 구간, 1Q 실적 Preview: 예상된 부진, 2Q에도 해외 發 실적 부진 예상, Covid19 확산 완화 시 하반기 이익 모멘텀 발생 기대, 투자의견 Buy, 목표주가 120,000원 제시, 반등場서 2조 쏜 연기금은 뭘 담았지?, 현대차그룹株, '정의선 효과'로 반등…현대·기아차 돌파구는, '코로나19' 한국 경제 여진 지속…기업들 실탄확보·주주친화 정책 가속화, 코스피 코스닥 동반하락 출발, 세우글로벌 코오롱 아이즈비전 급등</t>
   </si>
   <si>
     <t>위기 땐 '재무통'… 현대차·포스코·CJ·한화 CFO들 전면에, 코스피 코스닥 동반상승 출발, 대우부품 스맥 아이에이네트웍스 급등, 증권사 테마, 미래에셋대우 +4.94%, 한화투자증권 +4.23%, 코스피 ‘외국인 매수’로 3%대 급등해 1900선 회복, 코스닥도 상승, 총선에 따라 움직이는 증시...'진단키트'에서 '경협·와이파이'로, 코스피 코스닥 장중 상승폭 커져, 대우부품 시디즈 에코바이오 급등, 현대차그룹, 코로나 극복과 미래 성장을 위해 최선을 다하는 기업, 1,220원 하향 이탈 후 中 지표 확인…9.70원↓, 외국인 배당 오늘만 '3.2조'…서울환시서 역송금 압박 완화할까, 현대차 노사 위기극복 '어깨동무'… 주가방어-유연근무 合心, 연기금, 어떤 종목에 관심..."선거든 코로나든 연기금 투자원칙 못 벗어나"</t>
@@ -5944,19 +5944,19 @@
     <t>현대차그룹 이사회 의장 한 달 맞은 정의선…‘사람 중심 미래’ 박차</t>
   </si>
   <si>
-    <t>코스피 코스닥 동반상승 출발, 대웅제약 네이처셀 휴젤 에넥스 급등, &lt;오후여담&gt;임자 만난 행동주의 펀드, 코스피 코스닥 장중 동반상승 유지, 파미셀 현대로템 대아티아이 급등, 현대차-해외 일부 재가동 시작, 한국은 상대적으로 양호, 1분기 글로벌 산업수요는 24% 감소했고, 현대차의 도매/소매 판매는 13%/18% 감소, 매수의견을 유지하며 목표주가는 기존 180,000원에서 130,000원으로 하향</t>
-  </si>
-  <si>
-    <t>코로나로 몸값도 '뚝'···건설사 IPO 연기 속출, 현대차-외국인 비중 10년내 최저치, Why?, 현대차에 집중된 외국인 매도, 자동차업종, 내수주가 아니다, 20년도 하반기 에 금융법인 손실 리스크 점검, 항공 이어 자동차까지…현대車 임원 급여 20% 반납, 코스피 코스닥 동반하락 출발, 남광토건 삼호개발 이화공영 급등</t>
+    <t>코스피 코스닥 동반상승 출발, 대웅제약 네이처셀 휴젤 에넥스 급등, &lt;오후여담&gt;임자 만난 행동주의 펀드, 코스피 코스닥 장중 동반상승 유지, 파미셀 현대로템 대아티아이 급등, 해외 일부 재가동 시작, 한국은 상대적으로 양호, 1분기 글로벌 산업수요는 24% 감소했고, 현대차의 도매/소매 판매는 13%/18% 감소, 매수의견을 유지하며 목표주가는 기존 180,000원에서 130,000원으로 하향</t>
+  </si>
+  <si>
+    <t>코로나로 몸값도 '뚝'···건설사 IPO 연기 속출, 외국인 비중 10년내 최저치, Why?, 현대차에 집중된 외국인 매도, 자동차업종, 내수주가 아니다, 20년도 하반기 에 금융법인 손실 리스크 점검, 항공 이어 자동차까지…현대車 임원 급여 20% 반납, 코스피 코스닥 동반하락 출발, 남광토건 삼호개발 이화공영 급등</t>
   </si>
   <si>
     <t>(Today 공시)아시아나항공, 단기차입금 4조원대까지 늘려, 코스피 코스닥 동반하락 출발, 한진중공업 아시아나항공 오스템 급등</t>
   </si>
   <si>
-    <t>현대차-20년도 1분기 Review: 유동성, 유동성, 유동성, 판매감소를 상쇄한 믹스: 1분기 영업이익은 8,638억원. 믹스향상 및 원화약세가 물량감소를 상쇄, 년도년도 2분기 2분기 불확실성과 유동성 확보에 집중: 코로나19로 수요급감 영향은 년도년도 2분기 2분기 에 집중, 현대차-확인된 믹스개선과 원가절감 효과, 20년도 1분기 Review-믹스개선을 확인한 1분기, 낙관하기 어려운 업황이나 과도한 우려도 금물, 코스피 '기관 매수'에 1900선 회복, 코스닥도 2거래일째 올라, 코스피, 경기둔화 우려에도 상승 마감…연기금 매수에 1910선 회복, 코스피 코스닥 동반상승 출발, 데이타솔루션 소프트센 제이웨이 급등, 유리자산운용, 호텔신라에 자사주 활용 방안 물어본 이유, “폭락장서 자사주매입 효과 있네”…매입공시 코스닥사 95% ‘주가 급등’, "집중 투표제 의무화하면..." 투기자본 앞에 경영권 '무장해제', 4월 22일 주요 한인사회 소식</t>
-  </si>
-  <si>
-    <t>현대차-더 험난한 년도년도 2분기 2분기 , 내수가망,년도 분기 1Q20, 일회성 제외해도 in line, 험난한 년도년도 2분기 2분기 , 내수가망,년도 분기 바닥을 지나는 중, 현대차-우려 대비 양호했던 실적, 20년도 1분기 영업이익 8,640억원(전년 대비 증감율 +4.7%) 기록, 예상을 상회. 믹스 개선과 우호적 환율 효과 유효한 가운데, 일회성 이익도 발생, 금번 양호한 실적에 힘을 보탰던 북미 판매도 2Q부터 큰 폭으로 감소할 전망이고, 3월 중순 이후 고원가율 생산분의 수익비용 인식이 본격화되면서 2Q 실적은 크게 부진할 전망, 실적 불확실성이 높아져 있으나, 유럽, 미국 순으로 산업수요 회복세가 시작된다면 상승여력 부각될 전망. 현재 주가는 PBR 0.34x로, 회복을 가정하고 있는 2021년 이후의 정상 ROE 6% 대비 저평가 영역에 있음. 목표가 14만원(PBR 0.5x), 매수의견 유지, 현대차-어려운 업황에도 선방 중, 1분기 영업이익 8,638억원 (+4.7%) 으로 선방, 2분기 관건은 수출 회복 시점, 현대차-생각할수록 아깝다, OP 컨센서스 21% 상회, 판매부진이 우호적 환율과 믹스개선을 상쇄, 단 일회성 이익 제거 시 컨센서스 상회 폭은 6%로 축소, 코로나19 없었다면 역대급 신차 싸이클 가능했을 전망. 2분기 부진에 주목, 현대차-우려는 과도했으나 바깥은 여전히 안개 속, 20년도 1분기 Review: 우려가 과도했다, 2분기, 생존을 위한 조건, 투자의견 매수 유지, 목표주가 130,000원으로 하향, 현대차-판가 상승으로 잘 이겨낸 20년도 1분기 , 판매 감소에도 불구하고 매출 성장은 고무적 요인, 차량사업 매출 19,555십억원(전년 대비 증감율+5.1%), 일회성 제외 OP 464십억원(전년 대비 증감율-8.5%), 20년도 2분기 수요 둔화, 수익성 악화 예상. 그러나 이후 회복을 이끌어줄 신차 라인업 기대, 현대차-년도년도 2분기 1분기 Review: 빛 바랜 실적, 2분기가 고비, 년도년도 2분기 1분기 Review: 빛 바랜 실적, 3월 과잉 출고, 2분기 판매에 부정적, 이머징 리스크 우려, 비우호적인 대외변수 강화, 현대차-이미 지난 미래, 년도년도 2분기 2분기 , COVID-19 영향을 넘어선 신차과,년도 분기 1Q20 매출 서프라이즈, 모두가 알고 있는 년도년도 2분기 2분기 어닝쇼크는 이미 지난 미래, 현대차-2분기에 최악의 상황을 지날 것, 하반기 글로벌 생산/판매 점진적 회복 기대, 1분기 Review: 환율, 제품믹스 개선, 재고 실현효과, 현대차-년도년도 2분기 1분기 실적 Review: 예상보다 무난, 년도년도 2분기 1분기 실적 Review, 년도년도 2분기 2분기 실적 하향 압력 커질 것으로 예상, 투자의견 `Buy`, 목표주가 120,000원 유지, 현대차-2분기 저점 지나 하반기 회복 전망, 20년도 1분기 영업이익은 8,638억원(+4.7% 전년 대비 증감율, OPM 3.4%) 기록, 컨센서스 20.9% 상회, 20년도 2분기 각 국 이동제한 및 가동중단 영향으로 부진한 실적 기록할 전망, 현대차-코로나에 가려진 믹스개선 효과, 20년도 1분기 Review: 일회성 이익으로 컨센서스 상회, 코로나에 가려진 믹스개선 효과, 현대차-믹스 개선과 환율로 1분기 방어. 2분기 이후 코로나 영향 본격화, 2분기 부진은 상당부분 알려진 상태, 20년도 1분기 Review: 영업이익률 3.4% 기록, 컨퍼런스 콜의 주요 내용: 보수적 경영 방침을 재확인, 현대차-믹스로 1분기 방어, 2분기는 코로나 한가운데, 1분기 영업이익 컨센서스 소폭 상회, 투자의견 매수, 목표주가 130,000원, 현대차-우려는 과도했으나 바깥은 여전히 안개 속, 20년도 1분기 Review: 우려가 과도했다, 2분기, 생존을 위한 조건, 투자의견 매수 유지, 목표주가 130,000원으로 하향, 현대차-생각할수록 아깝다, OP 컨센서스 21% 상회, 판매부진이 우호적 환율과 믹스개선을 상쇄, 단 일회성 이익 제거 시 컨센서스 상회 폭은 6%로 축소, 코로나19 없었다면 역대급 신차 싸이클 가능했을 전망. 2분기 부진에 주목, 현대차 주식 매수의견 유지, "코로나19 위기에도 실적 선방 중", 정의선의 절묘한 신의 한수…현대차·모비스 자사주 사들이기, 대북 테마주 올라탄 현대로템 주가…CB 투심에는 '양날의 검', 코스피 코스닥 동반하락 출발, 대웅 모나리자 스페코 알서포트 급등, "현대차, 코로나에도 실적 '선방'...2분기 지켜봐야"...증권계</t>
+    <t>20년도 1분기 Review: 유동성, 유동성, 유동성, 판매감소를 상쇄한 믹스: 1분기 영업이익은 8,638억원. 믹스향상 및 원화약세가 물량감소를 상쇄, 년도년도 2분기 2분기 불확실성과 유동성 확보에 집중: 코로나19로 수요급감 영향은 년도년도 2분기 2분기 에 집중, 확인된 믹스개선과 원가절감 효과, 20년도 1분기 Review-믹스개선을 확인한 1분기, 낙관하기 어려운 업황이나 과도한 우려도 금물, 코스피 '기관 매수'에 1900선 회복, 코스닥도 2거래일째 올라, 코스피, 경기둔화 우려에도 상승 마감…연기금 매수에 1910선 회복, 코스피 코스닥 동반상승 출발, 데이타솔루션 소프트센 제이웨이 급등, 유리자산운용, 호텔신라에 자사주 활용 방안 물어본 이유, “폭락장서 자사주매입 효과 있네”…매입공시 코스닥사 95% ‘주가 급등’, "집중 투표제 의무화하면..." 투기자본 앞에 경영권 '무장해제', 4월 22일 주요 한인사회 소식</t>
+  </si>
+  <si>
+    <t>더 험난한 년도년도 2분기 2분기 , 내수가망,년도 분기 1Q20, 일회성 제외해도 in line, 험난한 년도년도 2분기 2분기 , 내수가망,년도 분기 바닥을 지나는 중, 우려 대비 양호했던 실적, 20년도 1분기 영업이익 8,640억원(전년 대비 증감율 +4.7%) 기록, 예상을 상회. 믹스 개선과 우호적 환율 효과 유효한 가운데, 일회성 이익도 발생, 금번 양호한 실적에 힘을 보탰던 북미 판매도 2Q부터 큰 폭으로 감소할 전망이고, 3월 중순 이후 고원가율 생산분의 수익비용 인식이 본격화되면서 2Q 실적은 크게 부진할 전망, 실적 불확실성이 높아져 있으나, 유럽, 미국 순으로 산업수요 회복세가 시작된다면 상승여력 부각될 전망. 현재 주가는 PBR 0.34x로, 회복을 가정하고 있는 2021년 이후의 정상 ROE 6% 대비 저평가 영역에 있음. 목표가 14만원(PBR 0.5x), 매수의견 유지, 어려운 업황에도 선방 중, 1분기 영업이익 8,638억원 (+4.7%) 으로 선방, 2분기 관건은 수출 회복 시점, 생각할수록 아깝다, OP 컨센서스 21% 상회, 판매부진이 우호적 환율과 믹스개선을 상쇄, 단 일회성 이익 제거 시 컨센서스 상회 폭은 6%로 축소, 코로나19 없었다면 역대급 신차 싸이클 가능했을 전망. 2분기 부진에 주목, 우려는 과도했으나 바깥은 여전히 안개 속, 20년도 1분기 Review: 우려가 과도했다, 2분기, 생존을 위한 조건, 투자의견 매수 유지, 목표주가 130,000원으로 하향, 판가 상승으로 잘 이겨낸 20년도 1분기 , 판매 감소에도 불구하고 매출 성장은 고무적 요인, 차량사업 매출 19,555십억원(전년 대비 증감율+5.1%), 일회성 제외 OP 464십억원(전년 대비 증감율-8.5%), 20년도 2분기 수요 둔화, 수익성 악화 예상. 그러나 이후 회복을 이끌어줄 신차 라인업 기대, 년도년도 2분기 1분기 Review: 빛 바랜 실적, 2분기가 고비, 년도년도 2분기 1분기 Review: 빛 바랜 실적, 3월 과잉 출고, 2분기 판매에 부정적, 이머징 리스크 우려, 비우호적인 대외변수 강화, 이미 지난 미래, 년도년도 2분기 2분기 , COVID-19 영향을 넘어선 신차과,년도 분기 1Q20 매출 서프라이즈, 모두가 알고 있는 년도년도 2분기 2분기 어닝쇼크는 이미 지난 미래, 2분기에 최악의 상황을 지날 것, 하반기 글로벌 생산/판매 점진적 회복 기대, 1분기 Review: 환율, 제품믹스 개선, 재고 실현효과, 년도년도 2분기 1분기 실적 Review: 예상보다 무난, 년도년도 2분기 1분기 실적 Review, 년도년도 2분기 2분기 실적 하향 압력 커질 것으로 예상, 투자의견 `Buy`, 목표주가 120,000원 유지, 2분기 저점 지나 하반기 회복 전망, 20년도 1분기 영업이익은 8,638억원(+4.7% 전년 대비 증감율, OPM 3.4%) 기록, 컨센서스 20.9% 상회, 20년도 2분기 각 국 이동제한 및 가동중단 영향으로 부진한 실적 기록할 전망, 코로나에 가려진 믹스개선 효과, 20년도 1분기 Review: 일회성 이익으로 컨센서스 상회, 코로나에 가려진 믹스개선 효과, 믹스 개선과 환율로 1분기 방어. 2분기 이후 코로나 영향 본격화, 2분기 부진은 상당부분 알려진 상태, 20년도 1분기 Review: 영업이익률 3.4% 기록, 컨퍼런스 콜의 주요 내용: 보수적 경영 방침을 재확인, 믹스로 1분기 방어, 2분기는 코로나 한가운데, 1분기 영업이익 컨센서스 소폭 상회, 투자의견 매수, 목표주가 130,000원, 우려는 과도했으나 바깥은 여전히 안개 속, 20년도 1분기 Review: 우려가 과도했다, 2분기, 생존을 위한 조건, 투자의견 매수 유지, 목표주가 130,000원으로 하향, 생각할수록 아깝다, OP 컨센서스 21% 상회, 판매부진이 우호적 환율과 믹스개선을 상쇄, 단 일회성 이익 제거 시 컨센서스 상회 폭은 6%로 축소, 코로나19 없었다면 역대급 신차 싸이클 가능했을 전망. 2분기 부진에 주목, 현대차 주식 매수의견 유지, "코로나19 위기에도 실적 선방 중", 정의선의 절묘한 신의 한수…현대차·모비스 자사주 사들이기, 대북 테마주 올라탄 현대로템 주가…CB 투심에는 '양날의 검', 코스피 코스닥 동반하락 출발, 대웅 모나리자 스페코 알서포트 급등, "현대차, 코로나에도 실적 '선방'...2분기 지켜봐야"...증권계</t>
   </si>
   <si>
     <t>코스피 1%대 코스닥 2%대 올라, 외국인과 기관 쌍끌이 매수, 코스피 코스닥 장중 상승폭 커져, 제주은행 골프존 W홀딩컴퍼니 급등, 정몽규 HDC그룹 회장, 증권사 테마, 미래에셋대우 +4.27%, 유진투자증권 +4.23%, 블록딜 주가에 악영향만 끼칠까요</t>
@@ -5992,13 +5992,13 @@
     <t>코스피 1940선 회복, 사흘만에 기지개, 코로나 시대, 동학개미는 새로운 유형의 투자자일까, 코스피, 연기금 등판에 사흘 만에 상승…2차전지株 '강세', 코로나 폭락장에 자사주 매입…정의선 시세차익만 230억, 코스피 코스닥 동반하락 출발, 대양금속 국동 키이스트 급등, "현대건설 주가 상승 가능", 사회간접자본사업과 자체사업 활발해, 정의선의 817억 자사주 쇼핑…한 달 만에 230억 차익, ③코로나 전쟁통에 혜성처럼 나타난 개미군단, 이종우 “정부와 대기업, 성장기업을 키워라”</t>
   </si>
   <si>
-    <t>현대차-e-GMP를 기반으로 전기차의 상품성 개선, 전기차 부문의 성장은 주가 재평가의 계기, 2021년부터 e-GMP 기반의 전용 모델을 투입, 2025년까지 연평균 27% 성장 예상, "한온시스템 주가 오를 힘 다져", 전기차시장 성장에 따른 수혜, "현대차 주가 상승 전망", 전기차 전용 플랫폼 내년 본격 가동, 코스피 코스닥 동반하락 출발, 신풍제약 유니온 삼진엘앤디 급등</t>
-  </si>
-  <si>
-    <t>현대차-제네시스와 전기차 두마리 토끼 모두 잡는다, 단기적인 업황은 어려울 수 밖에 없다, 단기적인 시각보다는 긴호흡으로 여정을 시작할 때, E-GMP, 이제 양산은 코앞에 두고 있다, 투자의견 Buy, 목표주가 110,000 원 유지, 자동차 업종 Top Pick, 현대차-돋보이는 Global Footprint, 코로나19 영향으로 글로벌 자동차 OEM의 가동률 급감한 가운데, 생산 의존도 높고 주력 시장인 한국에서의 회복세는 경쟁사 대비 변별 요인, 안정적인 생산/판매 포트폴리오를 통해 2020년 코로나19 영향에도 시장 수요 감소보다 상대적인 손실 회피가 뛰어나고(중국 외 현대 -14.8% vs. 평균 -16.4%), 2019년~2021년 상대적인 회복 강도 또한 탄력적일 것(중국 외 현대 -4.0% vs. 평균 -6.1%)으로 추정, 2020년 기준 지역별 공급/수요 회복 탄력도 추정에서도 시장대비 월 평균 1.3%p 공급 정상화 가능해 도요타 -0.9%p, VW -0.2%p 및 시장대비 탄력적인 가동 정상화 기대, '코로나 공황' 이후 상생협력 이렇게 하라, 수혜 기업마저… 맥 못 추는 저유가 테마주들, '원격의료'서 '비대면 진료'로 톤다운...협상여지 열어둔 靑 外</t>
-  </si>
-  <si>
-    <t>현대차-실적 추이 및 전망, 현대차, 2분기 영업이익 1,090억원 전망, 중장기 경쟁력에 주목, 투자의견 매수 유지, 현대차그룹주 급등, 현대위아 14%대 현대글로비스 11%대 상승</t>
+    <t>e-GMP를 기반으로 전기차의 상품성 개선, 전기차 부문의 성장은 주가 재평가의 계기, 2021년부터 e-GMP 기반의 전용 모델을 투입, 2025년까지 연평균 27% 성장 예상, "한온시스템 주가 오를 힘 다져", 전기차시장 성장에 따른 수혜, "현대차 주가 상승 전망", 전기차 전용 플랫폼 내년 본격 가동, 코스피 코스닥 동반하락 출발, 신풍제약 유니온 삼진엘앤디 급등</t>
+  </si>
+  <si>
+    <t>제네시스와 전기차 두마리 토끼 모두 잡는다, 단기적인 업황은 어려울 수 밖에 없다, 단기적인 시각보다는 긴호흡으로 여정을 시작할 때, E-GMP, 이제 양산은 코앞에 두고 있다, 투자의견 Buy, 목표주가 110,000 원 유지, 자동차 업종 Top Pick, 돋보이는 Global Footprint, 코로나19 영향으로 글로벌 자동차 OEM의 가동률 급감한 가운데, 생산 의존도 높고 주력 시장인 한국에서의 회복세는 경쟁사 대비 변별 요인, 안정적인 생산/판매 포트폴리오를 통해 2020년 코로나19 영향에도 시장 수요 감소보다 상대적인 손실 회피가 뛰어나고(중국 외 현대 -14.8% vs. 평균 -16.4%), 2019년~2021년 상대적인 회복 강도 또한 탄력적일 것(중국 외 현대 -4.0% vs. 평균 -6.1%)으로 추정, 2020년 기준 지역별 공급/수요 회복 탄력도 추정에서도 시장대비 월 평균 1.3%p 공급 정상화 가능해 도요타 -0.9%p, VW -0.2%p 및 시장대비 탄력적인 가동 정상화 기대, '코로나 공황' 이후 상생협력 이렇게 하라, 수혜 기업마저… 맥 못 추는 저유가 테마주들, '원격의료'서 '비대면 진료'로 톤다운...협상여지 열어둔 靑 外</t>
+  </si>
+  <si>
+    <t>실적 추이 및 전망, 현대차, 2분기 영업이익 1,090억원 전망, 중장기 경쟁력에 주목, 투자의견 매수 유지, 현대차그룹주 급등, 현대위아 14%대 현대글로비스 11%대 상승</t>
   </si>
   <si>
     <t>주식시장 4개 종목 상한가... 초록뱀·디피씨·파미셀에 몰리는 기대감, 오늘 가장 HOT한 종목은 무엇?, 20일 장 마감 후 주요 종목 뉴스</t>
@@ -6007,7 +6007,7 @@
     <t>20일 장 마감 후 주요 종목 뉴스, 미국식도 스웨덴식도 아닌, 새로운 기업지배구조를 모색할 때, 공인인증서 폐지 전망에 들썩이는 전자서명주</t>
   </si>
   <si>
-    <t>코스피 2000선 터치... 저평가 주식 찾는 방법, 현대차-짧은 상처, 긴 영광, 1Q Comment, 2Q Preview, 투자의견 BUY, 목표주가 12만원 제시</t>
+    <t>코스피 2000선 터치... 저평가 주식 찾는 방법, 짧은 상처, 긴 영광, 1Q Comment, 2Q Preview, 투자의견 BUY, 목표주가 12만원 제시</t>
   </si>
   <si>
     <t>현대차 제친 '카카오' 시총…언택트 업고 고공행진</t>
@@ -6019,13 +6019,13 @@
     <t>정의선, 자사주 매입 책임투자 소기 성과, KCC 수요예측서 흥행 참패...주채무계열 편입 소식에 주가 하락, “우선순위, 고용보다 산업 전환…화석연료 미련 버려야”, 네이버·카카오 몸값 '고공행진'…산업구조 개편 빨라지나, 현대차 주식 매수의견 유지, "안정적 재무구조로 수요 회복 때 강점"</t>
   </si>
   <si>
-    <t>현대차-정점을 지난 COVID-19, 회복을 시작할 기업가치, 단기 기업가치 방향성, COVID-19 관련 잡음이 아닌 수요회복의 신호에 더 강하게 반응할 전망, 위기 상황에서의 점유율 차별화 → 위기 국면 해제 이후 가장 높은 판매 및 실적 회복탄력으로 연결, 이동 수단에서 서비스 플랫폼으로의 전환기를 맞이한 자동차, 고도화된 BEV 제조업체 기업가치 부각 예정, 코로나19 이후 준비로 바빠진 5대 그룹 총수 행보 | 이재용·정의선 배터리 협력 합의 눈길, 최태원·신동빈은 화상회의 소통 강화, 현대차 시가총액 앞지른 카카오 '언택트', 지금 투자해도 되나, 코로나 이후 30대 재벌가 오너 지분 가치 변화 공개, 시총 8배 불어난 카카오…증권가도 장밋빛 전망, 코로나 넘어선 슈퍼여당 반기업쇼크에 국민밥솥 위태롭다, 한투증권, 매출·손익마저 오락가락 사업보고서…번복 잦아 투자자 신뢰 추락, 이재용 삼성전자 부회장의 대국민 사과와 文정부의 딜레마</t>
-  </si>
-  <si>
-    <t>현대차-멋진 제네시스, 그런데 주가는 왜?, 국내외 제네시스에 대한 호평으로, 럭셔리 세그먼트의 성공에 대한 기대감이 높아지고 있음. 실제 한국시장에서는 대기수요가 3~5달로 판매 호조, 그럼에도 외국인 지분율은 10년 내 최저치를 기록, 주가도 부진. 이는 신흥시장을 중심으로 내연기관차 수요위축 및 산업재편으로 인한 비용증가에 대한 우려가 원인., 8월 이후 미국시장에서 제네시스 성공을 통한 질적 성장과 2021년 초 E-GMP기반의 NE전기차 성공이 주가회복의 Key. 목표주가 산정기준을 2020년 수익추정 기반에서 2020년~2021년 평균으로 이동, Target Valuation도 주식시장 정상화를 반영하여 코로나19 이전으로 회귀하여 125,000원으로 19%상향, 오너 자사주 매입 상장사, 주가 반등 더 빛났다</t>
-  </si>
-  <si>
-    <t>외인 지분율 금융위기 이후 최저로 떨어진 현대차…지금이 매수기회?, 현대차-하반기 제네시스 효과 본격화, 20년도 2분기 해외 공장 가동률이 문제, 하반기 제네시스 효과 본격화, 굳건한 내수, 그리고 EV 경쟁력, 다음소프트, 공모 전량 신주로…기업가치 2000억 이상, '포스트 코로나' 한국의 중심이 되다, 현대차 주식 매수의견 유지, "해외 부진을 내수에서 제네시스로 만회", 구속 갈림길에 선 이재용 삼성 부회장...“경영공백 우려” vs “의혹 정점”, 외국인 지분 2008년 이후 최저…현대차 지금이 저가매수 기회?, 日 '엘리엇 방지법' 도입…외국자본이 지분 1%만 사도 정부 승인 받아야</t>
+    <t>정점을 지난 COVID-19, 회복을 시작할 기업가치, 단기 기업가치 방향성, COVID-19 관련 잡음이 아닌 수요회복의 신호에 더 강하게 반응할 전망, 위기 상황에서의 점유율 차별화 → 위기 국면 해제 이후 가장 높은 판매 및 실적 회복탄력으로 연결, 이동 수단에서 서비스 플랫폼으로의 전환기를 맞이한 자동차, 고도화된 BEV 제조업체 기업가치 부각 예정, 코로나19 이후 준비로 바빠진 5대 그룹 총수 행보 | 이재용·정의선 배터리 협력 합의 눈길, 최태원·신동빈은 화상회의 소통 강화, 현대차 시가총액 앞지른 카카오 '언택트', 지금 투자해도 되나, 코로나 이후 30대 재벌가 오너 지분 가치 변화 공개, 시총 8배 불어난 카카오…증권가도 장밋빛 전망, 코로나 넘어선 슈퍼여당 반기업쇼크에 국민밥솥 위태롭다, 한투증권, 매출·손익마저 오락가락 사업보고서…번복 잦아 투자자 신뢰 추락, 이재용 삼성전자 부회장의 대국민 사과와 文정부의 딜레마</t>
+  </si>
+  <si>
+    <t>멋진 제네시스, 그런데 주가는 왜?, 국내외 제네시스에 대한 호평으로, 럭셔리 세그먼트의 성공에 대한 기대감이 높아지고 있음. 실제 한국시장에서는 대기수요가 3~5달로 판매 호조, 그럼에도 외국인 지분율은 10년 내 최저치를 기록, 주가도 부진. 이는 신흥시장을 중심으로 내연기관차 수요위축 및 산업재편으로 인한 비용증가에 대한 우려가 원인., 8월 이후 미국시장에서 제네시스 성공을 통한 질적 성장과 2021년 초 E-GMP기반의 NE전기차 성공이 주가회복의 Key. 목표주가 산정기준을 2020년 수익추정 기반에서 2020년~2021년 평균으로 이동, Target Valuation도 주식시장 정상화를 반영하여 코로나19 이전으로 회귀하여 125,000원으로 19%상향, 오너 자사주 매입 상장사, 주가 반등 더 빛났다</t>
+  </si>
+  <si>
+    <t>외인 지분율 금융위기 이후 최저로 떨어진 현대차…지금이 매수기회?, 하반기 제네시스 효과 본격화, 20년도 2분기 해외 공장 가동률이 문제, 하반기 제네시스 효과 본격화, 굳건한 내수, 그리고 EV 경쟁력, 다음소프트, 공모 전량 신주로…기업가치 2000억 이상, '포스트 코로나' 한국의 중심이 되다, 현대차 주식 매수의견 유지, "해외 부진을 내수에서 제네시스로 만회", 구속 갈림길에 선 이재용 삼성 부회장...“경영공백 우려” vs “의혹 정점”, 외국인 지분 2008년 이후 최저…현대차 지금이 저가매수 기회?, 日 '엘리엇 방지법' 도입…외국자본이 지분 1%만 사도 정부 승인 받아야</t>
   </si>
   <si>
     <t>김기문 중소기업중앙회 회장</t>
@@ -6049,13 +6049,13 @@
     <t>코스피 코스닥 장중 동반하락, 신성통상 피씨디렉트 이녹스 급등, 코스피 코스닥 다 상승 출발, 현대비앤지스틸 동국제강 네온테크 급등, 주주 권익 지표 개선한 현대기아차…꾸준한 '주주 친화 경영' 결과물, 檢영장청구, 이재용 시민판단 호소 '무력화'…삼성 경제위기 극복도 '무력감', KB·하나금융 보험업 추가…포트폴리오 '완성' 이면에 우려도, 증권사 테마, 미래에셋대우 +4.03%, 교보증권 +3.32%</t>
   </si>
   <si>
-    <t>현대차-제네시스 Time: 거대한 포텐셜의 현실화 시작, 제네시스 판매 증가속도, 예상보다 빠르다: 연간판매량 17.5만대로 상향, G80 月1만대 시대 도래, 20년도 4분기 제네시스 총 7.3만대 판매 예상, 美시장 진출을 목전에 두고 국내 대성공 확인: TP 135,000원으로 상향, 현대차증권, '돌다리도 두들기며' IPO확대 나선다, 삼성바이오 주주님들, 안녕들 하신가요?, 코스피 코스닥 강보합 출발, 대한항공 드림텍 네온테크 옵티팜 급등</t>
+    <t>제네시스 Time: 거대한 포텐셜의 현실화 시작, 제네시스 판매 증가속도, 예상보다 빠르다: 연간판매량 17.5만대로 상향, G80 月1만대 시대 도래, 20년도 4분기 제네시스 총 7.3만대 판매 예상, 美시장 진출을 목전에 두고 국내 대성공 확인: TP 135,000원으로 상향, 현대차증권, '돌다리도 두들기며' IPO확대 나선다, 삼성바이오 주주님들, 안녕들 하신가요?, 코스피 코스닥 강보합 출발, 대한항공 드림텍 네온테크 옵티팜 급등</t>
   </si>
   <si>
     <t>주주권익 지표 개선한 현대·기아차…'주주 친화 경영' 결과물, ‘전기차 배터리’ 장착 엘지그룹, 현대차 젖히고 시총 3위로, 삼성·한화·교보 등 6곳 겨냥…금융그룹감독 법제화 재추진</t>
   </si>
   <si>
-    <t>현대차-시작된 EV 수익성 강화, 전기차 보조금 확대와 볼륨 증가, 2021년 E-GMP 출시로 이익 발생하기 시작, 기대되는 제네시스 북미 출시 효과, 뭉칫돈 들고 아파트 대신 주식으로</t>
+    <t>시작된 EV 수익성 강화, 전기차 보조금 확대와 볼륨 증가, 2021년 E-GMP 출시로 이익 발생하기 시작, 기대되는 제네시스 북미 출시 효과, 뭉칫돈 들고 아파트 대신 주식으로</t>
   </si>
   <si>
     <t>신풍제약·부광약품·제일약품 제약주에 관심 집중, 빅텍·스페코 방산주에 쏠렸던 기대감</t>
@@ -6082,7 +6082,7 @@
     <t>현대로템 CB 일반청약…1655억 모집에 7.9조 몰려, 코닥과 IBM의 흥망성쇠 /김동섭, 한국형 ‘수소전기차’, 독일 잡는다, 증권사 테마, SK증권 +14.71%, 유진투자증권 +5.08%, 1,650억 모집에 8조 뭉칫돈···현대로템 CB 흥행, 현대로템 전환사채 일반공모 청약 흥행, 1655억 모집에 8조 몰려, 코로나 시대 '인싸' 된 게임株…시총 40兆 넘본다, 공모주에 줄 선 뭉칫돈...제일모직 '30조 청약 신화' 깨질 수도</t>
   </si>
   <si>
-    <t>현대차-년도년도 2분기 2분기 Preivew: 하반기에 올 모멘텀에 주목, 년도년도 2분기 2분기 Preview: 코로나 19 영향으로 실적 부진 불가피, 하반기 SUV 신차 2종, 정상화 국면의 시작, 2021년 전기차 출시도 기대 요인, "잡으면 대박"···초저금리·유동성 타고 '줍줍' 나선 뭉칫돈, 현대로템 CB 일반청약에 8兆 몰려, 현대차 주식 매수의견 유지, "하반기 신차와 글로벌 회복 상승효과"</t>
+    <t>년도년도 2분기 2분기 Preivew: 하반기에 올 모멘텀에 주목, 년도년도 2분기 2분기 Preview: 코로나 19 영향으로 실적 부진 불가피, 하반기 SUV 신차 2종, 정상화 국면의 시작, 2021년 전기차 출시도 기대 요인, "잡으면 대박"···초저금리·유동성 타고 '줍줍' 나선 뭉칫돈, 현대로템 CB 일반청약에 8兆 몰려, 현대차 주식 매수의견 유지, "하반기 신차와 글로벌 회복 상승효과"</t>
   </si>
   <si>
     <t>현대엘리베이터(-5.21%) 주가 하락세... '자사주' 이슈에 상승흐름 보였던 전날과 대비, 코리아펀딩, 한 주간 장외주식 이슈 심층 분석, 상장후 주가관리 고려...SK바이오팜, 수요예측 흥행에도 공모가 안올려</t>
@@ -6103,13 +6103,13 @@
     <t>옵티머스사태 판매 증권사 공동대응 모색… 투자자 줄소송 전망, 코로나19 넉달새 4대그룹 시총 71조 증발...IT·바이오 4개사 독식, 현대차 · 기아차, 장중 주가 '껑충'..."전기차 등 시장 확대", 상한가 14종목, 현대건설우· 휴마시스 상한가 행진에 빅텍·스펙코 방산주 하한가, 대북주 대아티아이는 상한가 달성</t>
   </si>
   <si>
-    <t>현대차-기대감을 더 가져야 할 시점, 배터리 합작사 설립 가능성 확대, 동남아시아 시장 본격 진출의 신호탄, 전동화와 Motorization이 모두 본격화 되는 곳, 동남아시아로 간다, 유럽공장 정상화, 현재 EV 공급 본격화로 경쟁우위 확보 기대, 현대로템 임원 '수십명' CB매입 러시 이유는, "한국타이어앤테크놀로지 주가 상승 가능", 현대차와 협력관계 복원</t>
+    <t>기대감을 더 가져야 할 시점, 배터리 합작사 설립 가능성 확대, 동남아시아 시장 본격 진출의 신호탄, 전동화와 Motorization이 모두 본격화 되는 곳, 동남아시아로 간다, 유럽공장 정상화, 현재 EV 공급 본격화로 경쟁우위 확보 기대, 현대로템 임원 '수십명' CB매입 러시 이유는, "한국타이어앤테크놀로지 주가 상승 가능", 현대차와 협력관계 복원</t>
   </si>
   <si>
     <t>"코로나19로 미뤄진 IPO 하반기엔 쏠림… 신규상장 분산해야"</t>
   </si>
   <si>
-    <t>숨통 트인 IPO·증자…지난달 주식발행 254%↑, 5월 주식 발행 254% 급증…증시 회복에 IPO·증자 '숨통', 현대차-GENESIS에서 E-GMP로 이어지는 기대 요인, 20년도 2분기 매출 18,542십억원(전년 대비 증감율-31%), 영익151십억원(Y-88%) 전망, GENESIS &amp; SUV 믹스 확대에 따른 ASP 상승이 기대 요인, GENESIS에서 E-GMP로 이어지는 기대 요인, 현대차-년도년도 2분기 2분기 Preview - 판매대수로만 판단할 수없는년도 는분기 년도년도 2분기 2분기 , 목표주가 120,000원으로 9.1% 상향. 투자의견 Buy 유지, 년도년도 2분기 2분기 영업이익 1,752억원 (-85.8% 전년 대비 증감율) 예상. 시장 컨센서스를 하회할 것, 2020년 영업이익 3.0조원 (-15.9% 전년 대비 증감율) 예상. 기존 전망 대비 8.7% 하향조정, 판매 회복의 조짐은 기존 예상에 있던 부분</t>
+    <t>숨통 트인 IPO·증자…지난달 주식발행 254%↑, 5월 주식 발행 254% 급증…증시 회복에 IPO·증자 '숨통', GENESIS에서 E-GMP로 이어지는 기대 요인, 20년도 2분기 매출 18,542십억원(전년 대비 증감율-31%), 영익151십억원(Y-88%) 전망, GENESIS &amp; SUV 믹스 확대에 따른 ASP 상승이 기대 요인, GENESIS에서 E-GMP로 이어지는 기대 요인, 년도년도 2분기 2분기 Preview - 판매대수로만 판단할 수없는년도 는분기 년도년도 2분기 2분기 , 목표주가 120,000원으로 9.1% 상향. 투자의견 Buy 유지, 년도년도 2분기 2분기 영업이익 1,752억원 (-85.8% 전년 대비 증감율) 예상. 시장 컨센서스를 하회할 것, 2020년 영업이익 3.0조원 (-15.9% 전년 대비 증감율) 예상. 기존 전망 대비 8.7% 하향조정, 판매 회복의 조짐은 기존 예상에 있던 부분</t>
   </si>
   <si>
     <t>"수소트럭 시대 잡아라"…현대차, 다임러 출신 임원 영입, 현대카드, '연내 IPO' 불발될 듯.. "내년 이후 상황 보겠다", 현대차, 중국 영업 총괄 포드 출신 리홍펑에 맡긴다, 상반기 증시 코로나19에도 V자 반등, 하반기도 동학개미운동 활약할까</t>
@@ -6124,16 +6124,16 @@
     <t>한화시스템 주식 매수의견 유지, "사업영역 확장해 기업가치 긍정적"</t>
   </si>
   <si>
-    <t>현대차-엽기적인 내수 믹스, 20년도 2분기 영업이익은 1,633억원(-86.8% 전년 대비 증감율, OPM 0.9%)으로 컨센서스 52.3% 하회 전망, 5~6월 확인한 제네시스, SUV 등 내수 신차 중심 믹스 개선은 20년도 3분기 이후 미국 등 글로벌로 확대될 전망, 투자의견 BUY, 목표주가 140,000원, 업종 Top Picks 유지, 상반기 해외주식 직구 1위에 테슬라…주가는 151% 뛰어</t>
-  </si>
-  <si>
-    <t>코스피 코스닥 장중 동반하락, SG충방 글로스퍼랩스 조일알미늄 급등, '주가 100만원' 황제주 등극 앞둔 엔씨소프트…택진이형 '돈방석' 앉았다, 현대차-년도년도 2분기 2분기 Preview: Mix개선 화,년도 본분기 년도년도 2분기 2분기 Preview: 영업이익 2,360억원, Mix 대폭 개선으로 실적방어, 년도년도 2분기 2분기 을 저점으로 실적 급반등 예상: 실적 V자반등에 투자하라, 수소트럭 패권, 현대차-다가오는 회복과 성장의 시기, C19 직격탄을 맞은 20년도 2분기 실적, 그러나 전월 대비 증감율 판매회복 지속 중, 20년도 하반기 2021년 영업이익, 영업지표 개선과 기저효과로 +36%, +64% 전망, 투자의견 Buy, 적정주가 145,000원 유지, 업종 Top-pick 제시, 기간산업→IT→차·화·정→BBIG… 위기때마다 바뀐 간판기업, "현대차 주가 상승 가능", 판매 빠르게 회복해 3분기 실적반등 예상, 엔씨, 시총 10위 진입 '무서운 질주'</t>
+    <t>엽기적인 내수 믹스, 20년도 2분기 영업이익은 1,633억원(-86.8% 전년 대비 증감율, OPM 0.9%)으로 컨센서스 52.3% 하회 전망, 5~6월 확인한 제네시스, SUV 등 내수 신차 중심 믹스 개선은 20년도 3분기 이후 미국 등 글로벌로 확대될 전망, 투자의견 BUY, 목표주가 140,000원, 업종 Top Picks 유지, 상반기 해외주식 직구 1위에 테슬라…주가는 151% 뛰어</t>
+  </si>
+  <si>
+    <t>코스피 코스닥 장중 동반하락, SG충방 글로스퍼랩스 조일알미늄 급등, '주가 100만원' 황제주 등극 앞둔 엔씨소프트…택진이형 '돈방석' 앉았다, 년도년도 2분기 2분기 Preview: Mix개선 화,년도 본분기 년도년도 2분기 2분기 Preview: 영업이익 2,360억원, Mix 대폭 개선으로 실적방어, 년도년도 2분기 2분기 을 저점으로 실적 급반등 예상: 실적 V자반등에 투자하라, 수소트럭 패권, 다가오는 회복과 성장의 시기, C19 직격탄을 맞은 20년도 2분기 실적, 그러나 전월 대비 증감율 판매회복 지속 중, 20년도 하반기 2021년 영업이익, 영업지표 개선과 기저효과로 +36%, +64% 전망, 투자의견 Buy, 적정주가 145,000원 유지, 업종 Top-pick 제시, 기간산업→IT→차·화·정→BBIG… 위기때마다 바뀐 간판기업, "현대차 주가 상승 가능", 판매 빠르게 회복해 3분기 실적반등 예상, 엔씨, 시총 10위 진입 '무서운 질주'</t>
   </si>
   <si>
     <t>테슬라 또 폭발,나스닥 다우지수 폭락 속 배터리 우뚝… LG전자 삼성SDI SK이노 후끈, 최태원 SK그룹 회장, "SK바이오팜 기세 한풀 꺾였다"...주가 상장 1주일만에 '출렁', 주가 강세에 주목된 테슬라 '배터리데이'...국내 자동차업계 동맹 구축, 머스크가 '완전 바보'라고 조롱한 수소차…누가 바보?</t>
   </si>
   <si>
-    <t>상반기 50대 그룹 총수 주식평가액…서정진 회장 3조↑, S&amp;T모티브 주식 매수의견 유지, “현대차에 친환경차부품 공급 늘어”, 김승연 한화그룹 회장, 상반기 주식평가액, 서정진 회장 3조 급증…이건희 회장 1.7조↓, '상반기' 이건희 회장 주식재산 1조7000억원↓…서정진 회장 3조원↑, 코로나19에도 끄떡없는 이건희-이재용 '부자', 회사 '백척간두'인데...박정원·조원태, 주식재산은 '껑충', 상반기 삼성 이건희 회장 주식재산 1조7천억↓, 셀트리온 서정진 3조↑, 이건희·이재용 다음은 셀트리온 서정진…총수 주식재산 대변동, 코로나에 희비 엇갈린 주식부자…서정진, 재산 3조 늘었다, 국민연금, 2분기에 국내 배터리와 반도체기업 주식 주로 사들여, 현대차-변곡점 기대, 년도년도 2분기 2분기 실적 Preview: 해외 發 부진, 년도년도 2분기 2분기 기점으로 전분기 대비 증감율 이익 개선 흐름 예상, 제네시스와 EV 성장 기대감 확대될 것, 투자의견 Buy, 목표주가 120,000원 유지, 50대 그룹 총수 주식가치 희비… 이건희 회장 주식재산 1조 7천억 줄고 서정진 회장 3조 늘었다, 셀트리온 서정진 회장 주식가치 상반기에 3조원 급증…이건희 회장 1.7조원↓, 재벌 총수 주식가치 ‘희비’ 엇갈려…서정진 3조↑,이건희 1조 7000억↓, 올 상반기 주식재산 가장 많이 늘어난 총수는?, 국민연금, 엔씨소프트 판 돈으로 네이버 샀다, 현대로템은 어쩌다 '내놓은 자식'이 됐을까</t>
+    <t>상반기 50대 그룹 총수 주식평가액…서정진 회장 3조↑, S&amp;T모티브 주식 매수의견 유지, “현대차에 친환경차부품 공급 늘어”, 김승연 한화그룹 회장, 상반기 주식평가액, 서정진 회장 3조 급증…이건희 회장 1.7조↓, '상반기' 이건희 회장 주식재산 1조7000억원↓…서정진 회장 3조원↑, 코로나19에도 끄떡없는 이건희-이재용 '부자', 회사 '백척간두'인데...박정원·조원태, 주식재산은 '껑충', 상반기 삼성 이건희 회장 주식재산 1조7천억↓, 셀트리온 서정진 3조↑, 이건희·이재용 다음은 셀트리온 서정진…총수 주식재산 대변동, 코로나에 희비 엇갈린 주식부자…서정진, 재산 3조 늘었다, 국민연금, 2분기에 국내 배터리와 반도체기업 주식 주로 사들여, 변곡점 기대, 년도년도 2분기 2분기 실적 Preview: 해외 發 부진, 년도년도 2분기 2분기 기점으로 전분기 대비 증감율 이익 개선 흐름 예상, 제네시스와 EV 성장 기대감 확대될 것, 투자의견 Buy, 목표주가 120,000원 유지, 50대 그룹 총수 주식가치 희비… 이건희 회장 주식재산 1조 7천억 줄고 서정진 회장 3조 늘었다, 셀트리온 서정진 회장 주식가치 상반기에 3조원 급증…이건희 회장 1.7조원↓, 재벌 총수 주식가치 ‘희비’ 엇갈려…서정진 3조↑,이건희 1조 7000억↓, 올 상반기 주식재산 가장 많이 늘어난 총수는?, 국민연금, 엔씨소프트 판 돈으로 네이버 샀다, 현대로템은 어쩌다 '내놓은 자식'이 됐을까</t>
   </si>
   <si>
     <t>코스피 코스닥 장중 동반하락, 진양산업 써니전자 케이피에스 급등, 현대차 주식 매수의견 유지, "해외에서 하반기 신차로 실적회복", 주식 재산만 ‘3조’가 늘어난 사람이 있다</t>
@@ -6148,13 +6148,13 @@
     <t>시총 3→11위… 추락하는 현대차에 날개가 없다, 증권사 테마, 유진투자증권 +9.01%, 미래에셋대우 +4.09%</t>
   </si>
   <si>
-    <t>현대차 시총 3위→11위 추락… 코로나발 해외 판매 급감 ‘직격탄’, 현대로템CB 투자자, 한 달 만에 60% 수익?, 현대차-내수와 환율이 방어, 20년도 2분기 실적 매출액 21조 3,049억원(-21%전년 대비 증감율), 영업이익 3,367억원(-73%전년 대비 증감율)으로 컨센서스(2,951억원) 상회 전망, 환율과 내수, 제네시스 판매(+121%전년 대비 증감율) 강세가 실적 방어제 역할 예상, 높은 글로벌 물량 감소 감안해 20년 매출 추정치 4% 하향, 하반기 해외 공장 가동률 반등으로 실적 개선 가시화, 경쟁사들 대비 실적과 미래 경쟁력 모두 우위 구간, 투자 의견 BUY 유지</t>
+    <t>현대차 시총 3위→11위 추락… 코로나발 해외 판매 급감 ‘직격탄’, 현대로템CB 투자자, 한 달 만에 60% 수익?, 내수와 환율이 방어, 20년도 2분기 실적 매출액 21조 3,049억원(-21%전년 대비 증감율), 영업이익 3,367억원(-73%전년 대비 증감율)으로 컨센서스(2,951억원) 상회 전망, 환율과 내수, 제네시스 판매(+121%전년 대비 증감율) 강세가 실적 방어제 역할 예상, 높은 글로벌 물량 감소 감안해 20년 매출 추정치 4% 하향, 하반기 해외 공장 가동률 반등으로 실적 개선 가시화, 경쟁사들 대비 실적과 미래 경쟁력 모두 우위 구간, 투자 의견 BUY 유지</t>
   </si>
   <si>
     <t>유행 된 '현대차 시총을 넘어라'…문지기로 전락한 '재계 2위', ‘로또 맞자’...남은 공모주도 흥행예고, "수소차-전기차 전략 강화"...현대차·기아차, '장중 껑충', 한국판 뉴딜 발표에 관련 부산소재 관련 종목도 '들썩'</t>
   </si>
   <si>
-    <t>현대제철 주식 매수의견 유지, "그린뉴딜에 수소차 관련 사업 부각", 현대차-년도년도 2분기 2분기 Preview: 내수 ASP로 선방, 년도년도 2분기 2분기 연결 매출액 21.6조원(전년 대비 증감율 -19.8%), 영업이익 2,307억원(전년 대비 증감율 -81.4%) 전망, 자동차 부문 매출액 15.8조원(전년 대비 증감율 -25%), 영업이익 789억원(OPM 0.5%) 예상, 내수는 판매량과 더불어 ASP 크게 상승할 전망, '미래' 테마 올라탄 국내 기업들, 현재 가치평가 무의미해졌다, 현대로템, CB 콜옵션 임박…투자자 선택은?, 테슬라의 자율주행은 사기일까요?</t>
+    <t>현대제철 주식 매수의견 유지, "그린뉴딜에 수소차 관련 사업 부각", 년도년도 2분기 2분기 Preview: 내수 ASP로 선방, 년도년도 2분기 2분기 연결 매출액 21.6조원(전년 대비 증감율 -19.8%), 영업이익 2,307억원(전년 대비 증감율 -81.4%) 전망, 자동차 부문 매출액 15.8조원(전년 대비 증감율 -25%), 영업이익 789억원(OPM 0.5%) 예상, 내수는 판매량과 더불어 ASP 크게 상승할 전망, '미래' 테마 올라탄 국내 기업들, 현재 가치평가 무의미해졌다, 현대로템, CB 콜옵션 임박…투자자 선택은?, 테슬라의 자율주행은 사기일까요?</t>
   </si>
   <si>
     <t>언택트株 vs 콘택트株…당분간 시소게임 전망, 테슬라 날아갈 동안 잠잠하던 현대차…그린뉴딜로 뒤늦게 '친환경' 탑승, 먹거리 선점 위해서라면…기꺼이 카메라 앞에서는 회장님들, 개미들 이번엔 ‘2차전지’로 진격, 정몽구 현대차그룹 회장 입원 치료중…"염증 조절되는대로 퇴원" 外, 친환경차 · 전기차 이슈 속...현대차 · 기아차, 장중 '연일 강세'</t>
@@ -6166,7 +6166,7 @@
     <t>‘한국판 뉴딜’, 딜을 빠뜨리다, 경제 6단체 “상법 개정안, 주주의 재산권 침해-투기자본의 경영위협 우려”, 2200선 재탈환한 코스피, 소외된 가치株 공략해야…실적 돋보이는 파트론 관심</t>
   </si>
   <si>
-    <t>현대차-20년도 2분기 Preview-양호했던 6월 판매와 믹스 개선 효과, 영업이익 4,212억원 (-66.0% 전년 대비 증감율) 예상. 시장 컨센서스 37.5% 상회할 것, 지역 믹스 개선과 내수시장 모델 믹스 개선으로 대당 공헌이익도 급증했을 것, 2020년 영업이익 전망치 3.4조원. 시장 컨센서스를 7.1% 상회할 전망, "정의선-이재용 21일 회동"...현대차 · 기아차, 장중 '또 상승', 이참에 주식증여·매수…내로라하는 그룹은 다 했다, 니콜라 랠리 끝?...'상투' 잡은 개미 어쩌나, 발로 뛰는 정의선 현대차 부회장, 주가는 뒷걸음질...반등 언제쯤?, 코로나가 점령한 2분기…승자는 4차산업혁명株, 경제 6단체 “상법 개정, 투기자본의 경영위협 우려”, 현대차·하이트진로·SK·롯데</t>
+    <t>20년도 2분기 Preview-양호했던 6월 판매와 믹스 개선 효과, 영업이익 4,212억원 (-66.0% 전년 대비 증감율) 예상. 시장 컨센서스 37.5% 상회할 것, 지역 믹스 개선과 내수시장 모델 믹스 개선으로 대당 공헌이익도 급증했을 것, 2020년 영업이익 전망치 3.4조원. 시장 컨센서스를 7.1% 상회할 전망, "정의선-이재용 21일 회동"...현대차 · 기아차, 장중 '또 상승', 이참에 주식증여·매수…내로라하는 그룹은 다 했다, 니콜라 랠리 끝?...'상투' 잡은 개미 어쩌나, 발로 뛰는 정의선 현대차 부회장, 주가는 뒷걸음질...반등 언제쯤?, 코로나가 점령한 2분기…승자는 4차산업혁명株, 경제 6단체 “상법 개정, 투기자본의 경영위협 우려”, 현대차·하이트진로·SK·롯데</t>
   </si>
   <si>
     <t>조현범 한국타이어앤테크놀로지 사장, 美증시, 경기부양책·백신 개발 기대…주요지수 상승 마감, (창간1주년 기획:골격 수술 중인 재계)②에이치솔루션 덩치 키우는 한화…니콜라로 점화된 경영승계 시나리오</t>
@@ -6175,10 +6175,10 @@
     <t>국민연금, 제약‧바이오‧IT 담고 유통‧서비스‧제조업 뺐다, 'BBIG7' 뒤이을 차기 주도株 찾아라, '큰 손' 국민연금이 지분 10% 넘게 사들인 기업은?, 국민연금, '제약·바이오' 투자 늘리고 '조선·항공' 줄였다</t>
   </si>
   <si>
-    <t>오너들의 긍정마인드, 현대차-20년도 2분기 Review: 제네시스의 힘!, 판매감소를 상쇄한 믹스, 2020년, 코로나19에도 전년대비 이익증가, 내수판매가 이끈 서프라이즈믹스향상: 금융부분, 현대카드 실적회복으로 OPM 6.3%: 영업 외 실적 부진, 뚜렷한 믹스향상, 현대차-년도년도 2분기 2분기 Review - 믹스 개선 효과 생각보다 컸다, 목표주가 150,000원 (기존 대비 +7.1%), 투자의견 Buy 유지, 년도년도 2분기 2분기 영업이익 5,903억원 (-52.3% 전년 대비 증감율), 시장 컨센서스 크게 상회, 2020년 영업이익 전망치 5.1% 상향하나 당기순이익 전망치는 9.0% 하향, 투자포인트: 안정적 내수시장, 신차 사이클, 친환경차 대응전략 다변화</t>
-  </si>
-  <si>
-    <t>현대차-미래를 대비할 풍부한 곳간, 2분기 영업이익 5,903억원(-52.3%)으로 시장 기대치(3,192억원) 상회, 하반기 실적 개선에 대한 신뢰 강화, 공격적인 차세대 기술 확보 가능, 목표주가 145,000원으로 상향, 투자의견 매수 유지, 현대차·SK하이닉스, 같은 어닝 서프라이즈에도 엇갈린 증시 반응, 테슬라, 차 팔아 돈 번 게 아니다?…‘천슬라’ 앞날은?, "테슬라 날개 달고 주가 급등하는 LG화학" EV 배터리 빅딜에 주목, '잠행 경영' 신세계 정용진…'최악 실적' 포스코 최정우, 현대차-년도년도 2분기 2분기 Review: 올것이 오고 말았다, 현대차 년도년도 2분기 2분기 Review: 최악의 환경 에도 불구하고 원가율 개선!, 신차기반의 가동률 개선: 하반기에 펼쳐질 강력한 모멘텀이 투자하라, 투자의견 Buy 유지, 목표주가 165,000원으로 상향. 적극 비중확대 추천, 현대차-실적 바닥이 이 정도라면, 20년도 2분기 영업이익 5,903억원(전년 대비 증감율 -52%) 기록, 어닝 서프라이즈. 믹스 개선에 의한 실적방어력이 돋보였고, 우려했던 금융부문의 부진도 없었음, 사실상 최악의 시기에 예상보다 양호한 실적을 보여줌으로써 실적 눈높이를 높일 수 있게 되었음, 현대차-하반기 실적 방향성 긍정적 기대, 2020년 2분기 영업이익 컨센서스 98% 상회, 믹스개선과 비용통제를 통한 경쟁력 개선 추진, 수익 방어 능력 입증으로 하반기 이후 실적 방향성 긍정적, 현대차-2Q 상회. 놀라운 믹스 효과. 하반기 모멘텀 확대, 목표주가를 15만원으로 상향, 20년도 2분기 Review: 영업이익률 2.7% 기록, 컨퍼런스콜의 주요 내용: 수소 상용차 시장은 대형트럭 중심으로 성장, 현대차-하반기 실적 방향성 긍정적 기대, 2020년 2분기 영업이익 컨센서스 98% 상회, 믹스개선과 비용통제를 통한 경쟁력 개선 추진, 수익 방어 능력 입증으로 하반기 이후 실적 방향성 긍정적, 현대차-년도년도 2분기 2분기 Review: 올것이 오고 말았다, 현대차 년도년도 2분기 2분기 Review: 최악의 환경 에도 불구하고 원가율 개선!, 신차기반의 가동률 개선: 하반기에 펼쳐질 강력한 모멘텀이 투자하라, 투자의견 Buy 유지, 목표주가 165,000원으로 상향. 적극 비중확대 추천, 현대차-미래를 대비할 풍부한 곳간, 2분기 영업이익 5,903억원(-52.3%)으로 시장 기대치(3,192억원) 상회, 하반기 실적 개선에 대한 신뢰 강화, 공격적인 차세대 기술 확보 가능, 목표주가 145,000원으로 상향, 투자의견 매수 유지, 현대차-힘 빼고 쳐도 이 정도, 내수 호조로 영업이익 컨센서스 85% 상회, 신형 플랫폼과 제네시스가 이끄는 이익 개선 싸이클, 미래차 경쟁력 강화가 밸류에이션 재평가로 이어질 가능성에도 주목, 현대차-기대 이상의 판가 &amp; 믹스 효과, 연결 매출 21.9조원(전년 대비 증감율-18.9%), 영업이익 5천9백억원(전년 대비 증감율-52.3%, OPM 2.7%), ASP 상승과 믹스 개선이 영업이익 서프라이즈를 견인, 차량사업부 매출 16조원(전년 대비 증감율-23.6%), 영업이익 295십억원(전년 대비 증감율-71.6%), OPM 1.8%, 금융사업부 매출: 4.3조원(전년 대비 증감율+4.5%), 영업이익 272십억원(전년 대비 증감율+8.8%), OPM 6.3%, 기타사업부 매출 1.5조원(전년 대비 증감율-18%), 영업이익 42십억원(전년 대비 증감율-30%), OPM 2.9%, 현대차-실적 바닥이 이 정도라면, 20년도 2분기 영업이익 5,903억원(전년 대비 증감율 -52%) 기록, 어닝 서프라이즈. 믹스 개선에 의한 실적방어력이 돋보였고, 우려했던 금융부문의 부진도 없었음, 사실상 최악의 시기에 예상보다 양호한 실적을 보여줌으로써 실적 눈높이를 높일 수 있게 되었음, 현대차-2 분기 Review: 양호한 신차 효과와 제품믹스 개선, 2분기 매출액과 영업이익은 각각 21조8,590억원(-18.9% y-y), 5,903억원(-52.3% y-y, 영업이익률 2.7%)으로 당사 예상치를 상회, 2분기를 정점으로 내수 이익 기여도는 하락하겠지만, 2분기 실적을 통해 양호한 신차효과와 제품믹스 개선추세 확인했다는 점은 긍정적, 현대차- 제네시스 효과 확대 예상, 년도년도 2분기 2분기 Review : 시장 기대치 큰 폭 상회, Valuation 재평가 기대, 현대차-년도년도 2분기 2분기 Review: 제네시스 효과로 기대치 대폭 상회, 년도년도 2분기 2분기 Review: 제네시스 효과로 기대치 대폭 상회, 믹스 개선 효과 2분기 영업이익 1조원 기여, 목표주가 상향, 2분기가 실적의 저점, 현대차-이익 기대 상향과 수소서비스 진출 재평가, 년도년도 2분기 2분기 영업이익은 5,903억원(-31.7% 전년 대비 증감율, OPM 3.4%) 기록, 컨센서스 85.0% 상회, 년도년도 2분기 2분기 Review: 기대를 뛰어 넘은 믹스 개선의 효과, Key Takeaways: 수소, 나무에서 숲으로 사업 확대. 실적 개선 모멘텀까지, 현대차-더 이상 확인이 필요할까?, 20년도 2분기 , Surprise, 하반기 본격적인 실적 반등, 경쟁력 재차 확인, 현대차-호실적 그 이상의 의미, 2분기 실적은 제품 믹스 개선으로 인한 호실적, 3분기 이후 신차 싸이클의 지속을 기대</t>
+    <t>오너들의 긍정마인드, 20년도 2분기 Review: 제네시스의 힘!, 판매감소를 상쇄한 믹스, 2020년, 코로나19에도 전년대비 이익증가, 내수판매가 이끈 서프라이즈믹스향상: 금융부분, 현대카드 실적회복으로 OPM 6.3%: 영업 외 실적 부진, 뚜렷한 믹스향상, 년도년도 2분기 2분기 Review - 믹스 개선 효과 생각보다 컸다, 목표주가 150,000원 (기존 대비 +7.1%), 투자의견 Buy 유지, 년도년도 2분기 2분기 영업이익 5,903억원 (-52.3% 전년 대비 증감율), 시장 컨센서스 크게 상회, 2020년 영업이익 전망치 5.1% 상향하나 당기순이익 전망치는 9.0% 하향, 투자포인트: 안정적 내수시장, 신차 사이클, 친환경차 대응전략 다변화</t>
+  </si>
+  <si>
+    <t>미래를 대비할 풍부한 곳간, 2분기 영업이익 5,903억원(-52.3%)으로 시장 기대치(3,192억원) 상회, 하반기 실적 개선에 대한 신뢰 강화, 공격적인 차세대 기술 확보 가능, 목표주가 145,000원으로 상향, 투자의견 매수 유지, 현대차·SK하이닉스, 같은 어닝 서프라이즈에도 엇갈린 증시 반응, 테슬라, 차 팔아 돈 번 게 아니다?…‘천슬라’ 앞날은?, "테슬라 날개 달고 주가 급등하는 LG화학" EV 배터리 빅딜에 주목, '잠행 경영' 신세계 정용진…'최악 실적' 포스코 최정우, 년도년도 2분기 2분기 Review: 올것이 오고 말았다, 현대차 년도년도 2분기 2분기 Review: 최악의 환경 에도 불구하고 원가율 개선!, 신차기반의 가동률 개선: 하반기에 펼쳐질 강력한 모멘텀이 투자하라, 투자의견 Buy 유지, 목표주가 165,000원으로 상향. 적극 비중확대 추천, 실적 바닥이 이 정도라면, 20년도 2분기 영업이익 5,903억원(전년 대비 증감율 -52%) 기록, 어닝 서프라이즈. 믹스 개선에 의한 실적방어력이 돋보였고, 우려했던 금융부문의 부진도 없었음, 사실상 최악의 시기에 예상보다 양호한 실적을 보여줌으로써 실적 눈높이를 높일 수 있게 되었음, 하반기 실적 방향성 긍정적 기대, 2020년 2분기 영업이익 컨센서스 98% 상회, 믹스개선과 비용통제를 통한 경쟁력 개선 추진, 수익 방어 능력 입증으로 하반기 이후 실적 방향성 긍정적, 2Q 상회. 놀라운 믹스 효과. 하반기 모멘텀 확대, 목표주가를 15만원으로 상향, 20년도 2분기 Review: 영업이익률 2.7% 기록, 컨퍼런스콜의 주요 내용: 수소 상용차 시장은 대형트럭 중심으로 성장, 하반기 실적 방향성 긍정적 기대, 2020년 2분기 영업이익 컨센서스 98% 상회, 믹스개선과 비용통제를 통한 경쟁력 개선 추진, 수익 방어 능력 입증으로 하반기 이후 실적 방향성 긍정적, 년도년도 2분기 2분기 Review: 올것이 오고 말았다, 현대차 년도년도 2분기 2분기 Review: 최악의 환경 에도 불구하고 원가율 개선!, 신차기반의 가동률 개선: 하반기에 펼쳐질 강력한 모멘텀이 투자하라, 투자의견 Buy 유지, 목표주가 165,000원으로 상향. 적극 비중확대 추천, 미래를 대비할 풍부한 곳간, 2분기 영업이익 5,903억원(-52.3%)으로 시장 기대치(3,192억원) 상회, 하반기 실적 개선에 대한 신뢰 강화, 공격적인 차세대 기술 확보 가능, 목표주가 145,000원으로 상향, 투자의견 매수 유지, 힘 빼고 쳐도 이 정도, 내수 호조로 영업이익 컨센서스 85% 상회, 신형 플랫폼과 제네시스가 이끄는 이익 개선 싸이클, 미래차 경쟁력 강화가 밸류에이션 재평가로 이어질 가능성에도 주목, 기대 이상의 판가 &amp; 믹스 효과, 연결 매출 21.9조원(전년 대비 증감율-18.9%), 영업이익 5천9백억원(전년 대비 증감율-52.3%, OPM 2.7%), ASP 상승과 믹스 개선이 영업이익 서프라이즈를 견인, 차량사업부 매출 16조원(전년 대비 증감율-23.6%), 영업이익 295십억원(전년 대비 증감율-71.6%), OPM 1.8%, 금융사업부 매출: 4.3조원(전년 대비 증감율+4.5%), 영업이익 272십억원(전년 대비 증감율+8.8%), OPM 6.3%, 기타사업부 매출 1.5조원(전년 대비 증감율-18%), 영업이익 42십억원(전년 대비 증감율-30%), OPM 2.9%, 실적 바닥이 이 정도라면, 20년도 2분기 영업이익 5,903억원(전년 대비 증감율 -52%) 기록, 어닝 서프라이즈. 믹스 개선에 의한 실적방어력이 돋보였고, 우려했던 금융부문의 부진도 없었음, 사실상 최악의 시기에 예상보다 양호한 실적을 보여줌으로써 실적 눈높이를 높일 수 있게 되었음, 2 분기 Review: 양호한 신차 효과와 제품믹스 개선, 2분기 매출액과 영업이익은 각각 21조8,590억원(-18.9% y-y), 5,903억원(-52.3% y-y, 영업이익률 2.7%)으로 당사 예상치를 상회, 2분기를 정점으로 내수 이익 기여도는 하락하겠지만, 2분기 실적을 통해 양호한 신차효과와 제품믹스 개선추세 확인했다는 점은 긍정적, 제네시스 효과 확대 예상, 년도년도 2분기 2분기 Review : 시장 기대치 큰 폭 상회, Valuation 재평가 기대, 년도년도 2분기 2분기 Review: 제네시스 효과로 기대치 대폭 상회, 년도년도 2분기 2분기 Review: 제네시스 효과로 기대치 대폭 상회, 믹스 개선 효과 2분기 영업이익 1조원 기여, 목표주가 상향, 2분기가 실적의 저점, 이익 기대 상향과 수소서비스 진출 재평가, 년도년도 2분기 2분기 영업이익은 5,903억원(-31.7% 전년 대비 증감율, OPM 3.4%) 기록, 컨센서스 85.0% 상회, 년도년도 2분기 2분기 Review: 기대를 뛰어 넘은 믹스 개선의 효과, Key Takeaways: 수소, 나무에서 숲으로 사업 확대. 실적 개선 모멘텀까지, 더 이상 확인이 필요할까?, 20년도 2분기 , Surprise, 하반기 본격적인 실적 반등, 경쟁력 재차 확인, 호실적 그 이상의 의미, 2분기 실적은 제품 믹스 개선으로 인한 호실적, 3분기 이후 신차 싸이클의 지속을 기대</t>
   </si>
   <si>
     <t>NH투자증권, 옵티머스 선지급·지급비율 논의 外, 정의선 수석부회장 '통 큰' 매수, 연봉 10배로 돌아와···평가차익 500억원 웃돌아, ‘책임경영’ 정의선, 통 큰 매수…4개월 만에 500억 차익, 현대차 '정의선'…4개월 만에 주식, 연봉 대비 10배 올라, "코로나 충격 컸다"…기업 3곳 중 2곳 실적 악화</t>
@@ -6199,7 +6199,7 @@
     <t>(대한민국 재벌 신뢰지수)③김범수 카카오 의장 신뢰도 '껑충', S&amp;T모티브 주식 매수의견 유지, "현대차에 친환경차부품 공급 늘어", 삼성전자를 둘러싼 세 가지 리스크는</t>
   </si>
   <si>
-    <t>달러 약세에 달러인버스 수익률 '쏠쏠', [브릿지경제의 ‘신간(新刊) 베껴읽기’] &lt;재벌이 대체 무슨 죄를 지었다고&gt; 이병태, 현대차-운송분야 탄소중립 리딩기업 기대, 배터리전기차와 수소전기차 통한 친환경 리딩기업으로, 투자의견 매수, 목표주가 160,000원 유지, 현대차-운송분야 탄소중립 리딩기업 기대, 배터리전기차와 수소전기차 통한 친환경 리딩기업으로, 투자의견 매수, 목표주가 160,000원 유지, "네이버·카카오 계속 오르기 어려워…구경제로 자금 이동할수도", 조원태 대한항공 대표이사 겸 한진그룹 회장, 美경영학회 국제경영분과 회장 선출된 송재용 서울대 교수</t>
+    <t>달러 약세에 달러인버스 수익률 '쏠쏠', [브릿지경제의 ‘신간(新刊) 베껴읽기’] &lt;재벌이 대체 무슨 죄를 지었다고&gt; 이병태, 운송분야 탄소중립 리딩기업 기대, 배터리전기차와 수소전기차 통한 친환경 리딩기업으로, 투자의견 매수, 목표주가 160,000원 유지, 운송분야 탄소중립 리딩기업 기대, 배터리전기차와 수소전기차 통한 친환경 리딩기업으로, 투자의견 매수, 목표주가 160,000원 유지, "네이버·카카오 계속 오르기 어려워…구경제로 자금 이동할수도", 조원태 대한항공 대표이사 겸 한진그룹 회장, 美경영학회 국제경영분과 회장 선출된 송재용 서울대 교수</t>
   </si>
   <si>
     <t>페이스북·웨이보 연동 ELS, 돈 떼일 염려 가장 적네, 지난달 동남권 상장사 주가상승세…한국판 뉴딜·바이오 주 급등</t>
@@ -6208,13 +6208,13 @@
     <t>'역대 최고' 시총 LG,구광모 회장의 다음 단계는?, 현대로템 '수소 테마' 타고 달리자…CB 투자자, 고수익에 '함박웃음', 박정원 두산 대표이사 및 두산그룹 회장, KT&amp;G, 14년 만에 최대폭 상승</t>
   </si>
   <si>
-    <t>현대차-글로벌 전기차 1위, 꿈이 아닌 이유, 글로벌 전기차 1위의 꿈, EV 글로벌 4위, 2021년부터 경쟁력 강화 본격화, 하반기 이익 증가세 전환, 2021년 영업이익 5.6조원 전망, 현대로템 CB 조기상환···2,400억 유증 효과, 현대차-글로벌 전기차 1위, 꿈이 아닌 이유, 글로벌 전기차 1위의 꿈, EV 글로벌 4위, 2021년부터 경쟁력 강화 본격화, 하반기 이익 증가세 전환, 2021년 영업이익 5.6조원 전망</t>
+    <t>글로벌 전기차 1위, 꿈이 아닌 이유, 글로벌 전기차 1위의 꿈, EV 글로벌 4위, 2021년부터 경쟁력 강화 본격화, 하반기 이익 증가세 전환, 2021년 영업이익 5.6조원 전망, 현대로템 CB 조기상환···2,400억 유증 효과, 글로벌 전기차 1위, 꿈이 아닌 이유, 글로벌 전기차 1위의 꿈, EV 글로벌 4위, 2021년부터 경쟁력 강화 본격화, 하반기 이익 증가세 전환, 2021년 영업이익 5.6조원 전망</t>
   </si>
   <si>
     <t>신풍제약 얼마나 뜨겁길래...이름비슷한 신풍제지 매수후 낭패, 한미글로벌도, 뉴LG 최고 시총, '구광모 실용주의' 드높은 성가...다음 반등 포인트는?, “전기차 타고 랠리”…현대차, 국민연금 기대감 부응할까, PB 10명 중 7명 "해외주식 유망", 그린뉴딜 올라탄 현대차… 국민연금도 `합석`</t>
   </si>
   <si>
-    <t>젊은층 주식 투자 열풍… "미래에 대한 불확실성 확산 영향", 정의선 ‘아이오닉’으로 전기차 승부수… 4년내 3종 출격, 현대차-해외여행? 대신 제네시스 탄다!, 자동차, `Stay in Country`의 최대 수혜주, 현대차 제네시스, 수입차만큼 팔린다, 코스피, 1.4%대 상승…개인 매수 우위·자동차 업종 강세, 현대차-해외여행? 대신 제네시스 탄다!, 자동차, `Stay in Country`의 최대 수혜주, 현대차 제네시스, 수입차만큼 팔린다, 현대차 `아이오닉` 전기차 전용으로 키운다, 코로나19의 역설? 속으로 웃는 회장님들, 외국인 매수주춤 급변심?... 씨젠 삼성전자 상승제동?, 신풍제약 수젠텍 주목, '현대차株의 귀환' … 15%올라 시총 7위 복귀</t>
+    <t>젊은층 주식 투자 열풍… "미래에 대한 불확실성 확산 영향", 정의선 ‘아이오닉’으로 전기차 승부수… 4년내 3종 출격, 해외여행? 대신 제네시스 탄다!, 자동차, `Stay in Country`의 최대 수혜주, 현대차 제네시스, 수입차만큼 팔린다, 코스피, 1.4%대 상승…개인 매수 우위·자동차 업종 강세, 해외여행? 대신 제네시스 탄다!, 자동차, `Stay in Country`의 최대 수혜주, 현대차 제네시스, 수입차만큼 팔린다, 현대차 `아이오닉` 전기차 전용으로 키운다, 코로나19의 역설? 속으로 웃는 회장님들, 외국인 매수주춤 급변심?... 씨젠 삼성전자 상승제동?, 신풍제약 수젠텍 주목, '현대차株의 귀환' … 15%올라 시총 7위 복귀</t>
   </si>
   <si>
     <t>정의선 부회장, 현대차 주식 매수 5달만에 900억 수익, 정의선, 현대차 주식 산 지 5달 만에 900억원 벌어, 증시 파죽지세… 코스피 2400선 돌파, 현대차 주가 급등에 '친환경차 낙관론'…증권가 평가는 엇갈려</t>
@@ -6250,16 +6250,16 @@
     <t>삼성바이오, 시가총액 52조5350억원…시총 2위 등극, '빚투' 16조 파죽지세…"총알은 없어도 신용은 있다", 현대차, HMM과 관계 청산…주식 전량 처분, 이노션 주식 매수의견 유지, "현대차 전기차 광고 확대의 수혜 커져"</t>
   </si>
   <si>
-    <t>현대차-고생 끝에 낙이 오다, 투자의견 Buy, 목표주가 20만원 제시, 20년도 하반기 이익모멘텀 발생 예상, 업종별 주가 들썩들썩…달리는 말에 계속 탈까, 쉬었던 말로 갈아탈까, News Briefing, 현대차-고생 끝에 낙이 오다, 투자의견 Buy, 목표주가 20만원 제시, 20년도 하반기 이익모멘텀 발생 예상</t>
-  </si>
-  <si>
-    <t>"美 기술만족도 1 · 3위"...현대차 · 기아차 주가 '장중 껑충', 현대차-EBITDAC을 보면 주가가 보인다, 매수의견 유지, 목표주가 상향, 기대 믹스 개선 효과는 21년 더 크다, 달라진 시장, 달라진 시각, 현대차그룹, 보통주 시가총액 90조 돌파...정의선 자사주 수익율 100% 넘어서, 현대차-EBITDAC을 보면 주가가 보인다, 매수의견 유지, 목표주가 상향, 기대 믹스 개선 효과는 21년 더 크다, 달라진 시장, 달라진 시각</t>
-  </si>
-  <si>
-    <t>현대차-2021년 그린카 대격변의 시작, E-GMP 플랫폼 출시와 EV 속도전, 수소상용차 글로벌 출시 본격화, 목표주가 상향, 대전환기의 투자 기회, 현대차-2021년 그린카 대격변의 시작, E-GMP 플랫폼 출시와 EV 속도전, 수소상용차 글로벌 출시 본격화, 목표주가 상향, 대전환기의 투자 기회</t>
-  </si>
-  <si>
-    <t>이노션 주식 매수의견 유지, “현대차 제네시스 미국 광고수요 증가”, 최광욱 J&amp;J자산운용 대표 “주식시장, 역대급 유동성장 시작됐다”, 현대차-목표주가 상향, 아직 갈길이 멀다!, 목표주가 220,000원으로 상향, 미국시장 턴어라운드의 가시화 단계, 신차효과로 인해 지속적으로 놀라운 판매성과 달성 가능해짐, 변곡점에서 발견된 추세적 ASP 상승, 놀라운 원가율 개선에 투자하자, 현대차-목표주가 상향, 아직 갈길이 멀다!, 목표주가 220,000원으로 상향, 미국시장 턴어라운드의 가시화 단계, 신차효과로 인해 지속적으로 놀라운 판매성과 달성 가능해짐, 변곡점에서 발견된 추세적 ASP 상승, 놀라운 원가율 개선에 투자하자, 우리금융, 자본적정성 열위…주가 부양은 공염불?</t>
+    <t>고생 끝에 낙이 오다, 투자의견 Buy, 목표주가 20만원 제시, 20년도 하반기 이익모멘텀 발생 예상, 업종별 주가 들썩들썩…달리는 말에 계속 탈까, 쉬었던 말로 갈아탈까, News Briefing, 고생 끝에 낙이 오다, 투자의견 Buy, 목표주가 20만원 제시, 20년도 하반기 이익모멘텀 발생 예상</t>
+  </si>
+  <si>
+    <t>"美 기술만족도 1 · 3위"...현대차 · 기아차 주가 '장중 껑충', EBITDAC을 보면 주가가 보인다, 매수의견 유지, 목표주가 상향, 기대 믹스 개선 효과는 21년 더 크다, 달라진 시장, 달라진 시각, 현대차그룹, 보통주 시가총액 90조 돌파...정의선 자사주 수익율 100% 넘어서, EBITDAC을 보면 주가가 보인다, 매수의견 유지, 목표주가 상향, 기대 믹스 개선 효과는 21년 더 크다, 달라진 시장, 달라진 시각</t>
+  </si>
+  <si>
+    <t>2021년 그린카 대격변의 시작, E-GMP 플랫폼 출시와 EV 속도전, 수소상용차 글로벌 출시 본격화, 목표주가 상향, 대전환기의 투자 기회, 2021년 그린카 대격변의 시작, E-GMP 플랫폼 출시와 EV 속도전, 수소상용차 글로벌 출시 본격화, 목표주가 상향, 대전환기의 투자 기회</t>
+  </si>
+  <si>
+    <t>이노션 주식 매수의견 유지, “현대차 제네시스 미국 광고수요 증가”, 최광욱 J&amp;J자산운용 대표 “주식시장, 역대급 유동성장 시작됐다”, 목표주가 상향, 아직 갈길이 멀다!, 목표주가 220,000원으로 상향, 미국시장 턴어라운드의 가시화 단계, 신차효과로 인해 지속적으로 놀라운 판매성과 달성 가능해짐, 변곡점에서 발견된 추세적 ASP 상승, 놀라운 원가율 개선에 투자하자, 목표주가 상향, 아직 갈길이 멀다!, 목표주가 220,000원으로 상향, 미국시장 턴어라운드의 가시화 단계, 신차효과로 인해 지속적으로 놀라운 판매성과 달성 가능해짐, 변곡점에서 발견된 추세적 ASP 상승, 놀라운 원가율 개선에 투자하자, 우리금융, 자본적정성 열위…주가 부양은 공염불?</t>
   </si>
   <si>
     <t>외통위 국회의원 김홍걸 '대북주' 억대 보유, 현대차에 달린 車업계 신용도…현대차 예의주시하는 신평사, 현대차 · 기아차, 장중 주가 '껑충'...증권계 "신차 효과 등 주목", 신주 상장 앞둔 현대로템, 주가하락 '어쩌나'</t>
@@ -6268,7 +6268,7 @@
     <t>'수소경제' 속도전 내는 한국 기업들</t>
   </si>
   <si>
-    <t>현대차-새로운 도약의 시작, 3분기 영업이익 1.02조원 (전년 대비 증감율 +169.8%, 전분기 대비 증감율 72.0%)을 전망, 최근 동사의 주가는 2분기 시장 기대치를 상회하는 호실적과 니콜라의 협업 희망 보도 발표 이후 급등. 그러나 현재의 주가는 내년 실적 개선의 범위에 있다는 판단, "투자 어렵다면 새내기주 주목"… 올해 신규상장株 크게 오르고 적게 빠졌다, 현대차-새로운 도약의 시작, 3분기 영업이익 1.02조원 (전년 대비 증감율 +169.8%, 전분기 대비 증감율 72.0%)을 전망, 최근 동사의 주가는 2분기 시장 기대치를 상회하는 호실적과 니콜라의 협업 희망 보도 발표 이후 급등. 그러나 현재의 주가는 내년 실적 개선의 범위에 있다는 판단, 현대차-새로운 시대의 시작/새로운 성장의 시작, Tesla가 주도하는 모빌리티 데이터 플랫폼 시대의 개막, Non-Tesla 연합의 ‘마지막 퍼즐’이 될 현대차, 새로운 성장을 시작하기 위한 삼박자 준비, 방탄소년단(BTS)과 '콜라보' 속...현대차 · 기아차, 장중 주가 '급등', 국내 기업 무장해제에 엘리엇·소버린이 웃는다, 현대차-2021년 그린카 대격변의 시작, E GMP 플랫폼 출시와 EV 속도전, 수소상용차 글로벌 출시 본격화, 대전환기의 투자 기회, 은성수 금융위원회 위원장, 현대차그룹, 우선주 포함 시가총액 100조 '돌파'...정의선 자사주 평가이익만 942억 원, 6개월 연속 번 '필승' 동학개미 외, 현대차-새로운 시대의 시작/새로운 성장의 시작, Tesla가 주도하는 모빌리티 데이터 플랫폼 시대의 개막, Non-Tesla 연합의 ‘마지막 퍼즐’이 될 현대차, 새로운 성장을 시작하기 위한 삼박자 준비, 현대모비스 주식 매수의견 유지, “친환경차부품회사로 전환 본격화"</t>
+    <t>새로운 도약의 시작, 3분기 영업이익 1.02조원 (전년 대비 증감율 +169.8%, 전분기 대비 증감율 72.0%)을 전망, 최근 동사의 주가는 2분기 시장 기대치를 상회하는 호실적과 니콜라의 협업 희망 보도 발표 이후 급등. 그러나 현재의 주가는 내년 실적 개선의 범위에 있다는 판단, "투자 어렵다면 새내기주 주목"… 올해 신규상장株 크게 오르고 적게 빠졌다, 새로운 도약의 시작, 3분기 영업이익 1.02조원 (전년 대비 증감율 +169.8%, 전분기 대비 증감율 72.0%)을 전망, 최근 동사의 주가는 2분기 시장 기대치를 상회하는 호실적과 니콜라의 협업 희망 보도 발표 이후 급등. 그러나 현재의 주가는 내년 실적 개선의 범위에 있다는 판단, 새로운 시대의 시작/새로운 성장의 시작, Tesla가 주도하는 모빌리티 데이터 플랫폼 시대의 개막, Non-Tesla 연합의 ‘마지막 퍼즐’이 될 현대차, 새로운 성장을 시작하기 위한 삼박자 준비, 방탄소년단(BTS)과 '콜라보' 속...현대차 · 기아차, 장중 주가 '급등', 국내 기업 무장해제에 엘리엇·소버린이 웃는다, 2021년 그린카 대격변의 시작, E GMP 플랫폼 출시와 EV 속도전, 수소상용차 글로벌 출시 본격화, 대전환기의 투자 기회, 은성수 금융위원회 위원장, 현대차그룹, 우선주 포함 시가총액 100조 '돌파'...정의선 자사주 평가이익만 942억 원, 6개월 연속 번 '필승' 동학개미 외, 새로운 시대의 시작/새로운 성장의 시작, Tesla가 주도하는 모빌리티 데이터 플랫폼 시대의 개막, Non-Tesla 연합의 ‘마지막 퍼즐’이 될 현대차, 새로운 성장을 시작하기 위한 삼박자 준비, 현대모비스 주식 매수의견 유지, “친환경차부품회사로 전환 본격화"</t>
   </si>
   <si>
     <t>1일 장마감 후 주요 종목 뉴스, 막 오른 정기국회, 금융 법안 향방에 촉각, 9월 1주 주요 제조업 전망, 2주년 맞는 현대차 정의선 체제, 소통 늘리고 미래 대비 투자도 '착착', 주식시장, 삼성·현대차·SK 지배구조 개편 초미 관심</t>
@@ -6289,7 +6289,7 @@
     <t>'BTS 키운' 방시혁, 따상시 주식 부호 톱5 '정몽구 제칠까', 코스피 상승에도…심해지는 펀드 양극화</t>
   </si>
   <si>
-    <t>현대차-글로벌 수요 회복과 그린카 모멘텀, 글로벌 수요 회복, 3 분기 실적 대폭 개선될 전망, 실적 개선과 그린카 모멘텀, 현대차 대신 GM, 니콜라 주식 11% 취득. 설계 및 생산부문 제휴, 현대차 부자(父子)의 선방…전체 주식판 흔들다, 현대제철 주식 매수의견 유지, "현대차에 강판 공급 4분기부터 늘어", 중간배당 지갑 닫은 기업… 삼성전자 빼면 5100억</t>
+    <t>글로벌 수요 회복과 그린카 모멘텀, 글로벌 수요 회복, 3 분기 실적 대폭 개선될 전망, 실적 개선과 그린카 모멘텀, 현대차 대신 GM, 니콜라 주식 11% 취득. 설계 및 생산부문 제휴, 현대차 부자(父子)의 선방…전체 주식판 흔들다, 현대제철 주식 매수의견 유지, "현대차에 강판 공급 4분기부터 늘어", 중간배당 지갑 닫은 기업… 삼성전자 빼면 5100억</t>
   </si>
   <si>
     <t>현대차 '그린 뉴딜' 기대감… 국민연금도 지분 확대, 현대차 그린뉴딜 기대감....국민연금 지분 확대</t>
@@ -6307,16 +6307,16 @@
     <t>공정거래법 전면개정에 재계 ‘엄살’…사익편취·공익법인 규제 ‘사각지대’ 여전</t>
   </si>
   <si>
-    <t>현대차-년도년도 2분기 3분기 Preview: 전년비 이익 대폭 개선, 년도년도 2분기 3분기 Preview: 전년비 대폭 개선, 기대치 상회, 글로벌 수요 회복 추세 지속, 미국 제네시스 출시 임박, 실적 개선세 지속, 최선호주 추천 유지, 현대차-눈앞으로 다가온 미국시장의 성공, 미국 시장 영업지표 현격한 개선, 이보다 좋기 힘들다, 미국 시장 반등 예상되는 가운데 대폭 감소한 Fleet 비중, 펠리세이드 효과 지속 + 10 월 제네시스 미국 투입 기대, 투자의견 Buy, 목표주가 220,000 원 유지. 자동차 업종 Top Pick, “테슬라 멈춰라”…전기차 판 ‘갤럭시 신화’ 쓰는 현대차, 증시 회복에도 ELS 발행 부진··· 연초 대비 3분의1로 '뚝' 外, 현대차 주식 매수의견 유지, “미국에 새 제네시스 내놔 수익성 좋아져”, 현대위아 주식 매수의견 유지, “전기차와 수소차부품 매출 확대 기대”, 다시 뛰는 삼성전자…電車군단이 움직인다, 니콜라 논란에…누가 울고 웃나</t>
+    <t>년도년도 2분기 3분기 Preview: 전년비 이익 대폭 개선, 년도년도 2분기 3분기 Preview: 전년비 대폭 개선, 기대치 상회, 글로벌 수요 회복 추세 지속, 미국 제네시스 출시 임박, 실적 개선세 지속, 최선호주 추천 유지, 눈앞으로 다가온 미국시장의 성공, 미국 시장 영업지표 현격한 개선, 이보다 좋기 힘들다, 미국 시장 반등 예상되는 가운데 대폭 감소한 Fleet 비중, 펠리세이드 효과 지속 + 10 월 제네시스 미국 투입 기대, 투자의견 Buy, 목표주가 220,000 원 유지. 자동차 업종 Top Pick, “테슬라 멈춰라”…전기차 판 ‘갤럭시 신화’ 쓰는 현대차, 증시 회복에도 ELS 발행 부진··· 연초 대비 3분의1로 '뚝' 外, 현대차 주식 매수의견 유지, “미국에 새 제네시스 내놔 수익성 좋아져”, 현대위아 주식 매수의견 유지, “전기차와 수소차부품 매출 확대 기대”, 다시 뛰는 삼성전자…電車군단이 움직인다, 니콜라 논란에…누가 울고 웃나</t>
   </si>
   <si>
     <t>'이해 충돌' 논란 부른 의원님들의 요상한 주식 투자, ‘광기’ 논쟁 치닫는 美 기술주… Fed 눈 감으면 얼마나 더 오를까, 테슬라 5.19% 상승 , 니콜라 10.20% 하락 출발 ... 뉴욕증시 나스닥, 다우존스, S&amp;P500 상승 출발, 비주력사업 과감히 청산… 미래차 올인하는 정의선, 범현대가 지분 정리하는 정의선…미래차 `올인`, 니콜라 '사기설'… 현대차, 수소트럭 경쟁력 부각되나</t>
   </si>
   <si>
-    <t>현대차-현대차 상용 수소차 설명회 내용 및 시사점, 수소차 생산목표: 2020년 1.1만대 → 2022년 4만대 → 2025년 13만대 → 2030년 50만대 (기존 목표와 동일), 2021~2022년: 유럽, 중국, 미국에서 본격적인 상용 수소차 사업 개시 기대, 케이피엠테크 휴머니젠 소식에 2거래일 연속 상한가, 텔콘RF제약도 급등, 장 초반 화이자 관련주 시선 집중, 압타머사이언스 상장 첫날 고전, 현대차-전기차는 승용차, 수소차는 트럭, 상용 수소 설명회 개최, Q&amp;A 주요 내용, 물 들어올 때 노 젓자, 현대차-당신이 알던 현대차가 아니다, 투자의견 매수 유지, 목표주가 23만원으로 10% 상향, 7월 유럽 전기차 점유율 11% 기록, 글로벌 점유율 9.6% 기록 (중국 제외), E-GMP 기반 Ioniq 5 히트 예상, 정의선 현대차 부회장의 미래차 선구안... ‘선택적 무한확장’, LG화학, 내일 '배터리 분사' 긴급이사회...소액주주 반발 우려, 대림산업에게 필요한 찬성표 ‘43.55%', 니콜라에 울고 웃는 한화·현대차… '수소차 사기논란' 일파만파, 니콜라 사기 논란, 톱3 쫓는 제이알투자운용, 해외 오피스 '선전'</t>
-  </si>
-  <si>
-    <t>배터리 떼어내는 LG화학, 주가는 이틀째 하락세, 현대차-빠지는 구석이 없다!, 양수겸장, 실적 up, 점유율 good, 밸류에이션 re-rating, 목표주가 220,000원으로 상향, 투자의견 매수 유지, 현대차-많은기대를한몸에, 의심의여지없는No.1 수소차Player, BEV 본게임은이제시작, 현대차-New economy beyond the vehicle, 에너지 전환과 자동차 패러다임 변화에 대응을 위해 신규 사업 확장이 가능한 가치 사슬을 구축 중. 에너지 전환국면에서 FCEV, BEV를 활용한 생태계 확장으로 새로운 사업 가치 반영될 전망, COVID 19로 인한 경영환경 악화에도 예상을 뛰어넘는 20년도 2분기 이익을 실현하며 20년도 하반기 볼륨 회복과 믹스 개선에 따른 손익 개선은 뚜렷해질 전망. 신규 사업에 대한 가치를 배재하고 기존 사업의 이익 개선만으로 현 주가대비 높은 주가 상승 여력 기대, ‘제2 테슬라’ 수소차 니콜라 사기 의혹… 현대차 ‘쾌청’, LG화학 배터리 부문 분사 소식에 개인투자자들 '원성', LG화학, 지금이 매수 기회?...'배터리 분사'에 엇갈린 시선, LG화학 배터리 부문 분사한다…'LG에너지솔루션' 출범, LG화학 배터리 승부수 '동상이몽' 왜?, 4가지 시나리오는?, 상장 앞둔 빅히트엔터테인먼트...BTS와 함께 롱런 가능한 3가지 이유</t>
+    <t>현대차 상용 수소차 설명회 내용 및 시사점, 수소차 생산목표: 2020년 1.1만대 → 2022년 4만대 → 2025년 13만대 → 2030년 50만대 (기존 목표와 동일), 2021~2022년: 유럽, 중국, 미국에서 본격적인 상용 수소차 사업 개시 기대, 케이피엠테크 휴머니젠 소식에 2거래일 연속 상한가, 텔콘RF제약도 급등, 장 초반 화이자 관련주 시선 집중, 압타머사이언스 상장 첫날 고전, 전기차는 승용차, 수소차는 트럭, 상용 수소 설명회 개최, Q&amp;A 주요 내용, 물 들어올 때 노 젓자, 당신이 알던 현대차가 아니다, 투자의견 매수 유지, 목표주가 23만원으로 10% 상향, 7월 유럽 전기차 점유율 11% 기록, 글로벌 점유율 9.6% 기록 (중국 제외), E-GMP 기반 Ioniq 5 히트 예상, 정의선 현대차 부회장의 미래차 선구안... ‘선택적 무한확장’, LG화학, 내일 '배터리 분사' 긴급이사회...소액주주 반발 우려, 대림산업에게 필요한 찬성표 ‘43.55%', 니콜라에 울고 웃는 한화·현대차… '수소차 사기논란' 일파만파, 니콜라 사기 논란, 톱3 쫓는 제이알투자운용, 해외 오피스 '선전'</t>
+  </si>
+  <si>
+    <t>배터리 떼어내는 LG화학, 주가는 이틀째 하락세, 빠지는 구석이 없다!, 양수겸장, 실적 up, 점유율 good, 밸류에이션 re-rating, 목표주가 220,000원으로 상향, 투자의견 매수 유지, 많은기대를한몸에, 의심의여지없는No.1 수소차Player, BEV 본게임은이제시작, New economy beyond the vehicle, 에너지 전환과 자동차 패러다임 변화에 대응을 위해 신규 사업 확장이 가능한 가치 사슬을 구축 중. 에너지 전환국면에서 FCEV, BEV를 활용한 생태계 확장으로 새로운 사업 가치 반영될 전망, COVID 19로 인한 경영환경 악화에도 예상을 뛰어넘는 20년도 2분기 이익을 실현하며 20년도 하반기 볼륨 회복과 믹스 개선에 따른 손익 개선은 뚜렷해질 전망. 신규 사업에 대한 가치를 배재하고 기존 사업의 이익 개선만으로 현 주가대비 높은 주가 상승 여력 기대, ‘제2 테슬라’ 수소차 니콜라 사기 의혹… 현대차 ‘쾌청’, LG화학 배터리 부문 분사 소식에 개인투자자들 '원성', LG화학, 지금이 매수 기회?...'배터리 분사'에 엇갈린 시선, LG화학 배터리 부문 분사한다…'LG에너지솔루션' 출범, LG화학 배터리 승부수 '동상이몽' 왜?, 4가지 시나리오는?, 상장 앞둔 빅히트엔터테인먼트...BTS와 함께 롱런 가능한 3가지 이유</t>
   </si>
   <si>
     <t>LG화학 ‘개미’ 반발에도 물적 분할…세계 1위 굳힌다, 현대차 임협, 우리사주 지급 확대시 기본급 동결 합의 가능성, "분할·합병 결사반대"...주총서 무산된 사례 살펴보니, 힘세진 개미…LG화학 배터리 분사 후폭풍, '개미 위력'에 놀란 대기업…주주소통·주가관리 '비상', 태슬라 주가 연 이틀 하락 ... 5일 하락+5일 상승+2일째 하락, 3일째 오늘은, 현대모비스, 지배구조 개선 목표 멀어지나</t>
@@ -6325,7 +6325,7 @@
     <t>한화그룹, 한화손보 매각나서나.. 합작 디지털손보 지분 사내계열사에 매각</t>
   </si>
   <si>
-    <t>현대차그룹, 28개월만에 시총 100조원 돌파, 反기업 법에 골병드는 삼성…삼성생명법이 뭐길래, 원·달러 환율 떨어져도 '수출株' 현대차 강세…대한항공은 약세, ①‘사면초가’ 지배구조 개편...정의선 중심 지배력이 낳은 욕심, 제2의 테슬라로 불리던 '니콜라' 창업자 사퇴로 주식 폭락 예상, '니콜라 쇼크' 한화솔루션, 7% '급락'...경영 3세 김동관 괜찮을까, LG화학의 승부수, 배터리 분사 결정, '슬롯 여유' 대우조선, 2년 뒤 수주대박 예고(9월21일), SK하이닉스 10대기업 중 올해 주가 가장 '부진'...현대차는 정의선 자사주 매입후 '훨훨', 글로벌 배터리 전쟁 앞둔 LG화학…개미는 아군이 아니다, 현대모비스 주식 매수의견 유지, "전동화사업 성장 잠재력 매우 높아", LG화학 배터리 사업 분사, 손해 아닌 중장기적 이익 낸다, 현대차-위기에 강했던 면모, 이제는 격차로 이어질 시점, 수익성 개선은 지속 중, 위기에 강했던 면모, 이제는 격차로 이어질 시점, 재계 오너일가 자사주 매입 효과 '기대이상'...기업가치 상승에 평가이익까지</t>
+    <t>현대차그룹, 28개월만에 시총 100조원 돌파, 反기업 법에 골병드는 삼성…삼성생명법이 뭐길래, 원·달러 환율 떨어져도 '수출株' 현대차 강세…대한항공은 약세, ①‘사면초가’ 지배구조 개편...정의선 중심 지배력이 낳은 욕심, 제2의 테슬라로 불리던 '니콜라' 창업자 사퇴로 주식 폭락 예상, '니콜라 쇼크' 한화솔루션, 7% '급락'...경영 3세 김동관 괜찮을까, LG화학의 승부수, 배터리 분사 결정, '슬롯 여유' 대우조선, 2년 뒤 수주대박 예고(9월21일), SK하이닉스 10대기업 중 올해 주가 가장 '부진'...현대차는 정의선 자사주 매입후 '훨훨', 글로벌 배터리 전쟁 앞둔 LG화학…개미는 아군이 아니다, 현대모비스 주식 매수의견 유지, "전동화사업 성장 잠재력 매우 높아", LG화학 배터리 사업 분사, 손해 아닌 중장기적 이익 낸다, 위기에 강했던 면모, 이제는 격차로 이어질 시점, 수익성 개선은 지속 중, 위기에 강했던 면모, 이제는 격차로 이어질 시점, 재계 오너일가 자사주 매입 효과 '기대이상'...기업가치 상승에 평가이익까지</t>
   </si>
   <si>
     <t>현대제철 주식 매수의견 유지, "자동차강판 판매 4분기부터 증가", 악사손보 발 뺀 신한금융…한화손보 노리나, 빅테크 주가, '특허'는 알고 있다, - 08:00, 니콜라 후폭풍에…관련주 한화·한화솔루션 이틀째 급락, 현대차그룹, 28개월만에 시총 100조 회복… “수소차 세계1위 기대”, 테슬라 이번에도 혁신할까…배터리데이 D-1, 니콜라 연이어 하락 출발 ... 나스닥과 S&amp;P500지수는 상승 출발</t>
@@ -6334,7 +6334,7 @@
     <t>현대차 노사, 코로나 위기에 임금동결, 니콜라 언덕에서 굴릴때…현대차 스위스 산길 오른다, 니콜라 쇼크에 동학·사학 개미 '동공 지진', 반년 전 대출받아 5억 현대차 주식 몰빵한 아빠의 9월 현재 통장잔고, GM·보쉬·월스트리트가 '사기의혹' 니콜라 감싸는 이유, 급등 아니면 급락…해외 신사업 투자에 '롤러코스터' 타는 대기업들, LG화학 진통 계속…물적분할 '무산' 가능성은?</t>
   </si>
   <si>
-    <t>이동걸 KDB산업은행 회장, LG화학 물적분할에 뿔난 개미들… 임시 주총 흔드나, 현대차-차세대 모빌리티 업체로서의 밸류, 신차사이클 황금기, 차세대 모빌리티 업체로서의 가능성, 현대차 투자의견 BUY(TP 25만원), 최선호주 제시, 한신공영, 지주사 기형적 지분구조에 2세 승계 '막막'</t>
+    <t>이동걸 KDB산업은행 회장, LG화학 물적분할에 뿔난 개미들… 임시 주총 흔드나, 차세대 모빌리티 업체로서의 밸류, 신차사이클 황금기, 차세대 모빌리티 업체로서의 가능성, 현대차 투자의견 BUY(TP 25만원), 최선호주 제시, 한신공영, 지주사 기형적 지분구조에 2세 승계 '막막'</t>
   </si>
   <si>
     <t>물산 자사주매각, KCC '전략적 투자' 기회, "이사회 경영, 새로운 지평 연 주주행동주의", 테슬라, 니콜라 등 ‘꿈을 파는 기업들’…서학개미들의 구세주 될까, 이낙연 더불어민주당 대표</t>
@@ -6415,7 +6415,7 @@
     <t>현대차 사원도 디즈니 팀장도 ‘싸스 비서’와 일한다, 가스공사 주식 매수의견 유지, "수소경제 관련 신사업의 전망 밝아", 상법·공정거래법 개정 신중하게 접근해야, 지배구조 개편 노린 엘리엇 등 '벌처펀드' 들어오나, BBIG(배터리·바이오·인터넷·게임) 시대와 기업규제 3법의 기묘한 동거, 이재용, 경영능력 본격 시험대 오르다, 재계 ‘상속ㆍ증여세 폭탄’ 초비상, 엔진충당금 쌓고도···현대차 3분기 선방·기아차 흑자</t>
   </si>
   <si>
-    <t>현대차-눈높이 더 올려도 됩니다, 20년도 3분기 , Big Surprise, 미스 개선에 물량을 더한다, 높아진 수익성에 적응 중, 현대차-눈높이를 확실히 올려줄 수 있는 실적, 20년도 3분기 영업이익 -3,138억원(전년 대비 증감율 적자전환) 기록. 기 발표된 품질비용 2.1조원이 반영되었음, 주요 지역 가동률의 빠른 정상화에 믹스개선 더해지며 실적 개선 속도가 예상보다 빠름, 현대차-믹스 향상이 가져온 구조적 이익 개선, 3분기 일회성 제외한 조정 영업이익은 서프라이즈, 4분기 신차 모멘텀 이어질 전망, 현대차-3Q 상회. 실적 개선과 Valuation 재평가가 진행될 전망, SUV/럭셔리 사이클 유지. 친환경 기대감은 추가 확대, 20년도 3분기 Review: 영업이익률 -1.1% 기록, 컨퍼런스 콜의 주요 내용: 중국시장 경쟁력 제고에 노력할 것, 현대차-충당금의 아픔은 잊어도 좋을 실적, 3분기 충당금 제외 영업이익 1.82조원, 2021년 연간 영업이익 7.14조원 전망, 현대차-20년도 3분기 Review: 대규모 충당금을 쌓을 만했던 실적, 판매감소를 상쇄한 믹스, 최소 21년도 하반기 까지는 편안해진 실적전망, 믹스향상과 금융부분이 이끈 서프라이즈, 현대차-선순환 돌입 - 원가개선과 금융부문 회복, 원가개선과 금융부문 회복에 주목, 현대차-상상 그 이상, 20년도 3분기 영업적자는 3,138억원(적전 전년 대비 증감율, OPM -1.1%) 기록, 컨센서스 큰 폭 상회, 2021년 상반기까지 신차 출시로 인해 믹스 개선과 점유율 상승, 플랫폼 통합에 따른 비용 절감으로 수익성이 지속 개선되며 주가 상승은 지속되고 Valuation 부담은 낮출 전망, 현대차- 실적 개선세 돌입을 알리는 신호탄, 년도년도 2분기 3분기 Review : 뚜렷한 펀더멘탈 개선, 투자의견 ‘Buy’, 목표주가 220,000원, "충당금 제외 땐 호실적"...현대차 · 기아차, '장중 주가 급등', '이재용 리더십' 시험대 올라… 사법리스크 등 과제 산적, 현대차-뚜렷한 펀더멘털 개선 입증, 총성은 울렸다, 현대차 20년도 3분기 Review: 일회성 제외시 영업이익 1.8조원 기록, 여전히 이익개선 Cycle 초입: 20년도 4분기 영업이익 1조 9,570원 전망, 투자의견 Buy 유지, 목표주가 240,000원으로 상향. 비중확대 시점, 코로나19 이후 산업구조 전환기 맞아 기간산업 → 전자 → 차·화·정 → BBIG 시대로?, 현대차-펀더멘탈 개선은 이제 시작, 여전히 매력적인 Valuation, 3분기 Review: 글로벌 가동률 회복, 판매믹스 개선 지속, 현대차-년도년도 2분기 3분기 Review: 리콜 쇼크를 넘어선 펀더멘탈 서프라이즈, 년도년도 2분기 3분기 Review: 믹스 개선, 중고차 잔가 상승으로 실적 서프라이즈 기록, 년도년도 2분기 4분기 Preview: 6년만의 영업이익 2조원 달성 전망, 예상보다 강한 이익 체력, 아직 보여줄 게 남았다, 현대차-품질 이슈만 없었다면 역사적인 3분기, 20년도 3분기 연결 매출 27,576 십억원(전년 대비 증감율+2.3%), OP -314십억원(전년 대비 증감율 적전, OPM -1.1%), 투자의견 유지, 목표주가 20만원으로 상향, 현대차-유효슈팅, 매출액 27.6조원(+2.3% 전년 대비 증감율), 영업이익 -3,138억원(적전), 지배순이익 -3,361억원(적전), 추정치를 초과한 7천억원은 어디서 나왔을까?, 훼손 요인은 일회성, 개선 요인은 지속성, 현대차-와우..., Facts: 조정영업이익 컨센서스 60% 상회, Action: 구조적 이익개선은 이제 시작, 목표주가 26만원으로 상향 조정, 현대차-계속 좋아진다, 20년도 3분기 조정 영업이익 1.8조원(+381.2%)으로 추정치 대폭 상회, 20년도 4분기 영업이익 1.7조원(+42.3%)으로 상향 조정, 목표주가 23만원(+15%)으로 상향, 투자의견 매수 유지</t>
+    <t>눈높이 더 올려도 됩니다, 20년도 3분기 , Big Surprise, 미스 개선에 물량을 더한다, 높아진 수익성에 적응 중, 눈높이를 확실히 올려줄 수 있는 실적, 20년도 3분기 영업이익 -3,138억원(전년 대비 증감율 적자전환) 기록. 기 발표된 품질비용 2.1조원이 반영되었음, 주요 지역 가동률의 빠른 정상화에 믹스개선 더해지며 실적 개선 속도가 예상보다 빠름, 믹스 향상이 가져온 구조적 이익 개선, 3분기 일회성 제외한 조정 영업이익은 서프라이즈, 4분기 신차 모멘텀 이어질 전망, 3Q 상회. 실적 개선과 Valuation 재평가가 진행될 전망, SUV/럭셔리 사이클 유지. 친환경 기대감은 추가 확대, 20년도 3분기 Review: 영업이익률 -1.1% 기록, 컨퍼런스 콜의 주요 내용: 중국시장 경쟁력 제고에 노력할 것, 충당금의 아픔은 잊어도 좋을 실적, 3분기 충당금 제외 영업이익 1.82조원, 2021년 연간 영업이익 7.14조원 전망, 20년도 3분기 Review: 대규모 충당금을 쌓을 만했던 실적, 판매감소를 상쇄한 믹스, 최소 21년도 하반기 까지는 편안해진 실적전망, 믹스향상과 금융부분이 이끈 서프라이즈, 선순환 돌입 - 원가개선과 금융부문 회복, 원가개선과 금융부문 회복에 주목, 상상 그 이상, 20년도 3분기 영업적자는 3,138억원(적전 전년 대비 증감율, OPM -1.1%) 기록, 컨센서스 큰 폭 상회, 2021년 상반기까지 신차 출시로 인해 믹스 개선과 점유율 상승, 플랫폼 통합에 따른 비용 절감으로 수익성이 지속 개선되며 주가 상승은 지속되고 Valuation 부담은 낮출 전망, 실적 개선세 돌입을 알리는 신호탄, 년도년도 2분기 3분기 Review : 뚜렷한 펀더멘탈 개선, 투자의견 ‘Buy’, 목표주가 220,000원, "충당금 제외 땐 호실적"...현대차 · 기아차, '장중 주가 급등', '이재용 리더십' 시험대 올라… 사법리스크 등 과제 산적, 뚜렷한 펀더멘털 개선 입증, 총성은 울렸다, 현대차 20년도 3분기 Review: 일회성 제외시 영업이익 1.8조원 기록, 여전히 이익개선 Cycle 초입: 20년도 4분기 영업이익 1조 9,570원 전망, 투자의견 Buy 유지, 목표주가 240,000원으로 상향. 비중확대 시점, 코로나19 이후 산업구조 전환기 맞아 기간산업 → 전자 → 차·화·정 → BBIG 시대로?, 펀더멘탈 개선은 이제 시작, 여전히 매력적인 Valuation, 3분기 Review: 글로벌 가동률 회복, 판매믹스 개선 지속, 년도년도 2분기 3분기 Review: 리콜 쇼크를 넘어선 펀더멘탈 서프라이즈, 년도년도 2분기 3분기 Review: 믹스 개선, 중고차 잔가 상승으로 실적 서프라이즈 기록, 년도년도 2분기 4분기 Preview: 6년만의 영업이익 2조원 달성 전망, 예상보다 강한 이익 체력, 아직 보여줄 게 남았다, 품질 이슈만 없었다면 역사적인 3분기, 20년도 3분기 연결 매출 27,576 십억원(전년 대비 증감율+2.3%), OP -314십억원(전년 대비 증감율 적전, OPM -1.1%), 투자의견 유지, 목표주가 20만원으로 상향, 유효슈팅, 매출액 27.6조원(+2.3% 전년 대비 증감율), 영업이익 -3,138억원(적전), 지배순이익 -3,361억원(적전), 추정치를 초과한 7천억원은 어디서 나왔을까?, 훼손 요인은 일회성, 개선 요인은 지속성, 와우..., Facts: 조정영업이익 컨센서스 60% 상회, Action: 구조적 이익개선은 이제 시작, 목표주가 26만원으로 상향 조정, 계속 좋아진다, 20년도 3분기 조정 영업이익 1.8조원(+381.2%)으로 추정치 대폭 상회, 20년도 4분기 영업이익 1.7조원(+42.3%)으로 상향 조정, 목표주가 23만원(+15%)으로 상향, 투자의견 매수 유지</t>
   </si>
   <si>
     <t>국민연금, LG화학 분할 반대..."신산업까지 발목" 재계 반발, 동학개미들 '삼성'에 몰렸다…빚내 '영끌' 투자도 크게 늘어, LG화학의 물적분할 논란, '갈지자 행보' 코스피…증권가 "美 대선 끝나야 방향성 잡힐 것"</t>
@@ -6451,10 +6451,10 @@
     <t>(3) 앉아서 연 5배 성장, 재벌의 기괴한 꼼수 ‘사익편취’란?</t>
   </si>
   <si>
-    <t>바이든 시대, 주식시장 수혜주 Top Pick①-친환경주, 씨티그룹 "바이든시대 한국 4종목 추천...삼성·현대차·LG화학·NC소프트", 씨티가 꼽은 바이든 시대 한국 주식···삼성·현대차·NC소프트, 매경이 전하는 세상의 지식 (매-세-지, 11월 11일), 현대차-2021년 전망: 편안한 실적, 승부처는 G2시장, 2021년 실적은 걱정 없다, 답답한 주가, 돌파구는?, 현대차-자율주행 시대의 변곡점에 서다, 현대차는 현재 Level 2.5 수준의 자율주행 차량을 공급하고 있으며, 향후 Level 4+ 시대 준비하기 위한 그룹 내 자율주행 연구 방향성은 1) 인공지능에 기반한 이미지 처리 기술과 2) 인공지능망 훈련 역량에 기반한 의사 결정 모델 개발에 집중 되어야 할 것으로 판단. Motional 및 기타 업체들과의 협업 체제 구축을 통한 역량 강화를 기대하며, 2022년 로보택시 출시 이후 자율주행 역량 재평가를 기대, 자율주행 시대의 가속화를 위해 OTA(Over-the-air) 기능이 필수적이라는 생각이며, 향후 기능 완성도는 동사 기업 가치 재평가의 변곡점으로 작용할 전망. OTA는 요식적 기술의 의미가 아닌, ECU -&gt; 액츄에이터 -&gt; 구동으로 이어지는 자동차 작동의 메커니즘을 재정의. 현대차는 그룹사 OTA 기술 개발을 주도하고 있으며, 2021년 출시 예정인 아이오닉 5에 AVNT(오디오, 비디오, 내비게이션, 텔레매틱스) OTA를, 22년 출시 예정인 아이오닉 6에 제어 OTA를 제공할 것으로 예상, 테슬라 등 일부 업체를 제외한 글로벌 완성차 제조사 중 자율주행, OTA, 전동화 등의 기술에 대한 가장 빠른 타임라인을 제시하고 있는 현대차에 대한 관심을 환기</t>
-  </si>
-  <si>
-    <t>연말 실패하지 않는 배당주 공략법은?, 현대차-E-GMP로 전기차 판매증가와 함께 미래 대응력도 향상, 실적 개선과 Valuation 재평가 전망, 전기차 판매는 2021년 +45%, 향후 6년 평균 29% 증가, 자동차 개념변화 흐름 속에서의 대응력도 향상 중</t>
+    <t>바이든 시대, 주식시장 수혜주 Top Pick①-친환경주, 씨티그룹 "바이든시대 한국 4종목 추천...삼성·현대차·LG화학·NC소프트", 씨티가 꼽은 바이든 시대 한국 주식···삼성·현대차·NC소프트, 매경이 전하는 세상의 지식 (매-세-지, 11월 11일), 2021년 전망: 편안한 실적, 승부처는 G2시장, 2021년 실적은 걱정 없다, 답답한 주가, 돌파구는?, 자율주행 시대의 변곡점에 서다, 현대차는 현재 Level 2.5 수준의 자율주행 차량을 공급하고 있으며, 향후 Level 4+ 시대 준비하기 위한 그룹 내 자율주행 연구 방향성은 1) 인공지능에 기반한 이미지 처리 기술과 2) 인공지능망 훈련 역량에 기반한 의사 결정 모델 개발에 집중 되어야 할 것으로 판단. Motional 및 기타 업체들과의 협업 체제 구축을 통한 역량 강화를 기대하며, 2022년 로보택시 출시 이후 자율주행 역량 재평가를 기대, 자율주행 시대의 가속화를 위해 OTA(Over-the-air) 기능이 필수적이라는 생각이며, 향후 기능 완성도는 동사 기업 가치 재평가의 변곡점으로 작용할 전망. OTA는 요식적 기술의 의미가 아닌, ECU -&gt; 액츄에이터 -&gt; 구동으로 이어지는 자동차 작동의 메커니즘을 재정의. 현대차는 그룹사 OTA 기술 개발을 주도하고 있으며, 2021년 출시 예정인 아이오닉 5에 AVNT(오디오, 비디오, 내비게이션, 텔레매틱스) OTA를, 22년 출시 예정인 아이오닉 6에 제어 OTA를 제공할 것으로 예상, 테슬라 등 일부 업체를 제외한 글로벌 완성차 제조사 중 자율주행, OTA, 전동화 등의 기술에 대한 가장 빠른 타임라인을 제시하고 있는 현대차에 대한 관심을 환기</t>
+  </si>
+  <si>
+    <t>연말 실패하지 않는 배당주 공략법은?, E-GMP로 전기차 판매증가와 함께 미래 대응력도 향상, 실적 개선과 Valuation 재평가 전망, 전기차 판매는 2021년 +45%, 향후 6년 평균 29% 증가, 자동차 개념변화 흐름 속에서의 대응력도 향상 중</t>
   </si>
   <si>
     <t>美 '더블딥' 우려에…월가 "한국 주식 사라", 최준영 기아자동차 대표이사, 정의선, 홍라희 제치고 주식부호 5위 됐다, "현대차 중고차 진출? 글로비스 일감몰아주기 우려", 홍라희 제치고…정의선 주식부호 5위, 현대차株 강세…정의선, 주식재산 5위로</t>
@@ -6466,10 +6466,10 @@
     <t>실적 악화에 배당 여력 '뚝'…'배당컷' 고민에 빠진 기업, '핫 뜨거' LG화학 배터리…’충당금은 싫어요’, 현대글로비스, 지배구조·신사업 기대감에 주가 널뛰기, 위기 극복 '큰 손' 손정의, 투자전략 대전환 나섰다, 친환경 열풍에 바이든 효과… 전기차 관련株 ‘날개’ 달았다</t>
   </si>
   <si>
-    <t>현대차-2021년 키워드는 미래차 기술 혁신, 미래차 기술 혁신 본격화, 2021년 수익성 개선 지속, 목표주가 상향, 현대오토에버 '3박자 호재'…사상 최고가 눈앞, 현대차-고지가 많이 남았다, COVID-19 국면에서 경쟁사와 달리 신차 및 xEV 전략을 공격적으로 지속 추진하고 있어 2021-2023년 시장 변화에 탄력적인 대응과 적응이 기대, 주가는 일회성 비용 이슈에도 Fundamentals 개선이 예상보다 빠름을 재차 확인하며 견조한 흐름을 이어갈 전망</t>
-  </si>
-  <si>
-    <t>현대차-모빌리티 디바이스 구축의 중심, 그룹 모빌리티 투자의 중심, ‘이동 수단’에서 ‘데이터 디바이스’로의 전환 선도, 성공적 P-Cycle 진행 및 기아차 실적 개선 수혜 통해, 21년 영업이익 +154% 전망, 투자의견 Buy 유지, 적정주가 250,000원으로 상향, 현대차-기회의 2021 년, 내년 이익 모멘텀 기대, 제네시스와 EV 판매 호조 시 Valuation 재평가 흐름 나타날 것, 컨트롤타워 사라지면…급변하는 미래 어떻게 대응하나</t>
+    <t>2021년 키워드는 미래차 기술 혁신, 미래차 기술 혁신 본격화, 2021년 수익성 개선 지속, 목표주가 상향, 현대오토에버 '3박자 호재'…사상 최고가 눈앞, 고지가 많이 남았다, COVID-19 국면에서 경쟁사와 달리 신차 및 xEV 전략을 공격적으로 지속 추진하고 있어 2021-2023년 시장 변화에 탄력적인 대응과 적응이 기대, 주가는 일회성 비용 이슈에도 Fundamentals 개선이 예상보다 빠름을 재차 확인하며 견조한 흐름을 이어갈 전망</t>
+  </si>
+  <si>
+    <t>모빌리티 디바이스 구축의 중심, 그룹 모빌리티 투자의 중심, ‘이동 수단’에서 ‘데이터 디바이스’로의 전환 선도, 성공적 P-Cycle 진행 및 기아차 실적 개선 수혜 통해, 21년 영업이익 +154% 전망, 투자의견 Buy 유지, 적정주가 250,000원으로 상향, 기회의 2021 년, 내년 이익 모멘텀 기대, 제네시스와 EV 판매 호조 시 Valuation 재평가 흐름 나타날 것, 컨트롤타워 사라지면…급변하는 미래 어떻게 대응하나</t>
   </si>
   <si>
     <t>"삼성·현대차·SK, 지배구조 개편…시총 600조가 움직인다", 왜 `기업규제 3법`인가…핵심 쟁점 4가지, 왜 `공정경제`라 쓰고 `기업규제`로 읽는가?</t>
@@ -6481,7 +6481,7 @@
     <t>美 테슬라 주가 '하락'에도...LG화학 · 삼성SDI · SK이노베이션은 '장중 강세', 서학개미가 달라졌다…中·日 종목도 '베팅', 한진칼 "KCGI 임시주총 요구 졸속"…가처분소송은 이번주 결론</t>
   </si>
   <si>
-    <t>현대차-대표 세단, SUV 모델과 GENESIS의 해외 출시, 2020년 매출 114조원, 영업이익 7.1조원 (OPM 6.2% 전망), 투자의견 매수 유지, 목표주가 22만원 상향, 24일 장 마감 후 주요 종목뉴스</t>
+    <t>대표 세단, SUV 모델과 GENESIS의 해외 출시, 2020년 매출 114조원, 영업이익 7.1조원 (OPM 6.2% 전망), 투자의견 매수 유지, 목표주가 22만원 상향, 24일 장 마감 후 주요 종목뉴스</t>
   </si>
   <si>
     <t>24일 장 마감 후 주요 종목뉴스</t>
@@ -6493,7 +6493,7 @@
     <t>시총 불어난 10대 그룹…고평가 1위는 삼성, 저평가 1위는?, 현대모비스, 보유 상장 4개사 지분 가치 8조9천억원 넘어</t>
   </si>
   <si>
-    <t>현대위아 주가 상승 예상, “자동차부품 중심 내년 실적개선 본격화”, 현대차-Mix에 Q 더하기, 20년도 4분기 , in-line 전망, 21년 물량 개선 효과 +2.4조원 전망, 여전히 밸류에이션 저평가</t>
+    <t>현대위아 주가 상승 예상, “자동차부품 중심 내년 실적개선 본격화”, Mix에 Q 더하기, 20년도 4분기 , in-line 전망, 21년 물량 개선 효과 +2.4조원 전망, 여전히 밸류에이션 저평가</t>
   </si>
   <si>
     <t>카카오 '폭풍성장' 기획자 김범수 의장</t>
@@ -6514,16 +6514,16 @@
     <t>조지 소로스·워런 버핏의 '자기암시가설'로 본 한국 증시와 원·달러 환율 전망, 커피 한잔 값으로 `쿠팡` 건물주가 될 수 있다</t>
   </si>
   <si>
-    <t>현대차-현대차: 누가 비싸다는 소리를 내었는가, 제네시스 부활의 두번째 단추, GV70 공개, 글로벌 고급차 열풍에 편승, 제네시스의 현대차 내 이익 기여도 증가, 이건희 주식 연초보다 3조6천억 늘어…카카오 김범수 144％ 증가, 올해 주식재산 증가 1위 '故이건희'…상승률 최고 '김범수'</t>
-  </si>
-  <si>
-    <t>현대차-년도년도 2분기 4분기 Preview - 코로나19 재확산 영향 미미할 듯, 목표주가 250,000원 제시 (8.7% 상향) 투자의견 Buy 유지, 년도년도 2분기 4분기 예상 영업이익 1.9조원 (+58.9% 전년 대비 증감율), 시장 컨센서스 5.8% 상회 예상, 2021년 예상 영업이익 6.9조원 (+130.6% 전년 대비 증감율), 시장 컨센서스 1.7% 상회 전망, 투자포인트: ① 글로벌 자동차 시장 정상화 ② 모델 수익성 개선, ③ 전기차 전용플랫폼 출시, 현대차-누가 비싸다는 소리를 내었는가, 제네시스 부활의 두번째 단추, GV70 공개, 글로벌 고급차 열풍에 편승, 제네시스의 현대차 내 이익 기여도 증가, 거래소 서연이화 단기과열종목 지정, 에쓰씨엔지니어링은 기간 연장, 현대차 주식 매수의견 유지, “제네시스 호조로 내년 영업이익 급증”, '나 떨고 있니' 중기·중견, 기업규제 3법 상임위 통과에 패닉, 윤석열 관련주, 모베이스전자·서연·서연이화, 대권선호도 1위 소식에 급등, 2000만원으로 17억원을 벌었다… 소녀시대 덕분에 부자 된 남자팬의 사연, 이노션 주식 매수의견 유지, “현대차 기아차 마케팅 확대의 수혜”, 우버, 돈 안 되는 것은 다 판다…비행택시 사업부, 조비항공에 매각</t>
-  </si>
-  <si>
-    <t>현대글로비스 앞날 '캄캄'… 일감 40% 줄이거나 지분 10% 내놔야, 대기업, 사익편취 규제 강화 ‘전전긍긍’, 현대차-2020년 CEO Investor Day 내용 점검, 영업이익률 목표로 2021년 4~5%, 2022년 5.5%(하향), 2025년 8%(유지) 제시, 2022년 가이던스 하향은 산업수요 감소에 따른 자연스러운 결과, 목표주가 22만원 유지</t>
-  </si>
-  <si>
-    <t>HyundaiMtr-CEO Investor Day shows HMC fully prepared, 2021년, 2022년 가이던스 하향, 미래에 대한 준비: 전기차: 자율주행, 현대차-CEO Investor Day: 준비된 자, 2021년, 2022년 가이던스 하향, 미래에 대한 준비: 전기차: 자율주행, 현대차-CEO Investor Day 후기, 현대차, 투자자 대상 CEO Investor Day 진행, COVID-19 전후 글로벌 OEM의 경영전략이 후퇴하는 가운데 현대차그룹의 미래 전략의 속도와 방향성이 변하지 않음에 주목, 현대차-중장기 전략과 목표, 그리고 경쟁업체와 비교, 차량사업부 수익성 2022년 영업이익률 목표는 7%에서 5.5%로 하향. 그러나 2025 년 8% 유지, 중장기 Free Cash Flow 목표 하향, 전동화 전략 : 2025년 전기차 판매 56만대 기존과 동일 &amp; 2030년 전고체전지 전기차 양산, 현대차-현대차 2020 CEO Investor Day, 2021년 실적 전망(가이던스) 자동차 부문 OPM 4~5% 제시, 중장기 재무목표로 2020년~2025년 투자규모는 60.1조원으로 제시, 예상보다 낮은 가이던스 제시는 아쉬운 부분, 현대차-가슴이 웅장해지는 발표들, CEO Investor day 발표 주요 내용, 가이던스 하향 조정에 놀라지 말아야 하는 이유, 내주부터 '공포의 3% 룰' 적용… '세계 최고' 현대차 수소기술, 중국이 노린다, 금융당국 '배당 자제' 권고에 금융주 투자자 반발…국민청원도 등장, 지난주 전국 아파트값 8년7개월만에 최고상승, 기획 리포트 내고 인덱스 개발...‘ESG 바람’ 부는 여의도, 현대차 주식 매수의견 유지, "자율주행과 전기차의 방향성 명확해", "3%룰, 투기세력의 경영권 개입에 무방비··· 결국 기업 경쟁력 약화로"</t>
+    <t>현대차: 누가 비싸다는 소리를 내었는가, 제네시스 부활의 두번째 단추, GV70 공개, 글로벌 고급차 열풍에 편승, 제네시스의 현대차 내 이익 기여도 증가, 이건희 주식 연초보다 3조6천억 늘어…카카오 김범수 144％ 증가, 올해 주식재산 증가 1위 '故이건희'…상승률 최고 '김범수'</t>
+  </si>
+  <si>
+    <t>년도년도 2분기 4분기 Preview - 코로나19 재확산 영향 미미할 듯, 목표주가 250,000원 제시 (8.7% 상향) 투자의견 Buy 유지, 년도년도 2분기 4분기 예상 영업이익 1.9조원 (+58.9% 전년 대비 증감율), 시장 컨센서스 5.8% 상회 예상, 2021년 예상 영업이익 6.9조원 (+130.6% 전년 대비 증감율), 시장 컨센서스 1.7% 상회 전망, 투자포인트: ① 글로벌 자동차 시장 정상화 ② 모델 수익성 개선, ③ 전기차 전용플랫폼 출시, 누가 비싸다는 소리를 내었는가, 제네시스 부활의 두번째 단추, GV70 공개, 글로벌 고급차 열풍에 편승, 제네시스의 현대차 내 이익 기여도 증가, 거래소 서연이화 단기과열종목 지정, 에쓰씨엔지니어링은 기간 연장, 현대차 주식 매수의견 유지, “제네시스 호조로 내년 영업이익 급증”, '나 떨고 있니' 중기·중견, 기업규제 3법 상임위 통과에 패닉, 윤석열 관련주, 모베이스전자·서연·서연이화, 대권선호도 1위 소식에 급등, 2000만원으로 17억원을 벌었다… 소녀시대 덕분에 부자 된 남자팬의 사연, 이노션 주식 매수의견 유지, “현대차 기아차 마케팅 확대의 수혜”, 우버, 돈 안 되는 것은 다 판다…비행택시 사업부, 조비항공에 매각</t>
+  </si>
+  <si>
+    <t>현대글로비스 앞날 '캄캄'… 일감 40% 줄이거나 지분 10% 내놔야, 대기업, 사익편취 규제 강화 ‘전전긍긍’, 2020년 CEO Investor Day 내용 점검, 영업이익률 목표로 2021년 4~5%, 2022년 5.5%(하향), 2025년 8%(유지) 제시, 2022년 가이던스 하향은 산업수요 감소에 따른 자연스러운 결과, 목표주가 22만원 유지</t>
+  </si>
+  <si>
+    <t>HyundaiMtr-CEO Investor Day shows HMC fully prepared, 2021년, 2022년 가이던스 하향, 미래에 대한 준비: 전기차: 자율주행, CEO Investor Day: 준비된 자, 2021년, 2022년 가이던스 하향, 미래에 대한 준비: 전기차: 자율주행, CEO Investor Day 후기, 현대차, 투자자 대상 CEO Investor Day 진행, COVID-19 전후 글로벌 OEM의 경영전략이 후퇴하는 가운데 현대차그룹의 미래 전략의 속도와 방향성이 변하지 않음에 주목, 중장기 전략과 목표, 그리고 경쟁업체와 비교, 차량사업부 수익성 2022년 영업이익률 목표는 7%에서 5.5%로 하향. 그러나 2025 년 8% 유지, 중장기 Free Cash Flow 목표 하향, 전동화 전략 : 2025년 전기차 판매 56만대 기존과 동일 &amp; 2030년 전고체전지 전기차 양산, 현대차 2020 CEO Investor Day, 2021년 실적 전망(가이던스) 자동차 부문 OPM 4~5% 제시, 중장기 재무목표로 2020년~2025년 투자규모는 60.1조원으로 제시, 예상보다 낮은 가이던스 제시는 아쉬운 부분, 가슴이 웅장해지는 발표들, CEO Investor day 발표 주요 내용, 가이던스 하향 조정에 놀라지 말아야 하는 이유, 내주부터 '공포의 3% 룰' 적용… '세계 최고' 현대차 수소기술, 중국이 노린다, 금융당국 '배당 자제' 권고에 금융주 투자자 반발…국민청원도 등장, 지난주 전국 아파트값 8년7개월만에 최고상승, 기획 리포트 내고 인덱스 개발...‘ESG 바람’ 부는 여의도, 현대차 주식 매수의견 유지, "자율주행과 전기차의 방향성 명확해", "3%룰, 투기세력의 경영권 개입에 무방비··· 결국 기업 경쟁력 약화로"</t>
   </si>
   <si>
     <t>현대차 IT3사 합병, 현대엠엔소프트 소액주주들 반발 움직임, IPO 열풍에 활짝 웃은 손정의···올 주가 66% 치솟아, 또 '정의선 vs 소액주주'...이번엔 현대엠엔소프트 합병비율①</t>
@@ -6580,7 +6580,7 @@
     <t>쌍용차 투자처 "인수 의사 변함없다"·'한국판 라스베이거스' 영종도 복합카지노리조트, 개장 연기(12월4주차), "차익 실현이냐" vs "비중 확대냐"…새해 고민 깊어진 개미들</t>
   </si>
   <si>
-    <t>새해 첫날 코스피 최고가 경신…현대위아 상한가·삼성전자 신고가, 대기업 시총 글로벌 기업과 격차 줄었다, SK이노베이션, 20%대 급등, 자사주 팔아 성과급 급증, 2차전지 붐…삼성SDI 4%대 상승, 정의선 현대자동차그룹 회장, 현대차-시장은 그 이상을 원한다, 내연기관에서의 승리는 뚜렷하나, 2021년은 그 이상을 원한다, 20년도 4분기 이익: 분명 높은 수준 예상, 그러나 차별화의 핵심은 아님, 투자의견 Buy 유지, 목표주가는 230,000원으로 하향조정, 현대글로비스 주식 매수의견 유지, "신사업 진출로 장기적 가치 상승", ‘역대급’ 주가 상승에…자사주 팔아 성과급 급증, 경영일선 물러났지만…존재감 여전한 주식부호 정몽구, "코스피 3000 넘는다"…2021년 주식시장도 전망 '맑음' 外, 현대차 급등 속 전기차·2차전지 관련주 무더기 급등, 녹십자 그룹주도 급등하며 코스피 6거래일 연속 상승, 한국 주식, 지금 투자하면 늦을까</t>
+    <t>새해 첫날 코스피 최고가 경신…현대위아 상한가·삼성전자 신고가, 대기업 시총 글로벌 기업과 격차 줄었다, SK이노베이션, 20%대 급등, 자사주 팔아 성과급 급증, 2차전지 붐…삼성SDI 4%대 상승, 정의선 현대자동차그룹 회장, 시장은 그 이상을 원한다, 내연기관에서의 승리는 뚜렷하나, 2021년은 그 이상을 원한다, 20년도 4분기 이익: 분명 높은 수준 예상, 그러나 차별화의 핵심은 아님, 투자의견 Buy 유지, 목표주가는 230,000원으로 하향조정, 현대글로비스 주식 매수의견 유지, "신사업 진출로 장기적 가치 상승", ‘역대급’ 주가 상승에…자사주 팔아 성과급 급증, 경영일선 물러났지만…존재감 여전한 주식부호 정몽구, "코스피 3000 넘는다"…2021년 주식시장도 전망 '맑음' 外, 현대차 급등 속 전기차·2차전지 관련주 무더기 급등, 녹십자 그룹주도 급등하며 코스피 6거래일 연속 상승, 한국 주식, 지금 투자하면 늦을까</t>
   </si>
   <si>
     <t>누구나 `미래車 주식` 하나쯤은 있잖아요, 김승연 한화그룹 회장, 현대글로비스, 4분기 영업이익 전망치 하회 예상-대신</t>
@@ -6595,19 +6595,19 @@
     <t>현대차, 애플과 손잡고 미래차 판도 흔들까… 협력설에 주가 급등, 현대차 "애플과 전기차 협력논의중"...정의선 지분 4兆↑, 코스피 '외국인 매수'에 3%대 뛰어 3150 돌파, 코스닥 약간 밀려, 亞증시서 독주하는 코스피, 3150마저 돌파(종합), 애플과의 협력설에 정의선 회장 주식가치 4조원 돌파, "협력 초기단계"… 현대차-애플 맞손 가능성에 기대감↑, 급등 뒤엔 조정? 대형주는 상승 제한?…상식이 깨졌다, 현대차·애플 협력설에 정의선 회장 주식 가치 4조원 넘어, 애플發 자율차 희소식에…현대차·모비스 20%대 급등, 새해벽두부터 힘 받는 현대차 정의선의 전기수소차 비전, 현대위아 유니온커뮤니티 주식 단기과열종목 지정, 사흘 단일가 매매, '파죽지세' 코스피, 4% 폭등…3150선도 뚫었다, '애플 협력설' 현대차 정의선 회장 주식가치 4조 돌파, 애플의 자율주행차 '애플카',현대차에 손짓, 애플카 협업설에 정의선 회장 주식 가치 하루만에 3,000억 급증···4조원 돌파, "애플 고마워!" 정몽구·정의선 부자, 하루 새 자산 '2.2조원' 증가, 애플카 협력 기대감에…정의선 회장 주식가치 4조원 돌파, 현대차가 애플과 손잡고 '전기차' 만든다는 소식에 폭등한 오늘자 주식 상황, 머스크, 베이조스 제치고 세계 최고 부자 “얼마나 낯선지, 일하자”, '테크노믹스 시대의 부의 지도' 박상현·고태봉 저자, 전기차 타고 씽씽 주가 그 속살은?, 현대차 수소사업,현대글로비스에 관심 갖는 이유, 현대차, ‘애플카’ 수주 소식에 주가 급등… 회사는 “협의 진행 중“, 현대차가 애플카 만든다고?.."사실무근" 선 그었지만 부담스런 호기심, 현대차, '애플카' 만든다…모비스·위아·만도 등 관련주 급등, 현대차, 애플과 손잡고 애플카 공동개발 기대감에 24만원 돌파, 현대모비스도 36만원 육박, 현대차, 시가총액 상위 5대 기업 '우뚝'...셀트리온·삼성SDI·네이버 한방에 '추월', 현대차와 애플의 시너지, 애플카 몇 년 후 출시될까?, 현대자동차 주가가 하루 만에 20% 넘게 폭등한 이유를 알아봤습니다, 현대차, 애플과 전기차 공동개발 추진… “협의 초기단계”, 현대차가 애플카 생산?…“초기단계 협의 중, 결정된 것 아냐”, 현대차 애플과 협력?···‘애플카’ 기대에 이목 집중, 현대차·애플 전기차 협력 소식에 시장 ‘들썩’</t>
   </si>
   <si>
-    <t>팬덤 거느린 ‘테슬라’의 힘과 ‘애플’까지 가세하는 차 산업 [김도형 기자의 휴일차(車)담], 주식 투자자들이 오는 3월부터 역대급 '대폭락장'이라 예상하는 이유, 정의선 회장 '애플카'에 표정 관리중..현대차 주식가치 급등 첫 4조 돌파, 고용 쇼크에도 부양 기대…3대 지수 '또' 최고치, 뉴욕증시, '블루웨이브' 이룬 민주당 대규모 추가부양책 기대감에 상승…테슬라 또 7%대 급등-애플 0.86% 상승, 현대차-애플 ‘달리는 IT기기’ 큰 그림… 전기차 혁명 가속화, 현대차 '애플카 제작' 따낼까…시너지 기대감 증폭</t>
+    <t>팬덤 거느린 ‘테슬라’의 힘과 ‘애플’까지 가세하는 차 산업 [김도형 기자의 휴일차(車)담], 주식 투자자들이 오는 3월부터 역대급 '대폭락장'이라 예상하는 이유, 정의선 회장 '애플카'에 표정 관리중..현대차 주식가치 급등 첫 4조 돌파, 고용 쇼크에도 부양 기대…3대 지수 '또' 최고치, 뉴욕증시, '블루웨이브' 이룬 민주당 대규모 추가부양책 기대감에 상승…테슬라 또 7%대 급등-애플 0.86% 상승, 애플 ‘달리는 IT기기’ 큰 그림… 전기차 혁명 가속화, 현대차 '애플카 제작' 따낼까…시너지 기대감 증폭</t>
   </si>
   <si>
     <t>'삼성SDI 배터리' 탑재 전기차, 中 보조금 혜택‧'코로나 백신 효과' 대한항공 북미 전노선 복원(1월1주차), 코스피 3100선 돌파 신기록…루비니 교수 “비트코인 거품 1월15일 터진다”, 韓경제 기지개…조선업 올해 영업익 320% 뛴다, 현대자동차, 애플과 전기차 생산협력 협의중</t>
   </si>
   <si>
-    <t>현대차-미래차 협업 가능성 반영해 목표가 상향, 목표주가 285,000원 제시 (14.0% 상향), 투자의견 Buy 유지, 20년도 4분기 예상 영업이익 1.7조원 (47.0% 전년 대비 증감율), 시장 컨센서스 1.0% 하회 예상, 2021년 예상 영업이익 5.9조원 (+107.0% 전년 대비 증감율), 시장 컨센서스 14.0% 하회 전망, 투자포인트: ① 글로벌 IT업체와의 협력, ② 양호한 완성차 판매 실적, ③ 성공적인 모델 교체에 따른 수익성 개선, 현대차-사과(Apple)하세요, 년도년도 2분기 4분기 영업이익은 1.68조원(+44.0% 전년 대비 증감율, OPM 5.8%)으로 컨센서스 3.6% 하회 전망. 원화 강세에도 내수 중심 강세, 주요 지역 수요 회복 등 볼륨 회복과 믹스 개선, 기말환율 하락에 따른 판매보증충당금 환입 등 실적 회복 지속하며 시장 예상치에 부합하는 실적 기록 전망, 전기차 선두권 진입, 경쟁력 있는 전용 플랫폼 기반 BEV 확대, 애플의 협업 요청 등 현대차의 시장대비 Valuation 할인 해소되며 적정 수준으로 회복 중. 안정적인 년도년도 2분기 4분기 실적과 E-GMP 신차 출시로 주가는 outperform 전망. 투자의견 BUY 유지, 목표주가 300,000원으로 20.0% 상향, 애플카 등에 업은 현대차, 지금 살까 말까?, “정의선 회장님, 누리꾼들은 애플카 하지 말라고 합니다.”, 애플, 현대차에 전기차 협업 러브콜…현대차 선택은?, "주식 안 하면 바보 된다"…전세금까지 베팅하는 개미들, 롤러코스터 코스피…하루 변동폭 170P, 애플·테슬라·넷플릭스…美빅테크와 눈만 마주쳐도 주가는 날아간다, 조정만 오면 사들일 기세? 박스피 탈출 후 눈 밝아진 개미, 로봇 업체 인수, 애플카 협상, 현대차 과감한 도전, 현대차의 '애플카' 고민 시작됐다…전문가 "소프트웨어 주도권이 열쇠", 블랙홀 ‘애플카’ 적신호, 최대 수혜주 현대모비스 ‘급락’하는 이유, '애플카' 호재에 치솟는 현대차그룹株… 증권가 적정주가는?, 현대차 · 기아차, '장중 또 급등'...증권계 "애플 협업 주목", 코스피 장중 3200돌파…삼성전자·현대차 어디까지 달릴까?, 현대차-현대차-애플 협력 가능성 보도 관련, “Apple Car, 현대차와 공동개발” 보도, 2020년 연말부터 또 다시 수면 위로 떠오르는 Apple Car, 현대차-애플, 애플카 생산 협력설…전 세계 車업계 촉각, 삼성전자 '9만원' LG화학 '100만원'…코스피 3200선도 뚫었다, “동학개미들, 좀비기업 부도 쓰나미에 희생될까 걱정”</t>
-  </si>
-  <si>
-    <t>애플카 등에 업은 현대차, '대박' 아닌 '독 사과' 일 수도..., ‘개미’ 우려에도 전문가는 “공매도 재개 적절”…무슨 이유?, "대박 나는 현대차株"…국민연금은 두달간 수천억 손실, 반포 삼성전자, 압구정 현대차…강남아파트 된 대표주들, "예정대로 공매도 재개"...논란·반발은 여전, 개인 vs 기관 역대급 공방…캐스팅보트 쥔 外人 ‘귀환 채비’, 애플카는 자동차 업체에 '독이 든 성배'…"현대차 주가 과열", 개인vs기관 역대급 공방…캐스팅보트 쥔 外人 향배는, 현대차-SK, 50조 수소경제 시장 '한판 붙는다', 코스피, 하루새 3266→3096→3148 널뛰기… 개미는 불안불안, '애플카 이슈' 현대차, 글로벌 완성차 시총 '톱5' 눈앞…GM 추월 가시권, 숏커버링이 올렸나…삼전 대차잔고 4분의 1토막, 삼성전자, 현대차…강남아파트된 대표주들</t>
-  </si>
-  <si>
-    <t>현대차-달라지는 위상, 달라질 valuation, 20년도 4분기 Preview - 지속되는 실적 선순환, 달라지는 위상, 달라질 valuation, 이재명 관련주 또 급등, 동방 3연속 상한가, 현대차 이슈 속 디아이씨 급등, SNK 급락, 공매도 재개 찬반 토론, 현대차-진화의 시작, 20년도 4분기 실적 Preview, 2021년 실적 턴어라운드의 첫 해, 투자의견 Buy, 목표주가 300,000원 제시, `수소·전기차 시대` 플러그파워株 올해 100%↑…월가 구루 "테슬라 부분 익절 필요", 현대차 '애플카 협력' 최선일까, 펀드매니저가 뽑은 최고의 애널리스트는 ②, 코스피 나는데… 왜 내가 산 중소형주는 파란색일까, 공매도 재개 찬반 토론</t>
+    <t>미래차 협업 가능성 반영해 목표가 상향, 목표주가 285,000원 제시 (14.0% 상향), 투자의견 Buy 유지, 20년도 4분기 예상 영업이익 1.7조원 (47.0% 전년 대비 증감율), 시장 컨센서스 1.0% 하회 예상, 2021년 예상 영업이익 5.9조원 (+107.0% 전년 대비 증감율), 시장 컨센서스 14.0% 하회 전망, 투자포인트: ① 글로벌 IT업체와의 협력, ② 양호한 완성차 판매 실적, ③ 성공적인 모델 교체에 따른 수익성 개선, 사과(Apple)하세요, 년도년도 2분기 4분기 영업이익은 1.68조원(+44.0% 전년 대비 증감율, OPM 5.8%)으로 컨센서스 3.6% 하회 전망. 원화 강세에도 내수 중심 강세, 주요 지역 수요 회복 등 볼륨 회복과 믹스 개선, 기말환율 하락에 따른 판매보증충당금 환입 등 실적 회복 지속하며 시장 예상치에 부합하는 실적 기록 전망, 전기차 선두권 진입, 경쟁력 있는 전용 플랫폼 기반 BEV 확대, 애플의 협업 요청 등 현대차의 시장대비 Valuation 할인 해소되며 적정 수준으로 회복 중. 안정적인 년도년도 2분기 4분기 실적과 E-GMP 신차 출시로 주가는 outperform 전망. 투자의견 BUY 유지, 목표주가 300,000원으로 20.0% 상향, 애플카 등에 업은 현대차, 지금 살까 말까?, “정의선 회장님, 누리꾼들은 애플카 하지 말라고 합니다.”, 애플, 현대차에 전기차 협업 러브콜…현대차 선택은?, "주식 안 하면 바보 된다"…전세금까지 베팅하는 개미들, 롤러코스터 코스피…하루 변동폭 170P, 애플·테슬라·넷플릭스…美빅테크와 눈만 마주쳐도 주가는 날아간다, 조정만 오면 사들일 기세? 박스피 탈출 후 눈 밝아진 개미, 로봇 업체 인수, 애플카 협상, 현대차 과감한 도전, 현대차의 '애플카' 고민 시작됐다…전문가 "소프트웨어 주도권이 열쇠", 블랙홀 ‘애플카’ 적신호, 최대 수혜주 현대모비스 ‘급락’하는 이유, '애플카' 호재에 치솟는 현대차그룹株… 증권가 적정주가는?, 현대차 · 기아차, '장중 또 급등'...증권계 "애플 협업 주목", 코스피 장중 3200돌파…삼성전자·현대차 어디까지 달릴까?, 현대차-애플 협력 가능성 보도 관련, “Apple Car, 현대차와 공동개발” 보도, 2020년 연말부터 또 다시 수면 위로 떠오르는 Apple Car, 현대차-애플, 애플카 생산 협력설…전 세계 車업계 촉각, 삼성전자 '9만원' LG화학 '100만원'…코스피 3200선도 뚫었다, “동학개미들, 좀비기업 부도 쓰나미에 희생될까 걱정”</t>
+  </si>
+  <si>
+    <t>애플카 등에 업은 현대차, '대박' 아닌 '독 사과' 일 수도..., ‘개미’ 우려에도 전문가는 “공매도 재개 적절”…무슨 이유?, "대박 나는 현대차株"…국민연금은 두달간 수천억 손실, 반포 삼성전자, 압구정 현대차…강남아파트 된 대표주들, "예정대로 공매도 재개"...논란·반발은 여전, 개인 vs 기관 역대급 공방…캐스팅보트 쥔 外人 ‘귀환 채비’, 애플카는 자동차 업체에 '독이 든 성배'…"현대차 주가 과열", 개인vs기관 역대급 공방…캐스팅보트 쥔 外人 향배는, SK, 50조 수소경제 시장 '한판 붙는다', 코스피, 하루새 3266→3096→3148 널뛰기… 개미는 불안불안, '애플카 이슈' 현대차, 글로벌 완성차 시총 '톱5' 눈앞…GM 추월 가시권, 숏커버링이 올렸나…삼전 대차잔고 4분의 1토막, 삼성전자, 현대차…강남아파트된 대표주들</t>
+  </si>
+  <si>
+    <t>달라지는 위상, 달라질 valuation, 20년도 4분기 Preview - 지속되는 실적 선순환, 달라지는 위상, 달라질 valuation, 이재명 관련주 또 급등, 동방 3연속 상한가, 현대차 이슈 속 디아이씨 급등, SNK 급락, 공매도 재개 찬반 토론, 진화의 시작, 20년도 4분기 실적 Preview, 2021년 실적 턴어라운드의 첫 해, 투자의견 Buy, 목표주가 300,000원 제시, `수소·전기차 시대` 플러그파워株 올해 100%↑…월가 구루 "테슬라 부분 익절 필요", 현대차 '애플카 협력' 최선일까, 펀드매니저가 뽑은 최고의 애널리스트는 ②, 코스피 나는데… 왜 내가 산 중소형주는 파란색일까, 공매도 재개 찬반 토론</t>
   </si>
   <si>
     <t>현대차그룹 질주…새해 시총 29조 증가, ‘혁신 본능’ 삼성전자, 완성차 없이 자동차 산업 강자 될까?, 한국투자증권, ELW 449종목 신규 상장, 질주하는 현대차그룹, 새해 시총 29조 증가, "주가급변 이유 없어" 황소장 불청객 뜬소문</t>
@@ -6622,16 +6622,16 @@
     <t>주식 투자, 조바심에 하는 건 금물, 기아차 새 로고 'ΚИ' 적용 스포티지 포착‧'SM 인수' 키이스트, 디즈니플러스·애플TV 콘텐츠 공급계약 논의(1월2주차), 한주간 코스피에 동학개미 뭉칫돈 10조 유입…三電이 절반, ②명품시계 매출 늘고수입차·대형가전도 잘팔려, 수십년 성공공식 버렸다… 시총 폭발한 4대그룹, 3월 '공매도 유령'이 돌아온다…OOOO 많은 종목 피하라, 당신이 사려는 그 주식, 그만한 기업가치가 있습니까 [코스피3000 개미의 시험대 (1)]</t>
   </si>
   <si>
-    <t>현대차-년도년도 2분기 4분기 Preview: 재평가 기대가 이어질망,년도 분기 년도년도 2분기 4분기 연결 매출액 28.1조원(전년 대비 증감율 +1.2%), 영업이익 1조 7,578억원(전년 대비 증감율 +51%)망,년도 분기 자동차 부문 매출액 22.5조원(전년 대비 증감율 +1.1%), 영업이익 1.3조원(OPM 6.0%) 예상. 년도년도 2분기 4분기 글로벌 도매판매량은 113.8만대로 전년 대비 증감율 4.8% 감소했으나 중국 제외시는 100만대로 전년 대비 증감율 1.1% 증가, 업종 top-pick 의견과 목표주가 32만원으로 상향. 32만원은 2021E PER 12 x에 해당하는데 과거 대비 분명 높은 수준의 valuation이지만 그 동안 Toyota가 받아왔던 premium을 감안할 필요. 다양한 업체로부터 전동화 및 자율주행차량 개발 협력 제안 등 현대차 경쟁력이 부각되고 있음. 21년도 2분기 부터 아이오닉5 판매를 통해 HW적으로 우수한 성능의 EV spec 증명될 전망이며 미래차 선두권 경쟁 업체로 인식되기 시작할 것, 매수매도 타이밍, 주식 목표가 설정하는 법, 기관·외국인처럼 개미에게도 공매도 문 연다는데…피해야 할 종목은?, “회장님은 투자의 귀재”… 정의선 매입 자사주 10개월 새 3배 껑충, 정의선, 작년 3월 코로나19 때 사들인 800억 주식 3배 급증, 아시아나항공 무상감자 착시효과 327%↑…한파 수혜 백광산업, 엄마ㆍ아빠가 용돈 대신 삼성ㆍ현대차 주식을 사줬다, 매수매도 타이밍, 주식 목표가 설정하는 법, 현대차 정의선 회장, 1년 안돼 주식 시세차익만 '1550억원'…투자 귀재?</t>
-  </si>
-  <si>
-    <t>현대차-전년비 이익 큰 폭 개선, 본 게임은 2021년, 20년도 4분기 Preview: 전년비 이익 대폭 개선, 2021년 실적 개선 기대해도 좋을 듯, 모빌리티 기업으로 변화 중, 최선호주 추천 유지, 비상장사 ‘일방통행’...대주주 횡포에 소액주주 속수무책, 현대車·모비스 주식 샀던 정의선 현대차그룹 회장, 1년 만에 대박, 한국경제 버팀목 삼성…이재용 부재에 국가경쟁력 흔들리나, 현대차그룹주 초강세, 기아차 16%대 뛰고 현대차 현대모비스 급등, “회장님 따라 샀어야”… 정의선 800억 주식 3배 뛰어, 애플카 생산설에 기아차 주가 8만원 돌파...9년만에 처음</t>
+    <t>년도년도 2분기 4분기 Preview: 재평가 기대가 이어질망,년도 분기 년도년도 2분기 4분기 연결 매출액 28.1조원(전년 대비 증감율 +1.2%), 영업이익 1조 7,578억원(전년 대비 증감율 +51%)망,년도 분기 자동차 부문 매출액 22.5조원(전년 대비 증감율 +1.1%), 영업이익 1.3조원(OPM 6.0%) 예상. 년도년도 2분기 4분기 글로벌 도매판매량은 113.8만대로 전년 대비 증감율 4.8% 감소했으나 중국 제외시는 100만대로 전년 대비 증감율 1.1% 증가, 업종 top-pick 의견과 목표주가 32만원으로 상향. 32만원은 2021E PER 12 x에 해당하는데 과거 대비 분명 높은 수준의 valuation이지만 그 동안 Toyota가 받아왔던 premium을 감안할 필요. 다양한 업체로부터 전동화 및 자율주행차량 개발 협력 제안 등 현대차 경쟁력이 부각되고 있음. 21년도 2분기 부터 아이오닉5 판매를 통해 HW적으로 우수한 성능의 EV spec 증명될 전망이며 미래차 선두권 경쟁 업체로 인식되기 시작할 것, 매수매도 타이밍, 주식 목표가 설정하는 법, 기관·외국인처럼 개미에게도 공매도 문 연다는데…피해야 할 종목은?, “회장님은 투자의 귀재”… 정의선 매입 자사주 10개월 새 3배 껑충, 정의선, 작년 3월 코로나19 때 사들인 800억 주식 3배 급증, 아시아나항공 무상감자 착시효과 327%↑…한파 수혜 백광산업, 엄마ㆍ아빠가 용돈 대신 삼성ㆍ현대차 주식을 사줬다, 매수매도 타이밍, 주식 목표가 설정하는 법, 현대차 정의선 회장, 1년 안돼 주식 시세차익만 '1550억원'…투자 귀재?</t>
+  </si>
+  <si>
+    <t>전년비 이익 큰 폭 개선, 본 게임은 2021년, 20년도 4분기 Preview: 전년비 이익 대폭 개선, 2021년 실적 개선 기대해도 좋을 듯, 모빌리티 기업으로 변화 중, 최선호주 추천 유지, 비상장사 ‘일방통행’...대주주 횡포에 소액주주 속수무책, 현대車·모비스 주식 샀던 정의선 현대차그룹 회장, 1년 만에 대박, 한국경제 버팀목 삼성…이재용 부재에 국가경쟁력 흔들리나, 현대차그룹주 초강세, 기아차 16%대 뛰고 현대차 현대모비스 급등, “회장님 따라 샀어야”… 정의선 800억 주식 3배 뛰어, 애플카 생산설에 기아차 주가 8만원 돌파...9년만에 처음</t>
   </si>
   <si>
     <t>"주식 투자 나처럼 해"...현대차그룹 정의선 회장, 자사주 수익률 200% 넘고 평가이익 2천억 원 근접, 선익시스템 아바코 세코닉스 단기과열종목 지정, 3거래일간 단일가, 기아, 애플카 생산說에 "결정된 바 없다" 선 긋기, 기아, 사명 바꾸고 애플카 생산설까지...모빌리티 중심 미래사업 '가속페달', 연기금, 올해 5조 넘게 순매도했지만…건설·금속株엔 베팅, 이노션 주식 매수의견 유지, "현대차 기아차 홍보활동 증가에 힘입어", 스스로 용돈 벌어 보려고 주식 투자해 750만원 번 초등학생 유튜버, 서학개미, 새해들어 2조 넘게 부었다…테슬라 등 전기차 '올인', 기아차 주가 급등 배경은? 전일대비 16.64% 상승, 삼성, 4주간 완전 경영 공백…다음은 경영권 승계 재판, 현대제철, 올해 실적 회복 전망에 목표가↑-NH, 현대위아 목표주가 높아져, "전기차부품 개발로 기업가치 재평가", 현대·기아차 “애플카? 결정된 것 없다”지만…눈에 띄는 포석깔기, 테슬라 효과, 애플카로 이어가나… 현대·기아 협력설에 관심 집중, 한국파마·필룩스가 수상하다…"바이오주 리스크 크다" 잇단 경고, ‘부나방’처럼 뛰어드는 개미들, “사실 아니다” 해명에도 주가 급등, “석탄발전소 짓는 한전에 네델란드 연기금 투자 철회, 국내 기업 변화해야”, 실적 액셀 밟는 현대차… 2021년 영업익 6조대 예상</t>
   </si>
   <si>
-    <t>이노션 주식 매수의견 유지, "현대차 기아차 마케팅 확대의 수혜 커져", 현대차-Fast Follower에서 Game Changer로 변모 시도, 자율주행, 전기차, 로봇틱스 등 다양한분야에서 글로벌 선두주자들과 협업을 통해 경쟁력을 끌어 올리는 중., 20년도 4분기 중국을 제외한 연결 대상 지역 글로벌 도매 판매는 전년 대비 증감율+0.8% 증가, 특히 ASP가 높은 내수 판매가 증가(전년 대비 증감율+5.0%)했고, 내수 판매 중 Genesis 비중은 33%를 기록하며(전년 대비 증감율+8%p) 믹스 개선을 견인. 이를 통해 Covid19 여파로 판매가 전년 대비 증감율-15% 감소한 유럽 부진 영향을 방어할 수 있을 것으로 판단, 부진 장기화 여파로 1공장 폐쇄에도 불구하고 2020년 동사의 중국 공장 가동률이 34%를 기록, 회장님의 통큰 자사주 베팅…시세 얼마나 뛰었나?, 정의선의 주식 신공…'800억을 2400억원으로', 폭락장서 자사주 산 상장사..주주신뢰·차익 '일석이조'</t>
+    <t>이노션 주식 매수의견 유지, "현대차 기아차 마케팅 확대의 수혜 커져", Fast Follower에서 Game Changer로 변모 시도, 자율주행, 전기차, 로봇틱스 등 다양한분야에서 글로벌 선두주자들과 협업을 통해 경쟁력을 끌어 올리는 중., 20년도 4분기 중국을 제외한 연결 대상 지역 글로벌 도매 판매는 전년 대비 증감율+0.8% 증가, 특히 ASP가 높은 내수 판매가 증가(전년 대비 증감율+5.0%)했고, 내수 판매 중 Genesis 비중은 33%를 기록하며(전년 대비 증감율+8%p) 믹스 개선을 견인. 이를 통해 Covid19 여파로 판매가 전년 대비 증감율-15% 감소한 유럽 부진 영향을 방어할 수 있을 것으로 판단, 부진 장기화 여파로 1공장 폐쇄에도 불구하고 2020년 동사의 중국 공장 가동률이 34%를 기록, 회장님의 통큰 자사주 베팅…시세 얼마나 뛰었나?, 정의선의 주식 신공…'800억을 2400억원으로', 폭락장서 자사주 산 상장사..주주신뢰·차익 '일석이조'</t>
   </si>
   <si>
     <t>현대차 신고가 경신하자…임원들 줄줄이 매도, “현대차 살 돈으로 현대차 주식 샀어야…”, 애플차 합작설에 현대차 19%↑... 뜬소문에 춤추는 한국 증시</t>
@@ -6646,10 +6646,10 @@
     <t>연초 부진한 바이오株, 'BBIG' 위상 지킬까, ‘애플카’ 소식 전후로 자사주 판 현대차 임원들, 현대車 컬래버 ‘사과 로고’ 전기차 나온다면?, 정의선 회장 따라 '자사주' 사들인 현대차 임원들… "수천만원 벌었다", 저평가된 자사주 매입한 현대車‥200억원 시세차익 ‘대박’, “현대차株 고점 찍었나”… 애플카 덕에 주가 오르자 주식 판 현대차 임원들, 코스피 ‘기관과 외국인 매수’에 3200 넘어서, 코스닥 1천 돌파 눈앞, 어닝시즌 본격화에 희비교차 커질 듯, 조성환 현대모비스 대표이사 사장 내정자</t>
   </si>
   <si>
-    <t>현대차-연간 가이던스 제시는 자신감의 표현, 20년도 4분기 실적은 컨센서스 부합, 처음으로 연간 가이던스 제시, 현대차-예상을 하회한 년도년도 2분기 4분기 영업이익과 공격적인 2021년 계획, 투자의견 Buy 유지. 목표주가 300,000원으로 5.3% 상향, 년도년도 2분기 4분기 영업이익 1.6조원 (+40.9% 전년 대비 증감율), 시장 기대 하회, 2021년 영업이익 5.9조원 (+111.3% 전년 대비 증감율) 예상. 현대차 연간 사업계획은 ASP 상승이 특징, 투자포인트: E-GMP 기반 전기차 출시, Genesis 라인업 확대, 글로벌 업체 협업, 현대차-무난했던 4분기. 3월 말로 모아지는 초점, 목표주가 30.5만원으로 상향, 20년도 4분기 실적: 영업이익률 5.6% 기록, 컨퍼런스콜의 주요 내용: 2021년 도매판매 416만대, 자동차 매출액 +14% 목표, 현대차-중요해질 아이오닉과 제네시스, 중요해질 아이오닉과 제네시스, 도대체 '애플카'가 뭐길래?!, 주가 폭등한 현대차·대한항공 임원들은 자사주 팔아치웠다, 코스피 하루 만에 3,200선 붕괴...외국인 올해 최대 순매도, 정의선 회장 따라 자사주 산 현대차 임원들… 1년 만에 '잭팟', 지분투자부터 지배구조개편까지···현대차그룹-애플의 ‘설설설’, 애플, 실적 기대감에 2.77% 급등, 한국카본 주식 매수의견 유지, "LNG 보냉재 수주 올해 급증 예상", 현대비앤지스틸 29.92% 상한가..현대차 관련주 "LG하우시스 사업부 인수", 공매도는 정말 주가 하락의 원흉일까, ESG, 수익률 파죽지세…유망 투자처는, 도대체 '애플카'가 뭐길래?!, 코스피 급락 속 반도체 주목 받아... SFA반도체·아이에이·프로텍 등 상한가 달성, "테슬라는 '일론 머스크 스토리' 주식"…WSJ에 실린 버블 경고, 시대를 앞선 ‘경제 구루’ 이건희의 선견지명</t>
-  </si>
-  <si>
-    <t>국민연금,작년 증시 활황덕 57兆 벌었다, 현대차-하회했지만 괜찮아, 당초 기대 대비 아쉽지만 여전히 좋은 실적, 이익이 계속 좋아지니 밸류에이션 부담이 올 틈이 없다, 현대차-매출은 부합했으나, 아직 아쉬운 수익성, 20년도 4분기 매출 29조원 (전년 대비 증감율+ 6%), 영업이익 1.6조원 (+40.9%, OPM 5.6%), 투자의견 매수, 목표주가 31만원 유지(2021년 PBR 1.1배), 현대차-년도년도 2분기 4분기 Review: 컨센서스 부합, 연초 신차 효과에 주목, 년도년도 2분기 4분기 Review: 컨센서스 부합, 연초 신차 효과에 주목, 실적의 구조적 개선 싸이클, 국민연금공단 지난해 국내 증시에서 57조6839억 벌었다, 국민연금, 증시호황에 지난해 투자기업 평가이익 58조원, "땡큐, 삼성전자"…국민연금, 작년 증시 호황에 수십조 벌었다, 국민연금 삼성전자로만 20조 벌어, "국민연금 보유 지분 1년 간 58조원↑···삼성전자만 20조", 삼성전자 덕 크게 본 국민연금...주식 투자로 20조원 벌었다!, 현대차-20년도 4분기 Review: 아쉬운 자동차부문 수익성, 금융부분 실적 증가, 아이오닉5 출시시기까지 모멘텀 소강국면 예상, 믹스향상에도 자동차부문 수익성 Flat전년 대비 증감율, 2021년, 416만대 판매목표(+11%전년 대비 증감율), 현대차-기대 이상의 ASP 목표에 주목!, 20년도 4분기 영업이익은 1.64조원(+40.9% 전년 대비 증감율, OPM 5.6%) 기록, 컨센서스 부합, ASP 상승에 따른 판매보증금 증가 추세는 실적 부담 요인이나 기대 이상의 ASP 상승에 따른 매출 증가로 믹스와 원가율 개선 뚜렷해질 전망, 현대차-무난한 연말정산, 20년도 4분기 Review : 실적 개선세 지속, 투자의견 ‘Buy’, 목표주가 30 0,000, 현대차-장기 지속 가능성에 대해 신뢰, 선순환 효과 및 성공적인 사업구조 전환 기대, 4분기 Review: 원가율 개선 Vs 판관비율 상승, 현대차-영업 실적 개선 방향성 확인, 20년도 4분기 Review: 영업 실적 개선 방향성 지속, 데이터 디바이스 제조능력 검증의 시험대가 될 21년, 현대차-년도년도 2분기 4분기 Review: 컨센서스 부합, 연초 신차 효과에 주목, 년도년도 2분기 4분기 Review: 컨센서스 부합, 연초 신차 효과에 주목, 실적의 구조적 개선 싸이클, 현대차-매출은 부합했으나, 아직 아쉬운 수익성, 20년도 4분기 매출 29조원 (전년 대비 증감율+ 6%), 영업이익 1.6조원 (+40.9%, OPM 5.6%), 투자의견 매수, 목표주가 31만원 유지(2021년 PBR 1.1배), 국민연금, 보유 지분가치 58조 늘었다···'효자'는 역시 삼성전자, 현대차-기업가치 재평가 구간 지속, 20년도 4분기 영업이익 1.64조원(+40.9%)으로 기대치 부합, 2021년도 브랜드 파워의 재평가, OP 7.0조원(+153.0%) 전망, "땡큐 삼성" 국민연금, 지난해 삼성전자로만 20조 '평가이익', 국민연금,주가 상승 평가이익 58조 육박 …"삼성전자 1등 공신", 국민연금, 주가 상승에 '대박'…58조원 벌었다, 국민연금, 삼성전자 주식으로만 20조 평가이익, 국민연금, 작년 증시 호황에 삼성전자로만 20조원 벌었다, 뉴욕증시 다우지수 덜커덩 FOMC 테이퍼링 긴축발작 경고, 국채금리 급등, 국민연금, 작년 증시 호황에 58조원 벌었다…삼성전자로만 20조원, 국민연금, 반도체株 호황에 삼성전자서만 지난해 20조 평가익, 국민연금 삼성전자로 20조 벌었다, 국민연금, 지난해 증시 호황에 58조 벌었다, 국민연금, 작년 주식 평가익 58조···삼성전자로만 20조 벌었다, 국민연금, 작년 증시 호황에 삼성전자로만 20조 평가이익, 국민연금, 지난해 주가상승으로 58조 벌어...CEO스코어, 국민연금, 보유지분 가치 58조원 늘어…삼성전자로만 20억 벌어들였다, 치열하게 살아온 불굴의 미래인, 손정의, 국민연금, 작년 증시 호황에 삼성전자로만 20조 원 평가익, 국민연금, 작년 증시 호황에 평가이익 58조원 육박...삼성전자로만 20조원 수익, 4분기 실적 발표 속...현대차 주가, '장중 하락', 국민연금, 지난해 증시 호황으로 58조원 평가익, 국민연금, 작년 증시 호황에 58조 원 벌었다....삼성전자로만 20조원 평가익, 국민연금, 투자기업 평가이익 1년새 58조원, 국민연금, '투자 효자' 삼성전자 때문에 싱글벙글, 국민연금, 작년 증시 활황으로 삼성전자에서만 20조원 벌었다, 국민연금, 반도체株 호황에 삼성전자서만 20조원 벌었다., "국민연금 보유 지분 1년 간 58조원↑…삼성전자만 20조", 국민연금, 국내 증시 호황에 ‘잭팟’..삼성전자서만 20조원 벌었다, 국민연금, 삼성전자 주식으로 지난해 20조원 수익, 국민연금 수익률 끌어올린 효자 종목은…삼성전자·LG화학, 국민연금, 증시 호황에 '싱글벙글'… 삼성전자로만 20조 벌었다, 국민연금, 지난해 주가상승으로 58조원 ↑…"삼성전자가 효자", 신사업 품는 총수 지배기업…회사 성장 따라 지배력도, 현대차-하회했지만 괜찮아, 당초 기대 대비 아쉽지만 여전히 좋은 실적, 이익이 계속 좋아지니 밸류에이션 부담이 올 틈이 없다, '삼전이 효자' 국민연금, 지난해 삼성전자로만 20조원 벌어, 국민연금, 작년 증시 호황에 삼성전자로만 20조원 벌어, 국민연금, 반도체株 호황에 삼성전자서만 20조 평가익, 국민연금, 작년 반도체株 호황에 삼성전자서만 20조원 벌었다, 테슬라 거품 곧 터진다, WSJ 버블붕괴 경고 …배터리 태양광 전기차 몰락</t>
+    <t>연간 가이던스 제시는 자신감의 표현, 20년도 4분기 실적은 컨센서스 부합, 처음으로 연간 가이던스 제시, 예상을 하회한 년도년도 2분기 4분기 영업이익과 공격적인 2021년 계획, 투자의견 Buy 유지. 목표주가 300,000원으로 5.3% 상향, 년도년도 2분기 4분기 영업이익 1.6조원 (+40.9% 전년 대비 증감율), 시장 기대 하회, 2021년 영업이익 5.9조원 (+111.3% 전년 대비 증감율) 예상. 현대차 연간 사업계획은 ASP 상승이 특징, 투자포인트: E-GMP 기반 전기차 출시, Genesis 라인업 확대, 글로벌 업체 협업, 무난했던 4분기. 3월 말로 모아지는 초점, 목표주가 30.5만원으로 상향, 20년도 4분기 실적: 영업이익률 5.6% 기록, 컨퍼런스콜의 주요 내용: 2021년 도매판매 416만대, 자동차 매출액 +14% 목표, 중요해질 아이오닉과 제네시스, 중요해질 아이오닉과 제네시스, 도대체 '애플카'가 뭐길래?!, 주가 폭등한 현대차·대한항공 임원들은 자사주 팔아치웠다, 코스피 하루 만에 3,200선 붕괴...외국인 올해 최대 순매도, 정의선 회장 따라 자사주 산 현대차 임원들… 1년 만에 '잭팟', 지분투자부터 지배구조개편까지···현대차그룹-애플의 ‘설설설’, 애플, 실적 기대감에 2.77% 급등, 한국카본 주식 매수의견 유지, "LNG 보냉재 수주 올해 급증 예상", 현대비앤지스틸 29.92% 상한가..현대차 관련주 "LG하우시스 사업부 인수", 공매도는 정말 주가 하락의 원흉일까, ESG, 수익률 파죽지세…유망 투자처는, 도대체 '애플카'가 뭐길래?!, 코스피 급락 속 반도체 주목 받아... SFA반도체·아이에이·프로텍 등 상한가 달성, "테슬라는 '일론 머스크 스토리' 주식"…WSJ에 실린 버블 경고, 시대를 앞선 ‘경제 구루’ 이건희의 선견지명</t>
+  </si>
+  <si>
+    <t>국민연금,작년 증시 활황덕 57兆 벌었다, 하회했지만 괜찮아, 당초 기대 대비 아쉽지만 여전히 좋은 실적, 이익이 계속 좋아지니 밸류에이션 부담이 올 틈이 없다, 매출은 부합했으나, 아직 아쉬운 수익성, 20년도 4분기 매출 29조원 (전년 대비 증감율+ 6%), 영업이익 1.6조원 (+40.9%, OPM 5.6%), 투자의견 매수, 목표주가 31만원 유지(2021년 PBR 1.1배), 년도년도 2분기 4분기 Review: 컨센서스 부합, 연초 신차 효과에 주목, 년도년도 2분기 4분기 Review: 컨센서스 부합, 연초 신차 효과에 주목, 실적의 구조적 개선 싸이클, 국민연금공단 지난해 국내 증시에서 57조6839억 벌었다, 국민연금, 증시호황에 지난해 투자기업 평가이익 58조원, "땡큐, 삼성전자"…국민연금, 작년 증시 호황에 수십조 벌었다, 국민연금 삼성전자로만 20조 벌어, "국민연금 보유 지분 1년 간 58조원↑···삼성전자만 20조", 삼성전자 덕 크게 본 국민연금...주식 투자로 20조원 벌었다!, 20년도 4분기 Review: 아쉬운 자동차부문 수익성, 금융부분 실적 증가, 아이오닉5 출시시기까지 모멘텀 소강국면 예상, 믹스향상에도 자동차부문 수익성 Flat전년 대비 증감율, 2021년, 416만대 판매목표(+11%전년 대비 증감율), 기대 이상의 ASP 목표에 주목!, 20년도 4분기 영업이익은 1.64조원(+40.9% 전년 대비 증감율, OPM 5.6%) 기록, 컨센서스 부합, ASP 상승에 따른 판매보증금 증가 추세는 실적 부담 요인이나 기대 이상의 ASP 상승에 따른 매출 증가로 믹스와 원가율 개선 뚜렷해질 전망, 무난한 연말정산, 20년도 4분기 Review : 실적 개선세 지속, 투자의견 ‘Buy’, 목표주가 30 0,000, 장기 지속 가능성에 대해 신뢰, 선순환 효과 및 성공적인 사업구조 전환 기대, 4분기 Review: 원가율 개선 Vs 판관비율 상승, 영업 실적 개선 방향성 확인, 20년도 4분기 Review: 영업 실적 개선 방향성 지속, 데이터 디바이스 제조능력 검증의 시험대가 될 21년, 년도년도 2분기 4분기 Review: 컨센서스 부합, 연초 신차 효과에 주목, 년도년도 2분기 4분기 Review: 컨센서스 부합, 연초 신차 효과에 주목, 실적의 구조적 개선 싸이클, 매출은 부합했으나, 아직 아쉬운 수익성, 20년도 4분기 매출 29조원 (전년 대비 증감율+ 6%), 영업이익 1.6조원 (+40.9%, OPM 5.6%), 투자의견 매수, 목표주가 31만원 유지(2021년 PBR 1.1배), 국민연금, 보유 지분가치 58조 늘었다···'효자'는 역시 삼성전자, 기업가치 재평가 구간 지속, 20년도 4분기 영업이익 1.64조원(+40.9%)으로 기대치 부합, 2021년도 브랜드 파워의 재평가, OP 7.0조원(+153.0%) 전망, "땡큐 삼성" 국민연금, 지난해 삼성전자로만 20조 '평가이익', 국민연금,주가 상승 평가이익 58조 육박 …"삼성전자 1등 공신", 국민연금, 주가 상승에 '대박'…58조원 벌었다, 국민연금, 삼성전자 주식으로만 20조 평가이익, 국민연금, 작년 증시 호황에 삼성전자로만 20조원 벌었다, 뉴욕증시 다우지수 덜커덩 FOMC 테이퍼링 긴축발작 경고, 국채금리 급등, 국민연금, 작년 증시 호황에 58조원 벌었다…삼성전자로만 20조원, 국민연금, 반도체株 호황에 삼성전자서만 지난해 20조 평가익, 국민연금 삼성전자로 20조 벌었다, 국민연금, 지난해 증시 호황에 58조 벌었다, 국민연금, 작년 주식 평가익 58조···삼성전자로만 20조 벌었다, 국민연금, 작년 증시 호황에 삼성전자로만 20조 평가이익, 국민연금, 지난해 주가상승으로 58조 벌어...CEO스코어, 국민연금, 보유지분 가치 58조원 늘어…삼성전자로만 20억 벌어들였다, 치열하게 살아온 불굴의 미래인, 손정의, 국민연금, 작년 증시 호황에 삼성전자로만 20조 원 평가익, 국민연금, 작년 증시 호황에 평가이익 58조원 육박...삼성전자로만 20조원 수익, 4분기 실적 발표 속...현대차 주가, '장중 하락', 국민연금, 지난해 증시 호황으로 58조원 평가익, 국민연금, 작년 증시 호황에 58조 원 벌었다....삼성전자로만 20조원 평가익, 국민연금, 투자기업 평가이익 1년새 58조원, 국민연금, '투자 효자' 삼성전자 때문에 싱글벙글, 국민연금, 작년 증시 활황으로 삼성전자에서만 20조원 벌었다, 국민연금, 반도체株 호황에 삼성전자서만 20조원 벌었다., "국민연금 보유 지분 1년 간 58조원↑…삼성전자만 20조", 국민연금, 국내 증시 호황에 ‘잭팟’..삼성전자서만 20조원 벌었다, 국민연금, 삼성전자 주식으로 지난해 20조원 수익, 국민연금 수익률 끌어올린 효자 종목은…삼성전자·LG화학, 국민연금, 증시 호황에 '싱글벙글'… 삼성전자로만 20조 벌었다, 국민연금, 지난해 주가상승으로 58조원 ↑…"삼성전자가 효자", 신사업 품는 총수 지배기업…회사 성장 따라 지배력도, 하회했지만 괜찮아, 당초 기대 대비 아쉽지만 여전히 좋은 실적, 이익이 계속 좋아지니 밸류에이션 부담이 올 틈이 없다, '삼전이 효자' 국민연금, 지난해 삼성전자로만 20조원 벌어, 국민연금, 작년 증시 호황에 삼성전자로만 20조원 벌어, 국민연금, 반도체株 호황에 삼성전자서만 20조 평가익, 국민연금, 작년 반도체株 호황에 삼성전자서만 20조원 벌었다, 테슬라 거품 곧 터진다, WSJ 버블붕괴 경고 …배터리 태양광 전기차 몰락</t>
   </si>
   <si>
     <t>국민연금, 증시 호황에 '잭팟' … 1년간 58조 벌었다, '고갈 위기' 국민연금, 삼성전자 주가 상승으로 작년에만 20조 벌었다, 전기차 늘면 온실가스 줄어들까?, 여당의 착각···원화는 '기축통화' 아니다, 국민연금, 지난해 지분가치 상승으로 평가이익 58조</t>
@@ -6664,10 +6664,10 @@
     <t>불확실성의 시대, R&amp;D가 미래다, 현대비앤지스틸, LG하우시스 車부품사업부 인수 전망에 74%↑…대한전선, 블록딜 여파에 23%↓</t>
   </si>
   <si>
-    <t>현대차-년도년도 2분기 4분기 NDR Review: High five, IONIQ 5!, 년도년도 2분기 4분기 영업이익은 1.64조원(+40.9% 전년 대비 증감율, OPM 5.6%) 기록, 컨센서스 부합, 판매보증비 증가하나 ASP, 믹스 개선에 기인하므로 수익성 훼손보다는 개선에 방점, 삼천피 무너진 증시…동학개미, 실적 받혀주는 업종 골라야, 현대차 주식 매수의견 유지, “전기차 판매비중 커져 수익성 좋아져, 깜짝실적 자동차주 배당 보따리 푼다</t>
-  </si>
-  <si>
-    <t>현대차-봐야할 모멘텀이 많다!, 20년도 4분기 매출액 29.2조원/영업이익 1.6조원, 2021년 매출액 117.7조원/영업이익 6.9조원 전망, 美부양책에 고배당… 주식, 아직 매력적, 현대글로비스, HMM 인수 '그때는 맞고 지금은 다르다', 현대위아 주식 매수의견 유지, “자동차부품과 신사업 다 실적 좋아져", 차은우 소속사 판타지오, 동전주인데 액면분할?, 송종욱 광주은행 행장, 친환경 올라탄 '화·전·차' 주가↑…올해는 ESG 개미가 이끈다, 동학개미 보란 듯…연기금 26일간 9조 던졌다</t>
+    <t>년도년도 2분기 4분기 NDR Review: High five, IONIQ 5!, 년도년도 2분기 4분기 영업이익은 1.64조원(+40.9% 전년 대비 증감율, OPM 5.6%) 기록, 컨센서스 부합, 판매보증비 증가하나 ASP, 믹스 개선에 기인하므로 수익성 훼손보다는 개선에 방점, 삼천피 무너진 증시…동학개미, 실적 받혀주는 업종 골라야, 현대차 주식 매수의견 유지, “전기차 판매비중 커져 수익성 좋아져, 깜짝실적 자동차주 배당 보따리 푼다</t>
+  </si>
+  <si>
+    <t>봐야할 모멘텀이 많다!, 20년도 4분기 매출액 29.2조원/영업이익 1.6조원, 2021년 매출액 117.7조원/영업이익 6.9조원 전망, 美부양책에 고배당… 주식, 아직 매력적, 현대글로비스, HMM 인수 '그때는 맞고 지금은 다르다', 현대위아 주식 매수의견 유지, “자동차부품과 신사업 다 실적 좋아져", 차은우 소속사 판타지오, 동전주인데 액면분할?, 송종욱 광주은행 행장, 친환경 올라탄 '화·전·차' 주가↑…올해는 ESG 개미가 이끈다, 동학개미 보란 듯…연기금 26일간 9조 던졌다</t>
   </si>
   <si>
     <t>美 애플과 협력?...현대차 · 기아차, '장중 주가 급등', 기아차·애플카 이슈 속 구영테크 등 관련주들도 관심 집중, 레인보우로보틱스 따상 달성, 영화테크, 현대자동차와 부품 공급 계약 체결, 애플카 기아로 가닥?..."현대차, '명분 &amp; 실리' 다잡자", 현대차 주가를 긍정적으로 보는 이유, 딜링룸 24시…챙겨봐야할 국제경제뉴스</t>
@@ -6685,10 +6685,10 @@
     <t>‘애플카 협력 무산설’ 분분… 현대차 8일 입장 밝힌다, 현대차, 말 많은 애플카 이슈 8일 발표, “애플카 믿고 투자했는데”... 현대·기아차에 1.8조 베팅한 개미들 어쩌나, '극과 극' 치닫는 현대차 애플카 협력설 안갯속으로···시장 혼란 우려, "애플카 생산, 반도체 업계에도 잭팟"</t>
   </si>
   <si>
-    <t>'애플카가 뭐길래'…현대차그룹 급락, 日자동차株는 '껑충', 현대차-제네시스 확대와 아이오닉5 전기차 본격화, 2020년 4분기 컨센서스 부합, 2021년 제네시스 확대와 아이오닉5 전기차 본격 론칭, 투자의견 매수, 목표주가 310,000원, 현대차그룹-애플, 이대로 협력관계 끝나나, 현대차·기아 '애플카 개발협의 중단'에 주가 동반급락...전기차 협력 재시동 걸릴까, 13조원 증발한 현대차 공시..'자율주행 전기차' vs '자율주행차', 현대‧기아차 "애플카 없다"…한달간 개미는 사고, 현대차 임원은 팔고, '애플카' 기대감에 현대차그룹 1.5조 사들인 개미들 '허탈', "'애플카' 논의 없다" 현대·기아차, '차익 실현' 후 우상향?, 현대차그룹, 애플과 협의 공식 부인 “협의 진행하고 있지 않아”, 현대차, 애플카 협의 중단…동학개미 '패닉', ‘애플카 버블 30일’ 현대?기아차 협업 소문만 무성…결국 텃새 기업 간 충돌, 현대차·기아차 '애플카' 협력 부인에 뿔난 개미, 5조원 날린 현대차의 가벼운 입? 애플카 논란에 뿔난 개미들, 회장님 따라 주식 산 현대차 임원들, '애플카' 협력설에 주가 오르자 매도, 섣부른 '애플카' 보도, 개미 투자자만 큰 손해, 애플카 뭐길래…현대차그룹 풍문에 '어수선' 진화도 '난감', ‘애플카 협력 중단’ 공식화…현대차·기아 주가 후폭풍, 애플카, 이미지와 현실의 차이, ‘애플카 풍문 득본’ 현대차 임원들, 누가?얼마 차익 냈나?, '애플카 호재' 소멸한 현대차·기아…득실은?, 기아, 애플과 협업 중단…"협의 진행 안 해" 일축, 현대차-애플, 자율주행차 개발 '합승' 중단…"애플카 못탈까?", 현대차, “애플카 협업 갸우뚱”...하지만 美 전기차 ‘마이웨이’, 현대차 임원들, 애플 협력설 결렬 전 주식 매도…현대차그룹 장중 시총 12조↓ 外, 테슬라 대해부…'공간의 한계'를 넘는다, 애플카 협력 무산설에...현대차와 기아의 입장은?, 현대차·기아 "애플과 자율주행차량 개발 협의 진행 안 해", 현대자동차·기아 "애플카 협의 진행하고 있지 않다", 허일섭 녹십자홀딩스 대표이사 겸 GC녹십자 회장, 현대차, 애플카 협의 중단발표…"진행하고 있지 않아", 지난달 '자사주' 미리 팔아치운 현대차 임원들… "신의 한 수였네", 불확실한 애플카 보도에 동학개미 ‘패닉’...증권가 “흔들리지 마라”, 현대차·기아 "애플과 자율주행차 협의 안 해" 입장 밝혀, 현대차·기아 "애플카 협의 중단"…실망감에 주가 급락(종합), 애플과 협의 결렬전 현대차 주식 판 임원들…차익 3배까지도, 현대차-애플 논의 끝?…"완전 결렬은 아닌 듯" 전망 우세, '애플카'로 현대차 주가 급등하자 임원들 주식 팔았다, ‘애플과 자율주행차 협력’ 선 그은 현대차…가능성 사라졌나, 현대차 그룹 급락 속 상한가 6종목, 이아이디·이트론 러시아 백신 이슈에 급등</t>
-  </si>
-  <si>
-    <t>현대차-미래차 전략 차질 없다, 애플카 부인 공시로 전일 주가 급락, 미래차 전략 차질 없다, 연간 실적 개선, 미래차 중심 체질 개선 감안 시 저평가, ‘애플카 쇼크’에 정몽주·정의선 주식 가치 8천억 감소, '애플카' 개발협의 중단에…정몽구·정의선 주식 가치 8000억원 감소, 애플카 협의 중단에…정몽구·정의선 주식 가치 8천억 급감, '애플카 협의 중단'에 정몽구·정의선 주식 가치 8천억 감소(종합), '애플카' 타지 못한 현대·기아차, 실보다 득이 많다?, '애플카 쇼크'에 정몽구·정의선 주식 가치 급감···하루새 8,000억 증발(종합), 정몽구·정의선 주식 가치 8천억원 급감…"애플카 협의 중단 여파", 한국거래소 “현대·기아차 주식 이상 거래 여부 모니터링 중”, ‘애플카 협의 중단’에 정몽구ㆍ정의선 주식 가치 8000억원 감소, '애플카 협의 중단'에 정몽구·정의선 주식 가치 8천억 감소, 애플, 파트너 선택지 축소…"현대차·혼다·닛산·스텔란티스·BMW 정도" - CNN, 대원제약, 이것은 배당인가 무증인가, 이노션 주식 매수의견 유지, "현대차 기아차 마케팅 확대의 수혜 늘어", "애플과 협력 없었나"… 주식 미리 판 현대차 임원들 '눈초리', 애플카 주도권 싸움에 투자자 발만 동동, 현대차X애플카, 끝난걸까…공 넘어간 '물밑협상', "금감원, 현대차 임원 자사주 매각건 조사 없다"-로이터, 애플카 쇼크, 현대차그룹, 애플카 협상 무산…시총 13조 증발, 달아오른 ‘애플카 협업설’ 일단 냉각… 업계 “전기차엔 협력 여지”, 현대차-애플카 협업 중단 배경은…비트코인 변동성에 휩쓸린 S&amp;P 500 外, ‘애플카’ 쇼크에…현대차그룹株 13조 날아갔다, 뉴욕증시 · 비트코인 2차 폭발 애플카-현대 전기차 협상 재개 CNBC 보도, 바이든 부양책 유동성 살포</t>
+    <t>'애플카가 뭐길래'…현대차그룹 급락, 日자동차株는 '껑충', 제네시스 확대와 아이오닉5 전기차 본격화, 2020년 4분기 컨센서스 부합, 2021년 제네시스 확대와 아이오닉5 전기차 본격 론칭, 투자의견 매수, 목표주가 310,000원, 현대차그룹-애플, 이대로 협력관계 끝나나, 현대차·기아 '애플카 개발협의 중단'에 주가 동반급락...전기차 협력 재시동 걸릴까, 13조원 증발한 현대차 공시..'자율주행 전기차' vs '자율주행차', 현대‧기아차 "애플카 없다"…한달간 개미는 사고, 현대차 임원은 팔고, '애플카' 기대감에 현대차그룹 1.5조 사들인 개미들 '허탈', "'애플카' 논의 없다" 현대·기아차, '차익 실현' 후 우상향?, 현대차그룹, 애플과 협의 공식 부인 “협의 진행하고 있지 않아”, 현대차, 애플카 협의 중단…동학개미 '패닉', ‘애플카 버블 30일’ 현대?기아차 협업 소문만 무성…결국 텃새 기업 간 충돌, 현대차·기아차 '애플카' 협력 부인에 뿔난 개미, 5조원 날린 현대차의 가벼운 입? 애플카 논란에 뿔난 개미들, 회장님 따라 주식 산 현대차 임원들, '애플카' 협력설에 주가 오르자 매도, 섣부른 '애플카' 보도, 개미 투자자만 큰 손해, 애플카 뭐길래…현대차그룹 풍문에 '어수선' 진화도 '난감', ‘애플카 협력 중단’ 공식화…현대차·기아 주가 후폭풍, 애플카, 이미지와 현실의 차이, ‘애플카 풍문 득본’ 현대차 임원들, 누가?얼마 차익 냈나?, '애플카 호재' 소멸한 현대차·기아…득실은?, 기아, 애플과 협업 중단…"협의 진행 안 해" 일축, 애플, 자율주행차 개발 '합승' 중단…"애플카 못탈까?", 현대차, “애플카 협업 갸우뚱”...하지만 美 전기차 ‘마이웨이’, 현대차 임원들, 애플 협력설 결렬 전 주식 매도…현대차그룹 장중 시총 12조↓ 外, 테슬라 대해부…'공간의 한계'를 넘는다, 애플카 협력 무산설에...현대차와 기아의 입장은?, 현대차·기아 "애플과 자율주행차량 개발 협의 진행 안 해", 현대자동차·기아 "애플카 협의 진행하고 있지 않다", 허일섭 녹십자홀딩스 대표이사 겸 GC녹십자 회장, 현대차, 애플카 협의 중단발표…"진행하고 있지 않아", 지난달 '자사주' 미리 팔아치운 현대차 임원들… "신의 한 수였네", 불확실한 애플카 보도에 동학개미 ‘패닉’...증권가 “흔들리지 마라”, 현대차·기아 "애플과 자율주행차 협의 안 해" 입장 밝혀, 현대차·기아 "애플카 협의 중단"…실망감에 주가 급락(종합), 애플과 협의 결렬전 현대차 주식 판 임원들…차익 3배까지도, 애플 논의 끝?…"완전 결렬은 아닌 듯" 전망 우세, '애플카'로 현대차 주가 급등하자 임원들 주식 팔았다, ‘애플과 자율주행차 협력’ 선 그은 현대차…가능성 사라졌나, 현대차 그룹 급락 속 상한가 6종목, 이아이디·이트론 러시아 백신 이슈에 급등</t>
+  </si>
+  <si>
+    <t>미래차 전략 차질 없다, 애플카 부인 공시로 전일 주가 급락, 미래차 전략 차질 없다, 연간 실적 개선, 미래차 중심 체질 개선 감안 시 저평가, ‘애플카 쇼크’에 정몽주·정의선 주식 가치 8천억 감소, '애플카' 개발협의 중단에…정몽구·정의선 주식 가치 8000억원 감소, 애플카 협의 중단에…정몽구·정의선 주식 가치 8천억 급감, '애플카 협의 중단'에 정몽구·정의선 주식 가치 8천억 감소(종합), '애플카' 타지 못한 현대·기아차, 실보다 득이 많다?, '애플카 쇼크'에 정몽구·정의선 주식 가치 급감···하루새 8,000억 증발(종합), 정몽구·정의선 주식 가치 8천억원 급감…"애플카 협의 중단 여파", 한국거래소 “현대·기아차 주식 이상 거래 여부 모니터링 중”, ‘애플카 협의 중단’에 정몽구ㆍ정의선 주식 가치 8000억원 감소, '애플카 협의 중단'에 정몽구·정의선 주식 가치 8천억 감소, 애플, 파트너 선택지 축소…"현대차·혼다·닛산·스텔란티스·BMW 정도" - CNN, 대원제약, 이것은 배당인가 무증인가, 이노션 주식 매수의견 유지, "현대차 기아차 마케팅 확대의 수혜 늘어", "애플과 협력 없었나"… 주식 미리 판 현대차 임원들 '눈초리', 애플카 주도권 싸움에 투자자 발만 동동, 현대차X애플카, 끝난걸까…공 넘어간 '물밑협상', "금감원, 현대차 임원 자사주 매각건 조사 없다"-로이터, 애플카 쇼크, 현대차그룹, 애플카 협상 무산…시총 13조 증발, 달아오른 ‘애플카 협업설’ 일단 냉각… 업계 “전기차엔 협력 여지”, 현대차-애플카 협업 중단 배경은…비트코인 변동성에 휩쓸린 S&amp;P 500 外, ‘애플카’ 쇼크에…현대차그룹株 13조 날아갔다, 뉴욕증시 · 비트코인 2차 폭발 애플카-현대 전기차 협상 재개 CNBC 보도, 바이든 부양책 유동성 살포</t>
   </si>
   <si>
     <t>거래소, 현대차 임원 자사주 매도 불공정거래 여부 모니터링, 현대차 임원들은 ‘애플카’ 정보 미리 알고 주식 팔았을까, 명절 앞둔 옵션만기일 '3100선' 탈환</t>
@@ -6727,10 +6727,10 @@
     <t>상한가 4종목, 세방전지·삼보모터스 기대 모았으나 상승세 낮아, 이수앱지스 등 러시아 백신주 급락, 현대바이오 급등에 관심 쏠려</t>
   </si>
   <si>
-    <t>테슬라 주가 하락 진짜 이유는 전기차 경쟁 심화, 현대차-빠르고 공격적인 배터리 화재 리콜로 주가 부정적 영향 최소화 예상, 1조원 규모의 비용이 들어가는 리콜 발표했지만 주가 부정적 영향 가능성은 낮음, 특정 배터리가 들어간 모델에 대해 100% 배터리시스템 교체 결정. 총 1조원 비용 발생할 것, 회계적 비용의 추가 인식 가능성은 적음. 비교적 빠른 대응으로 인해 주가에 대한 부정적 영향은 제한적, 현대차-새 시대, 새 차, 전용 전기차 아이오닉 5 공개, 전기차의 진입장벽을 낮춘다, 현대차-아이오닉5 컨센 부합, 아이오닉5 월드프리미어, 아이오닉5 연간 판매 7만대 목표, 현대차-아이오닉5의 의미, 3월 말부터 아이오닉5 모멘텀 시작, 아이오닉5 공개: 72.6kWh와 58.0kWh의 두 가지 모델. 가격은 5천만원 대, 아이오닉5의 의미: 미래차에 적용될 E-GMP의 상품성 테스트, 한국 최고 유니콘 탄생…쿠팡 기업가치 55조의 비밀, 현대차 주식 매수의견 유지, "아이오닉5 출시로 전기차 경쟁력 커져", 김상조 청와대 대통령비서실 정책실장, "현대차 임원들 주식 폭락전 매도"… 불거진 '애플카' 부당 이득 의혹</t>
-  </si>
-  <si>
-    <t>현대차-다가올 모멘텀을 기다려야 할 시점, 투자의견 매수, 목표주가 300,000원 제시, 21년 영업이익은 7.4조 전망, 앞으로 모멘텀을 제공할 수 있는 이슈: 제네시스 판매량, 전기차 판매, 현대차-선제적인 리콜을 통한 신뢰 제고, 리콜 대상 차량 8.17만대, 비용 약 1조원, 인과 관계에 대한 명확한 규명 필요, 선리콜 조치로 적극적 고객 보호 및 신뢰 제고, 현대차-선제적 코나EV 리콜비용 반영으로 불확실성 해소, 현대차는 LG에너지솔루션(이하 LGES) 중국 남경공장 생산 배터리셀 제조 불량으로 탑재된 차량에 대해 고전압배터리시스템(BSA) 전량 교체 결정, 품질 문제와 관련한 부정 이슈를 선제적으로 해소하려는 의지로 판단, 현대차-코나 EV 등 리콜 관련 Comment, 코나 EV 등 리콜 결정, 관련 Comment, 현대차-나쁜 기억은 2020년에 묻고, LG에너지솔루션 중국 남경 공장에서 생산된 일부 배터리셀의 제조 불량으로 고전압 배터리시스템(BSA) 전량 교체, 음극탭의 접힘이 내부 단락으로 연결되면서 화재 발생 가능성, 대상은 2017년 11월부터 2020년 3월까지 생산된 코나/아이오닉/일렉시티 버스 EV 8.2만대, 현대차-코나EV 등에 대한 배터리 리콜 결정. 1조원 비용, 리콜 비용 1조원으로 배터리 전량 교환. 비용 분담률은 미확정, 국토부는 배터리셀의 음극탭 접힘을 원인 가능성으로 발표. 충전맵 로직 오적용은 추가 확인, 비용은 부정적. 아이오닉5 출시 전 관련 부담 해소가 상쇄, 현대차-선제적인 리콜, 배터리 불안감 해소, 현대차 EV 리콜, 배터리 불안감 해소, 본질은 변하지 않았다, 中, 디지털 위안화 확장 속 달러패권 재도전…현대차 임원들, 애플카 주식매도 부당이득 의혹조사 '급물살' 外, 현대차·아크인베스트·테슬라·한국타이어, LG화학 주식 매수의견 유지, "현대차 전기차 화재사고의 부담 적어", 법원 “형 집행 중 경영 불가”…이재용 옥중 경영 ‘난항’, 현대차 주식 매수의견 유지, "선제적 리콜로 전기차 신뢰도 높여", 현대차 임원 '애플카' 부당이득 의혹, 이르면 4월초 첫 판단 나온다</t>
+    <t>테슬라 주가 하락 진짜 이유는 전기차 경쟁 심화, 빠르고 공격적인 배터리 화재 리콜로 주가 부정적 영향 최소화 예상, 1조원 규모의 비용이 들어가는 리콜 발표했지만 주가 부정적 영향 가능성은 낮음, 특정 배터리가 들어간 모델에 대해 100% 배터리시스템 교체 결정. 총 1조원 비용 발생할 것, 회계적 비용의 추가 인식 가능성은 적음. 비교적 빠른 대응으로 인해 주가에 대한 부정적 영향은 제한적, 새 시대, 새 차, 전용 전기차 아이오닉 5 공개, 전기차의 진입장벽을 낮춘다, 아이오닉5 컨센 부합, 아이오닉5 월드프리미어, 아이오닉5 연간 판매 7만대 목표, 아이오닉5의 의미, 3월 말부터 아이오닉5 모멘텀 시작, 아이오닉5 공개: 72.6kWh와 58.0kWh의 두 가지 모델. 가격은 5천만원 대, 아이오닉5의 의미: 미래차에 적용될 E-GMP의 상품성 테스트, 한국 최고 유니콘 탄생…쿠팡 기업가치 55조의 비밀, 현대차 주식 매수의견 유지, "아이오닉5 출시로 전기차 경쟁력 커져", 김상조 청와대 대통령비서실 정책실장, "현대차 임원들 주식 폭락전 매도"… 불거진 '애플카' 부당 이득 의혹</t>
+  </si>
+  <si>
+    <t>다가올 모멘텀을 기다려야 할 시점, 투자의견 매수, 목표주가 300,000원 제시, 21년 영업이익은 7.4조 전망, 앞으로 모멘텀을 제공할 수 있는 이슈: 제네시스 판매량, 전기차 판매, 선제적인 리콜을 통한 신뢰 제고, 리콜 대상 차량 8.17만대, 비용 약 1조원, 인과 관계에 대한 명확한 규명 필요, 선리콜 조치로 적극적 고객 보호 및 신뢰 제고, 선제적 코나EV 리콜비용 반영으로 불확실성 해소, 현대차는 LG에너지솔루션(이하 LGES) 중국 남경공장 생산 배터리셀 제조 불량으로 탑재된 차량에 대해 고전압배터리시스템(BSA) 전량 교체 결정, 품질 문제와 관련한 부정 이슈를 선제적으로 해소하려는 의지로 판단, 코나 EV 등 리콜 관련 Comment, 코나 EV 등 리콜 결정, 관련 Comment, 나쁜 기억은 2020년에 묻고, LG에너지솔루션 중국 남경 공장에서 생산된 일부 배터리셀의 제조 불량으로 고전압 배터리시스템(BSA) 전량 교체, 음극탭의 접힘이 내부 단락으로 연결되면서 화재 발생 가능성, 대상은 2017년 11월부터 2020년 3월까지 생산된 코나/아이오닉/일렉시티 버스 EV 8.2만대, 코나EV 등에 대한 배터리 리콜 결정. 1조원 비용, 리콜 비용 1조원으로 배터리 전량 교환. 비용 분담률은 미확정, 국토부는 배터리셀의 음극탭 접힘을 원인 가능성으로 발표. 충전맵 로직 오적용은 추가 확인, 비용은 부정적. 아이오닉5 출시 전 관련 부담 해소가 상쇄, 선제적인 리콜, 배터리 불안감 해소, 현대차 EV 리콜, 배터리 불안감 해소, 본질은 변하지 않았다, 中, 디지털 위안화 확장 속 달러패권 재도전…현대차 임원들, 애플카 주식매도 부당이득 의혹조사 '급물살' 外, 현대차·아크인베스트·테슬라·한국타이어, LG화학 주식 매수의견 유지, "현대차 전기차 화재사고의 부담 적어", 법원 “형 집행 중 경영 불가”…이재용 옥중 경영 ‘난항’, 현대차 주식 매수의견 유지, "선제적 리콜로 전기차 신뢰도 높여", 현대차 임원 '애플카' 부당이득 의혹, 이르면 4월초 첫 판단 나온다</t>
   </si>
   <si>
     <t>민간 위성 시대, 한화 1100억 투자..."PEF 10% 룰 폐지" 전망은? 外, 아이오닉5, 2만5천대 사전계약, 엔브이에이치, 현대차 아이오닉5 연간목표 달성…애플카는 '플러스 알파', 카카오, 삼성전자 이어 국민주 되나...5대1 액면분할</t>
@@ -6742,16 +6742,16 @@
     <t>증권가 "ESG 핵심은 투명한 지배구조"…신한금융·현대차·LG디스플레이 'Top3', ‘동학개미 희비’ 배당금 20조원 푼 삼성…3500억 줄인 현대차, 정세균 수소경제 활성화 의지…재계 거인 힘 모은다 外</t>
   </si>
   <si>
-    <t>현대차-아이오닉 5 출시: 이걸 위해 기다렸다, 아이오닉 5 출시: 압도적으로 긍정적인 시장의 반응 확인, E-GMP 양산 본격화, 아이오닉 5 는 이제 시작일 뿐, 경쟁구도 감안시 아이오닉 5 의 과점구도 예상 가능, 투자의견 Buy 유지, 목표주가 330,000 원으로 상향, 이트론·이아이디·이화전기 러 백신 3총사 다시 상한가, 아이오닉5 완판 속 두올, 현대공업 급등, 책임 많고 권한 없는 韓기업, 글로벌 ESG 평가 최약체 전락, 수백억 배당금 받는 정의선, 자사주 추가매수 나설까, 이아이디·이트론·이화전기·한빛소프트·리더스기술투자 '러시아백신 강세', 쿠팡플레이, 오는 5일부터 ‘손흥민 EPL 경기’ 생중계, 2월 로스닥(LOSDAQ), 주가로 보는 물류·유통산업, 서연·덕성·동일제강·두올·대원산업 '윤석열·전기차 관련주 강세'</t>
+    <t>아이오닉 5 출시: 이걸 위해 기다렸다, 아이오닉 5 출시: 압도적으로 긍정적인 시장의 반응 확인, E-GMP 양산 본격화, 아이오닉 5 는 이제 시작일 뿐, 경쟁구도 감안시 아이오닉 5 의 과점구도 예상 가능, 투자의견 Buy 유지, 목표주가 330,000 원으로 상향, 이트론·이아이디·이화전기 러 백신 3총사 다시 상한가, 아이오닉5 완판 속 두올, 현대공업 급등, 책임 많고 권한 없는 韓기업, 글로벌 ESG 평가 최약체 전락, 수백억 배당금 받는 정의선, 자사주 추가매수 나설까, 이아이디·이트론·이화전기·한빛소프트·리더스기술투자 '러시아백신 강세', 쿠팡플레이, 오는 5일부터 ‘손흥민 EPL 경기’ 생중계, 2월 로스닥(LOSDAQ), 주가로 보는 물류·유통산업, 서연·덕성·동일제강·두올·대원산업 '윤석열·전기차 관련주 강세'</t>
   </si>
   <si>
     <t>세계 부자 1위, 테슬라 CEO 일론 머스크의 상상초월 생각을 엿볼 수 있는 책, SK, 기업공개 19개사로 대기업집단 1위…투명경영 선도, 아이오닉5 돌풍, 관련주 매매타이밍은?, 쿠팡이 밀고 소프트뱅크가 끌고…네이버 불 붙었다, 한국투자증권, 스텝다운형 TRUE ELS 18320회 모집…미래에셋대우, 대학생 챌린지 개최</t>
   </si>
   <si>
-    <t>삼성전자-TSMC, 초미세공정 이어 美파운드리 증산전쟁 돌입(3월4일), [EBN 오늘(4일) 이슈 종합] 증시 주춤에 머니무브, 제약·바이오 CEO 줄줄이 임기 만료 등, 4일 장 마감 후 주요 종목뉴스, 세계적인 부자 버핏 할아버지 유언장에 적혀 있는 ‘그거’ 뭐야?_주린이를 위한 경제 가이드 #4, 현대차-새로운 모빌리티의 시대에서 길을 묻다, 과거 자율주행 개발 초점이 인지-측위-판단-제어의 메커니즘 중 인지-측위에 있었다면, 센서 기술의 발전은 인지-측위 역량의 안정화를 가져옴. 향후에는 소프트웨어에 기반한 판단 역량 강화가 차별화를 가져올 것, 소프트웨어 2.0 시대가 도래하며, 인공지능이 실 적용 데이터와 가장 비슷한 분포의 데이터를 스스로 학습하는 방식으로 진화. 최근 애플 등 빅테크 업체의 자동차 산업에 대한 진입 시도도 소프트웨어 2.0으로의 전환이 빨라지는데 대한 위기감에서 출발하며, 자율주행 연구의 출발은 테스트셋(실 적용 데이터)과 가장 비슷한 주행 데이터 확보에 있임, 이러한 환경에서 현대차는 완성차 업체로서의 사업 기회 이 외에도 독자적인 역량 강화를 모색. 사내 인공지능 독립 기업(CIC) AIRS Company 출범과 데이터 오픈 플랫폼 디벨로퍼스 구축을 통해 소프트웨어 역량 강화를 향한 적극적인 움직임. 현대차는 2022년 중반까지 Lv.3 고속도로 자율주행 개발을 완료하고, 2024년 이후 Lv.4 도심 자율주행 서비스 상용화를 시작한다는 계획으로, 향후 기술 발전 추이를 주목</t>
-  </si>
-  <si>
-    <t>LG-SK ‘집안싸움’ 와중에 中 배터리업계만 노났다, 증권플러스 비상장, 2월에도 '카카오뱅크, 에스케이바이오사이언스' 강세, ‘카카오뱅크’, ‘SK바이오사이언스’ 강세…지엔티파마도 급부상, 이베이코리아, 카카오 피인수 앞두고 몸값 띄우기 나서나, 증권플러스 비상장, "2월에도 '카뱅, SK바이오사이언스' 강세", 증권플러스 비상장 "2월 카뱅·SK바이오사이언스 강세", 4일 장 마감 후 주요 종목뉴스, 증권플러스 비상장, 2월 관심종목 ‘지엔티파마’ 새롭게 부상, 증권플러스 비상장, 2월 인기 비상장 주식 키워드 발표, 현대차-코나EV 리콜비용 추가분은 최종 3,866억원으로 확정, 현대차가 4분기 비용으로 잡은 금액이 3,866억원, 이제는 아이오닉5에 집중, 목표주가 30.5만원 유지, 증권플러스 비상장, 2월 ‘카카오뱅크, 에스케이바이오사이언스’ 강세</t>
+    <t>삼성전자-TSMC, 초미세공정 이어 美파운드리 증산전쟁 돌입(3월4일), [EBN 오늘(4일) 이슈 종합] 증시 주춤에 머니무브, 제약·바이오 CEO 줄줄이 임기 만료 등, 4일 장 마감 후 주요 종목뉴스, 세계적인 부자 버핏 할아버지 유언장에 적혀 있는 ‘그거’ 뭐야?_주린이를 위한 경제 가이드 #4, 새로운 모빌리티의 시대에서 길을 묻다, 과거 자율주행 개발 초점이 인지-측위-판단-제어의 메커니즘 중 인지-측위에 있었다면, 센서 기술의 발전은 인지-측위 역량의 안정화를 가져옴. 향후에는 소프트웨어에 기반한 판단 역량 강화가 차별화를 가져올 것, 소프트웨어 2.0 시대가 도래하며, 인공지능이 실 적용 데이터와 가장 비슷한 분포의 데이터를 스스로 학습하는 방식으로 진화. 최근 애플 등 빅테크 업체의 자동차 산업에 대한 진입 시도도 소프트웨어 2.0으로의 전환이 빨라지는데 대한 위기감에서 출발하며, 자율주행 연구의 출발은 테스트셋(실 적용 데이터)과 가장 비슷한 주행 데이터 확보에 있임, 이러한 환경에서 현대차는 완성차 업체로서의 사업 기회 이 외에도 독자적인 역량 강화를 모색. 사내 인공지능 독립 기업(CIC) AIRS Company 출범과 데이터 오픈 플랫폼 디벨로퍼스 구축을 통해 소프트웨어 역량 강화를 향한 적극적인 움직임. 현대차는 2022년 중반까지 Lv.3 고속도로 자율주행 개발을 완료하고, 2024년 이후 Lv.4 도심 자율주행 서비스 상용화를 시작한다는 계획으로, 향후 기술 발전 추이를 주목</t>
+  </si>
+  <si>
+    <t>LG-SK ‘집안싸움’ 와중에 中 배터리업계만 노났다, 증권플러스 비상장, 2월에도 '카카오뱅크, 에스케이바이오사이언스' 강세, ‘카카오뱅크’, ‘SK바이오사이언스’ 강세…지엔티파마도 급부상, 이베이코리아, 카카오 피인수 앞두고 몸값 띄우기 나서나, 증권플러스 비상장, "2월에도 '카뱅, SK바이오사이언스' 강세", 증권플러스 비상장 "2월 카뱅·SK바이오사이언스 강세", 4일 장 마감 후 주요 종목뉴스, 증권플러스 비상장, 2월 관심종목 ‘지엔티파마’ 새롭게 부상, 증권플러스 비상장, 2월 인기 비상장 주식 키워드 발표, 코나EV 리콜비용 추가분은 최종 3,866억원으로 확정, 현대차가 4분기 비용으로 잡은 금액이 3,866억원, 이제는 아이오닉5에 집중, 목표주가 30.5만원 유지, 증권플러스 비상장, 2월 ‘카카오뱅크, 에스케이바이오사이언스’ 강세</t>
   </si>
   <si>
     <t>600달러 밑이 된 테슬라 주가, 치열해지는 전기차 경쟁 [김도형 기자의 휴일차(車)담]</t>
@@ -6763,16 +6763,16 @@
     <t>NE능률 3거래일 연속 상한가 속 웅진 윤석열 관련주로 지목되며 상한가... 이트론 다시 급등 속 바이넥스는 급락, 웅진·덕성·이아이디·동국알앤에스·NE능률·금강철강·이트론·이화전기·서울옥션 주가 강세, 변동성 커지며 서학개미 매수세 눈에 띄게 줄어, 윤석열 관련주 서연·덕성·서연탑메탈 강세...반면 반도체 관련주 SFA반도체·제주반도체 계속된 하락, 4대 자산운용사가 말하는 ETF (3) 금정섭 KB자산운용 ETF전략실장 “성장 테마로 5G·수소 관련 기업 주목”</t>
   </si>
   <si>
-    <t>성보화학·프레스티지바이오파마·원익큐브·원풍·국일제지·대한그린파워 주가 강세, 하이투자증권, 영업점 고객 대상 미국주식 이벤트 개최 外 신한금투, 포스코 임원 자사주 취득이 사익편취? 시민단체 주장 논란, 현대차-년도년도 2분기 1분기 프리뷰: 美 한파 영향 등으로 시장컨센서스 하회 예상, 투자의견 Buy, 목표주가 300,000원 유지, 년도년도 2분기 1분기 영업이익 1.2조원 (+39.7% 전년 대비 증감율) 예상. 시장 컨센서스 21.5% 하회할 것, 배터리 관련 리콜 비용은 년도년도 2분기 4분기 손익에 소급 반영. 21년도 1분기 손익에는 영향 없음, 리스크요인: 전기차 등 미래 기술 개발 경쟁 심화, 코로나19 재확산, 원화가치 절상, 신한금융그룹·한국투자증권·신한금융투자, 윤석열·쿠팡 관련주 강세보이던 중 일제히 하락...코로나19 백신 관련주 마저 내림세, 한국투자증권, 미국주식 오후 6시부터...무료 시세정보도 제공 外</t>
-  </si>
-  <si>
-    <t>`아이오닉5 수혜주` 두올 급등하자…이서진 등 지분 매각, 아이오닉5로 잘가던 때 지분 매각한 두올 대표 동생과 배우 이서진, 3월 기업 동향과 전망-자동차 조선 중공업 철강, 아이오닉5 덕에 주가급등…배우 이서진, 車내장재 두올 지분 모두 매각, 아이오닉5 흥행에 주가 급등···이서진, 車내장재 두올 주식 '풀매도', 배우 이서진, '아이오닉5' 흥행에 두올 주식 '풀매도', ‘아이오닉5 흥행에 주가 급등’…배우 이서진, ‘두올’ 지분 모두 매각, 백기사VS투기꾼···'자사株 매입' 딜레마, 현대차-UAM 진출 신호탄이 울리다, 현대차 미국 UAM 개발거점 설립, 또다른 여정의 시작, 전 세계에서 시장에서 UAM 시장 형성은 미국과 유럽 가장 빠를 것, eVTOL(전기추진 수직이착륙) 방식의 기체 생산, 주도권은 기체 제작, “무려 억대…” 배우 이서진, 아이오닉5 덕분에 돈 제대로 벌었다 (+이유)</t>
+    <t>성보화학·프레스티지바이오파마·원익큐브·원풍·국일제지·대한그린파워 주가 강세, 하이투자증권, 영업점 고객 대상 미국주식 이벤트 개최 外 신한금투, 포스코 임원 자사주 취득이 사익편취? 시민단체 주장 논란, 년도년도 2분기 1분기 프리뷰: 美 한파 영향 등으로 시장컨센서스 하회 예상, 투자의견 Buy, 목표주가 300,000원 유지, 년도년도 2분기 1분기 영업이익 1.2조원 (+39.7% 전년 대비 증감율) 예상. 시장 컨센서스 21.5% 하회할 것, 배터리 관련 리콜 비용은 년도년도 2분기 4분기 손익에 소급 반영. 21년도 1분기 손익에는 영향 없음, 리스크요인: 전기차 등 미래 기술 개발 경쟁 심화, 코로나19 재확산, 원화가치 절상, 신한금융그룹·한국투자증권·신한금융투자, 윤석열·쿠팡 관련주 강세보이던 중 일제히 하락...코로나19 백신 관련주 마저 내림세, 한국투자증권, 미국주식 오후 6시부터...무료 시세정보도 제공 外</t>
+  </si>
+  <si>
+    <t>`아이오닉5 수혜주` 두올 급등하자…이서진 등 지분 매각, 아이오닉5로 잘가던 때 지분 매각한 두올 대표 동생과 배우 이서진, 3월 기업 동향과 전망-자동차 조선 중공업 철강, 아이오닉5 덕에 주가급등…배우 이서진, 車내장재 두올 지분 모두 매각, 아이오닉5 흥행에 주가 급등···이서진, 車내장재 두올 주식 '풀매도', 배우 이서진, '아이오닉5' 흥행에 두올 주식 '풀매도', ‘아이오닉5 흥행에 주가 급등’…배우 이서진, ‘두올’ 지분 모두 매각, 백기사VS투기꾼···'자사株 매입' 딜레마, UAM 진출 신호탄이 울리다, 현대차 미국 UAM 개발거점 설립, 또다른 여정의 시작, 전 세계에서 시장에서 UAM 시장 형성은 미국과 유럽 가장 빠를 것, eVTOL(전기추진 수직이착륙) 방식의 기체 생산, 주도권은 기체 제작, “무려 억대…” 배우 이서진, 아이오닉5 덕분에 돈 제대로 벌었다 (+이유)</t>
   </si>
   <si>
     <t>금융당국 "현대차 임원 미공개정보 이용 의혹 거래소가 심리 중", 다른 기업도 샀는데…포스코 임원 주식 매입만 문제된 까닭은, 주총 D-1 포스코, 최정우 시즌2 통해 ‘리튬·수소’ 시대 연다, 이노션 주식 매수의견 유지, "현대차 기아 마케팅 강화의 수혜 커져", 최정우 포스코 대표이사 회장, '사외이사' 이서진, 두올 주식 팔아 '쏠쏠', 금융당국 "현대차 임원 부당이득 혐의 심리 中…엄격 처리", 금융당국 "현대차 임원 미공개정보이용 의혹 사건, 엄격히 처리", 금융위 "현대차 임원 '애플카' 부당이득 의혹 심리 중…엄격 처리", 금융당국, 자본시장 집중단속…‘현대차-애플카 미공개정보 이용’ 도마, 금융당국, 불공정거래 112건 조사…이달 시장조성자 불법공매도 조사 마무리, 거래소, 현대차 임원 ‘애플카 공동개발’ 주가 부당이득 혐의 심리</t>
   </si>
   <si>
-    <t>ESG의 전제는 바로 장기주의(Long-termism), 현대차-생존 경쟁의 첨병, 수익성 회복을 위한 M/S(전체) 확대와, 생존을 대변 할 M/S(EV) 확대, 투자의견 BUY, 목표주가 300,000원 제시, 쿠팡 김범석 "혁신 투자 지속"… 현대차 리콜에 LGES, 100조 기업가치 '휘청' 外, 현대차-On-track, 21년도 1분기 영업이익은 시장 컨센서스와 유사한 1.41조원을 기록할 것으로 전망, 환율 상황이 연말대비 개선되고 있어 사업 계획 수립대비 경영환경이 우호적, 정주영 만난 피터 드러커 “제가 잘못했습니다” 사과한 이유는, 쿠팡 뉴욕증시 성공적 상장…기업윤리·책임도 소홀히 말아야, 금융당국 "현대차 임원 미공개정보 이용 혐의, 염격 처리", 현대차 주식 매수의견 유지, “반도체 부족 걱정없고 아이오닉5 좋아”, 최정우 포스코 회장, 여권·노동계 압박 넘어 연임 성공할까</t>
+    <t>ESG의 전제는 바로 장기주의(Long-termism), 생존 경쟁의 첨병, 수익성 회복을 위한 M/S(전체) 확대와, 생존을 대변 할 M/S(EV) 확대, 투자의견 BUY, 목표주가 300,000원 제시, 쿠팡 김범석 "혁신 투자 지속"… 현대차 리콜에 LGES, 100조 기업가치 '휘청' 外, On-track, 21년도 1분기 영업이익은 시장 컨센서스와 유사한 1.41조원을 기록할 것으로 전망, 환율 상황이 연말대비 개선되고 있어 사업 계획 수립대비 경영환경이 우호적, 정주영 만난 피터 드러커 “제가 잘못했습니다” 사과한 이유는, 쿠팡 뉴욕증시 성공적 상장…기업윤리·책임도 소홀히 말아야, 금융당국 "현대차 임원 미공개정보 이용 혐의, 염격 처리", 현대차 주식 매수의견 유지, “반도체 부족 걱정없고 아이오닉5 좋아”, 최정우 포스코 회장, 여권·노동계 압박 넘어 연임 성공할까</t>
   </si>
   <si>
     <t>이주의 주식시장은? 윤석열 관련주 계속되는 강세, 오세훈 관련주 등 정치테마주 주목, 쿠팡 상장 후 마켓컬리 관련주에도 시선 쏠려</t>
@@ -6787,7 +6787,7 @@
     <t>지난해 주식 소유자 919만명…전년比 300만명 '급증', 쿠팡 상장으로 대박난 직원은 따로 있다...고액 연봉자만 잭팟?, '빅5'기업 주주 500만 시대</t>
   </si>
   <si>
-    <t>"폭스바겐, 2025년께 전기차판매 테슬라 추월"...UBS, 현대차-Platform Builds the Vehicle, 현대차그룹의 E-GMP 플랫폼은 고객이 요구하는 다양한 상품성을 만족시키고 전기차 고유의 성능을 극대화하는 한편, 기존 파생 EV 대비 안전성과 사용성을 크게 개선. 최근 공개된 아이오닉 5는 주행거리, 급속충전, V2L, 안전성과 실내 공간 확보 등 상품 경쟁력이 높은 E-GMP 첫 모델, e-Mobility 시장이 등장하면서 B2C 기반 내연기관 승용을 제조 판매하는 OEM 중심의 수직적 밸류 체인은 B2B/모빌리티 서비스향 전기차 기반 수평적 밸류체인으로 변화. 변화는 제조 기반 OEM과 전통적인 부품사의 가치를 낮추고. 모빌리티 서비스 업체나 전장, 배터리 업체, 자율주행 S/W의 가치를 더욱 높일 전망, 2021년 달라진 '관전 포인트', 현대차 주식 매수의견 유지, "아이오닉5 흥행에 GV80도 미국 공략"</t>
+    <t>"폭스바겐, 2025년께 전기차판매 테슬라 추월"...UBS, Platform Builds the Vehicle, 현대차그룹의 E-GMP 플랫폼은 고객이 요구하는 다양한 상품성을 만족시키고 전기차 고유의 성능을 극대화하는 한편, 기존 파생 EV 대비 안전성과 사용성을 크게 개선. 최근 공개된 아이오닉 5는 주행거리, 급속충전, V2L, 안전성과 실내 공간 확보 등 상품 경쟁력이 높은 E-GMP 첫 모델, e-Mobility 시장이 등장하면서 B2C 기반 내연기관 승용을 제조 판매하는 OEM 중심의 수직적 밸류 체인은 B2B/모빌리티 서비스향 전기차 기반 수평적 밸류체인으로 변화. 변화는 제조 기반 OEM과 전통적인 부품사의 가치를 낮추고. 모빌리티 서비스 업체나 전장, 배터리 업체, 자율주행 S/W의 가치를 더욱 높일 전망, 2021년 달라진 '관전 포인트', 현대차 주식 매수의견 유지, "아이오닉5 흥행에 GV80도 미국 공략"</t>
   </si>
   <si>
     <t>조중일 세종 변호사 "자본시장서 IT 기업 존재감 커진다", 변동성 확대에 가치평가 안갯속...'성장주' 셈법 복잡해진 한국 자본시장, 성장주 진통·소송 불확실성…LG화학·SK이노 '가치 흔들', "'거품 투성이' 테슬라 무너진다"…전기차 업계 지각변동</t>
@@ -6814,7 +6814,7 @@
     <t>만도 주식 매수의견으로 상향, "폴크스바겐으로 부품 공급 다변화", 정몽규 HDC 대표이사 겸 HDC그룹 회장, 댄 아이브스 "테슬라 시총 1조달러 간다…애플은 슈퍼 사이클", 백신 접종 본격화…유통주 실적 턴어라운드 주목, 댄 아이브스 "테슬라 시총 1조 달러 간다…애플은 슈퍼 사이클"</t>
   </si>
   <si>
-    <t>동학개미 1분기 4대 그룹주에 베팅…삼성전자 15.5조 압도적 1위, 현대위아 주식 매수의견 유지, "전기차 열관리모듈 개발해 수주", 현대차 주식 매수의견 유지, "전기차와 제네시스 중심 전환 성공적", 동학개미 ‘4대 그룹주’ 30조 쓸어 담았다, 현대차-First Mover로의 전환을 모색, 장기 지속 가능성에 대한 신뢰: 중장기 주가 재평가 지속 전망, 1분기 Preview: 사업구조 전환 순조롭게 진행 중, "주요 기업, 외국인 배당금 급증... 외환시장 변동성 커진다"</t>
+    <t>동학개미 1분기 4대 그룹주에 베팅…삼성전자 15.5조 압도적 1위, 현대위아 주식 매수의견 유지, "전기차 열관리모듈 개발해 수주", 현대차 주식 매수의견 유지, "전기차와 제네시스 중심 전환 성공적", 동학개미 ‘4대 그룹주’ 30조 쓸어 담았다, First Mover로의 전환을 모색, 장기 지속 가능성에 대한 신뢰: 중장기 주가 재평가 지속 전망, 1분기 Preview: 사업구조 전환 순조롭게 진행 중, "주요 기업, 외국인 배당금 급증... 외환시장 변동성 커진다"</t>
   </si>
   <si>
     <t>'현대차와 파트너 계약 체결'...교통솔루션 전문기업 에스트래픽, 3월 들어 주가 57% 급등</t>
@@ -6832,13 +6832,13 @@
     <t>"서울시장 누가 돼도 건설붐" 건설株 '주목'... "주간 수익률 1위 애널리스트 누구?" 外, "올해가 ESG 원년"…기업들, 경영의 格을 높인다</t>
   </si>
   <si>
-    <t>현대차-아직은 반도체 공급 차질 영향 없어요!, 투자의견 매수, 목표주가 300,000원 유지, 2021년 1분기 매출 18.4조, 영업이익 1.5조 전망, 향후 모멘텀을 더 적극적으로 판단해야 할 시기, 1분기 주식 희비…효성 웃고 이재용 6490억 증발, 조석래 효성 명예회장, 대기업 총수 중 1Q 주식재산 증가율 1위, ‘4월의 용돈’, 13조 늘어난 배당금…증시 훈풍 이끌까, 개미들 두둑한 '4월의 용돈' 올 배당금 13조 늘어 33조</t>
-  </si>
-  <si>
-    <t>현대차-불붙은글로벌신차효과, 매출액27.4조원(+8.3%전년 대비 증감율),영업이익1.4조원(+65.1%전년 대비 증감율)를 기록해 컨센서스 부합할 것으로 예상됨, 북미 SUV 판매 강화, 픽업 트럭(투싼 베이스) 최초 출시, 이건희 회장 별세로 서정진 셀트리온 회장 국내 최고부호 등극…포브스 집계</t>
-  </si>
-  <si>
-    <t>현대차-우리가 아직 몰랐던 전기차 경쟁력, 투자의견 매수, 목표주가 300,000원 유지, 당사의 밸류에이션 상향이 필요한 이유: 전기차 점유율 상승, 메카(M.E.C.A.)관련 경쟁력 보유, 현대차-년도년도 2분기 1분기 Preview: 없어서 못 파는 시기, 년도년도 2분기 1분기 연결매출액27.7조원(전년 대비 증감율 +9.6%), 영업이익1조6,781억원(전년 대비 증감율 +94%) 전망, 자동차 부문 매출액 21.8조원(전년 대비 증감율 +11.5%), 영업이익 1.24조원(OPM 5.7%) 예상, ASP 높은 내수 판매가 +17% 증가하며 지역믹스 개선 지속, 현대비앤지스틸, 올해 수익성 강화 목표, 이노션 주식 매수의견 유지, "현대차 기아 마케팅 강화의 수혜 커져", 게임주로 웃은 아재 3명의 이야기, "차량반도체 부족은 수요회복의 신호, 자동차업종 비중 확대해야"</t>
+    <t>아직은 반도체 공급 차질 영향 없어요!, 투자의견 매수, 목표주가 300,000원 유지, 2021년 1분기 매출 18.4조, 영업이익 1.5조 전망, 향후 모멘텀을 더 적극적으로 판단해야 할 시기, 1분기 주식 희비…효성 웃고 이재용 6490억 증발, 조석래 효성 명예회장, 대기업 총수 중 1Q 주식재산 증가율 1위, ‘4월의 용돈’, 13조 늘어난 배당금…증시 훈풍 이끌까, 개미들 두둑한 '4월의 용돈' 올 배당금 13조 늘어 33조</t>
+  </si>
+  <si>
+    <t>불붙은글로벌신차효과, 매출액27.4조원(+8.3%전년 대비 증감율),영업이익1.4조원(+65.1%전년 대비 증감율)를 기록해 컨센서스 부합할 것으로 예상됨, 북미 SUV 판매 강화, 픽업 트럭(투싼 베이스) 최초 출시, 이건희 회장 별세로 서정진 셀트리온 회장 국내 최고부호 등극…포브스 집계</t>
+  </si>
+  <si>
+    <t>우리가 아직 몰랐던 전기차 경쟁력, 투자의견 매수, 목표주가 300,000원 유지, 당사의 밸류에이션 상향이 필요한 이유: 전기차 점유율 상승, 메카(M.E.C.A.)관련 경쟁력 보유, 년도년도 2분기 1분기 Preview: 없어서 못 파는 시기, 년도년도 2분기 1분기 연결매출액27.7조원(전년 대비 증감율 +9.6%), 영업이익1조6,781억원(전년 대비 증감율 +94%) 전망, 자동차 부문 매출액 21.8조원(전년 대비 증감율 +11.5%), 영업이익 1.24조원(OPM 5.7%) 예상, ASP 높은 내수 판매가 +17% 증가하며 지역믹스 개선 지속, 현대비앤지스틸, 올해 수익성 강화 목표, 이노션 주식 매수의견 유지, "현대차 기아 마케팅 강화의 수혜 커져", 게임주로 웃은 아재 3명의 이야기, "차량반도체 부족은 수요회복의 신호, 자동차업종 비중 확대해야"</t>
   </si>
   <si>
     <t>이노션 주식 매수의견 유지, "현대차 기아 마케팅 강화에 올라타", 현대차 주식 매수의견 유지, "평균판매가격 올라 반도체 부족 극복"</t>
@@ -6847,19 +6847,19 @@
     <t>‘호재 만발’ 카카오, 11만원 액면분할 후에도 동학개미 쓸어담나?, 테슬라 전기트럭 '세미' 시범생산 돌입·삼성SDI, 골드만삭스 올해 추천종목 선정(4월1주차), 금융당국, 현대차 임원 '애플카 미공개정보 이용 의혹' 조사 착수, 금융당국, 현대차 임원 12명 '애플카' 관련 주식거래 의혹 조사, 현대차 임원진 '미공개 애플카' 주식거래···규명 가능할까, 금융당국, 현대차 임원 '애플카 미공개 정보이용' 의혹 조사 착수, 금융당국, ‘애플카 미공개정보 이용 의혹’ 현대차 임직원 조사 방침, 금융당국, ‘애플카 미공개정보 이용 의혹’ 현대차 임원 조사 착수</t>
   </si>
   <si>
-    <t>막 내린 LG-SK 배터리 분쟁…남은 과제는?, '현대차 애플카 만든다'…미공개 정보 이용 주식 거래 현대차 임원들 조사, 금융당국, '애플카 미공개 정보 이용 의혹' 현대차 임원들 조사, '액면분할'로 11만 원 되는 카카오…개미 매수행렬 이어질까?, "2분기는 광고株 투자 적기"…제일기획·이노션 목표가↑, 지수 상승하되 폭은 제한적일 듯, ①“카카오 주가 신발보다 싸다”…주가 상승세 이어질지 ‘주목’, "제일기획·이노션…광고株, 경기회복 수혜 본격 시작", “애플과 협의 없어” 공시전 주식 8.3억 매도…금융당국, 현대차 임원 조사, 액면분할 카카오 11만원에 산다… 동학개미 15일부터 쓸어 담을까, SK이노베이션·삼성전자·정의선 현대차·아마존, IMF·세계금융위기 이후 한국자본주의의 변모와 그 양상들, LG-SK 배터리 분쟁 극적 합의…중국에게 빼앗긴 시장 탈환하나, "강남 재건축 벌써 호가 3억 뛰어"…오세훈발 부동산시장 불안 시작?, 삼성증권 오현석 "반도체·車가 실적장 주도…코인 이미 비싸다", 보스턴 다이내믹스 '스팟' 군사훈련 출동…현대로템 '전투용 로봇' 개발 속도(4월12일), 현대차-내수 판매 호조에 힘입어 컨센서스 상회 예상, 21년도 1분기 매출 28조원(전년 대비 증감율+12%), 영업이익 1.6조원(+88%) 전망, 투자의견 매수 유지, 목표주가 31만원 유지, 현대차-이제는 위가 보인다, 21년도 1분기 Preview: 영업이익 1.7조원 달성, 시장 기대치 상회 예상, 판매의 질 개선은 구조적, 21년도 2분기 에도 실적 모멘텀 가능성 존재, 투자의견 Buy, 목표주가 330,000원 유지. 비중확대 전략 유효, 금융당국, '애플카 미공개 정보 이용' 현대차 임원들 조사</t>
+    <t>막 내린 LG-SK 배터리 분쟁…남은 과제는?, '현대차 애플카 만든다'…미공개 정보 이용 주식 거래 현대차 임원들 조사, 금융당국, '애플카 미공개 정보 이용 의혹' 현대차 임원들 조사, '액면분할'로 11만 원 되는 카카오…개미 매수행렬 이어질까?, "2분기는 광고株 투자 적기"…제일기획·이노션 목표가↑, 지수 상승하되 폭은 제한적일 듯, ①“카카오 주가 신발보다 싸다”…주가 상승세 이어질지 ‘주목’, "제일기획·이노션…광고株, 경기회복 수혜 본격 시작", “애플과 협의 없어” 공시전 주식 8.3억 매도…금융당국, 현대차 임원 조사, 액면분할 카카오 11만원에 산다… 동학개미 15일부터 쓸어 담을까, SK이노베이션·삼성전자·정의선 현대차·아마존, IMF·세계금융위기 이후 한국자본주의의 변모와 그 양상들, LG-SK 배터리 분쟁 극적 합의…중국에게 빼앗긴 시장 탈환하나, "강남 재건축 벌써 호가 3억 뛰어"…오세훈발 부동산시장 불안 시작?, 삼성증권 오현석 "반도체·車가 실적장 주도…코인 이미 비싸다", 보스턴 다이내믹스 '스팟' 군사훈련 출동…현대로템 '전투용 로봇' 개발 속도(4월12일), 내수 판매 호조에 힘입어 컨센서스 상회 예상, 21년도 1분기 매출 28조원(전년 대비 증감율+12%), 영업이익 1.6조원(+88%) 전망, 투자의견 매수 유지, 목표주가 31만원 유지, 이제는 위가 보인다, 21년도 1분기 Preview: 영업이익 1.7조원 달성, 시장 기대치 상회 예상, 판매의 질 개선은 구조적, 21년도 2분기 에도 실적 모멘텀 가능성 존재, 투자의견 Buy, 목표주가 330,000원 유지. 비중확대 전략 유효, 금융당국, '애플카 미공개 정보 이용' 현대차 임원들 조사</t>
   </si>
   <si>
     <t>'몸값 10조' 현대엔지니어링 코스피 상장한다…장외 주가 100만원 육박, 현대차그룹, 현대엔지니어링 상장 추진...지배구조 개편 ‘퍼즐 맞추기’에 촉각, ‘비상장 주가 102만원’ 현대엔지니어링 상장 초읽기, '아이오닉5' 공급사 동아화성, 자사주 팔아 캐파 확장 '방점', 삼성SDI, '장중 주가 급등'..."현대차 협업 · 美 공장 검토", 상장 추진하는 현대엔지니어링…하반기 최대 '대어'로 떠오를까</t>
   </si>
   <si>
-    <t>현대엔지니어링 상장 시동…영끌? 세금 마련?, 현대엔지니어링 상장, 정의선에 왜 중요한가, 계획 없다던 현대엔지니어링 상장, 왜?, 기업지배 구조 개편, 대대적 새판짜기…SKT·현대車, 미래 성장 기반 마련, 현대엔지니어링 상장하면 정의선 1조가량 확보, 지분 얼마나 매각할까, ELS도 역시 '삼성전자', 국내주식 기초자산 최다 포함, 현대차-현재까지 순항 중, 21년도 1분기 실적 Preview, 21년도 2분기 에도 이익 개선 흐름 유지 가능 예상, 주가 상승 트리거는 EV M/S 상승과 美 제네시스 판매 증가, 현대차-판매자 시장(Seller’s Market), 21년도 1분기 Preview: 기대치 상회하는 양호한 실적 전망, 판매자 시장 (Seller’s Market), 중고차 가격 상승으로 금융 법인 실적 개선, 현대차-그룹사 변화의 장점, 판매/믹스/신차 어디에도 약점이 없는 구성, 21년도 1분기 영업이익 1.60조원(+85.4%)으로 기대치 부합, 목표주가 300,000원으로 11% 상향, 투자의견 매수 유지</t>
+    <t>현대엔지니어링 상장 시동…영끌? 세금 마련?, 현대엔지니어링 상장, 정의선에 왜 중요한가, 계획 없다던 현대엔지니어링 상장, 왜?, 기업지배 구조 개편, 대대적 새판짜기…SKT·현대車, 미래 성장 기반 마련, 현대엔지니어링 상장하면 정의선 1조가량 확보, 지분 얼마나 매각할까, ELS도 역시 '삼성전자', 국내주식 기초자산 최다 포함, 현재까지 순항 중, 21년도 1분기 실적 Preview, 21년도 2분기 에도 이익 개선 흐름 유지 가능 예상, 주가 상승 트리거는 EV M/S 상승과 美 제네시스 판매 증가, 판매자 시장(Seller’s Market), 21년도 1분기 Preview: 기대치 상회하는 양호한 실적 전망, 판매자 시장 (Seller’s Market), 중고차 가격 상승으로 금융 법인 실적 개선, 그룹사 변화의 장점, 판매/믹스/신차 어디에도 약점이 없는 구성, 21년도 1분기 영업이익 1.60조원(+85.4%)으로 기대치 부합, 목표주가 300,000원으로 11% 상향, 투자의견 매수 유지</t>
   </si>
   <si>
     <t>‘현대엔지니어링 IPO로 재점화’ 현대차 지배구조 개편 묵은 숙제 풀까, 비상장 대장주 드디어 코스피 입성 채비…RFP 발송, 액면분할 '카카오' 날았다…첫날 7.6% 급등, 시총 5위로 껑충, 총수 지정ㆍ순환출자 해소....정의선, 글로비스 지분 매각 '촉각', 현대엔지니어링 몸값 10조?...'맏형' 현대건설 쑥스럽겠네, 현대모빌리티지주? 예상해본 정의선의 현대차그룹 지배구조 개편 '빅 픽처'</t>
   </si>
   <si>
-    <t>'시장의 공감'이 화두 된 주요 그룹 지배구조 개편, ‘액면분할’ 카카오 주가 7.59% 상승… 김범수 “5000억원대 매각”, 캐시 우드, 테슬라 팔고 코인베이스 샀다…2800억 수익, 빨라진 현대차 지배구조 개편 시계…글로비스 지분 활용 방안 수면 위로, 정의선의 지배구조 개편 ‘신호탄’…실적회복 바빠진 현대글로비스, 정의선 회장 지분 보유 계열사 ‘몸값 올리기’ 분주, "SK이노베이션, LG화학에 2조원 주고 전기차 운전석 안착" 비정상적인 비즈니스는 리스크, 현대차-분기 실적 및 전망, 21년도 1분기 영업이익은 1.52조원(+75.8% 전년 대비 증감율, OPM 5.4%), 컨센서스 0.8% 하회 전망, 반도체 수급 불안 이슈가 업종 전반 Valuation 하방 압력을 주고 있으나, 현 주가에서는 부정적 이슈 보다 긍정적 이슈에 주가 회복을 민감하게 할 것으로 판단</t>
+    <t>'시장의 공감'이 화두 된 주요 그룹 지배구조 개편, ‘액면분할’ 카카오 주가 7.59% 상승… 김범수 “5000억원대 매각”, 캐시 우드, 테슬라 팔고 코인베이스 샀다…2800억 수익, 빨라진 현대차 지배구조 개편 시계…글로비스 지분 활용 방안 수면 위로, 정의선의 지배구조 개편 ‘신호탄’…실적회복 바빠진 현대글로비스, 정의선 회장 지분 보유 계열사 ‘몸값 올리기’ 분주, "SK이노베이션, LG화학에 2조원 주고 전기차 운전석 안착" 비정상적인 비즈니스는 리스크, 분기 실적 및 전망, 21년도 1분기 영업이익은 1.52조원(+75.8% 전년 대비 증감율, OPM 5.4%), 컨센서스 0.8% 하회 전망, 반도체 수급 불안 이슈가 업종 전반 Valuation 하방 압력을 주고 있으나, 현 주가에서는 부정적 이슈 보다 긍정적 이슈에 주가 회복을 민감하게 할 것으로 판단</t>
   </si>
   <si>
     <t>삼성SDI, '테슬라 대항마' 리비안 고객사 확보·'애플카 유력후보' 마그나 "LG 모터·인버터 쓴 이빔 출시"(4월2주차)</t>
@@ -6874,10 +6874,10 @@
     <t>20일 장 마감 후 주요 공시, 현대차그룹, 해묵은 순환출자 고리 끊어내나...정의선 지분 방향은, 현대차 임원들 애플카 알고 팔았나…금융당국 조사, 구주 매출 유력…정의선 회장 지분 얼마나 나올까, 현대글로비스 주식 매수의견 유지, "현금 풍부해 신사업 투자 서둘러", 큐캐피탈, 서진오토모티브 EB로 40억대 수익, 50대그룹 총수 지난해 배당금만 1조7800억 원...이건희, 이재용 60% 차지</t>
   </si>
   <si>
-    <t>현대차-년도년도 2분기 1분기 리뷰: 금융사업 호조와 모델 믹스 개선효과, 기대 이상의 년도년도 2분기 1분기 영업이익은 향후 이익 전망에 긍정적, 금융사업의 호조와 기대 이상의 모델 믹스 개선 효과가 영업이익이 기대를 상회한 이유, 년도년도 2분기 2분기 이후 반도체 관련 영향 본격화되겠으나 누적 3,620억원의 비용을 발생시키는 수준으로 추정, EV경쟁력 제고 방안, 니콜라 '사기의혹'에 한화그룹 승계작업 '미묘한 기류', '반도체 수급 불안' 현대차, 2분기 관전법, 현대차, 고급차 수요 증가로 1분기 이익 4년 만에 3배 증가, 이재용 측 "삼성물산·제일모직 합병은 적법한 경영활동...불법행위 없었다"</t>
-  </si>
-  <si>
-    <t>현대차 주식 매수의견 유지, "평균판매가격 높아져 올해 실적 좋아져", "현대차, 車 반도체 부족 하반기엔 완화될 듯"...신한금융투자, 전기차 스타트업 카누, 새로운 CEO로 토니 아퀼라 선임, 현대차-21년도 1분기 Review: 높아진 눈높이, 차별화를 원한다, 견조한 실적, 글로벌 자동차, 모두 다 Level-up 된 주가, 현대차-물 들어오는데 노 좀 모자라면 어때, 1분기 영업이익 컨센서스 7% 상회, 차량용 반도체 부족의 핵심은 강한 수요회복, 현대차-반도체 차질이면 뭐하니?, 21년도 1분기 영업이익은 1.66조원(+91.8% 전년 대비 증감율, OPM 6.0%) 기록, 컨센서스 6.6% 상회 차량용 반도체 공급 차질로 주가는 전반적으로 하방 압력을 받고 있으나 4월 중 일부 공장에서 나타난 제한적 셧다운과 유사하거나 소폭 심화된 수준의 5월 생산 전망, 현대차- 금융 부문 호조로 시장 기대치 상회, 년도년도 2분기 1분기 Review: 시장 기대치 상회, 현대차-장기 지속가능성에 대해 신뢰, 중장기 주가 재평가 지속 전망: 어닝 모멘텀 + 성공적인 사업구조 전환, 1분기 Review: 올해 금융부문은 두 자릿수 영업이익률 회복 전망, 현대차-다 좋다, 21년도 1분기 실적, 시장 기대치 상회, 21년도 2분기 반도체 영향 감안해도, 시장 기대치 상회 실적 전망, 21년도 하반기 e-GMP 모델 판매 확대/세대 통합제어기 상용화에 주목, 현대차-년도년도 2분기 1분기 Review: 시작에 불과한 실적, 년도년도 2분기 1분기 Review: 기대치 상회한 호실적, 배터리 기술 개발에 박차, 1분기 실적 개선은 시작에 불과, 현대차-이제부터 중요한 것은 물량 효과, 21년도 1분기 연결매출 27조원, 영업이익 1,657십억원, OPM 6%, 결국 물량 회복이 실적을 좌우하는 상황, 반도체 수급 불균형은 6월 이후 완화, 현대차-물 들어오는데 노 좀 모자라면 어때, 1분기 영업이익 컨센서스 7% 상회, 차량용 반도체 부족의 핵심은 강한 수요회복, 현대차-년도년도 2분기 1분기 Review-금융부문의 서프라이즈와 지속되는 믹스개선 효과, 년도년도 2분기 1분기 Review ? 금융부문의 서프라이즈와 지속되는 믹스개선 효과, 현대차-실적이 수급 우려 해소, 21년도 1분기 , 기대치 상회, 과도한 반도체 우려, 여전히 저평가 구간, 현대차-대외 악재에도 굳건, 21년도 1분기 영업이익 1.66조원(+91.8%)으로 기대치 상회, 21년도 2분기 감산해도 연간 호실적에 영향 X, 현대차-21년도 1분기 Review: 높아진 눈높이, 차별화를 원한다, 견조한 실적, 글로벌 자동차, 모두 다 Level-up 된 주가, 현대차-년도년도 2분기 1분기 Review-금융부문의 서프라이즈와 지속되는 믹스개선 효과, 년도년도 2분기 1분기 Review ? 금융부문의 서프라이즈와 지속되는 믹스개선 효과, 현대차-반도체 차질이면 뭐하니?, 21년도 1분기 영업이익은 1.66조원(+91.8% 전년 대비 증감율, OPM 6.0%) 기록, 컨센서스 6.6% 상회 차량용 반도체 공급 차질로 주가는 전반적으로 하방 압력을 받고 있으나 4월 중 일부 공장에서 나타난 제한적 셧다운과 유사하거나 소폭 심화된 수준의 5월 생산 전망, 현대차- 금융 부문 호조로 시장 기대치 상회, 년도년도 2분기 1분기 Review: 시장 기대치 상회, 현대차-장기 지속가능성에 대해 신뢰, 중장기 주가 재평가 지속 전망: 어닝 모멘텀 + 성공적인 사업구조 전환, 1분기 Review: 올해 금융부문은 두 자릿수 영업이익률 회복 전망, 현대차-다 좋다, 21년도 1분기 실적, 시장 기대치 상회, 21년도 2분기 반도체 영향 감안해도, 시장 기대치 상회 실적 전망, 21년도 하반기 e-GMP 모델 판매 확대/세대 통합제어기 상용화에 주목, 현대차-년도년도 2분기 1분기 Review: 시작에 불과한 실적, 년도년도 2분기 1분기 Review: 기대치 상회한 호실적, 배터리 기술 개발에 박차, 1분기 실적 개선은 시작에 불과, 현대차-이제부터 중요한 것은 물량 효과, 21년도 1분기 연결매출 27조원, 영업이익 1,657십억원, OPM 6%, 결국 물량 회복이 실적을 좌우하는 상황, 반도체 수급 불균형은 6월 이후 완화</t>
+    <t>년도년도 2분기 1분기 리뷰: 금융사업 호조와 모델 믹스 개선효과, 기대 이상의 년도년도 2분기 1분기 영업이익은 향후 이익 전망에 긍정적, 금융사업의 호조와 기대 이상의 모델 믹스 개선 효과가 영업이익이 기대를 상회한 이유, 년도년도 2분기 2분기 이후 반도체 관련 영향 본격화되겠으나 누적 3,620억원의 비용을 발생시키는 수준으로 추정, EV경쟁력 제고 방안, 니콜라 '사기의혹'에 한화그룹 승계작업 '미묘한 기류', '반도체 수급 불안' 현대차, 2분기 관전법, 현대차, 고급차 수요 증가로 1분기 이익 4년 만에 3배 증가, 이재용 측 "삼성물산·제일모직 합병은 적법한 경영활동...불법행위 없었다"</t>
+  </si>
+  <si>
+    <t>현대차 주식 매수의견 유지, "평균판매가격 높아져 올해 실적 좋아져", "현대차, 車 반도체 부족 하반기엔 완화될 듯"...신한금융투자, 전기차 스타트업 카누, 새로운 CEO로 토니 아퀼라 선임, 21년도 1분기 Review: 높아진 눈높이, 차별화를 원한다, 견조한 실적, 글로벌 자동차, 모두 다 Level-up 된 주가, 물 들어오는데 노 좀 모자라면 어때, 1분기 영업이익 컨센서스 7% 상회, 차량용 반도체 부족의 핵심은 강한 수요회복, 반도체 차질이면 뭐하니?, 21년도 1분기 영업이익은 1.66조원(+91.8% 전년 대비 증감율, OPM 6.0%) 기록, 컨센서스 6.6% 상회 차량용 반도체 공급 차질로 주가는 전반적으로 하방 압력을 받고 있으나 4월 중 일부 공장에서 나타난 제한적 셧다운과 유사하거나 소폭 심화된 수준의 5월 생산 전망, 금융 부문 호조로 시장 기대치 상회, 년도년도 2분기 1분기 Review: 시장 기대치 상회, 장기 지속가능성에 대해 신뢰, 중장기 주가 재평가 지속 전망: 어닝 모멘텀 + 성공적인 사업구조 전환, 1분기 Review: 올해 금융부문은 두 자릿수 영업이익률 회복 전망, 다 좋다, 21년도 1분기 실적, 시장 기대치 상회, 21년도 2분기 반도체 영향 감안해도, 시장 기대치 상회 실적 전망, 21년도 하반기 e-GMP 모델 판매 확대/세대 통합제어기 상용화에 주목, 년도년도 2분기 1분기 Review: 시작에 불과한 실적, 년도년도 2분기 1분기 Review: 기대치 상회한 호실적, 배터리 기술 개발에 박차, 1분기 실적 개선은 시작에 불과, 이제부터 중요한 것은 물량 효과, 21년도 1분기 연결매출 27조원, 영업이익 1,657십억원, OPM 6%, 결국 물량 회복이 실적을 좌우하는 상황, 반도체 수급 불균형은 6월 이후 완화, 물 들어오는데 노 좀 모자라면 어때, 1분기 영업이익 컨센서스 7% 상회, 차량용 반도체 부족의 핵심은 강한 수요회복, 년도년도 2분기 1분기 Review-금융부문의 서프라이즈와 지속되는 믹스개선 효과, 년도년도 2분기 1분기 Review ? 금융부문의 서프라이즈와 지속되는 믹스개선 효과, 실적이 수급 우려 해소, 21년도 1분기 , 기대치 상회, 과도한 반도체 우려, 여전히 저평가 구간, 대외 악재에도 굳건, 21년도 1분기 영업이익 1.66조원(+91.8%)으로 기대치 상회, 21년도 2분기 감산해도 연간 호실적에 영향 X, 21년도 1분기 Review: 높아진 눈높이, 차별화를 원한다, 견조한 실적, 글로벌 자동차, 모두 다 Level-up 된 주가, 년도년도 2분기 1분기 Review-금융부문의 서프라이즈와 지속되는 믹스개선 효과, 년도년도 2분기 1분기 Review ? 금융부문의 서프라이즈와 지속되는 믹스개선 효과, 반도체 차질이면 뭐하니?, 21년도 1분기 영업이익은 1.66조원(+91.8% 전년 대비 증감율, OPM 6.0%) 기록, 컨센서스 6.6% 상회 차량용 반도체 공급 차질로 주가는 전반적으로 하방 압력을 받고 있으나 4월 중 일부 공장에서 나타난 제한적 셧다운과 유사하거나 소폭 심화된 수준의 5월 생산 전망, 금융 부문 호조로 시장 기대치 상회, 년도년도 2분기 1분기 Review: 시장 기대치 상회, 장기 지속가능성에 대해 신뢰, 중장기 주가 재평가 지속 전망: 어닝 모멘텀 + 성공적인 사업구조 전환, 1분기 Review: 올해 금융부문은 두 자릿수 영업이익률 회복 전망, 다 좋다, 21년도 1분기 실적, 시장 기대치 상회, 21년도 2분기 반도체 영향 감안해도, 시장 기대치 상회 실적 전망, 21년도 하반기 e-GMP 모델 판매 확대/세대 통합제어기 상용화에 주목, 년도년도 2분기 1분기 Review: 시작에 불과한 실적, 년도년도 2분기 1분기 Review: 기대치 상회한 호실적, 배터리 기술 개발에 박차, 1분기 실적 개선은 시작에 불과, 이제부터 중요한 것은 물량 효과, 21년도 1분기 연결매출 27조원, 영업이익 1,657십억원, OPM 6%, 결국 물량 회복이 실적을 좌우하는 상황, 반도체 수급 불균형은 6월 이후 완화</t>
   </si>
   <si>
     <t>이케아 카탈로그도 '듣는다'고?, 일진다이아, 하이솔루스로 3년치 매출액 확보, “국내·해외 무관, 주식형펀드 좋다”</t>
@@ -6943,34 +6943,34 @@
     <t>'한미회담 훈풍' 국내 증시 살릴까…"코스피 3,700도 기대"</t>
   </si>
   <si>
-    <t>현대차-차별화된 모빌리티/서비스로 밸류 에드 가능, 2021년 제네시스 확대와 아이오닉5 전기차 본격 론칭, 차별화된 모빌리티/서비스로 밸류 에드 가능, 투자의견 매수(유지), 목표주가 350,000(상향), 현대차-Smart Mobility Solution Provider를 향해, 중장기 자율주행 및 모빌리티 전략 점검 및 투자판단, 2025년까지는 미래 수익성 창출 기반을 구축하는 구간으로 이해, 자율주행 측면에서는 2021년말 신형 G90부터 Level 3 최초 적용 예정, (세모이배월)코엔텍, 버는 족족 배당하는 ‘배당몰빵주’, 이베스트 윤지호 센터장 "굳이 三電? 차라리 현대차…가치주가 답", &lt;국미연 특강&gt; 美 통화정책 및 인플레 논란, 시장 함의는?, 아니라는데…HMM, '매각설' 계속되는 이유</t>
-  </si>
-  <si>
-    <t>증시 불안정에 자금 부동화 뚜렷 外, 현대차-미국 진출 시나리오 가시화, 밸류에이션 상승 기대, 미국 전기차 투자 본격화, 미래 M/S 확대의 결정적 근거 확보, 반도체 공급 영향 Peak 는 5 월 예상, 실적우려는 6 월부터 완화, 투자의견 Buy, 목표주가 330,000 원 유지. 자동차 섹터 Top Pick</t>
-  </si>
-  <si>
-    <t>현대차-현대라는 브랜드 가치가 높아지는 중, 하반기에도 실적 모멘텀이 유지되는 가운데, Valuation 재평가가 진행될 것, 2025년 종합 모빌리티 솔루션을 제공하는 회사가 전략적 지향점, 자율주행에 대한 로드맵도 착실히 밟아가는 중, 현대차-모빌리티 디바이스 전략의 중심, 승차 공유 업체와의 협업 전개 시작 → 서비스 비즈니스 모델 확보 가시성 증가, 초과 수요 시장 환경 속 판매량 증가 ? 판매가격 상승 동반 → 21년 연간 EPS 컨센서스 +11% 상회 전망, 투자의견 Buy 유지 ? 적정주가 320,000원으로 상향, 최창원 SK디스커버리 대표이사 부회장, HMM 매각 적기는 언제일까, 공모주 열풍 흔들?…5월 새내기주 성적표 '우울'</t>
+    <t>차별화된 모빌리티/서비스로 밸류 에드 가능, 2021년 제네시스 확대와 아이오닉5 전기차 본격 론칭, 차별화된 모빌리티/서비스로 밸류 에드 가능, 투자의견 매수(유지), 목표주가 350,000(상향), Smart Mobility Solution Provider를 향해, 중장기 자율주행 및 모빌리티 전략 점검 및 투자판단, 2025년까지는 미래 수익성 창출 기반을 구축하는 구간으로 이해, 자율주행 측면에서는 2021년말 신형 G90부터 Level 3 최초 적용 예정, (세모이배월)코엔텍, 버는 족족 배당하는 ‘배당몰빵주’, 이베스트 윤지호 센터장 "굳이 三電? 차라리 현대차…가치주가 답", &lt;국미연 특강&gt; 美 통화정책 및 인플레 논란, 시장 함의는?, 아니라는데…HMM, '매각설' 계속되는 이유</t>
+  </si>
+  <si>
+    <t>증시 불안정에 자금 부동화 뚜렷 外, 미국 진출 시나리오 가시화, 밸류에이션 상승 기대, 미국 전기차 투자 본격화, 미래 M/S 확대의 결정적 근거 확보, 반도체 공급 영향 Peak 는 5 월 예상, 실적우려는 6 월부터 완화, 투자의견 Buy, 목표주가 330,000 원 유지. 자동차 섹터 Top Pick</t>
+  </si>
+  <si>
+    <t>현대라는 브랜드 가치가 높아지는 중, 하반기에도 실적 모멘텀이 유지되는 가운데, Valuation 재평가가 진행될 것, 2025년 종합 모빌리티 솔루션을 제공하는 회사가 전략적 지향점, 자율주행에 대한 로드맵도 착실히 밟아가는 중, 모빌리티 디바이스 전략의 중심, 승차 공유 업체와의 협업 전개 시작 → 서비스 비즈니스 모델 확보 가시성 증가, 초과 수요 시장 환경 속 판매량 증가 ? 판매가격 상승 동반 → 21년 연간 EPS 컨센서스 +11% 상회 전망, 투자의견 Buy 유지 ? 적정주가 320,000원으로 상향, 최창원 SK디스커버리 대표이사 부회장, HMM 매각 적기는 언제일까, 공모주 열풍 흔들?…5월 새내기주 성적표 '우울'</t>
   </si>
   <si>
     <t>美 헤지펀드 "삼성·현대차 등 韓기업 주가 상승 여력 충분", '형보다 아우가 낫네' 현대·LG그룹주 펀드 삼성그룹주 수익률 넘어서, 배당 확 줄이고 자사주 사들인다는데…'배당 맛집' 메리츠의 변심?, 모비스, 지배력 확대 방안은</t>
   </si>
   <si>
-    <t>국내 기업보다 더 많은 외국인 배당금, 현대차-금융 호조 &gt; 감산, 중고차 가격 상승에 연동될 호실적, 통제 불능의 공급 차질은 없었다</t>
+    <t>국내 기업보다 더 많은 외국인 배당금, 금융 호조 &gt; 감산, 중고차 가격 상승에 연동될 호실적, 통제 불능의 공급 차질은 없었다</t>
   </si>
   <si>
     <t>이주의 주식시장은? 메타버스 관련주, 러 백신 테마주 급등... 한미 정상회담 이후 미사일·원전 관련주 강세, 남양유업 매각 소식에 상한가</t>
   </si>
   <si>
-    <t>한화그룹, 지주사 전환 못하는 이유, 수출·제조업에 쏠린 '한국 증시'…"주식시장 대외 충격 취약", 한은 "한국 증시, '수출-제조업' 주로 대표…대외충격 취약", 한은 "주식시장, 실물경제 제대로 반영 못해", 한은 "국내 주식시장 제조업 위주…실물경제 반영 한계", 韓주식시장, 제조업 68.6% 차지…"실물경제 충격 반영 못해", 한은 “주식시장, 제조·상장기업 대표해 실물 경제와 괴리”, 현대차-실적, 제네시스 EV 출시가 주가 상승 동력, 차량용 반도체 수급 차질로 인한 생산 대란, 판매/금융 부문에는 호재, 제네시스 EV 출시</t>
-  </si>
-  <si>
-    <t>'애플카'로 거액 차익…현대차 임원 5명 더 있다, 경기회복기 '종합선물세트' 롯데지주의 재발견, 워런 버핏의 성공투자 핵심 포인트, 현대차-하반기 전망: 이제 볼륨 성장도 기대할 수 있다, 기타신흥시장 수요성장에 주목, 현대차, 금융부분 실적 호조 전망</t>
+    <t>한화그룹, 지주사 전환 못하는 이유, 수출·제조업에 쏠린 '한국 증시'…"주식시장 대외 충격 취약", 한은 "한국 증시, '수출-제조업' 주로 대표…대외충격 취약", 한은 "주식시장, 실물경제 제대로 반영 못해", 한은 "국내 주식시장 제조업 위주…실물경제 반영 한계", 韓주식시장, 제조업 68.6% 차지…"실물경제 충격 반영 못해", 한은 “주식시장, 제조·상장기업 대표해 실물 경제와 괴리”, 실적, 제네시스 EV 출시가 주가 상승 동력, 차량용 반도체 수급 차질로 인한 생산 대란, 판매/금융 부문에는 호재, 제네시스 EV 출시</t>
+  </si>
+  <si>
+    <t>'애플카'로 거액 차익…현대차 임원 5명 더 있다, 경기회복기 '종합선물세트' 롯데지주의 재발견, 워런 버핏의 성공투자 핵심 포인트, 하반기 전망: 이제 볼륨 성장도 기대할 수 있다, 기타신흥시장 수요성장에 주목, 현대차, 금융부분 실적 호조 전망</t>
   </si>
   <si>
     <t>성과급, 오너 배당...현대엔지니어링의 계산법, "'애플카로 거액 차익' 현대차 임원 5명 추가 조사 중", 현대차 영업실적 잠정 공시 외, '애플카'로 거액 차익…현대차 임원 5명 더 있다?, 호랑이의 등, CJ CGV, 2100억 '영구 CB' 흥행 예고</t>
   </si>
   <si>
-    <t>공매도 재개 한달차… 뚜껑 여니 영향 ‘미미’, '카카오·GS25' 논란 커진 이유…MZ세대 "이건 아니잖아!", 현대차-하반기 투자유망종목, 성공적인 신차 효과와 사업구조 전환 기대감이 중장기 주가 상승 동력, 장기 ROE(자기자본이익률) 상승 전환 초기 국면, Clean mobility 분야에서는 2021년부터 전기차 전용플랫폼(E-GMP) 도입에 따른 전기차 시장 대응능력 향상 기대, 현대차 주식 매수의견 유지, "친환경차 중심으로 사업구조 전환"</t>
+    <t>공매도 재개 한달차… 뚜껑 여니 영향 ‘미미’, '카카오·GS25' 논란 커진 이유…MZ세대 "이건 아니잖아!", 하반기 투자유망종목, 성공적인 신차 효과와 사업구조 전환 기대감이 중장기 주가 상승 동력, 장기 ROE(자기자본이익률) 상승 전환 초기 국면, Clean mobility 분야에서는 2021년부터 전기차 전용플랫폼(E-GMP) 도입에 따른 전기차 시장 대응능력 향상 기대, 현대차 주식 매수의견 유지, "친환경차 중심으로 사업구조 전환"</t>
   </si>
   <si>
     <t>'ESG 리더' 노리는 정의선…친환경과 협력사 상생으로 ESG 경영 가속화, "테이퍼링·중간배당"에 은행·금융株 주목...위기의 테슬라 "주가 500달러대" 外, 삼성증권, 현대차 목표가 내리자마자…골드만삭스 "현기차 사라", 금융위 “공매도 재개 한달 동안 주가와 연관성 없는 걸로 보여”</t>
@@ -6991,13 +6991,13 @@
     <t>해운업 청신호 켜졌는데... HMM 민영화에 산은 '고심', '반도체·車·여행주 증시 순환매'에 주도주 촉각..공모주, 하반기 수익률 주목 外, ‘Safer, Faster, Longer’ 배터리로 ‘글로벌 3위’ 급부상</t>
   </si>
   <si>
-    <t>K대주시스템 10월 서비스 확정...개인 공매도 확산은 '갸우뚱', 현대차-다시 한 번 비상을 꿈꾸다, 2분기 영업이익 1.87조원을 전망, 내수 시장 점유율 확대 및 제네시스 판매 호조세 지속, 하반기 아이오닉5 출고 본격화, 미국 GV70, 싼타크루즈 출시 등 신차 모먼텀은 이어질 전망</t>
+    <t>K대주시스템 10월 서비스 확정...개인 공매도 확산은 '갸우뚱', 다시 한 번 비상을 꿈꾸다, 2분기 영업이익 1.87조원을 전망, 내수 시장 점유율 확대 및 제네시스 판매 호조세 지속, 하반기 아이오닉5 출고 본격화, 미국 GV70, 싼타크루즈 출시 등 신차 모먼텀은 이어질 전망</t>
   </si>
   <si>
     <t>쌍방울 상한가, 쎄미시스코 다시 상한가로 부활, 대한전선 반등 성공... 시멘트주 강세 속 삼성제약·네이처셀 급등, 현대자 주식 매수의견 유지, "국내 점유율 오르고 미국 호조 지속", 국민연금의 기업투자, 경영간섭 경계해야</t>
   </si>
   <si>
-    <t>"현대차, 2분기 반도체 부족 영향 털어낼 듯"...KB증권, 현대차-년도년도 2분기 2분기 프리뷰: 반도체 부족 영향, 가볍게 털어낼 것, 년도년도 2분기 2분기 영업이익 1.9조원 (+215.0% 전년 대비 증감율) 예상. 시장 컨센서스 2.9% 상회할 것, 2021년 영업이익 6.6조원 (+173.9% 전년 대비 증감율). 반도체 문제에도 손익 영향 미미할 것, 리스크 요인: ① 투자 현금유출 증가, ② 원자재 가격 상승, ③ 원화가치 절상 가능성</t>
+    <t>"현대차, 2분기 반도체 부족 영향 털어낼 듯"...KB증권, 년도년도 2분기 2분기 프리뷰: 반도체 부족 영향, 가볍게 털어낼 것, 년도년도 2분기 2분기 영업이익 1.9조원 (+215.0% 전년 대비 증감율) 예상. 시장 컨센서스 2.9% 상회할 것, 2021년 영업이익 6.6조원 (+173.9% 전년 대비 증감율). 반도체 문제에도 손익 영향 미미할 것, 리스크 요인: ① 투자 현금유출 증가, ② 원자재 가격 상승, ③ 원화가치 절상 가능성</t>
   </si>
   <si>
     <t>언론 효과? 윤석열 후광?... 부인 사업에 협찬사 왜 늘었을까, 산업은행發 전환사채 소식에 HMM 주주들 반응은?, "윤석열과 김경율 만남에" 가비아 '상한가'...“원전활용 불가피” 대창스틸 등 관련주들 '강세' 外, 산은 HMM 매각설 ‘솔솔’ 인수 대상 기업은?</t>
@@ -7033,7 +7033,7 @@
     <t>카뱅·카페이 상장 예고…실손보험 7월부터 바뀐다, 이달에도 매도일색 국민연금 이 종목은 담았다</t>
   </si>
   <si>
-    <t>헬릭스미스, 주주 달래려 '신사업 카드' 꺼냈다, 메타버스 관련주 전성시대, 매출액·기술력에 따른 옥석가리기 필수, 현대차-거인의 어깨에 올라타다, 현대차그룹은 ‘25년까지 미국에 EV 생산설비와 수소, UAM, 로보틱스, 자율주행 등 투자 예정, 미국 전동화 시계가 빨라지고 있다, 최근 4월~5월 시장 우려와 달리 반도체 공급 차질 국면에서 유연한 생산과 재고 소진을 통해 판매 차질을 최소화, 테슬라 Vs 폭스바겐·GM·현대차…미래 전기차 시장 승자는 누구?</t>
+    <t>헬릭스미스, 주주 달래려 '신사업 카드' 꺼냈다, 메타버스 관련주 전성시대, 매출액·기술력에 따른 옥석가리기 필수, 거인의 어깨에 올라타다, 현대차그룹은 ‘25년까지 미국에 EV 생산설비와 수소, UAM, 로보틱스, 자율주행 등 투자 예정, 미국 전동화 시계가 빨라지고 있다, 최근 4월~5월 시장 우려와 달리 반도체 공급 차질 국면에서 유연한 생산과 재고 소진을 통해 판매 차질을 최소화, 테슬라 Vs 폭스바겐·GM·현대차…미래 전기차 시장 승자는 누구?</t>
   </si>
   <si>
     <t>상장 앞두고 '說說說'... 현대ENG 깎아내리기, 근거 있나, 이재용 삼성전자 부회장</t>
@@ -7045,19 +7045,19 @@
     <t>현대차 정의선號 상반기 성적표는?, “카카오 김범수 웃고, 셀트리온 서정진 울고”, 장마에도 화창한 기업 vs 폭우 속에 갇힌 기업</t>
   </si>
   <si>
-    <t>"운명의 날" 헬릭스미스 경영진 교체 vs 해임 반대, 최태원 SK그룹 회장 겸 대한상공회의소 회장, 현대차-시장 기대치 상회하는 영업이익 예상, 년도년도 2분기 2분기 글로벌 도매 전년 대비 증감율 +46% 증가, 년도년도 2분기 2분기 내수 판매 감소에도 불구하고 북미 판매 증가 &amp; 인센트브 축소가 실적 견인, 21년도 하반기 에는 충분한 재고 확보를 통한 북미 &amp; 유럽 수요 회복 대응이 관건, SK이노, 분할로 배터리사업 확대…현대차 투자로 내재화 '시동'</t>
-  </si>
-  <si>
-    <t>현대차-제네시스와 금융에 핀포인트, 21년도 2분기 영업이익 1.9조원으로 성장세 지속 예상, 하반기부터 본격화 될 BEV 모멘텀, 투자의견 Buy, 목표주가 320,000원 신규 제시하며 커버리지 개시, 현대차-미국 시장이 이끄는 실적 기대감, 투자의견 매수(Buy), 목표주가 300,000원 유지, 2021년 2분기 매출 27.4조, 영업이익 1.91조 전망, 인센티브가 지속적으로 감소하고 중고차지수가 최대인 미국시장 주목, ③ 현대차그룹, 순환출자 고리 해결 급선무…개정된 공정거래법 일감몰아주기 규제도 부담, 현대차 2분기 해외 판매 80.9%↑... 최근 한달간 주가는 2.3%↓, 이노션 주식 매수의견 유지, "현대차그룹 마케팅 강화의 수혜 늘어", "코스피, 호실적에 3500 간다"…하반기 노무라 선호株는</t>
-  </si>
-  <si>
-    <t>이노션 하반기 주가, 증권사 전망은?, 현대차-실적 개선과 제네시스 EV, 21년도 2분기 Preview: 판가 상승, 인센티브 하락으로 수익성 개선, 미국 시장이 수익성 개선을 주도, 아이오닉 5 생산량 증가와 제네시스 EV 공개 임박, 공모가 낮춰도 업계 1위, 크래프톤 그만한 가치 있을까?, 현대차-＇Level-up＇ 된 수익성 지속 전망, 생산 차질을 극복한 판매대수 증가, 21년도 하반기 판매대수 2,013천대(중국 제외 1,825천대)전망, 원가 부담 증가가 예상되난 판매가격 인상으로 대응 가능, 현대차-앞으로의 눈높이가 높아질 시점, 21년도 2분기 영업이익은 1.84조원(+212.1% 전년 대비 증감율, OPM 6.3%)으로 컨센서스 부합 전망, 차량용 반도체 수급 차질은 5월 저점으로 점진 회복 전망, 현대차 주식 매수의견 유지, "제네시스 전기차 3분기 공개 기대", '황금알 거위'에서 '애물단지'로 전락한 테슬라</t>
+    <t>"운명의 날" 헬릭스미스 경영진 교체 vs 해임 반대, 최태원 SK그룹 회장 겸 대한상공회의소 회장, 시장 기대치 상회하는 영업이익 예상, 년도년도 2분기 2분기 글로벌 도매 전년 대비 증감율 +46% 증가, 년도년도 2분기 2분기 내수 판매 감소에도 불구하고 북미 판매 증가 &amp; 인센트브 축소가 실적 견인, 21년도 하반기 에는 충분한 재고 확보를 통한 북미 &amp; 유럽 수요 회복 대응이 관건, SK이노, 분할로 배터리사업 확대…현대차 투자로 내재화 '시동'</t>
+  </si>
+  <si>
+    <t>제네시스와 금융에 핀포인트, 21년도 2분기 영업이익 1.9조원으로 성장세 지속 예상, 하반기부터 본격화 될 BEV 모멘텀, 투자의견 Buy, 목표주가 320,000원 신규 제시하며 커버리지 개시, 미국 시장이 이끄는 실적 기대감, 투자의견 매수(Buy), 목표주가 300,000원 유지, 2021년 2분기 매출 27.4조, 영업이익 1.91조 전망, 인센티브가 지속적으로 감소하고 중고차지수가 최대인 미국시장 주목, ③ 현대차그룹, 순환출자 고리 해결 급선무…개정된 공정거래법 일감몰아주기 규제도 부담, 현대차 2분기 해외 판매 80.9%↑... 최근 한달간 주가는 2.3%↓, 이노션 주식 매수의견 유지, "현대차그룹 마케팅 강화의 수혜 늘어", "코스피, 호실적에 3500 간다"…하반기 노무라 선호株는</t>
+  </si>
+  <si>
+    <t>이노션 하반기 주가, 증권사 전망은?, 실적 개선과 제네시스 EV, 21년도 2분기 Preview: 판가 상승, 인센티브 하락으로 수익성 개선, 미국 시장이 수익성 개선을 주도, 아이오닉 5 생산량 증가와 제네시스 EV 공개 임박, 공모가 낮춰도 업계 1위, 크래프톤 그만한 가치 있을까?, ＇Level-up＇ 된 수익성 지속 전망, 생산 차질을 극복한 판매대수 증가, 21년도 하반기 판매대수 2,013천대(중국 제외 1,825천대)전망, 원가 부담 증가가 예상되난 판매가격 인상으로 대응 가능, 앞으로의 눈높이가 높아질 시점, 21년도 2분기 영업이익은 1.84조원(+212.1% 전년 대비 증감율, OPM 6.3%)으로 컨센서스 부합 전망, 차량용 반도체 수급 차질은 5월 저점으로 점진 회복 전망, 현대차 주식 매수의견 유지, "제네시스 전기차 3분기 공개 기대", '황금알 거위'에서 '애물단지'로 전락한 테슬라</t>
   </si>
   <si>
     <t>② 스마트 개미, 반도체로 쓰린 투심 플랫폼으로 달랬다</t>
   </si>
   <si>
-    <t>크래프톤, ‘배틀그라운드’ 단편영화 공개…‘한국의 마블’ 될 수 있을까, 현대차-북미가 캐리, 21년도 2분기 , 컨센서스 상회 전망, 하반기 북미가 캐리, 실적에 주목, '친환경차 심장에 탑재"...동양피스톤, 수소전기차 부품 공급에 투자자 관심 증가, LG·현대차·구글·HMM</t>
+    <t>크래프톤, ‘배틀그라운드’ 단편영화 공개…‘한국의 마블’ 될 수 있을까, 북미가 캐리, 21년도 2분기 , 컨센서스 상회 전망, 하반기 북미가 캐리, 실적에 주목, '친환경차 심장에 탑재"...동양피스톤, 수소전기차 부품 공급에 투자자 관심 증가, LG·현대차·구글·HMM</t>
   </si>
   <si>
     <t>올 상반기 주식 부자 1위는 이재용, 김범수 카카오 의장은 3위</t>
@@ -7066,16 +7066,16 @@
     <t>‘어떤 주식 나올까?’ 편의점 도시락 사면 주식 준다, 이마트24 “도시락 사면 삼전 주식 1주 드려요”</t>
   </si>
   <si>
-    <t>현대차 주식 매수의견 유지, "생산 정상화와 신흥국 수요 증가 전망", 41만 네이버, 23만 현대차, 8만 삼성전자 주식... 4900원 도시락 하나면 받을 수 있다 (공식), 현대차-년도년도 2분기 2분기 Preview: 금융사업 통해 이익모멘텀 확보, 년도년도 2분기 2분기 Preview: 영업이익 1.95조원 예상, 금융부문이 이익 견인, 21년도 하반기 최대 관전 포인트는 결국 미국내 높은 판매흐름 지속, 투자의견 Buy, 목표주가 330,000원 유지. 비중확대 전략 유효, HMM 주가 '제2의 변곡점' 오나</t>
-  </si>
-  <si>
-    <t>삼성 8만전자에 펀드도 발목잡혔다, BTS 아버지 방시혁, 자산 2배 급증 3조 7000억 원...연예계 부호들 자산은?, 현대차-단기 우려보다 이후의 성장에 주목, 단기 우려보다 이후의 성장에 주목, 5000만 계좌시대, 증권사 '핀셋 마케팅'</t>
-  </si>
-  <si>
-    <t>41만원 주식 공짜로 드려요… 오늘(14일) 출시되는 4900원 도시락 (공식), 비나텍, '주가 4%↑' 수소연료전지 신공장 건립 추진, SD바이오센서,유가증권 시장 상장...에이치엘비파워, 바이오 사업 진출 본격화 外, 현대차-본업과 부업 모두 편안, 21년도 2분기 매출 28.6조원/OP 1.8조원(OPM 6.3%), ‘21년 매출 119조원(+14.4%)/OP 7.3조원(OPM 6.1%), 현대차 투자의견 BUY, 목표주가 30만원</t>
-  </si>
-  <si>
-    <t>현대차-기대되는 하반기, 21년도 2분기 실적 Preview, 21년도 하반기 실적 개선세 지속 예상, 투자의견 ‘Buy’, 목표주가 300,000원 유지, 이마트24, 도시락 사면 주식을? 주문 폭주로 이틀만에 행사 끝날듯, 시동 꺼진 현대차 주가…"하반기 성장에 베팅해야", '조창걸家 사익편취 논란' 한샘 계열사 지분 향방은?</t>
+    <t>현대차 주식 매수의견 유지, "생산 정상화와 신흥국 수요 증가 전망", 41만 네이버, 23만 현대차, 8만 삼성전자 주식... 4900원 도시락 하나면 받을 수 있다 (공식), 년도년도 2분기 2분기 Preview: 금융사업 통해 이익모멘텀 확보, 년도년도 2분기 2분기 Preview: 영업이익 1.95조원 예상, 금융부문이 이익 견인, 21년도 하반기 최대 관전 포인트는 결국 미국내 높은 판매흐름 지속, 투자의견 Buy, 목표주가 330,000원 유지. 비중확대 전략 유효, HMM 주가 '제2의 변곡점' 오나</t>
+  </si>
+  <si>
+    <t>삼성 8만전자에 펀드도 발목잡혔다, BTS 아버지 방시혁, 자산 2배 급증 3조 7000억 원...연예계 부호들 자산은?, 단기 우려보다 이후의 성장에 주목, 단기 우려보다 이후의 성장에 주목, 5000만 계좌시대, 증권사 '핀셋 마케팅'</t>
+  </si>
+  <si>
+    <t>41만원 주식 공짜로 드려요… 오늘(14일) 출시되는 4900원 도시락 (공식), 비나텍, '주가 4%↑' 수소연료전지 신공장 건립 추진, SD바이오센서,유가증권 시장 상장...에이치엘비파워, 바이오 사업 진출 본격화 外, 본업과 부업 모두 편안, 21년도 2분기 매출 28.6조원/OP 1.8조원(OPM 6.3%), ‘21년 매출 119조원(+14.4%)/OP 7.3조원(OPM 6.1%), 현대차 투자의견 BUY, 목표주가 30만원</t>
+  </si>
+  <si>
+    <t>기대되는 하반기, 21년도 2분기 실적 Preview, 21년도 하반기 실적 개선세 지속 예상, 투자의견 ‘Buy’, 목표주가 300,000원 유지, 이마트24, 도시락 사면 주식을? 주문 폭주로 이틀만에 행사 끝날듯, 시동 꺼진 현대차 주가…"하반기 성장에 베팅해야", '조창걸家 사익편취 논란' 한샘 계열사 지분 향방은?</t>
   </si>
   <si>
     <t>도시락·유튜브·메타버스… MZ세대 공략하는 금융사들, 51일 만에 돌아온 아시아나항공 ‘강세’…美증시, 파월 완화 기조 유지에 ‘혼조’, 삼프로TV 염승환 “한국은 美 최고의 파트너....중국 제조업 자리 꿰찰 것”</t>
@@ -7093,13 +7093,13 @@
     <t>더 달라는 노조 요구에 임단협 '난항'…현대차, 파업 분수령, 현대차 노사 오늘 협상 마지노선... "줄 것 다줬는데", 주식 vs 정년연장…GM노조도 쟁의권, 파업 가나?, 주가 주춤에 삼성그룹주 펀드 ‘한숨’…현대차-LG ‘함박웃음’</t>
   </si>
   <si>
-    <t>일진하이솔루스 "수소탱크로 수소시대 앞당깁니다", 노사관계·MZ 퇴사… 현대차, 역대급 실적에도 ‘시름’, 박용진 "민주당 당대표가 김어준? 내가 새물결 이끈다", '넘치는 곳간' SNT모티브, '동향기업' BNK지주 매입, 현대차-년도년도 2분기 2분기 영업손익 전망 업데이트 - 금융부문 호실적 예상, 년도년도 2분기 2분기 영업이익 2.1조원 (+252.0% 전년 대비 증감율) 예상. 시장 컨센서스를 9.0% 상회할 것, 투자포인트: 1) 금융부문 영업이익률 상승, 2) 현대차 점유율 상승, 3) 향상된 수익성, 리스크요인: 1) 원자재 가격 상승, 2) 원화 평가 절상</t>
-  </si>
-  <si>
-    <t>현대차-년도년도 2분기 2분기 리뷰: 시장 기대치를 소폭 하회, 년도년도 2분기 2분기 영업이익 시장 기대를 소폭 하회. 년도년도 2분기 3분기 에는 신형 전기차에 주목할요,년도 분기 년도년도 2분기 2분기 실적 핵심: 예상 밖 판매보증비 증가, 가마감 대비 적었던 판매대수, 예상보다 좋았던 믹스, 년도년도 2분기 3분기 전망: 일부 모델 재고 부족으로 판매에 부정적 영향이 있을 수 있음. Ioniq 5 생산 확대에 주목, 현대차-아쉬울 것 없는 실적, 21년도 2분기 영업이익 1조8,860억원(전년 대비 증감율 +219%, OPM 6.2%) 기록, 추정치 부합. 자동차 부문 뿐만 아니라 금융부문도 호실적 지속, 재고가 극단적으로 낮아져 있어 물리적인 영향으로 3Q 판매 차질은 일부 감안할 필요. 그러나 북미 위주 자동차 소비심리 강세는 하반기에도 이어질 것으로 기대하므로 incentive 추가 하락 및 ASP 상승기조 지속될 것으로 전망. 완성차 실적호조 연내 지속 예상, 반도체 수급 우려가 peak를 지난 이상, 이제 실적 우려는 크지 않고 향후 전개될 미래 모빌리티 전환을 위한 전략 update 등이 중요하다는 판단. EV 판매목표 강화 등이 주가에 모멘텀으로 작용할 전망. 업종 top-pick 의견 및 TP 32만원(12MF PER 10.2x) 유지, 현대차-21년도 2분기 Review: 늘 새로움을 원하는 시장, 금융부문 실적 증가, 하반기 믹스 둔화 우려, 모멘텀을 원하는 시장, "현대해상, 2분기 자동차보험 손해율 개선"...대신증권, 김학균 "금리, 지금 안 올리면 당분간 못 올려", 현대차 노사 잠정합의…3년 연속 무분규 타결 기대, 현대차-높아지는 실적 = 매력적 밸류에이션, 21년도 2분기 , 분기 매출 처음으로 30조원 돌파 ASP 신기록 경신, 기대 이상의 ASP 상승 효과 → 실적 눈높이 우상향 지속</t>
-  </si>
-  <si>
-    <t>현대차-이제부터 물량 효과가 관건, 21년도 2분기 연결 매출 30조원 (전년 대비 증감율+39 %), 영업이익 1,886십억원(전년 대비 증감율+220 %), OPM 6.2%, 21년도 3분기 매출 29조원 (전년 대비 증감율+6%), 영업이익 1.7조원(흑전, OPM 5.9%) 전망, 23일 장 마감, 공매도 거래대금 상위 카카오·SK하이닉스·HMM·LG생활건강·현대차, 현대차-맞바람에도 이 정도, 영업이익 컨센서스 부합, 스트레스 테스트 통과, 현대차 주식 매수의견 유지, "수요 정상화로 하반기 실적 더 좋아져", 팬데믹이 뒤흔든 주식부호 랭킹…1~20위 싹 바뀌었네, '매도가능 물량 33%' 맥스트, SI 결속 유지할까, 대학교 4년 공짜·빈곤층 지원 2배…기본소득 줄 돈으로 할 수 있는 5가지, 현대차-이제부터 물량 효과가 관건, 21년도 2분기 연결 매출 30조원 (전년 대비 증감율+39 %), 영업이익 1,886십억원(전년 대비 증감율+220 %), OPM 6.2%, 21년도 3분기 매출 29조원 (전년 대비 증감율+6%), 영업이익 1.7조원(흑전, OPM 5.9%) 전망, 현대차- 오프로드 무사 통과, 년도년도 2분기 2분기 Review: 시장 기대치 소폭 하회, 투자의견 ‘Buy’, 목표주가 300,000원, 현대차-분기 매출액 30조원 돌파, 공급 안정성 확보로 하반기 펀더멘탈 개선 지속, 2분기 Review: 분기 사상 최대 매출액 기록, 현대차-노사 합의로 하반기 리스크 완화, 21년도 2분기 영업이익은 1.89조원(+219.5% 전년 대비 증감율, OPM 6.2%) 기록, 컨센서스 1.1% 하회, 반도체 공급 차질 완화와 노사 합의로 파업 리스크 해소되며 하반기 생산 확대 전망, 현대차- 오프로드 무사 통과, 년도년도 2분기 2분기 Review: 시장 기대치 소폭 하회, 투자의견 ‘Buy’, 목표주가 300,000원, 현대차-분기 매출액 30조원 돌파, 공급 안정성 확보로 하반기 펀더멘탈 개선 지속, 2분기 Review: 분기 사상 최대 매출액 기록, 현대차-년도년도 2분기 2분기 Review: 피크 실적 우려 완화, 년도년도 2분기 2분기 Review: 전반적으로 컨센서스 부합한 실적, 금융 부문 실적과 판매보증충당금, 피크 실적 우려는 완화, 현대차-년도년도 2분기 2분기 Review: 피크 실적 우려 완화, 년도년도 2분기 2분기 Review: 전반적으로 컨센서스 부합한 실적, 금융 부문 실적과 판매보증충당금, 피크 실적 우려는 완화, 현대차-맞바람에도 이 정도, 영업이익 컨센서스 부합, 스트레스 테스트 통과, 현대차-금융이 만들어낸 기대와 아쉬움. 자동차는 선전, 예상보다 금융 기여가 작았으나, 자동차 부문은 기대치 부합, 21년도 2분기 Review: 영업이익률 6.2% 기록, 컨퍼런스콜의 주요 내용: 아이오닉5의 국내 계약대수는 4만대, 현대차-조금 아쉬운 호황, 21년도 2분기 영업이익 1.89조원(+219.5%)으로 기대치 부합, 하반기 관전 포인트는 생산 정상화, 신흥국, 비용 통제, 목표주가 29만원으로 -3.3% 하향, 투자의견 매수 유지, 현대차-단기적 숫자에 감춰진 큰 그림, 21년도 2분기 Review: 당사 추정치 및 가이던스에 부합하는 견조한 실적, 21년도 3분기 Preview: 점진적 생산 정상화와 신차 투입, 투자의견 Buy, 목표주가 320,000원 유지, 현대차-노사 합의로 하반기 리스크 완화, 21년도 2분기 영업이익은 1.89조원(+219.5% 전년 대비 증감율, OPM 6.2%) 기록, 컨센서스 1.1% 하회, 반도체 공급 차질 완화와 노사 합의로 파업 리스크 해소되며 하반기 생산 확대 전망, 현대차-년도년도 2분기 2분기 Review: 정상 궤도에 올라선 수익성, 년도년도 2분기 2분기 (P): 매출액 30조 3,260억원, 영업이익 1조 8,860억원, 생산 차질은 하반기로 갈수록 완화 예상, 지켜야 할 것이 많아지는 하반기, 현대차-21년도 2분기 Review - 판매증가 효과와 지속되는 금융부문 호실적, 비우호적인 환율환경과 믹스약화에도 불구, 판매증가가 수익성 개선에 기여. 상반기 부담요인이었던 차량용 반도체 수급 이슈는 점차 완화될 전망, 아이오닉 5 본격판매, 전기차라인업 강화, 신흥국 판매 확대 등이 주가의 모멘텀으로 작용할 전망, 현대차-일시적 비용 증가, 더 기대되는 하반기, 21년도 2분기 , 기대치 부합, 점진적인 생산 정상화 기대, 신차 사이클 여전히 유효, 현대차-역량 입증의 하반기, 2분기 영업이익 1.89조원, 당사 추정 및 컨센서스 부합, 역량 입증의 하반기, 목표주가 32만원 (유지)</t>
+    <t>일진하이솔루스 "수소탱크로 수소시대 앞당깁니다", 노사관계·MZ 퇴사… 현대차, 역대급 실적에도 ‘시름’, 박용진 "민주당 당대표가 김어준? 내가 새물결 이끈다", '넘치는 곳간' SNT모티브, '동향기업' BNK지주 매입, 년도년도 2분기 2분기 영업손익 전망 업데이트 - 금융부문 호실적 예상, 년도년도 2분기 2분기 영업이익 2.1조원 (+252.0% 전년 대비 증감율) 예상. 시장 컨센서스를 9.0% 상회할 것, 투자포인트: 1) 금융부문 영업이익률 상승, 2) 현대차 점유율 상승, 3) 향상된 수익성, 리스크요인: 1) 원자재 가격 상승, 2) 원화 평가 절상</t>
+  </si>
+  <si>
+    <t>년도년도 2분기 2분기 리뷰: 시장 기대치를 소폭 하회, 년도년도 2분기 2분기 영업이익 시장 기대를 소폭 하회. 년도년도 2분기 3분기 에는 신형 전기차에 주목할요,년도 분기 년도년도 2분기 2분기 실적 핵심: 예상 밖 판매보증비 증가, 가마감 대비 적었던 판매대수, 예상보다 좋았던 믹스, 년도년도 2분기 3분기 전망: 일부 모델 재고 부족으로 판매에 부정적 영향이 있을 수 있음. Ioniq 5 생산 확대에 주목, 아쉬울 것 없는 실적, 21년도 2분기 영업이익 1조8,860억원(전년 대비 증감율 +219%, OPM 6.2%) 기록, 추정치 부합. 자동차 부문 뿐만 아니라 금융부문도 호실적 지속, 재고가 극단적으로 낮아져 있어 물리적인 영향으로 3Q 판매 차질은 일부 감안할 필요. 그러나 북미 위주 자동차 소비심리 강세는 하반기에도 이어질 것으로 기대하므로 incentive 추가 하락 및 ASP 상승기조 지속될 것으로 전망. 완성차 실적호조 연내 지속 예상, 반도체 수급 우려가 peak를 지난 이상, 이제 실적 우려는 크지 않고 향후 전개될 미래 모빌리티 전환을 위한 전략 update 등이 중요하다는 판단. EV 판매목표 강화 등이 주가에 모멘텀으로 작용할 전망. 업종 top-pick 의견 및 TP 32만원(12MF PER 10.2x) 유지, 21년도 2분기 Review: 늘 새로움을 원하는 시장, 금융부문 실적 증가, 하반기 믹스 둔화 우려, 모멘텀을 원하는 시장, "현대해상, 2분기 자동차보험 손해율 개선"...대신증권, 김학균 "금리, 지금 안 올리면 당분간 못 올려", 현대차 노사 잠정합의…3년 연속 무분규 타결 기대, 높아지는 실적 = 매력적 밸류에이션, 21년도 2분기 , 분기 매출 처음으로 30조원 돌파 ASP 신기록 경신, 기대 이상의 ASP 상승 효과 → 실적 눈높이 우상향 지속</t>
+  </si>
+  <si>
+    <t>이제부터 물량 효과가 관건, 21년도 2분기 연결 매출 30조원 (전년 대비 증감율+39 %), 영업이익 1,886십억원(전년 대비 증감율+220 %), OPM 6.2%, 21년도 3분기 매출 29조원 (전년 대비 증감율+6%), 영업이익 1.7조원(흑전, OPM 5.9%) 전망, 23일 장 마감, 공매도 거래대금 상위 카카오·SK하이닉스·HMM·LG생활건강·현대차, 맞바람에도 이 정도, 영업이익 컨센서스 부합, 스트레스 테스트 통과, 현대차 주식 매수의견 유지, "수요 정상화로 하반기 실적 더 좋아져", 팬데믹이 뒤흔든 주식부호 랭킹…1~20위 싹 바뀌었네, '매도가능 물량 33%' 맥스트, SI 결속 유지할까, 대학교 4년 공짜·빈곤층 지원 2배…기본소득 줄 돈으로 할 수 있는 5가지, 이제부터 물량 효과가 관건, 21년도 2분기 연결 매출 30조원 (전년 대비 증감율+39 %), 영업이익 1,886십억원(전년 대비 증감율+220 %), OPM 6.2%, 21년도 3분기 매출 29조원 (전년 대비 증감율+6%), 영업이익 1.7조원(흑전, OPM 5.9%) 전망, 오프로드 무사 통과, 년도년도 2분기 2분기 Review: 시장 기대치 소폭 하회, 투자의견 ‘Buy’, 목표주가 300,000원, 분기 매출액 30조원 돌파, 공급 안정성 확보로 하반기 펀더멘탈 개선 지속, 2분기 Review: 분기 사상 최대 매출액 기록, 노사 합의로 하반기 리스크 완화, 21년도 2분기 영업이익은 1.89조원(+219.5% 전년 대비 증감율, OPM 6.2%) 기록, 컨센서스 1.1% 하회, 반도체 공급 차질 완화와 노사 합의로 파업 리스크 해소되며 하반기 생산 확대 전망, 오프로드 무사 통과, 년도년도 2분기 2분기 Review: 시장 기대치 소폭 하회, 투자의견 ‘Buy’, 목표주가 300,000원, 분기 매출액 30조원 돌파, 공급 안정성 확보로 하반기 펀더멘탈 개선 지속, 2분기 Review: 분기 사상 최대 매출액 기록, 년도년도 2분기 2분기 Review: 피크 실적 우려 완화, 년도년도 2분기 2분기 Review: 전반적으로 컨센서스 부합한 실적, 금융 부문 실적과 판매보증충당금, 피크 실적 우려는 완화, 년도년도 2분기 2분기 Review: 피크 실적 우려 완화, 년도년도 2분기 2분기 Review: 전반적으로 컨센서스 부합한 실적, 금융 부문 실적과 판매보증충당금, 피크 실적 우려는 완화, 맞바람에도 이 정도, 영업이익 컨센서스 부합, 스트레스 테스트 통과, 금융이 만들어낸 기대와 아쉬움. 자동차는 선전, 예상보다 금융 기여가 작았으나, 자동차 부문은 기대치 부합, 21년도 2분기 Review: 영업이익률 6.2% 기록, 컨퍼런스콜의 주요 내용: 아이오닉5의 국내 계약대수는 4만대, 조금 아쉬운 호황, 21년도 2분기 영업이익 1.89조원(+219.5%)으로 기대치 부합, 하반기 관전 포인트는 생산 정상화, 신흥국, 비용 통제, 목표주가 29만원으로 -3.3% 하향, 투자의견 매수 유지, 단기적 숫자에 감춰진 큰 그림, 21년도 2분기 Review: 당사 추정치 및 가이던스에 부합하는 견조한 실적, 21년도 3분기 Preview: 점진적 생산 정상화와 신차 투입, 투자의견 Buy, 목표주가 320,000원 유지, 노사 합의로 하반기 리스크 완화, 21년도 2분기 영업이익은 1.89조원(+219.5% 전년 대비 증감율, OPM 6.2%) 기록, 컨센서스 1.1% 하회, 반도체 공급 차질 완화와 노사 합의로 파업 리스크 해소되며 하반기 생산 확대 전망, 년도년도 2분기 2분기 Review: 정상 궤도에 올라선 수익성, 년도년도 2분기 2분기 (P): 매출액 30조 3,260억원, 영업이익 1조 8,860억원, 생산 차질은 하반기로 갈수록 완화 예상, 지켜야 할 것이 많아지는 하반기, 21년도 2분기 Review - 판매증가 효과와 지속되는 금융부문 호실적, 비우호적인 환율환경과 믹스약화에도 불구, 판매증가가 수익성 개선에 기여. 상반기 부담요인이었던 차량용 반도체 수급 이슈는 점차 완화될 전망, 아이오닉 5 본격판매, 전기차라인업 강화, 신흥국 판매 확대 등이 주가의 모멘텀으로 작용할 전망, 일시적 비용 증가, 더 기대되는 하반기, 21년도 2분기 , 기대치 부합, 점진적인 생산 정상화 기대, 신차 사이클 여전히 유효, 역량 입증의 하반기, 2분기 영업이익 1.89조원, 당사 추정 및 컨센서스 부합, 역량 입증의 하반기, 목표주가 32만원 (유지)</t>
   </si>
   <si>
     <t>美항모·셀트리온...이재명의 기본소득 안 주면 살 수 있는 것들</t>
@@ -7114,7 +7114,7 @@
     <t>車업계 '노사 갈등 리스크', 27일 기점 분수령, 코스피 영업이익 성장률 둔화… 돌아오지 않은 외국인 순매수 업종서 기회, 앞다퉈 미래계획 발표하는 자동차 제조사들, “주식투자를 도박으로 보는 한국…안정적 노후 생각하면 주식 사야”</t>
   </si>
   <si>
-    <t>현대차-아이오닉5와 제네시스로 전기차 확대, 2분기 영업이익률 6.2%(+3.5%p). 기대치 부합, 하반기 아이오닉5 증산. 제네시스 전동화 라인업. 금융 수익성 양호, 투자의견 BUY, 목표주가 31만원 제시. 업종 최선호주, 한투證 "현대차 노사 3년연속 무분규 타결…악재 걷히고 있어", 최성안 삼성엔지니어링 대표이사 사장, 현대車 노사, 3년 연속 무분규…위기극복 공감대 형성, "비과세 혜택 입소문?" 중개형ISA '광풍'...카카오페이 IPO 연기 外, 현대차-약해지는 노조 리스크, 현대차 노사, 3년 연속 무분규 임금협상 타결, 파업 실종은 구조적 현상이다, 이제 악재 뭐가 남았지?</t>
+    <t>아이오닉5와 제네시스로 전기차 확대, 2분기 영업이익률 6.2%(+3.5%p). 기대치 부합, 하반기 아이오닉5 증산. 제네시스 전동화 라인업. 금융 수익성 양호, 투자의견 BUY, 목표주가 31만원 제시. 업종 최선호주, 한투證 "현대차 노사 3년연속 무분규 타결…악재 걷히고 있어", 최성안 삼성엔지니어링 대표이사 사장, 현대車 노사, 3년 연속 무분규…위기극복 공감대 형성, "비과세 혜택 입소문?" 중개형ISA '광풍'...카카오페이 IPO 연기 外, 약해지는 노조 리스크, 현대차 노사, 3년 연속 무분규 임금협상 타결, 파업 실종은 구조적 현상이다, 이제 악재 뭐가 남았지?</t>
   </si>
   <si>
     <t>반도체 외면한 외인, 2차 전지 쓸어담는다</t>
@@ -7186,7 +7186,7 @@
     <t>'수소차' 탄 일진하이솔루스, 24일 청약...SK리츠 수요예측 개시</t>
   </si>
   <si>
-    <t>패닉에 빠진 증시 앞날…금통위와 잭슨홀 미팅이 가른다, 현대차-모빌리티 전쟁은 시작되었다, 자동차 이외의 영역으로 본격 진출: 모빌리티 기업으로 진화, 21년도 하반기 , 실적보다 중요한 것들: OTA, ccOS의 본격 도입, 로보택시 시장이 보인다: Motional로 Lyft와 함께 간다, 현대차-새로운 도약의 변곡점에서, 3분기 영업이익 1.81조원 전망, 전용 플랫폼 개발을 통한 경쟁사 대비 신속한 전동화 전환, SW 역량 강화를 위한 내재화 노력 (AIRS Company 등) 및 비유기적 협업 등을 통한 새로운 도약을 기대, 투자의견 Buy, 목표주가를 32만원 유지 (12mf EPS 23,763원, Target PER 13.5x), &lt; Leadership 클래스 &gt;김범수, 창업·M&amp;A ‘끝없는 도전’ 뒤 전문가에 ‘경영 위임’…재산 절반 사회환원도</t>
+    <t>패닉에 빠진 증시 앞날…금통위와 잭슨홀 미팅이 가른다, 모빌리티 전쟁은 시작되었다, 자동차 이외의 영역으로 본격 진출: 모빌리티 기업으로 진화, 21년도 하반기 , 실적보다 중요한 것들: OTA, ccOS의 본격 도입, 로보택시 시장이 보인다: Motional로 Lyft와 함께 간다, 새로운 도약의 변곡점에서, 3분기 영업이익 1.81조원 전망, 전용 플랫폼 개발을 통한 경쟁사 대비 신속한 전동화 전환, SW 역량 강화를 위한 내재화 노력 (AIRS Company 등) 및 비유기적 협업 등을 통한 새로운 도약을 기대, 투자의견 Buy, 목표주가를 32만원 유지 (12mf EPS 23,763원, Target PER 13.5x), &lt; Leadership 클래스 &gt;김범수, 창업·M&amp;A ‘끝없는 도전’ 뒤 전문가에 ‘경영 위임’…재산 절반 사회환원도</t>
   </si>
   <si>
     <t>정의선 회장, 상반기 경영 '잘' 했다 對 쌍용차 '흔들', 영앤드리치의 시대/주현진 산업부장</t>
@@ -7216,10 +7216,10 @@
     <t>수소株 일진하이솔루스, 코스피 상장 첫날 '따상' 마감(종합), 일단 전환사채로 데뷔? 'IPO 최대어' LG엔솔 연내 상장 불투명한 까닭, 일진하이솔루스, 상장 첫날 '따상'…29.88% 상승</t>
   </si>
   <si>
-    <t>"0.25%쯤이야"… 증시 빚투 다시 증가 外, 투자의 정석은 ‘분산투자’, 정말 그럴까?, 현대차-제네시스비전 : Dual Electrification과 탄소중립, 현대차, 제네시스 비전 공유, 일진하이솔루스, 상장 첫날 '따상'…남양유업, 매각 결렬 소식에 하락세 外</t>
-  </si>
-  <si>
-    <t>현대차-제네시스 브랜드의 전동화 목표 제시, 제네시스는 2030년부터 전동화 모델만 생산할 계획, 제네시스 판매대수는 2021년 20만대 전망, 주가 측면에서는 제한적인 플러스 효과, 국민연금 8월 국내주식 팔기 바빴다, 연말까지 4조 규모 더 팔아야, 현대차-제네시스 브랜드의 전동화 비전 발표, 2025년부터 신차는 전기차/수소차. 2030년 100% ZEV 전환 목표, 고급차 브랜드로 그룹 내 전동화 최선두 위치, 주가에 점진적으로 반영. 수소비전 발표는 추가적인 멀티플 변수</t>
+    <t>"0.25%쯤이야"… 증시 빚투 다시 증가 外, 투자의 정석은 ‘분산투자’, 정말 그럴까?, 제네시스비전 : Dual Electrification과 탄소중립, 현대차, 제네시스 비전 공유, 일진하이솔루스, 상장 첫날 '따상'…남양유업, 매각 결렬 소식에 하락세 外</t>
+  </si>
+  <si>
+    <t>제네시스 브랜드의 전동화 목표 제시, 제네시스는 2030년부터 전동화 모델만 생산할 계획, 제네시스 판매대수는 2021년 20만대 전망, 주가 측면에서는 제한적인 플러스 효과, 국민연금 8월 국내주식 팔기 바빴다, 연말까지 4조 규모 더 팔아야, 제네시스 브랜드의 전동화 비전 발표, 2025년부터 신차는 전기차/수소차. 2030년 100% ZEV 전환 목표, 고급차 브랜드로 그룹 내 전동화 최선두 위치, 주가에 점진적으로 반영. 수소비전 발표는 추가적인 멀티플 변수</t>
   </si>
   <si>
     <t>주식시장 시선은 지금 수소주에</t>
@@ -7228,16 +7228,16 @@
     <t>(토마토TV와 함께하는 주식투자)두산퓨얼셀, 2차전지 바통 이어받을 '수소전지' 대표, 지난주 특징주 브리핑…삼성SDI 배터리 ‘대장주’ 등극, LG화학 시총 추월</t>
   </si>
   <si>
-    <t>현대차-이벤트 시즌, 현대차 수익성 개선 지속, 미래를 위한 이벤트, 투자의견 BUY, 목표주가 30만원(유지), 솟아오른다, 수소 경제… 불꽃 랠리 이끌 종목은</t>
+    <t>이벤트 시즌, 현대차 수익성 개선 지속, 미래를 위한 이벤트, 투자의견 BUY, 목표주가 30만원(유지), 솟아오른다, 수소 경제… 불꽃 랠리 이끌 종목은</t>
   </si>
   <si>
     <t>현대차 내연차 생산 중단, 수소 사업 전환 속도전...수소 관련株도 '들썩', 이노션 주식 매수의견 유지, "국내외 광고 좋아 매체대행 실적 늘어"</t>
   </si>
   <si>
-    <t>조현범 한국앤컴퍼니 대표이사 사장, "현대차 수소경제 비전, 장기적으론 긍정적"...하나금융투자, 수소차 관련주 동양피스톤·효성첨단소재·우수AMS·기아 반색, "치킨 사면 주식 줄게, 어때?" 금융, 유통을 품다, 현대차그룹주 엇갈려, 현대오토에버 5%대 현대로템 2%대 밀려, 세 번의 개선안·1900억 자사주취득에도…내리막에 빠진 엔씨, 현대차-수소 언박싱, Hydrogen Wave 발표 주요 내용, 현대차의 7가지 보석상자, 현대차-탄소중립 비전 발표, 이제 실행 속도에 달렸다, 9/7일 행사: 독일 뮌헨 IAA에서 2045년 탄소중립 달성을 위한 3 가지 솔루션 발표, 9/8일 행사: Hydrogen Wave를 통해 상용차 중심의 수소연료전지 기술 발전 로드맵 제시, 현대차-＇하이드로젠 웨이브＇ 행사에서 수소 전략 발표, 2028년까지 모든 상용차 라인업에서 수소차 출시, 성능은 높이고 가격은 낮춘 3세대 수소연료전지 시스템을 개발 중, 수소 경제에 대한 비전 제시라는 측면에서 중장기로 긍정적 판단, 현대차-하이드로젠 웨이브에서 수소사업의 비전 제시, 요약: 2028년까지 상용차는 수소차 라인업. 차세대 연료전지 시스템 및 PBV 공개, 분석: ‘35년 유럽 전동화, ‘40년 글로벌 전동화, ‘45년 탄소중립을 위한 수소 전략, 판단: 세부적인 계획과 확장성은 긍정적. 개화속도에 따라 주가는 반영될 것</t>
-  </si>
-  <si>
-    <t>현대차-높아진 체력, 22년까지 우호적 사업 환경 지속 전망, 하반기 실적 다소 둔화될 전망이나 22년 개선 전망, 목표가 28만원, 매수 의견으로 커버리지 개시, 두올물산, K-OTC 신규 진입···13일부터 거래 가능, K-OTC, 두올물산 신규등록 승인…13일부터 거래, 두올물산 K-OTC 시장 진입, 현대중공업 일반청약 최종 경쟁률 404.29대 1…유진스팩7호, 13일 코스닥 상장 外</t>
+    <t>조현범 한국앤컴퍼니 대표이사 사장, "현대차 수소경제 비전, 장기적으론 긍정적"...하나금융투자, 수소차 관련주 동양피스톤·효성첨단소재·우수AMS·기아 반색, "치킨 사면 주식 줄게, 어때?" 금융, 유통을 품다, 현대차그룹주 엇갈려, 현대오토에버 5%대 현대로템 2%대 밀려, 세 번의 개선안·1900억 자사주취득에도…내리막에 빠진 엔씨, 수소 언박싱, Hydrogen Wave 발표 주요 내용, 현대차의 7가지 보석상자, 탄소중립 비전 발표, 이제 실행 속도에 달렸다, 9/7일 행사: 독일 뮌헨 IAA에서 2045년 탄소중립 달성을 위한 3 가지 솔루션 발표, 9/8일 행사: Hydrogen Wave를 통해 상용차 중심의 수소연료전지 기술 발전 로드맵 제시, ＇하이드로젠 웨이브＇ 행사에서 수소 전략 발표, 2028년까지 모든 상용차 라인업에서 수소차 출시, 성능은 높이고 가격은 낮춘 3세대 수소연료전지 시스템을 개발 중, 수소 경제에 대한 비전 제시라는 측면에서 중장기로 긍정적 판단, 하이드로젠 웨이브에서 수소사업의 비전 제시, 요약: 2028년까지 상용차는 수소차 라인업. 차세대 연료전지 시스템 및 PBV 공개, 분석: ‘35년 유럽 전동화, ‘40년 글로벌 전동화, ‘45년 탄소중립을 위한 수소 전략, 판단: 세부적인 계획과 확장성은 긍정적. 개화속도에 따라 주가는 반영될 것</t>
+  </si>
+  <si>
+    <t>높아진 체력, 22년까지 우호적 사업 환경 지속 전망, 하반기 실적 다소 둔화될 전망이나 22년 개선 전망, 목표가 28만원, 매수 의견으로 커버리지 개시, 두올물산, K-OTC 신규 진입···13일부터 거래 가능, K-OTC, 두올물산 신규등록 승인…13일부터 거래, 두올물산 K-OTC 시장 진입, 현대중공업 일반청약 최종 경쟁률 404.29대 1…유진스팩7호, 13일 코스닥 상장 外</t>
   </si>
   <si>
     <t>수소차 관련주 EG·동양피스톤 환호...삼기·한온시스템 흔들, 이벤트 중심의 투자전략, 수소 산업 빅 이벤트에 정책 기대감까지…수소주 ‘뿜뿜’, 9일 장 마감, 공매도 대금 상위 에코프로비엠·NAVER·LG생활건강·현대모비스·SK하이닉스</t>
@@ -7252,7 +7252,7 @@
     <t>현대경영 구루 명예의 전당, '수소 액셀' 밟았지만…현대차, 1월 대비 23% 하락</t>
   </si>
   <si>
-    <t>수소차 관련주 EG·일진하이솔루스·코로롱플라스틱·동아화성 환호성, 현대차 주식 매수의견 유지, "탄소중립 비전은 기업가치에 긍정적", “수소의 시대온다”···돈 몰리는 수소 ETF, 오랜만에 반등…엔씨 주가 바닥쳤나, 현대차-수소가 물결치면 현대가 춤을 춘다, 지난 9/7 발표한 수소 사회를 위한 비전(Hydrogen Wave; 수소 사회를 위한 새로운 물결) 이후 투자자와의 Q&amp;A 세션 진행, 공급망 정상화 이후 탄력적 공급 회복에 따른 물량 증가와 믹스 개선이 최근 발표한 탄소중립 비전과 구체화된 친환경차 전략과 맞물리며 주가 상승 견인할 전망</t>
+    <t>수소차 관련주 EG·일진하이솔루스·코로롱플라스틱·동아화성 환호성, 현대차 주식 매수의견 유지, "탄소중립 비전은 기업가치에 긍정적", “수소의 시대온다”···돈 몰리는 수소 ETF, 오랜만에 반등…엔씨 주가 바닥쳤나, 수소가 물결치면 현대가 춤을 춘다, 지난 9/7 발표한 수소 사회를 위한 비전(Hydrogen Wave; 수소 사회를 위한 새로운 물결) 이후 투자자와의 Q&amp;A 세션 진행, 공급망 정상화 이후 탄력적 공급 회복에 따른 물량 증가와 믹스 개선이 최근 발표한 탄소중립 비전과 구체화된 친환경차 전략과 맞물리며 주가 상승 견인할 전망</t>
   </si>
   <si>
     <t>IPO 본격화하는 현대엔지니어링…현대차그룹 지배구조 개편 탄력, 네이버·카카오 휘청이자 ELS 투자자도 ‘불안’, 네이버·카카오 휘청이자 ELS 투자자도 ‘불안’, 수소차 관련주 영화테크·상아프론테크·삼기·제이엔케이히터 환호성</t>
@@ -7279,13 +7279,13 @@
     <t>헝다發 리스크 여전하지만… 외국인 순매수 유입 종목 옥석가려라, “앞날에 성장이 펼쳐졌다” 뭉칫돈 몰리는 수소株·펀드</t>
   </si>
   <si>
-    <t>SK E&amp;S IPO '안하나, 못하나', 현대차-21년도 3분기 Review: 실적 선방, 이제 차별화 구간으로, 최악의 상황에서 보여준 체력, 반도체 부족은 점진적 개선 예상, 차별화 싸이클 진입, SK이노, 주가 하락에도 배터리 투자전략 ‘GO’, 현대차-이제 답을 제시할 때, 현대차, 모빌리티 시장에 대한 공격적 기술 진전, 협업 전개 필요, 실적, 낮은 재고, 적은 영업일수, 반도체 부족 우려 넘어 21년도 4분기 -2022년 우상향 기조 유지 전망, 투자의견 Buy 유지, 적정주가 285,000원 제시</t>
-  </si>
-  <si>
-    <t>미·중발 외풍에 대장주 ‘추풍낙엽’, 무너진 코스피 3100, 삼성공조, 상반기 국내외 고른 성장…PBR 0.67배, 공모가 대비 2배 오른 일진하이솔루스, 내일 보호예수 물량 128만주 해제, 현대차-2022년 최대 영업이익 전망, 실적 개선, 중장기 주가 재평가 기대, 3분기 Preview: 반도체 수급 차질 여파로 컨센서스 하회, 상속형 재벌 줄고, 창업형 부자 늘었다, 현대차-2022년 최대 영업이익 전망, 실적 개선, 중장기 주가 재평가 기대, 3분기 Preview: 반도체 수급 차질 여파로 컨센서스 하회</t>
-  </si>
-  <si>
-    <t>시총 상위 절반이 ‘파란불’…한숨 깊은 개미들, 전고체 배터리 관련주 한농화성, 상한가 '급등'...이달 들어 57% 상승 '주목', 방시혁, 주식 평가액 3조9000억…이수만·박진영 합쳐도 안되네, 현대차-ESG 총평, 환경(E) : 지난 9월 탄소중립 달성을 위한 비전, 수소 사회를 위한 비전 발표를 통해 친환경 전략을 대폭 강화, 사회(S) : 품질과 안전을 강화하기 위해 3세대 플랫폼 도입과 자율주행 리던던시 시스템 등 적용, 지배구조(G) : 주기적인 CEO investor day를 통해 적극적으로 주주와 소통, 현대차-사업 모델의 확장 기대, 탄탄한 친환경차 판매 실적에 기반한 선도적인 탄소중립 전략과 수소 전략 구체화, 4분기 탄력적 공급 회복 시 물량 증가와 믹스 개선이 최근 발표한 탄소중립 비전과 구체화된 친환경차 전략과 맞물리며 주가 상승을 견인할 전망, "3조 9천억" 방시혁 주식 평가액, 대기업 회장도 제쳤다, 현대차-ESG 총평, 환경(E) : 지난 9월 탄소중립 달성을 위한 비전, 수소 사회를 위한 비전 발표를 통해 친환경 전략을 대폭 강화, 사회(S) : 품질과 안전을 강화하기 위해 3세대 플랫폼 도입과 자율주행 리던던시 시스템 등 적용, 지배구조(G) : 주기적인 CEO investor day를 통해 적극적으로 주주와 소통, 현대차-사업 모델의 확장 기대, 탄탄한 친환경차 판매 실적에 기반한 선도적인 탄소중립 전략과 수소 전략 구체화, 4분기 탄력적 공급 회복 시 물량 증가와 믹스 개선이 최근 발표한 탄소중립 비전과 구체화된 친환경차 전략과 맞물리며 주가 상승을 견인할 전망</t>
+    <t>SK E&amp;S IPO '안하나, 못하나', 21년도 3분기 Review: 실적 선방, 이제 차별화 구간으로, 최악의 상황에서 보여준 체력, 반도체 부족은 점진적 개선 예상, 차별화 싸이클 진입, SK이노, 주가 하락에도 배터리 투자전략 ‘GO’, 이제 답을 제시할 때, 현대차, 모빌리티 시장에 대한 공격적 기술 진전, 협업 전개 필요, 실적, 낮은 재고, 적은 영업일수, 반도체 부족 우려 넘어 21년도 4분기 -2022년 우상향 기조 유지 전망, 투자의견 Buy 유지, 적정주가 285,000원 제시</t>
+  </si>
+  <si>
+    <t>미·중발 외풍에 대장주 ‘추풍낙엽’, 무너진 코스피 3100, 삼성공조, 상반기 국내외 고른 성장…PBR 0.67배, 공모가 대비 2배 오른 일진하이솔루스, 내일 보호예수 물량 128만주 해제, 2022년 최대 영업이익 전망, 실적 개선, 중장기 주가 재평가 기대, 3분기 Preview: 반도체 수급 차질 여파로 컨센서스 하회, 상속형 재벌 줄고, 창업형 부자 늘었다, 2022년 최대 영업이익 전망, 실적 개선, 중장기 주가 재평가 기대, 3분기 Preview: 반도체 수급 차질 여파로 컨센서스 하회</t>
+  </si>
+  <si>
+    <t>시총 상위 절반이 ‘파란불’…한숨 깊은 개미들, 전고체 배터리 관련주 한농화성, 상한가 '급등'...이달 들어 57% 상승 '주목', 방시혁, 주식 평가액 3조9000억…이수만·박진영 합쳐도 안되네, ESG 총평, 환경(E) : 지난 9월 탄소중립 달성을 위한 비전, 수소 사회를 위한 비전 발표를 통해 친환경 전략을 대폭 강화, 사회(S) : 품질과 안전을 강화하기 위해 3세대 플랫폼 도입과 자율주행 리던던시 시스템 등 적용, 지배구조(G) : 주기적인 CEO investor day를 통해 적극적으로 주주와 소통, 사업 모델의 확장 기대, 탄탄한 친환경차 판매 실적에 기반한 선도적인 탄소중립 전략과 수소 전략 구체화, 4분기 탄력적 공급 회복 시 물량 증가와 믹스 개선이 최근 발표한 탄소중립 비전과 구체화된 친환경차 전략과 맞물리며 주가 상승을 견인할 전망, "3조 9천억" 방시혁 주식 평가액, 대기업 회장도 제쳤다, ESG 총평, 환경(E) : 지난 9월 탄소중립 달성을 위한 비전, 수소 사회를 위한 비전 발표를 통해 친환경 전략을 대폭 강화, 사회(S) : 품질과 안전을 강화하기 위해 3세대 플랫폼 도입과 자율주행 리던던시 시스템 등 적용, 지배구조(G) : 주기적인 CEO investor day를 통해 적극적으로 주주와 소통, 사업 모델의 확장 기대, 탄탄한 친환경차 판매 실적에 기반한 선도적인 탄소중립 전략과 수소 전략 구체화, 4분기 탄력적 공급 회복 시 물량 증가와 믹스 개선이 최근 발표한 탄소중립 비전과 구체화된 친환경차 전략과 맞물리며 주가 상승을 견인할 전망</t>
   </si>
   <si>
     <t>한국경제신문 보도 독해법, 대기업 집단 지분율 82%</t>
@@ -7297,16 +7297,16 @@
     <t>배터리 자회사 'SK온' 출범…SK이노베이션 주가는?, '몸값 10조' 현대엔지니어링, 코스피 출격… 증권가 "제값할 것"</t>
   </si>
   <si>
-    <t>'갑' 배터리 3사보다 더 잘나가는 '을' 배터리 소재 3사, '3분기 주식부자' 1위 이재용…카카오 김범수, 3위로, 이재용, 총수 주식재산 '14조'로 1위...김범수는 2위(종합), 그룹 총수 주식 3분기 7조 증발···카카오 김범수 2.6조 '뚝', 국내 주식부자 1위에 이재용…셀트리온 서정진, 맹추격, 3분기 김범수 지분가치 2.6조 증발/ 나트라케어, 국내 온라인 공식몰 'WDAY24' 10월 오픈 등, 현대차-년도년도 2분기 3분기 볼륨 감소와 비우호적 환율이 부담, 년도년도 2분기 3분기 연결 매출 28조원 (전년 대비 증감율 +2 %), 영업이익 1.49조원 (흑전), OPM 5.3 % 전망, 년도년도 2분기 4분기 우호적 환율 효과는 기대 요인이나 생산 정상화와 재고 확보가 필요, 셀트리온 서정진, 비상장 포함 주식 13조 5546억... 주식 부자 1위 등극할까, 현대차-년도년도 2분기 3분기 볼륨 감소와 비우호적 환율이 부담, 년도년도 2분기 3분기 연결 매출 28조원 (전년 대비 증감율 +2 %), 영업이익 1.49조원 (흑전), OPM 5.3 % 전망, 년도년도 2분기 4분기 우호적 환율 효과는 기대 요인이나 생산 정상화와 재고 확보가 필요, 3분기 총수 주식재산 살펴보니…이재용, 14조원대 부동의 1위, 국내 주식부자 1위 '이재용'…서정진에 곧 추격 당할까, 3분기 총수 주식재산 성적표 살펴보니…KCC 정몽진 웃고 VS 카카오 김범수 울고</t>
-  </si>
-  <si>
-    <t>현대차-본질은 강력한 신차 판매, 다소 부진할 전망, 22년 Q 회복 지속, E-GMP, 신차 사이클 여전히 유효, 국내 50대 그룹 총수 주식 7.6조 증발…김범수는 2.6조 줄어, 수소산업 뜨자 LPG수입사 주가도 들썩, 현대엔지니어링, 코스피 입성 박차..정의선, 지배체제 강화 '실탄' 마련하나, 현대차-본질은 강력한 신차 판매, 다소 부진할 전망, 22년 Q 회복 지속, E-GMP, 신차 사이클 여전히 유효</t>
+    <t>'갑' 배터리 3사보다 더 잘나가는 '을' 배터리 소재 3사, '3분기 주식부자' 1위 이재용…카카오 김범수, 3위로, 이재용, 총수 주식재산 '14조'로 1위...김범수는 2위(종합), 그룹 총수 주식 3분기 7조 증발···카카오 김범수 2.6조 '뚝', 국내 주식부자 1위에 이재용…셀트리온 서정진, 맹추격, 3분기 김범수 지분가치 2.6조 증발/ 나트라케어, 국내 온라인 공식몰 'WDAY24' 10월 오픈 등, 년도년도 2분기 3분기 볼륨 감소와 비우호적 환율이 부담, 년도년도 2분기 3분기 연결 매출 28조원 (전년 대비 증감율 +2 %), 영업이익 1.49조원 (흑전), OPM 5.3 % 전망, 년도년도 2분기 4분기 우호적 환율 효과는 기대 요인이나 생산 정상화와 재고 확보가 필요, 셀트리온 서정진, 비상장 포함 주식 13조 5546억... 주식 부자 1위 등극할까, 년도년도 2분기 3분기 볼륨 감소와 비우호적 환율이 부담, 년도년도 2분기 3분기 연결 매출 28조원 (전년 대비 증감율 +2 %), 영업이익 1.49조원 (흑전), OPM 5.3 % 전망, 년도년도 2분기 4분기 우호적 환율 효과는 기대 요인이나 생산 정상화와 재고 확보가 필요, 3분기 총수 주식재산 살펴보니…이재용, 14조원대 부동의 1위, 국내 주식부자 1위 '이재용'…서정진에 곧 추격 당할까, 3분기 총수 주식재산 성적표 살펴보니…KCC 정몽진 웃고 VS 카카오 김범수 울고</t>
+  </si>
+  <si>
+    <t>본질은 강력한 신차 판매, 다소 부진할 전망, 22년 Q 회복 지속, E-GMP, 신차 사이클 여전히 유효, 국내 50대 그룹 총수 주식 7.6조 증발…김범수는 2.6조 줄어, 수소산업 뜨자 LPG수입사 주가도 들썩, 현대엔지니어링, 코스피 입성 박차..정의선, 지배체제 강화 '실탄' 마련하나, 본질은 강력한 신차 판매, 다소 부진할 전망, 22년 Q 회복 지속, E-GMP, 신차 사이클 여전히 유효</t>
   </si>
   <si>
     <t>현대차 수소차 죽음의 계곡 넘나, 정의선 수소사회로 뚝심, 현대차그룹주 다 올라, 현대위아 현대오토에버 기아 6% 이상 뛰어</t>
   </si>
   <si>
-    <t>현대차-21년도 3분기 Preview: 영업이익률 5.9% 예상, 3분기 출하/도매/소매판매는 각각 12%/11%/4% (전년 대비 증감율) 감소, 전년 기저가 낮은 아중동 (+7%)/중남미(+13%) 정도만이 증가, 정지선 현대백화점그룹 회장, 현대차그룹주 상승 많아, 현대오토에버 10%대 현대위아 4%대 올라, 코스피 나흘만에 1%대 반등…현대차 20만원 회복</t>
+    <t>21년도 3분기 Preview: 영업이익률 5.9% 예상, 3분기 출하/도매/소매판매는 각각 12%/11%/4% (전년 대비 증감율) 감소, 전년 기저가 낮은 아중동 (+7%)/중남미(+13%) 정도만이 증가, 정지선 현대백화점그룹 회장, 현대차그룹주 상승 많아, 현대오토에버 10%대 현대위아 4%대 올라, 코스피 나흘만에 1%대 반등…현대차 20만원 회복</t>
   </si>
   <si>
     <t>카카오페이·현대엔지니어링·SM상선…4분기 주목해야 할 신규 상장주는, 정의선 취임 후 1년간 현대차그룹 시총 28%↑, 정의선 취임 1년간 주가 ‘껑충’…현대차 시총 28.7% 늘었다</t>
@@ -7315,13 +7315,13 @@
     <t>“美 IPO 시장, 변동성 확대에도 연말까지 호황 지속”</t>
   </si>
   <si>
-    <t>개인투자자는 기관투자자들이 투자하는 esg기업을 보고 투자하세요, 반도체 수급난 해소 기대에 '현대차그룹주 강세', 현대차그룹주 다 올라, 현대비앤지스틸 6%대 현대위아 4%대 상승, 외인 탈출 러시… 모건스탠리 “SK하이닉스 8만원까지 하락”, 현대차-년도년도 2분기 3분기 Preview, 년도년도 2분기 3분기 영업이익은 1.63조원(흑전 전년 대비 증감율, OPM 5.6%), 컨센서스 6.3% 하회 전망, 주가 회복을 위해서는 자동차 공급망의 회복이 절실한 상황</t>
+    <t>개인투자자는 기관투자자들이 투자하는 esg기업을 보고 투자하세요, 반도체 수급난 해소 기대에 '현대차그룹주 강세', 현대차그룹주 다 올라, 현대비앤지스틸 6%대 현대위아 4%대 상승, 외인 탈출 러시… 모건스탠리 “SK하이닉스 8만원까지 하락”, 년도년도 2분기 3분기 Preview, 년도년도 2분기 3분기 영업이익은 1.63조원(흑전 전년 대비 증감율, OPM 5.6%), 컨센서스 6.3% 하회 전망, 주가 회복을 위해서는 자동차 공급망의 회복이 절실한 상황</t>
   </si>
   <si>
     <t>현대차 북미사장 "반도체 자체 개발에 공들이고 있다", 현대車, 반도체 내재화 큰 꿈 "많은 투자·시간 걸려도 해낼 것", '8.8조원' 美 전기차 투자 준비한 현대차 "인프라법 통과에 달려", 자동차 소재가 새 옷으로 재탄생…현대차, '리스타일 2021 프로젝트'..., 현대차그룹에 간부노조 생겼다, 취임 후 시총 30조 '쑥'...위기에도 '질주..., '알량한 자존심 버린' 그가 이끈 현대차의 변화, '자동차주' 바닥찍었나...외인·기관도 사들인 현대차·기아, 전망은?, 현대차·기아·두산퓨얼셀 '수소연료전지 분산 발전' 시범운전 착수, 현대차 북미사장 "반도체 자체 개발에 공들이고 있다", “반도체 확보가 곧 전기차 주도권”…현대차 ‘폭발적 수요’ 선제 대응, 車폐기물, 옷이 되다...현대차, 업사이클링 패션 공개, 현대차 아이오닉5로 자켓·후드·바지를 만든다?, “반도체 확보가 곧 전기차 주도권”…현대차 ‘폭발적 수요’ 선제 대응, 현대車, 반도체 내재화 큰 꿈 "많은 투자·시간 걸려도 해낼 것", '8.8조원' 美 전기차 투자 준비한 현대차 "인프라법 통과에 달려", 자동차 소재가 새 옷으로 재탄생…현대차, '리스타일 2021 프로젝트'..., 현대차그룹에 간부노조 생겼다, “현대차, 반도체 자체개발 원한다”, 현대차 아이오닉5로 자켓·후드·바지를 만든다?, 현대차 북미사장 "반도체 자체 개발에 공들이고 있다", 취임 후 시총 30조 '쑥'...위기에도 '질주..., '알량한 자존심 버린' 그가 이끈 현대차의 변화, '자동차주' 바닥찍었나...외인·기관도 사들인 현대차·기아, 전망은?, 현대차·기아·두산퓨얼셀 '수소연료전지 분산 발전' 시범운전 착수, “현대차, 반도체 자체개발 원한다”, 현대차 북미사장 "반도체 자체 개발에 공들이고 있다", 車폐기물, 옷이 되다...현대차, 업사이클링 패션 공개, 현대차 아이오닉5로 자켓·후드·바지를 만든다?, “반도체 확보가 곧 전기차 주도권”…현대차 ‘폭발적 수요’ 선제 대응, 현대車, 반도체 내재화 큰 꿈 "많은 투자·시간 걸려도 해낼 것", '8.8조원' 美 전기차 투자 준비한 현대차 "인프라법 통과에 달려", 자동차 소재가 새 옷으로 재탄생…현대차, '리스타일 2021 프로젝트'..., 현대차그룹에 간부노조 생겼다, 취임 후 시총 30조 '쑥'...위기에도 '질주..., '알량한 자존심 버린' 그가 이끈 현대차의 변화, '자동차주' 바닥찍었나...외인·기관도 사들인 현대차·기아, 전망은?, 현대차·기아·두산퓨얼셀 '수소연료전지 분산 발전' 시범운전 착수, “현대차, 반도체 자체개발 원한다”, 車폐기물, 옷이 되다...현대차, 업사이클링 패션 공개, '알량한 자존심 버린' 그가 이끈 현대차의 변화, '자동차주' 바닥찍었나...외인·기관도 사들인 현대차·기아, 전망은?, 현대차·기아·두산퓨얼셀 '수소연료전지 분산 발전' 시범운전 착수, '알량한 자존심 버린' 그가 이끈 현대차의 변화, '자동차주' 바닥찍었나...외인·기관도 사들인 현대차·기아, 전망은?, 현대차·기아·두산퓨얼셀 '수소연료전지 분산 발전' 시범운전 착수, “현대차, 반도체 자체개발 원한다”, 현대차 북미사장 "반도체 자체 개발에 공들이고 있다", 車폐기물, 옷이 되다...현대차, 업사이클링 패션 공개, 현대차 아이오닉5로 자켓·후드·바지를 만든다?, “반도체 확보가 곧 전기차 주도권”…현대차 ‘폭발적 수요’ 선제 대응, 현대車, 반도체 내재화 큰 꿈 "많은 투자·시간 걸려도 해낼 것", '8.8조원' 美 전기차 투자 준비한 현대차 "인프라법 통과에 달려", 자동차 소재가 새 옷으로 재탄생…현대차, '리스타일 2021 프로젝트'..., 현대차그룹에 간부노조 생겼다, 취임 후 시총 30조 '쑥'...위기에도 '질주..., '알량한 자존심 버린' 그가 이끈 현대차의 변화, '자동차주' 바닥찍었나...외인·기관도 사들인 현대차·기아, 전망은?, 현대차·기아·두산퓨얼셀 '수소연료전지 분산 발전' 시범운전 착수, “현대차, 반도체 자체개발 원한다”, 현대차 북미사장 "반도체 자체 개발에 공들이고 있다", 車폐기물, 옷이 되다...현대차, 업사이클링 패션 공개, 취임 후 시총 30조 '쑥'...위기에도 '질주..., 취임 후 시총 30조 '쑥'...위기에도 '질주..., 현대차그룹에 간부노조 생겼다, '8.8조원' 美 전기차 투자 준비한 현대차 "인프라법 통과에 달려", “현대차, 반도체 자체개발 원한다”, 현대차 북미사장 "반도체 자체 개발에 공들이고 있다", 車폐기물, 옷이 되다...현대차, 업사이클링 패션 공개, 현대차 아이오닉5로 자켓·후드·바지를 만든다?, “반도체 확보가 곧 전기차 주도권”…현대차 ‘폭발적 수요’ 선제 대응, 현대車, 반도체 내재화 큰 꿈 "많은 투자·시간 걸려도 해낼 것", '8.8조원' 美 전기차 투자 준비한 현대차 "인프라법 통과에 달려", 자동차 소재가 새 옷으로 재탄생…현대차, '리스타일 2021 프로젝트'..., 현대차그룹에 간부노조 생겼다, 취임 후 시총 30조 '쑥'...위기에도 '질주..., '알량한 자존심 버린' 그가 이끈 현대차의 변화, '자동차주' 바닥찍었나...외인·기관도 사들인 현대차·기아, 전망은?, 현대차·기아·두산퓨얼셀 '수소연료전지 분산 발전' 시범운전 착수, “현대차, 반도체 자체개발 원한다”, 현대차 북미사장 "반도체 자체 개발에 공들이고 있다", 車폐기물, 옷이 되다...현대차, 업사이클링 패션 공개, 현대차 아이오닉5로 자켓·후드·바지를 만든다?, “반도체 확보가 곧 전기차 주도권”…현대차 ‘폭발적 수요’ 선제 대응, 현대車, 반도체 내재화 큰 꿈 "많은 투자·시간 걸려도 해낼 것", 자동차 소재가 새 옷으로 재탄생…현대차, '리스타일 2021 프로젝트'..., 현대차그룹에 간부노조 생겼다, 현대車, 반도체 내재화 큰 꿈 "많은 투자·시간 걸려도 해낼 것", '8.8조원' 美 전기차 투자 준비한 현대차 "인프라법 통과에 달려", 현대차그룹에 간부노조 생겼다, 취임 후 시총 30조 '쑥'...위기에도 '질주..., '알량한 자존심 버린' 그가 이끈 현대차의 변화, '자동차주' 바닥찍었나...외인·기관도 사들인 현대차·기아, 전망은?, 현대차·기아·두산퓨얼셀 '수소연료전지 분산 발전' 시범운전 착수, “현대차, 반도체 자체개발 원한다”, 현대차 북미사장 "반도체 자체 개발에 공들이고 있다", 車폐기물, 옷이 되다...현대차, 업사이클링 패션 공개, 자동차 소재가 새 옷으로 재탄생…현대차, '리스타일 2021 프로젝트'..., 현대차 아이오닉5로 자켓·후드·바지를 만든다?, 현대車, 반도체 내재화 큰 꿈 "많은 투자·시간 걸려도 해낼 것", '8.8조원' 美 전기차 투자 준비한 현대차 "인프라법 통과에 달려", 자동차 소재가 새 옷으로 재탄생…현대차, '리스타일 2021 프로젝트'..., 현대차그룹에 간부노조 생겼다, 취임 후 시총 30조 '쑥'...위기에도 '질주..., '알량한 자존심 버린' 그가 이끈 현대차의 변화, '자동차주' 바닥찍었나...외인·기관도 사들인 현대차·기아, 전망은?, 현대차·기아·두산퓨얼셀 '수소연료전지 분산 발전' 시범운전 착수, “반도체 확보가 곧 전기차 주도권”…현대차 ‘폭발적 수요’ 선제 대응, “현대차, 반도체 자체개발 원한다”, '8.8조원' 美 전기차 투자 준비한 현대차 "인프라법 통과에 달려", “반도체 확보가 곧 전기차 주도권”…현대차 ‘폭발적 수요’ 선제 대응, 현대차·기아·두산퓨얼셀 '수소연료전지 분산 발전' 시범운전 착수, “현대차, 반도체 자체개발 원한다”, 현대차 북미사장 "반도체 자체 개발에 공들이고 있다", 車폐기물, 옷이 되다...현대차, 업사이클링 패션 공개, 현대차 아이오닉5로 자켓·후드·바지를 만든다?, “반도체 확보가 곧 전기차 주도권”…현대차 ‘폭발적 수요’ 선제 대응, 현대車, 반도체 내재화 큰 꿈 "많은 투자·시간 걸려도 해낼 것", '8.8조원' 美 전기차 투자 준비한 현대차 "인프라법 통과에 달려", 현대車, 반도체 내재화 큰 꿈 "많은 투자·시간 걸려도 해낼 것", 자동차 소재가 새 옷으로 재탄생…현대차, '리스타일 2021 프로젝트'..., 취임 후 시총 30조 '쑥'...위기에도 '질주..., '알량한 자존심 버린' 그가 이끈 현대차의 변화, '자동차주' 바닥찍었나...외인·기관도 사들인 현대차·기아, 전망은?, 현대차·기아·두산퓨얼셀 '수소연료전지 분산 발전' 시범운전 착수, “현대차, 반도체 자체개발 원한다”, 현대차 북미사장 "반도체 자체 개발에 공들이고 있다", 車폐기물, 옷이 되다...현대차, 업사이클링 패션 공개, 현대차 아이오닉5로 자켓·후드·바지를 만든다?, 현대차그룹에 간부노조 생겼다, 현대차 북미사장 "반도체 자체 개발에 공들이고 있다", 車폐기물, 옷이 되다...현대차, 업사이클링 패션 공개, 현대차 아이오닉5로 자켓·후드·바지를 만든다?, 현대차 북미사장 "반도체 자체 개발에 공들이고 있다", 車폐기물, 옷이 되다...현대차, 업사이클링 패션 공개, 현대차 아이오닉5로 자켓·후드·바지를 만든다?, “반도체 확보가 곧 전기차 주도권”…현대차 ‘폭발적 수요’ 선제 대응, 현대車, 반도체 내재화 큰 꿈 "많은 투자·시간 걸려도 해낼 것", '8.8조원' 美 전기차 투자 준비한 현대차 "인프라법 통과에 달려", 자동차 소재가 새 옷으로 재탄생…현대차, '리스타일 2021 프로젝트'..., 현대차그룹에 간부노조 생겼다, “현대차, 반도체 자체개발 원한다”, 취임 후 시총 30조 '쑥'...위기에도 '질주..., '자동차주' 바닥찍었나...외인·기관도 사들인 현대차·기아, 전망은?, 현대차·기아·두산퓨얼셀 '수소연료전지 분산 발전' 시범운전 착수, “현대차, 반도체 자체개발 원한다”, 현대차 북미사장 "반도체 자체 개발에 공들이고 있다", 車폐기물, 옷이 되다...현대차, 업사이클링 패션 공개, 현대차 아이오닉5로 자켓·후드·바지를 만든다?, “반도체 확보가 곧 전기차 주도권”…현대차 ‘폭발적 수요’ 선제 대응, 현대차 아이오닉5로 자켓·후드·바지를 만든다?, '알량한 자존심 버린' 그가 이끈 현대차의 변화, 현대차·기아·두산퓨얼셀 '수소연료전지 분산 발전' 시범운전 착수, '자동차주' 바닥찍었나...외인·기관도 사들인 현대차·기아, 전망은?, '알량한 자존심 버린' 그가 이끈 현대차의 변화, “반도체 확보가 곧 전기차 주도권”…현대차 ‘폭발적 수요’ 선제 대응, 현대車, 반도체 내재화 큰 꿈 "많은 투자·시간 걸려도 해낼 것", '8.8조원' 美 전기차 투자 준비한 현대차 "인프라법 통과에 달려", 자동차 소재가 새 옷으로 재탄생…현대차, '리스타일 2021 프로젝트'..., 현대차그룹에 간부노조 생겼다, 취임 후 시총 30조 '쑥'...위기에도 '질주..., '알량한 자존심 버린' 그가 이끈 현대차의 변화, '자동차주' 바닥찍었나...외인·기관도 사들인 현대차·기아, 전망은?, 현대차·기아·두산퓨얼셀 '수소연료전지 분산 발전' 시범운전 착수, “현대차, 반도체 자체개발 원한다”, 현대차 북미사장 "반도체 자체 개발에 공들이고 있다", 車폐기물, 옷이 되다...현대차, 업사이클링 패션 공개, 현대차 아이오닉5로 자켓·후드·바지를 만든다?, “반도체 확보가 곧 전기차 주도권”…현대차 ‘폭발적 수요’ 선제 대응, 현대車, 반도체 내재화 큰 꿈 "많은 투자·시간 걸려도 해낼 것", '8.8조원' 美 전기차 투자 준비한 현대차 "인프라법 통과에 달려", 자동차 소재가 새 옷으로 재탄생…현대차, '리스타일 2021 프로젝트'..., 현대차그룹에 간부노조 생겼다, 취임 후 시총 30조 '쑥'...위기에도 '질주..., 자동차 소재가 새 옷으로 재탄생…현대차, '리스타일 2021 프로젝트'..., “반도체 확보가 곧 전기차 주도권”…현대차 ‘폭발적 수요’ 선제 대응, '8.8조원' 美 전기차 투자 준비한 현대차 "인프라법 통과에 달려", '자동차주' 바닥찍었나...외인·기관도 사들인 현대차·기아, 전망은?, 현대차 북미사장 "반도체 자체 개발에 공들이고 있다", 車폐기물, 옷이 되다...현대차, 업사이클링 패션 공개, 현대차 아이오닉5로 자켓·후드·바지를 만든다?, “반도체 확보가 곧 전기차 주도권”…현대차 ‘폭발적 수요’ 선제 대응, 현대車, 반도체 내재화 큰 꿈 "많은 투자·시간 걸려도 해낼 것", '8.8조원' 美 전기차 투자 준비한 현대차 "인프라법 통과에 달려", 자동차 소재가 새 옷으로 재탄생…현대차, '리스타일 2021 프로젝트'..., 현대차그룹에 간부노조 생겼다, “현대차, 반도체 자체개발 원한다”, 취임 후 시총 30조 '쑥'...위기에도 '질주..., '자동차주' 바닥찍었나...외인·기관도 사들인 현대차·기아, 전망은?, 현대차·기아·두산퓨얼셀 '수소연료전지 분산 발전' 시범운전 착수, “현대차, 반도체 자체개발 원한다”, 현대차 북미사장 "반도체 자체 개발에 공들이고 있다", 車폐기물, 옷이 되다...현대차, 업사이클링 패션 공개, 현대차 아이오닉5로 자켓·후드·바지를 만든다?, “반도체 확보가 곧 전기차 주도권”…현대차 ‘폭발적 수요’ 선제 대응, 현대車, 반도체 내재화 큰 꿈 "많은 투자·시간 걸려도 해낼 것", '알량한 자존심 버린' 그가 이끈 현대차의 변화, '8.8조원' 美 전기차 투자 준비한 현대차 "인프라법 통과에 달려", 현대차·기아·두산퓨얼셀 '수소연료전지 분산 발전' 시범운전 착수, '알량한 자존심 버린' 그가 이끈 현대차의 변화, 현대車, 반도체 내재화 큰 꿈 "많은 투자·시간 걸려도 해낼 것", '8.8조원' 美 전기차 투자 준비한 현대차 "인프라법 통과에 달려", 자동차 소재가 새 옷으로 재탄생…현대차, '리스타일 2021 프로젝트'..., 현대차그룹에 간부노조 생겼다, 취임 후 시총 30조 '쑥'...위기에도 '질주..., '알량한 자존심 버린' 그가 이끈 현대차의 변화, '자동차주' 바닥찍었나...외인·기관도 사들인 현대차·기아, 전망은?, 현대차·기아·두산퓨얼셀 '수소연료전지 분산 발전' 시범운전 착수, '자동차주' 바닥찍었나...외인·기관도 사들인 현대차·기아, 전망은?, “현대차, 반도체 자체개발 원한다”, 車폐기물, 옷이 되다...현대차, 업사이클링 패션 공개, 현대차 아이오닉5로 자켓·후드·바지를 만든다?, “반도체 확보가 곧 전기차 주도권”…현대차 ‘폭발적 수요’ 선제 대응, 현대車, 반도체 내재화 큰 꿈 "많은 투자·시간 걸려도 해낼 것", '8.8조원' 美 전기차 투자 준비한 현대차 "인프라법 통과에 달려", 자동차 소재가 새 옷으로 재탄생…현대차, '리스타일 2021 프로젝트'..., 현대차그룹에 간부노조 생겼다, 취임 후 시총 30조 '쑥'...위기에도 '질주..., 현대차 북미사장 "반도체 자체 개발에 공들이고 있다", “반도체 확보가 곧 전기차 주도권”…현대차 ‘폭발적 수요’ 선제 대응, 자동차 소재가 새 옷으로 재탄생…현대차, '리스타일 2021 프로젝트'..., 취임 후 시총 30조 '쑥'...위기에도 '질주..., '8.8조원' 美 전기차 투자 준비한 현대차 "인프라법 통과에 달려", 자동차 소재가 새 옷으로 재탄생…현대차, '리스타일 2021 프로젝트'..., 현대차그룹에 간부노조 생겼다, 취임 후 시총 30조 '쑥'...위기에도 '질주..., '알량한 자존심 버린' 그가 이끈 현대차의 변화, '자동차주' 바닥찍었나...외인·기관도 사들인 현대차·기아, 전망은?, 현대차·기아·두산퓨얼셀 '수소연료전지 분산 발전' 시범운전 착수, “현대차, 반도체 자체개발 원한다”, 현대車, 반도체 내재화 큰 꿈 "많은 투자·시간 걸려도 해낼 것", 현대차 북미사장 "반도체 자체 개발에 공들이고 있다", 현대차 아이오닉5로 자켓·후드·바지를 만든다?, “반도체 확보가 곧 전기차 주도권”…현대차 ‘폭발적 수요’ 선제 대응, 현대車, 반도체 내재화 큰 꿈 "많은 투자·시간 걸려도 해낼 것", '8.8조원' 美 전기차 투자 준비한 현대차 "인프라법 통과에 달려", 자동차 소재가 새 옷으로 재탄생…현대차, '리스타일 2021 프로젝트'..., 현대차그룹에 간부노조 생겼다, 취임 후 시총 30조 '쑥'...위기에도 '질주..., '알량한 자존심 버린' 그가 이끈 현대차의 변화, 車폐기물, 옷이 되다...현대차, 업사이클링 패션 공개, 현대차그룹에 간부노조 생겼다, “반도체 확보가 곧 전기차 주도권”…현대차 ‘폭발적 수요’ 선제 대응, 車폐기물, 옷이 되다...현대차, 업사이클링 패션 공개, '알량한 자존심 버린' 그가 이끈 현대차의 변화, '자동차주' 바닥찍었나...외인·기관도 사들인 현대차·기아, 전망은?, 현대차·기아·두산퓨얼셀 '수소연료전지 분산 발전' 시범운전 착수, “현대차, 반도체 자체개발 원한다”, 현대차 북미사장 "반도체 자체 개발에 공들이고 있다", 車폐기물, 옷이 되다...현대차, 업사이클링 패션 공개, 현대차 아이오닉5로 자켓·후드·바지를 만든다?, “반도체 확보가 곧 전기차 주도권”…현대차 ‘폭발적 수요’ 선제 대응, 현대차 아이오닉5로 자켓·후드·바지를 만든다?, 현대車, 반도체 내재화 큰 꿈 "많은 투자·시간 걸려도 해낼 것", 자동차 소재가 새 옷으로 재탄생…현대차, '리스타일 2021 프로젝트'..., 현대차그룹에 간부노조 생겼다, 취임 후 시총 30조 '쑥'...위기에도 '질주..., '알량한 자존심 버린' 그가 이끈 현대차의 변화, '자동차주' 바닥찍었나...외인·기관도 사들인 현대차·기아, 전망은?, 현대차·기아·두산퓨얼셀 '수소연료전지 분산 발전' 시범운전 착수, “현대차, 반도체 자체개발 원한다”, 현대차 북미사장 "반도체 자체 개발에 공들이고 있다", '8.8조원' 美 전기차 투자 준비한 현대차 "인프라법 통과에 달려", 현대차 아이오닉5로 자켓·후드·바지를 만든다?, 車폐기물, 옷이 되다...현대차, 업사이클링 패션 공개, 현대차 북미사장 "반도체 자체 개발에 공들이고 있다", 현대차 아이오닉5로 자켓·후드·바지를 만든다?, “반도체 확보가 곧 전기차 주도권”…현대차 ‘폭발적 수요’ 선제 대응, 현대車, 반도체 내재화 큰 꿈 "많은 투자·시간 걸려도 해낼 것", '8.8조원' 美 전기차 투자 준비한 현대차 "인프라법 통과에 달려", 자동차 소재가 새 옷으로 재탄생…현대차, '리스타일 2021 프로젝트'..., 현대차그룹에 간부노조 생겼다, 취임 후 시총 30조 '쑥'...위기에도 '질주..., '알량한 자존심 버린' 그가 이끈 현대차의 변화, 車폐기물, 옷이 되다...현대차, 업사이클링 패션 공개, '자동차주' 바닥찍었나...외인·기관도 사들인 현대차·기아, 전망은?, “현대차, 반도체 자체개발 원한다”, 현대차 북미사장 "반도체 자체 개발에 공들이고 있다", 車폐기물, 옷이 되다...현대차, 업사이클링 패션 공개, 현대차 아이오닉5로 자켓·후드·바지를 만든다?, “반도체 확보가 곧 전기차 주도권”…현대차 ‘폭발적 수요’ 선제 대응, 현대車, 반도체 내재화 큰 꿈 "많은 투자·시간 걸려도 해낼 것", '8.8조원' 美 전기차 투자 준비한 현대차 "인프라법 통과에 달려", 자동차 소재가 새 옷으로 재탄생…현대차, '리스타일 2021 프로젝트'..., 현대차·기아·두산퓨얼셀 '수소연료전지 분산 발전' 시범운전 착수, 현대차그룹에 간부노조 생겼다, 현대차 북미사장 "반도체 자체 개발에 공들이고 있다", 현대차·기아·두산퓨얼셀 '수소연료전지 분산 발전' 시범운전 착수, 자동차 소재가 새 옷으로 재탄생…현대차, '리스타일 2021 프로젝트'..., 현대차그룹에 간부노조 생겼다, 취임 후 시총 30조 '쑥'...위기에도 '질주..., '알량한 자존심 버린' 그가 이끈 현대차의 변화, '자동차주' 바닥찍었나...외인·기관도 사들인 현대차·기아, 전망은?, 현대차·기아·두산퓨얼셀 '수소연료전지 분산 발전' 시범운전 착수, “현대차, 반도체 자체개발 원한다”, 현대차 북미사장 "반도체 자체 개발에 공들이고 있다", “현대차, 반도체 자체개발 원한다”, 車폐기물, 옷이 되다...현대차, 업사이클링 패션 공개, “반도체 확보가 곧 전기차 주도권”…현대차 ‘폭발적 수요’ 선제 대응, 현대車, 반도체 내재화 큰 꿈 "많은 투자·시간 걸려도 해낼 것", '8.8조원' 美 전기차 투자 준비한 현대차 "인프라법 통과에 달려", 자동차 소재가 새 옷으로 재탄생…현대차, '리스타일 2021 프로젝트'..., 현대차그룹에 간부노조 생겼다, 취임 후 시총 30조 '쑥'...위기에도 '질주..., '알량한 자존심 버린' 그가 이끈 현대차의 변화, '자동차주' 바닥찍었나...외인·기관도 사들인 현대차·기아, 전망은?, 현대차 아이오닉5로 자켓·후드·바지를 만든다?, 취임 후 시총 30조 '쑥'...위기에도 '질주..., '알량한 자존심 버린' 그가 이끈 현대차의 변화, '자동차주' 바닥찍었나...외인·기관도 사들인 현대차·기아, 전망은?, 취임 후 시총 30조 '쑥'...위기에도 '질주..., '알량한 자존심 버린' 그가 이끈 현대차의 변화, '자동차주' 바닥찍었나...외인·기관도 사들인 현대차·기아, 전망은?, 현대차·기아·두산퓨얼셀 '수소연료전지 분산 발전' 시범운전 착수, “현대차, 반도체 자체개발 원한다”, 현대차 북미사장 "반도체 자체 개발에 공들이고 있다", 車폐기물, 옷이 되다...현대차, 업사이클링 패션 공개, 현대차 아이오닉5로 자켓·후드·바지를 만든다?, 현대차그룹에 간부노조 생겼다, “반도체 확보가 곧 전기차 주도권”…현대차 ‘폭발적 수요’ 선제 대응, '8.8조원' 美 전기차 투자 준비한 현대차 "인프라법 통과에 달려", 자동차 소재가 새 옷으로 재탄생…현대차, '리스타일 2021 프로젝트'..., 현대차그룹에 간부노조 생겼다, 취임 후 시총 30조 '쑥'...위기에도 '질주..., '알량한 자존심 버린' 그가 이끈 현대차의 변화, '자동차주' 바닥찍었나...외인·기관도 사들인 현대차·기아, 전망은?, 현대차·기아·두산퓨얼셀 '수소연료전지 분산 발전' 시범운전 착수, “현대차, 반도체 자체개발 원한다”, 현대車, 반도체 내재화 큰 꿈 "많은 투자·시간 걸려도 해낼 것", 자동차 소재가 새 옷으로 재탄생…현대차, '리스타일 2021 프로젝트'..., '8.8조원' 美 전기차 투자 준비한 현대차 "인프라법 통과에 달려", 현대車, 반도체 내재화 큰 꿈 "많은 투자·시간 걸려도 해낼 것", 현대차·기아·두산퓨얼셀 '수소연료전지 분산 발전' 시범운전 착수, “현대차, 반도체 자체개발 원한다”, 현대차 북미사장 "반도체 자체 개발에 공들이고 있다", 車폐기물, 옷이 되다...현대차, 업사이클링 패션 공개, 현대차 아이오닉5로 자켓·후드·바지를 만든다?, “반도체 확보가 곧 전기차 주도권”…현대차 ‘폭발적 수요’ 선제 대응, 현대車, 반도체 내재화 큰 꿈 "많은 투자·시간 걸려도 해낼 것", '8.8조원' 美 전기차 투자 준비한 현대차 "인프라법 통과에 달려", 자동차 소재가 새 옷으로 재탄생…현대차, '리스타일 2021 프로젝트'..., 현대차그룹에 간부노조 생겼다, 취임 후 시총 30조 '쑥'...위기에도 '질주..., '알량한 자존심 버린' 그가 이끈 현대차의 변화, '자동차주' 바닥찍었나...외인·기관도 사들인 현대차·기아, 전망은?, 현대차·기아·두산퓨얼셀 '수소연료전지 분산 발전' 시범운전 착수, “현대차, 반도체 자체개발 원한다”, 현대차 북미사장 "반도체 자체 개발에 공들이고 있다", 車폐기물, 옷이 되다...현대차, 업사이클링 패션 공개, 현대차 아이오닉5로 자켓·후드·바지를 만든다?, “반도체 확보가 곧 전기차 주도권”…현대차 ‘폭발적 수요’ 선제 대응, 현대車, 반도체 내재화 큰 꿈 "많은 투자·시간 걸려도 해낼 것", '알량한 자존심 버린' 그가 이끈 현대차의 변화, 자동차 소재가 새 옷으로 재탄생…현대차, '리스타일 2021 프로젝트'..., 현대차그룹에 간부노조 생겼다, 현대차그룹에 간부노조 생겼다, 자동차 소재가 새 옷으로 재탄생…현대차, '리스타일 2021 프로젝트'..., '8.8조원' 美 전기차 투자 준비한 현대차 "인프라법 통과에 달려", 현대車, 반도체 내재화 큰 꿈 "많은 투자·시간 걸려도 해낼 것", “반도체 확보가 곧 전기차 주도권”…현대차 ‘폭발적 수요’ 선제 대응, 현대차 아이오닉5로 자켓·후드·바지를 만든다?, 車폐기물, 옷이 되다...현대차, 업사이클링 패션 공개, 현대차 북미사장 "반도체 자체 개발에 공들이고 있다", 취임 후 시총 30조 '쑥'...위기에도 '질주..., “현대차, 반도체 자체개발 원한다”, '자동차주' 바닥찍었나...외인·기관도 사들인 현대차·기아, 전망은?, '알량한 자존심 버린' 그가 이끈 현대차의 변화, 취임 후 시총 30조 '쑥'...위기에도 '질주..., 현대차그룹에 간부노조 생겼다, 자동차 소재가 새 옷으로 재탄생…현대차, '리스타일 2021 프로젝트'..., '8.8조원' 美 전기차 투자 준비한 현대차 "인프라법 통과에 달려", 현대車, 반도체 내재화 큰 꿈 "많은 투자·시간 걸려도 해낼 것", “반도체 확보가 곧 전기차 주도권”…현대차 ‘폭발적 수요’ 선제 대응, 현대차·기아·두산퓨얼셀 '수소연료전지 분산 발전' 시범운전 착수, 현대차 아이오닉5로 자켓·후드·바지를 만든다?, '알량한 자존심 버린' 그가 이끈 현대차의 변화, 현대차·기아·두산퓨얼셀 '수소연료전지 분산 발전' 시범운전 착수, “반도체 확보가 곧 전기차 주도권”…현대차 ‘폭발적 수요’ 선제 대응, 현대차 아이오닉5로 자켓·후드·바지를 만든다?, 車폐기물, 옷이 되다...현대차, 업사이클링 패션 공개, 현대차 북미사장 "반도체 자체 개발에 공들이고 있다", “현대차, 반도체 자체개발 원한다”, 현대차·기아·두산퓨얼셀 '수소연료전지 분산 발전' 시범운전 착수, '자동차주' 바닥찍었나...외인·기관도 사들인 현대차·기아, 전망은?, '알량한 자존심 버린' 그가 이끈 현대차의 변화, '자동차주' 바닥찍었나...외인·기관도 사들인 현대차·기아, 전망은?, 취임 후 시총 30조 '쑥'...위기에도 '질주..., 자동차 소재가 새 옷으로 재탄생…현대차, '리스타일 2021 프로젝트'..., '8.8조원' 美 전기차 투자 준비한 현대차 "인프라법 통과에 달려", 현대車, 반도체 내재화 큰 꿈 "많은 투자·시간 걸려도 해낼 것", “반도체 확보가 곧 전기차 주도권”…현대차 ‘폭발적 수요’ 선제 대응, 현대차 아이오닉5로 자켓·후드·바지를 만든다?, 車폐기물, 옷이 되다...현대차, 업사이클링 패션 공개, 현대차 북미사장 "반도체 자체 개발에 공들이고 있다", “현대차, 반도체 자체개발 원한다”, 현대차그룹에 간부노조 생겼다, 현대車, 반도체 내재화 큰 꿈 "많은 투자·시간 걸려도 해낼 것", 車폐기물, 옷이 되다...현대차, 업사이클링 패션 공개, “현대차, 반도체 자체개발 원한다”, 현대차 아이오닉5로 자켓·후드·바지를 만든다?, 車폐기물, 옷이 되다...현대차, 업사이클링 패션 공개, 현대차 북미사장 "반도체 자체 개발에 공들이고 있다", “현대차, 반도체 자체개발 원한다”, 현대차·기아·두산퓨얼셀 '수소연료전지 분산 발전' 시범운전 착수, '자동차주' 바닥찍었나...외인·기관도 사들인 현대차·기아, 전망은?, '알량한 자존심 버린' 그가 이끈 현대차의 변화, 취임 후 시총 30조 '쑥'...위기에도 '질주..., “반도체 확보가 곧 전기차 주도권”…현대차 ‘폭발적 수요’ 선제 대응, 현대차그룹에 간부노조 생겼다, '8.8조원' 美 전기차 투자 준비한 현대차 "인프라법 통과에 달려", 현대車, 반도체 내재화 큰 꿈 "많은 투자·시간 걸려도 해낼 것", “반도체 확보가 곧 전기차 주도권”…현대차 ‘폭발적 수요’ 선제 대응, 현대차 아이오닉5로 자켓·후드·바지를 만든다?, 車폐기물, 옷이 되다...현대차, 업사이클링 패션 공개, 현대차 북미사장 "반도체 자체 개발에 공들이고 있다", “현대차, 반도체 자체개발 원한다”, 현대차·기아·두산퓨얼셀 '수소연료전지 분산 발전' 시범운전 착수, 자동차 소재가 새 옷으로 재탄생…현대차, '리스타일 2021 프로젝트'..., 현대차 북미사장 "반도체 자체 개발에 공들이고 있다", 현대車, 반도체 내재화 큰 꿈 "많은 투자·시간 걸려도 해낼 것", 자동차 소재가 새 옷으로 재탄생…현대차, '리스타일 2021 프로젝트'..., 현대차·기아·두산퓨얼셀 '수소연료전지 분산 발전' 시범운전 착수, '자동차주' 바닥찍었나...외인·기관도 사들인 현대차·기아, 전망은?, '알량한 자존심 버린' 그가 이끈 현대차의 변화, 취임 후 시총 30조 '쑥'...위기에도 '질주..., 현대차그룹에 간부노조 생겼다, 자동차 소재가 새 옷으로 재탄생…현대차, '리스타일 2021 프로젝트'..., '8.8조원' 美 전기차 투자 준비한 현대차 "인프라법 통과에 달려", 현대車, 반도체 내재화 큰 꿈 "많은 투자·시간 걸려도 해낼 것", '8.8조원' 美 전기차 투자 준비한 현대차 "인프라법 통과에 달려", “반도체 확보가 곧 전기차 주도권”…현대차 ‘폭발적 수요’ 선제 대응, 車폐기물, 옷이 되다...현대차, 업사이클링 패션 공개, 현대차 북미사장 "반도체 자체 개발에 공들이고 있다", “현대차, 반도체 자체개발 원한다”, 현대차·기아·두산퓨얼셀 '수소연료전지 분산 발전' 시범운전 착수, '자동차주' 바닥찍었나...외인·기관도 사들인 현대차·기아, 전망은?, '알량한 자존심 버린' 그가 이끈 현대차의 변화, 취임 후 시총 30조 '쑥'...위기에도 '질주..., 현대차그룹에 간부노조 생겼다, 현대차 아이오닉5로 자켓·후드·바지를 만든다?, '8.8조원' 美 전기차 투자 준비한 현대차 "인프라법 통과에 달려", 자동차 소재가 새 옷으로 재탄생…현대차, '리스타일 2021 프로젝트'..., 현대차그룹에 간부노조 생겼다, '8.8조원' 美 전기차 투자 준비한 현대차 "인프라법 통과에 달려", 현대車, 반도체 내재화 큰 꿈 "많은 투자·시간 걸려도 해낼 것", “반도체 확보가 곧 전기차 주도권”…현대차 ‘폭발적 수요’ 선제 대응, 현대차 아이오닉5로 자켓·후드·바지를 만든다?, 車폐기물, 옷이 되다...현대차, 업사이클링 패션 공개, 현대차 북미사장 "반도체 자체 개발에 공들이고 있다", “현대차, 반도체 자체개발 원한다”, 현대차·기아·두산퓨얼셀 '수소연료전지 분산 발전' 시범운전 착수, 자동차 소재가 새 옷으로 재탄생…현대차, '리스타일 2021 프로젝트'..., '자동차주' 바닥찍었나...외인·기관도 사들인 현대차·기아, 전망은?, 취임 후 시총 30조 '쑥'...위기에도 '질주..., 현대차그룹에 간부노조 생겼다, 자동차 소재가 새 옷으로 재탄생…현대차, '리스타일 2021 프로젝트'..., '8.8조원' 美 전기차 투자 준비한 현대차 "인프라법 통과에 달려", 현대車, 반도체 내재화 큰 꿈 "많은 투자·시간 걸려도 해낼 것", “반도체 확보가 곧 전기차 주도권”…현대차 ‘폭발적 수요’ 선제 대응, 현대차 아이오닉5로 자켓·후드·바지를 만든다?, 車폐기물, 옷이 되다...현대차, 업사이클링 패션 공개, '알량한 자존심 버린' 그가 이끈 현대차의 변화, 현대차 북미사장 "반도체 자체 개발에 공들이고 있다", 현대차그룹에 간부노조 생겼다, '알량한 자존심 버린' 그가 이끈 현대차의 변화, 車폐기물, 옷이 되다...현대차, 업사이클링 패션 공개, 현대차 북미사장 "반도체 자체 개발에 공들이고 있다", “현대차, 반도체 자체개발 원한다”, 현대차·기아·두산퓨얼셀 '수소연료전지 분산 발전' 시범운전 착수, '자동차주' 바닥찍었나...외인·기관도 사들인 현대차·기아, 전망은?, '알량한 자존심 버린' 그가 이끈 현대차의 변화, 취임 후 시총 30조 '쑥'...위기에도 '질주..., 현대차그룹에 간부노조 생겼다, 취임 후 시총 30조 '쑥'...위기에도 '질주..., 자동차 소재가 새 옷으로 재탄생…현대차, '리스타일 2021 프로젝트'..., 현대車, 반도체 내재화 큰 꿈 "많은 투자·시간 걸려도 해낼 것", “반도체 확보가 곧 전기차 주도권”…현대차 ‘폭발적 수요’ 선제 대응, 현대차 아이오닉5로 자켓·후드·바지를 만든다?, 車폐기물, 옷이 되다...현대차, 업사이클링 패션 공개, 현대차 북미사장 "반도체 자체 개발에 공들이고 있다", “현대차, 반도체 자체개발 원한다”, 현대차·기아·두산퓨얼셀 '수소연료전지 분산 발전' 시범운전 착수, '자동차주' 바닥찍었나...외인·기관도 사들인 현대차·기아, 전망은?, '8.8조원' 美 전기차 투자 준비한 현대차 "인프라법 통과에 달려", “현대차, 반도체 자체개발 원한다”, 현대차·기아·두산퓨얼셀 '수소연료전지 분산 발전' 시범운전 착수, '자동차주' 바닥찍었나...외인·기관도 사들인 현대차·기아, 전망은?, “현대차, 반도체 자체개발 원한다”, 현대차·기아·두산퓨얼셀 '수소연료전지 분산 발전' 시범운전 착수, '자동차주' 바닥찍었나...외인·기관도 사들인 현대차·기아, 전망은?, '알량한 자존심 버린' 그가 이끈 현대차의 변화, 취임 후 시총 30조 '쑥'...위기에도 '질주..., 현대차그룹에 간부노조 생겼다, 자동차 소재가 새 옷으로 재탄생…현대차, '리스타일 2021 프로젝트'..., '8.8조원' 美 전기차 투자 준비한 현대차 "인프라법 통과에 달려", 현대차 북미사장 "반도체 자체 개발에 공들이고 있다", 현대車, 반도체 내재화 큰 꿈 "많은 투자·시간 걸려도 해낼 것", 현대차 아이오닉5로 자켓·후드·바지를 만든다?, 車폐기물, 옷이 되다...현대차, 업사이클링 패션 공개, 현대차 북미사장 "반도체 자체 개발에 공들이고 있다", “현대차, 반도체 자체개발 원한다”, 현대차·기아·두산퓨얼셀 '수소연료전지 분산 발전' 시범운전 착수, '자동차주' 바닥찍었나...외인·기관도 사들인 현대차·기아, 전망은?, '알량한 자존심 버린' 그가 이끈 현대차의 변화, 취임 후 시총 30조 '쑥'...위기에도 '질주..., “반도체 확보가 곧 전기차 주도권”…현대차 ‘폭발적 수요’ 선제 대응, 車폐기물, 옷이 되다...현대차, 업사이클링 패션 공개, 현대차 아이오닉5로 자켓·후드·바지를 만든다?, “반도체 확보가 곧 전기차 주도권”…현대차 ‘폭발적 수요’ 선제 대응, '알량한 자존심 버린' 그가 이끈 현대차의 변화, 취임 후 시총 30조 '쑥'...위기에도 '질주..., 현대차그룹에 간부노조 생겼다, 자동차 소재가 새 옷으로 재탄생…현대차, '리스타일 2021 프로젝트'..., '8.8조원' 美 전기차 투자 준비한 현대차 "인프라법 통과에 달려", 현대車, 반도체 내재화 큰 꿈 "많은 투자·시간 걸려도 해낼 것", “반도체 확보가 곧 전기차 주도권”…현대차 ‘폭발적 수요’ 선제 대응, 현대차 아이오닉5로 자켓·후드·바지를 만든다?, 車폐기물, 옷이 되다...현대차, 업사이클링 패션 공개, 현대차 북미사장 "반도체 자체 개발에 공들이고 있다", “현대차, 반도체 자체개발 원한다”, 현대차·기아·두산퓨얼셀 '수소연료전지 분산 발전' 시범운전 착수, '자동차주' 바닥찍었나...외인·기관도 사들인 현대차·기아, 전망은?, '알량한 자존심 버린' 그가 이끈 현대차의 변화, 취임 후 시총 30조 '쑥'...위기에도 '질주..., 현대차그룹에 간부노조 생겼다, 자동차 소재가 새 옷으로 재탄생…현대차, '리스타일 2021 프로젝트'..., '8.8조원' 美 전기차 투자 준비한 현대차 "인프라법 통과에 달려", 현대車, 반도체 내재화 큰 꿈 "많은 투자·시간 걸려도 해낼 것", '자동차주' 바닥찍었나...외인·기관도 사들인 현대차·기아, 전망은?, '알량한 자존심 버린' 그가 이끈 현대차의 변화, 취임 후 시총 30조 '쑥'...위기에도 '질주..., 현대차그룹에 간부노조 생겼다, “현대차, 반도체 자체개발 원한다”, 현대차·기아·두산퓨얼셀 '수소연료전지 분산 발전' 시범운전 착수, '자동차주' 바닥찍었나...외인·기관도 사들인 현대차·기아, 전망은?, '알량한 자존심 버린' 그가 이끈 현대차의 변화, 취임 후 시총 30조 '쑥'...위기에도 '질주..., 현대차그룹에 간부노조 생겼다, 자동차 소재가 새 옷으로 재탄생…현대차, '리스타일 2021 프로젝트'..., '8.8조원' 美 전기차 투자 준비한 현대차 "인프라법 통과에 달려", 현대차 북미사장 "반도체 자체 개발에 공들이고 있다", 현대車, 반도체 내재화 큰 꿈 "많은 투자·시간 걸려도 해낼 것", 현대차 아이오닉5로 자켓·후드·바지를 만든다?, 車폐기물, 옷이 되다...현대차, 업사이클링 패션 공개, 현대차 북미사장 "반도체 자체 개발에 공들이고 있다", “현대차, 반도체 자체개발 원한다”, 현대차·기아·두산퓨얼셀 '수소연료전지 분산 발전' 시범운전 착수, '자동차주' 바닥찍었나...외인·기관도 사들인 현대차·기아, 전망은?, '알량한 자존심 버린' 그가 이끈 현대차의 변화, 취임 후 시총 30조 '쑥'...위기에도 '질주..., “반도체 확보가 곧 전기차 주도권”…현대차 ‘폭발적 수요’ 선제 대응, 현대차그룹에 간부노조 생겼다, 車폐기물, 옷이 되다...현대차, 업사이클링 패션 공개, “반도체 확보가 곧 전기차 주도권”…현대차 ‘폭발적 수요’ 선제 대응, 취임 후 시총 30조 '쑥'...위기에도 '질주..., 현대차그룹에 간부노조 생겼다, 자동차 소재가 새 옷으로 재탄생…현대차, '리스타일 2021 프로젝트'..., '8.8조원' 美 전기차 투자 준비한 현대차 "인프라법 통과에 달려", 현대車, 반도체 내재화 큰 꿈 "많은 투자·시간 걸려도 해낼 것", “반도체 확보가 곧 전기차 주도권”…현대차 ‘폭발적 수요’ 선제 대응, 현대차 아이오닉5로 자켓·후드·바지를 만든다?, 車폐기물, 옷이 되다...현대차, 업사이클링 패션 공개, 현대차 아이오닉5로 자켓·후드·바지를 만든다?, 현대차 북미사장 "반도체 자체 개발에 공들이고 있다", 현대차·기아·두산퓨얼셀 '수소연료전지 분산 발전' 시범운전 착수, '자동차주' 바닥찍었나...외인·기관도 사들인 현대차·기아, 전망은?, '알량한 자존심 버린' 그가 이끈 현대차의 변화, 취임 후 시총 30조 '쑥'...위기에도 '질주..., 현대차그룹에 간부노조 생겼다, 자동차 소재가 새 옷으로 재탄생…현대차, '리스타일 2021 프로젝트'..., '8.8조원' 美 전기차 투자 준비한 현대차 "인프라법 통과에 달려", 현대車, 반도체 내재화 큰 꿈 "많은 투자·시간 걸려도 해낼 것", “현대차, 반도체 자체개발 원한다”, 자동차 소재가 새 옷으로 재탄생…현대차, '리스타일 2021 프로젝트'..., '8.8조원' 美 전기차 투자 준비한 현대차 "인프라법 통과에 달려", 현대車, 반도체 내재화 큰 꿈 "많은 투자·시간 걸려도 해낼 것", '8.8조원' 美 전기차 투자 준비한 현대차 "인프라법 통과에 달려", 현대차·기아, 수소경제 가속…수소연료전지 발전시스템 실증 착수, 현대차·기아·두산퓨얼셀 '수소연료전지 분산 발전' 시범운전 착수, “현대차, 반도체 자체개발 원한다”, 현대차 북미사장 "반도체 자체 개발에 공들이고 있다", 자동차 소재가 새 옷으로 재탄생…현대차, '리스타일 2021 프로젝트'..., 현대차그룹에 간부노조 생겼다, 취임 후 시총 30조 '쑥'...위기에도 '질주..., 현대차 '반도체' 직접 만들까? 고위 임원 "독자 개발 원한다", '알량한 자존심 버린' 그가 이끈 현대차의 변화, “현대차, 반도체 자체개발 원한다”, 현대차 북미사장 "반도체 자체 개발에 공들이고 있다", 車폐기물, 옷이 되다...현대차, 업사이클링 패션 공개, 현대차 아이오닉5로 자켓·후드·바지를 만든다?, “반도체 확보가 곧 전기차 주도권”…현대차 ‘폭발적 수요’ 선제 대응, 현대車, 반도체 내재화 큰 꿈 "많은 투자·시간 걸려도 해낼 것", '8.8조원' 美 전기차 투자 준비한 현대차 "인프라법 통과에 달려", '자동차주' 바닥찍었나...외인·기관도 사들인 현대차·기아, 전망은?, 현대차·기아·두산퓨얼셀 '수소연료전지 분산 발전' 시범운전 착수, 현대차·기아, 태양광·풍력 보완할 수소 발전시스템 실증 시작, 현대차·기아-두산, 수소연료전지 발전 시동…불안정한 태양광·풍력 보완, “반도체 확보가 곧 전기차 주도권”…현대차 ‘폭발적 수요’ 선제 대응, “반도체 확보가 곧 전기차 주도권”…현대차 ‘폭발적 수요’ 선제 대응, 현대차 아이오닉5로 자켓·후드·바지를 만든다?, 車폐기물, 옷이 되다...현대차, 업사이클링 패션 공개, 현대차 북미사장 "반도체 자체 개발에 공들이고 있다", “현대차, 반도체 자체개발 원한다”, 현대차·기아·두산퓨얼셀 '수소연료전지 분산 발전' 시범운전 착수, '자동차주' 바닥찍었나...외인·기관도 사들인 현대차·기아, 전망은?, '알량한 자존심 버린' 그가 이끈 현대차의 변화, 취임 후 시총 30조 '쑥'...위기에도 '질주..., 현대차 반도체 자체개발 추진, "반도체 직접 개발 원해" 현대차, 또 반도체 자립 선언...현대모비..., 부품조달 차질에···현대車, 반도체 자체개발, “현대차, 반도체 자체개발 원한다”, 현대차 "11월 반도체 공급 숨통"…연말 車생산 액셀 밟는다, 현대차 안전벨트로 옷 만들어, 현대차, 아이오닉5 친환경 소재 패션으로 재탄생, 현대차 안전벨트로 옷 만들어, 현대차, 아이오닉5 친환경 소재 패션으로 재탄생, "반도체 직접 개발 원해" 현대차, 또 반도체 자립 선언...현대모비스..., '알량한 자존심 버린' 그가 이끈 현대차의 변화, 취임 후 시총 30조 '쑥'...위기에도 '질주..., '자동차주' 바닥찍었나...외인·기관도 사들인 현대차·기아, 전망은?, “현대차, 반도체 자체개발 원한다”, '자동차주' 바닥찍었나...외인·기관도 사들인 현대차·기아, 전망은?, '알량한 자존심 버린' 그가 이끈 현대차의 변화, 취임 후 시총 30조 '쑥'...위기에도 '질주..., 현대차그룹에 간부노조 생겼다, 자동차 소재가 새 옷으로 재탄생…현대차, '리스타일 2021 프로젝트'..., '8.8조원' 美 전기차 투자 준비한 현대차 "인프라법 통과에 달려", 현대車, 반도체 내재화 큰 꿈 "많은 투자·시간 걸려도 해낼 것", “반도체 확보가 곧 전기차 주도권”…현대차 ‘폭발적 수요’ 선제 대응, 현대차·기아·두산퓨얼셀 '수소연료전지 분산 발전' 시범운전 착수, 현대차 아이오닉5로 자켓·후드·바지를 만든다?, 현대차 북미사장 "반도체 자체 개발에 공들이고 있다", “현대차, 반도체 자체개발 원한다”, 현대차·기아·두산퓨얼셀 '수소연료전지 분산 발전' 시범운전 착수, '자동차주' 바닥찍었나...외인·기관도 사들인 현대차·기아, 전망은?, '알량한 자존심 버린' 그가 이끈 현대차의 변화, 취임 후 시총 30조 '쑥'...위기에도 '질주..., 현대차그룹에 간부노조 생겼다, 자동차 소재가 새 옷으로 재탄생…현대차, '리스타일 2021 프로젝트'..., 車폐기물, 옷이 되다...현대차, 업사이클링 패션 공개, '8.8조원' 美 전기차 투자 준비한 현대차 "인프라법 통과에 달려", “현대차, 반도체 자체개발 원한다”, 車폐기물, 옷이 되다...현대차, 업사이클링 패션 공개, 자동차 소재가 새 옷으로 재탄생…현대차, '리스타일 2021 프로젝트'..., '8.8조원' 美 전기차 투자 준비한 현대차 "인프라법 통과에 달려", 현대車, 반도체 내재화 큰 꿈 "많은 투자·시간 걸려도 해낼 것", “반도체 확보가 곧 전기차 주도권”…현대차 ‘폭발적 수요’ 선제 대응, 현대차 아이오닉5로 자켓·후드·바지를 만든다?, 車폐기물, 옷이 되다...현대차, 업사이클링 패션 공개, 현대차 북미사장 "반도체 자체 개발에 공들이고 있다", “현대차, 반도체 자체개발 원한다”, 현대차 북미사장 "반도체 자체 개발에 공들이고 있다", 현대차·기아·두산퓨얼셀 '수소연료전지 분산 발전' 시범운전 착수, '알량한 자존심 버린' 그가 이끈 현대차의 변화, 취임 후 시총 30조 '쑥'...위기에도 '질주..., 현대차그룹에 간부노조 생겼다, 자동차 소재가 새 옷으로 재탄생…현대차, '리스타일 2021 프로젝트'..., '8.8조원' 美 전기차 투자 준비한 현대차 "인프라법 통과에 달려", 현대車, 반도체 내재화 큰 꿈 "많은 투자·시간 걸려도 해낼 것", “반도체 확보가 곧 전기차 주도권”…현대차 ‘폭발적 수요’ 선제 대응, 현대차 아이오닉5로 자켓·후드·바지를 만든다?, '자동차주' 바닥찍었나...외인·기관도 사들인 현대차·기아, 전망은?, 현대車, 반도체 내재화 큰 꿈 "많은 투자·시간 걸려도 해낼 것", “반도체 확보가 곧 전기차 주도권”…현대차 ‘폭발적 수요’ 선제 대응, 현대차 아이오닉5로 자켓·후드·바지를 만든다?, 현대車, 반도체 내재화 큰 꿈 "많은 투자·시간 걸려도 해낼 것", “반도체 확보가 곧 전기차 주도권”…현대차 ‘폭발적 수요’ 선제 대응, 현대차 아이오닉5로 자켓·후드·바지를 만든다?, 車폐기물, 옷이 되다...현대차, 업사이클링 패션 공개, 현대차 북미사장 "반도체 자체 개발에 공들이고 있다", “현대차, 반도체 자체개발 원한다”, 현대차·기아·두산퓨얼셀 '수소연료전지 분산 발전' 시범운전 착수, '자동차주' 바닥찍었나...외인·기관도 사들인 현대차·기아, 전망은?, '8.8조원' 美 전기차 투자 준비한 현대차 "인프라법 통과에 달려", '알량한 자존심 버린' 그가 이끈 현대차의 변화, 현대차그룹에 간부노조 생겼다, 자동차 소재가 새 옷으로 재탄생…현대차, '리스타일 2021 프로젝트'..., '8.8조원' 美 전기차 투자 준비한 현대차 "인프라법 통과에 달려", 현대車, 반도체 내재화 큰 꿈 "많은 투자·시간 걸려도 해낼 것", “반도체 확보가 곧 전기차 주도권”…현대차 ‘폭발적 수요’ 선제 대응, 현대차 아이오닉5로 자켓·후드·바지를 만든다?, 車폐기물, 옷이 되다...현대차, 업사이클링 패션 공개, 현대차 북미사장 "반도체 자체 개발에 공들이고 있다", 취임 후 시총 30조 '쑥'...위기에도 '질주..., 자동차 소재가 새 옷으로 재탄생…현대차, '리스타일 2021 프로젝트'..., 현대차그룹에 간부노조 생겼다, 취임 후 시총 30조 '쑥'...위기에도 '질주..., 車폐기물, 옷이 되다...현대차, 업사이클링 패션 공개, 현대차 북미사장 "반도체 자체 개발에 공들이고 있다", “현대차, 반도체 자체개발 원한다”, 현대차·기아·두산퓨얼셀 '수소연료전지 분산 발전' 시범운전 착수, '자동차주' 바닥찍었나...외인·기관도 사들인 현대차·기아, 전망은?, '알량한 자존심 버린' 그가 이끈 현대차의 변화, 취임 후 시총 30조 '쑥'...위기에도 '질주..., 현대차그룹에 간부노조 생겼다, 자동차 소재가 새 옷으로 재탄생…현대차, '리스타일 2021 프로젝트'..., '8.8조원' 美 전기차 투자 준비한 현대차 "인프라법 통과에 달려", 현대車, 반도체 내재화 큰 꿈 "많은 투자·시간 걸려도 해낼 것", “반도체 확보가 곧 전기차 주도권”…현대차 ‘폭발적 수요’ 선제 대응, 현대차 아이오닉5로 자켓·후드·바지를 만든다?, 車폐기물, 옷이 되다...현대차, 업사이클링 패션 공개, 현대차 북미사장 "반도체 자체 개발에 공들이고 있다", “현대차, 반도체 자체개발 원한다”, 현대차·기아·두산퓨얼셀 '수소연료전지 분산 발전' 시범운전 착수, '자동차주' 바닥찍었나...외인·기관도 사들인 현대차·기아, 전망은?, '알량한 자존심 버린' 그가 이끈 현대차의 변화, 현대차·기아·두산퓨얼셀 '수소연료전지 분산 발전' 시범운전 착수, 현대차·기아·두산퓨얼셀 '수소연료전지 분산 발전' 시범운전 착수, 車폐기물, 옷이 되다...현대차, 업사이클링 패션 공개, 현대차 북미사장 "반도체 자체 개발에 공들이고 있다", “현대차, 반도체 자체개발 원한다”, 현대차 북미사장 "반도체 자체 개발에 공들이고 있다", 車폐기물, 옷이 되다...현대차, 업사이클링 패션 공개, 현대차 아이오닉5로 자켓·후드·바지를 만든다?, “반도체 확보가 곧 전기차 주도권”…현대차 ‘폭발적 수요’ 선제 대응, 현대車, 반도체 내재화 큰 꿈 "많은 투자·시간 걸려도 해낼 것", '8.8조원' 美 전기차 투자 준비한 현대차 "인프라법 통과에 달려", 자동차 소재가 새 옷으로 재탄생…현대차, '리스타일 2021 프로젝트'..., 현대차·기아·두산퓨얼셀 '수소연료전지 분산 발전' 시범운전 착수, 현대차그룹에 간부노조 생겼다, '알량한 자존심 버린' 그가 이끈 현대차의 변화, '자동차주' 바닥찍었나...외인·기관도 사들인 현대차·기아, 전망은?, 현대차·기아·두산퓨얼셀 '수소연료전지 분산 발전' 시범운전 착수, “현대차, 반도체 자체개발 원한다”, 현대차 북미사장 "반도체 자체 개발에 공들이고 있다", 車폐기물, 옷이 되다...현대차, 업사이클링 패션 공개, 현대차 아이오닉5로 자켓·후드·바지를 만든다?, “반도체 확보가 곧 전기차 주도권”…현대차 ‘폭발적 수요’ 선제 대응, 취임 후 시총 30조 '쑥'...위기에도 '질주..., 현대車, 반도체 내재화 큰 꿈 "많은 투자·시간 걸려도 해낼 것", '자동차주' 바닥찍었나...외인·기관도 사들인 현대차·기아, 전망은?, 취임 후 시총 30조 '쑥'...위기에도 '질주..., “반도체 확보가 곧 전기차 주도권”…현대차 ‘폭발적 수요’ 선제 대응, 현대車, 반도체 내재화 큰 꿈 "많은 투자·시간 걸려도 해낼 것", '8.8조원' 美 전기차 투자 준비한 현대차 "인프라법 통과에 달려", 자동차 소재가 새 옷으로 재탄생…현대차, '리스타일 2021 프로젝트'..., 현대차그룹에 간부노조 생겼다, 취임 후 시총 30조 '쑥'...위기에도 '질주..., '알량한 자존심 버린' 그가 이끈 현대차의 변화, '자동차주' 바닥찍었나...외인·기관도 사들인 현대차·기아, 전망은?, '알량한 자존심 버린' 그가 이끈 현대차의 변화, 현대차·기아·두산퓨얼셀 '수소연료전지 분산 발전' 시범운전 착수, 현대차 북미사장 "반도체 자체 개발에 공들이고 있다", 車폐기물, 옷이 되다...현대차, 업사이클링 패션 공개, 현대차 아이오닉5로 자켓·후드·바지를 만든다?, “반도체 확보가 곧 전기차 주도권”…현대차 ‘폭발적 수요’ 선제 대응, 현대車, 반도체 내재화 큰 꿈 "많은 투자·시간 걸려도 해낼 것", '8.8조원' 美 전기차 투자 준비한 현대차 "인프라법 통과에 달려", 자동차 소재가 새 옷으로 재탄생…현대차, '리스타일 2021 프로젝트'..., 현대차그룹에 간부노조 생겼다, “현대차, 반도체 자체개발 원한다”, 현대차 아이오닉5로 자켓·후드·바지를 만든다?, '8.8조원' 美 전기차 투자 준비한 현대차 "인프라법 통과에 달려", 현대차그룹에 간부노조 생겼다, 현대車, 반도체 내재화 큰 꿈 "많은 투자·시간 걸려도 해낼 것", '8.8조원' 美 전기차 투자 준비한 현대차 "인프라법 통과에 달려", 자동차 소재가 새 옷으로 재탄생…현대차, '리스타일 2021 프로젝트'..., 현대차그룹에 간부노조 생겼다, 취임 후 시총 30조 '쑥'...위기에도 '질주..., '알량한 자존심 버린' 그가 이끈 현대차의 변화, '자동차주' 바닥찍었나...외인·기관도 사들인 현대차·기아, 전망은?, 현대차·기아·두산퓨얼셀 '수소연료전지 분산 발전' 시범운전 착수, “반도체 확보가 곧 전기차 주도권”…현대차 ‘폭발적 수요’ 선제 대응, “현대차, 반도체 자체개발 원한다”, 車폐기물, 옷이 되다...현대차, 업사이클링 패션 공개, 현대차 아이오닉5로 자켓·후드·바지를 만든다?, “반도체 확보가 곧 전기차 주도권”…현대차 ‘폭발적 수요’ 선제 대응, 현대車, 반도체 내재화 큰 꿈 "많은 투자·시간 걸려도 해낼 것", '8.8조원' 美 전기차 투자 준비한 현대차 "인프라법 통과에 달려", 자동차 소재가 새 옷으로 재탄생…현대차, '리스타일 2021 프로젝트'..., 현대차그룹에 간부노조 생겼다, 취임 후 시총 30조 '쑥'...위기에도 '질주..., 현대차 북미사장 "반도체 자체 개발에 공들이고 있다", 자동차 소재가 새 옷으로 재탄생…현대차, '리스타일 2021 프로젝트'..., 현대차 아이오닉5로 자켓·후드·바지를 만든다?, 현대차 북미사장 "반도체 자체 개발에 공들이고 있다", 취임 후 시총 30조 '쑥'...위기에도 '질주..., '알량한 자존심 버린' 그가 이끈 현대차의 변화, '자동차주' 바닥찍었나...외인·기관도 사들인 현대차·기아, 전망은?, 현대차·기아·두산퓨얼셀 '수소연료전지 분산 발전' 시범운전 착수, “현대차, 반도체 자체개발 원한다”, 현대차 북미사장 "반도체 자체 개발에 공들이고 있다", 車폐기물, 옷이 되다...현대차, 업사이클링 패션 공개, 현대차 아이오닉5로 자켓·후드·바지를 만든다?, 車폐기물, 옷이 되다...현대차, 업사이클링 패션 공개, “반도체 확보가 곧 전기차 주도권”…현대차 ‘폭발적 수요’ 선제 대응, '8.8조원' 美 전기차 투자 준비한 현대차 "인프라법 통과에 달려", 자동차 소재가 새 옷으로 재탄생…현대차, '리스타일 2021 프로젝트'..., 현대차그룹에 간부노조 생겼다, 취임 후 시총 30조 '쑥'...위기에도 '질주..., '알량한 자존심 버린' 그가 이끈 현대차의 변화, '자동차주' 바닥찍었나...외인·기관도 사들인 현대차·기아, 전망은?, 현대차·기아·두산퓨얼셀 '수소연료전지 분산 발전' 시범운전 착수, “현대차, 반도체 자체개발 원한다”, 현대車, 반도체 내재화 큰 꿈 "많은 투자·시간 걸려도 해낼 것", 車폐기물, 옷이 되다...현대차, 업사이클링 패션 공개, 현대차 북미사장 "반도체 자체 개발에 공들이고 있다", “현대차, 반도체 자체개발 원한다”, 車폐기물, 옷이 되다...현대차, 업사이클링 패션 공개, 현대차 아이오닉5로 자켓·후드·바지를 만든다?, “반도체 확보가 곧 전기차 주도권”…현대차 ‘폭발적 수요’ 선제 대응, 현대車, 반도체 내재화 큰 꿈 "많은 투자·시간 걸려도 해낼 것", '8.8조원' 美 전기차 투자 준비한 현대차 "인프라법 통과에 달려", 자동차 소재가 새 옷으로 재탄생…현대차, '리스타일 2021 프로젝트'..., 현대차그룹에 간부노조 생겼다, 취임 후 시총 30조 '쑥'...위기에도 '질주..., 현대차 북미사장 "반도체 자체 개발에 공들이고 있다", '알량한 자존심 버린' 그가 이끈 현대차의 변화, 현대차·기아·두산퓨얼셀 '수소연료전지 분산 발전' 시범운전 착수, “현대차, 반도체 자체개발 원한다”, 현대차 북미사장 "반도체 자체 개발에 공들이고 있다", 車폐기물, 옷이 되다...현대차, 업사이클링 패션 공개, 현대차 아이오닉5로 자켓·후드·바지를 만든다?, “반도체 확보가 곧 전기차 주도권”…현대차 ‘폭발적 수요’ 선제 대응, 현대車, 반도체 내재화 큰 꿈 "많은 투자·시간 걸려도 해낼 것", '8.8조원' 美 전기차 투자 준비한 현대차 "인프라법 통과에 달려", '자동차주' 바닥찍었나...외인·기관도 사들인 현대차·기아, 전망은?, 자동차 소재가 새 옷으로 재탄생…현대차, '리스타일 2021 프로젝트'..., “현대차, 반도체 자체개발 원한다”, '자동차주' 바닥찍었나...외인·기관도 사들인 현대차·기아, 전망은?, '8.8조원' 美 전기차 투자 준비한 현대차 "인프라법 통과에 달려", 자동차 소재가 새 옷으로 재탄생…현대차, '리스타일 2021 프로젝트'..., 현대차그룹에 간부노조 생겼다, 취임 후 시총 30조 '쑥'...위기에도 '질주..., '알량한 자존심 버린' 그가 이끈 현대차의 변화, '자동차주' 바닥찍었나...외인·기관도 사들인 현대차·기아, 전망은?, 현대차·기아·두산퓨얼셀 '수소연료전지 분산 발전' 시범운전 착수, “현대차, 반도체 자체개발 원한다”, 현대차·기아·두산퓨얼셀 '수소연료전지 분산 발전' 시범운전 착수, 현대차 북미사장 "반도체 자체 개발에 공들이고 있다", 현대차 아이오닉5로 자켓·후드·바지를 만든다?, “반도체 확보가 곧 전기차 주도권”…현대차 ‘폭발적 수요’ 선제 대응, 현대車, 반도체 내재화 큰 꿈 "많은 투자·시간 걸려도 해낼 것", '8.8조원' 美 전기차 투자 준비한 현대차 "인프라법 통과에 달려", 자동차 소재가 새 옷으로 재탄생…현대차, '리스타일 2021 프로젝트'..., 현대차그룹에 간부노조 생겼다, 취임 후 시총 30조 '쑥'...위기에도 '질주..., '알량한 자존심 버린' 그가 이끈 현대차의 변화, 車폐기물, 옷이 되다...현대차, 업사이클링 패션 공개, 현대차그룹에 간부노조 생겼다, 취임 후 시총 30조 '쑥'...위기에도 '질주..., '알량한 자존심 버린' 그가 이끈 현대차의 변화, 현대차그룹에 간부노조 생겼다, 취임 후 시총 30조 '쑥'...위기에도 '질주..., '알량한 자존심 버린' 그가 이끈 현대차의 변화, '자동차주' 바닥찍었나...외인·기관도 사들인 현대차·기아, 전망은?, 현대차·기아·두산퓨얼셀 '수소연료전지 분산 발전' 시범운전 착수, “현대차, 반도체 자체개발 원한다”, 현대차 북미사장 "반도체 자체 개발에 공들이고 있다", 車폐기물, 옷이 되다...현대차, 업사이클링 패션 공개, 자동차 소재가 새 옷으로 재탄생…현대차, '리스타일 2021 프로젝트'..., 현대차 아이오닉5로 자켓·후드·바지를 만든다?, 현대車, 반도체 내재화 큰 꿈 "많은 투자·시간 걸려도 해낼 것", '8.8조원' 美 전기차 투자 준비한 현대차 "인프라법 통과에 달려", 자동차 소재가 새 옷으로 재탄생…현대차, '리스타일 2021 프로젝트'..., 현대차그룹에 간부노조 생겼다, 취임 후 시총 30조 '쑥'...위기에도 '질주..., '알량한 자존심 버린' 그가 이끈 현대차의 변화, '자동차주' 바닥찍었나...외인·기관도 사들인 현대차·기아, 전망은?, 현대차·기아·두산퓨얼셀 '수소연료전지 분산 발전' 시범운전 착수, “반도체 확보가 곧 전기차 주도권”…현대차 ‘폭발적 수요’ 선제 대응, '8.8조원' 美 전기차 투자 준비한 현대차 "인프라법 통과에 달려", 현대車, 반도체 내재화 큰 꿈 "많은 투자·시간 걸려도 해낼 것", “반도체 확보가 곧 전기차 주도권”…현대차 ‘폭발적 수요’ 선제 대응, '자동차주' 바닥찍었나...외인·기관도 사들인 현대차·기아, 전망은?, 현대차·기아·두산퓨얼셀 '수소연료전지 분산 발전' 시범운전 착수, “현대차, 반도체 자체개발 원한다”, 현대차 북미사장 "반도체 자체 개발에 공들이고 있다", 車폐기물, 옷이 되다...현대차, 업사이클링 패션 공개, 현대차 아이오닉5로 자켓·후드·바지를 만든다?, “반도체 확보가 곧 전기차 주도권”…현대차 ‘폭발적 수요’ 선제 대응, 현대車, 반도체 내재화 큰 꿈 "많은 투자·시간 걸려도 해낼 것", '8.8조원' 美 전기차 투자 준비한 현대차 "인프라법 통과에 달려", 자동차 소재가 새 옷으로 재탄생…현대차, '리스타일 2021 프로젝트'..., 현대차그룹에 간부노조 생겼다, 취임 후 시총 30조 '쑥'...위기에도 '질주..., '알량한 자존심 버린' 그가 이끈 현대차의 변화, '자동차주' 바닥찍었나...외인·기관도 사들인 현대차·기아, 전망은?, 현대차·기아·두산퓨얼셀 '수소연료전지 분산 발전' 시범운전 착수, “현대차, 반도체 자체개발 원한다”, 현대차 북미사장 "반도체 자체 개발에 공들이고 있다", 車폐기물, 옷이 되다...현대차, 업사이클링 패션 공개, 현대차 아이오닉5로 자켓·후드·바지를 만든다?, '알량한 자존심 버린' 그가 이끈 현대차의 변화, '자동차주' 바닥찍었나...외인·기관도 사들인 현대차·기아, 전망은?, 현대차·기아·두산퓨얼셀 '수소연료전지 분산 발전' 시범운전 착수, “현대차, 반도체 자체개발 원한다”, 현대차·기아·두산퓨얼셀 '수소연료전지 분산 발전' 시범운전 착수, '자동차주' 바닥찍었나...외인·기관도 사들인 현대차·기아, 전망은?, '알량한 자존심 버린' 그가 이끈 현대차의 변화, 취임 후 시총 30조 '쑥'...위기에도 '질주..., 현대차그룹에 간부노조 생겼다, 자동차 소재가 새 옷으로 재탄생…현대차, '리스타일 2021 프로젝트'..., '8.8조원' 美 전기차 투자 준비한 현대차 "인프라법 통과에 달려", 현대車, 반도체 내재화 큰 꿈 "많은 투자·시간 걸려도 해낼 것", “현대차, 반도체 자체개발 원한다”, “반도체 확보가 곧 전기차 주도권”…현대차 ‘폭발적 수요’ 선제 대응, 車폐기물, 옷이 되다...현대차, 업사이클링 패션 공개, 현대차 북미사장 "반도체 자체 개발에 공들이고 있다", “현대차, 반도체 자체개발 원한다”, 현대차·기아·두산퓨얼셀 '수소연료전지 분산 발전' 시범운전 착수, '자동차주' 바닥찍었나...외인·기관도 사들인 현대차·기아, 전망은?, '알량한 자존심 버린' 그가 이끈 현대차의 변화, 취임 후 시총 30조 '쑥'...위기에도 '질주..., 현대차그룹에 간부노조 생겼다, 현대차 아이오닉5로 자켓·후드·바지를 만든다?, 자동차 소재가 새 옷으로 재탄생…현대차, '리스타일 2021 프로젝트'..., 현대차 북미사장 "반도체 자체 개발에 공들이고 있다", 현대차 아이오닉5로 자켓·후드·바지를 만든다?, 현대차·기아·두산퓨얼셀 '수소연료전지 분산 발전' 시범운전 착수, 현대차 아이오닉5로 자켓·후드·바지를 만든다?, '8.8조원' 美 전기차 투자 준비한 현대차 "인프라법 통과에 달려", 현대車, 반도체 내재화 큰 꿈 "많은 투자·시간 걸려도 해낼 것", “반도체 확보가 곧 전기차 주도권”…현대차 ‘폭발적 수요’ 선제 대응, 현대차 아이오닉5로 자켓·후드·바지를 만든다?, 車폐기물, 옷이 되다...현대차, 업사이클링 패션 공개, 현대차 북미사장 "반도체 자체 개발에 공들이고 있다", 車폐기물, 옷이 되다...현대차, 업사이클링 패션 공개, “현대차, 반도체 자체개발 원한다”, '자동차주' 바닥찍었나...외인·기관도 사들인 현대차·기아, 전망은?, '알량한 자존심 버린' 그가 이끈 현대차의 변화, 취임 후 시총 30조 '쑥'...위기에도 '질주..., 현대차그룹에 간부노조 생겼다, 자동차 소재가 새 옷으로 재탄생…현대차, '리스타일 2021 프로젝트'..., '8.8조원' 美 전기차 투자 준비한 현대차 "인프라법 통과에 달려", 현대車, 반도체 내재화 큰 꿈 "많은 투자·시간 걸려도 해낼 것", “반도체 확보가 곧 전기차 주도권”…현대차 ‘폭발적 수요’ 선제 대응, 현대차·기아·두산퓨얼셀 '수소연료전지 분산 발전' 시범운전 착수, '8.8조원' 美 전기차 투자 준비한 현대차 "인프라법 통과에 달려", 현대車, 반도체 내재화 큰 꿈 "많은 투자·시간 걸려도 해낼 것", “반도체 확보가 곧 전기차 주도권”…현대차 ‘폭발적 수요’ 선제 대응, '8.8조원' 美 전기차 투자 준비한 현대차 "인프라법 통과에 달려", 현대車, 반도체 내재화 큰 꿈 "많은 투자·시간 걸려도 해낼 것", “반도체 확보가 곧 전기차 주도권”…현대차 ‘폭발적 수요’ 선제 대응, 현대차 아이오닉5로 자켓·후드·바지를 만든다?, 車폐기물, 옷이 되다...현대차, 업사이클링 패션 공개, 현대차 북미사장 "반도체 자체 개발에 공들이고 있다", “현대차, 반도체 자체개발 원한다”, 현대차·기아·두산퓨얼셀 '수소연료전지 분산 발전' 시범운전 착수, 자동차 소재가 새 옷으로 재탄생…현대차, '리스타일 2021 프로젝트'..., '자동차주' 바닥찍었나...외인·기관도 사들인 현대차·기아, 전망은?, 취임 후 시총 30조 '쑥'...위기에도 '질주..., 현대차그룹에 간부노조 생겼다, 자동차 소재가 새 옷으로 재탄생…현대차, '리스타일 2021 프로젝트'..., '8.8조원' 美 전기차 투자 준비한 현대차 "인프라법 통과에 달려", 현대車, 반도체 내재화 큰 꿈 "많은 투자·시간 걸려도 해낼 것", “반도체 확보가 곧 전기차 주도권”…현대차 ‘폭발적 수요’ 선제 대응, 현대차 아이오닉5로 자켓·후드·바지를 만든다?, 車폐기물, 옷이 되다...현대차, 업사이클링 패션 공개, '알량한 자존심 버린' 그가 이끈 현대차의 변화, 현대차그룹에 간부노조 생겼다, 취임 후 시총 30조 '쑥'...위기에도 '질주..., '알량한 자존심 버린' 그가 이끈 현대차의 변화, 현대차 아이오닉5로 자켓·후드·바지를 만든다?, 車폐기물, 옷이 되다...현대차, 업사이클링 패션 공개, 현대차 북미사장 "반도체 자체 개발에 공들이고 있다", “현대차, 반도체 자체개발 원한다”, 현대차·기아·두산퓨얼셀 '수소연료전지 분산 발전' 시범운전 착수, '자동차주' 바닥찍었나...외인·기관도 사들인 현대차·기아, 전망은?, '알량한 자존심 버린' 그가 이끈 현대차의 변화, 취임 후 시총 30조 '쑥'...위기에도 '질주..., 현대차그룹에 간부노조 생겼다, 자동차 소재가 새 옷으로 재탄생…현대차, '리스타일 2021 프로젝트'..., '8.8조원' 美 전기차 투자 준비한 현대차 "인프라법 통과에 달려", 현대車, 반도체 내재화 큰 꿈 "많은 투자·시간 걸려도 해낼 것", “반도체 확보가 곧 전기차 주도권”…현대차 ‘폭발적 수요’ 선제 대응, 현대차 아이오닉5로 자켓·후드·바지를 만든다?, 車폐기물, 옷이 되다...현대차, 업사이클링 패션 공개, 현대차 북미사장 "반도체 자체 개발에 공들이고 있다", “현대차, 반도체 자체개발 원한다”, 현대차·기아·두산퓨얼셀 '수소연료전지 분산 발전' 시범운전 착수, '자동차주' 바닥찍었나...외인·기관도 사들인 현대차·기아, 전망은?, '자동차주' 바닥찍었나...외인·기관도 사들인 현대차·기아, 전망은?, 현대車, 반도체 내재화 큰 꿈 "많은 투자·시간 걸려도 해낼 것", '알량한 자존심 버린' 그가 이끈 현대차의 변화, 현대차그룹에 간부노조 생겼다, '알량한 자존심 버린' 그가 이끈 현대차의 변화, '자동차주' 바닥찍었나...외인·기관도 사들인 현대차·기아, 전망은?, 현대차·기아·두산퓨얼셀 '수소연료전지 분산 발전' 시범운전 착수, “현대차, 반도체 자체개발 원한다”, 현대차 북미사장 "반도체 자체 개발에 공들이고 있다", 車폐기물, 옷이 되다...현대차, 업사이클링 패션 공개, 현대차 아이오닉5로 자켓·후드·바지를 만든다?, “반도체 확보가 곧 전기차 주도권”…현대차 ‘폭발적 수요’ 선제 대응, 취임 후 시총 30조 '쑥'...위기에도 '질주..., 현대車, 반도체 내재화 큰 꿈 "많은 투자·시간 걸려도 해낼 것", 자동차 소재가 새 옷으로 재탄생…현대차, '리스타일 2021 프로젝트'..., 현대차그룹에 간부노조 생겼다, 취임 후 시총 30조 '쑥'...위기에도 '질주..., '알량한 자존심 버린' 그가 이끈 현대차의 변화, '자동차주' 바닥찍었나...외인·기관도 사들인 현대차·기아, 전망은?, 현대차·기아·두산퓨얼셀 '수소연료전지 분산 발전' 시범운전 착수, “현대차, 반도체 자체개발 원한다”, 현대차 북미사장 "반도체 자체 개발에 공들이고 있다", '8.8조원' 美 전기차 투자 준비한 현대차 "인프라법 통과에 달려", 車폐기물, 옷이 되다...현대차, 업사이클링 패션 공개, 현대차그룹에 간부노조 생겼다, '8.8조원' 美 전기차 투자 준비한 현대차 "인프라법 통과에 달려", 현대차 북미사장 "반도체 자체 개발에 공들이고 있다", 車폐기물, 옷이 되다...현대차, 업사이클링 패션 공개, 현대차 아이오닉5로 자켓·후드·바지를 만든다?, “반도체 확보가 곧 전기차 주도권”…현대차 ‘폭발적 수요’ 선제 대응, 현대</t>
   </si>
   <si>
-    <t>현대차-21년도 3분기 Preview, 3분기 영업이익 1.58조원, 컨센서스 하회 전망, 현대차·BNK證, ‘CERCG ABCP’ 1심 소송서 패소</t>
+    <t>21년도 3분기 Preview, 3분기 영업이익 1.58조원, 컨센서스 하회 전망, 현대차·BNK證, ‘CERCG ABCP’ 1심 소송서 패소</t>
   </si>
   <si>
     <t>삼성·현대차·SK가 탐내는 꿈의 기술 ‘무음극 배터리’, 1회 충전에 ..., 현대차가 짓는 자율주차타워 모습은?, 현대차 고성능 브랜드 N, 유럽서 ‘쾌속질주’, 현대차는 왜 반도체 자체 개발을 탐내나…오해와 진실, 현대차의 '반도체 자체 개발' 승부수…성공 '여기'에 달렸다 [박신영의..., 현대차가 짓는 자율주차타워 모습은?, 현대차의 '반도체 자체 개발' 승부수…성공 '여기'에 달렸다 [박신영의..., 현대차는 왜 반도체 자체 개발을 탐내나…오해와 진실, 현대차 고성능 브랜드 N, 유럽서 ‘쾌속질주’</t>
@@ -7330,10 +7330,10 @@
     <t>현대차그룹, 협력사 온라인 채용박람회 개최 "동반성장 모델 구축", 현대차그룹 내일부터 협력사 온라인 채용박람회 개최, 현대차그룹, 협력사 인재채용 지원 나선다…온라인 채용박람회, 美서 입증된 현대차·기아 '안전'..IIHS서 27개 차종 '최상위 ..., 유럽서 현대차·기아만 달렸다, 현대차그룹, 협력사 온라인 채용 박람회 개최, 현대차그룹, 협력사 채용박람회, 현대차 '넥쏘' 글로벌 2만대 돌파 수소 충전인프라 확산…판매 탄력, '현대차 타고 온 아저씨' 밥값 깎아줬는데…"그분 이었어요", 현대차, 美서 안전성 증명했다…IIHS 27개 차종 '최상위' 평가, 현대차 '넥쏘' 글로벌 2만대 돌파 수소 충전인프라 확산…판매 탄력, '현대차 타고 온 아저씨' 밥값 깎아줬는데…"그분 이었어요"</t>
   </si>
   <si>
-    <t>현대차, 최정상급 모터스포츠 3개 대회 석권…"전기차도 강세", 현대차가 꼽은 '전기차 대중화 조건 셋', 한화證 "현대차, 4분기엔 실적 회복할 것"...목표주가 유지, 하나은행, 현대·기아차 등과 커넥티드카 MOU, 하나은행, 현대·기아차&amp;핀다와 '커넥티드 카 기반 금융상품' MOU, 한화투자證, 中CERCG 관련 현대차證 소송서 승소, 하나은행·핀다·현대차·기아, '커넥티드 카' 금융 맞손, "주행거리로 우대금리" 하나銀-현대차·기아-핀다, 커넥티드카 금융상품 ..., 내연기관·전기차 동시에…현대차, 글로벌 모터스포츠 3개 대회 석권, "현대차는 안돼" 비웃더니 뻘쭘해졌네…정의선 '뚝심투자', 세계 최정상..., 현대차, 커넥티드카 운전자에 '우대금리', 현대차·기아 커넥티드카 운전자에 '우대금리', 현대차·기아, 핀다·하나銀과 커넥티드카 기반 금융상품 개발, 현대차·기아, 핀다·하나은행과 맞손, 美 배터리 사용·노조설립 압박···충족 못하면 보조금 ..., 내연기관부터 전기차까지 싹쓸이 현대차 모터스포츠 '트리플 크라운', 현대차, 모터스포츠 3개 대회 우승컵 싹쓸이, 현대차, 세계 최정상 모터스포츠 3개대회 동시 우승, 현대차, 세계 최정상급 모터스포츠 3개 대회 석권, 하나은행, 현대차·기아, 핀다와 '커넥티드 카 기반 금융상품 개발' ..., 기대와 우려 교차하는 현대차의 모빌리티 비즈니스, 내연기관도 전기차도…현대차, 모터스포츠 3개 대회 '석권', 하나은행·핀다·현대차·기아, '커넥티드 카' 금융 맞손, 현대차·기아, 핀다·하나銀과 커넥티드카 기반 금융상품 개발, 핀다·하나銀 손잡은 현대차·기아 커넥티드카 활용 금융상품 개발, 한화證 "현대차, 4분기엔 실적 회복할 것"...목표주가 유지, 현대차가 꼽은 '전기차 대중화 조건 셋', 자동차 역설적 투자 기회 왔다…기아 &gt; 현대차 &gt; 만도 ..., 현대차 타고 와 밥값 내준 아저씨…"정의선 인줄 몰랐다", "모빌리티 생태계 변화 대응"… 현대차·기아, 이종업계와 협력 확대, 하나은행, 현대차·기아, 핀다와 '커넥티드 카 기반 금융상품 개발' 협..., 핀다·하나銀 손잡은 현대차·기아 커넥티드카 활용 금융상품 개발, 현대차·기아, 핀다·하나銀 손잡고 커넥티드카 기반 금융상품 개발, 현대차, 세계 최정상급 모터스포츠 3개 대회 우승컵 '싹쓸이', 한화證 "현대차, 4분기엔 실적 회복할 것"...목표주가 유지, 현대차, 커넥티드카 운전자에 '우대금리', 현대차가 꼽은 '전기차 대중화 조건 셋', 자동차 역설적 투자 기회 왔다…기아 &gt; 현대차 &gt; 만도 ..., 현대차 타고 와 밥값 내준 아저씨…"정의선 인줄 몰랐다", 하나은행, 현대차와 '커넥티드 카 기반 금융상품 개발', 하나은행, 현대·기아차 등과 커넥티드카 MOU, 하나은행·핀다·현대차·기아, '커넥티드 카' 금융 맞손, 현대차-시그널로 확인한 하방 지지대, 21년도 3분기 매출 27.4조원, OP 1.6조원(OPM 5.9%), 2022년 매출 126.0조원, OP 8.1조원(OPM 6.4%), 투자의견 BUY(유지), 목표주가 28만원(하향), 기대와 우려 교차하는 현대차의 모빌리티 비즈니스, 내연기관부터 전기차까지 싹쓸이 현대차 모터스포츠 '트리플 크라운', "주행거리로 우대금리" 하나銀-현대차·기아-핀다, 커넥티드카 금융상품 ..., 현대차, 모터스포츠 3개 대회 우승컵 싹쓸이, 현대차·기아, 핀다·하나은행과 맞손, 현대차·기아, 핀다·하나銀과 커넥티드카 기반 금융상품 개발, 현대차-과속 방지턱 통과, 21년도 3분기 실적 Preview, 21년도 4분기 반도체 공급 차질 완화 기대, 실적과 모멘텀 개선이 기대되는 내년, 투자의견 Buy, 목표주가 300,000원 유지, 현대차, 모터스포츠 3개 대회 우승컵 싹쓸이, 美 배터리 사용·노조설립 압박···충족 못하면 보조금 ..., 美 배터리 사용·노조설립 압박···충족 못하면 보조금 ..., 현대차·기아, 핀다·하나은행과 맞손, 현대차·기아, 핀다·하나銀과 커넥티드카 기반 금융상품 개발, 현대차·기아 커넥티드카 운전자에 '우대금리', 현대차, 커넥티드카 운전자에 '우대금리', "현대차는 안돼" 비웃더니 뻘쭘해졌네…정의선 '뚝심투자', 세계 최정상..., 현대차, 세계 최정상급 모터스포츠 3개 대회 석권, 한화투자證, 中CERCG 관련 현대차證 소송서 승소, 내연기관부터 전기차까지 싹쓸이 현대차 모터스포츠 '트리플 크라운'</t>
-  </si>
-  <si>
-    <t>현대차·기아, 유럽 점유율 8.4% 사상 최고, 현대차·기아, 유럽시장서 대약진 "종주국 獨·英서 선전", 현대차·기아, 친환경차 유럽 질주…‘자동차 강국’ 獨·英 사로잡다, 현대차·기아, 친환경차 유럽 쾌속질주...‘자동차 강국’ 獨·英 사로잡..., “현대차, 정점(Peak) 아니라 바닥(Bottom)에서 벗어날 것”-..., 獨·英 홀렸다… 현대차·기아, 유럽 점유율 11% 첫 돌파, “현대차, 정점(Peak) 아니라 바닥(Bottom)에서 벗어날 것”-..., 전기차로 車본고장 獨·英 잡은 현대차·기아, 현대차·기아, 獨·英서 질주, 현대차·기아, 친환경차 유럽 쾌속질주...‘자동차 강국’ 獨·英 사로..., 獨·英 홀렸다… 현대차·기아, 유럽 점유율 11% 첫 돌파, 전기차로 車본고장 獨·英 잡은 현대차·기아, 현대차·기아, 獨·英서 질주, 현대차·기아, 친환경차 유럽 쾌속질주...‘자동차 강국’ 獨·英 사로..., 현대차, 현대캐피탈 지분 20% 인수계약 2개월 연장, 대유플러스, 현대기아차에 대유합금 LPI사업부 양수, 獨·英 홀렸다… 현대차·기아, 유럽 점유율 11% 첫 돌파, 전기차로 車본고장 獨·英 잡은 현대차·기아, 현대차·기아, 獨·英서 질주, 현대차·기아, 친환경차 유럽 쾌속질주...‘자동차 강국’ 獨·英 사로..., 현대차, 현대캐피탈 지분 20% 인수계약 2개월 연장, 대유플러스, 현대기아차에 대유합금 LPI사업부 양수, 현대차, 차량용 반도체 부족에 3Q 실적 우려-유진, 현대차, 현대캐피탈 지분 20% 인수계약 2개월 연장, 현대차, 차량용 반도체 부족에 3Q 실적 우려-유진, 현대차-년도년도 2분기 3분기 프리뷰 - 반도체 부족으로 기대 하회할 것, 투자의견 Buy, 목표주가 300,000원 유지, 년도년도 2분기 3분기 영업이익 1.6조원 (흑전 전년 대비 증감율)으로 시장 컨센서스 4.1% 하회할 것, 2022년에는 금융부문 이익 줄어들면서 영업이익이 전년대비 3.0% 줄어들 것, 현대차-Peak Out에서 Bottom Out으로, 21년도 3분기 실적은 기대치 하회, Peak Out에서 Bottom Out으로, 기대되는 2022년 신차/EV 모멘텀</t>
+    <t>현대차, 최정상급 모터스포츠 3개 대회 석권…"전기차도 강세", 현대차가 꼽은 '전기차 대중화 조건 셋', 한화證 "현대차, 4분기엔 실적 회복할 것"...목표주가 유지, 하나은행, 현대·기아차 등과 커넥티드카 MOU, 하나은행, 현대·기아차&amp;핀다와 '커넥티드 카 기반 금융상품' MOU, 한화투자證, 中CERCG 관련 현대차證 소송서 승소, 하나은행·핀다·현대차·기아, '커넥티드 카' 금융 맞손, "주행거리로 우대금리" 하나銀-현대차·기아-핀다, 커넥티드카 금융상품 ..., 내연기관·전기차 동시에…현대차, 글로벌 모터스포츠 3개 대회 석권, "현대차는 안돼" 비웃더니 뻘쭘해졌네…정의선 '뚝심투자', 세계 최정상..., 현대차, 커넥티드카 운전자에 '우대금리', 현대차·기아 커넥티드카 운전자에 '우대금리', 현대차·기아, 핀다·하나銀과 커넥티드카 기반 금융상품 개발, 현대차·기아, 핀다·하나은행과 맞손, 美 배터리 사용·노조설립 압박···충족 못하면 보조금 ..., 내연기관부터 전기차까지 싹쓸이 현대차 모터스포츠 '트리플 크라운', 현대차, 모터스포츠 3개 대회 우승컵 싹쓸이, 현대차, 세계 최정상 모터스포츠 3개대회 동시 우승, 현대차, 세계 최정상급 모터스포츠 3개 대회 석권, 하나은행, 현대차·기아, 핀다와 '커넥티드 카 기반 금융상품 개발' ..., 기대와 우려 교차하는 현대차의 모빌리티 비즈니스, 내연기관도 전기차도…현대차, 모터스포츠 3개 대회 '석권', 하나은행·핀다·현대차·기아, '커넥티드 카' 금융 맞손, 현대차·기아, 핀다·하나銀과 커넥티드카 기반 금융상품 개발, 핀다·하나銀 손잡은 현대차·기아 커넥티드카 활용 금융상품 개발, 한화證 "현대차, 4분기엔 실적 회복할 것"...목표주가 유지, 현대차가 꼽은 '전기차 대중화 조건 셋', 자동차 역설적 투자 기회 왔다…기아 &gt; 현대차 &gt; 만도 ..., 현대차 타고 와 밥값 내준 아저씨…"정의선 인줄 몰랐다", "모빌리티 생태계 변화 대응"… 현대차·기아, 이종업계와 협력 확대, 하나은행, 현대차·기아, 핀다와 '커넥티드 카 기반 금융상품 개발' 협..., 핀다·하나銀 손잡은 현대차·기아 커넥티드카 활용 금융상품 개발, 현대차·기아, 핀다·하나銀 손잡고 커넥티드카 기반 금융상품 개발, 현대차, 세계 최정상급 모터스포츠 3개 대회 우승컵 '싹쓸이', 한화證 "현대차, 4분기엔 실적 회복할 것"...목표주가 유지, 현대차, 커넥티드카 운전자에 '우대금리', 현대차가 꼽은 '전기차 대중화 조건 셋', 자동차 역설적 투자 기회 왔다…기아 &gt; 현대차 &gt; 만도 ..., 현대차 타고 와 밥값 내준 아저씨…"정의선 인줄 몰랐다", 하나은행, 현대차와 '커넥티드 카 기반 금융상품 개발', 하나은행, 현대·기아차 등과 커넥티드카 MOU, 하나은행·핀다·현대차·기아, '커넥티드 카' 금융 맞손, 시그널로 확인한 하방 지지대, 21년도 3분기 매출 27.4조원, OP 1.6조원(OPM 5.9%), 2022년 매출 126.0조원, OP 8.1조원(OPM 6.4%), 투자의견 BUY(유지), 목표주가 28만원(하향), 기대와 우려 교차하는 현대차의 모빌리티 비즈니스, 내연기관부터 전기차까지 싹쓸이 현대차 모터스포츠 '트리플 크라운', "주행거리로 우대금리" 하나銀-현대차·기아-핀다, 커넥티드카 금융상품 ..., 현대차, 모터스포츠 3개 대회 우승컵 싹쓸이, 현대차·기아, 핀다·하나은행과 맞손, 현대차·기아, 핀다·하나銀과 커넥티드카 기반 금융상품 개발, 과속 방지턱 통과, 21년도 3분기 실적 Preview, 21년도 4분기 반도체 공급 차질 완화 기대, 실적과 모멘텀 개선이 기대되는 내년, 투자의견 Buy, 목표주가 300,000원 유지, 현대차, 모터스포츠 3개 대회 우승컵 싹쓸이, 美 배터리 사용·노조설립 압박···충족 못하면 보조금 ..., 美 배터리 사용·노조설립 압박···충족 못하면 보조금 ..., 현대차·기아, 핀다·하나은행과 맞손, 현대차·기아, 핀다·하나銀과 커넥티드카 기반 금융상품 개발, 현대차·기아 커넥티드카 운전자에 '우대금리', 현대차, 커넥티드카 운전자에 '우대금리', "현대차는 안돼" 비웃더니 뻘쭘해졌네…정의선 '뚝심투자', 세계 최정상..., 현대차, 세계 최정상급 모터스포츠 3개 대회 석권, 한화투자證, 中CERCG 관련 현대차證 소송서 승소, 내연기관부터 전기차까지 싹쓸이 현대차 모터스포츠 '트리플 크라운'</t>
+  </si>
+  <si>
+    <t>현대차·기아, 유럽 점유율 8.4% 사상 최고, 현대차·기아, 유럽시장서 대약진 "종주국 獨·英서 선전", 현대차·기아, 친환경차 유럽 질주…‘자동차 강국’ 獨·英 사로잡다, 현대차·기아, 친환경차 유럽 쾌속질주...‘자동차 강국’ 獨·英 사로잡..., “현대차, 정점(Peak) 아니라 바닥(Bottom)에서 벗어날 것”-..., 獨·英 홀렸다… 현대차·기아, 유럽 점유율 11% 첫 돌파, “현대차, 정점(Peak) 아니라 바닥(Bottom)에서 벗어날 것”-..., 전기차로 車본고장 獨·英 잡은 현대차·기아, 현대차·기아, 獨·英서 질주, 현대차·기아, 친환경차 유럽 쾌속질주...‘자동차 강국’ 獨·英 사로..., 獨·英 홀렸다… 현대차·기아, 유럽 점유율 11% 첫 돌파, 전기차로 車본고장 獨·英 잡은 현대차·기아, 현대차·기아, 獨·英서 질주, 현대차·기아, 친환경차 유럽 쾌속질주...‘자동차 강국’ 獨·英 사로..., 현대차, 현대캐피탈 지분 20% 인수계약 2개월 연장, 대유플러스, 현대기아차에 대유합금 LPI사업부 양수, 獨·英 홀렸다… 현대차·기아, 유럽 점유율 11% 첫 돌파, 전기차로 車본고장 獨·英 잡은 현대차·기아, 현대차·기아, 獨·英서 질주, 현대차·기아, 친환경차 유럽 쾌속질주...‘자동차 강국’ 獨·英 사로..., 현대차, 현대캐피탈 지분 20% 인수계약 2개월 연장, 대유플러스, 현대기아차에 대유합금 LPI사업부 양수, 현대차, 차량용 반도체 부족에 3Q 실적 우려-유진, 현대차, 현대캐피탈 지분 20% 인수계약 2개월 연장, 현대차, 차량용 반도체 부족에 3Q 실적 우려-유진, 년도년도 2분기 3분기 프리뷰 - 반도체 부족으로 기대 하회할 것, 투자의견 Buy, 목표주가 300,000원 유지, 년도년도 2분기 3분기 영업이익 1.6조원 (흑전 전년 대비 증감율)으로 시장 컨센서스 4.1% 하회할 것, 2022년에는 금융부문 이익 줄어들면서 영업이익이 전년대비 3.0% 줄어들 것, Peak Out에서 Bottom Out으로, 21년도 3분기 실적은 기대치 하회, Peak Out에서 Bottom Out으로, 기대되는 2022년 신차/EV 모멘텀</t>
   </si>
   <si>
     <t>현대차, BTS와 탄소중립 캠페인, 현대차, 방탄소년단과 '탄소중립' 디지털 참여형 캠페인, "탄소중립, MZ세대가 알리자"…현대차, 방탄소년단과 디지털 캠페인, 현대차, BTS와 탄소중립 캠페인, "탄소중립, MZ세대가 알리자"…현대차, 방탄소년단과 디지털 캠페인, 현대차, 방탄소년단과 '탄소중립' 디지털 참여형 캠페인, "탄소중립, MZ세대가 알리자"…현대차, 방탄소년단과 디지털 캠페인, 현대차, BTS와 함께 ‘탄소중립’ 디지털 참여형 캠페인 연다, 현대차, 방탄소년단과 '탄소중립' 디지털 참여형 캠페인, “현대차, UAM 플랫폼 만든다…2028년 택시·화물용 기체 공개”, 현대차, BTS 손잡고 ‘탄소중립’ 참여형 캠페인, “현대차, UAM 플랫폼 만든다…2028년 택시·화물용 기체 공개”, 현대차, BTS 손잡고 ‘탄소중립’ 참여형 캠페인</t>
@@ -7354,10 +7354,10 @@
     <t>현대차, 전국 초등·특수학교 통학 환경 개선 'H-스쿨케어', 현대차, 어린이 통학환경 개선 위한 ‘H-스쿨케어 캠페인’ 실시, 현대차, 어린이 통학환경 개선 위한 ‘H-스쿨케어 캠페인’ 실시, 현대차, 어린이 통학환경 개선 ‘H-스쿨케어 캠페인’ 실시, 현대차, 2년연속 대한민국명장·우수숙련기술자 배출, 덕양산업, 현대자동차 신차 3종 품질 무결점 우수 협력사 선정, 덕양산업, 현대자동차 신차 3차종 연속 품질 무결점 달성 우수 협력사 ..., 현대차, 특수학교 학생들 위해 'H-스쿨케어' 캠페인 실시, 현대차, 어린이 통학버스 무상 안전케어, 현대차, 특수학교 학생들 위해 'H-스쿨케어' 캠페인 실시, 현대차, 어린이 통학버스 무상 안전케어, 현대차, 내년부터 印尼서 전기차 생산…"EV 생태계 구축", 현대차 노조, 이번엔 ‘람다 엔진’ 두고 갈등, 현대百 “흰디 하트 에디션 사고 함께 유기견 도와요”</t>
   </si>
   <si>
-    <t>결국 발목잡은 반도체..현대차 3분기 판매 9.9% 감소, 현대차 3분기 영업이익 1조6067억원…전년동기 대비 흑자전환, 현대차 3분기 영업이익 1조6067억원…반도체·환율난에도 선방, 현대차, 3분기 영업익 1조6067억…'품질비용' 기저효과 흑자, '車 반도체 쇼티지' 주춤 현대차, 3분기 영업익 1조6067억, 현대차, 3분기 영업익 1조6067억…'품질비용' 기저효과 흑자, 현대차 3분기 영업이익 1조6067억원…전년동기 대비 흑자전환, 현대차 3분기 영업이익 1조6067억원…반도체·환율난에도 선방, 현대차, 3분기 영업익 1조6067억…흑자전환, "올 연말 제네시스 신형 G90 출시 예정"-현대차 컨콜, "제네시스·SUV 덕에 살았다"…적게 팔았다던 현대차에 벌어진 일, 고급·전기차 집중한 현대차…적게 팔아도 영업이익 선방, 현대차 "3분기 글로벌 EV 누적 9만9400대 판매", 반도체 대란에 車판매 줄었지만…현대차, 3Q 영업익 1.6조 흑자전환, 현대차 "반도체 수급난 4분기 일부 개선…영향은 내년까지", "제네시스, 2030년 전기수소차 8종 출시…연간 40만대 목표"-현대..., 현대차 "올해 연말 제네시스 신형 G90출시 예정", "올 연말 제네시스 신형 G90 출시 예정"-현대차 컨콜, 현대차 "3분기 글로벌 전기차 판매 9만9400대", 현대차, 3분기 영업익 1조6067억…흑자전환, 현대차, 3분기 영업익 1조6,6067억원 ‘흑자 전환’···연간 판매..., "4분기 '車 반도체 공급 차질 탓'…3분기보다는 다소 숨통"-현대차 ..., "3분기 글로벌 EV 9만9400대 판매…아이오닉5 유럽서 3만대 돌..., 현대차 3분기 영업익 1.6조…반도체 위기 속 선방(종합), 현대자동차 3분기 영업이익 1조6067억원…판매 믹스 개선으로 흑자 ..., "반도체 공급난 여파 계속"…현대차, 3분기 실적 '주춤', 현대차, 3분기 영업이익 1조6067억원…흑자 전환, 현대차 "3분기 글로벌 EV 누적 9만9400대 판매", 3분기 실적 발표한 현대차, 주가는 소폭 상승, 10대 중 9대가 일본車인 나라…현대차, 전기차로 뚫는다, '반도체 공급난'에 판매 주춤한 현대차…3분기 영업익 1조6067억원 ..., "반도체 공급난 여파 계속"…현대차, 3분기 실적 '주춤', 현대차 "2023년까지 전기차 배터리 모두 확보…올 전기차판매 10만대..., 현대차, 반도체에 발목…내년 수급도 불안, 결국 발목잡은 반도체..현대차 3분기 판매 9.9% 감소, 반도체 대란에도...현대車 영업익 1.6조 '선방', 현대차 "신형 제네시스 G90, 연말 출시 예정", 현대차 "4분기도 반도체 수급난…수익성 방어에 최선", '동남아發, 반도체 공급 차질 탓'…현대차, 3분기 실적 주춤(종합), "車반도체 쇼티지 탓"…현대차 3분기 실적 '주춤', 반도체가 가른 3Q 실적 희비…현대차 `주춤` SK하이닉스 `방긋`, '동남아發, 반도체 공급 차질 탓'…현대차, 3분기 실적 주춤(종합), "車반도체 쇼티지 탓"…현대차 3분기 실적 '주춤', "반도체 공급 숨통트인다"…현대차, 투싼 등 車생산 박차, 반도체가 가른 3Q 실적 희비…현대차 `주춤` SK하이닉스 `방긋`, 현대차, 3분기 영업익 1조 6066억…흑자전환, 현대차, 3분기 영업이익 1조6067억원…전년比 흑자 전환, 현대차, 3분기 글로벌 판매 89만8906대…전년比 9.9%↓, 현대차-년도년도 2분기 3분기 리뷰 - 예상보다 좋았던 수익성은 향후 이익 전망에 긍정적, 년도년도 2분기 3분기 현대차 영업이익은 시장 기대에 부합. 향후 손익 전망에 긍정적으로 작용할 것, 판매부족에도 불구하고 양호한 마진으로 선방. 반도체 상황 및 환율효과는 향후 긍정적으로 바뀔 것, 생산 위축에도 불구하고 유리한 판매 환경을 감안한 연간 목표 조정, 현대차, 3분기 매출액 28조8672억…전년比 4.7%↑, 현대차-우호적 수요 환경 지속, 최근 낮아진 기대치 수준의 실적: 판매 감소 VS 믹스 개선, 단기 실적은 반도체 수급에 좌우될 전망이나 구조적인 문제는 아니라고 판단, 22년까지 우호적 수요 환경 지속 전망, 현대차-조용한 실적 · 아직은 조용한 비전, 21년도 3분기 , 반도체 부족 영향으로 외형 성장 둔화, 점진적 반도체 공급 회복 의미하는 2021년 판매 가이던스 제시, 2022년 초로 예상되는 미래 모빌리티 비전 공개에 주목, 현대차·기아, 기술, 인력 공유에 특허권 이전까지…R&amp;D 상생은 이렇게, "車반도체 쇼티지 탓"…현대차 3분기 실적 '주춤', 현대차 싼타크루즈, 픽업트럭 본고장 美서도 통했다, 현대차, 3분기 영업이익 1조6067억원…흑자 전환, 현대차, 3분기 매출액 28조8672억원…전년比 4.7%↑, 현대차, 3분기 영업이익 1조6067억원…흑자 전환, 현대모비스 자사주 취득 완료...현대차 지배구조 개편 절차 돌입, 현대차 싼타크루즈, 픽업트럭 본고장 美서도 ‘엄지척’, "삼성 갤럭시가 애플 아이폰 잡았듯, 현대차도 테슬라 잡을 것"</t>
-  </si>
-  <si>
-    <t>차량 반도체 기술 확보나선 현대차…獨 인피니언과 스타트업 공동 투자, 현대차, 일자리 사업 '굿잡 5060'으로 368명 재취업, 현대차, 신중년 일자리 창출 사업 ‘굿잡 5060’ 2021 성과 공유..., 현대차그룹 아이오닉5·EV6, '2022 독일 올해의 차' 부문별 1위, 현대차 투싼PHEV, 獨 3대 자동차 전문지 비교평가서 ‘종합 1위’, 현대차그룹 아이오닉5·EV6, '2022 독일 올해의 차' 부문별 1위, 현대차 투싼PHEV, 獨 3대 자동차 전문지 비교평가서 ‘종합 1위’, 현대차 '투싼 PHEV' 성능 유럽차 제치고 1위, 현대차 디지털 모터스포츠 대회 '현대 N e-페스티벌' 개최, 현대차그룹 '굿잡 5060', 신중년 368명 재취업 지원…취업률 6..., 현대차證, 기업지배구조원 ESG 평가서 2년 연속 ‘A’, 현대차 투싼 PHEV, 獨 3대 자동차 전문지 비교평가서 종합 1위, 독일 3대 車전문지 평가 1위 휩쓴 '현대차 투싼 PHEV' 원동력은..., 현대차, 억눌린 수요에도 3분기 실적 기대치 부합-신한금투, 현대차, 차화정 시대 이후 최대 실적 호황기 진입할 것-NH, 현대차 '투싼 PHEV' 성능 유럽차 제치고 1위, 현대차, 일자리 사업 '굿잡 5060'으로 368명 재취업, 현대차, 디지털 모터스포츠 '현대 N e-페스티벌' 개최, 현대차, 일자리 사업 '굿잡 5060'으로 368명 재취업, "현대차, 2022년 실적 최대 호황기 진입할 것"-NH투자증권, "가상트랙 질주 짜릿할까"..현대차 온라인 車경주대회 개최, 현대차 투싼 PHEV, 獨 3대 자동차 전문지 비교평가서 1위 달성, 온라인서 자웅 겨룬다…현대차, 디지털 모터스포츠 '현대 N e-페스티벌..., 현대차 투싼 PHEV, 독일 3대 자동차 매체 평가서 모두 1위, 현대두산인프라, 원자재 급등에 채굴 수요 ↑…명가재건 날갯짓, 현대케피코, 전기이륜차 구동시스템으로 인도네시아 시장 공략, 현대케피코, 전기이륜차 구동시스템으로 '인니' 공략 나선다, 현대케피코, 전기이륜차 구동시스템으로 인도네시아 시장 공략, 현대차, 신중년 일자리 창출 사업 ‘굿잡 5060’ 2021 성과 공유..., 현대케피코, 전기이륜차 구동시스템으로 '인니' 공략 나선다, '아반떼 N' 타고 온라인 경주…'현대 N e-페스티벌' 열린다, 현대차 투싼 PHEV, 독일 3대 자동차 매체 평가서 모두 1위, 현대차 투싼PHEV, 獨 3대 자동차 전문지 비교평가서 ‘종합 1위’, 주춤한 현대차 "4Q 반도체 수급 다소 풀릴 것", 현대百 7社 ESG A등급, “현대차 유리천장도 금 갔다”…2년간 3배 늘어난 현대차 여성임원, 현대차, 디지털 모터스포츠 대회 ‘N e-페스티벌’ 개최, 각자 브랜드 유지하는 '중흥-대우', '현대-기아차'처럼 성공할까, 차량 반도체 기술 확보나선 현대차…獨 인피니언과 스타트업 공동 투자, "가상트랙 질주 짜릿할까"..현대차 온라인 車경주대회 개최, 현대차, 디지털 모터스포츠 축제 '현대 N e-페스티벌' 개최, 현대차-점차 중요해지는 생산정상화, 점차 중요해지는 생산정상화, 현대차, 억눌린 수요에도 3분기 실적 기대치 부합-신한금투, 현대차-단단해진 바닥, 21년도 3분기 영업이익은 1.61조원(흑전 전년 대비 증감율, OPM 5.6%) 기록, 글로벌 부품사의 공급망 문제와 물류 불안은 지속되나 델타변이 확산으로 급작스러운 반도체 공급 위축은 점진 개선 기대, 견조한 수요에 편승한 가격/믹스 중심의 이익 개선 전략은 타이트한 공급 상황에서 지지될 전망, 독일 3대 車전문지 평가 1위 휩쓴 '현대차 투싼 PHEV' 원동력은?, 현대차- 예상대로, 년도년도 2분기 3분기 Review: 시장 기대치 부합, 투자의견 ＇Buy＇, 목표주가 300.000원 유지, 현대차-볼륨 사이클의 시작, 생산 안정성 개선에 따른 선순환 구조 진입, 3분기 Review: 제품믹스 개선 긍정적, 현대차-년도년도 2분기 3분기 Review: 우려 대비 선방한 실적과 가이던스 상향, 년도년도 2분기 3분기 Review: 우려 대비 선방한 실적, 자동차 부문 영업이익 가이던스 상향 조정, 4 분기 실적 개선 기대갑 Up, 현대차-결국 관건은 반도체 확보와 생산 정상화, 21년도 3분기 연결 매출 29조원(전년 대비 증감율+4.7%), 영업이익 1.6조원(전년 대비 증감율흑전), OPM 5.6%, 특근 계획은 기 수립, 결국 11월 실행 여부 및 생산 정상화가 단기 주가 변수, 현대차-좋아질 일만 남았다, 영업이익은 추정치와 컨센서스에 부합, 가이던스 상향으로 4분기 실적 자신감 표명, 현대차-년도년도 2분기 3분기 Review: 가까워진 불확실성 해소 시기, 년도년도 2분기 3분기 (P): 매출액 28조 8,672억원, 영업이익 1조 6,067억원, 수정된 가이던스에 따라 년도년도 2분기 4분기 실적 가시성은 높아져, 2022년, 판매대수 회복이 실적 개선 견인 전망, 현대차-반도체 없어도 이 실적, 21년도 3분기 영업이익 1.61조원(흑자전환)으로 기대치 부합, 억눌린 수요를 안고 가는 길, 목표주가 27만원, 투자의견 매수 유지, 현대차-볼륨 사이클의 시작, 생산 안정성 개선에 따른 선순환 구조 진입, 3분기 Review: 제품믹스 개선 긍정적, 현대차-년도년도 2분기 3분기 Review: 우려 대비 선방한 실적과 가이던스 상향, 년도년도 2분기 3분기 Review: 우려 대비 선방한 실적, 자동차 부문 영업이익 가이던스 상향 조정, 4 분기 실적 개선 기대갑 Up, 현대차-좋아질 일만 남았다, 영업이익은 추정치와 컨센서스에 부합, 가이던스 상향으로 4분기 실적 자신감 표명, 현대차 투싼 PHEV, 獨 3대 자동차 전문지 비교평가서 1위 달성, MZ세대가 뽑은 톱 브랜드 15…‘GS25’·‘현대차’·‘KB국민카드’..., 현대차, 4Q 반도체 수급 개선…하반기 호실적 전망 -한국, 현대차, 영업실적 바닥 다진 3분기…믹스 개선으로 방어 -하이, “현대차, PER 6.9배 불과…점진적 가동률 정상화 전망”, 현대케피코, 전기이륜차 구동시스템으로 인도네시아 시장 공략, "현대차, 2022년 실적 최대 호황기 진입할 것"-NH투자증권, 현대차, 차화정 시대 이후 최대 실적 호황기 진입할 것-NH, 현대차-결국 관건은 반도체 확보와 생산 정상화, 21년도 3분기 연결 매출 29조원(전년 대비 증감율+4.7%), 영업이익 1.6조원(전년 대비 증감율흑전), OPM 5.6%, 특근 계획은 기 수립, 결국 11월 실행 여부 및 생산 정상화가 단기 주가 변수, 현대차, 3분기 부진 주가 선반영…바닥통과 관점 접근</t>
+    <t>결국 발목잡은 반도체..현대차 3분기 판매 9.9% 감소, 현대차 3분기 영업이익 1조6067억원…전년동기 대비 흑자전환, 현대차 3분기 영업이익 1조6067억원…반도체·환율난에도 선방, 현대차, 3분기 영업익 1조6067억…'품질비용' 기저효과 흑자, '車 반도체 쇼티지' 주춤 현대차, 3분기 영업익 1조6067억, 현대차, 3분기 영업익 1조6067억…'품질비용' 기저효과 흑자, 현대차 3분기 영업이익 1조6067억원…전년동기 대비 흑자전환, 현대차 3분기 영업이익 1조6067억원…반도체·환율난에도 선방, 현대차, 3분기 영업익 1조6067억…흑자전환, "올 연말 제네시스 신형 G90 출시 예정"-현대차 컨콜, "제네시스·SUV 덕에 살았다"…적게 팔았다던 현대차에 벌어진 일, 고급·전기차 집중한 현대차…적게 팔아도 영업이익 선방, 현대차 "3분기 글로벌 EV 누적 9만9400대 판매", 반도체 대란에 車판매 줄었지만…현대차, 3Q 영업익 1.6조 흑자전환, 현대차 "반도체 수급난 4분기 일부 개선…영향은 내년까지", "제네시스, 2030년 전기수소차 8종 출시…연간 40만대 목표"-현대..., 현대차 "올해 연말 제네시스 신형 G90출시 예정", "올 연말 제네시스 신형 G90 출시 예정"-현대차 컨콜, 현대차 "3분기 글로벌 전기차 판매 9만9400대", 현대차, 3분기 영업익 1조6067억…흑자전환, 현대차, 3분기 영업익 1조6,6067억원 ‘흑자 전환’···연간 판매..., "4분기 '車 반도체 공급 차질 탓'…3분기보다는 다소 숨통"-현대차 ..., "3분기 글로벌 EV 9만9400대 판매…아이오닉5 유럽서 3만대 돌..., 현대차 3분기 영업익 1.6조…반도체 위기 속 선방(종합), 현대자동차 3분기 영업이익 1조6067억원…판매 믹스 개선으로 흑자 ..., "반도체 공급난 여파 계속"…현대차, 3분기 실적 '주춤', 현대차, 3분기 영업이익 1조6067억원…흑자 전환, 현대차 "3분기 글로벌 EV 누적 9만9400대 판매", 3분기 실적 발표한 현대차, 주가는 소폭 상승, 10대 중 9대가 일본車인 나라…현대차, 전기차로 뚫는다, '반도체 공급난'에 판매 주춤한 현대차…3분기 영업익 1조6067억원 ..., "반도체 공급난 여파 계속"…현대차, 3분기 실적 '주춤', 현대차 "2023년까지 전기차 배터리 모두 확보…올 전기차판매 10만대..., 현대차, 반도체에 발목…내년 수급도 불안, 결국 발목잡은 반도체..현대차 3분기 판매 9.9% 감소, 반도체 대란에도...현대車 영업익 1.6조 '선방', 현대차 "신형 제네시스 G90, 연말 출시 예정", 현대차 "4분기도 반도체 수급난…수익성 방어에 최선", '동남아發, 반도체 공급 차질 탓'…현대차, 3분기 실적 주춤(종합), "車반도체 쇼티지 탓"…현대차 3분기 실적 '주춤', 반도체가 가른 3Q 실적 희비…현대차 `주춤` SK하이닉스 `방긋`, '동남아發, 반도체 공급 차질 탓'…현대차, 3분기 실적 주춤(종합), "車반도체 쇼티지 탓"…현대차 3분기 실적 '주춤', "반도체 공급 숨통트인다"…현대차, 투싼 등 車생산 박차, 반도체가 가른 3Q 실적 희비…현대차 `주춤` SK하이닉스 `방긋`, 현대차, 3분기 영업익 1조 6066억…흑자전환, 현대차, 3분기 영업이익 1조6067억원…전년比 흑자 전환, 현대차, 3분기 글로벌 판매 89만8906대…전년比 9.9%↓, 년도년도 2분기 3분기 리뷰 - 예상보다 좋았던 수익성은 향후 이익 전망에 긍정적, 년도년도 2분기 3분기 현대차 영업이익은 시장 기대에 부합. 향후 손익 전망에 긍정적으로 작용할 것, 판매부족에도 불구하고 양호한 마진으로 선방. 반도체 상황 및 환율효과는 향후 긍정적으로 바뀔 것, 생산 위축에도 불구하고 유리한 판매 환경을 감안한 연간 목표 조정, 현대차, 3분기 매출액 28조8672억…전년比 4.7%↑, 우호적 수요 환경 지속, 최근 낮아진 기대치 수준의 실적: 판매 감소 VS 믹스 개선, 단기 실적은 반도체 수급에 좌우될 전망이나 구조적인 문제는 아니라고 판단, 22년까지 우호적 수요 환경 지속 전망, 조용한 실적 · 아직은 조용한 비전, 21년도 3분기 , 반도체 부족 영향으로 외형 성장 둔화, 점진적 반도체 공급 회복 의미하는 2021년 판매 가이던스 제시, 2022년 초로 예상되는 미래 모빌리티 비전 공개에 주목, 현대차·기아, 기술, 인력 공유에 특허권 이전까지…R&amp;D 상생은 이렇게, "車반도체 쇼티지 탓"…현대차 3분기 실적 '주춤', 현대차 싼타크루즈, 픽업트럭 본고장 美서도 통했다, 현대차, 3분기 영업이익 1조6067억원…흑자 전환, 현대차, 3분기 매출액 28조8672억원…전년比 4.7%↑, 현대차, 3분기 영업이익 1조6067억원…흑자 전환, 현대모비스 자사주 취득 완료...현대차 지배구조 개편 절차 돌입, 현대차 싼타크루즈, 픽업트럭 본고장 美서도 ‘엄지척’, "삼성 갤럭시가 애플 아이폰 잡았듯, 현대차도 테슬라 잡을 것"</t>
+  </si>
+  <si>
+    <t>차량 반도체 기술 확보나선 현대차…獨 인피니언과 스타트업 공동 투자, 현대차, 일자리 사업 '굿잡 5060'으로 368명 재취업, 현대차, 신중년 일자리 창출 사업 ‘굿잡 5060’ 2021 성과 공유..., 현대차그룹 아이오닉5·EV6, '2022 독일 올해의 차' 부문별 1위, 현대차 투싼PHEV, 獨 3대 자동차 전문지 비교평가서 ‘종합 1위’, 현대차그룹 아이오닉5·EV6, '2022 독일 올해의 차' 부문별 1위, 현대차 투싼PHEV, 獨 3대 자동차 전문지 비교평가서 ‘종합 1위’, 현대차 '투싼 PHEV' 성능 유럽차 제치고 1위, 현대차 디지털 모터스포츠 대회 '현대 N e-페스티벌' 개최, 현대차그룹 '굿잡 5060', 신중년 368명 재취업 지원…취업률 6..., 현대차證, 기업지배구조원 ESG 평가서 2년 연속 ‘A’, 현대차 투싼 PHEV, 獨 3대 자동차 전문지 비교평가서 종합 1위, 독일 3대 車전문지 평가 1위 휩쓴 '현대차 투싼 PHEV' 원동력은..., 현대차, 억눌린 수요에도 3분기 실적 기대치 부합-신한금투, 현대차, 차화정 시대 이후 최대 실적 호황기 진입할 것-NH, 현대차 '투싼 PHEV' 성능 유럽차 제치고 1위, 현대차, 일자리 사업 '굿잡 5060'으로 368명 재취업, 현대차, 디지털 모터스포츠 '현대 N e-페스티벌' 개최, 현대차, 일자리 사업 '굿잡 5060'으로 368명 재취업, "현대차, 2022년 실적 최대 호황기 진입할 것"-NH투자증권, "가상트랙 질주 짜릿할까"..현대차 온라인 車경주대회 개최, 현대차 투싼 PHEV, 獨 3대 자동차 전문지 비교평가서 1위 달성, 온라인서 자웅 겨룬다…현대차, 디지털 모터스포츠 '현대 N e-페스티벌..., 현대차 투싼 PHEV, 독일 3대 자동차 매체 평가서 모두 1위, 현대두산인프라, 원자재 급등에 채굴 수요 ↑…명가재건 날갯짓, 현대케피코, 전기이륜차 구동시스템으로 인도네시아 시장 공략, 현대케피코, 전기이륜차 구동시스템으로 '인니' 공략 나선다, 현대케피코, 전기이륜차 구동시스템으로 인도네시아 시장 공략, 현대차, 신중년 일자리 창출 사업 ‘굿잡 5060’ 2021 성과 공유..., 현대케피코, 전기이륜차 구동시스템으로 '인니' 공략 나선다, '아반떼 N' 타고 온라인 경주…'현대 N e-페스티벌' 열린다, 현대차 투싼 PHEV, 독일 3대 자동차 매체 평가서 모두 1위, 현대차 투싼PHEV, 獨 3대 자동차 전문지 비교평가서 ‘종합 1위’, 주춤한 현대차 "4Q 반도체 수급 다소 풀릴 것", 현대百 7社 ESG A등급, “현대차 유리천장도 금 갔다”…2년간 3배 늘어난 현대차 여성임원, 현대차, 디지털 모터스포츠 대회 ‘N e-페스티벌’ 개최, 각자 브랜드 유지하는 '중흥-대우', '현대-기아차'처럼 성공할까, 차량 반도체 기술 확보나선 현대차…獨 인피니언과 스타트업 공동 투자, "가상트랙 질주 짜릿할까"..현대차 온라인 車경주대회 개최, 현대차, 디지털 모터스포츠 축제 '현대 N e-페스티벌' 개최, 점차 중요해지는 생산정상화, 점차 중요해지는 생산정상화, 현대차, 억눌린 수요에도 3분기 실적 기대치 부합-신한금투, 단단해진 바닥, 21년도 3분기 영업이익은 1.61조원(흑전 전년 대비 증감율, OPM 5.6%) 기록, 글로벌 부품사의 공급망 문제와 물류 불안은 지속되나 델타변이 확산으로 급작스러운 반도체 공급 위축은 점진 개선 기대, 견조한 수요에 편승한 가격/믹스 중심의 이익 개선 전략은 타이트한 공급 상황에서 지지될 전망, 독일 3대 車전문지 평가 1위 휩쓴 '현대차 투싼 PHEV' 원동력은?, 예상대로, 년도년도 2분기 3분기 Review: 시장 기대치 부합, 투자의견 ＇Buy＇, 목표주가 300.000원 유지, 볼륨 사이클의 시작, 생산 안정성 개선에 따른 선순환 구조 진입, 3분기 Review: 제품믹스 개선 긍정적, 년도년도 2분기 3분기 Review: 우려 대비 선방한 실적과 가이던스 상향, 년도년도 2분기 3분기 Review: 우려 대비 선방한 실적, 자동차 부문 영업이익 가이던스 상향 조정, 4 분기 실적 개선 기대갑 Up, 결국 관건은 반도체 확보와 생산 정상화, 21년도 3분기 연결 매출 29조원(전년 대비 증감율+4.7%), 영업이익 1.6조원(전년 대비 증감율흑전), OPM 5.6%, 특근 계획은 기 수립, 결국 11월 실행 여부 및 생산 정상화가 단기 주가 변수, 좋아질 일만 남았다, 영업이익은 추정치와 컨센서스에 부합, 가이던스 상향으로 4분기 실적 자신감 표명, 년도년도 2분기 3분기 Review: 가까워진 불확실성 해소 시기, 년도년도 2분기 3분기 (P): 매출액 28조 8,672억원, 영업이익 1조 6,067억원, 수정된 가이던스에 따라 년도년도 2분기 4분기 실적 가시성은 높아져, 2022년, 판매대수 회복이 실적 개선 견인 전망, 반도체 없어도 이 실적, 21년도 3분기 영업이익 1.61조원(흑자전환)으로 기대치 부합, 억눌린 수요를 안고 가는 길, 목표주가 27만원, 투자의견 매수 유지, 볼륨 사이클의 시작, 생산 안정성 개선에 따른 선순환 구조 진입, 3분기 Review: 제품믹스 개선 긍정적, 년도년도 2분기 3분기 Review: 우려 대비 선방한 실적과 가이던스 상향, 년도년도 2분기 3분기 Review: 우려 대비 선방한 실적, 자동차 부문 영업이익 가이던스 상향 조정, 4 분기 실적 개선 기대갑 Up, 좋아질 일만 남았다, 영업이익은 추정치와 컨센서스에 부합, 가이던스 상향으로 4분기 실적 자신감 표명, 현대차 투싼 PHEV, 獨 3대 자동차 전문지 비교평가서 1위 달성, MZ세대가 뽑은 톱 브랜드 15…‘GS25’·‘현대차’·‘KB국민카드’..., 현대차, 4Q 반도체 수급 개선…하반기 호실적 전망 -한국, 현대차, 영업실적 바닥 다진 3분기…믹스 개선으로 방어 -하이, “현대차, PER 6.9배 불과…점진적 가동률 정상화 전망”, 현대케피코, 전기이륜차 구동시스템으로 인도네시아 시장 공략, "현대차, 2022년 실적 최대 호황기 진입할 것"-NH투자증권, 현대차, 차화정 시대 이후 최대 실적 호황기 진입할 것-NH, 결국 관건은 반도체 확보와 생산 정상화, 21년도 3분기 연결 매출 29조원(전년 대비 증감율+4.7%), 영업이익 1.6조원(전년 대비 증감율흑전), OPM 5.6%, 특근 계획은 기 수립, 결국 11월 실행 여부 및 생산 정상화가 단기 주가 변수, 현대차, 3분기 부진 주가 선반영…바닥통과 관점 접근</t>
   </si>
   <si>
     <t>현대자동차, ‘N라인 에디션 자전거’ 공개, 현대차·기아-한국전자통신연구원, 미래 모빌리티 활성화 MOU 체결, 현대차 투싼·아이오닉5, 유로NCAP 최고등급 획득, 별이 5개…현대차 아이오닉5·투싼, 유럽서 '가장 안전한 車', 현대·기아차, 쏘나타·카니발 등 4개차종 31만7902대 '리콜', 현대차·볼보 등 6개사 33만대 리콜…방향지시등 결함 등, "자전거와 브랜드 N의 만남"…현대차, 두 번째 N-라인 자전거 공개, 현대차·기아 자율주행-로보틱스 인공지능 시스템 구축 가속화, 현대차, '운전의 재미 담은' N라인 에디션 자전거 공개, 현대차가 만든 고성능 자전거 타볼까..N 라인 에디션 공개, 현대차, '운전의 재미 담은' N라인 에디션 자전거 공개, 현대차가 만든 고성능 자전거 타볼까..N 라인 에디션 공개, 반도체 위기 뚫은 현대차·기아…고수익 차종이 살렸다, '구식'이라고 외면받더니…테슬라·벤츠 이어 현대차도 '눈독', 현대차·기아, 전자통신연구원과 AI 개발한다, 車반도체가 실적 갈랐다…GM 이익 반토막, 현대차·테슬라 질주, 운전의 재미를 자전거에 담다...현대차 ‘N 라인 에디션 자전거’ 공..., 일상 속 라이딩… 현대차 'N 라인 에디션 자전거'로 즐긴다, 현대차證 3분기 영업익 405억, 車반도체가 실적 갈랐다…GM 이익 반토막, 현대차·테슬라 질주, 운전의 재미를 자전거에 담다...현대차 ‘N 라인 에디션 자전거’ 공..., 일상 속 라이딩… 현대차 'N 라인 에디션 자전거'로 즐긴다, 현대차證 3분기 영업익 405억, 현대차·기아, 한국전자통신연구원과 '자율주행 모빌리티' 협력, 현대차·기아, 한국전자통신연구원과 '자율주행 모빌리티' 협력, 현대차 아이오닉5·투싼, 유로 NCAP에서 최고 안전 등급 획득, 현대차, 고성능 로드바이크 'N 라인 에디션 자전거' 공개, 운전의 재미, 자전거에 담다…현대차, ‘N 라인 에디션 자전거’ 공개, 현대·기아차, 쏘나타·카니발 등 4개차종 31만7902대 '리콜', 현대차·기아-한국전자통신연구원, 미래 모빌리티 활성화 위해 손잡아, 현대차·기아-ETRI, 미래 모빌리티 활성화위해 '맞손', 현대차·볼보 등 6개사 33만대 리콜…방향지시등 결함 등, 현대차, 美 전기차 생산 계기···SK온과 밀월 강화되나, 현대차, 美 전기차 생산 계기···SK온과 밀월 강화되나</t>
@@ -7372,7 +7372,7 @@
     <t>'반도체 공급차질'…현대차 10월 판매 전년비 20.7% 감소, 반도체에 휘청거린 車판매..그랜저 선전에도 현대차·기아 20% 급감, ‘반도체 부족’에···현대차, 10월 30만7039대 판매 전년比 21..., '반도체 공급차질'…현대차 10월 판매 전년비 20.7% 감소, 현대차, 지난달 글로벌 30.7만대 판매…반도체..., 반도체에 휘청거린 車판매..그랜저 선전에도 현대차·기아 20% 급감, ‘반도체 부족’에···현대차, 10월 30만7039대 판매 전년比 21..., 반도체에 휘청거린 車판매..그랜저 선전에도 현대차·기아 20% 급감, 현대차, 지난달 글로벌 30.7만대 판매…반도체...</t>
   </si>
   <si>
-    <t>현대차그룹 R&amp;D 리더 ‘총출동’…미래車 신기술 개발자들과 공유, 현대차그룹 창의인재 페스티벌 '제로원데이' 개최, 현대차, 로봇·UAM 등 미래 모빌리티 '풀악셀', 내년 증시 키워드 '전약후강, 현차삼전, 메타버스', 현대차 판매량 사상 첫 '세계 3위', 현대차그룹 R&amp;D 리더 ‘총출동’…미래車 신기술 개발자들과 공유, 현대차그룹 R&amp;D 스타 총출동..첫 개발자 컨퍼런스 10일 개막, 현대차그룹, 'HMG 콘퍼런스'서 미래기술 소개, "달리는 車창에 고흐 그림이"..현대차 창의문화 확산 나선다, 현대차, 로봇·UAM 등 미래 모빌리티 '풀악셀', 현대차 울산공장, 고용부에 특별연장근로 인가 신청, 현대차그룹, 'HMG 콘퍼런스'서 미래기술 소개, 현대차그룹 창의인재 페스티벌 '제로원데이' 개최, "달리는 車창에 고흐 그림이"..현대차 창의문화 확산 나선다, "주문 적체 해소"…현대차 울산공장, '특별연장근로' 신청, 현대차, 특별연장근로 신청…투싼·싼타페 출고 당겨지나, 현대차그룹 R&amp;D 리더 ‘총출동’…미래車 신기술 개발자들과 공유, 현대차 'HMG 개발자 컨퍼런스' 세계 리더 한자리에, 현대차·기아, 반도체 악재 뚫고 '친환경차 20만대 시대' 연다, 현대차, 특별연장근로 신청…투싼·싼타페 출고 당겨지나, "주문 적체 해소"…현대차 울산공장, '특별연장근로' 신청, "달리는 車창에 고흐 그림이"..현대차 창의문화 확산 나선다, 현대차 울산공장, 노동부에 특별연장근로 인가 신청, 현대차-국립현대미술관, '프로젝트 해시태그 2021' 개최, 현대차그룹 R&amp;D 스타 총출동..첫 개발자 컨퍼런스 10일 개막, 현대차·SK·두산 '연료전지 퍼스트 무버' 노린다, 현대차그룹 R&amp;D 리더 ‘총출동’…미래車 신기술 개발자들과 공유, 현대차그룹 창의인재 페스티벌 '제로원데이' 개최, 현대차-국립현대미술관, '프로젝트 해시태그 2021' 개최, 현대차-국립현대미술관 &lt;프로젝트 해시태그 2021&gt; 개최, 현대차·SK·두산 '연료전지 퍼스트 무버' 노린다, 현대차 'HMG 개발자 컨퍼런스' 세계 리더 한자리에, 현대차·기아, 반도체 악재 뚫고 '친환경차 20만대 시대' 연다, 현대차·SK·두산 '연료전지 퍼스트 무버' 노린다, 현대차-국립현대미술관 &lt;프로젝트 해시태그 2021&gt; 개최</t>
+    <t>현대차그룹 R&amp;D 리더 ‘총출동’…미래車 신기술 개발자들과 공유, 현대차그룹 창의인재 페스티벌 '제로원데이' 개최, 현대차, 로봇·UAM 등 미래 모빌리티 '풀악셀', 내년 증시 키워드 '전약후강, 현차삼전, 메타버스', 현대차 판매량 사상 첫 '세계 3위', 현대차그룹 R&amp;D 리더 ‘총출동’…미래車 신기술 개발자들과 공유, 현대차그룹 R&amp;D 스타 총출동..첫 개발자 컨퍼런스 10일 개막, 현대차그룹, 'HMG 콘퍼런스'서 미래기술 소개, "달리는 車창에 고흐 그림이"..현대차 창의문화 확산 나선다, 현대차, 로봇·UAM 등 미래 모빌리티 '풀악셀', 현대차 울산공장, 고용부에 특별연장근로 인가 신청, 현대차그룹, 'HMG 콘퍼런스'서 미래기술 소개, 현대차그룹 창의인재 페스티벌 '제로원데이' 개최, "달리는 車창에 고흐 그림이"..현대차 창의문화 확산 나선다, "주문 적체 해소"…현대차 울산공장, '특별연장근로' 신청, 현대차, 특별연장근로 신청…투싼·싼타페 출고 당겨지나, 현대차그룹 R&amp;D 리더 ‘총출동’…미래車 신기술 개발자들과 공유, 현대차 'HMG 개발자 컨퍼런스' 세계 리더 한자리에, 현대차·기아, 반도체 악재 뚫고 '친환경차 20만대 시대' 연다, 현대차, 특별연장근로 신청…투싼·싼타페 출고 당겨지나, "주문 적체 해소"…현대차 울산공장, '특별연장근로' 신청, "달리는 車창에 고흐 그림이"..현대차 창의문화 확산 나선다, 현대차 울산공장, 노동부에 특별연장근로 인가 신청, 국립현대미술관, '프로젝트 해시태그 2021' 개최, 현대차그룹 R&amp;D 스타 총출동..첫 개발자 컨퍼런스 10일 개막, 현대차·SK·두산 '연료전지 퍼스트 무버' 노린다, 현대차그룹 R&amp;D 리더 ‘총출동’…미래車 신기술 개발자들과 공유, 현대차그룹 창의인재 페스티벌 '제로원데이' 개최, 국립현대미술관, '프로젝트 해시태그 2021' 개최, 국립현대미술관 &lt;프로젝트 해시태그 2021&gt; 개최, 현대차·SK·두산 '연료전지 퍼스트 무버' 노린다, 현대차 'HMG 개발자 컨퍼런스' 세계 리더 한자리에, 현대차·기아, 반도체 악재 뚫고 '친환경차 20만대 시대' 연다, 현대차·SK·두산 '연료전지 퍼스트 무버' 노린다, 국립현대미술관 &lt;프로젝트 해시태그 2021&gt; 개최</t>
   </si>
   <si>
     <t>현대차·기아, 10월 美판매 선방…제네시스 사상최대 실적, 제네시스·친환경차의 힘...현대차, 반도체난 뚫고 美시장 질주, 현대차그룹-서울대, 배터리 공동연구센터 만든다…미래차 주도권, 현대차그룹·서울대 ‘배터리 공동연구센터’ 설립…“10년간 300억원 투..., 현대차그룹, 300억 투자 서울대와 배터리 공동연구센터 설립, 현대차그룹-서울대, 배터리 공동연구센터 만든다…미래차 주도권, 현대차, 해외 석·박사 인재 끌어모은다···'토크쇼 채용설명회' 개최, 현대차그룹, 300억 투자 서울대와 배터리 공동연구센터 설립, 카카오그룹, 카카오페이 업고 시총 100조 돌파…현대·LG 맹추격, 자율주행부터 로봇공학까지···현대차 개발자 컨퍼런스에 임원 총출동, 현대자동차·기아, 車판매 줄었지만 매출·영업익 늘었다…제네시스·SUV ..., 현대차 승부수…GV70 전기차 美서 생산, 현대차 "서울대와 배터리 연구…300억 투자", 현대차그룹·서울대 ‘배터리 공동연구센터’ 설립…“10년간 300억원 투..., 제네시스 美 판매 신기록 질주…현대차·기아, 올해 혼다 넘는다, 현대차, 해외 우수인재 채용 온라인 라이브 설명회 개최, 현대차, 교통사고 유자녀 후원, 현대차그룹-서울대, 차세대 배터리 공동개발 ···정의선 “미래 전기차 ..., 현대차그룹·서울대 ‘배터리 공동연구센터’ 설립…“10년간 300억원 ..., 제네시스·친환경차의 힘… 반도체 대란 뚫고 美서 달렸다 [현대차·기아 ..., 현대차·기아, 10월 美 실적 선방…"제네시스·친환경차 약진", "전동화 물결 거스를 수 없는 큰 흐름"…현대차, 서울대에 배터리 공동..., 현대차그룹, 300억 투자 서울대와 배터리 공동연구센터 설립, 현대차그룹-서울대, 차세대 배터리 공동개발 ···정의선 “미래 전기차 ..., 현대차그룹·서울대 ‘배터리 공동연구센터’ 설립…“10년간 300억원 ..., "전동화 물결 거스를 수 없는 큰 흐름"…현대차, 서울대에 배터리 공동..., 현대차·기아, 10월 美 실적 선방…"제네시스·친환경차 약진", 현대차그룹, 300억 투자 서울대와 배터리 공동연구센터 설립, 현대차·기아, 10월 美 실적 선방…"제네시스·친환경차 약진", 현대차, 서울대와 차세대 배터리 기술 개발…300억 투자, 현대차 "서울대와 배터리 연구…300억 투자", 현대차, 교통사고 유자녀에 후원금, 현대차, 교통사고 유자녀 후원, 현대차그룹, 전기차 ‘톱 5’…3분기 글로벌 점유율 4.8%, 현대차 승부수…GV70 전기차 美서 생산, 현대자동차·기아, 車판매 줄었지만 매출·영업익 늘었다…제네시스·SUV ..., 현대차, 교통사고 유자녀에 후원금, 제네시스·친환경차의 힘… 반도체 대란 뚫고 美서 달렸다 [현대차·기아 ..., 테슬라 잡은 현대차, 국내 전기차 판매 1위 질주, 현대차, 9일 국내외 기관투자자 대상 기업설명회, 현대자동차, 교통사고 유자녀에 후원금 2000만원 전달, 현대차, 교통사고 유자녀 후원금 2000만원 전달, 테슬라 질주하는데…현대차는 언제 달릴까, 현대차·기아, 지난달 미국판매 실적 업계 평균 넘어, 현대차, 우수 카마스터와 교통사고 유자녀 후원금 전달, 현대차, 교통사고 유자녀에 후원금 전달, 현대차, 이달 5일 '해외 석·박사 채용 온라인 라이브 설명회' 개최, 테슬라 질주하는데…현대차는 언제 달릴까, 현대차·기아, 지난달 미국판매 실적 업계 평균 넘어, 현대차, 교통사고 유자녀 돕는다…후원금 2000만원 전달, 현대자동차, 교통사고 유자녀에 후원금 2000만원 전달, 현대차, 5일 해외 석·박사 채용 온라인 라이브 설명회, 현대차, '해외 우수인재 채용' 온라인 라이브 설명회 개최, 현대차, 해외 우수인재 채용 온라인 라이브 설명회 개최, 제네시스·친환경차의 힘…현대차, 반도체난 속 美 판매량 신장, 현대차·기아, 지난달 미국판매 실적 업계 평균 넘어…친환경차 판매 22..., 테슬라 질주하는데…현대차는 언제 달릴까, 현대차·기아, 지난달 미국판매 실적 업계 평균 넘어, 현대차, '해외 우수인재 채용' 온라인 라이브 설명회 개최, 현대차, 해외 우수인재 채용 온라인 라이브 설명회 개최, 현대차그룹, 3분기 글로벌 전기차 판매 ‘톱 5’…점유율 4.8%, 현대자동차, 교통사고 유자녀 돕기 나선다…2000만원 기부</t>
@@ -7390,10 +7390,10 @@
     <t>현대차그룹, 인도네시아에서 '현대 스타트업 챌린지' 개최, 현대차그룹, 인도네시아 소셜벤처 15팀에 사업비 지원, 현대차, 내년 일본 재진출 최종 검토 중, 정의선 현대차그룹 회장, “다음세대 위해 지속가능한 세상 만들 것”, 현대차, 인니 공략 앞두고 ‘스타트업 챌린지’ 실시, 인니 공장 가동 앞둔 현대차…현지벤처 15곳 사업자금 지원, 2022년 실적 기대주…현대차보다 기아, 사고 친 KT는 ‘반전 매력’, 현대차 노·노 갈등…생산확대 물건너가나, 현대차그룹, 인니서 스타트업 챌린지...15개팀 전략적 지원, 인니 공장 가동 앞둔 현대차…현지벤처 15곳 사업자금 지원, 현대차그룹, 인도네시아 소셜벤처 15팀에 사업비 지원, 현대차 노·노 갈등…생산확대 물건너가나, 2022년 실적 기대주…현대차보다 기아, 사고 친 KT는 ‘반전 매력’, 현대차그룹, 인니서 스타트업 챌린지...15개팀 전략적 지원, 현대차그룹, 인도네시아에서 '현대 스타트업 챌린지' 개최, 현대차그룹, 인니서 '2021 현대 스타트업 챌린지' 개최</t>
   </si>
   <si>
-    <t>현대차-고려대의료원, 이동형 병원 공동연구 MOU, 현대차 정몽구 재단, 9년간 소방관 자녀 1800명에 19억원 지원, 현대차 정몽구 재단, 소방관 자녀 1,800명에 19억원 지원, 현대車, 현대차證서 600억 규모 MMT 매수, 현대차그룹 띄운 '슈퍼널' 뭐지?..UAM 美법인명 확정-사업 탄력, 현대차그룹, 美 UAM 법인 새 이름 '슈퍼널' 공개…사업 박차, 금감원, 현대차·메리츠·키움증권·하나금융투자 리스크관리 미흡 제재했다, 현대차·메리츠증권 등 리스크관리 미흡 '무더기 제재', 현대차그룹 AAM 파트너십 확대…도심항공 기준 세운다, 현대차그룹 AAM 파트너십 확대...도심항공 기준 세운다, 고려대의료원, 현대자동차와 미래형 이동형 병원 개발, 현대차-고려대의료원, 이동형 병원 공동연구 MOU, 카카오 다음 주자는 카카오엔터?…현대차證 “내년 상반기, 카카오엔터 I..., 현대차 정몽구 재단, 9년간 소방관 자녀 1800명에 19억원 지원, 현대차 정몽구 재단, 소방관 자녀 1,800명에 19억원 지원, 현대車, 현대차證서 600억 규모 MMT 매수, 현대차 美 도심항공모빌리티 법인 새 이름 '슈퍼널' 확정, 현대차그룹, 美 UAM 법인 ‘슈퍼널’ 공개…하늘길 넓힌다, 현대차, 美UAM 시장공략…새 이름은 '슈퍼널', 현대차 美 UAM 법인명은'슈퍼널', 현대車, 현대차證서 600억 규모 MMT 매수, 현대차 美 도심항공모빌리티 법인 새 이름 '슈퍼널' 확정, 현대차그룹, 美 UAM 법인 ‘슈퍼널’ 공개…하늘길 넓힌다, 현대차, 美UAM 시장공략…새 이름은 '슈퍼널', 현대차 美 UAM 법인명은'슈퍼널', 현대차 美 UAM 법인명은'슈퍼널', 현대차, 美UAM 시장공략…새 이름은 '슈퍼널', 고려대의료원, 현대자동차와 미래형 이동형 병원 개발, 현대차그룹 AAM 파트너십 확대...도심항공 기준 세운다, 카카오 다음 주자는 카카오엔터?…현대차證 “내년 상반기, 카카오엔터 I..., 현대차·메리츠증권 등 리스크관리 미흡 '무더기 제재', 현대차그룹 AAM 파트너십 확대…도심항공 기준 세운다, 현대차-21년도 3분기 실적 해외 NDR - Key Takeaways, 반도체 칩 부족 상황 및 소싱 변화, 전기차 반도체는 다른가?, 원자재 가격 상승, 물류비 상승에 따른 원가 부담?, 시장에서 현대차 전기차의 성장성에 주목하지 않는 이유? 배터리 조달 전략은?, 정부의 脫탄소 마케팅?…현대車 수소탱크 투자유치에 숟가락..., 배터리 회사와 협업하고, 연구센터 짓고…'꿈의 배터리'를 위한 현대차의..., 현대차, 고대의료원과 '스마트 의료기기-이동형 병원' 공동 연구·개발, 고려대의료원, 현대자동차와 미래형 이동형 병원 개발, 금감원, 현대차·메리츠·키움증권·하나금융투자 리스크관리 미흡 제재했다, 현대차-고려대의료원, 미래형 모빌리티 의료 서비스 MOU, 움직이는 병원 나온다..현대차-고려대 방문진료 서비스 시범운영, 배터리 회사와 협업하고, 연구센터 짓고…'꿈의 배터리'를 위한 현대차의..., 움직이는 병원 나온다..현대차-고려대 방문진료 서비스 시범운영, 현대차-고려대의료원, 미래형 모빌리티 의료 서비스 ‘맞손’, 현대차그룹 AAM 파트너십 확대…도심항공 기준 세운다, 금감원, 현대차·메리츠·키움증권·하나금융투자 리스크관리 미흡 제재했다</t>
-  </si>
-  <si>
-    <t>현대차그룹 미디어 아티스트 어워드 그랑프리에 로렌스 렉, 큰손 사랑 '현대차·기아' 好好, 현대차 엔진결함 제보한 내부고발자, 美서 280억원대 포상금, "현대차 세타 2엔진 결함" 고발 직원…美 정부서 280억원 받는 이유..., 美교통당국, 현대차·기아 내부고발자에 280억 포상금 첫 지급, 현대차 미디어아트 공모전…로렌스 렉 작가 '그랑프리', 현대차 "스마트 모빌리티 디바이스 통합 네트워크 개발", 버튼 누르면 스스로 발레파킹…현대차 기술 이정도라니, 美교통당국, 현대차·기아 내부고발자에 포상금 280억원 지급, 현대차·기아도 美상무부에 반도체 자료 제출, 현대차, '레벨 3' 자율주행車 내년부터 양산, 현대차, '레벨 3' 자율주행車 내년부터 양산, 현대차그룹, 차세대 미디어 예술가 발굴 '제 4회 VH 어워드' 개최, 현대차그룹 미디어 아티스트 어워드 그랑프리에 로렌스 렉, 현대차 “내년 ‘레벨3’ 자율주행차 양산...2024년 ‘레벨4’ 현..., 현대차·기아도 美상무부에 반도체 자료 제출, 현대차·기아도 美 상무부에 반도체 자료 제출, 현대차 “내년 ‘레벨3’ 자율주행차 양산...2024년 ‘레벨4’ 현..., 현대차 "車·로봇·UAM·에너지 아우르는 디바이스 네트워크 개발", "미래모빌리티, 함께 만들자"…현대차그룹, HMG 개발자 컨퍼런스 첫 ..., 큰손 사랑 '현대차·기아' 好好, 현대차·기아도 美 상무부에 반도체 자료 제출, 현대차 “내년 ‘레벨3’ 자율주행차 양산...2024년 ‘레벨4’ 현실..., 현대차 엔진결함 제보한 내부고발자, 美서 280억원대 포상금, 현대차·기아, 美상무부에 마감 직전 반도체 자료 제출(종합), 현대차 “내년 ‘레벨3’ 자율주행 기술 양산…2024년 ‘레벨4’ 현..., 현대차-수소 상용차, 경쟁 상대가 없다, 수소 상용차, 경쟁 상대가 없다, 수소상용차 보급은 대중화의 촉매, 미래차 전략 강화로 중장기 성장성 부각, 현대차-모빌리티 주도권을 향한 여정, 4분기 영업이익 1.93조원 전망, 차량용 반도체 수급난 완화에 따른 가동률 점진적 개선 전망, 내년 아이오닉6 출시, 미국 현지 전기차 생산 등을 통한 친환경차 시장 선점 기대, 美교통당국, 현대차·기아 내부고발자에 280억 포상금 첫 지급, 美교통당국, 현대차·기아 내부고발자에 포상금 280억원 지급, 현대차·기아 미국법인, 美상무부에 반도체 자료 제출, 현대차 엔진결함 제보한 내부고발자, 美서 280억원대 포상금, 현대차그룹 ‘VH 어워드’ 개최…“차세대 미디어 아티스트 지원”, 현대차그룹, 차세대 미디어 예술가 발굴 '제 4회 VH 어워드' 개최, 현대차·기아 미국법인, 美상무부에 반도체 자료 제출, "현대차 세타 2엔진 결함" 고발 직원…美 정부서 280억원 받는 이유...</t>
+    <t>고려대의료원, 이동형 병원 공동연구 MOU, 현대차 정몽구 재단, 9년간 소방관 자녀 1800명에 19억원 지원, 현대차 정몽구 재단, 소방관 자녀 1,800명에 19억원 지원, 현대車, 현대차證서 600억 규모 MMT 매수, 현대차그룹 띄운 '슈퍼널' 뭐지?..UAM 美법인명 확정-사업 탄력, 현대차그룹, 美 UAM 법인 새 이름 '슈퍼널' 공개…사업 박차, 금감원, 현대차·메리츠·키움증권·하나금융투자 리스크관리 미흡 제재했다, 현대차·메리츠증권 등 리스크관리 미흡 '무더기 제재', 현대차그룹 AAM 파트너십 확대…도심항공 기준 세운다, 현대차그룹 AAM 파트너십 확대...도심항공 기준 세운다, 고려대의료원, 현대자동차와 미래형 이동형 병원 개발, 고려대의료원, 이동형 병원 공동연구 MOU, 카카오 다음 주자는 카카오엔터?…현대차證 “내년 상반기, 카카오엔터 I..., 현대차 정몽구 재단, 9년간 소방관 자녀 1800명에 19억원 지원, 현대차 정몽구 재단, 소방관 자녀 1,800명에 19억원 지원, 현대車, 현대차證서 600억 규모 MMT 매수, 현대차 美 도심항공모빌리티 법인 새 이름 '슈퍼널' 확정, 현대차그룹, 美 UAM 법인 ‘슈퍼널’ 공개…하늘길 넓힌다, 현대차, 美UAM 시장공략…새 이름은 '슈퍼널', 현대차 美 UAM 법인명은'슈퍼널', 현대車, 현대차證서 600억 규모 MMT 매수, 현대차 美 도심항공모빌리티 법인 새 이름 '슈퍼널' 확정, 현대차그룹, 美 UAM 법인 ‘슈퍼널’ 공개…하늘길 넓힌다, 현대차, 美UAM 시장공략…새 이름은 '슈퍼널', 현대차 美 UAM 법인명은'슈퍼널', 현대차 美 UAM 법인명은'슈퍼널', 현대차, 美UAM 시장공략…새 이름은 '슈퍼널', 고려대의료원, 현대자동차와 미래형 이동형 병원 개발, 현대차그룹 AAM 파트너십 확대...도심항공 기준 세운다, 카카오 다음 주자는 카카오엔터?…현대차證 “내년 상반기, 카카오엔터 I..., 현대차·메리츠증권 등 리스크관리 미흡 '무더기 제재', 현대차그룹 AAM 파트너십 확대…도심항공 기준 세운다, 21년도 3분기 실적 해외 NDR - Key Takeaways, 반도체 칩 부족 상황 및 소싱 변화, 전기차 반도체는 다른가?, 원자재 가격 상승, 물류비 상승에 따른 원가 부담?, 시장에서 현대차 전기차의 성장성에 주목하지 않는 이유? 배터리 조달 전략은?, 정부의 脫탄소 마케팅?…현대車 수소탱크 투자유치에 숟가락..., 배터리 회사와 협업하고, 연구센터 짓고…'꿈의 배터리'를 위한 현대차의..., 현대차, 고대의료원과 '스마트 의료기기-이동형 병원' 공동 연구·개발, 고려대의료원, 현대자동차와 미래형 이동형 병원 개발, 금감원, 현대차·메리츠·키움증권·하나금융투자 리스크관리 미흡 제재했다, 고려대의료원, 미래형 모빌리티 의료 서비스 MOU, 움직이는 병원 나온다..현대차-고려대 방문진료 서비스 시범운영, 배터리 회사와 협업하고, 연구센터 짓고…'꿈의 배터리'를 위한 현대차의..., 움직이는 병원 나온다..현대차-고려대 방문진료 서비스 시범운영, 고려대의료원, 미래형 모빌리티 의료 서비스 ‘맞손’, 현대차그룹 AAM 파트너십 확대…도심항공 기준 세운다, 금감원, 현대차·메리츠·키움증권·하나금융투자 리스크관리 미흡 제재했다</t>
+  </si>
+  <si>
+    <t>현대차그룹 미디어 아티스트 어워드 그랑프리에 로렌스 렉, 큰손 사랑 '현대차·기아' 好好, 현대차 엔진결함 제보한 내부고발자, 美서 280억원대 포상금, "현대차 세타 2엔진 결함" 고발 직원…美 정부서 280억원 받는 이유..., 美교통당국, 현대차·기아 내부고발자에 280억 포상금 첫 지급, 현대차 미디어아트 공모전…로렌스 렉 작가 '그랑프리', 현대차 "스마트 모빌리티 디바이스 통합 네트워크 개발", 버튼 누르면 스스로 발레파킹…현대차 기술 이정도라니, 美교통당국, 현대차·기아 내부고발자에 포상금 280억원 지급, 현대차·기아도 美상무부에 반도체 자료 제출, 현대차, '레벨 3' 자율주행車 내년부터 양산, 현대차, '레벨 3' 자율주행車 내년부터 양산, 현대차그룹, 차세대 미디어 예술가 발굴 '제 4회 VH 어워드' 개최, 현대차그룹 미디어 아티스트 어워드 그랑프리에 로렌스 렉, 현대차 “내년 ‘레벨3’ 자율주행차 양산...2024년 ‘레벨4’ 현..., 현대차·기아도 美상무부에 반도체 자료 제출, 현대차·기아도 美 상무부에 반도체 자료 제출, 현대차 “내년 ‘레벨3’ 자율주행차 양산...2024년 ‘레벨4’ 현..., 현대차 "車·로봇·UAM·에너지 아우르는 디바이스 네트워크 개발", "미래모빌리티, 함께 만들자"…현대차그룹, HMG 개발자 컨퍼런스 첫 ..., 큰손 사랑 '현대차·기아' 好好, 현대차·기아도 美 상무부에 반도체 자료 제출, 현대차 “내년 ‘레벨3’ 자율주행차 양산...2024년 ‘레벨4’ 현실..., 현대차 엔진결함 제보한 내부고발자, 美서 280억원대 포상금, 현대차·기아, 美상무부에 마감 직전 반도체 자료 제출(종합), 현대차 “내년 ‘레벨3’ 자율주행 기술 양산…2024년 ‘레벨4’ 현..., 수소 상용차, 경쟁 상대가 없다, 수소 상용차, 경쟁 상대가 없다, 수소상용차 보급은 대중화의 촉매, 미래차 전략 강화로 중장기 성장성 부각, 모빌리티 주도권을 향한 여정, 4분기 영업이익 1.93조원 전망, 차량용 반도체 수급난 완화에 따른 가동률 점진적 개선 전망, 내년 아이오닉6 출시, 미국 현지 전기차 생산 등을 통한 친환경차 시장 선점 기대, 美교통당국, 현대차·기아 내부고발자에 280억 포상금 첫 지급, 美교통당국, 현대차·기아 내부고발자에 포상금 280억원 지급, 현대차·기아 미국법인, 美상무부에 반도체 자료 제출, 현대차 엔진결함 제보한 내부고발자, 美서 280억원대 포상금, 현대차그룹 ‘VH 어워드’ 개최…“차세대 미디어 아티스트 지원”, 현대차그룹, 차세대 미디어 예술가 발굴 '제 4회 VH 어워드' 개최, 현대차·기아 미국법인, 美상무부에 반도체 자료 제출, "현대차 세타 2엔진 결함" 고발 직원…美 정부서 280억원 받는 이유...</t>
   </si>
   <si>
     <t>내년 현대차·기아 새 지도 플랫폼 탑재한다, 현대차 북미사장 "최악 지났다…올 4분기 납품 정상화 목표", 현대차 북미사장 "공급 차질 최악 시기 넘겨···4분기 생산 목표 달성..., 車계의 '앱스토어' 만들자…현대차그룹이 '데이터 호수' 만드는 이유, "현대차 부품난 최악 지났다" 현대차 북미사장 언급, 현대ENG, 스마트건설기술 공모 수상작 선정…자율주행 페인팅 로봇 등, 현대차, 자율주행에 '바보장치' 고집하는 이유, 현대차, 2%대 하락세…3거래일 연속 하락, 현대차그룹, 애플·구글에 도전장 "내년에 자동차용 플랫폼 공개할 것", 부릉, 현대차그룹 개발자 컨퍼런스서 'AI 운영 노하우' 공개, 현대차·LG, 글로벌 자율주행 특허 'TOP 10', 현대차 북미사장 "공급망 대란, 최악의 시기는 지났다"(종합), 파워로직스, 현대차 폐배터리 재사용 ESS 생산한다, 현대차그룹, 2045년 모든 국가서 내연기관차 판매 전면중단, 김부겸 총리, 정의선 현대차 회장 만난다…청년 일자리 확대 논의, (영상)"내년엔 손 놓고 운전" 자율주행 기술 자신감 내비친 현대차, 현대차·기아 차세대 전기차 '세븐-EV9' 美서 나란히 첫 공개, 현대차그룹 2045년 탄소중립… 원자재·부품까지 다 바꾼다 [저무는 내..., 현대차그룹, 2045년 모든 국가서 내연기관차 판매 전면중단, 현대차에서 걸려온 전화 한 통에…코오롱인더 '수소차 소재기업' 변신, 현대차·기아 2040년부터 경유·휘발유車 퇴출..전기차만 판매, 폐배터리 재활용 위해 뭉쳤다... 삼성·현대차·SK·LG, 첫...</t>
@@ -7408,13 +7408,13 @@
     <t>현대차 개발자콘퍼런스 성료…"스마트 모빌리티 개발자들이 중심", 현대차그룹, 美 뉴스위크 '오토 어워즈' 7개 부문 석권, “스마트 모빌리티의 중심은 개발자”···현대차그룹, 개발자 컨퍼런스 성..., 현대차·LG전자·삼바…다우존스 지속가능지수 월드 편입, 정의선 현대차그룹 회장, 아시아양궁연맹 회장 5선 연임, 현대차그룹, 美 뉴스위크 '오토 어워즈' 7개 부문 석권, 현대차·LG전자·삼바…다우존스 지속가능지수 월드 편입, 현대차·삼성바이오·SKT 등 6곳, 다우 글로벌지속가능지수 편입, 현대차 개발자 콘퍼런스 성료…온라인 6500명 참관, 정의선 현대차그룹 회장, 아시아양궁연맹 회장 5선 연임, 정의선 현대차그룹 회장 '아시아양궁연맹회장' 5연속 선임, 현대·기아차, 마그네슘 재고 1.5개월···中 감산 장기화땐 車산업 멈..., 현대차, 다우존스 지속가능지수 편입, 정의선 현대차그룹 회장, 아시아양궁연맹 5회 연속 회장 선임, 현대차그룹, 첫 HMG 개발자 콘퍼런스 성료…6500명 참가, 정의선 현대차그룹 회장, 아시아양궁연맹 회장 5연임 성공, 정의선 현대차 회장, 아시아양궁연맹 회장 5회 연속 선임</t>
   </si>
   <si>
-    <t>정의선 현대차그룹회장, 5연속 아시아양궁연맹 회장 선임, 현대차 정몽구 재단, 온드림 앙상블 콘서트 개최, 현대차 글로벌 전기차 판매 5위...한국은 내수 7위로 상승, 아멕스 센츄리온 카드, 삼성·현대 어느 카드 ..., 현대차 정몽구 재단, 온드림 앙상블 콘서트 개최, 정의선 현대차그룹회장, 5연속 아시아양궁연맹 회장 선임, 현대차 글로벌 전기차 판매 5위...한국은 내수 7위로 상승, 아멕스 센츄리온 카드, 삼성·현대 어느 카드 ..., 현대차-침묵을 깨고 방향을 제시할 시기, 2022년 초 미래 모빌리티 비전 공개에 주목, 반도체 공급 완화 통한 점진적 판매 회복 → 2022년 실적 눈높이 및 밸류에이션 매력도 상향, 투자의견 Buy, 적정주가 285,000원 유지, ‘2021 DJSI월드’ 삼바·SKT·카카오·현대차 등 신규편입, 현대차 남양연구소 직원 21명 코로나19 확진…전원 재택근무 전환, 현대차 남양연구소서 집단감염 발생, 21명 확진, 파죽지세 현대차·기아 전용전기차… 연내 수출 5만대 넘긴다, 요소수 필요 없는 현대차 수소트럭 등판, 현대차 남양연구소서 집단감염 발생, 21명 확진, 현대차 남양연구소 직원 21명 코로나19 집단감염, 정의선 현대차그룹 회장, 아시아양궁연맹 회장 첫 5회 연속 선임, 한국 전기차 판매 세계 7위···현대차는 中 BYD 이어 5위, 현대트랜시스, 2021지속가능경영보고서 발표…ESG 경영 확대</t>
-  </si>
-  <si>
-    <t>현대차·기아 유럽서 '전기차 질주' …올해 첫 10만대 판매 돌파, HPC 설비 가동으로 잉여현금창출 확대 점쳐지는 현대케미칼, 삼성·현대차·SK 내부거래 100조…효성, 공시 누락, 현대차-지금까지는 추진력을 얻기 위함이었다, COVID-19 국면에서 경쟁사와 달리 신차 및 xEV 전략을 공격적으로 지속 추진한 결과 2023년까지 시장 변화에 탄력적인 대응과 적응이 기대, 글로벌 부품사의 공급 문제 지속, 대한항공, 현대차 등 5개사 'K-UAM' 드림팀 뭉쳤다, 대한항공, 'K-UAM 어벤저스' 합류···현대차 등 5개사와 MOU ..., '현대차' 띄운 도심항공기 올라탄 '대한항공'..730조 시장 공략, 현대차·대한항공 등 5개사 도심항공길 산업화에 속도, “2년간 보호예수” 주요주주로 현대차 업은 오토앤 다음달 코..., 현대건설기계, 현대중공투자에 1464억 출자, "K-UAM 어벤져스" 현대차·KT·대한항공 등 5개사 MOU 체결, "730조 UAM 잡아라" 롯데 출사표, 현대차·대한항공 맞손, 현대건설기계, 현대중공투자에 1464억 출자, "K-UAM 어벤져스" 현대차·KT·대한항공 등 5개사 MOU 체결, "730조 UAM 잡아라" 롯데 출사표, 현대차·대한항공 맞손, 현대차, 항공·공항·건설·통신사 손 잡고 UAM 사업 활성화, 현대차·인천공항·현대건설·KT·대한항공 'K-UAM 어밴저스' 떴다, 현대차證, 부동산 유튜브 콘텐츠 인기…“전문가 인터뷰 영상 40만뷰 돌..., 대한항공, 현대차 등 5개사 'K-UAM' 드림팀 뭉쳤다, 삼성·현대차·SK 내부거래 100조…효성, 공시 누락, 현대차證, 부동산 유튜브 콘텐츠 인기…“전문가 인터뷰 영상 40만뷰 돌..., 현대차·기아 유럽서 '전기차 질주' …올해 첫 10만대 판매 돌파, HPC 설비 가동으로 잉여현금창출 확대 점쳐지는 현대케미칼, 현대차·카카오·쏘카 '깐부'로 나서자…물 만난 자율주행 스타트업, 현대차·대한항공·KT 등 5개사 UAM활성화위해 맞손</t>
-  </si>
-  <si>
-    <t>'정의선式 탄소중립·친환경차 전략' 전기차 수출 속도 내는 현대차·기아, 현대ENG, 세계최대 'LNG 터미널' 준공, 정의선도 다시 모셨다…현대차 디자인 살려낸 거장의 삶, 현대차그룹 디자이너 '피터 슈라이어' 조명한 책 나온다, 코로나·반도체 위기에도…현대차 역대 최대 고용, '정의선式 탄소중립·친환경차 전략' 전기차 수출 속도 내는 현대차·기아, 코로나로 급식 멈추자…대안 찾은 CJ·신세계 웃고, 삼성·현대 울었다, 현대차와 협력 강화? 中 CATL, K-배터리 안방에 지사 설립, 코로나·반도체 위기에도…현대차 역대 최대 고용, 배터리 1위 中 CATL, 한국 진출…현대차와 협력 강화하나, 현대자동차, 전국 28곳에 '드라이빙 라운지' 운영…비대면으로 시승 체..., 현대차 아이오닉5, 호주 ‘올해의차’에…인기행진 이어간다, 현대차와 협력 강화? 中 CATL, K-배터리 안방에 지사 설립, 배터리 1위 中 CATL, 한국 진출…현대차와 협력 강화하나, 현대차 아이오닉5, 호주 ‘올해의차’에…인기행진 이어간다, 현대차그룹 디자이너 '피터 슈라이어' 조명한 책 나온다, 현대자동차, 전국 28곳에 '드라이빙 라운지' 운영…비대면으로 시승 체..., 현대ENG, 세계최대 'LNG 터미널' 준공, ‘현대차 사내벤처’ 오토앤, 다음달 코스닥 입성, "테슬라는 자고 나면 오르는데…" 현대차 주가 내년엔 뛴다, "쌍용차가 살아야 현대차도 산다"…강영권 에디슨모터스 회장 일침, 전기차 시대 열렸는데…현대차가 내연기관용 배터리에 관심 갖는 이유, 현대차-2022년 BEV 해외 현지 생산 개시를 기대하며, 21년도 4분기 추정치를 매출액 30.9조 원, 영업이익 2.0조 원에서 매출액 32.7조 원, 영업이익 2.1조 원으로 상향 조정, Buy 투자의견과 목표주가 320,000원을 유지, 2025E 연간 글로벌 BEV 판매량 상향 조정 및 BEV 해외 현지 생산 계획 업데이트 기대, 정의선도 다시 모셨다…현대차 디자인 살려낸 거장의 삶, 전기차 시대 열렸는데…현대차가 내연기관용 배터리에 관심 갖는 이유</t>
+    <t>정의선 현대차그룹회장, 5연속 아시아양궁연맹 회장 선임, 현대차 정몽구 재단, 온드림 앙상블 콘서트 개최, 현대차 글로벌 전기차 판매 5위...한국은 내수 7위로 상승, 아멕스 센츄리온 카드, 삼성·현대 어느 카드 ..., 현대차 정몽구 재단, 온드림 앙상블 콘서트 개최, 정의선 현대차그룹회장, 5연속 아시아양궁연맹 회장 선임, 현대차 글로벌 전기차 판매 5위...한국은 내수 7위로 상승, 아멕스 센츄리온 카드, 삼성·현대 어느 카드 ..., 침묵을 깨고 방향을 제시할 시기, 2022년 초 미래 모빌리티 비전 공개에 주목, 반도체 공급 완화 통한 점진적 판매 회복 → 2022년 실적 눈높이 및 밸류에이션 매력도 상향, 투자의견 Buy, 적정주가 285,000원 유지, ‘2021 DJSI월드’ 삼바·SKT·카카오·현대차 등 신규편입, 현대차 남양연구소 직원 21명 코로나19 확진…전원 재택근무 전환, 현대차 남양연구소서 집단감염 발생, 21명 확진, 파죽지세 현대차·기아 전용전기차… 연내 수출 5만대 넘긴다, 요소수 필요 없는 현대차 수소트럭 등판, 현대차 남양연구소서 집단감염 발생, 21명 확진, 현대차 남양연구소 직원 21명 코로나19 집단감염, 정의선 현대차그룹 회장, 아시아양궁연맹 회장 첫 5회 연속 선임, 한국 전기차 판매 세계 7위···현대차는 中 BYD 이어 5위, 현대트랜시스, 2021지속가능경영보고서 발표…ESG 경영 확대</t>
+  </si>
+  <si>
+    <t>현대차·기아 유럽서 '전기차 질주' …올해 첫 10만대 판매 돌파, HPC 설비 가동으로 잉여현금창출 확대 점쳐지는 현대케미칼, 삼성·현대차·SK 내부거래 100조…효성, 공시 누락, 지금까지는 추진력을 얻기 위함이었다, COVID-19 국면에서 경쟁사와 달리 신차 및 xEV 전략을 공격적으로 지속 추진한 결과 2023년까지 시장 변화에 탄력적인 대응과 적응이 기대, 글로벌 부품사의 공급 문제 지속, 대한항공, 현대차 등 5개사 'K-UAM' 드림팀 뭉쳤다, 대한항공, 'K-UAM 어벤저스' 합류···현대차 등 5개사와 MOU ..., '현대차' 띄운 도심항공기 올라탄 '대한항공'..730조 시장 공략, 현대차·대한항공 등 5개사 도심항공길 산업화에 속도, “2년간 보호예수” 주요주주로 현대차 업은 오토앤 다음달 코..., 현대건설기계, 현대중공투자에 1464억 출자, "K-UAM 어벤져스" 현대차·KT·대한항공 등 5개사 MOU 체결, "730조 UAM 잡아라" 롯데 출사표, 현대차·대한항공 맞손, 현대건설기계, 현대중공투자에 1464억 출자, "K-UAM 어벤져스" 현대차·KT·대한항공 등 5개사 MOU 체결, "730조 UAM 잡아라" 롯데 출사표, 현대차·대한항공 맞손, 현대차, 항공·공항·건설·통신사 손 잡고 UAM 사업 활성화, 현대차·인천공항·현대건설·KT·대한항공 'K-UAM 어밴저스' 떴다, 현대차證, 부동산 유튜브 콘텐츠 인기…“전문가 인터뷰 영상 40만뷰 돌..., 대한항공, 현대차 등 5개사 'K-UAM' 드림팀 뭉쳤다, 삼성·현대차·SK 내부거래 100조…효성, 공시 누락, 현대차證, 부동산 유튜브 콘텐츠 인기…“전문가 인터뷰 영상 40만뷰 돌..., 현대차·기아 유럽서 '전기차 질주' …올해 첫 10만대 판매 돌파, HPC 설비 가동으로 잉여현금창출 확대 점쳐지는 현대케미칼, 현대차·카카오·쏘카 '깐부'로 나서자…물 만난 자율주행 스타트업, 현대차·대한항공·KT 등 5개사 UAM활성화위해 맞손</t>
+  </si>
+  <si>
+    <t>'정의선式 탄소중립·친환경차 전략' 전기차 수출 속도 내는 현대차·기아, 현대ENG, 세계최대 'LNG 터미널' 준공, 정의선도 다시 모셨다…현대차 디자인 살려낸 거장의 삶, 현대차그룹 디자이너 '피터 슈라이어' 조명한 책 나온다, 코로나·반도체 위기에도…현대차 역대 최대 고용, '정의선式 탄소중립·친환경차 전략' 전기차 수출 속도 내는 현대차·기아, 코로나로 급식 멈추자…대안 찾은 CJ·신세계 웃고, 삼성·현대 울었다, 현대차와 협력 강화? 中 CATL, K-배터리 안방에 지사 설립, 코로나·반도체 위기에도…현대차 역대 최대 고용, 배터리 1위 中 CATL, 한국 진출…현대차와 협력 강화하나, 현대자동차, 전국 28곳에 '드라이빙 라운지' 운영…비대면으로 시승 체..., 현대차 아이오닉5, 호주 ‘올해의차’에…인기행진 이어간다, 현대차와 협력 강화? 中 CATL, K-배터리 안방에 지사 설립, 배터리 1위 中 CATL, 한국 진출…현대차와 협력 강화하나, 현대차 아이오닉5, 호주 ‘올해의차’에…인기행진 이어간다, 현대차그룹 디자이너 '피터 슈라이어' 조명한 책 나온다, 현대자동차, 전국 28곳에 '드라이빙 라운지' 운영…비대면으로 시승 체..., 현대ENG, 세계최대 'LNG 터미널' 준공, ‘현대차 사내벤처’ 오토앤, 다음달 코스닥 입성, "테슬라는 자고 나면 오르는데…" 현대차 주가 내년엔 뛴다, "쌍용차가 살아야 현대차도 산다"…강영권 에디슨모터스 회장 일침, 전기차 시대 열렸는데…현대차가 내연기관용 배터리에 관심 갖는 이유, 2022년 BEV 해외 현지 생산 개시를 기대하며, 21년도 4분기 추정치를 매출액 30.9조 원, 영업이익 2.0조 원에서 매출액 32.7조 원, 영업이익 2.1조 원으로 상향 조정, Buy 투자의견과 목표주가 320,000원을 유지, 2025E 연간 글로벌 BEV 판매량 상향 조정 및 BEV 해외 현지 생산 계획 업데이트 기대, 정의선도 다시 모셨다…현대차 디자인 살려낸 거장의 삶, 전기차 시대 열렸는데…현대차가 내연기관용 배터리에 관심 갖는 이유</t>
   </si>
   <si>
     <t>"자동차야, 라운지야" 현대차·기아, 美LA서 전기 SUV 콘셉트카 선..., 현대차·기아, 대형 전기차 SUV...‘스윗 카 라이프’ 시대 성큼, 중국 물량 공세에···현대 전기차 점유율 한 단계 떨어진 5위, "따라올테면 따라와봐" 세계 전기차 1위는 테슬라…현대차는?, 현대차 전기차 충전소 '이핏'…앱으로 다른 충전소서도 이용, 현대차, 전기차 충전 생태계 이끈다…'E-pit 연합' 결성, "한국은 슈퍼차저 아니라 'E-PIT'"···현대차·6개 충전사업자 ..., 현대차 '아이오닉7'…이렇게 나올겁니다, "충전 더 편해질까?" ?현대차그룹, 국내 전기차 충전사업자와 연합 네..., 현대차·기아, 유럽시장 전기차 판매량 10만대 돌파, 현대차·기아, LA 오토쇼서 전기SUV 콘셉트카 `세븐·..., 현대차, LA 오토쇼에서 전기 SUV 콘셉트카 '세븐' 공개, 현대차 대형 전기 SUV '세븐' 콘셉트카 공개..아이오닉 3번째 라..., 전기 SUV 탄 현대차·기아, LA 떴다, 현대차 ‘H-온드림’ 10년간 3816개 일자리 창출, 현대차 유럽 전기차 판매량 첫 10만대 돌파, 현대차 전기차 충전소 '이핏'…앱으로 다른 충전소서도 이용, 현대차 ‘H-온드림’ 10년간 3816개 일자리 창출, 현대차·기아, 유럽서 전기차 누적 판매 10만대 돌파, 현대차·기아, 유럽 전기차 판매 10만대 돌파…3개월째 두자리 점유율, 현대차 2년만에 자사주 매입, 5천억 규모, 현대차 아이오닉5·싼타크루즈·GV70 美서 리비안·루시드 넘을까, 현대차, 5045억원 규모 자사주 매입…"주주가치 제고", 현대차·기아, 첫 대형 전기차 '세븐·EV9' LA오토쇼 동시 출격, "자동차야, 라운지야" 현대차·기아, 美LA서 전기 SUV 콘셉트카 선..., 현대차·기아, 대형 전기차 SUV...‘스윗 카 라이프’ 시대 성큼, 현대차 '아이오닉7'…이렇게 나올겁니다, "주주가치 제고"…현대차, 5000억원 규모 자사주 매입, 23개월만에 주주 달래기 나선 현대차 5045억 자사주 매입, 현대차·기아, 첫 대형 전기차 '세븐·EV9' LA오토쇼 동시 출격, 중국 물량 공세에···현대 전기차 점유율 한 단계 떨어진 5위, "따라올테면 따라와봐" 세계 전기차 1위는 테슬라…현대차는?, 현대차, 전기차 충전 생태계 이끈다…'E-pit 연합' 결성, 현대차그룹·정몽구 재단 일자리 3816개 창출..'H-온드림' 성과 ..., 아이오닉5, 현대차 전기차 최초로 ‘북미 올해의 차’ 후보 올라, 현대차그룹·정몽구 재단 일자리 3816개 창출..'H-온드림' 성과 ..., 현대차, LA 오토쇼에서 전기 SUV 콘셉트카 '세븐' 공개, 현대차, 5000억 규모 자사주 취득 결정, 현대차·기아, LA 오토쇼서 전기SUV 콘셉트카 `세븐·..., 현대차, 아이오닉7 베일벗는다…콘셉카 '세븐' 최초 공개, "내연기관 SUV는 잊어라"···기아 'EV9' 현대 '세븐' 동시출격, "내연기관 SUV는 잊어라"···기아 'EV9' 현대 '세븐' 동시출격, 현대차, 아이오닉7 베일벗는다…콘셉카 '세븐' 최초 공개, 현대차,LA오토쇼서 대형 SUV 콘셉트카 '세븐' 공개, 세계 전기차 1위는 테슬라…현대차·기아 5위로 밀려, 현대차그룹 전기차 충전 어벤져스 띄운다..6개 사업자와 '맞손', 현대차그룹, 전기차 충전 6개사와 'E-pit 얼라이언스' 결성, ‘정의선號’ 출항 1년, 현대차그룹 ‘미래 항로’ 그렸다, 현대차 ‘H-온드림’ 10년간 일자리 3800개 창출, 현대차 정몽구 재단 'H-온드림' 10주년...사회적일자리 3816개 ..., 현대트랜시스, 이앤알과 '친환경 재생가죽' 연구개발 MOU 체결, "한국은 슈퍼차저 아니라 'E-PIT'"···현대차·6개 충전사업자 손..., 현대차 대형 전기 SUV '세븐' 콘셉트카 공개..아이오닉 3번째 라..., 현대차그룹 ‘E-pit 얼라이언스’ 결성…국내 충전사업자 6개사 참여, 현대차그룹·정몽구 재단 일자리 3816개 창출..'H-온드림' 성과 공..., 현대차 정몽구 재단 'H-온드림' 10주년...사회적일자리 3816개..., 현대차 아이오닉5·싼타크루즈·GV70 美서 리비안·루시드 넘을까, 아이오닉5, 현대차 전기차 최초로 ‘북미 올해의 차’ 후보 올라, 전기 SUV 탄 현대차·기아, LA 떴다, 현대차, LA오토쇼서 전기 SUV 콘셉트카 '세븐' 첫 공개, 현대차, 아이오닉 대형 SUV 콘셉트카 세븐(SEVEN) 첨단항균기술 ..., "한국은 슈퍼차저 아니라 'E-PIT'"···현대차·6개 충전사업자 손..., 현대차그룹 ‘E-pit 얼라이언스’ 결성…국내 충전사업자 6개사 참여, ‘정의선號’ 출항 1년, 현대차그룹 ‘미래 항로’ 그렸다, 현대차, 전기차 충전 생태계 이끈다…'E-pit 연합' 결성</t>
@@ -7429,19 +7429,19 @@
     <t>현대차 정비업무 전환형 인턴 모집…"우수자 정규직 채용", 현대차 정비업무 전환형 인턴 모집…"우수자 정규직 채용", 현대차, 22일부터 서비스 하이테크 인턴사원 모집, 매출 1000억원 벤처기업 633개사… 총 종사자 현대차그룹보다 많아, 현대차 자율차·로보틱스 40대 임원 대거 약진, 현대차, 22일부터 서비스 하이테크 인턴사원 모집</t>
   </si>
   <si>
-    <t>현대차, 모빌리티 구독 플랫폼 '현대 셀렉션' 제주 진출, 현대차그룹 ‘4만6천개 일자리 약속’…3만명 직접 채용, 현대차 차량구독서비스 '현대 셀렉션' 제주로 확대, 정의선 현대차 회장 "청년일자리 4만6000개 창출", 정의선 "일자리 창출, 현대차의 의무"…3년간 4만6000개 약속, "혁신 기술 한 자리에" 현대차그룹, '오픈 이노베이션 라운지', 현대차, 모빌리티 구독 플랫폼 '현대 셀렉션' 제주 진출, 현대차 차량구독서비스 '현대 셀렉션' 제주로 확대, 레드캡렌터카, 현대차와 제주서 '아이오닉5' 구독서비스 운영, "혁신 기술 한자리에" 현대차그룹 '2021 오픈 이노베이션 라운지', "혁신 기술 한 자리에" 현대차그룹, '오픈 이노베이션 라운지', 레드캡렌터카, 현대차와 제주서 '아이오닉5' 구독서비스 운영, "혁신 기술 한자리에" 현대차그룹 '2021 오픈 이노베이션 라운지', 정의선 현대차 회장 "청년일자리 4만6000개 창출", UAM·자율주행 등 3만명 직접 채용… 청년창업도 전폭 지원[현대차 청..., 정의선 "일자리 4만6천개 창출…청년 더 뽑는 게 현대차의 의무", 현대차 차량구독서비스 '현대 셀렉션' 제주로 확대, 레드캡렌터카, 현대차와 제주서 '아이오닉5' 구독서비스 운영, 현대차그룹 ‘4만6천개 일자리 약속’…3만명 직접 채용, "오토데스크 설계플랫폼서 테슬라·현대차·폭스바겐…미래 혁신기술 그려냈...., 현대차, 3만명 직접채용 등 일자리 4만6000개 늘린다, 현대차 차량구독서비스 '현대 셀렉션' 제주로 확대, 현대차-2022년 최선호주: 한편의 드라마를 준비한다, 2022년 변화를 위한 시도들, 윤곽을 드러낼 것, 해외 전기차 생산거점 확보는 주가의 강한 촉매제, 2022년 자동차 업종 밸류에이션의 새로운 손님: 로보택시, "광주서 '캐스퍼' 모르면 간첩인디"…시민 자랑된 현대 SUV, 현대차에 40대 임원 대거 약진 왜?, 김총리 만난 정의선 현대차 회장 "3년간 4.6만개 일자리 창출", 정의선 "일자리 4만6천개 창출…청년 더 뽑는 게 현대차의 의무", 김 총리-정의선 22일 회동…현대차, 청년 일자리 4만개 약속할듯, 현대차에 40대 임원 대거 약진 왜?, '혁신 기술 한 자리에'…현대차그룹, '2021 오픈 이노베이션 라운..., 현대차-스타트업 협업한 유망혁신기술 한지리에 모였다, 모빌리티 구독 플랫폼 '현대 셀렉션' 제주 상륙, 현대차, 모빌리티 구독 플랫폼 ‘현대 셀렉션’ 제주 진출, 현대차그룹, 향후 3년 청년일자리 4.6만개 창출…김부겸 "최대규모 감..., 김 총리-정의선 22일 회동…현대차, 청년 일자리 4만개 약속할듯, 김총리 만난 정의선 현대차 회장 "3년간 4.6만개 일자리 창출", 현대차그룹, 직접채용 3만명 등 일자리 4만6000개 만든다, 현대차-스타트업 협업한 유망혁신기술 한지리에 모였다, 현대차와 함께 '청년희망 ON', 현대차, 모빌리티 구독 플랫폼 ‘현대 셀렉션’ 제주 진출, 정의선 현대차 회장 인사말, 안경덕 고용부 장관, 현대차그룹에 '청년고용 응원 멤버십' 증서 수여, "혁신 기술 한 자리에" 현대차그룹, '오픈 이노베이션 라운지', 현대차, 3년간 일자리 4만6000개 만든다…로봇·자율주행 등, 현대차, 3만명 직접채용 등 일자리 4만6000개 늘린다, 현대차와 함께 '청년희망 ON', 정의선 현대차 회장 인사말, 안경덕 고용부 장관, 현대차그룹에 '청년고용 응원 멤버십' 증서 수여, 선루프 조명, 자동충전로봇…현대차 그룹이 그리는 미래차 모습, UAM·자율주행 등 3만명 직접 채용… 청년창업도 전폭 지원[현대차 청...</t>
-  </si>
-  <si>
-    <t>현대차-전기차 라인업 확대. 미래 기술에 대한 주도적 투자, 전동화 전략을 가속화할 전망, 2022년 이슈 (1) 전기차 라인업 확대, 2022년 이슈 (2) 미래차 기술에 대한 주도적 투자, 현대차, 취약계층에 '찾아가는 건강의료서비스' 지원, 현대차 아이오닉5·투싼, '스파이더맨: 노 웨이 홈' 명품 조연 등장, "현대차·기아, 판매증가+밸류 회복으로 내년 반등 전망", 삼성이 앞장선 일감몰아주기 해소... 현대차·SK 등 경쟁입찰 도입 전..., SK, ICT계열 시너지협의회 신설···현대차, 수소전지사업 확대, 현대차 아이오닉5 타는 스파이더맨, 스파이더맨에 '아이오닉 5·투싼' 나온다..현대차-소니 첫 작품, 현대기아차 주가 30% 오를거라고 전망되는 이유는?, 현대차, 미국서 '전기차 생산시기' 일부러 늦추려는 이유는 [車 UP ..., 삼성이 앞장선 일감몰아주기 해소... 현대차·SK 등 경쟁입찰 도입 전..., SK, ICT계열 시너지협의회 신설···현대차, 수소전지사업 확대, 현대차 아이오닉5 타는 스파이더맨, "스파이더맨에 아이오닉 5가?" 현대차-소니픽쳐스 협업 첫 결실, 현대기아차 주가 30% 오를거라고 전망되는 이유는?, 현대차 아이오닉5·투싼, 스파이더맨 시리즈 새 영화에서 깜짝 등장, 현대차 '아이오닉5·투싼' 12월 스파이더맨에 뜬다, 현대차, 부산 소외계층 위해 '찾아가는 건강의료버스' 기부, "현대차·기아, 판매증가+밸류 회복으로 내년 반등 전망", 스파이더맨에 '아이오닉 5·투싼' 나온다..현대차-소니 첫 작품, 현대차 '움직이는 병원' 갖춘 전기버스 부산에 기부, 현대차, 취약계층에 ‘찾아가는 건강의료서비스’, 현대차 아이오닉5·투싼, 스파이더맨 시리즈 새 영화에서 깜짝 등장, 현대차, 미국서 '전기차 생산시기' 일부러 늦추려는 이유는 [車 UP ...</t>
-  </si>
-  <si>
-    <t>현대차-신차 싸이클에 이어 신규 투자 싸이클로, 년도년도 하반기 하반기 인센티브 하락과,년도 하반기 2H22 볼륨 효과 기대, 년도년도 하반기 하반기 투싼 신차 효과 지속 &amp; 내수 매출 성장 예상, 투자의견 매수, 목표주가 28만원 유지, 현대차 ‘H-모빌리티 클래스’ 모집, 현대차 '채용 특전' 미래차 R&amp;D 인재 키운다..700명 선발, 디와이오토 '센서 클리닝'…현대차 무인택시에 장착, '슈퍼카 전시장'서 도요타 제쳤다…중동 경찰들 현대차 탄다, 현대차 'H-모빌리티 클래스' 모집…이공계 700명 선발, 포드 124% 오를 때 현대차는 고작 2%대, 현대차 'H-모빌리티 클래스' 모집…이공계 700명 선발, 현대차, 전기차·자율주행 교육프로그램에 이공계 대학생 700명 선발, 현대모터클럽 사회공헌 ‘드라이브인 무빙 씨어터’ 성료, 현대모터클럽 ‘드라이브인 무빙 씨어터’ 성료, '미래차 인재 양성' 나선 현대차···이공계 700명에 무상 교육, "미래차 인재 양성"…현대차, 2022년 상반기 ‘H-모빌리티 클래스..., 현대케피코, 세계 최대 국제 모터사이클 전시회 EICMA 참가, 현대차, 부품기업 미래차 전환 돕고…사회적 기업가 창업 지원도, 현대차, 전기차·자율주행 교육프로그램에 이공계 대학생 700명 선발</t>
-  </si>
-  <si>
-    <t>LG엔솔·현대ENG… 내년 역대급 IPO 시장 열린다, 현대차-2022년 전망 - 이익 증가 요인과 상쇄 요인, 목표주가 285,000원으로 기존대비 5.0% 하향하나 투자의견 Buy 유지, 투자포인트: 1) 코로나 및 반도체 수급 이슈 개선 2) SUV 및 Genesis 라인업 확대 통한 글로벌 시장 점유율 상승 3) 환율환경, 2022년 영업이익 7.9조원 (+10.5% 전년 대비 증감율) 전망, 현대차-그린 모빌리티의 중심으로, 친환경 물류 시스템의 도입, 수소 트럭 양산 본격화 예정, 2022년 영업이익 7.9조원 전망, 글로벌 신형 전기차 총출동… 현대차, 친환경 미래비전 제시[서울모빌리티..., 현대차 "로보라이드, 내년 봄 서울에 등장", 현대차, 내년 영업익 증가·전기차 점유율 하락…목표가↓-KB, 현대차, 자율주행부터 일상까지 미래 모빌리티 확인, 'K5 아버지'가 드러낸 전기차 포부 "현대차가 새 시대 열 ..., 현대차 아이오닉5 완전 자율주행차 내년 서울서 달린다, "현대차 그린 모빌리티 업고 내년 주가 모멘텀 강화될 것", 현대차 "내년 서울서 자율주행 모빌리티 시범 서비스", '전기차만? 충전소도 경쟁'…현대차 '갯수보다 초고속', "현대차 그린 모빌리티 업고 내년 주가 모멘텀 강화될 것", 현대차 "내년 서울서 자율주행 모빌리티 시범 서비스", 현대차, 내년 영업익 증가·전기차 점유율 하락…목표가↓-KB</t>
-  </si>
-  <si>
-    <t>현대차 아이오닉5 독일서 '올해의 차', 독일차 다 제치고…현대차 아이오닉5 '獨 올해의 차', 현대차 아이오닉5 독일서 '올해의 차', 현대차, LG전자서 디자인인재 영입, 현대차 커넥티드카 서비스 이용하면 서울시 車마일리지 쌓는다, 현대차그룹?서울시, 승용차 마일리지 활성화 위해 손 잡는다, 현대차, 오는 12월2일 기업설명회 개최, 현대차-2022년 전망 : 제네시스 , 디지털과 럭셔리의 상징으로, 제네시스와 SUV 판매증가에 따른 ASP 상승 지속. 글로벌 판매대수는 신흥시장 수요회복 및 인도네시아 공장 및 러시아 공장 가동으로 4.2백만 대(+7%전년 대비 증감율) 예상, 내연기관차 보다 전기차 신모델 출시가 많은 첫해. 미국 시장에 제네시스 브랜드 안착을 위해 디지털 마케팅, 글로벌 업체와의 협업 등 기술 선도 스토리 예상., 경쟁사의 공격적인 EV 전환 계획에 따라 미래차 부분 경쟁우위 평가가 희석 중. 22년도 1분기 에 개최될 CEO Investor Day에서 Top3에 달성을 위한 비전 발표 기대, 현대차, LG전자서 디자인인재 영입, 현대차 커넥티드카 서비스 이용하면 서울시 車마일리지 쌓는다, 현대차, 에어플러그 통째 인수…커넥티드카 '가속', 현대차 아이오닉 5, 자동차 본고장 독일서 ‘2022 올해의 차’ 선..., 현대자동차 아이오닉 5, ‘2022 독일 올해의 차’ 선정, 현대차 '아이오닉 5' 獨서 일냈다..포르쉐 제치고 '올해의 차'로, 현대차, 에어플러그 통째 인수…커넥티드카 '가속', (영상) 현대차 "내년부터 레벨4 자율주행차 서울 도심 달린다", 현대차 '아이오닉 5' 獨서 일냈다..포르쉐 제치고 '올해의 차'로, 현대차 아이오닉 5, 獨 ‘2022 올해의 차’ 선정, 미래 모빌리티 이끌 ‘쌍두마차’는 현대차·기아, 현대차그룹·서울시, 승용차 마일리지 자동 적립 시스템 구축, 현대자동차 아이오닉 5, ‘2022 독일 올해의 차’ 선정, 삼성 ‘지배구조·뉴 삼성’·현대차 ‘기술혁신·세대교체’에 방점, 현대차, 오는 12월2일 기업설명회 개최, 현대차그룹?서울시, 승용차 마일리지 활성화 위해 손 잡는다</t>
+    <t>현대차, 모빌리티 구독 플랫폼 '현대 셀렉션' 제주 진출, 현대차그룹 ‘4만6천개 일자리 약속’…3만명 직접 채용, 현대차 차량구독서비스 '현대 셀렉션' 제주로 확대, 정의선 현대차 회장 "청년일자리 4만6000개 창출", 정의선 "일자리 창출, 현대차의 의무"…3년간 4만6000개 약속, "혁신 기술 한 자리에" 현대차그룹, '오픈 이노베이션 라운지', 현대차, 모빌리티 구독 플랫폼 '현대 셀렉션' 제주 진출, 현대차 차량구독서비스 '현대 셀렉션' 제주로 확대, 레드캡렌터카, 현대차와 제주서 '아이오닉5' 구독서비스 운영, "혁신 기술 한자리에" 현대차그룹 '2021 오픈 이노베이션 라운지', "혁신 기술 한 자리에" 현대차그룹, '오픈 이노베이션 라운지', 레드캡렌터카, 현대차와 제주서 '아이오닉5' 구독서비스 운영, "혁신 기술 한자리에" 현대차그룹 '2021 오픈 이노베이션 라운지', 정의선 현대차 회장 "청년일자리 4만6000개 창출", UAM·자율주행 등 3만명 직접 채용… 청년창업도 전폭 지원[현대차 청..., 정의선 "일자리 4만6천개 창출…청년 더 뽑는 게 현대차의 의무", 현대차 차량구독서비스 '현대 셀렉션' 제주로 확대, 레드캡렌터카, 현대차와 제주서 '아이오닉5' 구독서비스 운영, 현대차그룹 ‘4만6천개 일자리 약속’…3만명 직접 채용, "오토데스크 설계플랫폼서 테슬라·현대차·폭스바겐…미래 혁신기술 그려냈...., 현대차, 3만명 직접채용 등 일자리 4만6000개 늘린다, 현대차 차량구독서비스 '현대 셀렉션' 제주로 확대, 2022년 최선호주: 한편의 드라마를 준비한다, 2022년 변화를 위한 시도들, 윤곽을 드러낼 것, 해외 전기차 생산거점 확보는 주가의 강한 촉매제, 2022년 자동차 업종 밸류에이션의 새로운 손님: 로보택시, "광주서 '캐스퍼' 모르면 간첩인디"…시민 자랑된 현대 SUV, 현대차에 40대 임원 대거 약진 왜?, 김총리 만난 정의선 현대차 회장 "3년간 4.6만개 일자리 창출", 정의선 "일자리 4만6천개 창출…청년 더 뽑는 게 현대차의 의무", 김 총리-정의선 22일 회동…현대차, 청년 일자리 4만개 약속할듯, 현대차에 40대 임원 대거 약진 왜?, '혁신 기술 한 자리에'…현대차그룹, '2021 오픈 이노베이션 라운..., 스타트업 협업한 유망혁신기술 한지리에 모였다, 모빌리티 구독 플랫폼 '현대 셀렉션' 제주 상륙, 현대차, 모빌리티 구독 플랫폼 ‘현대 셀렉션’ 제주 진출, 현대차그룹, 향후 3년 청년일자리 4.6만개 창출…김부겸 "최대규모 감..., 김 총리-정의선 22일 회동…현대차, 청년 일자리 4만개 약속할듯, 김총리 만난 정의선 현대차 회장 "3년간 4.6만개 일자리 창출", 현대차그룹, 직접채용 3만명 등 일자리 4만6000개 만든다, 스타트업 협업한 유망혁신기술 한지리에 모였다, 현대차와 함께 '청년희망 ON', 현대차, 모빌리티 구독 플랫폼 ‘현대 셀렉션’ 제주 진출, 정의선 현대차 회장 인사말, 안경덕 고용부 장관, 현대차그룹에 '청년고용 응원 멤버십' 증서 수여, "혁신 기술 한 자리에" 현대차그룹, '오픈 이노베이션 라운지', 현대차, 3년간 일자리 4만6000개 만든다…로봇·자율주행 등, 현대차, 3만명 직접채용 등 일자리 4만6000개 늘린다, 현대차와 함께 '청년희망 ON', 정의선 현대차 회장 인사말, 안경덕 고용부 장관, 현대차그룹에 '청년고용 응원 멤버십' 증서 수여, 선루프 조명, 자동충전로봇…현대차 그룹이 그리는 미래차 모습, UAM·자율주행 등 3만명 직접 채용… 청년창업도 전폭 지원[현대차 청...</t>
+  </si>
+  <si>
+    <t>전기차 라인업 확대. 미래 기술에 대한 주도적 투자, 전동화 전략을 가속화할 전망, 2022년 이슈 (1) 전기차 라인업 확대, 2022년 이슈 (2) 미래차 기술에 대한 주도적 투자, 현대차, 취약계층에 '찾아가는 건강의료서비스' 지원, 현대차 아이오닉5·투싼, '스파이더맨: 노 웨이 홈' 명품 조연 등장, "현대차·기아, 판매증가+밸류 회복으로 내년 반등 전망", 삼성이 앞장선 일감몰아주기 해소... 현대차·SK 등 경쟁입찰 도입 전..., SK, ICT계열 시너지협의회 신설···현대차, 수소전지사업 확대, 현대차 아이오닉5 타는 스파이더맨, 스파이더맨에 '아이오닉 5·투싼' 나온다..현대차-소니 첫 작품, 현대기아차 주가 30% 오를거라고 전망되는 이유는?, 현대차, 미국서 '전기차 생산시기' 일부러 늦추려는 이유는 [車 UP ..., 삼성이 앞장선 일감몰아주기 해소... 현대차·SK 등 경쟁입찰 도입 전..., SK, ICT계열 시너지협의회 신설···현대차, 수소전지사업 확대, 현대차 아이오닉5 타는 스파이더맨, "스파이더맨에 아이오닉 5가?" 현대차-소니픽쳐스 협업 첫 결실, 현대기아차 주가 30% 오를거라고 전망되는 이유는?, 현대차 아이오닉5·투싼, 스파이더맨 시리즈 새 영화에서 깜짝 등장, 현대차 '아이오닉5·투싼' 12월 스파이더맨에 뜬다, 현대차, 부산 소외계층 위해 '찾아가는 건강의료버스' 기부, "현대차·기아, 판매증가+밸류 회복으로 내년 반등 전망", 스파이더맨에 '아이오닉 5·투싼' 나온다..현대차-소니 첫 작품, 현대차 '움직이는 병원' 갖춘 전기버스 부산에 기부, 현대차, 취약계층에 ‘찾아가는 건강의료서비스’, 현대차 아이오닉5·투싼, 스파이더맨 시리즈 새 영화에서 깜짝 등장, 현대차, 미국서 '전기차 생산시기' 일부러 늦추려는 이유는 [車 UP ...</t>
+  </si>
+  <si>
+    <t>신차 싸이클에 이어 신규 투자 싸이클로, 년도년도 하반기 하반기 인센티브 하락과,년도 하반기 2H22 볼륨 효과 기대, 년도년도 하반기 하반기 투싼 신차 효과 지속 &amp; 내수 매출 성장 예상, 투자의견 매수, 목표주가 28만원 유지, 현대차 ‘H-모빌리티 클래스’ 모집, 현대차 '채용 특전' 미래차 R&amp;D 인재 키운다..700명 선발, 디와이오토 '센서 클리닝'…현대차 무인택시에 장착, '슈퍼카 전시장'서 도요타 제쳤다…중동 경찰들 현대차 탄다, 현대차 'H-모빌리티 클래스' 모집…이공계 700명 선발, 포드 124% 오를 때 현대차는 고작 2%대, 현대차 'H-모빌리티 클래스' 모집…이공계 700명 선발, 현대차, 전기차·자율주행 교육프로그램에 이공계 대학생 700명 선발, 현대모터클럽 사회공헌 ‘드라이브인 무빙 씨어터’ 성료, 현대모터클럽 ‘드라이브인 무빙 씨어터’ 성료, '미래차 인재 양성' 나선 현대차···이공계 700명에 무상 교육, "미래차 인재 양성"…현대차, 2022년 상반기 ‘H-모빌리티 클래스..., 현대케피코, 세계 최대 국제 모터사이클 전시회 EICMA 참가, 현대차, 부품기업 미래차 전환 돕고…사회적 기업가 창업 지원도, 현대차, 전기차·자율주행 교육프로그램에 이공계 대학생 700명 선발</t>
+  </si>
+  <si>
+    <t>LG엔솔·현대ENG… 내년 역대급 IPO 시장 열린다, 2022년 전망 - 이익 증가 요인과 상쇄 요인, 목표주가 285,000원으로 기존대비 5.0% 하향하나 투자의견 Buy 유지, 투자포인트: 1) 코로나 및 반도체 수급 이슈 개선 2) SUV 및 Genesis 라인업 확대 통한 글로벌 시장 점유율 상승 3) 환율환경, 2022년 영업이익 7.9조원 (+10.5% 전년 대비 증감율) 전망, 그린 모빌리티의 중심으로, 친환경 물류 시스템의 도입, 수소 트럭 양산 본격화 예정, 2022년 영업이익 7.9조원 전망, 글로벌 신형 전기차 총출동… 현대차, 친환경 미래비전 제시[서울모빌리티..., 현대차 "로보라이드, 내년 봄 서울에 등장", 현대차, 내년 영업익 증가·전기차 점유율 하락…목표가↓-KB, 현대차, 자율주행부터 일상까지 미래 모빌리티 확인, 'K5 아버지'가 드러낸 전기차 포부 "현대차가 새 시대 열 ..., 현대차 아이오닉5 완전 자율주행차 내년 서울서 달린다, "현대차 그린 모빌리티 업고 내년 주가 모멘텀 강화될 것", 현대차 "내년 서울서 자율주행 모빌리티 시범 서비스", '전기차만? 충전소도 경쟁'…현대차 '갯수보다 초고속', "현대차 그린 모빌리티 업고 내년 주가 모멘텀 강화될 것", 현대차 "내년 서울서 자율주행 모빌리티 시범 서비스", 현대차, 내년 영업익 증가·전기차 점유율 하락…목표가↓-KB</t>
+  </si>
+  <si>
+    <t>현대차 아이오닉5 독일서 '올해의 차', 독일차 다 제치고…현대차 아이오닉5 '獨 올해의 차', 현대차 아이오닉5 독일서 '올해의 차', 현대차, LG전자서 디자인인재 영입, 현대차 커넥티드카 서비스 이용하면 서울시 車마일리지 쌓는다, 현대차그룹?서울시, 승용차 마일리지 활성화 위해 손 잡는다, 현대차, 오는 12월2일 기업설명회 개최, 2022년 전망 : 제네시스 , 디지털과 럭셔리의 상징으로, 제네시스와 SUV 판매증가에 따른 ASP 상승 지속. 글로벌 판매대수는 신흥시장 수요회복 및 인도네시아 공장 및 러시아 공장 가동으로 4.2백만 대(+7%전년 대비 증감율) 예상, 내연기관차 보다 전기차 신모델 출시가 많은 첫해. 미국 시장에 제네시스 브랜드 안착을 위해 디지털 마케팅, 글로벌 업체와의 협업 등 기술 선도 스토리 예상., 경쟁사의 공격적인 EV 전환 계획에 따라 미래차 부분 경쟁우위 평가가 희석 중. 22년도 1분기 에 개최될 CEO Investor Day에서 Top3에 달성을 위한 비전 발표 기대, 현대차, LG전자서 디자인인재 영입, 현대차 커넥티드카 서비스 이용하면 서울시 車마일리지 쌓는다, 현대차, 에어플러그 통째 인수…커넥티드카 '가속', 현대차 아이오닉 5, 자동차 본고장 독일서 ‘2022 올해의 차’ 선..., 현대자동차 아이오닉 5, ‘2022 독일 올해의 차’ 선정, 현대차 '아이오닉 5' 獨서 일냈다..포르쉐 제치고 '올해의 차'로, 현대차, 에어플러그 통째 인수…커넥티드카 '가속', (영상) 현대차 "내년부터 레벨4 자율주행차 서울 도심 달린다", 현대차 '아이오닉 5' 獨서 일냈다..포르쉐 제치고 '올해의 차'로, 현대차 아이오닉 5, 獨 ‘2022 올해의 차’ 선정, 미래 모빌리티 이끌 ‘쌍두마차’는 현대차·기아, 현대차그룹·서울시, 승용차 마일리지 자동 적립 시스템 구축, 현대자동차 아이오닉 5, ‘2022 독일 올해의 차’ 선정, 삼성 ‘지배구조·뉴 삼성’·현대차 ‘기술혁신·세대교체’에 방점, 현대차, 오는 12월2일 기업설명회 개최, 현대차그룹?서울시, 승용차 마일리지 활성화 위해 손 잡는다</t>
   </si>
   <si>
     <t>삼성·현대차·LG 등이 만드는 청년일자리 '18만개', 현대차, 모빌리티 구독 플랫폼 제주 진출, ‘현대차가 파는 중고차’ 이번엔 살 수 있을까…협상 재시작, ‘현대차가 파는 중고차’ 이번엔 살 수 있을까…협상 재시작</t>
@@ -7492,7 +7492,7 @@
     <t>현대자동차, ‘2022 싼타페’ 출시, 피터 슈라이어 디자인 담당 사장 교체...현대차그룹 이번주 임원인사, 현대차 R&amp;D·디자인 수장 비어만·슈라이어 물러날 듯, 현대차도 쇄신 인사···R&amp;D·디자인 수장 교체, 현대자동차, ‘2022 싼타페’ 출시, 피터 슈라이어 디자인 담당 사장 교체...현대차그룹 이번주 임원인사, 현대차 R&amp;D·디자인 수장 비어만·슈라이어 물러날 듯, 현대차도 쇄신 인사···R&amp;D·디자인 수장 교체</t>
   </si>
   <si>
-    <t>중고차 시장, "못 믿어" 소비자 대다수인데…현대차 진출 또 물 건너가..., 현대차 정몽구 재단 ‘온드림스쿨’ 10년의 결실, 현대차그룹, 사회복지공동모금회에 이웃돕기 성금 250억원 전달, 현대차그룹, 이웃돕기 성금 250억원 전달···19년간 3,340억원 ..., 현대차정몽구재단, 10년간 농·산·어촌 교육에 180억 투입, 현대차 울산은 '특근'하는데…180도 다른 전주공장 상황, 현대차그룹 이웃돕기 성금 250억원 전달, 현대차·기아 印시장 급성장…18년만에 中 판매량 넘어섰다, 현대차 정몽구 재단 ‘온드림스쿨’ 10년의 결실, 현대차정몽구재단, 10년간 농·산·어촌 교육에 180억 투입, 현대차그룹, 사회복지공동모금회에 이웃돕기 성금 250억원 전달, 현대차그룹 이웃돕기 성금 250억원 전달, 현대차그룹, 이웃돕기 성금 250억원 전달, 현대차그룹 250억·포스코그룹 100억 '이웃돕기 성금', LG-협동로봇 확대·현대車-물류로봇 선점·삼성-로봇사업팀 승격, 현대차그룹 250억·포스코그룹 100억 '이웃돕기 성금', 현대자동차그룹, 임원인사 임박…외국인 경영진 교체?, 현대차·기아 印시장 급성장…18년만에 中 판매량 넘어섰다, 현대차, 주요 섬 찾아가 방문 정비 서비스, 현대차-년도년도 2분기 4분기 프리뷰: 생산회복 지연에도 영업이익 기대 부합할 것, 판매부진에도 년도년도 2분기 4분기 영업이익 (2.0조원 예상)은 시장 컨센서스를 0.9% 상회할 것, 투자포인트: 1) 판매 회복, 2) 제한적인 대당 공헌이익 감소, 3) 중고차 가격 상승, 리스크요인: 1) 재고부족, 2) 원화가치 절상, 3) 경쟁 심화, 현대ENG, 증권신고서 제출…“내년 2월 코스피 상장 계획”, 현대커머셜, ‘대출 유동화’로 1800억 영업자금 확보 이유..., 현대차, 전국 주요 섬 지역 상용차 ‘특별 케어 서비스’ 실시, 현대ENG, 증권신고서 제출…“내년 2월 코스피 상장 계획”, 현대차, 백령도 등 섬 지역 상용차 방문 점검, 현대차, 전국 주요 섬 지역 상용차 ‘특별 케어 서비스’ 실시, 현대차, 백령도 등 섬 지역 상용차 방문 점검, 현대차그룹, 이웃돕기 성금 250억원 전달, 현대차그룹 연말 이웃돕기 성금 250억..19년간 3340억 기탁, 현대차 정몽구 재단, 10년간 농산어촌 교육에 180억 투입…3만50..., 현대차 정몽구 재단 ‘온드림스쿨’ 10년의 결실, 현대차, 섬 지역 ‘상용차 고객’ 찾아간다, 현대차, 주요 섬 찾아가 방문 정비 서비스, 현대차그룹, 사회복지공동모금회에 이웃돕기 성금 250억원 전달, 현대차, 섬 지역 ‘상용차 고객’ 찾아간다</t>
+    <t>중고차 시장, "못 믿어" 소비자 대다수인데…현대차 진출 또 물 건너가..., 현대차 정몽구 재단 ‘온드림스쿨’ 10년의 결실, 현대차그룹, 사회복지공동모금회에 이웃돕기 성금 250억원 전달, 현대차그룹, 이웃돕기 성금 250억원 전달···19년간 3,340억원 ..., 현대차정몽구재단, 10년간 농·산·어촌 교육에 180억 투입, 현대차 울산은 '특근'하는데…180도 다른 전주공장 상황, 현대차그룹 이웃돕기 성금 250억원 전달, 현대차·기아 印시장 급성장…18년만에 中 판매량 넘어섰다, 현대차 정몽구 재단 ‘온드림스쿨’ 10년의 결실, 현대차정몽구재단, 10년간 농·산·어촌 교육에 180억 투입, 현대차그룹, 사회복지공동모금회에 이웃돕기 성금 250억원 전달, 현대차그룹 이웃돕기 성금 250억원 전달, 현대차그룹, 이웃돕기 성금 250억원 전달, 현대차그룹 250억·포스코그룹 100억 '이웃돕기 성금', LG-협동로봇 확대·현대車-물류로봇 선점·삼성-로봇사업팀 승격, 현대차그룹 250억·포스코그룹 100억 '이웃돕기 성금', 현대자동차그룹, 임원인사 임박…외국인 경영진 교체?, 현대차·기아 印시장 급성장…18년만에 中 판매량 넘어섰다, 현대차, 주요 섬 찾아가 방문 정비 서비스, 년도년도 2분기 4분기 프리뷰: 생산회복 지연에도 영업이익 기대 부합할 것, 판매부진에도 년도년도 2분기 4분기 영업이익 (2.0조원 예상)은 시장 컨센서스를 0.9% 상회할 것, 투자포인트: 1) 판매 회복, 2) 제한적인 대당 공헌이익 감소, 3) 중고차 가격 상승, 리스크요인: 1) 재고부족, 2) 원화가치 절상, 3) 경쟁 심화, 현대ENG, 증권신고서 제출…“내년 2월 코스피 상장 계획”, 현대커머셜, ‘대출 유동화’로 1800억 영업자금 확보 이유..., 현대차, 전국 주요 섬 지역 상용차 ‘특별 케어 서비스’ 실시, 현대ENG, 증권신고서 제출…“내년 2월 코스피 상장 계획”, 현대차, 백령도 등 섬 지역 상용차 방문 점검, 현대차, 전국 주요 섬 지역 상용차 ‘특별 케어 서비스’ 실시, 현대차, 백령도 등 섬 지역 상용차 방문 점검, 현대차그룹, 이웃돕기 성금 250억원 전달, 현대차그룹 연말 이웃돕기 성금 250억..19년간 3340억 기탁, 현대차 정몽구 재단, 10년간 농산어촌 교육에 180억 투입…3만50..., 현대차 정몽구 재단 ‘온드림스쿨’ 10년의 결실, 현대차, 섬 지역 ‘상용차 고객’ 찾아간다, 현대차, 주요 섬 찾아가 방문 정비 서비스, 현대차그룹, 사회복지공동모금회에 이웃돕기 성금 250억원 전달, 현대차, 섬 지역 ‘상용차 고객’ 찾아간다</t>
   </si>
   <si>
     <t>현대차, 최우수 엔지니어 ‘그랜드마스터’ 17명 선발, 현대차, 생산회복 지연에도 4분기 영업이익 기대 부합할 것-KB, 현대차, 4분기 생산 차질에도 선방한 듯…KB證 “영업이익 기대 부합”..., 한국타이어 장기 파업에…현대차 등 돌렸다, 일본차 비켜! 현대차 인니공장 내년 1월 가동, 한국타이어 장기 파업에…현대차 등 돌렸다, 현대차, 최우수 엔지니어 ‘그랜드마스터’ 17명 선발, 일본차 비켜! 현대차 인니공장 내년 1월 가동, 현대차, 최우수 엔지니어 17명에 '그랜드마스터' 자격 부여, 현대차, 최우수 엔지니어 17명에 '그랜드마스터' 자격 부여, 현대차 정비장인 17명 '그랜드마스터' 자격 부여..순금패 포상, 현대자동차, 우수 인재는 특별 성과급…집 주변서 일하는 '거점 오피스'..., 글로벌 수소차 시장 연평균 57% 성장 전망…현대차가 주도, 현대차 ‘그랜드마스터 테크 페스타’ 개최…“블루핸즈 기술인력 양성”, 무노조 깨진 '스타벅스' 강성 노조 택한 '현대차', 현대모터클럽 ‘온택트’ 송년행사 성료, 현대차, 4분기 생산회복 지연에도 영업익 기대치 부합 예상-KB, 12년만의 판매량 최저 위기…현대차·기아, 왜 中서 외면당하나, 현대차, 최우수 엔지니어 17명 선발 '그랜드마스터' 부여, 현대차, 최우수 엔지니어 17명에 '그랜드마스터' 자격 부여, 현대모터클럽 ‘온택트’ 송년행사 성료, 현대차, 이웃돕기 성금 250억...19년간 3340억, 현대차, 생산회복 지연에도 4분기 영업이익 기대 부합할 것-KB</t>
@@ -7555,7 +7555,7 @@
     <t>삼성전자 '십만전자' 가능…현대차·네이버 기세등등, 니로HEV 밀고, 아이오닉5·EV6 끌고... 현대차그룹 친환경차 수출..., 현대차·기아 연간 친환경차 수출 30만대 첫 돌파, 새해 맞이 드론쇼 개최한 현대차, 드론 600여대로 희망 메시지, "니로·아이오닉5 효과"…현대차·기아, 친환경차 수출 첫 30만대 돌..., 현대차그룹 친환경차 수출 첫 30만대 돌파</t>
   </si>
   <si>
-    <t>현대자동차, 정의선·장재훈 각자 대표 체제로, 현대차, 2021년 389만 981대 판매…전년比 3.9%↑, '7전 8기' 현대차·기아…올해 판매 목표 12%↑, 코로나 이전 복귀, 현대차·애경·OCI, 메타버스 시무식, 정의선 현대차그룹 회장 신년 메시지, 정의선 현대차 회장 "올해 로봇 상용화", 작년 선방 현대·기아차 "올 판매 12% 늘릴 것", '메타버스 신년회' 코로나에도 현대차 임직원 수천명 모였다, 전세계 현대차 직원 4,000명 ‘메타버스 신년회’, 현대차·기아 "전기차 등 新車 가속… 올 747만대 판매 목표", 이게 '아이오닉6'라고?…현대차가 작심하고 만든 신형 전기차, 현대차 아산공장, 1월 생산 중단 이유?…"전기차 생산 위한 설비 공사..., 차량용 반도체 공급난에도…현대차·기아 실적 '선방', 현대자동차, 정의선·장재훈 각자 대표 체제로, 현대차 하언태 사장 사임…정의선·장재훈 2인 대표 체제로, 삼성 '모빌리티' 현대차 '로봇'…기술융합 미래 연다, 송윤화 카123제스퍼 대표 "현대차와 국내車 구독서비스 시장 개척", 현대차 노조 “정년 연장·정규직 충원해야”, 현대차·기아 "올해 글로벌 판매목표 747만3000대", 오미크론 난리인데..전세계 임직원 만난 '현대차그룹 파크' 뭐길래, '메타버스 신년회' 코로나에도 현대차 임직원 수천명 모였다, 현대차·롯데·포스코 “미래위한 혁신, 조직쇄신 집중해야”, 친환경차 전진기지, 현대차 체코 공장, 현대차 점유율 역전극 비결은 '車반도체 공수작전', 이게 '아이오닉6'라고?…현대차가 작심하고 만든 신형 전기차, 현대차, 올해 432만대 글로벌 판매 목표, 현대차, 작년 누적판매량 390만대…전년비 3.9%↑, 현대차 "올해 자동차 판매목표 432만대", '메타버스 신년회' 코로나에도 현대차 임직원 수천명 모였다, 현대차·롯데·포스코 “미래위한 혁신, 조직쇄신 집중해야”, 친환경차 전진기지, 현대차 체코 공장, 현대차 점유율 역전극 비결은 '車반도체 공수작전', 이게 '아이오닉6'라고?…현대차가 작심하고 만든 신형 전기차, 현대차, 올해 432만대 글로벌 판매 목표, 현대차 "올해 자동차 판매목표 432만대", 현대차-UAM 모빌리티 기업으로 진화, 22년 물량 회복 전망, 22년까지 지속될 신차 효과, 오미크론 난리인데..전세계 임직원 만난 '현대차그룹 파크' 뭐길래, 정의선 현대차그룹 회장 “가능성을 고객의 일상으로”, 메타버스 등장한 정의선 현대차 회장…"가능성을 일상으로 실현", 정의선 현대차그룹 회장 신년 메시지, 정의선 현대차 회장 "신기술이 고객의 일상으로 전환되는 한해", 정의선 현대차그룹 회장 “가능성을 고객의 일상으로”, 정의선 현대차그룹 회장 신년 메시지, 메타버스 등장한 정의선 현대차 회장…"가능성을 일상으로 실현", 바이든·시진핑이 타는 G80 전기차, 현대차 ‘이 팀’이 준비한다[뒷북..., 정의선 현대차 회장 "신기술이 고객의 일상으로 전환되는 한해", 속도 내는 에어택시 상용화…현대차·롯데·한화 ‘3파전’, 현대차·기아, 7년 내 모든 상용차에 수소연료 심장 이식 목표, 현대차, 하언태 대표 사임…정의선·장재훈 각자대표로 변경</t>
+    <t>현대자동차, 정의선·장재훈 각자 대표 체제로, 현대차, 2021년 389만 981대 판매…전년比 3.9%↑, '7전 8기' 현대차·기아…올해 판매 목표 12%↑, 코로나 이전 복귀, 현대차·애경·OCI, 메타버스 시무식, 정의선 현대차그룹 회장 신년 메시지, 정의선 현대차 회장 "올해 로봇 상용화", 작년 선방 현대·기아차 "올 판매 12% 늘릴 것", '메타버스 신년회' 코로나에도 현대차 임직원 수천명 모였다, 전세계 현대차 직원 4,000명 ‘메타버스 신년회’, 현대차·기아 "전기차 등 新車 가속… 올 747만대 판매 목표", 이게 '아이오닉6'라고?…현대차가 작심하고 만든 신형 전기차, 현대차 아산공장, 1월 생산 중단 이유?…"전기차 생산 위한 설비 공사..., 차량용 반도체 공급난에도…현대차·기아 실적 '선방', 현대자동차, 정의선·장재훈 각자 대표 체제로, 현대차 하언태 사장 사임…정의선·장재훈 2인 대표 체제로, 삼성 '모빌리티' 현대차 '로봇'…기술융합 미래 연다, 송윤화 카123제스퍼 대표 "현대차와 국내車 구독서비스 시장 개척", 현대차 노조 “정년 연장·정규직 충원해야”, 현대차·기아 "올해 글로벌 판매목표 747만3000대", 오미크론 난리인데..전세계 임직원 만난 '현대차그룹 파크' 뭐길래, '메타버스 신년회' 코로나에도 현대차 임직원 수천명 모였다, 현대차·롯데·포스코 “미래위한 혁신, 조직쇄신 집중해야”, 친환경차 전진기지, 현대차 체코 공장, 현대차 점유율 역전극 비결은 '車반도체 공수작전', 이게 '아이오닉6'라고?…현대차가 작심하고 만든 신형 전기차, 현대차, 올해 432만대 글로벌 판매 목표, 현대차, 작년 누적판매량 390만대…전년비 3.9%↑, 현대차 "올해 자동차 판매목표 432만대", '메타버스 신년회' 코로나에도 현대차 임직원 수천명 모였다, 현대차·롯데·포스코 “미래위한 혁신, 조직쇄신 집중해야”, 친환경차 전진기지, 현대차 체코 공장, 현대차 점유율 역전극 비결은 '車반도체 공수작전', 이게 '아이오닉6'라고?…현대차가 작심하고 만든 신형 전기차, 현대차, 올해 432만대 글로벌 판매 목표, 현대차 "올해 자동차 판매목표 432만대", UAM 모빌리티 기업으로 진화, 22년 물량 회복 전망, 22년까지 지속될 신차 효과, 오미크론 난리인데..전세계 임직원 만난 '현대차그룹 파크' 뭐길래, 정의선 현대차그룹 회장 “가능성을 고객의 일상으로”, 메타버스 등장한 정의선 현대차 회장…"가능성을 일상으로 실현", 정의선 현대차그룹 회장 신년 메시지, 정의선 현대차 회장 "신기술이 고객의 일상으로 전환되는 한해", 정의선 현대차그룹 회장 “가능성을 고객의 일상으로”, 정의선 현대차그룹 회장 신년 메시지, 메타버스 등장한 정의선 현대차 회장…"가능성을 일상으로 실현", 바이든·시진핑이 타는 G80 전기차, 현대차 ‘이 팀’이 준비한다[뒷북..., 정의선 현대차 회장 "신기술이 고객의 일상으로 전환되는 한해", 속도 내는 에어택시 상용화…현대차·롯데·한화 ‘3파전’, 현대차·기아, 7년 내 모든 상용차에 수소연료 심장 이식 목표, 현대차, 하언태 대표 사임…정의선·장재훈 각자대표로 변경</t>
   </si>
   <si>
     <t>현대차, 물량 회복과 UAM 기대감, '역시 삼성과 현대', 해외 건설시장 수주 1~4위 휩쓸었다, 현대차그룹, 올해 목표 달성 열쇠는 '생산 정상화'-유진, 코스피·코스닥 상승 출발, 현대차·기아 동반 오름세, 수출이 살린 '현대차·기아' 막판 뒤집기 '르노삼성'..쌍·쉐만 울상, 작년 선방한 현대차·기아, 올해 10% 이상 더 판다, "백악관이 최대 변수"…삼성·현대 왜 워싱턴으로 가나, 현대차·기아 美서 5년만에 판매 신기록..비결 3가지는?, 에스피지, 로봇 핵심 감속기 가동률 100%…삼성·LG·현대차..., 로봇이 세배하고 마당놀이를? 현대차그룹, 신년 광고 ‘눈길’, 로봇이 세배에 사물놀이까지...신기술로 희망 전한 현대차그룹, 로봇이 세배하고 춤추네?…현대차 새해 광고 '눈길', 현대차·기아 친환경차 질주... 작년 국내서 22만대 팔았다, (영상)현대차·기아, `글로벌·친환경`으로 `반도체 부족` 넘는다, (영상)현대차·기아, `글로벌·친환경`으로 `반도체 부족` 넘는다, 현대차그룹 계열에서 현대종합설계 떼낸다, 로봇이 세배하고 마당놀이를? 현대차그룹, 신년 광고 ‘눈길’</t>
@@ -7564,7 +7564,7 @@
     <t>현대차그룹, 작년 美서 ‘역대 최다’ 149만대 팔았다, 2018년부터 핵심 전략 분야로…현대차그룹 ‘로보틱스에 진심’, 2018년부터 이미 핵심전략 분야로…현대차그룹의 ‘편안한 삶’ 제공 의..., "車 타고 메타버스로"…현대차, 미래 로보틱스 비전 공개 [CES 2..., 美판매 호조 현대차·기아 매수 몰려, 로보틱스 비전 공개…정의선 "인류에 기여, 이것이 현대차의 목적", 현대차그룹 美 역대 최다 판매 "148만대 이상 팔았다"(종합), 현대차·기아, 美서 혼다 제쳤다…작년 149만대 판매 '톱5', 정의선 현대차그룹 회장 “모든 사물에 대한..., 현대차·기아, 달린다…美 판매량 증가·CES 참여 호재, 현대차·기아, 美 판매 호조에 CES 효과까지...2% 강세, 신차 대기 줄섰고 반도체 공급난 풀려간다…현대차·기아 강세, 현대차그룹, 작년 미국서 149만여대 팔았다…“역대 최다”, 현대차의 車없는 미래, 이동한계 극복 '메타모빌리티' 공개, 제네시스 인기에···현대차, 美서 혼다 추월, 현대차그룹, 작년 美서 ‘역대 최다’ 149만대 팔았다, "車 타고 메타버스로"…현대차, 미래 로보틱스 비전 공개 [CES 2..., 로보틱스 비전 공개…정의선 "인류에 기여, 이것이 현대차의 목적", "이동의 고정관념을 깼다" 현대차 새 로봇들 대거 공..., 정의선 회장 "현대차 로보틱스 , 인류 이동 자유롭게..., 삼전 LG디플 현대차…5일 개막 'CES 2022' 효과 보나, 현대차그룹 美 역대 최다 판매 "148만대 이상 팔았다"(종합), 현대차·기아 동반 상승…지난해 美 판매 신기록에 CES도 긍정적 영향, 반도체 못 구해 공장 문닫은 현대차, 車반도체 내재화 진행 [2022 ..., "이동의 고정관념을 깼다" 현대차 새 로봇들 대거 ..., 車 대신 로봇만 대거 전시한 현대차, 현대차그룹, 혼다 제치고 美 판매 톱5 올랐다, 현대차·기아, '반도체 위기'에도 美 시장서 날았다, "현대차가 달라졌어"…정의선, 자동차 대신 20번이나 외친 단어는, 현대차그룹, 작년 미국서 149만여대 팔았다…“역대 최다”, 현대차의 신무기 PnD 모듈, MoT 시대 문을 연..., 현대차의 車없는 미래, 이동한계 극복 '메타모빌리티' 공개, 현대차그룹, 작년 미국서 149만여대 팔았다…“역대 최다”, "현대차가 달라졌어"…정의선, 자동차 대신 20번이나 외친 단어는, 제네시스 인기에···현대차, 美서 혼다 추월, 현대차·기아, '반도체 위기'에도 美 시장서 날았다, 현대차그룹, 혼다 제치고 美 판매 톱5 올랐다, 현대차·기아 동반 상승…지난해 美 판매 신기록에 CES도 긍정적 영향, '35년만에 혼다 넘었다'…현대차·기아, 작년 미국서 역대 최다 판매, 기아 작년 美판매 신기록, 현대차는 19% 증가, 현대차, CES에서 車 지웠다···"로봇이 새 모빌리티", 정의선 회장 "현대차 로보틱스 비전, 인류의 무한한 ..., '車 대신 로봇' 내세운 정의선…현대차 '로봇드림'은 8년전부터, 현대차, 최첨단 로봇 기술 대거 공개···"인간 한계 넘어선다", "모베드·스팟·아틀라스"…현대차, 미래모빌리티 신기술..., 목표 못 채운 현대차·기아…올해는 달릴까, 정의선 회장 "현대차 로보틱스 비전, 인류의 무한한..., 현대차, 미래 로보틱스 비전은 '메타모빌리티', '車 대신 로봇' 내세운 정의선…현대차 '로봇드림'은 8년전부터, "삶의 질 향상 목표"…현대차그룹, 로보틱스 신사업 ..., 현대차, CES에서 車 지웠다···"로봇이 새 모빌리티", 기아 작년 美판매 신기록, 현대차는 19% 증가, "車 타고 메타버스로"…현대차, 미래 로보틱스 비전 공개 [CES 20..., 현대차의 신무기 PnD 모듈, MoT 시대 문을 연..., 현대차·기아, 달린다…美 판매량 증가·CES 참여 호재, "이동의 고정관념을 깼다" 현대차 새 로봇들 대거 공..., 신차 대기 줄섰고 반도체 공급난 풀려간다…현대차·기아 강세, 현대차·기아, 美 판매 호조에 CES 효과까지...2% 강세</t>
   </si>
   <si>
-    <t>현대차그룹 수소청소트럭 캠페인 영상 조회수 1,000만회 돌파, 현대중공업, 현대엔진 지분 100% 290억원에 취득, 현대차가 선보인 최첨단 로보틱스 기술 Pn..., 현대차그룹, ‘디어 마이 히어로’ 영상 조회수 1000만 회 돌파, '현대차 사내벤처 1호 상장사' 오토앤 "종합 모빌리티 플랫폼으로 도..., 현대차 ‘수소청소트럭 영상’ 일주일만에 1000만뷰 돌파, 현대차그룹 수소청소트럭 캠페인 영상 조회수 1,000만회 돌파, 현대중공업, 현대엔진 지분 100% 290억원에 취득, 현대차 사내벤처 '오토앤', 코스닥 상장으로 종합 모빌리티 ..., '현대차 사내벤처 1호 상장사' 오토앤 "종합 모빌리티 플랫폼으로 도..., 현대車 지배구조 개편 빨라지나…불확실성 해소에 글로비스 급등, 현대차가 선보인 최첨단 로보틱스 기술 Pn..., CES 현대차에 인파 몰린 이유…로봇개 군무에 아바타 체험까지, '깜짝등장' 칼라일, 현대차 혁신전략 도우미 급부상, 삼성·현대차·LG 일감몰아주기 규제 피했다..'총수 지분' 지각변동, 현대차그룹, ‘디어 마이 히어로’ 영상 조회수 1000만 회 돌파, 현대차 ‘수소청소트럭 캠페인’ 조회수 1000만 돌파, 위상 달라진 현대차그룹의 ‘두뇌’…“이제 세계가 우리 기술을..., 현대차그룹, ‘디어 마이 히어로’ 영상 조회수 1000만 회 돌파, 현대차 ‘수소청소트럭 캠페인’ 조회수 1000만 돌파, 현대차-CES 2022 - 메타버스 코인 탑승, 메타모빌리티의 탄생, 모빌리티 사업자로서의 정체성 강화, 현대차 사내벤처 '오토앤', 코스닥 상장으로 종합 모빌리티 ..., 삼성·현대차·LG 일감몰아주기 규제 피했다..'총수 지분' 지각변동, ‘로봇개' BTS 노래에 춤추고 스핀 도는 ..., '정의선 회장 지분매각' 현대차그룹 지배구조 개편 신호탄되나, 현대차, CES서 메타모빌리티 선보여…정체성 강화 -한국, 현대차, 메타버스 코인 탑승-한투, "제네시스 GV60 닮았다"…소니 전기차에 현대차 직원들 '술렁' [C..., 현대차-아직은 빡빡한 반도체 수급, 반도체 악재는 부정적이지만, 향후 반전의 가능성으로도 작용, 현대차 21년도 4분기 Review: 영업이익률 4.9% 기록, 컨퍼런스 콜의 주요 내용: 반도체 이슈는 하반기 안정화를 전망 중, 'BTS 노래에 칼군무'···현대차, 로봇개 '탄성' [CES..., 현대차그룹, '수소청소트럭 캠페인' 영상 조회수 1000만회 돌파, 수소 접목한 청소트럭, 이렇게 깨끗하다니…현대차 캠페인 영상 ‘..., 현대차그룹 모베드 ‘김연아 턴’에 “와우!”…로봇개 스팟 화려..., 현대ENG, '암모니아에서 고순도 수소 생산' 사업화 추진, 음악 나오자 춤추는 로봇개 "와우"…현대차 부스 앞엔 30분 대기줄[C..., 현대ENG, 암모니아 분해해 수소 생산하는 사업 추진, 현대차그룹, '디어 마이 히어로' 영상 조회수 1000만회 돌파, 현대차그룹 모베드 ‘김연아 턴’에 “와우!”…로봇개 스팟 화..., 정의선 현대차 회장, CES 첫 데뷔 정기선 현대重 대표 '응원..., BTS 처럼, 김연아 같이...현대차 로보틱스에 탄성, '정의선 회장 지분매각' 현대차그룹 지배구조 개편 신호탄되나, '차 없는 현대차 CES 전시장'…미래 모빌리티로 가득..., BTS 처럼, 김연아 같이...현대차 로보틱스에 탄성, 수소 접목한 청소트럭, 이렇게 깨끗하다니…현대차 캠페인 영상 ..., 현대차그룹 고급차-전기차 나란히 판매량 20만대, 현대차 사내벤처 오토앤 "종합 모빌리티 플랫폼 도약", BTS 노래에 칼군무…현대차 로봇, 관람객 뒤집어놨다 (영상) [CES..., 현대차 ‘수소청소트럭 영상’ 일주일만에 1000만뷰 돌파</t>
+    <t>현대차그룹 수소청소트럭 캠페인 영상 조회수 1,000만회 돌파, 현대중공업, 현대엔진 지분 100% 290억원에 취득, 현대차가 선보인 최첨단 로보틱스 기술 Pn..., 현대차그룹, ‘디어 마이 히어로’ 영상 조회수 1000만 회 돌파, '현대차 사내벤처 1호 상장사' 오토앤 "종합 모빌리티 플랫폼으로 도..., 현대차 ‘수소청소트럭 영상’ 일주일만에 1000만뷰 돌파, 현대차그룹 수소청소트럭 캠페인 영상 조회수 1,000만회 돌파, 현대중공업, 현대엔진 지분 100% 290억원에 취득, 현대차 사내벤처 '오토앤', 코스닥 상장으로 종합 모빌리티 ..., '현대차 사내벤처 1호 상장사' 오토앤 "종합 모빌리티 플랫폼으로 도..., 현대車 지배구조 개편 빨라지나…불확실성 해소에 글로비스 급등, 현대차가 선보인 최첨단 로보틱스 기술 Pn..., CES 현대차에 인파 몰린 이유…로봇개 군무에 아바타 체험까지, '깜짝등장' 칼라일, 현대차 혁신전략 도우미 급부상, 삼성·현대차·LG 일감몰아주기 규제 피했다..'총수 지분' 지각변동, 현대차그룹, ‘디어 마이 히어로’ 영상 조회수 1000만 회 돌파, 현대차 ‘수소청소트럭 캠페인’ 조회수 1000만 돌파, 위상 달라진 현대차그룹의 ‘두뇌’…“이제 세계가 우리 기술을..., 현대차그룹, ‘디어 마이 히어로’ 영상 조회수 1000만 회 돌파, 현대차 ‘수소청소트럭 캠페인’ 조회수 1000만 돌파, CES 2022 - 메타버스 코인 탑승, 메타모빌리티의 탄생, 모빌리티 사업자로서의 정체성 강화, 현대차 사내벤처 '오토앤', 코스닥 상장으로 종합 모빌리티 ..., 삼성·현대차·LG 일감몰아주기 규제 피했다..'총수 지분' 지각변동, ‘로봇개' BTS 노래에 춤추고 스핀 도는 ..., '정의선 회장 지분매각' 현대차그룹 지배구조 개편 신호탄되나, 현대차, CES서 메타모빌리티 선보여…정체성 강화 -한국, 현대차, 메타버스 코인 탑승-한투, "제네시스 GV60 닮았다"…소니 전기차에 현대차 직원들 '술렁' [C..., 아직은 빡빡한 반도체 수급, 반도체 악재는 부정적이지만, 향후 반전의 가능성으로도 작용, 현대차 21년도 4분기 Review: 영업이익률 4.9% 기록, 컨퍼런스 콜의 주요 내용: 반도체 이슈는 하반기 안정화를 전망 중, 'BTS 노래에 칼군무'···현대차, 로봇개 '탄성' [CES..., 현대차그룹, '수소청소트럭 캠페인' 영상 조회수 1000만회 돌파, 수소 접목한 청소트럭, 이렇게 깨끗하다니…현대차 캠페인 영상 ‘..., 현대차그룹 모베드 ‘김연아 턴’에 “와우!”…로봇개 스팟 화려..., 현대ENG, '암모니아에서 고순도 수소 생산' 사업화 추진, 음악 나오자 춤추는 로봇개 "와우"…현대차 부스 앞엔 30분 대기줄[C..., 현대ENG, 암모니아 분해해 수소 생산하는 사업 추진, 현대차그룹, '디어 마이 히어로' 영상 조회수 1000만회 돌파, 현대차그룹 모베드 ‘김연아 턴’에 “와우!”…로봇개 스팟 화..., 정의선 현대차 회장, CES 첫 데뷔 정기선 현대重 대표 '응원..., BTS 처럼, 김연아 같이...현대차 로보틱스에 탄성, '정의선 회장 지분매각' 현대차그룹 지배구조 개편 신호탄되나, '차 없는 현대차 CES 전시장'…미래 모빌리티로 가득..., BTS 처럼, 김연아 같이...현대차 로보틱스에 탄성, 수소 접목한 청소트럭, 이렇게 깨끗하다니…현대차 캠페인 영상 ..., 현대차그룹 고급차-전기차 나란히 판매량 20만대, 현대차 사내벤처 오토앤 "종합 모빌리티 플랫폼 도약", BTS 노래에 칼군무…현대차 로봇, 관람객 뒤집어놨다 (영상) [CES..., 현대차 ‘수소청소트럭 영상’ 일주일만에 1000만뷰 돌파</t>
   </si>
   <si>
     <t>현대차, 메타버스 기반 디지털 공장 '메타팩토리' 구축한..., "자율주행에 완성차 위축"…현대차, 괜찮나?, 현실과 똑같이…현대차, 가상공간에 '쌍둥이 공장' 짓는다, 현대차 사내벤처 1호 '오토앤' 13년 만에 코스닥 데뷔, 현대차 '싱가포르 혁신센터'…메타버스 공장으로도 탄생, 현대차, 메타버스 기반 디지털 공장 '메타팩토리' 구축한..., "자율주행에 완성차 위축"…현대차, 괜찮나?, 현대차 '싱가포르 혁신센터'…메타버스 공장으로도 탄생, 세종공업, 삼성發 로봇 M&amp;A 예고에 삼성·현대·LG 협력 ..., “현대차 ‘두뇌’는 글로벌 톱…경쟁사 너도나도 분석중”, 세종공업, 삼성發 로봇 M&amp;A 예고에 삼성·현대·LG 협력 ..., 현대차, 디지털 가상공장 ‘메타팩토리’ 구축, 현대차 사내벤처 1호 '오토앤' 13년 만에 코스닥 데뷔, 현대중공업, 계열사 현대엔진 지분 100% 290억원에 취득, 현대차의 로보틱스 기술...인간·사물의 한계 극복한다, 현대차, 연말까지 '메타버스 공장' 구축…"지구 반대편서 문제 해결", 현대차, 싱가포르 글로벌 혁신센터 가상공간에 구축한다, 현실과 똑같은 메타버스 공장 나온다…현대..., 테슬라 전부 합쳐도…현대차 아이오닉5보다 덜 팔렸다, 해외공장 문제 생겨도 국내서 '뚝딱'…현대차, 메타버스공장 만든다 [C..., 현대차, 유니티와 맞손…"연내 메타팩토리 가동시작..., 테슬라 전부 합쳐도…현대차 아이오닉5보다 덜 팔렸다, “현대차 ‘두뇌’는 글로벌 톱…경쟁사 너도나도 분석중”, 현실과 똑같이…현대차, 가상공간에 '쌍둥이 공장' 짓는다, 美서 혼다 제치고 5위 달성…C...</t>
@@ -7576,19 +7576,19 @@
     <t>車 두고온 현대차·車 가져온 삼성·소니···CES서 확인한 산업재편, 현대차, SKT만 한다고? 우리도 ‘하늘 나는 택시’ 드라이브 [비즈3..., 현대차 "SUV·친환경차·제네시스 앞세워 美시장서 지속성장" [CES ..., 호세 무뇨스 사장 "현대차, 日 혼다 넘었다"…친환경..., "현대차, 2030년까지 美 판매 절반 친환경차로", 현대차, SKT만 한다고? 우리도 ‘하늘 나는 택시’ 드라이브 [비즈3..., 현대차 북미본부장 “2030년 판매 절반을 친환경차로”, 車 두고온 현대차·車 가져온 삼성·소니···CES서 확인한 산업재편</t>
   </si>
   <si>
-    <t>현대차그룹 넘보던 카카오 그룹株, 겹악재에 시총 100조원 깨졌다, 현대차, 지속가능한 미래 연다...글로벌 CSV 프로젝트 '컨티뉴' ..., 현대차, 지속가능경영 글로벌 CSV 프로젝트 '컨티뉴' 공개, 현동진 현대차 상무 "2년내 소형 모빌리티 모베드 양산···보스턴다이내..., 현대차그룹이 로봇을 만드는 이유…"로보틱스는 새로운 사업의 씨앗", 현대차, SBS '지금 헤어지는 중입니다'서 아이오닉5 지원…"친밀감 ..., 현대차 "더 나은 삶 위해 로봇과 새 서비스 결합…결..., 현대차-모빌리티 시장의 변곡점이 될 2022년, 적극적 기술 전략 기대, 변화하는 시장환경, 2022년이 모빌리티 시장 성장의 변곡점 될 것, 모빌리티 시장의 부상 속 생존과 성장 전략 구축 필요, 2022년 실적보다 중요한 미래 비전 제시와 기술 및 협력 파트너 확보, 현대차, SBS '지금 헤어지는 중입니다'서 아이오닉5 지원…"친밀감 ..., 현대차그룹 넘봤는데…카카오그룹株, 잇단 악재에 100조 '붕괴', 현대차그룹 넘보던 카카오 그룹株, 겹악재에 시총 100조원 깨졌다, 현대차 "더 나은 삶 위해 로봇과 새 서비스 결합…결..., "현대차-보스턴다이내믹스 로보틱스 협업, 1~2년 내 결과물 낼 것" ..., 현대차-모빌리티 시장의 변곡점이 될 2022년, 적극적 기술 전략 기대, 변화하는 시장환경, 2022년이 모빌리티 시장 성장의 변곡점 될 것, 모빌리티 시장의 부상 속 생존과 성장 전략 구축 필요, 2022년 실적보다 중요한 미래 비전 제시와 기술 및 협력 파트너 확보, 현대차·기아, 내년 비건레더 신차 나온다…방글라데시 공장 신설도, "현대차-보스턴다이내믹스 로보틱스 협업, 1~2년 내 결과물 낼 것" ..., "현대차-보스턴 다이내믹스 협업 진행…내년 이후 결과물 보여줄 것", 현대차그룹 넘봤는데…카카오그룹株, 잇단 악재에 100조 '붕괴', 현동진 현대차 상무 "2년내 소형 모빌리티 모베드 양산···보스턴다이내..., SK·현대차 제로원, 모빌리티 충전 플랫폼 '소프트베리'..., 美서 혼다 제친 현대차 "美서 전기차 생산..., 현대차그룹 "로보틱스는 새 사업 모델 만드는 '씨앗..., 현대차·삼성전자 로봇사업 확대… K로봇 관련株 급등, 현대차, 공유가치창출 세계에 알린다 '컨티뉴' 프로젝트 공개, 현대차, 글로벌 CSV 프로젝트 ‘컨티뉴’ 공개…청정 미래를 그린다, 현대차, 글로벌 공유가치창출 프로젝트 '컨티뉴' 공개, 현대차 '친환경·모빌리티·미래세대' 방점 공유가치 프로젝트 공개, SK·현대차 제로원, 모빌리티 충전 플랫폼 '소프트베리'..., '현대차그룹 사내벤처' 오토앤, 수요예측 1713대 1…"공모가 상단 ..., 현대차, 지속가능경영 글로벌 CSV 프로젝트 '컨티뉴' 공개, 美서 혼다 제친 현대차 "美서 전기차 생산..., 현대차·삼성전자 로봇사업 확대… K로봇 관련株 급등, 현대차, 글로벌 공유가치창출 프로젝트 '컨티뉴' 공개, 현대차 '친환경·모빌리티·미래세대' 방점 공유가치 프로젝트 공개, 미국에서 혼다 제친 현대차, 이유 있는 질주, “2030년 美 판매 절반은 친환경차…현대차, 현지에서 전기차 생산할것..., 현대차, 지속가능한 미래 연다...글로벌 CSV 프로젝트 '컨티뉴' ..., 현대차·기아, 내년 비건레더 신차 나온다…방글라데시 공장 신설도</t>
-  </si>
-  <si>
-    <t>“현대차, 생산 정상화가 중요한 시점”, 현대차·기아·제네시스 6개 차종 美 ‘2021 굿디자인 어워드’ 수상, 현대차그룹 6개 차종...美 '굿디자인 어워드' 싹쓸이, "생산성 2위 현대차 몽고메리 공장…비결은 美인센티브 정책·노동 유연..., 현대차 앨러배마 공장 높은 생산성 비결은 "노동유연성", 전기차 주도권 충전소에 달렸다…현대차 "상반기까지 20곳", 현대차-21년 하프스윙, 22년 풀스윙, 21년도 4분기 영업이익 1.76조원(+40.3%)으로 소폭 부진할 전망, 이제는 정말 중요해진 생산 정상화의 시점에 근거 있는 자신감, 목표주가 27만원, 투자의견 매수 유지, "한국에선 불가능"…현대차 '美 역대급 판매' 뒤엔 '이것' 있었다, 현대차-21년 하프스윙, 22년 풀스윙, 21년도 4분기 영업이익 1.76조원(+40.3%)으로 소폭 부진할 전망, 이제는 정말 중요해진 생산 정상화의 시점에 근거 있는 자신감, 목표주가 27만원, 투자의견 매수 유지, 전기차 주도권 충전소에 달렸다…현대차 "상반기까지 20곳", 피제이전자, 현대차 ‘로봇 열풍’ 타고 상한가 달성, 美공략 시동 현대차 아이오닉 5·기아 EV6 디자인 통했다, 아이오닉5· X 콘셉트 등 현대차그룹 6개 차 굿디자인 어워드 수상, 현대차, 목표주가 27만원 유지-신한, 현대차·기아·제네시스, 권위있는 미국 디자인상 대거 수상, “현대차, 생산 정상화가 중요한 시점”, 현대차, 목표주가 27만원 유지-신한, 현대ENG, 초소형모듈원전 美회사 투자..글로벌 EPC 독점권 확보, 아이오닉5·GV70 등 현대차그룹 차량 6종 굿디자인어워드 수상, “크래프톤, 신작 매출 정상화 지연”…현대차證 목표가 내려, 아이오닉5· X 콘셉트 등 현대차그룹 6개 차 굿디자인 어워드 수상, 현대ENG, 미국 USNC사 지분 투자…4세대 초소형모듈원전 EPC 독..., 美공략 시동 현대차 아이오닉 5·기아 EV6 디자인 통했다, 현대차기아제네시스 6개 차종. 美 ‘2021 굿디자인 어워드’ 수상, 현대차·기아·제네시스 6개 차종 美 ‘2021 굿디자인 어워드’ 수상, "생산성 2위 현대차 몽고메리 공장…비결은 美인센티브 정책·노동 유연성..., 현대ENG, 미국 USNC사 지분 투자…4세대 초소형모듈원전 EPC 독...</t>
-  </si>
-  <si>
-    <t>현대차-2022년 생산 정상화 기대, 2022년 생산 안정성 회복에 따른 실적 개선 기대, 4분기 Preview: 더딘 생산회복의 여파, 현대차-21년도 4분기 프리뷰: 중요한 건 미래차 비전, 4분기 영업이익률 5.9%(+1.6%p). 기대치 하회 예상, 2022년은 물량 회복과 더불어 미래차 경쟁력 제고가 관건, 투자의견 BUY, 목표주가 28만원 유지. 업종 내 Top Pick, 현대차 새 노조위원장 "전기차 시대 고용안정 대책 세워야", ‘순정부품만 써야’ 거짓 광고한 현대·기아차…공정위, 경고, 삼성이 택한 '급식 맛집' 풀무원, 현대차도 뚫었다, ‘순정부품 안 쓰면 고장’…현대차·기아 표시광고법 위반 ‘제재’, ‘순정부품 안 쓰면 고장’…공정위, 거짓 광고한 현대차에 ‘경고만’(종..., ‘순정부품만 써야’ 거짓 광고한 현대·기아차…공정위, 경고, "순정부품 안쓰면 고장?" 거짓 광고한 현대차에 경고 조치, 현대차, 베트남서 도요타 누르고 2년연속 판매 1위, 현대차-2022년 생산 정상화 기대, 2022년 생산 안정성 회복에 따른 실적 개선 기대, 4분기 Preview: 더딘 생산회복의 여파, 현대차, 베트남서 도요타 제치고 2년 연속 판매 1위, ‘순정부품 안 쓰면 고장’…현대차·기아 표시광고법 위반 ‘제재’, ‘순정부품 안 쓰면 고장’…공정위, 거짓 광고한 현대차에 ‘경고만’(종..., 현대차-21년도 4분기 프리뷰: 중요한 건 미래차 비전, 4분기 영업이익률 5.9%(+1.6%p). 기대치 하회 예상, 2022년은 물량 회복과 더불어 미래차 경쟁력 제고가 관건, 투자의견 BUY, 목표주가 28만원 유지. 업종 내 Top Pick, "순정부품 안쓰면 고장?" 거짓 광고한 현대차에 경고 조치, 현대차, 베트남서 도요타 누르고 2년연속 판매 1위, 현대차, 베트남서 도요타 제치고 2년 연속 판매 1위, 삼성이 택한 '급식 맛집' 풀무원, 현대차도 뚫었다, 현대차證, ESG 투자 원칙 제정..."탈석탄 금융 선언", 현대차 엔진결함 고발 김광호 강사 "고객 최우선 가치 위해 신고", 현대차가 2조원 투자한 이 회사, 아이오닉5 완전자율주행으로 미국 달린..., 삼성·LG·현대차도 뛰어들었다…한달새 2배 뛴 로봇株, 현대차, 4분기 영업익 컨센서스 하회…"올해 생산 정상화 기대"-NH, NH “현대차 생산 회복 재개로 실적 개선 기대...목표가 30만원”, 삼성·LG·현대차도 뛰어들었다…한달새 2배 뛴 로봇株, 현대차, 올해 2분기부터 생산 회복 전망…"중장기 좋다"-NH, 현대차, 올 2분기부터 생산 회복에 따라 실적 개선 전망-NH, 산업부, '디지털산업혁신펀드 2호' 800억원 결성…현대차 등 참여, 현대차, 베트남서 도요타 누르고 2년연속 판매 1위, 뉴인텍, 커패시터 모든 현대차 전기차 기본 탑재…美·獨 전기차..., 산업부, '디지털산업혁신펀드 2호' 800억원 결성…현대차 등 참여, “순정부품 안 쓰면 車 고장”이라던 현대·기아차...허위 광고였다, 공정위 "현대차·기아, 비순정부품 사용시 車성능 저하·고장 유발 광고..., ‘순정부품 안 쓰면 고장’…현대차·기아 표시광고법 위반 ‘제재’, 현대차證, ESG 투자 원칙 제정..."탈석탄 금융 선언", 뉴인텍, 커패시터 모든 현대차 전기차 기본 탑재…美·獨 전기차..., 현대차가 2조원 투자한 이 회사, 아이오닉5 완전자율주행으로 미국 달린...</t>
-  </si>
-  <si>
-    <t>장재훈 현대차 사장 “제네시스 올 22만대, G90 年2만대 판매목표..., "제네시스, 인피니티 이미 추월… 올 22만대 팔것" [현대차 2022..., 장재훈 현대차 사장 “제네시스 올 22만대, G90 年2만대 판매목표..., "제네시스, 인피니티 이미 추월… 올 22만대 팔것" [현대차 2022..., 車판매 하반기부터 회복… 코로나 이전 수준은 내년에나 가능 [현대차 2..., 현대차-전년 대비 증감율로 보고, 전분기 대비 증감율로 봐도 증익, 21년도 4분기 Preview: 제한적이었던 자동차 부문, 든든한 금융 부문, 2022년, 아이오닉6 출시에 따른 BEV 모멘텀 기대, 투자의견 Buy, 목표주가 320,000원 유지, 현대차가 본 올해 車시장 "신차 가격 대폭 오른다", 장재훈 현대차 사장 “제네시스 G90 글로벌 연간 2만 대 판매 목표”, 현대차 사장 "제네시스 경쟁력, 벤츠 95% 수준 ", 현대차, 작년 4분기 바닥 다져…"아이오닉6 출시 모멘텀 기대"-하이, 운전자 개입없이도 자율주행.. ‘레벨3’ 수준 G90 4분기 출시 [현...</t>
-  </si>
-  <si>
-    <t>한화투자증권 “현대차, 중장기 성장 기대감 유효…투자 비중 늘려야”, 현대차, 수소차·제네시스 앞세워 중동 본격 공략, 삼성-현대차 '車반도체 드림팀' 뭉쳤다, 현대차-닻을 올리다, 21년도 4분기 실적 Preview: 시장 기대치 하회 전망, 올해 물량 증가를 통해 성장세 지속 전망, 투자의견 Buy, 목표주가 300,000원 유지, 현대차-21년도 4분기 Preview, 4분기 영업이익 1.74조원 전망, 자동차 4분기 글로벌 도매 판매 95.6만대, 연결 기준 86만대 (전분기 대비 증감율 7.3%, 4.2%) 전분기 기저를 반영한 회복세</t>
+    <t>현대차그룹 넘보던 카카오 그룹株, 겹악재에 시총 100조원 깨졌다, 현대차, 지속가능한 미래 연다...글로벌 CSV 프로젝트 '컨티뉴' ..., 현대차, 지속가능경영 글로벌 CSV 프로젝트 '컨티뉴' 공개, 현동진 현대차 상무 "2년내 소형 모빌리티 모베드 양산···보스턴다이내..., 현대차그룹이 로봇을 만드는 이유…"로보틱스는 새로운 사업의 씨앗", 현대차, SBS '지금 헤어지는 중입니다'서 아이오닉5 지원…"친밀감 ..., 현대차 "더 나은 삶 위해 로봇과 새 서비스 결합…결..., 모빌리티 시장의 변곡점이 될 2022년, 적극적 기술 전략 기대, 변화하는 시장환경, 2022년이 모빌리티 시장 성장의 변곡점 될 것, 모빌리티 시장의 부상 속 생존과 성장 전략 구축 필요, 2022년 실적보다 중요한 미래 비전 제시와 기술 및 협력 파트너 확보, 현대차, SBS '지금 헤어지는 중입니다'서 아이오닉5 지원…"친밀감 ..., 현대차그룹 넘봤는데…카카오그룹株, 잇단 악재에 100조 '붕괴', 현대차그룹 넘보던 카카오 그룹株, 겹악재에 시총 100조원 깨졌다, 현대차 "더 나은 삶 위해 로봇과 새 서비스 결합…결..., "현대차-보스턴다이내믹스 로보틱스 협업, 1~2년 내 결과물 낼 것" ..., 모빌리티 시장의 변곡점이 될 2022년, 적극적 기술 전략 기대, 변화하는 시장환경, 2022년이 모빌리티 시장 성장의 변곡점 될 것, 모빌리티 시장의 부상 속 생존과 성장 전략 구축 필요, 2022년 실적보다 중요한 미래 비전 제시와 기술 및 협력 파트너 확보, 현대차·기아, 내년 비건레더 신차 나온다…방글라데시 공장 신설도, "현대차-보스턴다이내믹스 로보틱스 협업, 1~2년 내 결과물 낼 것" ..., "현대차-보스턴 다이내믹스 협업 진행…내년 이후 결과물 보여줄 것", 현대차그룹 넘봤는데…카카오그룹株, 잇단 악재에 100조 '붕괴', 현동진 현대차 상무 "2년내 소형 모빌리티 모베드 양산···보스턴다이내..., SK·현대차 제로원, 모빌리티 충전 플랫폼 '소프트베리'..., 美서 혼다 제친 현대차 "美서 전기차 생산..., 현대차그룹 "로보틱스는 새 사업 모델 만드는 '씨앗..., 현대차·삼성전자 로봇사업 확대… K로봇 관련株 급등, 현대차, 공유가치창출 세계에 알린다 '컨티뉴' 프로젝트 공개, 현대차, 글로벌 CSV 프로젝트 ‘컨티뉴’ 공개…청정 미래를 그린다, 현대차, 글로벌 공유가치창출 프로젝트 '컨티뉴' 공개, 현대차 '친환경·모빌리티·미래세대' 방점 공유가치 프로젝트 공개, SK·현대차 제로원, 모빌리티 충전 플랫폼 '소프트베리'..., '현대차그룹 사내벤처' 오토앤, 수요예측 1713대 1…"공모가 상단 ..., 현대차, 지속가능경영 글로벌 CSV 프로젝트 '컨티뉴' 공개, 美서 혼다 제친 현대차 "美서 전기차 생산..., 현대차·삼성전자 로봇사업 확대… K로봇 관련株 급등, 현대차, 글로벌 공유가치창출 프로젝트 '컨티뉴' 공개, 현대차 '친환경·모빌리티·미래세대' 방점 공유가치 프로젝트 공개, 미국에서 혼다 제친 현대차, 이유 있는 질주, “2030년 美 판매 절반은 친환경차…현대차, 현지에서 전기차 생산할것..., 현대차, 지속가능한 미래 연다...글로벌 CSV 프로젝트 '컨티뉴' ..., 현대차·기아, 내년 비건레더 신차 나온다…방글라데시 공장 신설도</t>
+  </si>
+  <si>
+    <t>“현대차, 생산 정상화가 중요한 시점”, 현대차·기아·제네시스 6개 차종 美 ‘2021 굿디자인 어워드’ 수상, 현대차그룹 6개 차종...美 '굿디자인 어워드' 싹쓸이, "생산성 2위 현대차 몽고메리 공장…비결은 美인센티브 정책·노동 유연..., 현대차 앨러배마 공장 높은 생산성 비결은 "노동유연성", 전기차 주도권 충전소에 달렸다…현대차 "상반기까지 20곳", 21년 하프스윙, 22년 풀스윙, 21년도 4분기 영업이익 1.76조원(+40.3%)으로 소폭 부진할 전망, 이제는 정말 중요해진 생산 정상화의 시점에 근거 있는 자신감, 목표주가 27만원, 투자의견 매수 유지, "한국에선 불가능"…현대차 '美 역대급 판매' 뒤엔 '이것' 있었다, 21년 하프스윙, 22년 풀스윙, 21년도 4분기 영업이익 1.76조원(+40.3%)으로 소폭 부진할 전망, 이제는 정말 중요해진 생산 정상화의 시점에 근거 있는 자신감, 목표주가 27만원, 투자의견 매수 유지, 전기차 주도권 충전소에 달렸다…현대차 "상반기까지 20곳", 피제이전자, 현대차 ‘로봇 열풍’ 타고 상한가 달성, 美공략 시동 현대차 아이오닉 5·기아 EV6 디자인 통했다, 아이오닉5· X 콘셉트 등 현대차그룹 6개 차 굿디자인 어워드 수상, 현대차, 목표주가 27만원 유지-신한, 현대차·기아·제네시스, 권위있는 미국 디자인상 대거 수상, “현대차, 생산 정상화가 중요한 시점”, 현대차, 목표주가 27만원 유지-신한, 현대ENG, 초소형모듈원전 美회사 투자..글로벌 EPC 독점권 확보, 아이오닉5·GV70 등 현대차그룹 차량 6종 굿디자인어워드 수상, “크래프톤, 신작 매출 정상화 지연”…현대차證 목표가 내려, 아이오닉5· X 콘셉트 등 현대차그룹 6개 차 굿디자인 어워드 수상, 현대ENG, 미국 USNC사 지분 투자…4세대 초소형모듈원전 EPC 독..., 美공략 시동 현대차 아이오닉 5·기아 EV6 디자인 통했다, 현대차기아제네시스 6개 차종. 美 ‘2021 굿디자인 어워드’ 수상, 현대차·기아·제네시스 6개 차종 美 ‘2021 굿디자인 어워드’ 수상, "생산성 2위 현대차 몽고메리 공장…비결은 美인센티브 정책·노동 유연성..., 현대ENG, 미국 USNC사 지분 투자…4세대 초소형모듈원전 EPC 독...</t>
+  </si>
+  <si>
+    <t>2022년 생산 정상화 기대, 2022년 생산 안정성 회복에 따른 실적 개선 기대, 4분기 Preview: 더딘 생산회복의 여파, 21년도 4분기 프리뷰: 중요한 건 미래차 비전, 4분기 영업이익률 5.9%(+1.6%p). 기대치 하회 예상, 2022년은 물량 회복과 더불어 미래차 경쟁력 제고가 관건, 투자의견 BUY, 목표주가 28만원 유지. 업종 내 Top Pick, 현대차 새 노조위원장 "전기차 시대 고용안정 대책 세워야", ‘순정부품만 써야’ 거짓 광고한 현대·기아차…공정위, 경고, 삼성이 택한 '급식 맛집' 풀무원, 현대차도 뚫었다, ‘순정부품 안 쓰면 고장’…현대차·기아 표시광고법 위반 ‘제재’, ‘순정부품 안 쓰면 고장’…공정위, 거짓 광고한 현대차에 ‘경고만’(종..., ‘순정부품만 써야’ 거짓 광고한 현대·기아차…공정위, 경고, "순정부품 안쓰면 고장?" 거짓 광고한 현대차에 경고 조치, 현대차, 베트남서 도요타 누르고 2년연속 판매 1위, 2022년 생산 정상화 기대, 2022년 생산 안정성 회복에 따른 실적 개선 기대, 4분기 Preview: 더딘 생산회복의 여파, 현대차, 베트남서 도요타 제치고 2년 연속 판매 1위, ‘순정부품 안 쓰면 고장’…현대차·기아 표시광고법 위반 ‘제재’, ‘순정부품 안 쓰면 고장’…공정위, 거짓 광고한 현대차에 ‘경고만’(종..., 21년도 4분기 프리뷰: 중요한 건 미래차 비전, 4분기 영업이익률 5.9%(+1.6%p). 기대치 하회 예상, 2022년은 물량 회복과 더불어 미래차 경쟁력 제고가 관건, 투자의견 BUY, 목표주가 28만원 유지. 업종 내 Top Pick, "순정부품 안쓰면 고장?" 거짓 광고한 현대차에 경고 조치, 현대차, 베트남서 도요타 누르고 2년연속 판매 1위, 현대차, 베트남서 도요타 제치고 2년 연속 판매 1위, 삼성이 택한 '급식 맛집' 풀무원, 현대차도 뚫었다, 현대차證, ESG 투자 원칙 제정..."탈석탄 금융 선언", 현대차 엔진결함 고발 김광호 강사 "고객 최우선 가치 위해 신고", 현대차가 2조원 투자한 이 회사, 아이오닉5 완전자율주행으로 미국 달린..., 삼성·LG·현대차도 뛰어들었다…한달새 2배 뛴 로봇株, 현대차, 4분기 영업익 컨센서스 하회…"올해 생산 정상화 기대"-NH, NH “현대차 생산 회복 재개로 실적 개선 기대...목표가 30만원”, 삼성·LG·현대차도 뛰어들었다…한달새 2배 뛴 로봇株, 현대차, 올해 2분기부터 생산 회복 전망…"중장기 좋다"-NH, 현대차, 올 2분기부터 생산 회복에 따라 실적 개선 전망-NH, 산업부, '디지털산업혁신펀드 2호' 800억원 결성…현대차 등 참여, 현대차, 베트남서 도요타 누르고 2년연속 판매 1위, 뉴인텍, 커패시터 모든 현대차 전기차 기본 탑재…美·獨 전기차..., 산업부, '디지털산업혁신펀드 2호' 800억원 결성…현대차 등 참여, “순정부품 안 쓰면 車 고장”이라던 현대·기아차...허위 광고였다, 공정위 "현대차·기아, 비순정부품 사용시 車성능 저하·고장 유발 광고..., ‘순정부품 안 쓰면 고장’…현대차·기아 표시광고법 위반 ‘제재’, 현대차證, ESG 투자 원칙 제정..."탈석탄 금융 선언", 뉴인텍, 커패시터 모든 현대차 전기차 기본 탑재…美·獨 전기차..., 현대차가 2조원 투자한 이 회사, 아이오닉5 완전자율주행으로 미국 달린...</t>
+  </si>
+  <si>
+    <t>장재훈 현대차 사장 “제네시스 올 22만대, G90 年2만대 판매목표..., "제네시스, 인피니티 이미 추월… 올 22만대 팔것" [현대차 2022..., 장재훈 현대차 사장 “제네시스 올 22만대, G90 年2만대 판매목표..., "제네시스, 인피니티 이미 추월… 올 22만대 팔것" [현대차 2022..., 車판매 하반기부터 회복… 코로나 이전 수준은 내년에나 가능 [현대차 2..., 전년 대비 증감율로 보고, 전분기 대비 증감율로 봐도 증익, 21년도 4분기 Preview: 제한적이었던 자동차 부문, 든든한 금융 부문, 2022년, 아이오닉6 출시에 따른 BEV 모멘텀 기대, 투자의견 Buy, 목표주가 320,000원 유지, 현대차가 본 올해 車시장 "신차 가격 대폭 오른다", 장재훈 현대차 사장 “제네시스 G90 글로벌 연간 2만 대 판매 목표”, 현대차 사장 "제네시스 경쟁력, 벤츠 95% 수준 ", 현대차, 작년 4분기 바닥 다져…"아이오닉6 출시 모멘텀 기대"-하이, 운전자 개입없이도 자율주행.. ‘레벨3’ 수준 G90 4분기 출시 [현...</t>
+  </si>
+  <si>
+    <t>한화투자증권 “현대차, 중장기 성장 기대감 유효…투자 비중 늘려야”, 현대차, 수소차·제네시스 앞세워 중동 본격 공략, 삼성-현대차 '車반도체 드림팀' 뭉쳤다, 닻을 올리다, 21년도 4분기 실적 Preview: 시장 기대치 하회 전망, 올해 물량 증가를 통해 성장세 지속 전망, 투자의견 Buy, 목표주가 300,000원 유지, 21년도 4분기 Preview, 4분기 영업이익 1.74조원 전망, 자동차 4분기 글로벌 도매 판매 95.6만대, 연결 기준 86만대 (전분기 대비 증감율 7.3%, 4.2%) 전분기 기저를 반영한 회복세</t>
   </si>
   <si>
     <t>정의선·정기선, 미래 이끄는 현대家 ‘투선’ 체제 주목, 현대차, 인도 공략 '고삐'…2조8천억대 배터리 사업 입찰, 현대차는 완성차 최선호주 "매수 비중 확대하라", 정의선·정기선, 미래 이끄는 현대家 ‘투선’ 체제 주목</t>
@@ -7597,10 +7597,10 @@
     <t>LG그룹 시가총액 3위로 껑충…현대차그룹 제쳤다, “현대차, 물량 증가·전기차 성장 등 주가 재평가 기대”, 현대차그룹, 설 연휴 전 협력사에 1.4조 조기지급, 2025년 가상공간서 개발한 현대車 나온다, 현대차證, ‘경기도 양주 덕계 공동주택’ 520억 PF 주관, 2025년 가상공간서 개발한 현대車 나온다, 현대차, 설 앞두고 협력사 납품대금 조기지급…1조4402억원 규모, 현대차證, ‘경기도 양주 덕계 공동주택’ 520억 PF 주관, 현대차·기아·제네시스 6개 차종, 美 2021 굿디자인 어워드 수상, 현대차그룹, 설 연휴 전 협력사에 1.4조 조기지급, '상생합시다' 현대차그룹, 협력사 납품대금 1.4조 조기지급, 현대차그룹, 납품대금 1조4402억 설 연휴전 조기지급, 현대차그룹, 납품대금 1조4402억원 조기지급…"협력사 자금난 해소", 현대차·기아·제네시스 6개 차종, 美 2021 굿디자인 어워드 수상, 현대두산인프라·현대건설기계, 영하 20도 철원서 혹한지 테스트, 현대차그룹, 납품대금 1조4402억 설 연휴전 조기지급, 현대차그룹, 설 연휴 앞두고 납품대금 1.4조 조기 지급, 현대차, 설 앞두고 협력사 납품대금 조기지급…1조4402억원 규모, LG그룹 시가총액 3위로 껑충…현대차그룹 제쳤다, “현대차, 물량 증가·전기차 성장 등 주가 재평가 기대”</t>
   </si>
   <si>
-    <t>중고차 사업 정지 권고···중기부, 현대차에 요청, 현대ENG, 블루수소로 탄소중립.."글로벌 친환경기업될 것", 중기부, 현대차에 ‘중고차 사업개시 일시정지’ 권고, 중기부, 현대차 중고차 사업진출 ‘제동’, 현대차·기아 동반 하락, LG이노텍 4%대 ↓, 현대자동차, 자율주행·로보틱스 전환 가속…"일상에서 미래 기술 실현한다..., 현대차그룹 '커넥티드카' 3종류 통합 추진, 현대차·기아 동반 하락, LG이노텍 4%대 ↓, 현대ENG, 블루수소로 탄소중립.."글로벌 친환경기업될 것", 현대ENG, 청정 수소인 '블루수소'에 투자한다, 중기부, 현대차에 중고차 사업개시 일시정지 권고, 현대자동차, 자율주행·로보틱스 전환 가속…"일상에서 미래 기술 실현한다..., 현대차그룹 '커넥티드카' 3종류 통합 추진, 현대차·기아 동반 하락, LG이노텍 4%대 ↓, 현대차-원가 부담 심화, 반도체 쇼티지 지속, 21년도 4분기 Preview, 본격적인 물량 회복은 하반기, 22년 실적 개선 지속 예상, 현대ENG, 청정 수소인 '블루수소'에 투자한다</t>
-  </si>
-  <si>
-    <t>현대차 정몽구 재단, 농산어촌 초등학생 위한 '온드림스쿨' 운영, 현대차·기아 車사려는 사람 줄섰지만..4Q 실적 반도체 영향은?, “아이폰 ‘디지털키’ 기능, 올 여름 현대차에도 적용”, "유럽에서 현대차·기아 더 잘 팔리겠네"…현대캐피탈, '자동차 금융영토..., 밀린주문만 100만대…현대차 지금 사도 올해 안에 못탈수도, “메타버스로 학습을” 현대차 정몽구재단 교육 봉사, 현대차 정몽구 재단, 농산어촌 초등학생 위한 '온드림스쿨' 운영, 글로벌 시장 선전에도…中서 힘 못쓴 현대차·기아, "유럽에서 현대차·기아 더 잘 팔리겠네"…현대캐피탈, '자동차 금융영토..., 현대차·기아 車사려는 사람 줄섰지만..4Q 실적 반도체 영향은?, “메타버스로 학습을” 현대차 정몽구재단 교육 봉사, 글로벌 시장 선전에도…中서 힘 못쓴 현대차·기아, 현대차-로봇에 메타버스까지 접수, CES2022를 통해 메타버스와 로보틱스 기술을 결합해 이동의 역할과 형태에 대해 새로운 변화상을 제시, 21년도 4분기 영업이익은 1.60조원(+27.2% 전년 대비 증감율)을 기록해 컨센서스 14% 하회 전망, 2022년 공급망 불안에도 볼륨 회복에 대한 의지가 높아 경쟁사 대비 안정적인 출하 흐름은 지속될 전망, 특근 다시 사라진 현대차·기아, 반도체난 상반기 내내 지속될듯, 현대차·기아, 유럽서도 질주… BMW 제치고 4위 되찾았다, '애플 디지털키' 현대차에 온다고? "국내 일부 차종 이미 iOS 호환..., 실탄 1조원…정의선 회장과 현대차그룹 미래는, 와디즈, 현대차와 손잡고 '아이오닉' 전용 상품개발 지원, 현대차 직할체제 된 현대캐피탈…佛시장 공략, 현대차·기아, 유럽서도 질주… BMW 제치고 4위 되찾았다, 현대차그룹, BMW 제치고 유럽 4위 탈환, 현대차·기아 인도에 신차 대거 투입…시장 삼킨다, “아이폰 ‘디지털키’ 기능, 올 여름 현대차에도 적용”, 현대차그룹, BMW 제치고 유럽 4위 탈환, 현대차·기아, 작년 유럽서 BMW 제쳐, 현대차·기아, EU 시장서 100만대 판매 회복…시장점유율 4위 등극, 실탄 1조원…정의선 회장과 현대차그룹 미래는, '애플 디지털키' 현대차에 온다고? "국내 일부 차종 이미 iOS 호환..., 현대차·기아, 中서 25% 판매 급감…중국인들 '자국 전기차' 탄다, “아이폰 ‘디지털키’ 기능, 올 여름 현대차에도 적용”, 현대차·기아 인도에 신차 대거 투입…시장 삼킨다</t>
+    <t>중고차 사업 정지 권고···중기부, 현대차에 요청, 현대ENG, 블루수소로 탄소중립.."글로벌 친환경기업될 것", 중기부, 현대차에 ‘중고차 사업개시 일시정지’ 권고, 중기부, 현대차 중고차 사업진출 ‘제동’, 현대차·기아 동반 하락, LG이노텍 4%대 ↓, 현대자동차, 자율주행·로보틱스 전환 가속…"일상에서 미래 기술 실현한다..., 현대차그룹 '커넥티드카' 3종류 통합 추진, 현대차·기아 동반 하락, LG이노텍 4%대 ↓, 현대ENG, 블루수소로 탄소중립.."글로벌 친환경기업될 것", 현대ENG, 청정 수소인 '블루수소'에 투자한다, 중기부, 현대차에 중고차 사업개시 일시정지 권고, 현대자동차, 자율주행·로보틱스 전환 가속…"일상에서 미래 기술 실현한다..., 현대차그룹 '커넥티드카' 3종류 통합 추진, 현대차·기아 동반 하락, LG이노텍 4%대 ↓, 원가 부담 심화, 반도체 쇼티지 지속, 21년도 4분기 Preview, 본격적인 물량 회복은 하반기, 22년 실적 개선 지속 예상, 현대ENG, 청정 수소인 '블루수소'에 투자한다</t>
+  </si>
+  <si>
+    <t>현대차 정몽구 재단, 농산어촌 초등학생 위한 '온드림스쿨' 운영, 현대차·기아 車사려는 사람 줄섰지만..4Q 실적 반도체 영향은?, “아이폰 ‘디지털키’ 기능, 올 여름 현대차에도 적용”, "유럽에서 현대차·기아 더 잘 팔리겠네"…현대캐피탈, '자동차 금융영토..., 밀린주문만 100만대…현대차 지금 사도 올해 안에 못탈수도, “메타버스로 학습을” 현대차 정몽구재단 교육 봉사, 현대차 정몽구 재단, 농산어촌 초등학생 위한 '온드림스쿨' 운영, 글로벌 시장 선전에도…中서 힘 못쓴 현대차·기아, "유럽에서 현대차·기아 더 잘 팔리겠네"…현대캐피탈, '자동차 금융영토..., 현대차·기아 車사려는 사람 줄섰지만..4Q 실적 반도체 영향은?, “메타버스로 학습을” 현대차 정몽구재단 교육 봉사, 글로벌 시장 선전에도…中서 힘 못쓴 현대차·기아, 로봇에 메타버스까지 접수, CES2022를 통해 메타버스와 로보틱스 기술을 결합해 이동의 역할과 형태에 대해 새로운 변화상을 제시, 21년도 4분기 영업이익은 1.60조원(+27.2% 전년 대비 증감율)을 기록해 컨센서스 14% 하회 전망, 2022년 공급망 불안에도 볼륨 회복에 대한 의지가 높아 경쟁사 대비 안정적인 출하 흐름은 지속될 전망, 특근 다시 사라진 현대차·기아, 반도체난 상반기 내내 지속될듯, 현대차·기아, 유럽서도 질주… BMW 제치고 4위 되찾았다, '애플 디지털키' 현대차에 온다고? "국내 일부 차종 이미 iOS 호환..., 실탄 1조원…정의선 회장과 현대차그룹 미래는, 와디즈, 현대차와 손잡고 '아이오닉' 전용 상품개발 지원, 현대차 직할체제 된 현대캐피탈…佛시장 공략, 현대차·기아, 유럽서도 질주… BMW 제치고 4위 되찾았다, 현대차그룹, BMW 제치고 유럽 4위 탈환, 현대차·기아 인도에 신차 대거 투입…시장 삼킨다, “아이폰 ‘디지털키’ 기능, 올 여름 현대차에도 적용”, 현대차그룹, BMW 제치고 유럽 4위 탈환, 현대차·기아, 작년 유럽서 BMW 제쳐, 현대차·기아, EU 시장서 100만대 판매 회복…시장점유율 4위 등극, 실탄 1조원…정의선 회장과 현대차그룹 미래는, '애플 디지털키' 현대차에 온다고? "국내 일부 차종 이미 iOS 호환..., 현대차·기아, 中서 25% 판매 급감…중국인들 '자국 전기차' 탄다, “아이폰 ‘디지털키’ 기능, 올 여름 현대차에도 적용”, 현대차·기아 인도에 신차 대거 투입…시장 삼킨다</t>
   </si>
   <si>
     <t>현대엔지니어링 IPO, 현대차그룹 지배구조개편 '열쇠', 현대차, 수소차에 몰두하는 까닭…"미래 대비", 광주참사 여파, 현대엔지 상장 비상, (영상)현대차·기아 작년 유럽서 BMW 제치고 점유율 4위, 현대차, 수소차에 몰두하는 까닭…"미래 대비", 현대차, 부울경과 수소버스 보급 확대 '맞손', (영상)현대차·기아 작년 유럽서 BMW 제치고 점유율 4위, 광주참사 여파, 현대엔지 상장 비상, 현대엔지니어링 IPO, 현대차그룹 지배구조개편 '열쇠', 현대차, 부산·울산·경남에 수소버스 年 100대 공급한다, 현대ENG, 글로벌 건설업계 상위권 'ESG' 경영체계 입증, 현대차, 부울경에 연간 100대 이상 수소버스 보급, 현대차, 부울경에 연간 100대 이상 수소버스 보급 협력, 현대차, 부산·울산·경남에 수소버스 年 100대 공급한다, 현대차, 부울경에 연간 100대 이상 수소버스 보급, 현대차, 부·울·경에 연간 100대 이상 수소버스 보급, 현대차, 부·울·경에 연간 100대 이상 수소버스 보급, 현대ENG, 글로벌 건설업계 상위권 'ESG' 경영체계 입증, 현대차, 부울경에 연간 100대 이상 수소버스 보급 협력, 현대차, 부울경과 수소버스 보급 확대 '맞손'</t>
@@ -7612,16 +7612,16 @@
     <t>현대차 이어 기아도 유럽 휩쓴다…EV6, 英 '왓 카 어워즈' 올해의 ..., 현대차?기아, 용인?정읍에 중고차 매매업 신청, 현대차?기아, 용인?정읍에 중고차 매매업 신청, LG엔솔, 현대차보다 GM 합작사에 '입김' 더 센 이유, 현대차 "제3 외부 기관 통해 조직문화 전반 조사하겠다", 현대차그룹의 ‘백기사’로 나선 칼라일그룹…주주가치 제고·불확실성 해소, 드림시큐리티, 현대차 양자컴퓨터로 차세대 배터리 개발 소식에..., 현대차 이어 기아도 유럽 휩쓴다…EV6, 英 '왓 카 어워즈' 올해의 ..., 드림시큐리티, 현대차 양자컴퓨터로 차세대 배터리 개발 소식에..., 현대차·기아 "외부기관 통해 조직문화 점검", "현대차 연구소 조직문화 외부기관에 점검 맡길것", 현대차그룹의 ‘백기사’로 나선 칼라일그룹…주주가치 제고·불확실성 해소, "현대차 연구소 조직문화 외부기관에 점검 맡길것", 현대차·기아 "외부기관 통해 조직문화 점검", LG엔솔, 현대차보다 GM 합작사에 '입김' 더 센 이유</t>
   </si>
   <si>
-    <t>"GM은 美서 현대중고차 파는데…" 규제 발목잡힌 韓 차업계, 현대차·기아, 미국서 ‘최고 고객가치상’ 최다 수상, 현대차·기아, 美 주간지 선정 '2022 최고의 고객가치상' 최다 수..., 현대차·기아, 美 ‘2022 최고의 고객가치상’ 석권, 현대차·기아 美 주간지 선정 ‘최고 고객가치상’ 최다 수상, "GM은 美서 현대중고차 파는데…" 규제 발목잡힌 韓 차업계, 현대차·기아, 미국서 ‘최고 고객가치상’ 최다 수상, 美서 상복 터진 현대차·기아…'최고의 車' 휩쓸었다, 현대차·기아 美 주간지 선정 ‘최고 고객가치상’ 최다 수상, 테슬라·벤츠 사러 온라인몰… 현대차는 매장으로, 현대차-기아, 美 ‘최고의 고객가치상’ 최다 수상, 현대차-기아, 美 ‘최고의 고객가치상’ 최다 수상, 美서 상복 터진 현대차·기아…'최고의 車' 휩쓸었다</t>
+    <t>"GM은 美서 현대중고차 파는데…" 규제 발목잡힌 韓 차업계, 현대차·기아, 미국서 ‘최고 고객가치상’ 최다 수상, 현대차·기아, 美 주간지 선정 '2022 최고의 고객가치상' 최다 수..., 현대차·기아, 美 ‘2022 최고의 고객가치상’ 석권, 현대차·기아 美 주간지 선정 ‘최고 고객가치상’ 최다 수상, "GM은 美서 현대중고차 파는데…" 규제 발목잡힌 韓 차업계, 현대차·기아, 미국서 ‘최고 고객가치상’ 최다 수상, 美서 상복 터진 현대차·기아…'최고의 車' 휩쓸었다, 현대차·기아 美 주간지 선정 ‘최고 고객가치상’ 최다 수상, 테슬라·벤츠 사러 온라인몰… 현대차는 매장으로, 기아, 美 ‘최고의 고객가치상’ 최다 수상, 기아, 美 ‘최고의 고객가치상’ 최다 수상, 美서 상복 터진 현대차·기아…'최고의 車' 휩쓸었다</t>
   </si>
   <si>
     <t>현대차·기아·GM·르노삼성 "설 연휴 무상점검 서비스 실시", 현대차그룹 사내 스타트업, 코스닥 상장 '대박', 현대차·기아, 중대재해처벌법 앞두고 '최고안전책임자' 신설, 현대차그룹 사내 스타트업 지원 결실…오토앤 코스닥 상장, '현대 N e-페스티벌' 글로벌 예선 시작…온라인 레이싱 대회, '사내 스타트업→분사→상장' 현대차그룹 첫 성공신화 만들었다, '현대 N e-페스티벌' 글로벌 예선 시작…온라인 레이싱 대회, e-레이싱대회 현대 N e-페스티벌 '글로벌 리그' 시작, '사내 스타트업→분사→상장' 현대차그룹 첫 성공신화 만들었다, e-레이싱대회 현대 N e-페스티벌 '글로벌 리그' 시작, 현대차, '현대 N e-페스티벌' 글로벌 리그 개최, 현대차·기아 '최고안전책임자' 선임…중대재해처벌법 대응, "독과점" 현대차 중고차 사업 막자 스타트업 오히려 실망한 이유, 현대차 사내 스타트업 육성 결실.. 1호 상장사 ‘오토앤’ 코스닥 돌풍, 창업 분사 ‘오토앤’ 코스닥 시장 돌풍…현대차그룹 사내 스타트업 지원 ..., 현대차, 스타트업 지원 요람으로…차량용품 개발 '오토앤' 첫상장, “韓, 삼성·현대차 직원수 만큼 일자리 감소”, 중대재해법 시행 앞두고···현대차그룹, CSO직 신설, 현대차·기아 CSO 신설… ‘안전 컨트롤타워’ 높이는 기업들 [중대재..., "車반도체 공급난에도"…현대차·기아 작년 역대급 실적 전망, 'IPO 대어' 또 온다···현대엔지 설 직후 청약, 현대차·기아, 최고안전책임자 자리 신설…"안전 관리 총력", 현대차·기아 최고안전책임자 신설…이동석·최준영 선임, "사내 스타트업 쑥쑥 잘 자랐네"...현대차그룹, '오토앤’ 코스닥 ..., 韓제조업 고용, 5년 간 삼성전·현대차 국내직원수 만큼 감소, 창업 분사 ‘오토앤’ 코스닥 시장 돌풍…현대차그룹 사내 스타트업 지원 ..., 현대차그룹 사내 스타트업, 코스닥 상장 '대박', 현대차·기아, 최고안전책임자 자리 신설…"안전 관리 총력", 현대차·기아 최고안전책임자 신설…이동석·최준영 선임, 韓제조업 고용, 5년 간 삼성전·현대차 국내직원수 만큼 감소, 韓제조업 고용, 최근 5년간 '삼전+현차 직원수'만큼 줄었다, “韓, 삼성·현대차 직원수 만큼 일자리 감소”, 제조업 취업자 수, 5년간 18만명 뚝…삼성전자·현대차 직원수와 맞먹..., 韓제조업 고용, 최근 5년간 '삼전+현차 직원수'만큼 줄었다, 현대차·기아, ‘최고안전책임자’직 신설…이동석·최준영 선임, "제조업 취업자 5년간 18만명 감소…삼성·현대차 국내 직원 사라진 셈..., 현대차그룹 사내 스타트업, 코스닥 상장 '대박', 현대차·기아·GM·르노삼성 "설 연휴 무상점검 서비스 실시", "'제조업 강국' 외쳤지만, 국내 고용은 뒷걸음…삼성전자·현대차 직원..., 韓제조업 고용, 최근 5년간 '삼전+현차 직원수'만큼 줄었다, 현대차, '현대 N e-페스티벌' 글로벌 리그 개최, ‘오토앤’ 코스닥 시장 돌풍…현대차그룹 사내 스타트업 지원 빛났다, 현대차, ‘현대 N e-페스티벌’ 글로벌 리그 개막…스피드왕 가린다, 현대차·기아, CSO직 신설…이동석·최준영 선임, 현대차·기아·GM·르노삼성 "설 연휴 무상점검 서비스 실시", "'제조업 강국' 외쳤지만, 국내 고용은 뒷걸음…삼성전자·현대차 직원..., 韓제조업 고용, 최근 5년간 '삼전+현차 직원수'만큼 줄었다, 현대차, '현대 N e-페스티벌' 글로벌 리그 개최, "독과점" 현대차 중고차 사업 막자 스타트업 오히려 실망한 이유, 현대차그룹 사내 스타트업 출발 오토앤 상장…육성노력 '결실', 현대차, 온라인 레이싱 대회 '현대 N e-페스티벌 글로벌 리그' 개최</t>
   </si>
   <si>
-    <t>현대차 "올해 판매 목표 432만대…투자계획은 9.2조", 현대차 "아이오닉6 전기차, 올해 하반기 국내 출시", "117.6조원"…현대차, 매출 창사 이래 최대(상보), 현대차, 지난해 영업이익 6조6789억원, 현대차, 지난해 4분기 영업이익 1조5297억원…전년동기比 2..., 현대차 "올해 판매 목표 432만대… 투자 계획 9.2조" [주목 e..., 현대차, 車반도체난 뚫고 '사상 최대 실적'…"올해 432만대 팔겠다"..., 현대차, 지난해 4분기 영업이익 1조5297억원…전년동기比 2..., 정의선의 현대차, 악재뚫고 질주…작년 매출 117조 '사상 최대', 현대차, 지난해 기말 배당금 4000원…전년보다 1000원 인상, 현대차, 4분기 영업익 21.9% 증가…"제네시스가 효자"(상보), 현대차 작년 영업익 6조6789억원…"반도체난 뛰어 넘었다"(종합), 현대차 "올해 3분기 車 반도체 공급 정상화 전망", "올해 친환경차 판매 목표 대수 56.4만대"-현대차 컨콜, "그랜저 풀체인지·아이오닉6 출시…올해 내수 판매량 73.2만대 목표"..., 현대차, 지난해 영업이익 6조6789억원, 현대차, 지난해 영업이익 6조6789억원, "그랜저 풀체인지·아이오닉6 출시…올해 내수 판매량 73.2만대 목표"..., 현대차, 보통주 4000원·종류주 4100원 현금배당 결정, "올해 3분기 차량용 반도체 공급 정상화 예상"-현대차 컨콜, 현대차, 보통주 주당 4000원 현금배당 결정, 현대차, 車반도체난 뚫고 '사상 최대 실적'…"올해 432만대 팔겠다"..., 햇살론 카드 발급 실적 1위는 삼성카드 ... 현대·신한 뒤이어, 현대차, 보통주 1주당 4000원 기말 현금배당 결정, (영상)내달 상장 앞둔 현대ENG…오너 자금줄? 신사업 박차?, "현대ENG 공모로 친환경 1.5조 투자", 현대차, 올 판매목표 432만대… 전기차 56% 늘린다, 현대차, 매출 117조 '신기록'…올 9.2조 투자, '구주매출' 우려 속 건설대장주 노린다…현대엔지, 코스피 출격, 반도체 품귀 넘었다... 현대차 역대급 실적, "매출 117조6000억원"…현대차, 새 역사 썼다, "고맙다, 제네시스"…현대차, 반도체 부족에도 역대최대 매출, 제네시스·아이오닉5, 역시 어려울 때 효자…현대차 4분기 영업익 1조..., 현대차 '반도체 대란' 뚫고 최대실적…"올 432만대 판다", "고맙다, 제네시스"…현대차, 반도체 부족에도 역대최대 매출, 제네시스·아이오닉5, 역시 어려울 때 효자…현대차 4분기 영업익 1조..., "현대ENG 공모로 친환경 1.5조 투자", 현대ENG “2030년 플랜트·건축·신사업 3각 포트폴리오 구축”, 현대차 '반도체 대란' 뚫고 최대실적…"올 432만대 판다", 현대차, 작년 4분기 영업익 1조5297억원...전년比 22%↑, 비상걸린 삼성·LG전자·현대차…달러결제 금지하면 수출입도 직격탄, “삼성·현대차도 불안” 러시아·우크라 싸움 불똥이 왜 우리 기업한테…..., 현대차 "아이오닉6·그랜저 풀체인지, 올 하반기 국내 출시", 현대차 "아이오닉6 전기차, 올해 하반기 국내 출시", 현대차 “올해 제네시스·SUV 내수 판매 비중 50%로…전동화 박차”, 현대차, 지난해 기말 배당금 4000원…전년보다 1000원 인상, 현대차, 4분기 영업익 1조5297억원…전년보다 21.9%↑, 현대ENG IPO 임박..현대차 지배구조 개편 나서나, 현대자동차 지난해 영업익 6조6789억원…전년 대비 178.9%↑, "117.6조원"…현대차, 매출 창사 이래 최대(상보), 현대차-점진적 개선 전망, 반도체 공급 차질, 비용 증가 등으로 컨센서스 하회, 반도체 공급 부족 3분기에는 정상화될 것으로 예상, 22년 판매 목표 432만대 제시, 목표가 25만원으로 11% 하향, 매수 의견 유지, 현대차-년도년도 2분기 4분기 Review: 큰 실망은 필요다,년도 분기 년도년도 2분기 4분기 영업손익은 시장 및 KB증권의 전망을 하회했지만 크게 실망할 필요는다,년도 분기 년도년도 2분기 4분기 영업이익 1.5조원 (+21.9% 전년 대비 증감율), 시장 컨센서스를 15.0% 하회, 현재까지 원재료비 증가에 따른 수익성 압박은 없다는 점, 반도체 수급에 대한 우호적 전망에 주목해야, 현대차-빛 바랜 분기 최대 매출, 21년도 4분기 영업이익 세전이익, 컨센서스 -15%, -29% 하회, 2022년, C19 기저 효과 신차 효과보다 더 중요한 모빌리티 비전 구체화, "매출 117조, 영업익 7조"…현대차, 작년 역대급 실적 기대, “삼성·현대차도 불안” 러시아·우크라 싸움 불똥이 왜 우리 기업한테…[..., '대한민국 최고의 차' 막판 명승부 펼친다…"벤츠·BMW냐 제네시스·현..., ‘내비게이션까지 차질’...현대차 반도체 수급난에 출고 1년 넘게 걸린..., '구주매출' 우려 속 건설대장주 노린다…현대엔지, 코스피 출격, 상장 앞둔 현대엔지니어링 “현대차그룹 에너지 전담 회사로 거듭나겠다”, 유럽서 벤츠·BMW 꺾은 현대차, 비결은, 김창학 현대ENG 대표 "상장 계기로 친환경사업 역량 강화", IPO 대어 또 온다…현대ENG, 고평가 논란 털고 건설 대장주 등극?, 현대차, 4분기 영업익 1.53조원…전년比 21.9%↑, 현대차, 2021년 4분기 매출 31조· 영업익 1.5조…전년比 6·5..., 현대차, 4분기 영업익 1조5297억...전년비 21.9% 증가, 현대차, 작년 영업익 6.67조원…전년比 178.9%↑, 현대차, 4분기 영업익 1조5297억…전년비 21.9% ↑, 현대차, 지난해 영업익 6조6789억…전년비 178.9% ↑, 현대차 "올해 판매 목표 432만대… 투자 계획 9.2조" [주목 e공..., 현대차, 4분기 영업익 1조5297억…전년비 21.9% ↑, 현대차, 4분기 영업익 21.9% 증가…"제네시스가 효자"(상보), 현대차, 작년 영업이익 6조 6,789억 원...전년比 178.9% 증..., 현대차 4분기 매출 31조265억-영업이익 1조5297억, 현대차, 작년 매출액 117조원…전년比 13.1%↑, 현대차, 4분기 영업익 1조5297억원…전년보다 21.9%↑, 현대차, 작년 영업익 6조6789억…연간 389만대 판매, 현대차, 지난해 매출 117조 사상 최대…영업익 전년比 178.9%↑, 현대차, 2021년 매출 117.6조·영업익 6.7조원…전년比 ..., 현대차, 4분기 매출액 31조원…전년比 6.1%↑</t>
-  </si>
-  <si>
-    <t>현대차, 올해 아프리카·중동서 30만대 이상 판다, 현대차·모비스, 반도체 품귀에 발목…기아만 애플카 기대↑, 차량용 반도체 품귀 불똥…현대차·모비스 ‘고전’, 현대차, 올해 아프리카·중동서 30만대 이상 판다, 현대차그룹, 싱가포르 주롱도시공사와 미래 교통수요 분석 위한 MOU, 차량용 반도체 품귀 불똥…현대차·모비스 ‘고전’, 현대차證, 영업익 1500억원 돌파···“IB 부문 성과가 견인”, 현대차證, 사상 첫 영업이익 1,500억 돌파, ‘미래 교통체계 실증’ 현대차그룹, 싱가포르 주롱도시공사와 MOU, 현대차·모비스, 반도체 품귀에 발목…기아만 애플카 기대↑, ‘현대차 사내 벤처 출신’ 오토앤, 장 초반 18% 급등, 현대차그룹, 싱가포르서 '자율주행·전기차' 미래 교통수요 분석, 현대차 "개인용 비행체(PAV) 시제품, ..., 그린모빌리티상 '최우석 현대차 전동화시험센..., 공정위, 현대차-LG엔솔 합작사 등 전기차 M&amp;A 줄줄이 승인, 공정위 "현대차-LG엔솔 합작사 등 전기차 M&amp;A심사 신속 승인", 현대ENG 국내 최고층 모듈러 주택 '용인 영덕' 이달 착공, 현대ENG, 13층 국내 최고층 모듈러주택 이달 말 착공, 현대차그룹, 싱가포르 주롱도시공사와 미래 교통수요 분석 위한 MOU, 헌혈하려고 사는 공혈견…현대차·건대, 문제 해결위해 머리 맞댄다, 현대차, 싱가포르 스마트시티 조성 나선다...미래 교통분석 MOU 체결, 현대자동차, 건국대학교와 반려견 헌혈 문화 조성 MOU, '수입차 무덤' 일본에 또…현대차, 13년 만의 재도전 성공할까, 현대차그룹, 싱가포르와 미래교통수요 분석 협약, '수입차 무덤' 일본에 또…현대차, 13년 만의 재도전 성공할까, 현대차그룹 4형제, 지난해 나란히 역대 최대 실적 기록(종합), IB가 실적 견인… 현대차證 영업익 1500억원 돌파, 현대차證, 사상 첫 영업이익 1,500억 돌파, '급락장 유탄’ 맞은 현대엔지, 공모가 하단 유력, 현대차그룹 '미래차 시험기지' 싱가포르 낙점, 현대차그룹, 싱가포르와 미래교통수요 분석 협약, 현대차그룹, 싱가포르 주롱도시공사와 MOU…미래 교통체계 실증한다, 현대차그룹 4형제, 지난해 나란히 역대 최대 실적 기록(종합), IB가 실적 견인… 현대차證 영업익 1500억원 돌파, 현대차證, 사상 첫 영업이익 1,500억 돌파, '급락장 유탄’ 맞은 현대엔지, 공모가 하단 유력, 현대차그룹 '미래차 시험기지' 싱가포르 낙점, 현대차그룹, 싱가포르와 미래교통수요 분석 협약, 현대차-건국대 ‘반려견 헌혈문화 조성’ 업무협약, 현대차, 건국대에 10억 후원 '반려동물 헌혈센터' 설립, 현대차 52주 신저가 경신…기아는 1.57%↑, 공정위, 현대차-LG엔솔 합작사 설립 승인…"전기차 M&amp;A 신속 심사", 공정위, 현대차-LG엔솔 합작 등 "전기차 시장 M&amp;A 활성화", IB 활약에…현대차·KTB證 역대급 실적, 현대차證, 작년 4Q 영업익 33% 증가, 현대차, 싱가포르 스마트시티 조성 나선다...미래 교통분석 MOU 체..., 헌혈하려고 사는 공혈견…현대차·건대, 문제 해결위해 머리 맞댄다, 현대차그룹, 싱가포르 주롱도시공사와 MOU…미래 교통체계 실증한다, 현대차그룹, 싱가포르서 '자율주행·전기차' 미래 교통수요 분석, 현대차, 빛 바랜 분기 최대 매출-메리츠, 이제 내 차 빨리 받을 수 있을까…현대차 "올 3분기 車 반도체 정상화..., 현대차, GV80 내세워 작년 美 최다판매…올해는 '제네시스 G90' ..., 이제 내 차 빨리 받을 수 있을까…현대차 "올 3분기 車 반도체 정상화..., 현대차, 빛 바랜 분기 최대 매출-메리츠, 현대차, GV80 내세워 작년 美 최다판매…올해는 '제네시스 G90' ..., 현대차-아쉬운 수익성과 희망적 가이던스, 4분기 영업이익 1.53조원, 당사 추정 및 컨센서스 하회, 2022년 판매목표 432만대, 희망적 가이던스, 현대차-아쉬움과 기대감이 공존하는 구간, 21년도 4분기 Review: 자동차 부문의 수익성 악화가 아쉬웠으나, 22년도 1분기 Preview: 차량용 반도체 쇼티지는 지속, CEO Investor Day 기대감, 현대차-건국대, 반려견 헌혈 문화 조성 위한 MOU 체결, 현대차, 빛 바랜 분기 최대 매출, 현대차-년도년도 2분기 4분기 Review-여전히 남아있는 생산차질 우려, 년도년도 2분기 4분기 Review-여전히 남아있는 생산차질 우려, 월초 판매/생산 데이터에 주목할 필요, 현대차-년도년도 2분기 4분기 Review: 개선될 여지가 많은 2022년, 년도년도 2분기 4분기 (P): 매출액 31조 265억원, 영업이익 1조 5,297억원, 2022년 판매대수 429만대로 전년 대비 증감율 +10.3% 증가 전망, 수익성 개선은 믹스 변화로, 성장은 전기차로, 현대차-매출액 130조원 시대 개막, 투자포인트 및 결론, 주요이슈 및 실적전망, 주가전망 및 Valuation, 현대차- 4분기 부진보다는 올해 긍정적 가이던스 주목, 년도년도 2분기 4분기 Review: 시장 기대치 하회, 22년 긍정적 가이던스 제시, 투자의견 ‘Buy’, 목표주가 300,000원 유지, 현대차-빛 바랜 분기 최대 매출, 21년도 4분기 영업이익 세전이익, 컨센서스 -15%, -29% 하회, 2022년, C19 기저 효과 신차 효과보다 더 중요한 모빌리티 비전 구체화, 현대차-년도년도 2분기 4분기 Review: 실적 쇼크는 피했다, 년도년도 2분기 4분기 Review: 실적 쇼크는 피했다, 2022 년 영업이익률 5.5~6.5% 가이던스 제시, 대외 불확실성 크지만 펀더멘탈 리스크는 크지 않은 상황, 현대차-22년도 1분기 반도체 품귀 현상 지속, 21년도 4분기 연결 매출 31조원(전년 대비 증감율+6%), 영업이익 1.53조원(+22%), OPM 4.9%, 차량사업 매출 25조원(전년 대비 증감율+7%), 영업이익 1.06조원(+49.2%), OPM 4.2%, 사측은 반도체 수급 22년도 2분기 점진적 개선, 22년도 3분기 정상화 예상., 현대차-간만에 집 정리 좀 했습니다, 비용 증가로 영업이익 컨센서스 15% 하회, 상품 경쟁력은 여전히 탄탄, 전기차 경쟁력 회복에 주목, 현대차-4Q Review: 안도감을 준 원가율과 가이던스, 4분기 영업이익 하회, 긍정 요인, 배당과 2022년 가이던스, 완성차, 사업구조 변화의 시기, 현대차, 자동차 수익성은 아쉽지만 '판매 목표 기대', 현대차-근본적인 변화가 필요한 시점, 21년도 4분기 , 낮아진 기대치도 하회, 생산 정상화 시점과 원가 부담, 3월 전후 변곡점, 현대차, 생산 지난해 3분기 저점…"판매 개선 지속"-키움, “스마트시티 초석 다진다” 현대차그룹, 싱가포르서 미래 교통수요 분석, 현대ENG 국내 최고층 모듈러 주택 '용인 영덕' 이달 착공, 현대ENG, 13층 국내 최고층 모듈러주택 이달 말 착공, 현대차, 올해 생산 정상화, 추가 성장 가능 기대 -신한, 헌혈하려고 사는 공혈견…현대차·건대, 문제 해결위해 머리 맞댄다, 현대차-건국대, 반려견 헌혈 문화 조성 위한 MOU 체결, 현대차, 생산차질 우려 여전…목표주가 17% 하향-SK, '현대차+제네시스' SUV 판매비중 50% 넘었다, 현대차, 건국대에 10억 후원 '반려동물 헌혈센터' 설립, 현대차, 건국대에 5년간 10억원 지원…반려견 헌혈 문화 조성한다, 현대차그룹, 싱가포르 주롱도시공사와 미래 교통수요 분석 위한 MOU, "현대차, 물류 비용·원자재 가격 상승 부담 확대에 목표가↓"-메리츠, "현대차, 물류·원자재 비용 부담…목표가 12% ↓", 현대차, 4분기 실적 예상보다 하회…올해 추가적인 성장 기대-하이, "현대차, 물류 비용·원자재 가격 상승 부담 확대에 목표가↓"-메리츠, "현대차, 물류·원자재 비용 부담…목표가 12% ↓", 현대차, 건국대에 5년간 10억원 지원…반려견 헌혈 문화 조성한다, 현대차, 건국대에 10억 후원 '반려동물 헌혈센터' 설립, 현대차그룹, 싱가포르 주롱도시공사와 MOU…미래 교통체계 실증한다, 현대차, 생산 지난해 3분기 저점…"판매 개선 지속"-키움, 현대차, 4분기 실적 예상보다 하회…올해 추가적인 성장 기대-하이</t>
+    <t>현대차 "올해 판매 목표 432만대…투자계획은 9.2조", 현대차 "아이오닉6 전기차, 올해 하반기 국내 출시", "117.6조원"…현대차, 매출 창사 이래 최대(상보), 현대차, 지난해 영업이익 6조6789억원, 현대차, 지난해 4분기 영업이익 1조5297억원…전년동기比 2..., 현대차 "올해 판매 목표 432만대… 투자 계획 9.2조" [주목 e..., 현대차, 車반도체난 뚫고 '사상 최대 실적'…"올해 432만대 팔겠다"..., 현대차, 지난해 4분기 영업이익 1조5297억원…전년동기比 2..., 정의선의 현대차, 악재뚫고 질주…작년 매출 117조 '사상 최대', 현대차, 지난해 기말 배당금 4000원…전년보다 1000원 인상, 현대차, 4분기 영업익 21.9% 증가…"제네시스가 효자"(상보), 현대차 작년 영업익 6조6789억원…"반도체난 뛰어 넘었다"(종합), 현대차 "올해 3분기 車 반도체 공급 정상화 전망", "올해 친환경차 판매 목표 대수 56.4만대"-현대차 컨콜, "그랜저 풀체인지·아이오닉6 출시…올해 내수 판매량 73.2만대 목표"..., 현대차, 지난해 영업이익 6조6789억원, 현대차, 지난해 영업이익 6조6789억원, "그랜저 풀체인지·아이오닉6 출시…올해 내수 판매량 73.2만대 목표"..., 현대차, 보통주 4000원·종류주 4100원 현금배당 결정, "올해 3분기 차량용 반도체 공급 정상화 예상"-현대차 컨콜, 현대차, 보통주 주당 4000원 현금배당 결정, 현대차, 車반도체난 뚫고 '사상 최대 실적'…"올해 432만대 팔겠다"..., 햇살론 카드 발급 실적 1위는 삼성카드 ... 현대·신한 뒤이어, 현대차, 보통주 1주당 4000원 기말 현금배당 결정, (영상)내달 상장 앞둔 현대ENG…오너 자금줄? 신사업 박차?, "현대ENG 공모로 친환경 1.5조 투자", 현대차, 올 판매목표 432만대… 전기차 56% 늘린다, 현대차, 매출 117조 '신기록'…올 9.2조 투자, '구주매출' 우려 속 건설대장주 노린다…현대엔지, 코스피 출격, 반도체 품귀 넘었다... 현대차 역대급 실적, "매출 117조6000억원"…현대차, 새 역사 썼다, "고맙다, 제네시스"…현대차, 반도체 부족에도 역대최대 매출, 제네시스·아이오닉5, 역시 어려울 때 효자…현대차 4분기 영업익 1조..., 현대차 '반도체 대란' 뚫고 최대실적…"올 432만대 판다", "고맙다, 제네시스"…현대차, 반도체 부족에도 역대최대 매출, 제네시스·아이오닉5, 역시 어려울 때 효자…현대차 4분기 영업익 1조..., "현대ENG 공모로 친환경 1.5조 투자", 현대ENG “2030년 플랜트·건축·신사업 3각 포트폴리오 구축”, 현대차 '반도체 대란' 뚫고 최대실적…"올 432만대 판다", 현대차, 작년 4분기 영업익 1조5297억원...전년比 22%↑, 비상걸린 삼성·LG전자·현대차…달러결제 금지하면 수출입도 직격탄, “삼성·현대차도 불안” 러시아·우크라 싸움 불똥이 왜 우리 기업한테…..., 현대차 "아이오닉6·그랜저 풀체인지, 올 하반기 국내 출시", 현대차 "아이오닉6 전기차, 올해 하반기 국내 출시", 현대차 “올해 제네시스·SUV 내수 판매 비중 50%로…전동화 박차”, 현대차, 지난해 기말 배당금 4000원…전년보다 1000원 인상, 현대차, 4분기 영업익 1조5297억원…전년보다 21.9%↑, 현대ENG IPO 임박..현대차 지배구조 개편 나서나, 현대자동차 지난해 영업익 6조6789억원…전년 대비 178.9%↑, "117.6조원"…현대차, 매출 창사 이래 최대(상보), 점진적 개선 전망, 반도체 공급 차질, 비용 증가 등으로 컨센서스 하회, 반도체 공급 부족 3분기에는 정상화될 것으로 예상, 22년 판매 목표 432만대 제시, 목표가 25만원으로 11% 하향, 매수 의견 유지, 년도년도 2분기 4분기 Review: 큰 실망은 필요다,년도 분기 년도년도 2분기 4분기 영업손익은 시장 및 KB증권의 전망을 하회했지만 크게 실망할 필요는다,년도 분기 년도년도 2분기 4분기 영업이익 1.5조원 (+21.9% 전년 대비 증감율), 시장 컨센서스를 15.0% 하회, 현재까지 원재료비 증가에 따른 수익성 압박은 없다는 점, 반도체 수급에 대한 우호적 전망에 주목해야, 빛 바랜 분기 최대 매출, 21년도 4분기 영업이익 세전이익, 컨센서스 -15%, -29% 하회, 2022년, C19 기저 효과 신차 효과보다 더 중요한 모빌리티 비전 구체화, "매출 117조, 영업익 7조"…현대차, 작년 역대급 실적 기대, “삼성·현대차도 불안” 러시아·우크라 싸움 불똥이 왜 우리 기업한테…[..., '대한민국 최고의 차' 막판 명승부 펼친다…"벤츠·BMW냐 제네시스·현..., ‘내비게이션까지 차질’...현대차 반도체 수급난에 출고 1년 넘게 걸린..., '구주매출' 우려 속 건설대장주 노린다…현대엔지, 코스피 출격, 상장 앞둔 현대엔지니어링 “현대차그룹 에너지 전담 회사로 거듭나겠다”, 유럽서 벤츠·BMW 꺾은 현대차, 비결은, 김창학 현대ENG 대표 "상장 계기로 친환경사업 역량 강화", IPO 대어 또 온다…현대ENG, 고평가 논란 털고 건설 대장주 등극?, 현대차, 4분기 영업익 1.53조원…전년比 21.9%↑, 현대차, 2021년 4분기 매출 31조· 영업익 1.5조…전년比 6·5..., 현대차, 4분기 영업익 1조5297억...전년비 21.9% 증가, 현대차, 작년 영업익 6.67조원…전년比 178.9%↑, 현대차, 4분기 영업익 1조5297억…전년비 21.9% ↑, 현대차, 지난해 영업익 6조6789억…전년비 178.9% ↑, 현대차 "올해 판매 목표 432만대… 투자 계획 9.2조" [주목 e공..., 현대차, 4분기 영업익 1조5297억…전년비 21.9% ↑, 현대차, 4분기 영업익 21.9% 증가…"제네시스가 효자"(상보), 현대차, 작년 영업이익 6조 6,789억 원...전년比 178.9% 증..., 현대차 4분기 매출 31조265억-영업이익 1조5297억, 현대차, 작년 매출액 117조원…전년比 13.1%↑, 현대차, 4분기 영업익 1조5297억원…전년보다 21.9%↑, 현대차, 작년 영업익 6조6789억…연간 389만대 판매, 현대차, 지난해 매출 117조 사상 최대…영업익 전년比 178.9%↑, 현대차, 2021년 매출 117.6조·영업익 6.7조원…전년比 ..., 현대차, 4분기 매출액 31조원…전년比 6.1%↑</t>
+  </si>
+  <si>
+    <t>현대차, 올해 아프리카·중동서 30만대 이상 판다, 현대차·모비스, 반도체 품귀에 발목…기아만 애플카 기대↑, 차량용 반도체 품귀 불똥…현대차·모비스 ‘고전’, 현대차, 올해 아프리카·중동서 30만대 이상 판다, 현대차그룹, 싱가포르 주롱도시공사와 미래 교통수요 분석 위한 MOU, 차량용 반도체 품귀 불똥…현대차·모비스 ‘고전’, 현대차證, 영업익 1500억원 돌파···“IB 부문 성과가 견인”, 현대차證, 사상 첫 영업이익 1,500억 돌파, ‘미래 교통체계 실증’ 현대차그룹, 싱가포르 주롱도시공사와 MOU, 현대차·모비스, 반도체 품귀에 발목…기아만 애플카 기대↑, ‘현대차 사내 벤처 출신’ 오토앤, 장 초반 18% 급등, 현대차그룹, 싱가포르서 '자율주행·전기차' 미래 교통수요 분석, 현대차 "개인용 비행체(PAV) 시제품, ..., 그린모빌리티상 '최우석 현대차 전동화시험센..., 공정위, 현대차-LG엔솔 합작사 등 전기차 M&amp;A 줄줄이 승인, 공정위 "현대차-LG엔솔 합작사 등 전기차 M&amp;A심사 신속 승인", 현대ENG 국내 최고층 모듈러 주택 '용인 영덕' 이달 착공, 현대ENG, 13층 국내 최고층 모듈러주택 이달 말 착공, 현대차그룹, 싱가포르 주롱도시공사와 미래 교통수요 분석 위한 MOU, 헌혈하려고 사는 공혈견…현대차·건대, 문제 해결위해 머리 맞댄다, 현대차, 싱가포르 스마트시티 조성 나선다...미래 교통분석 MOU 체결, 현대자동차, 건국대학교와 반려견 헌혈 문화 조성 MOU, '수입차 무덤' 일본에 또…현대차, 13년 만의 재도전 성공할까, 현대차그룹, 싱가포르와 미래교통수요 분석 협약, '수입차 무덤' 일본에 또…현대차, 13년 만의 재도전 성공할까, 현대차그룹 4형제, 지난해 나란히 역대 최대 실적 기록(종합), IB가 실적 견인… 현대차證 영업익 1500억원 돌파, 현대차證, 사상 첫 영업이익 1,500억 돌파, '급락장 유탄’ 맞은 현대엔지, 공모가 하단 유력, 현대차그룹 '미래차 시험기지' 싱가포르 낙점, 현대차그룹, 싱가포르와 미래교통수요 분석 협약, 현대차그룹, 싱가포르 주롱도시공사와 MOU…미래 교통체계 실증한다, 현대차그룹 4형제, 지난해 나란히 역대 최대 실적 기록(종합), IB가 실적 견인… 현대차證 영업익 1500억원 돌파, 현대차證, 사상 첫 영업이익 1,500억 돌파, '급락장 유탄’ 맞은 현대엔지, 공모가 하단 유력, 현대차그룹 '미래차 시험기지' 싱가포르 낙점, 현대차그룹, 싱가포르와 미래교통수요 분석 협약, 건국대 ‘반려견 헌혈문화 조성’ 업무협약, 현대차, 건국대에 10억 후원 '반려동물 헌혈센터' 설립, 현대차 52주 신저가 경신…기아는 1.57%↑, 공정위, 현대차-LG엔솔 합작사 설립 승인…"전기차 M&amp;A 신속 심사", 공정위, 현대차-LG엔솔 합작 등 "전기차 시장 M&amp;A 활성화", IB 활약에…현대차·KTB證 역대급 실적, 현대차證, 작년 4Q 영업익 33% 증가, 현대차, 싱가포르 스마트시티 조성 나선다...미래 교통분석 MOU 체..., 헌혈하려고 사는 공혈견…현대차·건대, 문제 해결위해 머리 맞댄다, 현대차그룹, 싱가포르 주롱도시공사와 MOU…미래 교통체계 실증한다, 현대차그룹, 싱가포르서 '자율주행·전기차' 미래 교통수요 분석, 현대차, 빛 바랜 분기 최대 매출-메리츠, 이제 내 차 빨리 받을 수 있을까…현대차 "올 3분기 車 반도체 정상화..., 현대차, GV80 내세워 작년 美 최다판매…올해는 '제네시스 G90' ..., 이제 내 차 빨리 받을 수 있을까…현대차 "올 3분기 車 반도체 정상화..., 현대차, 빛 바랜 분기 최대 매출-메리츠, 현대차, GV80 내세워 작년 美 최다판매…올해는 '제네시스 G90' ..., 아쉬운 수익성과 희망적 가이던스, 4분기 영업이익 1.53조원, 당사 추정 및 컨센서스 하회, 2022년 판매목표 432만대, 희망적 가이던스, 아쉬움과 기대감이 공존하는 구간, 21년도 4분기 Review: 자동차 부문의 수익성 악화가 아쉬웠으나, 22년도 1분기 Preview: 차량용 반도체 쇼티지는 지속, CEO Investor Day 기대감, 건국대, 반려견 헌혈 문화 조성 위한 MOU 체결, 현대차, 빛 바랜 분기 최대 매출, 년도년도 2분기 4분기 Review-여전히 남아있는 생산차질 우려, 년도년도 2분기 4분기 Review-여전히 남아있는 생산차질 우려, 월초 판매/생산 데이터에 주목할 필요, 년도년도 2분기 4분기 Review: 개선될 여지가 많은 2022년, 년도년도 2분기 4분기 (P): 매출액 31조 265억원, 영업이익 1조 5,297억원, 2022년 판매대수 429만대로 전년 대비 증감율 +10.3% 증가 전망, 수익성 개선은 믹스 변화로, 성장은 전기차로, 매출액 130조원 시대 개막, 투자포인트 및 결론, 주요이슈 및 실적전망, 주가전망 및 Valuation, 4분기 부진보다는 올해 긍정적 가이던스 주목, 년도년도 2분기 4분기 Review: 시장 기대치 하회, 22년 긍정적 가이던스 제시, 투자의견 ‘Buy’, 목표주가 300,000원 유지, 빛 바랜 분기 최대 매출, 21년도 4분기 영업이익 세전이익, 컨센서스 -15%, -29% 하회, 2022년, C19 기저 효과 신차 효과보다 더 중요한 모빌리티 비전 구체화, 년도년도 2분기 4분기 Review: 실적 쇼크는 피했다, 년도년도 2분기 4분기 Review: 실적 쇼크는 피했다, 2022 년 영업이익률 5.5~6.5% 가이던스 제시, 대외 불확실성 크지만 펀더멘탈 리스크는 크지 않은 상황, 22년도 1분기 반도체 품귀 현상 지속, 21년도 4분기 연결 매출 31조원(전년 대비 증감율+6%), 영업이익 1.53조원(+22%), OPM 4.9%, 차량사업 매출 25조원(전년 대비 증감율+7%), 영업이익 1.06조원(+49.2%), OPM 4.2%, 사측은 반도체 수급 22년도 2분기 점진적 개선, 22년도 3분기 정상화 예상., 간만에 집 정리 좀 했습니다, 비용 증가로 영업이익 컨센서스 15% 하회, 상품 경쟁력은 여전히 탄탄, 전기차 경쟁력 회복에 주목, 4Q Review: 안도감을 준 원가율과 가이던스, 4분기 영업이익 하회, 긍정 요인, 배당과 2022년 가이던스, 완성차, 사업구조 변화의 시기, 현대차, 자동차 수익성은 아쉽지만 '판매 목표 기대', 근본적인 변화가 필요한 시점, 21년도 4분기 , 낮아진 기대치도 하회, 생산 정상화 시점과 원가 부담, 3월 전후 변곡점, 현대차, 생산 지난해 3분기 저점…"판매 개선 지속"-키움, “스마트시티 초석 다진다” 현대차그룹, 싱가포르서 미래 교통수요 분석, 현대ENG 국내 최고층 모듈러 주택 '용인 영덕' 이달 착공, 현대ENG, 13층 국내 최고층 모듈러주택 이달 말 착공, 현대차, 올해 생산 정상화, 추가 성장 가능 기대 -신한, 헌혈하려고 사는 공혈견…현대차·건대, 문제 해결위해 머리 맞댄다, 건국대, 반려견 헌혈 문화 조성 위한 MOU 체결, 현대차, 생산차질 우려 여전…목표주가 17% 하향-SK, '현대차+제네시스' SUV 판매비중 50% 넘었다, 현대차, 건국대에 10억 후원 '반려동물 헌혈센터' 설립, 현대차, 건국대에 5년간 10억원 지원…반려견 헌혈 문화 조성한다, 현대차그룹, 싱가포르 주롱도시공사와 미래 교통수요 분석 위한 MOU, "현대차, 물류 비용·원자재 가격 상승 부담 확대에 목표가↓"-메리츠, "현대차, 물류·원자재 비용 부담…목표가 12% ↓", 현대차, 4분기 실적 예상보다 하회…올해 추가적인 성장 기대-하이, "현대차, 물류 비용·원자재 가격 상승 부담 확대에 목표가↓"-메리츠, "현대차, 물류·원자재 비용 부담…목표가 12% ↓", 현대차, 건국대에 5년간 10억원 지원…반려견 헌혈 문화 조성한다, 현대차, 건국대에 10억 후원 '반려동물 헌혈센터' 설립, 현대차그룹, 싱가포르 주롱도시공사와 MOU…미래 교통체계 실증한다, 현대차, 생산 지난해 3분기 저점…"판매 개선 지속"-키움, 현대차, 4분기 실적 예상보다 하회…올해 추가적인 성장 기대-하이</t>
   </si>
   <si>
     <t>현대ENG, 수요예측 기관들 ‘냉랭’…상장 여부 ‘안갯속’, 현대트랜시스, 미래 모빌리티 시트 콘셉트 공개, 현대차·기아, 올해 목표 747만대…관건은 ‘반도체’, 현대차 13년만에 일본차 시장 재진출, '현대차 판매왕' 年 423대 팔았다…"매번 아쉬운 2위였는데 드디어..., 현대차 ‘반려견 헌혈문화 조성’ 5년간 10억원 후원, 신사업 따라가면 ‘현대차 미래’ 보인다, 현대차 ‘2021년 전국 판매왕’ 김기양 대전지점 영업부장, 신사업 따라가면 ‘현대차 미래’ 보인다, 현대트랜시스, 미래 모빌리티 시트 콘셉트 공개, 현대차그룹, 건설·철강 협력사 안전관리에 870억원 지원, '현대차 판매왕' 年 423대 팔았다…"매번 아쉬운 2위였는데 드디어", "혼자서 5364대 팔았다, 아이오닉5도 큰힘"…'현대차 판매왕'에 ..., 현대차그룹, 건설·철강 분야 협력업체 안전관리에 870억원 투입, 한발 앞선 현대차·기아, 유럽서 사이버보안 인증, 작년 현대차 최다 판매 직원 배출한 지역은?, 현대차 대전지점 김기양 영업부장 ‘판매왕’…작년 423대 판매, 현대차그룹, 협력업체 중대재해도 막는다...예산 2배로 늘려, 현대차그룹, 건설·철강 분야 협력업체 안전관리에 870억원 투입, 현대차, 건설·철강 협력사 안전관리에 870억 투입…'2배 상향', 현대차그룹, 건설?철강 협력업체 안전관리 지원 강화, (영상)빨간불 켜진 현대ENG IPO…외면받는 이유는, 현대차그룹, 건설·철강 협력사 안전관리에 870억 투입, "현장 안전 최우선" 현대차그룹, 협력사에 870억, 현대차 노사, 사회공헌 기금 10억 기탁, 현대차그룹, 건설·철강 분야 협력업체 안전관리에 870억원 투입, 현대차그룹, 협력사에 870억 지원…현대重, 안전인력 20% 증원, 현대차 ‘2021년 전국 판매왕’ 김기양 대전지점 영업부장, 만년 2위였던 영업부장, 현대차 '판매왕' 올랐다</t>
@@ -7645,7 +7645,7 @@
     <t>SUV·친환경차 앞세운 현대차 1월에도 美서 신기록, 현대차·기아 매출 200조 시대 연다, SUV·친환경차 앞세운 현대차 1월에도 美서 신기록, 현대차·기아 매출 200조 시대 연다, 지난해 출시 현대차·기아 전기차 10만대 돌파...성장 속도 붙어, 현대차·기아, 전용 전기차 판매 10만대 돌파, 지난해 출시 현대차·기아 전기차 10만대 돌파...성장 속도 붙어, 변동성엔 안정적 실적 주목…현대차·삼바, 미국 판매 역주행하는 일본차…현대차·기아 홀로 '1월 신기록', '1월 美판매 신기록' 현대차, 올해 제네시스 전기차로 호실적 이어간..., 현대차 '동남아 진격'…90% 점유한 일본車에 도전, 현대차·기아, 전용 전기차 판매 10만대 돌파, 현대차 '동남아 진격'…90% 점유한 일본車에 도전, 현대차 1월 美 판매 신기록…기아는 친환경차 선전, 변동성엔 안정적 실적 주목…현대차·삼바, 10개월만에 10만대 돌파…현대차·기아 전용 전기차 ‘가속페달’, 현대차, 1월 美 판매 ‘역대 최다’…기아는 전기차 신기록, 네이버·현대차 푹 빠진 '디지털트윈' 뭐길래, 현대차 호주에 수소충전소 건립…‘탄소배출 제로’ 탄력, 현대차 사위家 코렌텍 오너 형제의 CB 딜레마, 네이버·현대차 푹 빠진 '디지털트윈' 뭐길래, 현대차, 1월 美 판매 ‘역대 최다’…기아는 전기차 신기록, 현대차 1월 美 판매 신기록…기아는 친환경차 선전, 현대차 사위家 코렌텍 오너 형제의 CB 딜레마, 현대차·기아 전용 전기차, 글로벌 판매 10만 대 돌파, 현대차 호주에 수소충전소 건립…‘탄소배출 제로’ 탄력, 변동성엔 안정적 실적 주목…현대차·삼바</t>
   </si>
   <si>
-    <t>현대차, 아산공장 생산 재개…전기차 생산 준비 완료, 현대차, 아산공장 전기차 생산라인 구축...아이오닉6 나온다, 현대차, '캐스퍼 밴' 출시…뒷좌석 비워 적재공간 940ℓ 확보, 27년간 5000대 판 김주선 현대차 부장 '판매 거장'반열에, 현대차, '캐스퍼 밴' 출시…뒷좌석 비워 적재공간 940ℓ 확보, 김주선 현대차 영업부장, ‘5000대 판매거장’ 선정, 현대차, 1월 28만2204대 판매...전년대비 12.1% 감소, 카드사-대형가맹점 수수료 줄다리기 돌입…3년전 현대차 전철 밟나 우려, 현대차, 1월 28만2204대 판매…전년비 12.1% 감소, '현대엔지' 없지만…이달 강소기업 9곳 IPO 출격, 현대차 공간 활용성 높인 ‘캐스퍼 밴’ 출시, '다마스 대신할까' 현대차, '적재 특화' 캐스퍼 밴 출시…1375만..., "트렁크 넓어졌네"…현대차, 캐스퍼 밴 출시, 카드사, 2019년 현대차 전철 밟을까 노심초사…대형 가맹점과 수수료..., 삼성·현대차·SK·LG가 떤다…기업들 연초부터 ‘비상’ 왜? [비즈36..., 이어지는 생산차질…현대차, 판매량 전년비 12%↓, 현대차, 1월 28만2204대 판매…작년보다 12.1% 줄었다, 반도체 품귀에 출고 지연…현대차 1월 판매 12% '뚝', 27년간 5000대 판 김주선 현대차 부장 '판매 거장'반열에, 현대차, 아산공장 전기차 생산라인 구축...아이오닉6 나온다, (영상)"현대ENG 참패했는데" 2월 공모기업 9개사...흥행할까, 반도체 부족에…현대차 1월 판매 12%↓, 현대차, 1월 28만2204대 판매…작년보다 12.1% 줄었다, 현대차 ‘15번째 판매거장’ 김주선 영업부장, 27년간 5000대 판 김주선 현대차 부장 '판매 거장'반열에, 반도체 품귀에 출고 지연…현대차 1월 판매 12% '뚝', "트렁크 넓어졌네"…현대차, 캐스퍼 밴 출시, 현대차, '캐스퍼 밴' 출시…뒷좌석 비워 적재공간 940ℓ 확보, (영상)"현대ENG 참패했는데" 2월 공모기업 9개사...흥행할까, 반도체 부족에…현대차 1월 판매 12%↓, 현대차, 1월 28만2204대 판매…작년보다 12.1% 줄었다, 현대차 ‘15번째 판매거장’ 김주선 영업부장, 현대차, 반도체난에 설연휴 휴업···1월 판매 12.1%↓, 반도체 품귀에 출고 지연…현대차 1월 판매 12% '뚝', "트렁크 넓어졌네"…현대차, 캐스퍼 밴 출시, 현대차, 아산공장 생산 재개…전기차 생산 준비 완료, 현대차 아산공장 전기차 생산준비 완료…아이오닉6 출격 준비, '현대엔지' 없지만…이달 강소기업 9곳 IPO 출격, 적재량 940ℓ…현대차, ‘캐스퍼 밴’ 출시, 현대차, 아산공장 전기차 라인 공사 마쳐…하반기 아이오닉6 출시 채비, 현대차, '캐스퍼 밴' 출시…뒷좌석 비워 적재공간 940ℓ 확보, 현대자동차, 아산공장 생산재개, 카드사, 2019년 현대차 전철 밟을까 노심초사…대형 가맹점과 수수료 ..., '다마스 대신할까' 현대차, '적재 특화' 캐스퍼 밴 출시…1375만원, "현대차·기아 지지부진한 BEV 전략…현대위아 목표가↓"-메리츠, 현대자동차, 아산공장 생산재개, 현대차, '캐스퍼 밴' 출시…뒷좌석 비워 적재공간 940ℓ 확보, 현대차-년도년도 2분기 4분기 NDR Review: ASP 상승과 EV 투자 감,년도 자분기 년도년도 2분기 4분기 영업이익은 1.53조원(+21.9% 전년 대비 증감율, OPM 4.9%) 기록, 컨센서스 15.0% 하회, 년도년도 2분기 4분기 총평: 반도체 차질과 재고 부족으로 글로벌 도매판매 감소, 가이던스: 도매판매 11% 증가에도 연결 매출액이 13% 증가하는 배경에는 2021년 사업 호조에 따른 금융 부분의 보수적인 목표 설정과 환율의 부정적 효과를 반영함에 기인, "현대차·기아 지지부진한 BEV 전략…현대위아 목표가↓"-메리츠, 현대차 김주선 영업부장, ‘판매거장’ 선정, 현대차, 캐스퍼 밴 출시…공간 활용성 높인 ‘꼬마 장사’, 더 넓어진 캐스퍼...현대차 '캐스퍼 밴' 출시, 적재량 940ℓ…현대차, ‘캐스퍼 밴’ 출시, 카드사, 2019년 현대차 전철 밟을까 노심초사…대형 가맹점과 수수료 ..., 현대차, 캐스퍼 밴 출시…공간 활용성 높인 ‘꼬마 장사’, (영상)현대차·기아, 美시장 1월 판매 `역대 최다`…친환경차 판매 급..., 김주선 현대차 영업부장, ‘5000대 판매거장’ 선정, 누적 5000대 ‘판매거장’ 김주선 현대차 영업부장, 현대차 공간 활용성 높인 ‘캐스퍼 밴’ 출시, '다마스 대신할까' 현대차, '적재 특화' 캐스퍼 밴 출시…1375만..., 카드사-대형가맹점 수수료 줄다리기 돌입…3년전 현대차 전철 밟나 우려, 카드사, 2019년 현대차 전철 밟을까 노심초사…대형 가맹점과 수수료..., 현대차 캐스퍼, 이번엔 밴으로 나왔다…적재공간 940L, 삼성·현대차·SK·LG가 떤다…기업들 연초부터 ‘비상’ 왜? [비즈36..., 현대차 캐스퍼, 이번엔 밴으로 나왔다…적재공간 940L, 현대차, 캐스퍼 밴 출시…공간 활용성 높인 ‘꼬마 장사’, 현대차, '캐스퍼 밴' 출시…뒷좌석 비워 적재공간 940ℓ 확보, 적재량 940ℓ…현대차, ‘캐스퍼 밴’ 출시, "혼자서 5000대 팔았다"…'현대차 판매거장' 탄생, 14명 더 있다, 현대차 5000대 넘게 판 '판매거장' 비결 들어보니, 삼성·현대차·SK·LG가 떤다…기업들 연초부터 ‘비상’ 왜? [비즈36..., (영상)현대차·기아, 美시장 1월 판매 `역대 최다`…친환경차 판매 급..., '다마스 대신할까' 현대차, '적재 특화' 캐스퍼 밴 출시…1375만원</t>
+    <t>현대차, 아산공장 생산 재개…전기차 생산 준비 완료, 현대차, 아산공장 전기차 생산라인 구축...아이오닉6 나온다, 현대차, '캐스퍼 밴' 출시…뒷좌석 비워 적재공간 940ℓ 확보, 27년간 5000대 판 김주선 현대차 부장 '판매 거장'반열에, 현대차, '캐스퍼 밴' 출시…뒷좌석 비워 적재공간 940ℓ 확보, 김주선 현대차 영업부장, ‘5000대 판매거장’ 선정, 현대차, 1월 28만2204대 판매...전년대비 12.1% 감소, 카드사-대형가맹점 수수료 줄다리기 돌입…3년전 현대차 전철 밟나 우려, 현대차, 1월 28만2204대 판매…전년비 12.1% 감소, '현대엔지' 없지만…이달 강소기업 9곳 IPO 출격, 현대차 공간 활용성 높인 ‘캐스퍼 밴’ 출시, '다마스 대신할까' 현대차, '적재 특화' 캐스퍼 밴 출시…1375만..., "트렁크 넓어졌네"…현대차, 캐스퍼 밴 출시, 카드사, 2019년 현대차 전철 밟을까 노심초사…대형 가맹점과 수수료..., 삼성·현대차·SK·LG가 떤다…기업들 연초부터 ‘비상’ 왜? [비즈36..., 이어지는 생산차질…현대차, 판매량 전년비 12%↓, 현대차, 1월 28만2204대 판매…작년보다 12.1% 줄었다, 반도체 품귀에 출고 지연…현대차 1월 판매 12% '뚝', 27년간 5000대 판 김주선 현대차 부장 '판매 거장'반열에, 현대차, 아산공장 전기차 생산라인 구축...아이오닉6 나온다, (영상)"현대ENG 참패했는데" 2월 공모기업 9개사...흥행할까, 반도체 부족에…현대차 1월 판매 12%↓, 현대차, 1월 28만2204대 판매…작년보다 12.1% 줄었다, 현대차 ‘15번째 판매거장’ 김주선 영업부장, 27년간 5000대 판 김주선 현대차 부장 '판매 거장'반열에, 반도체 품귀에 출고 지연…현대차 1월 판매 12% '뚝', "트렁크 넓어졌네"…현대차, 캐스퍼 밴 출시, 현대차, '캐스퍼 밴' 출시…뒷좌석 비워 적재공간 940ℓ 확보, (영상)"현대ENG 참패했는데" 2월 공모기업 9개사...흥행할까, 반도체 부족에…현대차 1월 판매 12%↓, 현대차, 1월 28만2204대 판매…작년보다 12.1% 줄었다, 현대차 ‘15번째 판매거장’ 김주선 영업부장, 현대차, 반도체난에 설연휴 휴업···1월 판매 12.1%↓, 반도체 품귀에 출고 지연…현대차 1월 판매 12% '뚝', "트렁크 넓어졌네"…현대차, 캐스퍼 밴 출시, 현대차, 아산공장 생산 재개…전기차 생산 준비 완료, 현대차 아산공장 전기차 생산준비 완료…아이오닉6 출격 준비, '현대엔지' 없지만…이달 강소기업 9곳 IPO 출격, 적재량 940ℓ…현대차, ‘캐스퍼 밴’ 출시, 현대차, 아산공장 전기차 라인 공사 마쳐…하반기 아이오닉6 출시 채비, 현대차, '캐스퍼 밴' 출시…뒷좌석 비워 적재공간 940ℓ 확보, 현대자동차, 아산공장 생산재개, 카드사, 2019년 현대차 전철 밟을까 노심초사…대형 가맹점과 수수료 ..., '다마스 대신할까' 현대차, '적재 특화' 캐스퍼 밴 출시…1375만원, "현대차·기아 지지부진한 BEV 전략…현대위아 목표가↓"-메리츠, 현대자동차, 아산공장 생산재개, 현대차, '캐스퍼 밴' 출시…뒷좌석 비워 적재공간 940ℓ 확보, 년도년도 2분기 4분기 NDR Review: ASP 상승과 EV 투자 감,년도 자분기 년도년도 2분기 4분기 영업이익은 1.53조원(+21.9% 전년 대비 증감율, OPM 4.9%) 기록, 컨센서스 15.0% 하회, 년도년도 2분기 4분기 총평: 반도체 차질과 재고 부족으로 글로벌 도매판매 감소, 가이던스: 도매판매 11% 증가에도 연결 매출액이 13% 증가하는 배경에는 2021년 사업 호조에 따른 금융 부분의 보수적인 목표 설정과 환율의 부정적 효과를 반영함에 기인, "현대차·기아 지지부진한 BEV 전략…현대위아 목표가↓"-메리츠, 현대차 김주선 영업부장, ‘판매거장’ 선정, 현대차, 캐스퍼 밴 출시…공간 활용성 높인 ‘꼬마 장사’, 더 넓어진 캐스퍼...현대차 '캐스퍼 밴' 출시, 적재량 940ℓ…현대차, ‘캐스퍼 밴’ 출시, 카드사, 2019년 현대차 전철 밟을까 노심초사…대형 가맹점과 수수료 ..., 현대차, 캐스퍼 밴 출시…공간 활용성 높인 ‘꼬마 장사’, (영상)현대차·기아, 美시장 1월 판매 `역대 최다`…친환경차 판매 급..., 김주선 현대차 영업부장, ‘5000대 판매거장’ 선정, 누적 5000대 ‘판매거장’ 김주선 현대차 영업부장, 현대차 공간 활용성 높인 ‘캐스퍼 밴’ 출시, '다마스 대신할까' 현대차, '적재 특화' 캐스퍼 밴 출시…1375만..., 카드사-대형가맹점 수수료 줄다리기 돌입…3년전 현대차 전철 밟나 우려, 카드사, 2019년 현대차 전철 밟을까 노심초사…대형 가맹점과 수수료..., 현대차 캐스퍼, 이번엔 밴으로 나왔다…적재공간 940L, 삼성·현대차·SK·LG가 떤다…기업들 연초부터 ‘비상’ 왜? [비즈36..., 현대차 캐스퍼, 이번엔 밴으로 나왔다…적재공간 940L, 현대차, 캐스퍼 밴 출시…공간 활용성 높인 ‘꼬마 장사’, 현대차, '캐스퍼 밴' 출시…뒷좌석 비워 적재공간 940ℓ 확보, 적재량 940ℓ…현대차, ‘캐스퍼 밴’ 출시, "혼자서 5000대 팔았다"…'현대차 판매거장' 탄생, 14명 더 있다, 현대차 5000대 넘게 판 '판매거장' 비결 들어보니, 삼성·현대차·SK·LG가 떤다…기업들 연초부터 ‘비상’ 왜? [비즈36..., (영상)현대차·기아, 美시장 1월 판매 `역대 최다`…친환경차 판매 급..., '다마스 대신할까' 현대차, '적재 특화' 캐스퍼 밴 출시…1375만원</t>
   </si>
   <si>
     <t>현대차, 13년 만에 日재진출 임박…"전기차 100% 온라인 판매", 日 재진출 현대차 '온라인'으로 승부, 현대차 투싼·GV80·G80, 美영화 '언차티드'에 등장, 현대차 투싼, 스파이더맨 이어 영화 ‘언차티드’서 활약한다, 현대차 투싼, 영화 '언차티드'서 강력한 존재감 뽐낸다, 현대차 투싼·GV80·G80, 美영화 '언차티드'에 등장, 현대차, 13년 만에 日재진출 임박…"전기차 100% 온라인 판매", 日 재진출 현대차 '온라인'으로 승부, 톰 홀랜드 주연 영화 ‘언차티드’에 현대차 투싼, 신스틸러로, 현대차 투싼, 영화 '언차티드'서 강력한 존재감 뽐낸다, 지영조 현대차 사장 "도시와 일상의 변화, 핵심은 모빌리티", 톰 홀랜드 주연 영화 ‘언차티드’에 현대차 투싼, 신스틸러로, 현대차 투싼, 스파이더맨 이어 영화 ‘언차티드’서 활약한다, '톰 홀랜드 주연' 영화 언차티드에 현대차 투싼·제네시스 나온다, 현대자동차 '투싼' 영화 '언차티드'서 등장…"신스틸러로 활약", 톰 홀랜드 주연 영화 ‘언차티드’에 현대차 투싼, 신스틸러로, 현대차 투싼, 영화 '언차티드'서 강력한 존재감 뽐낸다, 현대차·기아, 탁송료 10% 가까이 올랐다, 현대차·기아, 탁송료 10% 가까이 올랐다, 지영조 현대차 사장 “스마트시티 핵심은 모빌리티”, 지영조 현대차그룹 사장 "모빌리티 혁신 위해선 메타버스 필수"</t>
@@ -7657,7 +7657,7 @@
     <t>현대차·SK가 투자한 SES, NYSE에 상장, 삼성·현대차·SK·LG 채용 스타트…인재 쟁탈전 '후끈', “일본을 다시 공략하라”…전기차 내세운 현대차, 성공할까, 삼성·현대차·SK·LG 채용 스타트…인재 쟁탈전 '후끈', 현대차·SK가 투자한 SES, NYSE에 상장, “일본을 다시 공략하라”…전기차 내세운 현대차, 성공할까</t>
   </si>
   <si>
-    <t>이상엽 현대차 디자인센터장, 직원 극단 선택에 결국 사과, 경쟁사 전기차 생산 확대하는데…현대차그룹은 ‘안갯속’, 일진하이솔루스 수소저장장치, 현대차 美수출 트럭 공급, 일진하이솔루스, 현대차와 북미 대형 수소트럭 시장 진출, "모빌리티 유망 벤처 모여라"…현대차 '제로원 액셀러레이터', 반도체 수급난에 막힌 현대기아차株, 언제쯤 달릴까, 새해에 달리지 못하는 현대기아차 주가..."3월 돼야 회복", 현대차·기아, 새 합작사·전기차로 中시장 재도약 나선다, 현대차, 글로벌 전기차 판매 톱5... 국내 시장선 테슬라 제치고 1위, 현대차-테슬라, 국내 전기차 양강구도…관건은 보조금, 일진하이솔루스, 현대차와 북미 대형 수소트럭 시장 진출, 현대차-테슬라, 국내 전기차 양강구도…관건은 보조금, 삼성도 현대차도 "웬만하면 나오지 마"…기업들 '초비상', 일진하이솔루스 수소저장장치, 현대차 美수출 트럭 공급, 일진하이솔루스, 현대차와 북미 대형 수소트럭 시장 진출, 반도체 수급난에 막힌 현대기아차株, 언제쯤 달릴까, 삼성도 현대차도 "웬만하면 나오지 마"…기업들 '초비상', 현대차·기아, 새 합작사·전기차로 中시장 재도약 나선다, 현대차, 글로벌 전기차 판매 톱5... 국내 시장선 테슬라 제치고 1위, 이상엽 현대차 부사장 “故 이찬희 애도…책임있다면 처벌 감당..., 일진하이솔루스, ?현대차와 북미 대형 수소 트럭 시장 진출, 현대차-테슬라, 국내 전기차 양강구도…관건은 보조금, 새해에 달리지 못하는 현대기아차 주가..."3월 돼야 회복", 현대차그룹 ‘제로원 엑셀러레이터’ 스타트업 모집, 현대차-생산확대 속 로봇 등 미래가치반영기대, 2022년판매 +11%, 매출액 +13~14%, OPM5.5~6.5%제시, Boston Dynamics인수 이후 메타모빌리티 등시너지 확대, 투자의견 매수, 목표주가 300,000원, 현대차그룹 ‘제로원 엑셀러레이터’ 스타트업 모집, 국내 전기차 시장, 현대차-테슬라 '양강구도' 뚜렷, 현대차그룹 글로벌 전기차 ‘톱5’…국내선 테슬라와 양강구도, 국내 전기차 시장, 현대차-테슬라 '양강구도' 뚜렷, 현대차그룹 글로벌 전기차 ‘톱5’…국내선 테슬라와 양강구도, "현대차, 생산 확대 속 로봇 등 미래가치 반영 기대"-IBK, 현대차그룹, 상반기 '제로원 엑셀러레이터' 스타트업 모집, "현대차그룹 현업팀과 함께 일할 스타트업 오세요", 현대차그룹, 첨단車 기술 스타트업 머리 맞댄다…내달까지 공모접수, 현대차그룹, 전기차·모빌리티 스타트업 발굴한다, 가상세계 ‘제페토’에서 현대車 소나타N 탄다, 일진하이솔루스, 현대차 대형 수소트럭 저장시스템 공급, 일진하이솔루스, 현대차 북미 수소트럭 연료탱크 공급사 선정, "현대차, 생산 확대 속 로봇 등 미래가치 반영 기대"-IBK, 현대차그룹, 상반기 '제로원 엑셀러레이터' 스타트업 모집, "현대차그룹 현업팀과 함께 일할 스타트업 오세요", 가상세계 ‘제페토’에서 현대車 소나타N 탄다, 현대캐피탈, 2월 현대차·제네시스·기아 전 차종 특별 프로모션, 이상엽 현대차 부사장 “故 이찬희 애도…책임있다면 처벌 감당할..., 현대차그룹, 상반기 '제로원 엑셀러레이터' 참가 스타트업 모집, 현대차그룹 글로벌 전기차 ‘톱5’…국내선 테슬라와 양강구도, 경쟁사 전기차 생산 확대하는데…현대차그룹은 ‘안갯속’</t>
+    <t>이상엽 현대차 디자인센터장, 직원 극단 선택에 결국 사과, 경쟁사 전기차 생산 확대하는데…현대차그룹은 ‘안갯속’, 일진하이솔루스 수소저장장치, 현대차 美수출 트럭 공급, 일진하이솔루스, 현대차와 북미 대형 수소트럭 시장 진출, "모빌리티 유망 벤처 모여라"…현대차 '제로원 액셀러레이터', 반도체 수급난에 막힌 현대기아차株, 언제쯤 달릴까, 새해에 달리지 못하는 현대기아차 주가..."3월 돼야 회복", 현대차·기아, 새 합작사·전기차로 中시장 재도약 나선다, 현대차, 글로벌 전기차 판매 톱5... 국내 시장선 테슬라 제치고 1위, 테슬라, 국내 전기차 양강구도…관건은 보조금, 일진하이솔루스, 현대차와 북미 대형 수소트럭 시장 진출, 테슬라, 국내 전기차 양강구도…관건은 보조금, 삼성도 현대차도 "웬만하면 나오지 마"…기업들 '초비상', 일진하이솔루스 수소저장장치, 현대차 美수출 트럭 공급, 일진하이솔루스, 현대차와 북미 대형 수소트럭 시장 진출, 반도체 수급난에 막힌 현대기아차株, 언제쯤 달릴까, 삼성도 현대차도 "웬만하면 나오지 마"…기업들 '초비상', 현대차·기아, 새 합작사·전기차로 中시장 재도약 나선다, 현대차, 글로벌 전기차 판매 톱5... 국내 시장선 테슬라 제치고 1위, 이상엽 현대차 부사장 “故 이찬희 애도…책임있다면 처벌 감당..., 일진하이솔루스, ?현대차와 북미 대형 수소 트럭 시장 진출, 테슬라, 국내 전기차 양강구도…관건은 보조금, 새해에 달리지 못하는 현대기아차 주가..."3월 돼야 회복", 현대차그룹 ‘제로원 엑셀러레이터’ 스타트업 모집, 생산확대 속 로봇 등 미래가치반영기대, 2022년판매 +11%, 매출액 +13~14%, OPM5.5~6.5%제시, Boston Dynamics인수 이후 메타모빌리티 등시너지 확대, 투자의견 매수, 목표주가 300,000원, 현대차그룹 ‘제로원 엑셀러레이터’ 스타트업 모집, 국내 전기차 시장, 현대차-테슬라 '양강구도' 뚜렷, 현대차그룹 글로벌 전기차 ‘톱5’…국내선 테슬라와 양강구도, 국내 전기차 시장, 현대차-테슬라 '양강구도' 뚜렷, 현대차그룹 글로벌 전기차 ‘톱5’…국내선 테슬라와 양강구도, "현대차, 생산 확대 속 로봇 등 미래가치 반영 기대"-IBK, 현대차그룹, 상반기 '제로원 엑셀러레이터' 스타트업 모집, "현대차그룹 현업팀과 함께 일할 스타트업 오세요", 현대차그룹, 첨단車 기술 스타트업 머리 맞댄다…내달까지 공모접수, 현대차그룹, 전기차·모빌리티 스타트업 발굴한다, 가상세계 ‘제페토’에서 현대車 소나타N 탄다, 일진하이솔루스, 현대차 대형 수소트럭 저장시스템 공급, 일진하이솔루스, 현대차 북미 수소트럭 연료탱크 공급사 선정, "현대차, 생산 확대 속 로봇 등 미래가치 반영 기대"-IBK, 현대차그룹, 상반기 '제로원 엑셀러레이터' 스타트업 모집, "현대차그룹 현업팀과 함께 일할 스타트업 오세요", 가상세계 ‘제페토’에서 현대車 소나타N 탄다, 현대캐피탈, 2월 현대차·제네시스·기아 전 차종 특별 프로모션, 이상엽 현대차 부사장 “故 이찬희 애도…책임있다면 처벌 감당할..., 현대차그룹, 상반기 '제로원 엑셀러레이터' 참가 스타트업 모집, 현대차그룹 글로벌 전기차 ‘톱5’…국내선 테슬라와 양강구도, 경쟁사 전기차 생산 확대하는데…현대차그룹은 ‘안갯속’</t>
   </si>
   <si>
     <t>'엔진 시대' 끝나간다…현대차 이어 닛산도 엔진 개발 종료, 현대차, 美 ‘에디터스 초이스 어워드’ 최다 수상…11개 모델 선정, 현대차, '차' 떼고 일본 재진출, 아이오닉5 앞세운 현대차, 日 시장 재도전…"두 번 실패 않겠다", 현대차, 美 ‘에디터스 초이스 어워드’ 최다 수상, 현대차그룹, 美자동차 전문지 시상식서 22개 모델 수상, 아이오닉5 앞세운 현대차, 日 시장 재도전…"두 번 실패 않겠다", 현대차, 부진 실적 딛고 日 승용차 시장 12년 만에 재진출, "아이오닉5·넥쏘 전면에"…현대차, 12년만에 일본 재진출, 현대차 日재진출 공식화…전기차 공유서비스, 현대차 사장 '유창한 일본어' 발표...日언론 "철저히 준비한 것 같..., 현대차의 심기일전… 12년만에 日 재진출, 현대·기아차 미국서 48만여대 리콜…“멈춰선 상태서 불 날 수 있어”, "美서 현대·기아차 미국서 48만여대 리콜", 현대차, 美 '에디터스 초이스 어워드' 11개 모델 선정…최다 수상, 현대·기아차 미국서 48만여대 리콜…“멈춰선 상태서 불 날 수 있어”, "美서 현대·기아차 미국서 48만여대 리콜", 현대차 사장 '유창한 일본어' 발표...日언론 "철저히 준비한 것 같다..., "미도지반의 자세" 현대차, 12년만에 日시장 재진출...5월 첫 판..., '수소차 양강' 현대차 넥쏘 vs 도요타 미라이 진검승부, "아이오닉5·넥쏘 전면에"…현대차, 12년만에 일본 재진출, 세계 수소차 1만7000대 팔렸다…현대차 점유율 53%, '엔진 시대' 끝나간다…현대차 이어 닛산도 엔진 개발 종료, 현대차, 美 전문지 선정 '에디터스 초이스 어워드' 최다 수상, 현대차, 12년만에 日시장 재진출…아이오닉5·넥쏘 친환경차 승부수, 현대차, 美 ‘에디터스 초이스 어워드’ 최다 수상, 두 배 커진 수소차시장, 절반은 현대차…3년 연속 1위, 현대차, 글로벌 수소차 판매 점유율 3년 연속 1위, 현대차가 '수입차 무덤' 日에 재진출 하는 이유…"전기차·온라인으로 승..., 현대차그룹, 美자동차 전문지 평가서 22개 모델 수상, 현대차, 美 전문지 선정 '에디터스 초이스 어워드' 최다 수상, 12년만에 日 재진출하는 현대차…온라인·친환경·카셰어링 앞세운다, 12년만에 日 재진출하는 현대차…온라인·친환경·카셰어링 앞세운다, 현대차, 글로벌 수소차 판매 점유율 3년 연속 1위, 현대자동차·기아, 올해 자율주행 로보택시 도심 달린다…"미래로봇 상용화..., 두 배 커진 수소차시장, 절반은 현대차…3년 연속 1위, 현대차, 美 ‘에디터스 초이스 어워드’ 최다 수상, 현대차그룹, 美자동차 전문지 평가서 22개 모델 수상</t>
@@ -7699,10 +7699,10 @@
     <t>강남 재건축, 호재에도 ‘관망세’… 압구정현대는 80억 신고가, 현대두산인프라, 삼성물산과 건설 장비 무인화 기술 추진, 현대두산인프라, 삼성물산과 건설 장비 무인화 기술 추진</t>
   </si>
   <si>
-    <t>베이징현대 충칭공장 가동 중단…"中 시장 판매 하락 원인", 현대차-턴어라운드 임박, 상저하고 기대, 2022년 글로벌 도매판매량은 419.4만대(전년 대비 증감율 +8.0%) 전망, 그룹사 내 영업이익률 개선이 2022~2024년에 걸쳐 가장 가파르게 개선, 금년 동사의 주가 catalyst는 E-GMP기반 차종의 해외 확대전개 속도, 베이징현대 충칭공장 가동 중단…"中 시장 판매 하락 원인", 로보틱스 선점 나선 현대차… 국내외 대규모 인재 채용, 로보틱스 선점 나선 현대차… 국내외 대규모 인재 채용, 현대차證 “대한제강 저평가 매력 충분”…목표가 2만5천원 ↑, 갈 길 먼 현대차 지배구조 개편, 정의선 선택은?, 폭스콘 전기차, 이젠 동남아도 달린다…현대차?LG에너지솔루..., "현대차, 연말로 갈수록 선명한 이익모멘텀…턴어라운드 기대", 폭스콘 전기차, 이젠 동남아도 달린다…현대차?LG에너지솔루...</t>
-  </si>
-  <si>
-    <t>현대차 中 충칭공장, 작년 12월 가동중단, 중국 판매 부진… 현대차 충칭 공장 셧다운, (영상)러시아-우크라 '일촉즉발'...현대차그룹 손익 타격 우려, 현대차-E-GMP 라인업 확대, 단기 불확실성 감안해도 Valuation 매력 높아, 2022년 자동차매출액 100조원 상회. 1분기 저점, 분기별 실적개선 전망, 현대차 G90, 기자들이 뽑은 올해의 차 선정, 현대차 中 충칭공장, 작년 12월 가동중단, 현대차 G90, 기자들이 뽑은 올해의 차 선정, (영상)러시아-우크라 '일촉즉발'...현대차그룹 손익 타격 우려, "현대차 25만대·롯데 에틸렌 연 100만t 생산"…韓-인니 협력 확대, 현대차 中 충칭공장, 작년 12월 가동중단, 중국 판매 부진… 현대차 충칭 공장 셧다운, (영상)러시아-우크라 '일촉즉발'...현대차그룹 손익 타격 우려, "현대차 25만대·롯데 에틸렌 연 100만t 생산"…韓-인니 협력 확대, 중국 판매 부진… 현대차 충칭 공장 셧다운</t>
+    <t>베이징현대 충칭공장 가동 중단…"中 시장 판매 하락 원인", 턴어라운드 임박, 상저하고 기대, 2022년 글로벌 도매판매량은 419.4만대(전년 대비 증감율 +8.0%) 전망, 그룹사 내 영업이익률 개선이 2022~2024년에 걸쳐 가장 가파르게 개선, 금년 동사의 주가 catalyst는 E-GMP기반 차종의 해외 확대전개 속도, 베이징현대 충칭공장 가동 중단…"中 시장 판매 하락 원인", 로보틱스 선점 나선 현대차… 국내외 대규모 인재 채용, 로보틱스 선점 나선 현대차… 국내외 대규모 인재 채용, 현대차證 “대한제강 저평가 매력 충분”…목표가 2만5천원 ↑, 갈 길 먼 현대차 지배구조 개편, 정의선 선택은?, 폭스콘 전기차, 이젠 동남아도 달린다…현대차?LG에너지솔루..., "현대차, 연말로 갈수록 선명한 이익모멘텀…턴어라운드 기대", 폭스콘 전기차, 이젠 동남아도 달린다…현대차?LG에너지솔루...</t>
+  </si>
+  <si>
+    <t>현대차 中 충칭공장, 작년 12월 가동중단, 중국 판매 부진… 현대차 충칭 공장 셧다운, (영상)러시아-우크라 '일촉즉발'...현대차그룹 손익 타격 우려, E-GMP 라인업 확대, 단기 불확실성 감안해도 Valuation 매력 높아, 2022년 자동차매출액 100조원 상회. 1분기 저점, 분기별 실적개선 전망, 현대차 G90, 기자들이 뽑은 올해의 차 선정, 현대차 中 충칭공장, 작년 12월 가동중단, 현대차 G90, 기자들이 뽑은 올해의 차 선정, (영상)러시아-우크라 '일촉즉발'...현대차그룹 손익 타격 우려, "현대차 25만대·롯데 에틸렌 연 100만t 생산"…韓-인니 협력 확대, 현대차 中 충칭공장, 작년 12월 가동중단, 중국 판매 부진… 현대차 충칭 공장 셧다운, (영상)러시아-우크라 '일촉즉발'...현대차그룹 손익 타격 우려, "현대차 25만대·롯데 에틸렌 연 100만t 생산"…韓-인니 협력 확대, 중국 판매 부진… 현대차 충칭 공장 셧다운</t>
   </si>
   <si>
     <t>현대자동차, 현대차증권 550억 MMT 매수, 현대차, 내달 24일 주총…정의선 사내이사로 재선임, 현대차, 정의선 회장 사내이사 재선임…내달 24일 주주총회, 루크 동커볼케 현대차 부사장, '세계 올해의 자동차인' 수상, 세계 올해의 자동차인에 동커볼케 현대차 부사장, 루크 동커볼케 현대차 부사장, '세계 올해의 자동차인' 수상, 중국서 고전하는 현대차?기아, 충칭공장 가동 ‘잠정 중단’, 중국서 고전하는 현대차?기아, 충칭공장 가동 ‘잠정 중단’, 세계 올해의 자동차인에 동커볼케 현대차 부사장, 현대차·기아, 충칭공장 스톱…中서 5년째 내리막, 중국서 고전하는 현대차?기아, 충칭공장 가동 ‘잠정 중단’, 현대차·기아, 충칭공장 스톱…中서 5년째 내리막, 현대차·기아, 충칭공장 스톱…中서 5년째 내리막, 루크 동커볼케 현대차 부사장, '세계 올해의 자동차인' 수상, 루크 동커볼케 현대차 부사장, '세계 올해의 자동차인' 수상, 루크 동커볼케 현대차그룹 부사장, ‘세계 올해의 자동차인’, KIAT, 인니 전기차 인프라 구축 나선다…현대차 ‘지원사격’, 세계 올해의 자동차인에 동커볼케 현대차 부사장, 루크 동커볼케 현대차그룹 부사장, '세계 올해의 자동차인' 선정, 동커볼케 현대차그룹 부사장, ‘세계 올해의 자동차인’ 선정, 루크 동커볼케 현대차그룹 부사장, '세계 올해의 자동차인' 선정, 동커볼케 현대차 부사장 ‘세계 올해의 자동차인’, KIAT, 인니 전기차 인프라 구축 나선다…현대차 ‘지원사격’, 동커볼케 현대차그룹 부사장, ‘세계 올해의 자동차인’ 선정, 회장님만 뽑히던 '세계 올해의 자동차인' 현대차 부사장이 선정됐다, 현대자동차, 현대차증권 550억 MMT 매수, 현대차, 내달 24일 주총…정의선 사내이사로 재선임, 현대차, 정의선 회장 사내이사 재선임…내달 24일 주주총회, 루크 동커볼케 현대차그룹 부사장, ‘세계 올해의 자동차인’</t>
@@ -7729,7 +7729,7 @@
     <t>현대차·기아, 2월 52만5765대 판매…전년比 2.7% 증가(종합), 현대차, 글로벌서 30만4613대 판매…8개월만 ..., 현대차, 2월 30만4613대 판매…전년比 1.4% '↑', 현대차, 2030년까지 100조 투자..영업이익률 10%로 올린다, 푸틴만큼 무서운 반도체난…현대차·기아 주가 하락 언제까지?, 현대차·기아, 2월 52만5765대 판매…전년比 2.7% 증가(종합), 현대차, 글로벌서 30만4613대 판매…8개월만 ..., 현대차, 2월 30만4613대 판매…전년比 1.4% '↑', 현대차, 2030년 전기차 187만대 판다, 현대차, 美친 질주 "2월 판매 역대 최다"…전기차 급성장, 현대차, 전기차 전환 박차…"2030년엔 17종 187만대 판매", 현대차, 2030년까지 100조 투자..영업이익률 10%로 올린다, 현대차 "2030년 17종 EV 라인업 구축…글로벌 MS 7% 달성", 해외에서 잇따라 상 받자…현대차·기아, 전 직원에게 400만원 특별격려..., ‘위기 속 성과’ 현대차?기아, 전 직원에 400만원 격려금, 현대차·제네시스, 전기차 17종 출격…'eM·eS' 새 플랫폼 만든다, 푸틴만큼 무서운 반도체난…현대차·기아 주가 하락 언제까지?, 美 시장 10% 고꾸라졌는데…현대차·기아는 만드는 족족 팔려, 美 시장 10% 고꾸라졌는데…현대차·기아는 만드는 족족 팔려, 현대차 "2030년 17종 EV 라인업 구축…글로벌 MS 7% 달성", 현대차·기아 전 직원에 품질성과 격려금 400만원, 전 직원에 400만원씩…현대차·기아 '통큰 격려', 전직원 격려금 400만원…현대차·기아, 성과 공유, 현대차, 2030년 전기차 187만대 판매·점유율 7% 추진, 현대차, 배터리 종합 전략 추진…"2023년 전기차 187만대 배터리..., "2030년 전기차 187만대 판매" 현대차, 전동화 가속페달 밟다, 현대차 "8년간 95조 투자…전기차 187만대 판매", 현대차·제네시스 전기차 17종으로 확대… 전고체 등 배터리 다변화 나선..., "전기차 회사로 탈바꿈"…현대차, 2030년까지 17종 출시, 현대차·기아, 전직원에 400만원 격려금, "세계시장서 잇단 낭보"…현대차·기아, 전 직원에 격려금 지급, 현대차, 2030년 전기차 187만대 판매·점유율 7% 추진, 현대차 "2030년 17종 EV 라인업 구축…글로벌 MS 7% 달성", "2030년 전기차 187만대 판매" 현대차, 전동화 가속페달 밟다, 현대차 "8년간 95조 투자…전기차 187만대 판매", 현대차·제네시스 전기차 17종으로 확대… 전고체 등 배터리 다변화 나선..., "전기차 회사로 탈바꿈"…현대차, 2030년까지 17종 출시, 현대차·기아, 전직원에 400만원 격려금, "세계시장서 잇단 낭보"…현대차·기아, 전 직원에 격려금 지급, 전직원 격려금 400만원…현대차·기아, 성과 공유, 美 시장 10% 고꾸라졌는데…현대차·기아 6%↑ '고공비행', 현대차, 2025년 신규 전용 EV플랫폼 도입…"아이오닉5 대비 주행거..., 현대차 “2030년 전기차 187만대 판매”…승용·PBV 신규 플랫폼..., 현대차 “2030년 전기차 187만대 판매”…승용·PBV 신규 플랫폼..., 현대성우그룹, 창립 35주년 전 계열사 홈페이지 전면 개편, 현대성우그룹, 그룹사 홈페이지 전면 개편, 현대차, 美 2월 소매 판매량 ‘사상 최다’, “현대엔지 상장 재추진?…주주환원 구체적 공개 필요”, 현대차, 러시아 공장 가동 일시 중단 소식에 주가 하락, 현대차·기아, 2월 美 판매 10만대 넘겨…쪼그라든 도요타·혼다 대조, 현대차, 美 2월 소매 판매량 ‘사상 최다’, 현대차·기아, 全직원에 400만원 격려금, "전 직원에 400만원"…현대차기아, 특별 격려금 쐈다, “현대엔지 상장 재추진?…주주환원 구체적 공개 필요”, 현대차, 러시아 공장 가동 일시 중단 소식에 주가 하락, 현대차 러시아 공장 일시 가동중단에 약세, 현대성우그룹, 그룹사 홈페이지 전면 개편, 현대차 2월 美 판매 사상최대...실적 두자릿수 늘어, "현대차·기아, 러시아 악재 과도하게 선반영", 현대차·기아, 2월 美 판매 10만대 넘겨…쪼그라든 도요타·혼다 대조, 현대무벡스는 자금줄?…현정은 회장은 다 계획이 있었구나, 현대차 "2030년 17종 EV 라인업 구축…글로벌 MS 7% 달성", '연락 끊긴 우크라' 두배 뛴 반도체 소재…"현대차 4500억 손실", "현대차·기아, 러시아 악재 과도하게 선반영", 현대차·기아, 러시아 판매 차질 우려에 나란히 하락, 현대차 러시아 공장 일시 가동중단에 약세, 토요타·혼다 주춤할동안…현대차·제네시스 美 2월 판매 사상 최다, 해외에서 잇따라 상 받자…현대차·기아, 전 직원에게 400만원 특별격려..., ‘위기 속 성과’ 현대차?기아, 전 직원에 400만원 격려금, “현대차 공장 중단, 시작에 불과?” 러시아에 스마트폰, 배터리도 떤다..., "17개 차종, 187만대 판매" 전기차 시장 잡겠다는 현대차, 현대차·제네시스, 전기차 17종 출격…'eM·eS' 새 플랫폼 만든다, 현대차, 배터리 종합 전략 추진…"2023년 전기차 187만대 배터리..., 현대차, 2025년 신규 전용 EV플랫폼 도입…"아이오닉5 대비 주행거..., "글로벌 점유율 7% 달성" 장재훈 현대차 사장이 내놓은 계획은?, 현대차, 美친 질주 "2월 판매 역대 최다"…전기차 급성장, 현대차 2월 美판매 신기록…SUV 인기(종합), 현대차, 2030년 전기차 187만대 판다, 현대차·기아, 전직원에 400만원씩 쏜다…"세계서 이룬 성취에 보답", “현대차 공장 중단, 시작에 불과?” 러시아에 스마트폰, 배터리도 떤다..., 현대차·기아, 러시아 판매 차질 우려에 나란히 하락, 현대차 2월 美판매 신기록…SUV 인기(종합), "현대차·기아, 러시아 악재 과도하게 선반영", ‘위기 속 성과’ 현대차?기아, 전 직원에 400만원 격려금, 현대차·기아, 통 크게 쏜다…전 직원에 '400만원 격려금', "세계시장서 잇단 낭보"…현대차·기아, 전 직원에 격려금 지급, "세계시장서 잇단 낭보"…현대차·기아, 전 직원에 격려금 지급, 현대차·기아, 전직원에 400만원씩 쏜다…"세계서 이룬 성취에 보답"</t>
   </si>
   <si>
-    <t>(영상)'DNA 싹 바꾼다'...현대차그룹, 전기차로 '승부수', '코로나 타격' 삼성 2차 벤더사 현대플렉스, 매물로, 삼성 2차 벤더 '현대플렉스' 매물로, 현대차-CEO Investor day-한 번에 몰아서 보고 싶다, 전동화 가속화 전략, 에피소드는 모두 한 번에 공개해야 시선을 끈다, 현대차, 신태용 印尼감독에 차량 후원, 현대차 ‘EV 플랫폼·배터리’ 박차…R&amp;D·설비 등 95조5000억 ..., 현대차-기다림 대비 조금은 아쉬운 목표, 경쟁사 대비 보수적인 EV 판매 목표, 그러나 공격적인 EV 점유율 목표. 목표 달성 위해서는 중국 재건 필요, 전기차 현지 생산 최적화 &amp; 배터리 조달 다변화 발표: LFP 전지와 Cell To Pack(C2P) 공식 언급, 빅 데이터 등 S/W 관련 매출 비중을 2030년 30%까지 확대. 그러나 전사 영업이익률 목표는 10%, 현대차-CEO investor day 후기: 전동화가 답이다, 투자포인트 및 결론, 주요이슈 및 실적전망, 주가전망 및 Valuation, (영상)'DNA 싹 바꾼다'...현대차그룹, 전기차로 '승부수', 현대차-CEO Investor Day 후기 : 전기차 시대에도 성장 지속 가능성 제시, 전동화 가속화 전략, 중장기 수익성 가이던스, 시사점과 투자의견, 현대차-원대한 목표, 부족한 실행 계획, EV를 26년 84만대 30년 187만대 판매해 글로벌 M/S 7% 를 달성할 계획, 중장기적인 EV 판매 및 재무 목표를 공유, Nothing Surprise, 새로운 EV 판매 목표는 기존 대비 상향됐지만 , 21 년 말 언론을 통해 공개된 수치와 동일, 배터리 조달 방안과 EV 현지 생산 CAPA 증설과 같은 구체적인 계획들이 부재, SW 매출 30% 를 달성하기 위한 계획은 전무, 과도한 우려, 현대차-2022년 CEO Investor Day 핵심내용, 2026년/2030년 전기차 판매 84만대/187만대 목표, 목표 상향은 시장의 전기차 전환 가속을 반영한 것, 목표주가 28만원 유지, 현대차-온도차가 있었던 EV 전략 발표, 전기차 판매목표 상향 긍정적, 전기차 현지생산을 위한 계획은 점진적, 배터리 확보, LFP, S/W 매출 등은 좀더 구체적이고 새로운 변화, 2030년 전기차 영업이익률 10% 이상 목표, 현대차-중장기 계획 업데이트, 중장기 계획 update, 전동화의 디테일한 밑그림을 확인 중, SW 고도화는 모든 완성차의 숙제이자 기회, 휴대폰·車 'FDPR' 예외…한숨 돌린 삼성·현대차, 현대차 ‘EV 플랫폼·배터리’ 박차…R&amp;D·설비 등 95조5000억 ..., 삼성·현대차 안도의 한숨.. 美 "스마트폰·자동차, 러 수출통제 예외..., 현대차, 전동화 가속·소프트웨어 전환 집중…목표가 유지-신한, 우크라 사태에 불똥 튄 현대차·기아…주가 바닥찍었나, "5년 내 6배" 美·유럽 사로잡은 현대차, 전기차 목표치 더 높였다, 현대차 전기차 점유율 목표에 담긴 의미, 현대차, 목표주가 '28만원'…전기차 패스트팔로워 역량 구축 -하나, 토요타·애플 등 잇단 탈러시아…압박받는 현대차·삼성·LG, 삼성·현대차 안도의 한숨.. 美 "스마트폰·자동차, 러 수출통제 예외", 1월 세계 수소차 판매 30% 증가…현대차 1위, 삼성·현대차 안도의 한숨.. 美 "스마트폰·자동차, 러 수출통제 예외", 1월 세계 수소차 판매 30% 증가…현대차 1위, 현대차, 전기차 시대 '패스트 팔로워' 역량 구축-하나, 美 FOMC 불확실성 해소에 코스피 상승, 현대차 3.52% ↑ [개장..., 현대차 "2030년까지 전기차 187만대 판매"…장 초반 강세, "5년 후 전기차 14종" 기아도 전동화 속도…2030년 현대·기아 3..., 이지트로닉스, 정의선 빅픽쳐 '전기차 심장' 으뜸…폐배터리 금..., 신저가 행진에도 현대?기아차 베팅하는 개미…5일 만에 4500억 샀다, 현대차그룹, 전기차 31종 출시…“2030년 300만대 이상 팔겠다”, 현대차 ‘EV 플랫폼·배터리’ 박차…R&amp;D·설비 등 95조5000억 투..., 'FPCB 제조업체' 현대플렉스 매물로</t>
+    <t>(영상)'DNA 싹 바꾼다'...현대차그룹, 전기차로 '승부수', '코로나 타격' 삼성 2차 벤더사 현대플렉스, 매물로, 삼성 2차 벤더 '현대플렉스' 매물로, CEO Investor day-한 번에 몰아서 보고 싶다, 전동화 가속화 전략, 에피소드는 모두 한 번에 공개해야 시선을 끈다, 현대차, 신태용 印尼감독에 차량 후원, 현대차 ‘EV 플랫폼·배터리’ 박차…R&amp;D·설비 등 95조5000억 ..., 기다림 대비 조금은 아쉬운 목표, 경쟁사 대비 보수적인 EV 판매 목표, 그러나 공격적인 EV 점유율 목표. 목표 달성 위해서는 중국 재건 필요, 전기차 현지 생산 최적화 &amp; 배터리 조달 다변화 발표: LFP 전지와 Cell To Pack(C2P) 공식 언급, 빅 데이터 등 S/W 관련 매출 비중을 2030년 30%까지 확대. 그러나 전사 영업이익률 목표는 10%, CEO investor day 후기: 전동화가 답이다, 투자포인트 및 결론, 주요이슈 및 실적전망, 주가전망 및 Valuation, (영상)'DNA 싹 바꾼다'...현대차그룹, 전기차로 '승부수', CEO Investor Day 후기 : 전기차 시대에도 성장 지속 가능성 제시, 전동화 가속화 전략, 중장기 수익성 가이던스, 시사점과 투자의견, 원대한 목표, 부족한 실행 계획, EV를 26년 84만대 30년 187만대 판매해 글로벌 M/S 7% 를 달성할 계획, 중장기적인 EV 판매 및 재무 목표를 공유, Nothing Surprise, 새로운 EV 판매 목표는 기존 대비 상향됐지만 , 21 년 말 언론을 통해 공개된 수치와 동일, 배터리 조달 방안과 EV 현지 생산 CAPA 증설과 같은 구체적인 계획들이 부재, SW 매출 30% 를 달성하기 위한 계획은 전무, 과도한 우려, 2022년 CEO Investor Day 핵심내용, 2026년/2030년 전기차 판매 84만대/187만대 목표, 목표 상향은 시장의 전기차 전환 가속을 반영한 것, 목표주가 28만원 유지, 온도차가 있었던 EV 전략 발표, 전기차 판매목표 상향 긍정적, 전기차 현지생산을 위한 계획은 점진적, 배터리 확보, LFP, S/W 매출 등은 좀더 구체적이고 새로운 변화, 2030년 전기차 영업이익률 10% 이상 목표, 중장기 계획 업데이트, 중장기 계획 update, 전동화의 디테일한 밑그림을 확인 중, SW 고도화는 모든 완성차의 숙제이자 기회, 휴대폰·車 'FDPR' 예외…한숨 돌린 삼성·현대차, 현대차 ‘EV 플랫폼·배터리’ 박차…R&amp;D·설비 등 95조5000억 ..., 삼성·현대차 안도의 한숨.. 美 "스마트폰·자동차, 러 수출통제 예외..., 현대차, 전동화 가속·소프트웨어 전환 집중…목표가 유지-신한, 우크라 사태에 불똥 튄 현대차·기아…주가 바닥찍었나, "5년 내 6배" 美·유럽 사로잡은 현대차, 전기차 목표치 더 높였다, 현대차 전기차 점유율 목표에 담긴 의미, 현대차, 목표주가 '28만원'…전기차 패스트팔로워 역량 구축 -하나, 토요타·애플 등 잇단 탈러시아…압박받는 현대차·삼성·LG, 삼성·현대차 안도의 한숨.. 美 "스마트폰·자동차, 러 수출통제 예외", 1월 세계 수소차 판매 30% 증가…현대차 1위, 삼성·현대차 안도의 한숨.. 美 "스마트폰·자동차, 러 수출통제 예외", 1월 세계 수소차 판매 30% 증가…현대차 1위, 현대차, 전기차 시대 '패스트 팔로워' 역량 구축-하나, 美 FOMC 불확실성 해소에 코스피 상승, 현대차 3.52% ↑ [개장..., 현대차 "2030년까지 전기차 187만대 판매"…장 초반 강세, "5년 후 전기차 14종" 기아도 전동화 속도…2030년 현대·기아 3..., 이지트로닉스, 정의선 빅픽쳐 '전기차 심장' 으뜸…폐배터리 금..., 신저가 행진에도 현대?기아차 베팅하는 개미…5일 만에 4500억 샀다, 현대차그룹, 전기차 31종 출시…“2030년 300만대 이상 팔겠다”, 현대차 ‘EV 플랫폼·배터리’ 박차…R&amp;D·설비 등 95조5000억 투..., 'FPCB 제조업체' 현대플렉스 매물로</t>
   </si>
   <si>
     <t>현대이지웰, 한국거래소 '코스닥시장 공시 우수법인' 선정, 현대이지웰, 한국거래소 '코스닥시장 공시우수법인' 선정, "현대차, 3월 러 생산 반토막"…유연탄값 하루새 45% 폭등, 현대차연구소 조직문화 개선위 "직원 사망사건 사과·보상" 권고, 현대차연구소 조직문화 개선위 "직원 사망사건 사과·보상" 권고, 현대이지웰, 한국거래소 '코스닥시장 공시 우수법인' 선정, 현대이지웰, 한국거래소 '코스닥시장 공시우수법인' 선정, 현대차 남양연구소 개선위 “직원 사망사건 관련 사과·보상” 권고, 현대차 아이오닉5, 벤츠 안방에서 전기차 ‘판정승’, 현대차 남양연구소 개선위 “직원 사망사건 관련 사과·보상” 권고, 獨 전문지, 전기차 비교평가서 벤츠 아닌 현대 손들어줬다, "현대차, 3월 러 생산 반토막"…유연탄값 하루새 45% 폭등, 현대차 아이오닉5, 獨전문지 평가서 벤츠 EQB에 '완승', 러시아 진출 韓기업 초긴장…현대차·기아도 영향권, "자동차주 환멸스럽다"…개미들, 현대차·기아로 한달새 300억 넘게 잃..., 현대오토에버, 현대차그룹 소프트웨어 투자의 주역-유진, "2030년 유럽 판매 70%가 전기차" 현대차·기아의 이유있는 자신감, '러 불똥' 튄 현대차·기아…3월 이후 회복..., 현대오토에버, 현대차그룹 소프트웨어 투자의 주역-유진, 러시아 진출 韓기업 초긴장…현대차·기아도 영향권, "2030년 유럽 판매 70%가 전기차" 현대차·기아의 이유있는 자신감, 주가 급락한 현대?기아차, 그래도 미국 시장 점유율은 올랐..., 현대차그룹, 통합 홈페이지 문 열어…"모든 것 한 눈에", (영상)전국삼성전자노조 새 위원장 "현대차·기아 등 노조와 연대", 현대차그룹 홈페이지 통합 개편…"디지털·환경 소통 강화", 현대이지웰, 한국거래소 '코스닥시장 공시 우수법인' 선정, 현대차 아이오닉5, 독일 안방서 벤츠 제쳤다…전기차 비교평가, 현대차그룹, 통합 홈페이지 통해 고객 소통 강화, (영상)전국삼성전자노조 새 위원장 "현대차·기아 등 노조와 연대", 현대차 아이오닉5, 독일 안방서 벤츠 제쳤다…전기차 비교평가, 현대차그룹, 통합 홈페이지 오픈 고객소통 강화, 현대차그룹, 통합 홈페이지 통해 고객 소통 강화, '러 불똥' 튄 현대차·기아…3월 이후 회복..., 현대차그룹, 통합 홈페이지 오픈 고객소통 강화</t>
@@ -7741,7 +7741,7 @@
     <t>삼성, 러시아行 선적 중단…현대차는 현지 생산 축소, 삼성·현대차·SK…산불 피해에 팔 걷고 나서는 대기업들, 삼성·현대차·롯데·두산, 강원 산불 피해복구 성금 기부 릴레이, 2주간 5383억 매수… 개미, 현대차·기아 물타기 성공할까, '개미 물타기'로 가는 현대기아차...개미의 상상은 현실이 될까, 현대차·기아 '전기차 선진국' 북유럽도 휩쓴다, 바스프 "ESG경영 의지 강한 삼성·현대차 등과 협업 확대", 현대차, 러 공장 9일 재개… 수급 차질에 감산 장기화 우려, 2주간 5383억 매수… 개미, 현대차·기아 물타기 성공할까, “테슬라 잡는다”…현대차·포드 등 글로벌 완성차 전략은, 현대차·기아 '전기차 선진국' 북유럽도 휩쓴다, “테슬라 잡는다”…현대차·포드 등 글로벌 완성차 전략은, 현대차 시트에 배터리 들어간다...왜?, 삼성·현대차·롯데·두산, 강원 산불 피해복구 성금 기부 릴레이, '현대차의 전동화 전략' 증권가 눈높이에는 역부족…"실행 계획이 아쉽다..., 현대차그룹, 울진·삼척 산불 피해복구 성금 50억원 전달, '개미 물타기'로 가는 현대기아차...개미의 상상은 현실이 될까, 울진·삼척 산불에 삼성·현대차·SK 등 재계 지원 잇따라, 산불 이재민 마음 달랜 기업들…현대차·삼성·SK·두산 기부 행렬, 현대차그룹, 피해복구 성금 50억원 기부…세탁차량도 지원, 산불 이재민 마음 달랜 기업들…현대차·삼성·SK·두산 기부 행렬, 울진·삼척 산불 …삼성·현대차·SK 등 재계, 기부 릴레이, 현대ENG, 美 폐플라스틱 사업 연간 45만t 규모 설비 계약, 삼성, 러시아行 선적 중단…현대차, 9일 재가동 불투명, 현대코퍼, 車 수출 스톱…조선사, 수천억대 평가손실 떠안을 판, 삼성, 러시아行 선적 중단…현대차는 현지 생산 축소, 현대차, 러 공장 9일 재개… 수급 차질에 감산 장기화 우려, 바스프 "ESG경영 의지 강한 삼성·현대차 등과 협업 확대", 울진·삼척 산불에 삼성·현대차·SK 등 재계 지원 잇따라</t>
   </si>
   <si>
-    <t>현대차, 중고차 진출 공식화…"신차급 車로 시장 공략", 소비자 편익·상생 강조한 현대차…중고차 허브 역할 담당한다(종합), 러 제재에 휘청이는 車업계…현대·기아차 또 신저가, 러시아-우크라 전쟁에 자동차 업계 먹구름…현대차 기아 또 신저가, (영상)러시아發 물류대란 현실로...현대차·삼성전자 등 피해 속출, 다른 車 회사는 안 하는데…현대차, 반려동물 지원하는 이유, 현대차 중고차 진출 공식화…“5년, 10만㎞ 내 차량 신차 수준 상품화..., 현대차 중고차 진출 공식화…“5년, 10만㎞ 내 차량 신차 수준 상품화..., 현대차 “중고차 진출” 공식화…“5년, 10만㎞내 신차 수준 판매”, 현대차-이베코그룹 ‘맞손’…상용차 부문 협력한다, KBI동국실업, 현대차 신규 전기차용 센터콘솔 1200억원 수주, KBI동국실업, 현대차 신규 전기차 센터콘솔 부품 공급, "16층도 위기다"…'또 신저가' 현대차, 두 달 새 20% 급락, 현대차, 伊 이베코와 손 잡는다…"상용차 부문 협력", 1월 강남구 아파트 거래, 절반 이상이 신고가 경신... 압구정 현대 ..., 현대차, 伊 상용차 이베코와 손 잡아, 현대차, 러 공장 재가동 불발… "재개 시점 미정", 러 제재에 휘청이는 車업계…현대·기아차 또 신저가, 러, 韓 비우호국 지정…삼성·LG전자·현대차 줄타격 우려, 현대차그룹, 우크라이나에 '인도적 지원' 100만달러 기부, 현대차, 이베코그룹과 상용차 부문 협력…MOU 체결, 현대차-이베코그룹, 상용차 부문 상호 협력 방안 모색, 러, 韓 비우호국 지정…삼성·LG전자·현대차 줄타격 우려, 현대차그룹, 우크라이나에 '인도적 지원' 100만달러 기부, 현대차, 이베코그룹과 상용차 부문 협력…MOU 체결, 러시아-우크라 전쟁에 자동차 업계 먹구름…현대차 기아 또 신저가, 현대차-이베코그룹, 상용차 부문 상호 협력 방안 모색, 현대차 중고차 진출 공식화…“5년, 10만㎞ 내 차량 신차 수준 상품..., 현대차 "5년 10만㎞ 이내 중고차만 판매", 현대차 "중고차 사업, 인증중고차만...점유율도 자체 제한", 현대차·伊이베코 "상용차 협력", 현대차, 伊 상용차 이베코와 손 잡아, 현대차, '운명의 날' 앞서 중고차 사업 공식화한 배경, 현대차, 중고차 진출 공식화…"신차급 車로 시장 공략", 현대차 이미 삽 떴는데…17일께 중고차 적합업종 심의위 개최, 현대차-이베코그룹, 상용차 부문 상호 협력 방안 모색, 현대차-이베코그룹, 상용차 부문 상호 협력 방안 모색, 현대차, 伊 이베코그룹과 손잡는다…"상용차 부문 협력", 현대차, 중고차 시장 진출 공식화…"신차 수준으로 상품화", 현대차, 신뢰 잃은 중고차 시장 확 바꾸나…"200개 검사 통과해야 ..., 현대차, '중고차 시장 진출' 공식화…"5년·10만㎞ 내 신차 수준 상..., 현대차, 중고차 진출 공식화…“5년 10만㎞ 내 차량 신차 수준 상품화..., 현대차, 자동차용품·생활용품 판매하는 온라인몰 열어, 현대차 자동차·생활용품 온라인몰 통합, 현대차證, 홀세일사업 강화 위한 조직개편 나서, HMM 새 대표 ‘현대차맨’ 김경배 낙점한 진짜 배경은?, 현대차그룹 파트너 얀덱스, 美 영업 중단…자율주행 기술 개발 차질, "허위매물 퇴출·투명한 정보 제공"…중고차 시장 허브 자임한 현대차, 현대차, 자동차용품·생활용품 판매하는 온라인 쇼핑몰 '현대숍' 오픈, KBI동국실업, 현대차 신규 전기차 센터콘솔 부품 공급, 현대차-이베코그룹 ‘맞손’…상용차 부문 협력한다, KBI동국실업, 현대차 신규 전기차 센터콘솔 공급한다, KBI동국실업, 현대차 신규 전기차 센터콘솔 부품 공급, KBI동국실업, 현대차 신규 전기차 센터콘솔 공급한다, 현대차 자동차·생활용품 온라인몰 통합, 현대차, 온라인 통합 커머스몰 ‘현대Shop’ 활짝, 삼성·현대차·SK 산불 피해복구 성금, 삼성 30억 현대차 50억 SK 20억…산불 피해 돕는 한국 경제 버..., 저점 탈출한 현대·기아…점진적 회복? 엇갈리는 전망, 현대차證, 홀세일사업 강화 위한 조직개편 나서, 현대차 자동차·생활용품 온라인몰 통합, 현대차 “중고차 진출” 공식화…“5년, 10만㎞내 신차 수준 판매”, 현대차, 신뢰 잃은 중고차 시장 확 바꾸나…"200개 검사 통과해야 ..., 현대차·기아 언제 달리나…엇갈린 시선 속 개인 풀매수, 중기부, 소부장 혁신 스타트업 모집…삼성·현대 기술수요 제시, 현대코퍼, 러-우크라 변수에 신사업 안갯속, 삼성전자 장중 7만원 붕괴, 현대차도 52주 신저가, 현대엘리베이터·현대무벡스, 상반기 신입사원 공채, "16층도 위기다"…'또 신저가' 현대차, 두 달 새 20% 급락, 중기부, 소부장 혁신 스타트업 모집…삼성·현대 기술수요 제시, 현대차·기아 언제 달리나…엇갈린 시선 속 개인 풀매수, 현대엘리베이터·현대무벡스, 상반기 신입사원 공채, 현대차 “중고차 진출” 공식화…“5년, 10만㎞내 신차 수준 판매”, 현대엘리베이터·현대무벡스, 미래 이끌 ‘MZ세대 인재’ 찾는다, KBI동국실업, 현대차 신규 전기차용 센터콘솔 1200억원 수주, KBI동국실업, 현대차 신규 전기차 센터콘솔 부품 공급, 현대차, 중고차 시장 진출 공식화…"신차 수준으로 상품화", 현대차, 드디어 '중고차' 판다…"5년·10만㎞내 인증매물", 현대차 "중고차 사업, 인증중고차만...점유율도 자체 제한", 삼성·현대차·SK 산불 피해복구 성금, 현대차, 자동차용품·생활용품 판매하는 온라인몰 열어, 현대차그룹 파트너 얀덱스, 美 영업 중단…자율주행 기술 개발 차질, 현대차 파트너 얀덱스, 美 영업중단…자율주행 협력 ‘먹구름’, 현대차 “중고차, 신차 수준 상품화 후 판매”, 삼성·현대차·SK…재계, 산불 구호성금·지원 줄이어</t>
+    <t>현대차, 중고차 진출 공식화…"신차급 車로 시장 공략", 소비자 편익·상생 강조한 현대차…중고차 허브 역할 담당한다(종합), 러 제재에 휘청이는 車업계…현대·기아차 또 신저가, 러시아-우크라 전쟁에 자동차 업계 먹구름…현대차 기아 또 신저가, (영상)러시아發 물류대란 현실로...현대차·삼성전자 등 피해 속출, 다른 車 회사는 안 하는데…현대차, 반려동물 지원하는 이유, 현대차 중고차 진출 공식화…“5년, 10만㎞ 내 차량 신차 수준 상품화..., 현대차 중고차 진출 공식화…“5년, 10만㎞ 내 차량 신차 수준 상품화..., 현대차 “중고차 진출” 공식화…“5년, 10만㎞내 신차 수준 판매”, 이베코그룹 ‘맞손’…상용차 부문 협력한다, KBI동국실업, 현대차 신규 전기차용 센터콘솔 1200억원 수주, KBI동국실업, 현대차 신규 전기차 센터콘솔 부품 공급, "16층도 위기다"…'또 신저가' 현대차, 두 달 새 20% 급락, 현대차, 伊 이베코와 손 잡는다…"상용차 부문 협력", 1월 강남구 아파트 거래, 절반 이상이 신고가 경신... 압구정 현대 ..., 현대차, 伊 상용차 이베코와 손 잡아, 현대차, 러 공장 재가동 불발… "재개 시점 미정", 러 제재에 휘청이는 車업계…현대·기아차 또 신저가, 러, 韓 비우호국 지정…삼성·LG전자·현대차 줄타격 우려, 현대차그룹, 우크라이나에 '인도적 지원' 100만달러 기부, 현대차, 이베코그룹과 상용차 부문 협력…MOU 체결, 이베코그룹, 상용차 부문 상호 협력 방안 모색, 러, 韓 비우호국 지정…삼성·LG전자·현대차 줄타격 우려, 현대차그룹, 우크라이나에 '인도적 지원' 100만달러 기부, 현대차, 이베코그룹과 상용차 부문 협력…MOU 체결, 러시아-우크라 전쟁에 자동차 업계 먹구름…현대차 기아 또 신저가, 이베코그룹, 상용차 부문 상호 협력 방안 모색, 현대차 중고차 진출 공식화…“5년, 10만㎞ 내 차량 신차 수준 상품..., 현대차 "5년 10만㎞ 이내 중고차만 판매", 현대차 "중고차 사업, 인증중고차만...점유율도 자체 제한", 현대차·伊이베코 "상용차 협력", 현대차, 伊 상용차 이베코와 손 잡아, 현대차, '운명의 날' 앞서 중고차 사업 공식화한 배경, 현대차, 중고차 진출 공식화…"신차급 車로 시장 공략", 현대차 이미 삽 떴는데…17일께 중고차 적합업종 심의위 개최, 이베코그룹, 상용차 부문 상호 협력 방안 모색, 이베코그룹, 상용차 부문 상호 협력 방안 모색, 현대차, 伊 이베코그룹과 손잡는다…"상용차 부문 협력", 현대차, 중고차 시장 진출 공식화…"신차 수준으로 상품화", 현대차, 신뢰 잃은 중고차 시장 확 바꾸나…"200개 검사 통과해야 ..., 현대차, '중고차 시장 진출' 공식화…"5년·10만㎞ 내 신차 수준 상..., 현대차, 중고차 진출 공식화…“5년 10만㎞ 내 차량 신차 수준 상품화..., 현대차, 자동차용품·생활용품 판매하는 온라인몰 열어, 현대차 자동차·생활용품 온라인몰 통합, 현대차證, 홀세일사업 강화 위한 조직개편 나서, HMM 새 대표 ‘현대차맨’ 김경배 낙점한 진짜 배경은?, 현대차그룹 파트너 얀덱스, 美 영업 중단…자율주행 기술 개발 차질, "허위매물 퇴출·투명한 정보 제공"…중고차 시장 허브 자임한 현대차, 현대차, 자동차용품·생활용품 판매하는 온라인 쇼핑몰 '현대숍' 오픈, KBI동국실업, 현대차 신규 전기차 센터콘솔 부품 공급, 이베코그룹 ‘맞손’…상용차 부문 협력한다, KBI동국실업, 현대차 신규 전기차 센터콘솔 공급한다, KBI동국실업, 현대차 신규 전기차 센터콘솔 부품 공급, KBI동국실업, 현대차 신규 전기차 센터콘솔 공급한다, 현대차 자동차·생활용품 온라인몰 통합, 현대차, 온라인 통합 커머스몰 ‘현대Shop’ 활짝, 삼성·현대차·SK 산불 피해복구 성금, 삼성 30억 현대차 50억 SK 20억…산불 피해 돕는 한국 경제 버..., 저점 탈출한 현대·기아…점진적 회복? 엇갈리는 전망, 현대차證, 홀세일사업 강화 위한 조직개편 나서, 현대차 자동차·생활용품 온라인몰 통합, 현대차 “중고차 진출” 공식화…“5년, 10만㎞내 신차 수준 판매”, 현대차, 신뢰 잃은 중고차 시장 확 바꾸나…"200개 검사 통과해야 ..., 현대차·기아 언제 달리나…엇갈린 시선 속 개인 풀매수, 중기부, 소부장 혁신 스타트업 모집…삼성·현대 기술수요 제시, 현대코퍼, 러-우크라 변수에 신사업 안갯속, 삼성전자 장중 7만원 붕괴, 현대차도 52주 신저가, 현대엘리베이터·현대무벡스, 상반기 신입사원 공채, "16층도 위기다"…'또 신저가' 현대차, 두 달 새 20% 급락, 중기부, 소부장 혁신 스타트업 모집…삼성·현대 기술수요 제시, 현대차·기아 언제 달리나…엇갈린 시선 속 개인 풀매수, 현대엘리베이터·현대무벡스, 상반기 신입사원 공채, 현대차 “중고차 진출” 공식화…“5년, 10만㎞내 신차 수준 판매”, 현대엘리베이터·현대무벡스, 미래 이끌 ‘MZ세대 인재’ 찾는다, KBI동국실업, 현대차 신규 전기차용 센터콘솔 1200억원 수주, KBI동국실업, 현대차 신규 전기차 센터콘솔 부품 공급, 현대차, 중고차 시장 진출 공식화…"신차 수준으로 상품화", 현대차, 드디어 '중고차' 판다…"5년·10만㎞내 인증매물", 현대차 "중고차 사업, 인증중고차만...점유율도 자체 제한", 삼성·현대차·SK 산불 피해복구 성금, 현대차, 자동차용품·생활용품 판매하는 온라인몰 열어, 현대차그룹 파트너 얀덱스, 美 영업 중단…자율주행 기술 개발 차질, 현대차 파트너 얀덱스, 美 영업중단…자율주행 협력 ‘먹구름’, 현대차 “중고차, 신차 수준 상품화 후 판매”, 삼성·현대차·SK…재계, 산불 구호성금·지원 줄이어</t>
   </si>
   <si>
     <t>현대차 아이오닉 5, 獨 이어 '영국 올해의 차'도 수상했다, 현대차 아이오닉 5, 獨이어 英서도 ‘올해의 차’ 올라, "현대차는 '바퀴달린 냉장고' 비난하더니"…아이오닉5, 고상한 영국인도..., 현대차 아이오닉 5, 獨이어 英서도 ‘올해의 차’ 올라, “주가는 언제 오르나?” 현대차·기아 주주들, 깊어지는 근심, 우크라 사태 여파…멈춰선 현대차 러시아 공장, "부품 구할 길 없어"…현대차 러시아 공장 가동 중단, 현대차 '아이오닉 5', ‘영국 올해의 차’ 수상, 현대차 아이오닉 5, 獨 이어 '영국 올해의 차'도 수상했다, 현대차 아이오닉5 ‘영국 올해의 차’에…“디자인·성능·실용성 최고”, "현대차는 '바퀴달린 냉장고' 비난하더니"…아이오닉5, 고상한 영국인도..., 현대차 아이오닉5 ‘영국 올해의 차’에…“디자인·성능·실용성 최고”, 현대차·모비스, 러 공장 ‘셧다운’… 월 2만대 생산차질, "중고차 시장 외연 확대" 진입 지연에 답답한 현대차, 사업 청사진 ..., ‘중고차 진출’ 공식화한 현대차…“신차 수준 상품화”, "중고차 시장 외연 확대" 진입 지연에 답답한 현대차, 사업 청사진 ..., ‘중고차 진출’ 공식화한 현대차…“신차 수준 상품화”, "1500만원대 아반떼 이제 없다"…현대, 기본 트림 수동 없애, "정신혼미 대형株" 현대차·LG화학·삼성SDI '52주 신저가' [특징..., 현대차·기아 "나란히 52주 신저가 경신", 최강 준중형 세단 나왔다...현대차 '2022 아반떼' 출시, 현대차 아이오닉 5, 獨이어 英서도 ‘올해의 차’ 올라, 현대차, 정숙성 높인 ‘2022 아반떼’ 내놨다, 현대차, ‘2022 아반떼’ 판매 시작…1866만원부터, 현대차, ‘2022 아반떼’ 출시…1866만~2892만원, "부품 구할 길 없어"…현대차 러시아 공장 가동 중단, 현대차, 러시아 공장 재가동 보류…셧다운 장기화 조짐, "러 시장 진퇴양난" 바짝 엎드린 삼성·현대차, 현대 전기차 콘솔 수주한 KBI동국실업 "공급가는 양산 시점에 합의", 현대차정몽구재단 ‘온드림스쿨’ 개강…“10년간 3만5000명 참여”, 러, 韓 비우호국가 지정 영향은?…삼성·LG·현대차 직격탄 우려, "돈 떼일라"…러시아, 韓경제 제재로 삼성·현대차 타격 예상(종합)</t>
@@ -7783,7 +7783,7 @@
     <t>"삼성·현대차 '인재 중심주의'로 글로벌 기업 돼…경제정책, 전문가에게..., 현대차그룹, 캐나다서 도요타 추월, 현대차, 중국 법인에 1조2000억 긴급 수혈, 아산 정주영 21주기, 범 현대가 한자리에, 정주영 21주기에 범 현대가 모여…정몽준·정의선 등 참석, 현대차, 중국 합작 법인 베이징현대 1조원대 증자…전기차 집중, 고전 중인 베이징현대 1.1兆 증자한다, 아산 정주영 21주기, 범 현대가 한자리에, 현대차그룹, 캐나다서 도요타 추월, 고전 중인 베이징현대 1.1兆 증자한다, 현대차, 중국 합작 법인 베이징현대 1조원대 증자…전기차 집중, "삼성·현대차 '인재 중심주의'로 글로벌 기업 돼…경제정책, 전문가에게..., 현대차그룹, 캐나다서 도요타 추월, 현대차, 중국 법인에 1조2000억 긴급 수혈, 현대차, '제네시스' 인기몰이에 활짝…캐나다선 토요타 추월, 현대차, 중국 합작 법인 베이징현대 1조원대 증자…전기차 집중, 현대차, 中 합작사에 1조 수혈… 전기차 사업 확대, "삼성·현대차 '인재 중심주의'로 글로벌 기업 돼…경제정책, 전문가에게..., 정주영 21주기에 범 현대가 모여…정몽준·정의선 등 참석, 현대차, 중국 법인에 1조2000억 긴급 수혈, 현대차, '제네시스' 인기몰이에 활짝…캐나다선 토요타 추월</t>
   </si>
   <si>
-    <t>현대차 후원…‘바바라 크루거’ LACMA 개인전, 현대차, 美 미술가'‘바버라 크루거’ LA 개인전 후원, 현대차 "인구 6억 아세안 시장 공략"…印尼에 전기차 생산 거점, 현대차, LACMA서 '바바라 크루거' 작품전 개막…"더 현대 6번째..., 中사업 승부수 거나…베이징현대, 1조원 대 증자, 현대차-ESG 총평, 환경(E), 사회(S), 지배구조(G), 현대차, 고전하던 中법인에 5600억 수혈…"전기차 키운다", 현대차·기아, 반도체 공급난에도 해외법인들 흑자 기록, 中서 부진한 베이징현대 1.2조 증자 결정…2년간 2조원 손실, 현대글로비스, 2% 강세…현대차그룹 중고차 사업 진출 수혜, (영상)지난해 현대차 주요 해외법인 모두 흑자 기록, 현대글로비스, 2% 강세…현대차그룹 중고차 사업 진출 수혜, 현대글로비스, 현대차그룹 중고차 사업 진출 수혜…목표가 13%↑-KT..., 떨어질 때 더 떨어진 현대차…중고차 앞세워 반등할까, 현대차·LACMA 파트너십, '바바라 크루거' 전시 개막, 현대차·기아, 반도체 공급난에도 해외법인들 흑자 기록, "현대글로비스, 현대차의 중고차 사업 직간접 수혜…목표..., '더 현대 프로젝트' 여섯번째 전시, 바바라 크루거 개인전 개막, 현대차·기아, 주요해외법인 지난해 흑자…공장가동률 개선, 현대차, LACMA서 '바바라 크루거' 작품전 개막…"더 현대 6번째..., 현대차 후원…‘바바라 크루거’ LACMA 개인전, 떨어질 때 더 떨어진 현대차…중고차 앞세워 반등할까, 현대차, 고전하던 中법인에 5600억 수혈…"전기차 키운다", 현대글로비스, 현대차그룹 중고차 사업 진출 수혜…목표가 13%↑-KT..., 현대글로비스, 현대차그룹 중고차 사업 진출 수혜…목표가↑-KTB, (영상)지난해 현대차 주요 해외법인 모두 흑자 기록</t>
+    <t>현대차 후원…‘바바라 크루거’ LACMA 개인전, 현대차, 美 미술가'‘바버라 크루거’ LA 개인전 후원, 현대차 "인구 6억 아세안 시장 공략"…印尼에 전기차 생산 거점, 현대차, LACMA서 '바바라 크루거' 작품전 개막…"더 현대 6번째..., 中사업 승부수 거나…베이징현대, 1조원 대 증자, ESG 총평, 환경(E), 사회(S), 지배구조(G), 현대차, 고전하던 中법인에 5600억 수혈…"전기차 키운다", 현대차·기아, 반도체 공급난에도 해외법인들 흑자 기록, 中서 부진한 베이징현대 1.2조 증자 결정…2년간 2조원 손실, 현대글로비스, 2% 강세…현대차그룹 중고차 사업 진출 수혜, (영상)지난해 현대차 주요 해외법인 모두 흑자 기록, 현대글로비스, 2% 강세…현대차그룹 중고차 사업 진출 수혜, 현대글로비스, 현대차그룹 중고차 사업 진출 수혜…목표가 13%↑-KT..., 떨어질 때 더 떨어진 현대차…중고차 앞세워 반등할까, 현대차·LACMA 파트너십, '바바라 크루거' 전시 개막, 현대차·기아, 반도체 공급난에도 해외법인들 흑자 기록, "현대글로비스, 현대차의 중고차 사업 직간접 수혜…목표..., '더 현대 프로젝트' 여섯번째 전시, 바바라 크루거 개인전 개막, 현대차·기아, 주요해외법인 지난해 흑자…공장가동률 개선, 현대차, LACMA서 '바바라 크루거' 작품전 개막…"더 현대 6번째..., 현대차 후원…‘바바라 크루거’ LACMA 개인전, 떨어질 때 더 떨어진 현대차…중고차 앞세워 반등할까, 현대차, 고전하던 中법인에 5600억 수혈…"전기차 키운다", 현대글로비스, 현대차그룹 중고차 사업 진출 수혜…목표가 13%↑-KT..., 현대글로비스, 현대차그룹 중고차 사업 진출 수혜…목표가↑-KTB, (영상)지난해 현대차 주요 해외법인 모두 흑자 기록</t>
   </si>
   <si>
     <t>'동학개미 궁금증 해결'…국민주 반열 오른 현대차, 현대차, 어린이 통학차량 운행정보 기록장치 지원, 잠실현대·문정현대도 조합설립 인가…속도붙은 ‘송파구 리모델링’, '동학개미 궁금증 해결'…국민주 반열 오른 현대차, 잠실현대·문정현대도 조합설립 인가…속도붙은 ‘송파구 리모델링’, 현대차 사상 최고액 2조2664억원… 전년보다..., 현대차, 중고차 진출…계열사 더 크게 웃는다, 현대百, '아마존 1위 매트리스' 지누스 7747억에 인수, 현대차, 어린이 통학차량 운행정보 기록장치 지원, 현대차, 어린이 통학차에 전자식 기록장치 지원, 현대百, '아마존 1위 매트리스' 지누스 7747억에 인수, 현대차, 어린이 통학차량에 운행정보 기록장치 지원, 부품대란에 현대차 ‘토요특근 중단’…내 차 출고 더 늦어지나 [비즈36..., SK가스, 현대차 등과 ‘LPG 어린이 통학 차량 활성화’에 맞손, 현대차, 어린이 통학차에 전자식 기록장치 지원, 현대차, '어린이 통학차량 안전운전 캠페인' 실시, 테슬라와 손잡은 獨 총리…현대차가 긴장하는 이유, 잇단 악재에도 현대차·기아, 해외법인 호실적…"올해 투자 확대", 현대차, 토요특근 또 멈춘다…전쟁·코로나·부품난 ‘3중고’</t>
@@ -7801,13 +7801,13 @@
     <t>"현대글로비스 목표주가 27만원‥현대차 수출 증가 효과", "현대글로비스 목표주가 27만원‥현대차 수출 증가 효과", 정의선 현대차그룹 회장, 인니에 전기차 생산 거점…인구..., 정의선 현대차그룹 회장, 인니에 전기차 생산 거점…인구..., "현대글로비스 목표주가 27만원‥현대차 수출 증가 효과", 정의선 현대차그룹 회장, 인니에 전기차 생산 거점…인구...</t>
   </si>
   <si>
-    <t>트럭·버스 등 상용차 고객 전용 ‘Hyundai Mobility카드’..., 쏘카·현대차 ‘커넥티드카 OS’ 손잡는다, 쏘카, 현대차 커넥티드 카 전용 SW와 연계한다, 현대차·기아·모비스, 국내 외 특허 5만건 돌파, 현대차-쏘카, '커넥티드카' 맞손, 쏘카에 현대차 커넥티드카 OS 들어온다, 현대차 '혼류생산' 본격 가동…한 라인서 10차종 만든다, "현대차 러 공장 푸틴에 뺏길 판" 국유화 피해 볼 가능성↑, 현대카드, 트럭?버스 등 고객 전용 '현대 모빌리티카드(상용차)' 공개, 현대차, 신입·경력 세자릿수 채용…"R&amp;D 인재 확보", 중고차 1대당 판매수익, 신차보다 커... “현대차·기아 수익 5조원에..., "현대차 러 공장 푸틴에 뺏길 판" 국유화 피해 볼 가능성↑, 중고차 1대당 판매수익, 신차보다 커... “현대차·기아 수익 5조원에..., 모빌리티 전문가 모십니다…현대차, R&amp;D 신입·경력 채용, 현대차, 연구개발본부 신입·경력 대규모 채용…11일까지 접수, 초고유가 시대, 경유값 아껴요…현대차, 상용차 전용 카드 출시, 현대차, R&amp;D 신입·경력 각각 세자릿수 채용, 현대차, R&amp;D 신입·경력 각각 세자릿수 채용, 현대차-현대카드, 상용차 고객 전용 카드 출시, 현대차, 쏘카와 커넥티드 카 운영체제 연계를 위한 업무협약 체결, 현대차, 상용차 고객 위한 ‘현대 모빌리티 카드(상용차)’ 론칭, 현대자동차, 쏘카와 커넥티드 카 운영체제 연계 업무협약, 나에게 맞춘 공유車 내놓는다…현대차·쏘카 업무협약, 쏘카에 현대차 커넥티드카 OS 들어온다, 모빌리티 전문가 모십니다…현대차, R&amp;D 신입·경력 채용, 현대차 "R&amp;D 인재 미리 확보하자"…로보틱스·배터리 등 대거 채용, 현대차, R&amp;D 신입·경력 각각 세자릿수 채용, 현대차, 신입·경력 세자릿수 채용…"R&amp;D 인재 확보", 쏘카, 현대차 커넥티드 카 전용 SW와 연계한다, 트럭·버스 등 상용차 고객 전용 ‘Hyundai Mobility카드’..., 현대카드, 트럭?버스 등 고객 전용 '현대 모빌리티카드(상용차)' 공개, 현대차, 상용차 고객 위한 ‘현대 모빌리티 카드(상용차)’ 론칭</t>
+    <t>트럭·버스 등 상용차 고객 전용 ‘Hyundai Mobility카드’..., 쏘카·현대차 ‘커넥티드카 OS’ 손잡는다, 쏘카, 현대차 커넥티드 카 전용 SW와 연계한다, 현대차·기아·모비스, 국내 외 특허 5만건 돌파, 쏘카, '커넥티드카' 맞손, 쏘카에 현대차 커넥티드카 OS 들어온다, 현대차 '혼류생산' 본격 가동…한 라인서 10차종 만든다, "현대차 러 공장 푸틴에 뺏길 판" 국유화 피해 볼 가능성↑, 현대카드, 트럭?버스 등 고객 전용 '현대 모빌리티카드(상용차)' 공개, 현대차, 신입·경력 세자릿수 채용…"R&amp;D 인재 확보", 중고차 1대당 판매수익, 신차보다 커... “현대차·기아 수익 5조원에..., "현대차 러 공장 푸틴에 뺏길 판" 국유화 피해 볼 가능성↑, 중고차 1대당 판매수익, 신차보다 커... “현대차·기아 수익 5조원에..., 모빌리티 전문가 모십니다…현대차, R&amp;D 신입·경력 채용, 현대차, 연구개발본부 신입·경력 대규모 채용…11일까지 접수, 초고유가 시대, 경유값 아껴요…현대차, 상용차 전용 카드 출시, 현대차, R&amp;D 신입·경력 각각 세자릿수 채용, 현대차, R&amp;D 신입·경력 각각 세자릿수 채용, 현대카드, 상용차 고객 전용 카드 출시, 현대차, 쏘카와 커넥티드 카 운영체제 연계를 위한 업무협약 체결, 현대차, 상용차 고객 위한 ‘현대 모빌리티 카드(상용차)’ 론칭, 현대자동차, 쏘카와 커넥티드 카 운영체제 연계 업무협약, 나에게 맞춘 공유車 내놓는다…현대차·쏘카 업무협약, 쏘카에 현대차 커넥티드카 OS 들어온다, 모빌리티 전문가 모십니다…현대차, R&amp;D 신입·경력 채용, 현대차 "R&amp;D 인재 미리 확보하자"…로보틱스·배터리 등 대거 채용, 현대차, R&amp;D 신입·경력 각각 세자릿수 채용, 현대차, 신입·경력 세자릿수 채용…"R&amp;D 인재 확보", 쏘카, 현대차 커넥티드 카 전용 SW와 연계한다, 트럭·버스 등 상용차 고객 전용 ‘Hyundai Mobility카드’..., 현대카드, 트럭?버스 등 고객 전용 '현대 모빌리티카드(상용차)' 공개, 현대차, 상용차 고객 위한 ‘현대 모빌리티 카드(상용차)’ 론칭</t>
   </si>
   <si>
     <t>현대차 전용 전기차 ‘아이오닉5’ 독일서 아우디·폴스타 넘어섰다, 현대차 아이오닉 5, 독일서 아우디·폴스타 전기차 제쳤다, "포르쉐·테슬라보다 현대차 좋다"…또다시 독일 놀래킨 아이오닉5 [왜몰..., 현대차 전용 전기차 ‘아이오닉5’ 독일서 아우디·폴스타 넘어섰다, 현대차 아이오닉 5, 독일서 아우디·폴스타 전기차 제쳤다, 현대차그룹, 작년 토요타·폭스바겐 제치고 매출성장률 1위, "포르쉐·테슬라보다 현대차 좋다"…또다시 독일 놀래킨 아이오닉5 [왜몰..., 현대차, 올 하반기 ‘레벨3’ G90 출시…산업장관 “미래차 생태계 키..., "포르쉐·테슬라보다 현대차 좋다"…또다시 독일 놀래킨 아이오닉5 [왜몰..., "현대·기아차, 중고차 시장 대안 아냐"…中企업계 릴레이 집회(종합), 현대차·기아, 지난해 매출성장률 글로벌 완성차 1위, 현대차 아이오닉 5, 독일서 아우디·폴스타 전기차 제쳤다, 현대차 전용 전기차 ‘아이오닉5’ 독일서 아우디·폴스타 넘어섰다, 현대차그룹, 작년 토요타·폭스바겐 제치고 매출성장률 1위, 현대차, 올 하반기 ‘레벨3’ G90 출시…산업장관 “미래차 생태계 키..., ‘HD현대’로 사명 바꾼 현대重지주, 정기선 체제 본격화, "현대·기아차, 중고차 시장 대안 아냐"…中企업계 릴레이 집회(종합), (영상)현대차그룹, 美 친환경차 누적판매 50만대 돌파, ‘HD현대’로 사명 바꾼 현대重지주, 정기선 체제 본격화, 현대차 아이오닉5, 獨 아우토빌트 평가서 1위…아우디·폴스타 추월, ‘친환경 톱 티어’ 공언한 현대차, 美 누적판매 50만대 돌파, 현대차·기아, 지난해 매출성장률 글로벌 완성차 1위, (영상)현대차그룹, 美 친환경차 누적판매 50만대 돌파, ‘친환경 톱 티어’ 공언한 현대차, 美 누적판매 50만대 돌파, 현대 아이오닉5, 獨 전문지 평가서 아우디·폴스타 제쳐</t>
   </si>
   <si>
-    <t>현대차그룹, 獨레드닷 디자인상 5개 석권, 현대차-년도년도 2분기 1분기 Preview - 판매는 부진하지만 환율은 긍정적, 목표주가 240,000원으로 기존대비 15.8% 하향하나 투자의견 Buy 유지, 년도년도 2분기 1분기 영업이익 1.7조원 (+2.8% 전년 대비 증감율) 전망, 투자포인트: 1) 자동차 소비시장에 대한 우려 완화, 2) 원화가치 절하, 3) 전기차 점유율 반등, 리스크 요인: 1) 소비심리 위축, 2) 반도체 부족 및 원자재 가격 상승, 3) 인센티브 축소 여력 부족, 현대차, ‘레드닷 어워드’ 5개 부문 수상, 현대차그룹, 獨레드닷 디자인상 5개 석권, 중고차매매업 “독점 재벌 현대기아차 매매업 진출 결사 반대”, 현대차 중고차 시장 진출…레몬마켓 바꾸는 ‘메기’ 될까, 현대차그룹, '레드 닷 어워드' 제품 디자인 최우수상 등 5개 수상, 현대차, 車판매부진에 年영업익 9% 하향…목표가↓-KB, 현대차, ‘레드닷 어워드’ 5개 부문 수상, 현대차, 스타리아로 '레드 닷 어워드' 최우수상 수상, 현대차, 자동차 판매 부진에도 투심 개선…'매수' 의견 유지 -KB證, KB證 "현대차, 자동차 판매량 예상보다 부진" 목표주가 15.8% ↓, 현대차그룹, 2022 레드 닷 어워드 휩쓸어…5개 부문 석권, 현대차그룹, 獨레드닷 디자인상 5개 석권, 현대차, 자동차 판매 부진에도 투심 개선…'매수' 의견 유지 -KB證, KB證 "현대차, 자동차 판매량 예상보다 부진" 목표주가 15.8% ↓, 현대차그룹, 獨레드닷 디자인상 5개 석권, 현대차, 獨서 디자인상 휩쓸었다, 현대차그룹, 세계 3대 디자인상 '레드 닷 어워드'에서 5개 상 받아, 중고차 업계 "현대차·기아 매집 제한해야…유예기간 3년 필요"</t>
+    <t>현대차그룹, 獨레드닷 디자인상 5개 석권, 년도년도 2분기 1분기 Preview - 판매는 부진하지만 환율은 긍정적, 목표주가 240,000원으로 기존대비 15.8% 하향하나 투자의견 Buy 유지, 년도년도 2분기 1분기 영업이익 1.7조원 (+2.8% 전년 대비 증감율) 전망, 투자포인트: 1) 자동차 소비시장에 대한 우려 완화, 2) 원화가치 절하, 3) 전기차 점유율 반등, 리스크 요인: 1) 소비심리 위축, 2) 반도체 부족 및 원자재 가격 상승, 3) 인센티브 축소 여력 부족, 현대차, ‘레드닷 어워드’ 5개 부문 수상, 현대차그룹, 獨레드닷 디자인상 5개 석권, 중고차매매업 “독점 재벌 현대기아차 매매업 진출 결사 반대”, 현대차 중고차 시장 진출…레몬마켓 바꾸는 ‘메기’ 될까, 현대차그룹, '레드 닷 어워드' 제품 디자인 최우수상 등 5개 수상, 현대차, 車판매부진에 年영업익 9% 하향…목표가↓-KB, 현대차, ‘레드닷 어워드’ 5개 부문 수상, 현대차, 스타리아로 '레드 닷 어워드' 최우수상 수상, 현대차, 자동차 판매 부진에도 투심 개선…'매수' 의견 유지 -KB證, KB證 "현대차, 자동차 판매량 예상보다 부진" 목표주가 15.8% ↓, 현대차그룹, 2022 레드 닷 어워드 휩쓸어…5개 부문 석권, 현대차그룹, 獨레드닷 디자인상 5개 석권, 현대차, 자동차 판매 부진에도 투심 개선…'매수' 의견 유지 -KB證, KB證 "현대차, 자동차 판매량 예상보다 부진" 목표주가 15.8% ↓, 현대차그룹, 獨레드닷 디자인상 5개 석권, 현대차, 獨서 디자인상 휩쓸었다, 현대차그룹, 세계 3대 디자인상 '레드 닷 어워드'에서 5개 상 받아, 중고차 업계 "현대차·기아 매집 제한해야…유예기간 3년 필요"</t>
   </si>
   <si>
     <t>기관 ‘사자’에 코스피 상승 마감…현대차·기아 2%대 오름세 [마감시황..., 저점 대비 12% 반등한 현대차…악재 반영 끝났나, 외국인 올라탄 현대차, 반등 시동 걸었다, 현대차그룹, 아람코와 친환경 엔진·연료 개발, 현대차, 아람코와 내연車 친환경 엔진·연료 공동개발, 외국인 올라탄 현대차, 반등 시동 걸었다, 저점 대비 12% 반등한 현대차…악재 반영 끝났나, 현대차그룹, 아람코와 친환경 엔진·연료 개발, 현대차, 아람코와 내연車 친환경 엔진·연료 공동개발, 기관 ‘사자’에 코스피 상승 마감…현대차·기아 2%대 오름세 [마감시황..., '천슬라' 날아오르는데…개미들 "현대차·기아 언제 쫓아가나", 현대차 ‘온실가스 저감’ 엔진·연료 개발한다, 현대차, 아람코와 친환경 엔진 개발, 아람코, 현대차와 첨단연료 공동 연구개발 추진, "CO2 적게, 더 적게" 아람코·현대차 첨단연료 합작개발 나선다, 현대차, 1~2월 전 세계 수소차 판매 1위…점유율 48.5％, 건설사 잇따라 회사채 발행…삼성 이어 롯데·현대도, 현대차, 아람코와 친환경 엔진 개발, 현대차그룹, 사우디 아람코와 '협력'…친환경 엔진·연료 개발, 현대차 장 초반 강세, 드디어 움직이나…우크라 사태 해결 조짐·아람코..., 현대차그룹, 사우디 아람코와 '협력'…친환경 엔진·연료 개발, 기관 ‘사자’에 코스피 상승 마감…현대차·기아 2%대 오름세 [마감시황..., "에너지 전환 과도기, 적합한 엔진·연료 찾자"…현대차·사우디 아람코 ..., '천슬라' 날아오르는데…개미들 "현대차·기아 언제 쫓아가나", 건설사 잇따라 회사채 발행…삼성 이어 롯데·현대도, "에너지 전환 과도기, 적합한 엔진·연료 찾자"…현대차·사우디 아람코 ..., 현대차그룹·아람코·KAUST, ‘온실가스 저감’ 친환경 엔진·연료 개..., "CO2 적게, 더 적게" 아람코·현대차 첨단연료 합작개발 나선다, 현대차·아람코, 내연기관차용 친환경 엔진·연료 공동개발, 저점 대비 12% 반등한 현대차…악재 반영 끝났나, 외국인 올라탄 현대차, 반등 시동 걸었다, "CO2 적게, 더 적게" 아람코·현대차 첨단연료 합작개발 나선다, 아람코, 현대차와 첨단연료 공동 연구개발 추진, 현대차그룹·아람코·KAUST, ‘온실가스 저감’ 친환경 엔진·연료 개...</t>
@@ -7828,10 +7828,10 @@
     <t>삼성·현대차·SK 임원 죄다 ‘SKY’ 출신인데…LG는 ‘이 대학’이 ..., “지금사면 손해?”...현대차, 아이오닉5 주행거리 더 늘린다, 유럽 질주 '현대기아 전기차', 올 하반기 이후 녹록지않다, 삼성·현대차·SK 임원 죄다 ‘SKY’ 출신인데…LG는 ‘이 대학’이 ..., "上, 上, 上 7번의 상한가" 524% 수익률 현대사료 미스터리, 전기차 인력 감소에도 노조는 “인력충원”…현대차 임단협 험로 예고 [..., 현대차, 올 노사협상 ‘가시밭길’ 예고, 전기차 인력 감소에도 노조는 “인력충원”…현대차 임단협 험로 예고 [..., 유럽 질주 '현대기아 전기차', 올 하반기 이후 녹록지않다, 유럽서 테슬라 제친 현대·기아 전기차, 하반기 이후 쉽지 않다(종합), “지금사면 손해?”...현대차, 아이오닉5 주행거리 더 늘린다, 현대차, 올 노사협상 ‘가시밭길’ 예고</t>
   </si>
   <si>
-    <t>작년 세계 전기차 판매 두 배 급증…현대차·기아 5위, 현대차-22년도 1분기 Preview: 차별화에 시간이 필요, 1분기 글로벌 판매 대수는 90만 대로 느린 회복, 2021년 신흥시장 판매 비중이 46%로 글로벌 업체 중 가장 높음, 단기 모멘텀 부재로 당분간 주가는 박스권에서 횡보할 것으로 예상, 현대차, 상반기 채용전환형 인턴 모집, 전기동력차 판매 1년새 2배로… 현대차·기아 5위, 작년 전기차 666만대 팔려…테슬라 압도적 1위, 현대차기아는?, 현대차 국내사업본부, 상반기 채용전환 인턴 모집, 현대차 국내사업본부 상반기 채용전환형 인턴 모집, 현대차·기아, 전기차 글로벌 '톱5', 현대커머셜, 현대차 트럭 구매자에 '맞춤형 할부' 제공, 현대차, 국내사업본부 상반기 채용전환형 인턴 모집, 현대캐피탈, 현대자동차 상용 트럭 구입 차주 대상 맞춤형 할부 프로그램..., 현대커머셜, 현대차 트럭 구매자에 '맞춤형 할부' 제공, 현대커머셜, 상용트럭 구입 차주에 최대 10년 할부 지원, '코로나격려금' 언제 주나··· 현대차그룹 계열사 성과급 갈등은 '현재..., 현대차, 실적 전망치 소폭 하회할 듯…단기 모멘텀 부재-삼성, 올해 코스피 시총 순위 보니…금융주 '맑음' 현대차·카카오 '흐림', 현대커머셜, 유류비 지출 커진 화물차 기사 부담 던다, '코로나격려금' 언제 주나··· 현대차그룹 계열사 성과급 갈등은 '현재..., 현대차 국내사업본부, 상반기 채용전환형 인턴 모집, 현대차 국내사업본부 상반기 채용전환형 인턴 모집, 현대커머셜, 상용트럭 구입 차주에 최대 10년 할부 지원, 전기동력차, 작년 2배 성장했다는데…현대차·기아 순위는?, 올해 코스피 시총 순위 보니…금융주 '맑음' 현대차·카카오 '흐림', 전기동력차, 작년 2배 성장했다는데…현대차·기아 순위는? [비즈360..., 작년 세계 전기차 판매 두 배 급증…현대차·기아 5위, 현대차 국내사업본부 상반기 채용전환형 인턴 모집, 지난해 글로벌 전기동력차 666만대 판매 '두배 성장'…현대차·기아 '..., 현대차, 실적 전망치 소폭 하회할 듯…단기 모멘텀 부재-삼성, '코로나격려금' 언제 주나··· 현대차그룹 계열사 성과급 갈등은 '현재..., 현대차, 실적 전망치 소폭 하회할 듯…단기 모멘텀 부재-삼성, 현대캐피탈, 현대자동차 상용 트럭 구입 차주 대상 맞춤형 할부 프로그램...</t>
-  </si>
-  <si>
-    <t>현대차-일당백이 되어가는 제네시스, 22년도 1분기 Preview: Q는 부진했으나 제네시스 성장으로 P 확보, 출고판매량 회복세 확인 필요, 그러나 추가적인 전동화 전략 발표 기대감도, 투자의견 Buy 유지, 목표주가 280,000원으로 하향, 현대차-하반기 가동률 개선 기대, 하반기 정상화 감안한 Valuation 매력 보유, 1분기 Preview: 우려대비 양호한 수익성, 현대차 "독자기술" SK온 "포드와 합작"…폐배터리 공략 가속도, 현대차 "독자기술" SK온 "포드와 합작"…폐배터리 공략 가속도, 스페인 물류대란에도…기아·현대차, 현지 점유율 1·2위, "생산 정상화 가시성 높아져야…현대차 목표가 12.5%↓"-하이, "현대차, 대외적 불확실성 지속에 글로벌 판매량↓…목표가 12.5% 하..., 현대ENG, 미국기계학회서 원자력 시공 기술력 인정받았다, 스페인 물류대란에도…기아·현대차, 현지 점유율 1·2위, "현대차, 대외적 불확실성 지속에 글로벌 판매량↓…목표가 12.5% 하..., "생산 정상화 가시성 높아져야…현대차 목표가 12.5%↓"-하이, 메타버스엔터테인먼트, 현대자동차그룹 제로원 펀드 투자 유치, 넷마블 ‘디지털휴먼’ 현대차그룹 펀드서 투자 유치, 현대차그룹, 넷마블 '가상인간' 사업에 20억원 투자, 현대차·기아, 전동화 전환 '가속페달'…지속가능한 모빌리티 기업 도약, "테슬라·구글 잡자"…현대차도 OS 경쟁, 현대ENG, 미국기계학회서 원자력 시공 기술력 인정받았다</t>
+    <t>작년 세계 전기차 판매 두 배 급증…현대차·기아 5위, 22년도 1분기 Preview: 차별화에 시간이 필요, 1분기 글로벌 판매 대수는 90만 대로 느린 회복, 2021년 신흥시장 판매 비중이 46%로 글로벌 업체 중 가장 높음, 단기 모멘텀 부재로 당분간 주가는 박스권에서 횡보할 것으로 예상, 현대차, 상반기 채용전환형 인턴 모집, 전기동력차 판매 1년새 2배로… 현대차·기아 5위, 작년 전기차 666만대 팔려…테슬라 압도적 1위, 현대차기아는?, 현대차 국내사업본부, 상반기 채용전환 인턴 모집, 현대차 국내사업본부 상반기 채용전환형 인턴 모집, 현대차·기아, 전기차 글로벌 '톱5', 현대커머셜, 현대차 트럭 구매자에 '맞춤형 할부' 제공, 현대차, 국내사업본부 상반기 채용전환형 인턴 모집, 현대캐피탈, 현대자동차 상용 트럭 구입 차주 대상 맞춤형 할부 프로그램..., 현대커머셜, 현대차 트럭 구매자에 '맞춤형 할부' 제공, 현대커머셜, 상용트럭 구입 차주에 최대 10년 할부 지원, '코로나격려금' 언제 주나··· 현대차그룹 계열사 성과급 갈등은 '현재..., 현대차, 실적 전망치 소폭 하회할 듯…단기 모멘텀 부재-삼성, 올해 코스피 시총 순위 보니…금융주 '맑음' 현대차·카카오 '흐림', 현대커머셜, 유류비 지출 커진 화물차 기사 부담 던다, '코로나격려금' 언제 주나··· 현대차그룹 계열사 성과급 갈등은 '현재..., 현대차 국내사업본부, 상반기 채용전환형 인턴 모집, 현대차 국내사업본부 상반기 채용전환형 인턴 모집, 현대커머셜, 상용트럭 구입 차주에 최대 10년 할부 지원, 전기동력차, 작년 2배 성장했다는데…현대차·기아 순위는?, 올해 코스피 시총 순위 보니…금융주 '맑음' 현대차·카카오 '흐림', 전기동력차, 작년 2배 성장했다는데…현대차·기아 순위는? [비즈360..., 작년 세계 전기차 판매 두 배 급증…현대차·기아 5위, 현대차 국내사업본부 상반기 채용전환형 인턴 모집, 지난해 글로벌 전기동력차 666만대 판매 '두배 성장'…현대차·기아 '..., 현대차, 실적 전망치 소폭 하회할 듯…단기 모멘텀 부재-삼성, '코로나격려금' 언제 주나··· 현대차그룹 계열사 성과급 갈등은 '현재..., 현대차, 실적 전망치 소폭 하회할 듯…단기 모멘텀 부재-삼성, 현대캐피탈, 현대자동차 상용 트럭 구입 차주 대상 맞춤형 할부 프로그램...</t>
+  </si>
+  <si>
+    <t>일당백이 되어가는 제네시스, 22년도 1분기 Preview: Q는 부진했으나 제네시스 성장으로 P 확보, 출고판매량 회복세 확인 필요, 그러나 추가적인 전동화 전략 발표 기대감도, 투자의견 Buy 유지, 목표주가 280,000원으로 하향, 하반기 가동률 개선 기대, 하반기 정상화 감안한 Valuation 매력 보유, 1분기 Preview: 우려대비 양호한 수익성, 현대차 "독자기술" SK온 "포드와 합작"…폐배터리 공략 가속도, 현대차 "독자기술" SK온 "포드와 합작"…폐배터리 공략 가속도, 스페인 물류대란에도…기아·현대차, 현지 점유율 1·2위, "생산 정상화 가시성 높아져야…현대차 목표가 12.5%↓"-하이, "현대차, 대외적 불확실성 지속에 글로벌 판매량↓…목표가 12.5% 하..., 현대ENG, 미국기계학회서 원자력 시공 기술력 인정받았다, 스페인 물류대란에도…기아·현대차, 현지 점유율 1·2위, "현대차, 대외적 불확실성 지속에 글로벌 판매량↓…목표가 12.5% 하..., "생산 정상화 가시성 높아져야…현대차 목표가 12.5%↓"-하이, 메타버스엔터테인먼트, 현대자동차그룹 제로원 펀드 투자 유치, 넷마블 ‘디지털휴먼’ 현대차그룹 펀드서 투자 유치, 현대차그룹, 넷마블 '가상인간' 사업에 20억원 투자, 현대차·기아, 전동화 전환 '가속페달'…지속가능한 모빌리티 기업 도약, "테슬라·구글 잡자"…현대차도 OS 경쟁, 현대ENG, 미국기계학회서 원자력 시공 기술력 인정받았다</t>
   </si>
   <si>
     <t>현대차·기아, 러시아 전쟁 여파에 현지 판매 68% 급감, 강경파 돌아온 현대차 노조 '품질협의체' 중단 선언 [새정부, 춘투가 ..., 현대차·기아 러시아 판매 전쟁 여파로 68% 급감, 전기차 충전시간 절반으로…현대차 新기술, 대통령상..., 안철수, 8일 현대·기아차 방문…미래 모빌리티 육성 머리 맞댄다, 기아·현대·폭스바겐·벤츠·맥라렌 등 23만3557대 시정조치, 현대차 GV80·넥쏘 안전기준 부적합… 리콜 후 과징금 부과, 현대차, 더 뉴 팰리세이드 티저 이미지 공개, 현대차 '더 뉴 팰리세이드' 13일 공개한다, 더 웅장하게 돌아왔다…현대차 ‘더 뉴 팰리세이드’ 티저 공개, 1분기 車판매량 보니… 현대차·한국지엠 판매량↓, 1분기 車판매량 보니… 현대차·한국지엠 판매량↓, 현대차·기아, 美 학술기업 선정 글로벌 100대 혁신기업 선정, 벤츠·맥라렌 에어백 불량…기아·현대 등 23만여대 '리콜', ‘파라메트릭 실드’로 웅장하게 돌아왔다…현대차, 팰리세이드 부분변경 ..., 현대차, 신형 팰리세이드 티저이미지 공개…뉴욕오토쇼서 세계 첫선, 테슬라 생산 차질 '직격탄' 맞았는데…현대차는 괜찮은 이유, 삼성전자 이어 현대차…경제계 메시지 보내는 인수위, 기아·현대·폭스바겐·벤츠·맥라렌 등 23만3557대 시정조치, 현대차·기아, 美 학술기업 선정 글로벌 100대 혁신기업 선정, 기아·현대·폭스바겐·벤츠·기흥 판매한 9개 차종 ‘리콜’, 테슬라 생산 차질 '직격탄' 맞았는데…현대차는 괜찮은 이유, 현대차, 신형 팰리세이드 티저이미지 공개…뉴욕오토쇼서 세계 첫선, ‘파라메트릭 실드’로 웅장하게 돌아왔다…현대차, 팰리세이드 부분변경 ...</t>
@@ -7846,16 +7846,16 @@
     <t>돌아온 외국인·리오프닝 기대감…반등 시동 건 현대차 주가, 현대차·기아, 1분기 친환경차 판매 비중 20% 넘어, 올해 팔린 현대차·기아 5대 중 1대가 친환경차</t>
   </si>
   <si>
-    <t>현대·기아차, 친환경차 판매 호조에 강세, 친환경 판매 호조 속에 현대·기아차 강세, 현대차, 초고속 전기 충전소 '이피트'에 차세대 플랫폼 적용, '국내 1위 복지몰' 현대이지웰에 꽂힌 큰손들, 친환경 판매 호조 속에 현대·기아차 강세, 현대차그룹, ‘E-pit’ 차세대 플랫폼 적용...충전 생태계 선도, "올해 삼전·하이닉스·현대차 시총 14%↓…외국인 매도 영향", “충전 생태계 선도”…현대차, ‘이피트’에 전기차 충전서비스 플랫폼 ..., 현대차, ‘이피트’에 차세대 충전플랫폼 적용, 현대차-22년도 1분기 Preview: 생각보다 선방, 1분기 실적 선방 전망, 루블화에 울었지만 달러에 웃었다, 전기차 경쟁력 기준의 변화, 목표주가 26만원으로 16% 하향, 현대차-가격 요인이 전사 수익성 방어 견인, 투자포인트 및 결론, 주요이슈 및 실적전망, 주가전망 및 Valuation, 현대차-판매 감소에도 불구하고 우려 대비 선방 전망, 매출 29조원, 영업이익 1.69조원 기록하며 기대치 부합 예상, 22년도 2분기 관건은 북미 회복 속도, 그리고 금융사업부, 기대 요인은 ASP 상승과 인센티브 하락, 현대·기아차, 친환경차 판매 호조에 강세, "현대차 초고속 충전시스템은 도로 삼킬 쿠데타", 현대차그룹, ‘E-pit’ 차세대 플랫폼 적용...충전 생태계 선도, NYT “현대차, 전기차 산업의 다크호스…테슬라 대안 될 것”, “테슬라 싫다고? 아이오닉5 어때”…뉴욕타임스, 현대차 극찬, 현대차, 목표주가 31만→26만-한투, 현대차, 목표주가 하향…이익 증가 모멘텀은 여전, 현대차, 미국 전기차 투자 기대감 주춤...목표가↓ -한국, 환율 상승 덕에 웃은 현대차…목표주가는 하향-한국투자증권, 핀다, 현대·기아차 전용 대출상품 출시, 현대차, 목표주가 31만→26만-한투, 현대차, 목표주가 하향…이익 증가 모멘텀은 여전, 현대차, 미국 전기차 투자 기대감 주춤...목표가↓ -한국, 환율 상승 덕에 웃은 현대차…목표주가는 하향-한국투자증권, "올해 삼전·하이닉스·현대차 시총 14%↓…외국인 매도 영향", 핀다, 현대차·기아 특화 '오토론' 출시…핀테크 업계 최초, '핀테크 업계 최초' 핀다, 현대·기아차 전용 대출상품 출시, 현대·기아차, 친환경차 판매 호조에 강세, 현대차그룹, ‘이피트’에 차세대 충전 플랫폼 적용…전기차 생태계 넓힌..., 현대차·현대중공업 중대재해법 조사, 현대차그룹, E-pit 충전 서비스 플랫폼 개방…"생태계 저변 확대", 뉴욕타임즈 "현대차, 전기차 산업의 다크호스 된다", 정의선 현대차그룹 회장, 뉴욕오토쇼 간다, 현대차·현대중공업 중대재해법 조사, 삼성, 회식·출장·대면회의 '재개'…현대차도 사내 방역지침 완화, 정의선 현대차그룹 회장, 뉴욕오토쇼 간다, 핀다, 현대차·기아 전용 비대면 오토론 상품 출시, 핀다, 핀테크 최초 현대·기아차 전용 대출상품 출시, 포스코·현대제철 vs 현대차·기아, 1조원 짜리 ‘강판값 줄다리기’, 현대차그룹, 초고속충전소 '이피트' 업그레이드...이달 제주 신규오픈, 현대차그룹, 차세대 충전 플랫폼 '개방…"생태계 선도", 뉴욕타임즈 "현대차가 전기차 산업의 다크호스 될 것", 삼성, 회식·출장·대면회의 '재개'…현대차도 사내 방역지침 완화</t>
+    <t>현대·기아차, 친환경차 판매 호조에 강세, 친환경 판매 호조 속에 현대·기아차 강세, 현대차, 초고속 전기 충전소 '이피트'에 차세대 플랫폼 적용, '국내 1위 복지몰' 현대이지웰에 꽂힌 큰손들, 친환경 판매 호조 속에 현대·기아차 강세, 현대차그룹, ‘E-pit’ 차세대 플랫폼 적용...충전 생태계 선도, "올해 삼전·하이닉스·현대차 시총 14%↓…외국인 매도 영향", “충전 생태계 선도”…현대차, ‘이피트’에 전기차 충전서비스 플랫폼 ..., 현대차, ‘이피트’에 차세대 충전플랫폼 적용, 22년도 1분기 Preview: 생각보다 선방, 1분기 실적 선방 전망, 루블화에 울었지만 달러에 웃었다, 전기차 경쟁력 기준의 변화, 목표주가 26만원으로 16% 하향, 가격 요인이 전사 수익성 방어 견인, 투자포인트 및 결론, 주요이슈 및 실적전망, 주가전망 및 Valuation, 판매 감소에도 불구하고 우려 대비 선방 전망, 매출 29조원, 영업이익 1.69조원 기록하며 기대치 부합 예상, 22년도 2분기 관건은 북미 회복 속도, 그리고 금융사업부, 기대 요인은 ASP 상승과 인센티브 하락, 현대·기아차, 친환경차 판매 호조에 강세, "현대차 초고속 충전시스템은 도로 삼킬 쿠데타", 현대차그룹, ‘E-pit’ 차세대 플랫폼 적용...충전 생태계 선도, NYT “현대차, 전기차 산업의 다크호스…테슬라 대안 될 것”, “테슬라 싫다고? 아이오닉5 어때”…뉴욕타임스, 현대차 극찬, 현대차, 목표주가 31만→26만-한투, 현대차, 목표주가 하향…이익 증가 모멘텀은 여전, 현대차, 미국 전기차 투자 기대감 주춤...목표가↓ -한국, 환율 상승 덕에 웃은 현대차…목표주가는 하향-한국투자증권, 핀다, 현대·기아차 전용 대출상품 출시, 현대차, 목표주가 31만→26만-한투, 현대차, 목표주가 하향…이익 증가 모멘텀은 여전, 현대차, 미국 전기차 투자 기대감 주춤...목표가↓ -한국, 환율 상승 덕에 웃은 현대차…목표주가는 하향-한국투자증권, "올해 삼전·하이닉스·현대차 시총 14%↓…외국인 매도 영향", 핀다, 현대차·기아 특화 '오토론' 출시…핀테크 업계 최초, '핀테크 업계 최초' 핀다, 현대·기아차 전용 대출상품 출시, 현대·기아차, 친환경차 판매 호조에 강세, 현대차그룹, ‘이피트’에 차세대 충전 플랫폼 적용…전기차 생태계 넓힌..., 현대차·현대중공업 중대재해법 조사, 현대차그룹, E-pit 충전 서비스 플랫폼 개방…"생태계 저변 확대", 뉴욕타임즈 "현대차, 전기차 산업의 다크호스 된다", 정의선 현대차그룹 회장, 뉴욕오토쇼 간다, 현대차·현대중공업 중대재해법 조사, 삼성, 회식·출장·대면회의 '재개'…현대차도 사내 방역지침 완화, 정의선 현대차그룹 회장, 뉴욕오토쇼 간다, 핀다, 현대차·기아 전용 비대면 오토론 상품 출시, 핀다, 핀테크 최초 현대·기아차 전용 대출상품 출시, 포스코·현대제철 vs 현대차·기아, 1조원 짜리 ‘강판값 줄다리기’, 현대차그룹, 초고속충전소 '이피트' 업그레이드...이달 제주 신규오픈, 현대차그룹, 차세대 충전 플랫폼 '개방…"생태계 선도", 뉴욕타임즈 "현대차가 전기차 산업의 다크호스 될 것", 삼성, 회식·출장·대면회의 '재개'…현대차도 사내 방역지침 완화</t>
   </si>
   <si>
     <t>고가차 선전… 현대차 1분기 매출 30조 기대, 구영테크, 현대차 美 공장 선정 소식에 상한가, 인스타서 자주 보던 캐릭터 '르르르'…현대차 작품이었네, 인스타서 자주 보던 캐릭터 '르르르'…현대차 작품이었네, 고가차 선전… 현대차 1분기 매출 30조 기대, 구영테크, 현대차 친환경차 사업확장 기대감에 상한가, 구영테크, 현대차 친환경차 사업확장 기대감에 상한가, 현대차 ‘2022 코나’ 출시…안전·편의 높여 상품성 ↑, ‘선호사양 기본화’ 현대차 2022 코나 출시…가격 2144만원부터, "반도체·러시아 때문에" 현대차, 1분기 이익성장 0%대 그칠 듯, 삼성·현대차 등 ‘로봇 경쟁’ 불붙었지만…정부 인증기준도 미비[뒷북비즈..., 현대차 '2022 코나' 출시...가격 2144만원부터, 구영테크, 현대차 美 공장 선정 소식에 상한가, "반도체·러시아 때문에" 현대차, 1분기 이익성장 0%대 그칠 듯, 삼성·현대차 등 ‘로봇 경쟁’ 불붙었지만…정부 인증기준도 미비[뒷북비즈..., 현대차 ‘2022 코나’ 출시…안전·편의 높여 상품성 ↑, 현대차, 상품성 강화한 '2022 코나' 출시, 현대차, ‘2022 코나’ 출시…"2144만원부터", "스마트폰만 있으면 차문이 활짝"…현대차그룹, '디지털 키 2' 서비스..., 현대차, 러시아 공장 출하대수 83％ ‘뚝’…정상화는 언제? [비즈36..., 현대차 '2022 코나' 출시…2140만원부터 최대 3050만원, "LNG 운송도 잘해요"…현대車만 나르던 현대글로비스의 '환골탈태', 스마트폰 안꺼내도 차 문 열고 시동 건다...현대차그룹 '디지털 키 ..., 현대차, 스마트폰으로 문 열고 시동까지 건다, 현대차·기아, 협력사 설날자금 1조4천억 미리 지급…우수 R&amp;D기업도 ..., 아진산업, 현대차 美전기차 공장선정.. 아진USA 수혜 기대..., 현대차 '2022 코나' 출시…2140만원부터 최대 3050만원, 현대차 ‘2022 코나’ 출시…안전·편의 높여 상품성 ↑, 현대차그룹, 비접촉식 ‘디지털 키 2’ 서비스 제공, 현대차, 스마트폰으로 문 열고 시동까지 건다, 아진산업, 현대차 美전기차 공장선정.. 아진USA 수혜 기대..., "LNG 운송도 잘해요"…현대車만 나르던 현대글로비스의 '환골탈태'</t>
   </si>
   <si>
-    <t>"인기 車 받으려면 1년씩 대기해야"…현대차, 실적도 '적신호', 현대차, 테슬라에 맞불…美서 전기차 만든다, 현대차-제네시스가 주는 안정감, 투자의견 매수, 목표주가 210,000원으로 커버리지 개시, 22년도 1분기 를 저점으로 전년 대비 증감율 증익 흐름 지속, 제네시스 라인업/지역 확장에 따른 안정적 성장, 현대차, 美앨라배마 공장에 3600억 투자…GV70 전기차 생산 [종..., "차키 깜빡해도 괜찮아요" 현대차, 스마트폰으로 차문 열고 시동 건다, "인기 車 받으려면 1년씩 대기해야"…현대차, 실적도 '적신호', 현대차 美 앨라배마 공장, 전기차 생산 거점된다, 현대차, 美 앨라배마에 3600억 투자…전기차 생산라인 늘린다, 현대차, 美 3천억대 투자에 외국인 현대家 '담자', "현대차, 제네시스 확장으로 안정적 성장할 것", 대신증권 “현대차, 제네시스 라인업 확장에 수익성 개선 전망…목표가 2..., 현대모비스, 현대차그룹과 함께 성장…목표가 25만원-대신, "현대차, 제네시스 확장으로 안정적 성장할 것", 현대차, 올해 1분기가 '저점'...목표주가 21만원 -대신證, 현대차, 3억달러 투자해 美서 전기차 만든다, 현대차, 美서 전기차 만든다...앨라배마공장에 3700억 투자, "현대차는 안돼" 비웃음 사라졌다…'상상예찬' 정의선, 창조적 파괴자 ..., "정의선, 미래 30년 車산업 이끌 리더"…현대차 6개 부문 절반 석권, 현대차, 美 첫 전기차 생산기지…앨라배마서 GV70 EV 만든다, 현대차 美 앨라배마 공장, 전기차 생산 거점된다, 현대모비스, 현대차그룹과 함께 성장…목표가 25만원-대신, "차키 깜빡해도 괜찮아요" 현대차, 스마트폰으로 차문 열고 시동 건다</t>
-  </si>
-  <si>
-    <t>아이오닉5 '세계 최고 車' 된 날…정의선 "현대차 아직 갈 길 멀다", 현대무벡스, 세계 최초 로봇 전용 엘리베이터 상용화, 현대차 '우선주'로 달리나, 현대차-선방 후 역습 시작, 년도년도 2분기 1분기 실적 Preview, 년도년도 2분기 1분기 이후 분기 실적 개선 지속, 글로벌 전기차 M/S 반등에 따른 주가 멀티플 상승 기대, “변화는 진행형” 정의선 회장이 밝힌 현대차그룹의 과제, "20대가 아니었다"...현대차 캐스퍼, 주요 구매층은?, 현대차-우선주 매수 적기, 바로 지금, 우선주 투자 매력도 점검, 반도체 공급 정상화 + 낮은 재고 = 단기 실적 및 배당 눈높이 강화 근거, 인도 빠른 현대차그룹, 1분기 국내 판매 테슬라에 '승전보', 美서 '3관왕'했지만 겸손한 정의선 "현대차는 아직...", 현대차·기아, 뉴욕오토쇼서 뉴 팰리세이드·텔루라이드 첫 선, 美서 '3관왕'했지만 겸손한 정의선 "현대차는 아직...", 현대무벡스, 세계 최초 ‘로봇 전용 엘리베이터’ 상용화, 포드·현대·혼다·테슬라 등 7개사 5만4390대 시정조치, 美 전기차 공략 나선 현대차…선봉장은 'GV70', 메리츠증권 “현대차, 단기 실적·배당 눈높이 상향 가능성…우선주 주목해..., 현대차, 펠리세이드 부분변경 모델 공개…5월 중 국내 출시, 현대차, 더 뉴 팰리세이드 공개...더 웅장하고 고급스러워졌다, 현대차 정몽구 재단, 21일부터 ‘온드림 소사이어티 위크’, 현대차, 포드·벤츠 제쳐…아이오닉5 '2022 세계 올해의 자동차', 현대차, 3년 만에 열린 뉴욕오토쇼서 신형 팰리세이드·텔루라이드 공개, 현대차 아이오닉5, 전 세계 No.1 전기차 등극, 티에이치엔, 현대수소차 넥쏘 中신에너지차 정식 라이센스 취득..., 뉴인텍, 현대수소차 中보조금 날개...콘덴서 독점공급 업체 ..., 유니크, 현대차 수소차 ‘넥쏘’ 中 보조금 혜택 소식에↑, 정의선의 '퍼스트 무버' 전략...현대차그룹 '전기차의 명가' 반열에, 현대차, 더 뉴 팰리세이드 공개...더 웅장하고 고급스러워졌다, 더 웅장하고 똑똑해졌다…현대차 ‘더 뉴 팰리세이드’ 세계 최초 공개, 정의선 회장 "현대차의 적은 우리 자신…'변화'가 중요", 정의선의 '퍼스트 무버' 전략...현대차그룹 '전기차의 명가' 반열에, 현대차, 더 뉴 팰리세이드 공개...더 웅장하고 고급스러워졌다, 더 웅장하고 똑똑해졌다…현대차 ‘더 뉴 팰리세이드’ 세계 최초 공개, 정의선 회장 "현대차의 적은 우리 자신…'변화'가 중요", 美 전기차 공략 나선 현대차…선봉장은 'GV70', 동원금속, 현대차 美앨라배마 전기차 현지 최초 생산...미국..., 현대ENG '2022 HEC 주거트렌드' 발표, 현대차, 3년 만에 열린 뉴욕오토쇼서 신형 팰리세이드·텔루라이드 공개, 현대차·기아, 뉴욕오토쇼서 뉴 팰리세이드·텔루라이드 첫 선, 인도 빠른 현대차그룹, 1분기 국내 판매 테슬라에 '승전보', "10개 승강기 순환하며 로봇 이송" 현대무벡스, 네이버 신사옥서 상..., 현대차, 3년 만에 열린 뉴욕오토쇼서 신형 팰리세이드·텔루라이드 공개, 유니크, 현대차 수소차 ‘넥쏘’ 中 보조금 혜택 소식에↑</t>
+    <t>"인기 車 받으려면 1년씩 대기해야"…현대차, 실적도 '적신호', 현대차, 테슬라에 맞불…美서 전기차 만든다, 제네시스가 주는 안정감, 투자의견 매수, 목표주가 210,000원으로 커버리지 개시, 22년도 1분기 를 저점으로 전년 대비 증감율 증익 흐름 지속, 제네시스 라인업/지역 확장에 따른 안정적 성장, 현대차, 美앨라배마 공장에 3600억 투자…GV70 전기차 생산 [종..., "차키 깜빡해도 괜찮아요" 현대차, 스마트폰으로 차문 열고 시동 건다, "인기 車 받으려면 1년씩 대기해야"…현대차, 실적도 '적신호', 현대차 美 앨라배마 공장, 전기차 생산 거점된다, 현대차, 美 앨라배마에 3600억 투자…전기차 생산라인 늘린다, 현대차, 美 3천억대 투자에 외국인 현대家 '담자', "현대차, 제네시스 확장으로 안정적 성장할 것", 대신증권 “현대차, 제네시스 라인업 확장에 수익성 개선 전망…목표가 2..., 현대모비스, 현대차그룹과 함께 성장…목표가 25만원-대신, "현대차, 제네시스 확장으로 안정적 성장할 것", 현대차, 올해 1분기가 '저점'...목표주가 21만원 -대신證, 현대차, 3억달러 투자해 美서 전기차 만든다, 현대차, 美서 전기차 만든다...앨라배마공장에 3700억 투자, "현대차는 안돼" 비웃음 사라졌다…'상상예찬' 정의선, 창조적 파괴자 ..., "정의선, 미래 30년 車산업 이끌 리더"…현대차 6개 부문 절반 석권, 현대차, 美 첫 전기차 생산기지…앨라배마서 GV70 EV 만든다, 현대차 美 앨라배마 공장, 전기차 생산 거점된다, 현대모비스, 현대차그룹과 함께 성장…목표가 25만원-대신, "차키 깜빡해도 괜찮아요" 현대차, 스마트폰으로 차문 열고 시동 건다</t>
+  </si>
+  <si>
+    <t>아이오닉5 '세계 최고 車' 된 날…정의선 "현대차 아직 갈 길 멀다", 현대무벡스, 세계 최초 로봇 전용 엘리베이터 상용화, 현대차 '우선주'로 달리나, 선방 후 역습 시작, 년도년도 2분기 1분기 실적 Preview, 년도년도 2분기 1분기 이후 분기 실적 개선 지속, 글로벌 전기차 M/S 반등에 따른 주가 멀티플 상승 기대, “변화는 진행형” 정의선 회장이 밝힌 현대차그룹의 과제, "20대가 아니었다"...현대차 캐스퍼, 주요 구매층은?, 우선주 매수 적기, 바로 지금, 우선주 투자 매력도 점검, 반도체 공급 정상화 + 낮은 재고 = 단기 실적 및 배당 눈높이 강화 근거, 인도 빠른 현대차그룹, 1분기 국내 판매 테슬라에 '승전보', 美서 '3관왕'했지만 겸손한 정의선 "현대차는 아직...", 현대차·기아, 뉴욕오토쇼서 뉴 팰리세이드·텔루라이드 첫 선, 美서 '3관왕'했지만 겸손한 정의선 "현대차는 아직...", 현대무벡스, 세계 최초 ‘로봇 전용 엘리베이터’ 상용화, 포드·현대·혼다·테슬라 등 7개사 5만4390대 시정조치, 美 전기차 공략 나선 현대차…선봉장은 'GV70', 메리츠증권 “현대차, 단기 실적·배당 눈높이 상향 가능성…우선주 주목해..., 현대차, 펠리세이드 부분변경 모델 공개…5월 중 국내 출시, 현대차, 더 뉴 팰리세이드 공개...더 웅장하고 고급스러워졌다, 현대차 정몽구 재단, 21일부터 ‘온드림 소사이어티 위크’, 현대차, 포드·벤츠 제쳐…아이오닉5 '2022 세계 올해의 자동차', 현대차, 3년 만에 열린 뉴욕오토쇼서 신형 팰리세이드·텔루라이드 공개, 현대차 아이오닉5, 전 세계 No.1 전기차 등극, 티에이치엔, 현대수소차 넥쏘 中신에너지차 정식 라이센스 취득..., 뉴인텍, 현대수소차 中보조금 날개...콘덴서 독점공급 업체 ..., 유니크, 현대차 수소차 ‘넥쏘’ 中 보조금 혜택 소식에↑, 정의선의 '퍼스트 무버' 전략...현대차그룹 '전기차의 명가' 반열에, 현대차, 더 뉴 팰리세이드 공개...더 웅장하고 고급스러워졌다, 더 웅장하고 똑똑해졌다…현대차 ‘더 뉴 팰리세이드’ 세계 최초 공개, 정의선 회장 "현대차의 적은 우리 자신…'변화'가 중요", 정의선의 '퍼스트 무버' 전략...현대차그룹 '전기차의 명가' 반열에, 현대차, 더 뉴 팰리세이드 공개...더 웅장하고 고급스러워졌다, 더 웅장하고 똑똑해졌다…현대차 ‘더 뉴 팰리세이드’ 세계 최초 공개, 정의선 회장 "현대차의 적은 우리 자신…'변화'가 중요", 美 전기차 공략 나선 현대차…선봉장은 'GV70', 동원금속, 현대차 美앨라배마 전기차 현지 최초 생산...미국..., 현대ENG '2022 HEC 주거트렌드' 발표, 현대차, 3년 만에 열린 뉴욕오토쇼서 신형 팰리세이드·텔루라이드 공개, 현대차·기아, 뉴욕오토쇼서 뉴 팰리세이드·텔루라이드 첫 선, 인도 빠른 현대차그룹, 1분기 국내 판매 테슬라에 '승전보', "10개 승강기 순환하며 로봇 이송" 현대무벡스, 네이버 신사옥서 상..., 현대차, 3년 만에 열린 뉴욕오토쇼서 신형 팰리세이드·텔루라이드 공개, 유니크, 현대차 수소차 ‘넥쏘’ 中 보조금 혜택 소식에↑</t>
   </si>
   <si>
     <t>대유에이피, 현대차그룹 선정 ‘품질 5스타’ 달성, 현대무벡스, 네이버 신사옥에 ‘로보 포트’ 공급, 美·유럽 입모아 "현대차그룹 전기차가 1등"…재조명받는 '정의선 리더십..., 현대무벡스, 네이버 신사옥에 세계 최초 ‘로봇 전용 엘리베이터’ 구축, "기아 레이 잡는다"... 현대차 캐스퍼, 턱밑까지 추격, 글로벌 기세 올리는 현대차…정의선회장 '변화 예고', 이지트로닉스, 현대차도 70조 규모 '폐배터리 시장' 눈독↑..., 현대무벡스, 네이버 신사옥에 세계 최초 ‘로봇 전용 엘리베이터’ 구축, 현대차·기아, '회식 자제' 지침 해제…재택근무 축소, 엠플러스, 현대차 9조원 美 SK배터리 JV 설립 기대 속 장..., 코로나·더현대 때문에 안될 줄 알았는데…IFC몰, 방문객 오히려 늘었다</t>
@@ -7873,10 +7873,10 @@
     <t>전기차發 인력재편 '신호탄'... 현대차 직원 12년만에 감소 [전기차..., 전기차發 인력재편 '신호탄'... 현대차 직원 12년만에 감소 [전기차..., 전기차發 인력재편 '신호탄'... 현대차 직원 12년만에 감소 [전기차..., 현대차, 스타리아 라운지 리무진·캠퍼 출시, 현대차·기아 중고차, 언제부터 살 수 있나…사업계획 공식 발표, 현대차·기아, 반도체·코로나·전쟁 악재 극복할 카드는, 현대차, 스타리아 라운지 리무진·스타리아 캠퍼 출시, 현대차, 스타리아 리무진·캠퍼 모델 출시, 더 넓고 편하게…현대차, ‘스타리아 라운지 리무진·캠퍼’ 출시, 현대차 자동차 업계 최초 커뮤니티 기반 NFT 시장 진출, 현대차, 스타리아 라운지 리무진?캠퍼 출시, "미래 車산업 변화, 능동 대처하자" 현대차 노사 머리 맞대, “미래차 변화 속 직원 고용안정 모색”…현대차 고용안정위 4기 위촉, “미래차 변화 속 직원 고용안정 모색”…현대차 고용안정위 4기 위촉, 현대차·기아 전기차 '급속충전'…급변하는 시장 선두권 질주, "미래 車산업 변화, 능동 대처하자" 현대차 노사 머리 맞대, 현대차 ‘스타리아’, 리무진·캠퍼 모델 출시, 철강 가격·유가 상승에...현대코퍼, 영업이익률 1% 회복하나, 전기차發 인력재편 '신호탄'... 현대차 직원 12년만에 감소 [전기차..., 현대차 ‘스타리아’, 리무진·캠퍼 모델 출시, 현대차, 스타리아 라운지 리무진·캠퍼 출시, 현대차·기아, 반도체·코로나·전쟁 악재 극복할 카드는, 현대차 노사 "중대재해 예방-안전한 일터 조성" 선언, 철강 가격·유가 상승에...현대코퍼, 영업이익률 1% 회복하나, 현대차도 뛰어든 NFT, 지금 올라타도 될까요?, 현대차 자동차 업계 최초 커뮤니티 기반 NFT 시장 진출</t>
   </si>
   <si>
-    <t>현대차 “2025년까지 주요 도심에 초고속 충전기 5000기 설치”, KB자산운용, 현대차·롯데그룹과 도심형 전기차 초고속 충전소 구축, 이노션, 현대차와 NFT 사업 본격화…메타콩즈 한정판 발행, 전기차 생태계 넓히는 현대차, 롯데·KB와 '맞손', 이노션, NFT 사업 개시… ‘현대차 유니버스’ 운영, 현대차·기아 유럽서 1분기 26만대 팔아…현지시장 점유율 9.8% ‘3..., 현대차그룹, 2025년까지 초고속 충전기 총 5000기 설치 목표, 현대차·롯데·KB자산운용, 전국에 전기차 초고속 충전기 5000기 설치, 전기차 생태계 넓히는 현대차, 롯데·KB와 '맞손', 현대차·기아 1분기 유럽 판매 21% ↑…'톱 3' 올랐다, 현대차·기아, 유럽 1분기 점유율 3위로, 현대차·롯데·KB자산운용, 전국에 전기차 초고속 충전기 5000기 설치, 현대차·기아, 유럽 점유율 첫 3위, 현대차·기아 1분기 유럽 판매 21% ↑…'톱 3' 올랐다, 현대차-롯데지주-KB자산, 도심 전기차 충전기 설치 '맞손', 현대차·롯데·KB운용, 2025년까지 전기차 초고속 충전기 5000기 ..., 현대차·기아, 유럽 점유율 첫 3위, 현대차·롯데·KB자산운용, 전국에 전기차 초고속 충전기 5000기 설치, KB자산운용, 현대차·롯데그룹과 전기차 초고속 충전 인프라 구축 나선..., 현대차그룹, 2025년까지 초고속 충전기 총 5000기 설치 목표, 롯데, 현대차·KB자산운용과 ‘전기차 초고속 충전 인프라’ 구축 나선..., 전기차부터 하이브리드까지…"친환경차는 기아 〉 현대", 현대차 노조 “정규직 충원·순이익 30％ 성과급 달라”, 현대차 노조 ‘정규직 충원’ 요구…전기차 시대, 갈등 본격화? [비즈..., 전기차 생태계 넓히는 현대차, 롯데·KB와 '맞손', 현대차그룹, 전기차 초고속 충전 인프라 SPC 설립 추진…"2025년..., 현대차, 롯데·KB자산운용과 전기차 초고속 충전 인프라 구축 나선다, 현대차 노조 ‘정규직 충원’ 요구…전기차 시대, 갈등 본격화? [비즈3..., 현대차그룹, 전기차 초고속 충전기 5000기 설치한다, 롯데, 현대차·KB자산운용과 ‘전기차 초고속 충전 인프라’ 구축 나선다, 롯데·현대차·KB, 전기차 충전 인프라 특수목적법인 설립, 현대차그룹, 전기차 초고속 충전 인프라 SPC 설립 추진…"2025년까..., 현대차·롯데, 도심에 초고속 전기차 충전기 5000기 설치한다, 이노션, NFT 사업 개시… ‘현대차 유니버스’ 운영, 이노션, 현대·메타콩즈 협업 NFT 발행…사업 본격화, KB운용, 현대차·롯데그룹과 전기차 초고속 충전소 구축, 현대차-롯데지주-KB자산, 도심 전기차 충전기 설치 '맞손', 롯데그룹, 현대차그룹·KB운용과 전기차 초고속충전 인프라 법인 설립한다, 현대차그룹, 전기차 초고속 충전기 5000기 설치한다, 현대차그룹, 전기차 초고속 충전기 5000기 설치, 이노션, NFT 사업 개시… ‘현대차 유니버스’ 운영, KB자산운용, 현대차·롯데그룹과 전기차 초고속 충전 인프라 구축 나선..., 이노션, 현대차와 NFT 사업 본격화…메타콩즈 한정판 발행, 현대차 “2025년까지 주요 도심에 초고속 충전기 5000기 설치”, 이노션, NFT 사업 개시… ‘현대차 유니버스’ 운영, KB자산운용, 현대차·롯데그룹과 도심형 전기차 초고속 충전소 구축, 롯데, 현대차·KB자산운용과 ‘전기차 초고속 충전 인프라’ 구축 나선..., 전기차부터 하이브리드까지…"친환경차는 기아 〉 현대", 롯데그룹, 현대차그룹·KB운용과 전기차 초고속충전 인프라 법인 설립한다, 현대차 노조 ‘정규직 충원’ 요구…전기차 시대, 갈등 본격화? [비즈..., 현대차그룹, 전기차 초고속 충전기 5000기 설치, 현대차그룹, 전기차 초고속 충전 인프라 SPC 설립 추진…"2025년..., "전기차가 이끌었다"…현대차·기아 1분기 유럽 판매량 전년比 21% '..., KB자산운용, 현대차·롯데그룹과 도심형 전기차 초고속 충전소 구축, KB자산운용, 현대차·롯데그룹과 전기차 초고속 충전 인프라 구축 나선..., 이노션, 현대차와 NFT 사업 본격화…메타콩즈 한정판 발행, 현대차 노조 “정규직 충원·순이익 30％ 성과급 달라”, 현대차 “2025년까지 주요 도심에 초고속 충전기 5000기 설치”</t>
-  </si>
-  <si>
-    <t>현대차, 50대 간부 '인생 2막' 돕는다, 현대차, 캠핑 체험프로그램 '휠핑' 참가자 모집, "아이오닉5와 함께 캠핑을"…현대차, '휠핑' 참가자 모집, 현대차, 중고차 사업 시작 못하는 이유, 현대차·기아 중고차 시장 진출, 이달 말 결론나나, 중기부, 현대차·기아 중고차 판매 4월 말까지 결론, 현대차, 중고차 사업 시작 못하는 이유, 현대차, 50대 간부 '인생 2막' 돕는다, 현대차, 캠핑 체험프로그램 '휠핑' 참가자 모집, "아이오닉5와 함께 캠핑을"…현대차, '휠핑' 참가자 모집, 현대차·기아 중고차 시장 진출, 이달 말 결론나나, 중기부, 현대차·기아 중고차 판매 4월 말까지 결론, 현대차, 어린이 통학 차량 '무상점검'…28일까지 신청, 현대차, 어린이 통학차량 '무상 케어 서비스' 실시, 현대차, 캠핑 체험프로그램 '휠핑' 참가자 모집, 현대차證, 1분기 영업익 전년대비 30.8%↓…394억, 현대차, 어린이 통학차량 ‘무상 케어 서비스’, 현대차·GM·혼다가 투자한 美 SES, '차세대 배터리'를 말하다, 현대차, 어린이 통학차량 '무상 케어 서비스' 실시, 현대차, 어린이 통학차량 무상점검, 현대차 정몽구 재단, 공간 플랫폼 ‘온드림 소사이어티’ 활짝, 현대차정몽구재단, 공간 플랫폼 ‘온드림 소사이어티’ 개관, 현대차, 카타르 월드컵 공식 후원…"친환경 월드컵에 기여", 현대차-롯데-KB자산, 전기차 충전 생태계 확장에 손 잡았다, 현대차, 어린이집·유치원 400곳 통학차량 무료 점검, 현대차정몽구재단, 공간 플랫폼 ‘온드림 소사이어티’ 개관, 현대차정몽구재단, 소셜 임팩트 공간 '온드림 소사이어티' 개관, 현대차, 캠핑 체험프로그램 '휠핑' 참가자 모집, 현대차, 캠핑 체험 플랫폼 ‘휠핑’ 시즌3 참가자 모집, 현대차-롯데-KB자산, 전기차 충전 생태계 확장에 손 잡았다, 현대차, 어린이 통학차량 무상점검, 현대차, 아이오닉5 타는 캠핑 지원한다…'휠핑' 시진3 참가자 모집, "친환경 캠핑 즐겨요" 현대차, 휠핑 참가자 접수, 현대차 2022 FIFA 월드컵 공식 후원...공식 차량으로 '아이오닉..., 현대차, 어린이 통학 차량 '무상점검'…28일까지 신청, 현대차, 어린이 통학차량 '무상 케어 서비스' 실시, 현대차·기아 중고차 시장 진출, 이달 말 결론나나, 현대차 중고차 시장 진출, 연내 가능할까…이달말 결론, 현대차, 카타르 월드컵 공식 후원…"친환경 월드컵에 기여", 현대차證, 1분기 영업익 전년대비 30.8%↓…394억, 현대차 카타르 월드컵 공식후원...대회 차량 592대 지원, 현대차 2022 FIFA 월드컵 공식 후원...공식 차량으로 '아이오닉..., 현대차 노조 "정년 후 단기알바 없애고 정년 연장"…요구안 확정, 현대차 카타르 월드컵 공식후원...대회 차량 592대 지원, 현대차, 아이오닉5 타는 캠핑 지원한다…'휠핑' 시진3 참가자 모집, "친환경 캠핑 즐겨요" 현대차, 휠핑 참가자 접수, 현대차, 어린이 통학차량 ‘무상 케어 서비스’, 현대차·GM·혼다가 투자한 美 SES, '차세대 배터리'를 말하다, 현대차 정몽구 재단, 공간 플랫폼 ‘온드림 소사이어티’ 활짝, 현대차정몽구재단, 공간 플랫폼 ‘온드림 소사이어티’ 개관</t>
+    <t>현대차 “2025년까지 주요 도심에 초고속 충전기 5000기 설치”, KB자산운용, 현대차·롯데그룹과 도심형 전기차 초고속 충전소 구축, 이노션, 현대차와 NFT 사업 본격화…메타콩즈 한정판 발행, 전기차 생태계 넓히는 현대차, 롯데·KB와 '맞손', 이노션, NFT 사업 개시… ‘현대차 유니버스’ 운영, 현대차·기아 유럽서 1분기 26만대 팔아…현지시장 점유율 9.8% ‘3..., 현대차그룹, 2025년까지 초고속 충전기 총 5000기 설치 목표, 현대차·롯데·KB자산운용, 전국에 전기차 초고속 충전기 5000기 설치, 전기차 생태계 넓히는 현대차, 롯데·KB와 '맞손', 현대차·기아 1분기 유럽 판매 21% ↑…'톱 3' 올랐다, 현대차·기아, 유럽 1분기 점유율 3위로, 현대차·롯데·KB자산운용, 전국에 전기차 초고속 충전기 5000기 설치, 현대차·기아, 유럽 점유율 첫 3위, 현대차·기아 1분기 유럽 판매 21% ↑…'톱 3' 올랐다, 롯데지주-KB자산, 도심 전기차 충전기 설치 '맞손', 현대차·롯데·KB운용, 2025년까지 전기차 초고속 충전기 5000기 ..., 현대차·기아, 유럽 점유율 첫 3위, 현대차·롯데·KB자산운용, 전국에 전기차 초고속 충전기 5000기 설치, KB자산운용, 현대차·롯데그룹과 전기차 초고속 충전 인프라 구축 나선..., 현대차그룹, 2025년까지 초고속 충전기 총 5000기 설치 목표, 롯데, 현대차·KB자산운용과 ‘전기차 초고속 충전 인프라’ 구축 나선..., 전기차부터 하이브리드까지…"친환경차는 기아 〉 현대", 현대차 노조 “정규직 충원·순이익 30％ 성과급 달라”, 현대차 노조 ‘정규직 충원’ 요구…전기차 시대, 갈등 본격화? [비즈..., 전기차 생태계 넓히는 현대차, 롯데·KB와 '맞손', 현대차그룹, 전기차 초고속 충전 인프라 SPC 설립 추진…"2025년..., 현대차, 롯데·KB자산운용과 전기차 초고속 충전 인프라 구축 나선다, 현대차 노조 ‘정규직 충원’ 요구…전기차 시대, 갈등 본격화? [비즈3..., 현대차그룹, 전기차 초고속 충전기 5000기 설치한다, 롯데, 현대차·KB자산운용과 ‘전기차 초고속 충전 인프라’ 구축 나선다, 롯데·현대차·KB, 전기차 충전 인프라 특수목적법인 설립, 현대차그룹, 전기차 초고속 충전 인프라 SPC 설립 추진…"2025년까..., 현대차·롯데, 도심에 초고속 전기차 충전기 5000기 설치한다, 이노션, NFT 사업 개시… ‘현대차 유니버스’ 운영, 이노션, 현대·메타콩즈 협업 NFT 발행…사업 본격화, KB운용, 현대차·롯데그룹과 전기차 초고속 충전소 구축, 롯데지주-KB자산, 도심 전기차 충전기 설치 '맞손', 롯데그룹, 현대차그룹·KB운용과 전기차 초고속충전 인프라 법인 설립한다, 현대차그룹, 전기차 초고속 충전기 5000기 설치한다, 현대차그룹, 전기차 초고속 충전기 5000기 설치, 이노션, NFT 사업 개시… ‘현대차 유니버스’ 운영, KB자산운용, 현대차·롯데그룹과 전기차 초고속 충전 인프라 구축 나선..., 이노션, 현대차와 NFT 사업 본격화…메타콩즈 한정판 발행, 현대차 “2025년까지 주요 도심에 초고속 충전기 5000기 설치”, 이노션, NFT 사업 개시… ‘현대차 유니버스’ 운영, KB자산운용, 현대차·롯데그룹과 도심형 전기차 초고속 충전소 구축, 롯데, 현대차·KB자산운용과 ‘전기차 초고속 충전 인프라’ 구축 나선..., 전기차부터 하이브리드까지…"친환경차는 기아 〉 현대", 롯데그룹, 현대차그룹·KB운용과 전기차 초고속충전 인프라 법인 설립한다, 현대차 노조 ‘정규직 충원’ 요구…전기차 시대, 갈등 본격화? [비즈..., 현대차그룹, 전기차 초고속 충전기 5000기 설치, 현대차그룹, 전기차 초고속 충전 인프라 SPC 설립 추진…"2025년..., "전기차가 이끌었다"…현대차·기아 1분기 유럽 판매량 전년比 21% '..., KB자산운용, 현대차·롯데그룹과 도심형 전기차 초고속 충전소 구축, KB자산운용, 현대차·롯데그룹과 전기차 초고속 충전 인프라 구축 나선..., 이노션, 현대차와 NFT 사업 본격화…메타콩즈 한정판 발행, 현대차 노조 “정규직 충원·순이익 30％ 성과급 달라”, 현대차 “2025년까지 주요 도심에 초고속 충전기 5000기 설치”</t>
+  </si>
+  <si>
+    <t>현대차, 50대 간부 '인생 2막' 돕는다, 현대차, 캠핑 체험프로그램 '휠핑' 참가자 모집, "아이오닉5와 함께 캠핑을"…현대차, '휠핑' 참가자 모집, 현대차, 중고차 사업 시작 못하는 이유, 현대차·기아 중고차 시장 진출, 이달 말 결론나나, 중기부, 현대차·기아 중고차 판매 4월 말까지 결론, 현대차, 중고차 사업 시작 못하는 이유, 현대차, 50대 간부 '인생 2막' 돕는다, 현대차, 캠핑 체험프로그램 '휠핑' 참가자 모집, "아이오닉5와 함께 캠핑을"…현대차, '휠핑' 참가자 모집, 현대차·기아 중고차 시장 진출, 이달 말 결론나나, 중기부, 현대차·기아 중고차 판매 4월 말까지 결론, 현대차, 어린이 통학 차량 '무상점검'…28일까지 신청, 현대차, 어린이 통학차량 '무상 케어 서비스' 실시, 현대차, 캠핑 체험프로그램 '휠핑' 참가자 모집, 현대차證, 1분기 영업익 전년대비 30.8%↓…394억, 현대차, 어린이 통학차량 ‘무상 케어 서비스’, 현대차·GM·혼다가 투자한 美 SES, '차세대 배터리'를 말하다, 현대차, 어린이 통학차량 '무상 케어 서비스' 실시, 현대차, 어린이 통학차량 무상점검, 현대차 정몽구 재단, 공간 플랫폼 ‘온드림 소사이어티’ 활짝, 현대차정몽구재단, 공간 플랫폼 ‘온드림 소사이어티’ 개관, 현대차, 카타르 월드컵 공식 후원…"친환경 월드컵에 기여", 롯데-KB자산, 전기차 충전 생태계 확장에 손 잡았다, 현대차, 어린이집·유치원 400곳 통학차량 무료 점검, 현대차정몽구재단, 공간 플랫폼 ‘온드림 소사이어티’ 개관, 현대차정몽구재단, 소셜 임팩트 공간 '온드림 소사이어티' 개관, 현대차, 캠핑 체험프로그램 '휠핑' 참가자 모집, 현대차, 캠핑 체험 플랫폼 ‘휠핑’ 시즌3 참가자 모집, 롯데-KB자산, 전기차 충전 생태계 확장에 손 잡았다, 현대차, 어린이 통학차량 무상점검, 현대차, 아이오닉5 타는 캠핑 지원한다…'휠핑' 시진3 참가자 모집, "친환경 캠핑 즐겨요" 현대차, 휠핑 참가자 접수, 현대차 2022 FIFA 월드컵 공식 후원...공식 차량으로 '아이오닉..., 현대차, 어린이 통학 차량 '무상점검'…28일까지 신청, 현대차, 어린이 통학차량 '무상 케어 서비스' 실시, 현대차·기아 중고차 시장 진출, 이달 말 결론나나, 현대차 중고차 시장 진출, 연내 가능할까…이달말 결론, 현대차, 카타르 월드컵 공식 후원…"친환경 월드컵에 기여", 현대차證, 1분기 영업익 전년대비 30.8%↓…394억, 현대차 카타르 월드컵 공식후원...대회 차량 592대 지원, 현대차 2022 FIFA 월드컵 공식 후원...공식 차량으로 '아이오닉..., 현대차 노조 "정년 후 단기알바 없애고 정년 연장"…요구안 확정, 현대차 카타르 월드컵 공식후원...대회 차량 592대 지원, 현대차, 아이오닉5 타는 캠핑 지원한다…'휠핑' 시진3 참가자 모집, "친환경 캠핑 즐겨요" 현대차, 휠핑 참가자 접수, 현대차, 어린이 통학차량 ‘무상 케어 서비스’, 현대차·GM·혼다가 투자한 美 SES, '차세대 배터리'를 말하다, 현대차 정몽구 재단, 공간 플랫폼 ‘온드림 소사이어티’ 활짝, 현대차정몽구재단, 공간 플랫폼 ‘온드림 소사이어티’ 개관</t>
   </si>
   <si>
     <t>현대차, 코나 신형 출시…가격은 2144만원부터, "묻고 더블로"…현대차 노조, 역대급 임금 인상 요구 [김일규의 네 바..., 현대차 정몽구 재단, 소셜 임팩트 공간 플랫폼 ‘온드림 소사이어티’ 개..., 현대차, 코나 신형 출시…가격은 2144만원부터, "묻고 더블로"…현대차 노조, 역대급 임금 인상 요구 [김일규의 네 바..., 현대차, 베니스 비엔날레 한국관 후원, 현대차그룹, 독일 디자인상 17관왕 '쾌거', 현대성우그룹 기업 브로슈어 세계3대 디자인 어워드 ‘iF 디자인 어워..., 현대성우그룹, 기업 브로슈어 '2022 iF 디자인 어워드' 수상, 현대차·기아·제네시스 ‘iF 디자인 어워드’ 17개 본상 쾌거, 현대차그룹, 독일 'iF 디자인 어워드'서 본상 17개 휩쓸어, 현대차그룹, ‘2022 iF 디자인 어워드’ 본상 17개 수상, 현대차·기아·제네시스, ‘iF 디자인 어워드’ 휩쓸었다…"본상 17개", 현대차 ‘제59회 베니스 비엔날레’ 한국관 후원한다, 덕양산업, 현대차 美SES 차세대 배터리 공장 시제품 생산...., 현대성우그룹, 기업 브로슈어 '2022 iF 디자인 어워드' 수상, 현대차·기아·제네시스, ‘iF 디자인 어워드’ 휩쓸었다…"본상 17개", 덕양산업, 현대차 美SES 차세대 배터리 공장 시제품 생산...., "중기부에 달렸다"…현대차·기아 중고차 판매여부 다음주 결론, 현대차, '베네치아 비엔날레' 한국관 공식 후원, 현대차 정몽구 재단, 소셜 임팩트 공간 플랫폼 ‘온드림 소사이어티’ 개..., 현대성우그룹 기업 브로슈어 세계3대 디자인 어워드 ‘iF 디자인 어워..., 현대차, 베니스 비엔날레 한국관 공식 후원, 현대차그룹, ‘2022 iF 디자인 어워드’ 본상 17개 수상, 현대차, 베니스 비엔날레 한국관 공식 후원, 전기차 전환시 일손 줄어드는데…현대차 노조 "정규직 뽑아라", 현대차, ‘제59회 베니스 비엔날레’ 한국관 공식 후원, 현대차그룹, '2022 iF 디자인 어워드' 휩쓸어...본상 17개 수..., 현대차그룹, ‘2022 iF 디자인 어워드’ 본상 17개 수상, 전기차 전환시 일손 줄어드는데…현대차 노조 "정규직 뽑아라", 현대차·기아·제네시스 ‘iF 디자인 어워드’ 17개 본상 쾌거, 현대차, ‘베니스 비엔날레’ 한국관 공식 후원한다, 현대차 ‘제59회 베니스 비엔날레’ 한국관 후원</t>
@@ -7888,13 +7888,13 @@
     <t>현대차·LG이노텍…이젠 '1분기 실적의 시간', 현대차·LG이노텍…이젠 '1분기 실적의 시간'</t>
   </si>
   <si>
-    <t>현대차·칼라일, 글로비스 가치 띄우기 나섰다, 공급망 직접 챙기는 현대차, 배터리 원자재 ‘직구’ 검토[현대차·기아 ..., 현대차, 고급차로 반도체 악재 뛰어넘었다, 반도체난 뚫고 '역대급 실적'…현대차·기아 "올해판매 자신", ‘친환경’ 주도하는 현대차그룹…주요 계열사 4곳 RE100 가입 승인, '주춤하던' 현대차, 깜짝 실적 발표에 반등…1% 넘게 올라, 현대차 1분기 영업익 1.9조…판매 감소에도 매출·영업이익 모두 늘었..., "비싼차 많이 팔렸다"...현대차, 1분기 영업익 16.4%↑, 현대차그룹 4개사, RE100 가입 승인, 현대차그룹 4개사, RE100 가입, 현대차 "원자재 전담조직 신설…러시아 외 생산확대 추진", 현대차, 車 반도체·러시아 악재에도 ‘어닝 서프라이즈’…1분기 영업이..., 공급망 직접 챙기는 현대차, 배터리 원자재 ‘직구’ 검토[현대차·기아 ..., 현대차그룹 4개사, RE100 가입 승인, 현대차그룹 4개사, RE100 가입, 현대차 "원자재 전담조직 신설…러시아 외 생산확대 추진", 현대차, 車 반도체·러시아 악재에도 ‘어닝 서프라이즈’…1분기 영업이..., 3중 악재 넘었다... 현대차 깜짝실적, 현대차, 악재 뚫고 역대급 실적…'제네시스·환율 덕봤다', 현대차-우려보다 견조했던 실적, 긍정적 환율 효과 등으로 최근 낮아진 컨센서스 상회, 지속적인 자동차 공급 차질에 따른 초과 수요 국면 지속, 박스권 주가 흐름 예상, 목표가 및 매수 의견 유지, 현대차-우려보다 견조했던 실적, 긍정적 환율 효과 등으로 최근 낮아진 컨센서스 상회, 지속적인 자동차 공급 차질에 따른 초과 수요 국면 지속, 박스권 주가 흐름 예상, 목표가 및 매수 의견 유지, "원자재 가격 상승 반영 3개월~1년…영향 최소화"-현대차 컨콜, 현대차-년도년도 2분기 1분기 리뷰 - 반도체 부족은 호재였다, 기상의년도 대분기 년도년도 2분기 1분기 영업이익 발표. 반도체 부족의 긍정적 효과가 부정적 효과보다 더 크다는 것 확인, 년도년도 2분기 1분기 영업이익 1.9조원 (시장 컨센서스 17% 상회). 비용 증가보다 ASP 상승이 빨랐음, 년도년도 2분기 2분기 이후에도 비용-ASP 통제 능력이 유지될지 관찰 필요. 매크로 환경에 주목할 필요, 3중 악재 넘었다... 현대차 깜짝실적, "3월 말 기준 국내 미출고 물량 52.2만대…대기 수요 이어져"-현대..., "SUV 끌고 RV 밀고" …현대차·기아, 1분기 어닝서프라이즈(종합), 현대차 “러시아 수요 30% 하락…반도체 공급난·원자재가 상승 악재”, 현대차가 나섰더니 달동네가 관광 명소로…”尹정부도 기업과 이런 협업 해..., 현대차그룹 4개사, RE100 가입 승인 완료, 현대차그룹 4개사, ‘RE100’ 가입 승인…“탄소중립 가속도”, 현대차·기아·모비스·위아 'RE100' 가입..."탄소중립 앞장", 현대차·기아·모비스·위아, RE100 가입, 지니뮤직 현대 기아차 적용 차량 확대한다, 현대차 "원자재 전담조직 신설…러시아 외 생산확대 추진", 현대차그룹 4개사, ‘RE100’ 이니셔티브 가입 승인, 외국인 때문에? 형님 누른 동생들…삼성전자보다 SDI, 현대차보다 기아..., 현대차그룹 4개사, ‘RE100’ 가입 승인…“탄소중립 가속도”, 제네시스·현대차·기아 32개 차종 인포테인먼트 시스템에 멜론 탑재, 외국인 때문에? 형님 누른 동생들…삼성전자보다 SDI, 현대차보다 기아..., 멜론, 제네시스-현대차-기아 차량에 인포테인먼트 접목, “스마트폰 연결 없이 음악을” 지니뮤직, 현대·기아차 32종에 서비스..., 현대차 1분기 매출 20조2986억-영업익 1조9289억, 현대차·기아 중고차 판매 28일 결판난다, 현대차그룹 4개사, ‘RE100’ 이니셔티브 가입 승인, 현대차그룹 4개사, ‘RE100’ 가입 승인…“탄소중립 가속도”, 제네시스·현대차·기아 32개 차종 인포테인먼트 시스템에 멜론 탑재, 멜론, 제네시스-현대차-기아 차량에 인포테인먼트 접목, 지니뮤직, 현대차·기아에 서비스 적용 차종 확대, “스마트폰 연결 없이 음악을” 지니뮤직, 현대·기아차 32종에 서비스..., ‘친환경’ 주도하는 현대차그룹…주요 계열사 4곳 RE100 가입 승인, 현대차?기아?현대모비스?현대위아 ‘RE100’ 가입…친환경 속도, 지니뮤직, 현대차·기아에 서비스 적용 차종 확대, 현대차그룹 4개사, RE100 가입 승인, 현대차가 나섰더니 달동네가 관광 명소로…”尹정부도 기업과 이런 협업 해..., 현대차·기아 중고차 판매 여부 '28일 결론', "전기차 5만2천대 판매…이중 아이오닉 5가 3만대 "-현대차 컨콜, 현대차 1분기 영업익 1.9조…판매 감소에도 매출·영업이익 모두 늘었다, "반도체 수급난에도"…현대차, 1분기 실적 선방(상보), 현대차·기아 중고차 판매 여부 '28일 결론', 현대차·기아 중고차 판매 28일 결판난다, "1Q 러시아 판매 25% 감소…러 시장 수익성 방어할 것"-현대차 컨..., 현대차·기아 중고차 판매 28일 결판난다, 현대차 1분기 영업익 1조9289억...판매 줄었지만 이익은 늘어, 현대차, 1Q 영업익 1.9조원…전년비 16.4%↑, "반도체 수급난에도"…현대차, 1분기 실적 선방(상보), 현대차, 1분기 영업익 1조9289억…전년비 16.4% ↑, 현대차, 1분기 매출 30조2986억원…전년比 10.6%↑, 현대차, 1분기 영업익 1조9289억원‥전년比 16.4%↑, 현대자동차, 1분기 영업익 1.9조...전년比 16.4%↑, 현대차 1분기 매출 20조2986억-영업익 1조9289억, "3월 말 기준 국내 미출고 물량 52.2만대…대기 수요 이어져"-현대..., "원자재 가격 상승 반영 3개월~1년…영향 최소화"-현대차 컨콜, '주춤하던' 현대차, 깜짝 실적 발표에 반등…1% 넘게 올라, 현대차, 반도체 공급난에도 영업익 1.9조원…고부가가치 제품 판매 증..., 현대차, 전망치 상회하는 1분기 실적에 주가 '상승세'로 반전</t>
-  </si>
-  <si>
-    <t>현대차-불확실한 시장의 확실한 대안, 년도년도 2분기 1분기 , 대외 불확실성 확장 우려를 불식시킨 호실적 기록, 년도년도 2분기 1분기 실적 개선 요인, 년도년도 2분기 2분기 에 더욱 강화, 1분기 어닝 서프라이즈... 현대차·기아 동반 상승, 현대차 UAM 법인 '슈퍼널', 英에 첫 수직이착륙장 건립, '현대차 UAM 법인' 슈퍼널, 英에 첫 수직이착륙장 세웠다, 현대차-다시 가시권에 들어온 영업이익 8조원, 연결 매출 30조원(전년 대비 증감율+11%), 영업이익 1.9조원(+16%), OPM 6.4%, 차량사업 매출 24조원(전년 대비 증감율+11%), 영업이익 1.3조원(+13%), OPM 5.6%, 금융 매출 4.4조원(전년 대비 증감율+2%), 영업이익 540십억원(+4%), OPM 12.6%, 다시 가시권에 들어온 연간 영업이익 8조원, 현대차·기아, 어닝 서프라이즈에 동반 상승..기관 매수세 몰려, 현대차-가슴이 웅장해지는 실적, 22년도 1분기 영업이익 1.9조원(+16.4%)으로 시장 기대치 +17% 상회, 우려(생산 차질, 원가, 보틀넥)를 이기는 수요, 목표주가 260,000원, 투자의견 매수 유지, 현대차-영업이익 +17% 서프. 관건은 지속성, 투자의견 매수, 목표주가 210,000원 유지, 22년도 1분기 매출 30.3조원(전년 대비 증감율 +11%), OP 1.9조원(+16%), OPM 6.4% 시현, 2022년 매출 128.7조원(+9.4%), OP 7.7조원(+15.4%), OPM 5.1% 전망, 현대차-년도년도 2분기 1분기 Review: 돌아왔다, 년도년도 2분기 1분기 현대차 실적 Review 및 투자의견 재점검, 현대차-아이고, 깜짝이야. 기분 좋은 서프라이즈, 1분기 실적 서프라이즈 기록, 현대차 22년도 1분기 Review: 영업이익률 6.4% 기록, 컨퍼런스 콜의 주요 내용: 영업이익률 가이던스 5.5%~6.5% 유지, 현대차-모든 우려를 불식시킨 실적, 1분기 영업이익 1.93조원, 당사 추정 및 시장 기대치 상회, 모든 우려를 불식시킨 실적, 현대차-자동차 부문이 견인한 호실적, 22년도 1분기 Review: 예상보다 컸던 우호적 환율 효과, 22년도 2분기 Preview: 원재료비 상승의 본격 반영, 그래도 수익성 개선세는 지속, 투자의견 Buy, 목표주가 280,000원 유지, 현대차-Back to Earnings, 22년도 1분기 , Surpise, 비용도 내려갈 전망, 본질로 돌아가자, 현대차-22년도 1분기 Review: 슈퍼 파워를 갖추어 가는 현대차, 1분기 실적 서프라이즈, 2년간 극심한 공급망 대란의 결과, 부가가치 확장의 시기, 현대차-년도년도 2분기 1분기 Review: 부진한 Q를 넘어선 P효과, 년도년도 2분기 1분기 (P): 매출액 30조 2,990억원, 영업이익 1조 9,290억원, 2022년 판매대수 전망 하향, 환율과 Mix 개선이 이익 방어, 하반기부터 제조원가 부담은 커질 전망, 현대차-낮아진 기대도 리콜이 되나요, 투자포인트 및 결론, 주요이슈 및 실적전망, 주가전망 및 Valuation, 현대차- 제품 Mix 개선의 힘, 년도년도 2분기 1분기 Review: 시장 기대치 상회, 투자의견 ‘Buy’, 목표주가 230,000원 유지, 현대차-하반기 공급 안정성 회복 기대, 2022년 자동차부문 매출액 100조원 상회 전망, 1분기 Review: 가격변수 개선 &gt; 물량감소 우려, 현대차-다시 가시권에 들어온 영업이익 8조원, 연결 매출 30조원(전년 대비 증감율+11%), 영업이익 1.9조원(+16%), OPM 6.4%, 차량사업 매출 24조원(전년 대비 증감율+11%), 영업이익 1.3조원(+13%), OPM 5.6%, 금융 매출 4.4조원(전년 대비 증감율+2%), 영업이익 540십억원(+4%), OPM 12.6%, 다시 가시권에 들어온 연간 영업이익 8조원, ‘깜짝 실적’ 현대차, 영업익 8조 시대 9년만에 다시 여나, 현대차-다시 가시권에 들어온 영업이익 8조원, 연결 매출 30조원(전년 대비 증감율+11%), 영업이익 1.9조원(+16%), OPM 6.4%, 차량사업 매출 24조원(전년 대비 증감율+11%), 영업이익 1.3조원(+13%), OPM 5.6%, 금융 매출 4.4조원(전년 대비 증감율+2%), 영업이익 540십억원(+4%), OPM 12.6%, 다시 가시권에 들어온 연간 영업이익 8조원, 1분기 어닝서프라이즈 낸 현대차·기아, 드디어 날았다, 현대차·기아, 1분기 호실적에 나란히 '강세'...3%대 상승, 현대차, 연간 영업이익 '8조원' 회복한다…목표가 25만원 -신영證, 하나금투 “현대차, 1분기 ‘깜짝’ 호실적…2분기 이후에도 견조한 실적..., 현대차, 1분기 깜짝 실적…향후 견조한 실적 전망-하나금투, '깜짝 실적' 현대차, "주가 너무 싸다"…목표가 26만원 -신한, "현대차, 우려 이기는 수요…2분기 실적도 양호 예상"-신한, 현대차, 반도체 공급 정상화 지연에도 가격 변수에 양호한 수익성-NH, 현대차, 하반기 공급안정성 회복…중장기 실적개선 유효 -NH, 현대차, 1Q 실적 개선에…성수기 2Q 기대 커진다-신한, '깜짝 실적' 현대차, "주가 너무 싸다"…목표가 26만원 -신한, "현대차, 우려 이기는 수요…2분기 실적도 양호 예상"-신한, 현대차, 반도체 공급 정상화 지연에도 가격 변수에 양호한 수익성-NH, 현대차, 하반기 공급안정성 회복…중장기 실적개선 유효 -NH, 현대차, 1Q 실적 개선에…성수기 2Q 기대 커진다-신한, 현대차, 인플레이션 방어력+공급망 관리력 입증-삼성證, 현대차, 1분기 판매 대수 감소에도 'SUV·제네시스'덕에 매출액 증가..., 현대차, 우려보다 견조한 실적 이어질 것-하나금융투자, "현대차, 1Q '깜짝' 실적…우려보다 견조한 실적 ..., 1분기 어닝서프라이즈 낸 현대차·기아, 드디어 날았다, 1분기 호실적·중장기 성장 전망에 현대차·기아 강세, '어닝서프라이즈'에 현대차·기아 강세, 현대차·기아, 1분기 ‘깜짝’ 호실적에 동반 상승, 코스피·코스닥 상승 출발, 1분기 호실적에 현대차·기아 강세 [개장시황..., 현대차·기아 깜짝실적…주가도 속도낼까, 현대차 이어 삼성도 RE100 만지작…"원전 아닌 재생에너지 필요", 현대차그룹 UAM社…英에 세계 첫 이착륙장, "실적 좋으면 뭐하나요"…성토 쏟아낸 삼전·현대차 개미들, 제네시스 생산 라인 헛돌린다…현대차에도 닥친 중국發 '공포', 폭스바겐·BMW 등 판매량 급감했는데…유럽서 '나홀로 성장' 현대차, 악재 딛고 '깜짝 실적'…현대차 주가 상승, 이것에 달렸다, 현대차·기아, 1분기 ‘깜짝 실적’에도 주가 전망은 ‘박스권’ 왜?, 폭스바겐·BMW 등 판매량 급감했는데…유럽서 '나홀로 성장' 현대차, 현대차-년도년도 2분기 1분기 Review: 올해 영업이익 전망치 9조원으로 상향 조정, 년도년도 2분기 1분기 Review: 실적 서프라이즈, 사업 부문별 실적 요약, 2022년 연간 영업이익 추정치 9조원으로 상향 조정, 악재 딛고 '깜짝 실적'…현대차 주가 상승, 이것에 달렸다, 현대차·기아, 호실적에 주가도 화답…5%대 ↑, 현대차·기아, 어닝 서프라이즈에 동반 상승..기관 매수세 몰려, 쏠라이트 인디고 레이싱, 2022 시즌 출정식 진행…현대성우그룹 임직원..., "원자재 관리 강화"…현대차·기아, 최대실적에도 고삐 더 죄는 배경은, 다올투자증권 “현대차, 돌아왔다”, 오토앤, 현대차·기아 중고차 진출 조정안 논의 소식에 오름세, 오토앤, 현대 기아차 '중고차사업' 본격 진출 소식에 강세, 코스피·코스닥 상승 출발, 1분기 호실적에 현대차·기아 강세 [개장시황..., 오토앤, 현대 기아차 '중고차사업' 본격 진출 소식에 강세, (영상)현대차·기아 1분기 '깜짝실적'...고수익차 판매증가 등, 실적 질주한 현대차 기아…주가 '깜짝 반등', '호실적' 현대차·기아 내달렸다, '호실적' 현대차·기아 내달렸다, ‘깜짝 실적’ 현대차, 영업익 8조 시대 9년만에 다시 여나, 현대차·기아, 어닝 서프라이즈에 동반 상승..기관 매수세 몰려, 1분기 어닝 서프라이즈... 현대차·기아 동반 상승</t>
-  </si>
-  <si>
-    <t>현대차 제치고 SK…'업비트 운영' 두나무, 대기업 반열에[2022 대..., “2024년 유럽 출시 목표”…현대차, 경형 전기 SUV 개발 중, SK, 현대車 제치고 자산 2위…두나무, 대기업 지정, "저탄소·디지털 전환" 현대차 등 14곳, 올해 재직자 5000명 직무..., 반도체 호황 후광효과…SK, 현대차 제치고 재계 서열 2위 등극, SK, 현대차 제치고 ‘재계 2위’…올해도 쿠팡 총수는 ‘쿠팡’, “2024년 유럽 출시 목표”…현대차, 경형 전기 SUV 개발 중, 현대차 등 14곳 5372명 직무전환 훈련, "저탄소·디지털 전환" 현대차 등 14곳, 올해 재직자 5000명 직..., 반도체 호황 후광효과…SK, 현대차 제치고 재계 서열 2위 등극, 역시 반도체의 힘…현대차 제치고 재계 2위 된 SK, SK, 현대차 제치고 사상 첫 재계 2위…업비트도 '대기업', 전기차로 뜨는 현대차·기아 “이번엔 인도”, 현대차-생산차질을 이겨낸 믹스, 1분기 컨센서스 상회, SUV와 제네시스 중심의 믹스 개선, 전기차 전환 모멘텀 지속 전망, 투자의견 매수, 목표주가 300,000원, 현대두산인프라, 中 위축에도 선방..1Q 영업익 1049억원, 현대차 UAM 법인 ‘슈퍼널’, 영국에 첫 수직이착륙장 세웠다, 친환경 캠핑 브랜드 '디어디어'…더현대서울에 '팝업스토어' 오픈, 범 삼성·현대家 혼맥… 한솔 장남·현대종합금속 장녀 결혼</t>
+    <t>현대차·칼라일, 글로비스 가치 띄우기 나섰다, 공급망 직접 챙기는 현대차, 배터리 원자재 ‘직구’ 검토[현대차·기아 ..., 현대차, 고급차로 반도체 악재 뛰어넘었다, 반도체난 뚫고 '역대급 실적'…현대차·기아 "올해판매 자신", ‘친환경’ 주도하는 현대차그룹…주요 계열사 4곳 RE100 가입 승인, '주춤하던' 현대차, 깜짝 실적 발표에 반등…1% 넘게 올라, 현대차 1분기 영업익 1.9조…판매 감소에도 매출·영업이익 모두 늘었..., "비싼차 많이 팔렸다"...현대차, 1분기 영업익 16.4%↑, 현대차그룹 4개사, RE100 가입 승인, 현대차그룹 4개사, RE100 가입, 현대차 "원자재 전담조직 신설…러시아 외 생산확대 추진", 현대차, 車 반도체·러시아 악재에도 ‘어닝 서프라이즈’…1분기 영업이..., 공급망 직접 챙기는 현대차, 배터리 원자재 ‘직구’ 검토[현대차·기아 ..., 현대차그룹 4개사, RE100 가입 승인, 현대차그룹 4개사, RE100 가입, 현대차 "원자재 전담조직 신설…러시아 외 생산확대 추진", 현대차, 車 반도체·러시아 악재에도 ‘어닝 서프라이즈’…1분기 영업이..., 3중 악재 넘었다... 현대차 깜짝실적, 현대차, 악재 뚫고 역대급 실적…'제네시스·환율 덕봤다', 우려보다 견조했던 실적, 긍정적 환율 효과 등으로 최근 낮아진 컨센서스 상회, 지속적인 자동차 공급 차질에 따른 초과 수요 국면 지속, 박스권 주가 흐름 예상, 목표가 및 매수 의견 유지, 우려보다 견조했던 실적, 긍정적 환율 효과 등으로 최근 낮아진 컨센서스 상회, 지속적인 자동차 공급 차질에 따른 초과 수요 국면 지속, 박스권 주가 흐름 예상, 목표가 및 매수 의견 유지, "원자재 가격 상승 반영 3개월~1년…영향 최소화"-현대차 컨콜, 년도년도 2분기 1분기 리뷰 - 반도체 부족은 호재였다, 기상의년도 대분기 년도년도 2분기 1분기 영업이익 발표. 반도체 부족의 긍정적 효과가 부정적 효과보다 더 크다는 것 확인, 년도년도 2분기 1분기 영업이익 1.9조원 (시장 컨센서스 17% 상회). 비용 증가보다 ASP 상승이 빨랐음, 년도년도 2분기 2분기 이후에도 비용-ASP 통제 능력이 유지될지 관찰 필요. 매크로 환경에 주목할 필요, 3중 악재 넘었다... 현대차 깜짝실적, "3월 말 기준 국내 미출고 물량 52.2만대…대기 수요 이어져"-현대..., "SUV 끌고 RV 밀고" …현대차·기아, 1분기 어닝서프라이즈(종합), 현대차 “러시아 수요 30% 하락…반도체 공급난·원자재가 상승 악재”, 현대차가 나섰더니 달동네가 관광 명소로…”尹정부도 기업과 이런 협업 해..., 현대차그룹 4개사, RE100 가입 승인 완료, 현대차그룹 4개사, ‘RE100’ 가입 승인…“탄소중립 가속도”, 현대차·기아·모비스·위아 'RE100' 가입..."탄소중립 앞장", 현대차·기아·모비스·위아, RE100 가입, 지니뮤직 현대 기아차 적용 차량 확대한다, 현대차 "원자재 전담조직 신설…러시아 외 생산확대 추진", 현대차그룹 4개사, ‘RE100’ 이니셔티브 가입 승인, 외국인 때문에? 형님 누른 동생들…삼성전자보다 SDI, 현대차보다 기아..., 현대차그룹 4개사, ‘RE100’ 가입 승인…“탄소중립 가속도”, 제네시스·현대차·기아 32개 차종 인포테인먼트 시스템에 멜론 탑재, 외국인 때문에? 형님 누른 동생들…삼성전자보다 SDI, 현대차보다 기아..., 멜론, 제네시스-현대차-기아 차량에 인포테인먼트 접목, “스마트폰 연결 없이 음악을” 지니뮤직, 현대·기아차 32종에 서비스..., 현대차 1분기 매출 20조2986억-영업익 1조9289억, 현대차·기아 중고차 판매 28일 결판난다, 현대차그룹 4개사, ‘RE100’ 이니셔티브 가입 승인, 현대차그룹 4개사, ‘RE100’ 가입 승인…“탄소중립 가속도”, 제네시스·현대차·기아 32개 차종 인포테인먼트 시스템에 멜론 탑재, 멜론, 제네시스-현대차-기아 차량에 인포테인먼트 접목, 지니뮤직, 현대차·기아에 서비스 적용 차종 확대, “스마트폰 연결 없이 음악을” 지니뮤직, 현대·기아차 32종에 서비스..., ‘친환경’ 주도하는 현대차그룹…주요 계열사 4곳 RE100 가입 승인, 현대차?기아?현대모비스?현대위아 ‘RE100’ 가입…친환경 속도, 지니뮤직, 현대차·기아에 서비스 적용 차종 확대, 현대차그룹 4개사, RE100 가입 승인, 현대차가 나섰더니 달동네가 관광 명소로…”尹정부도 기업과 이런 협업 해..., 현대차·기아 중고차 판매 여부 '28일 결론', "전기차 5만2천대 판매…이중 아이오닉 5가 3만대 "-현대차 컨콜, 현대차 1분기 영업익 1.9조…판매 감소에도 매출·영업이익 모두 늘었다, "반도체 수급난에도"…현대차, 1분기 실적 선방(상보), 현대차·기아 중고차 판매 여부 '28일 결론', 현대차·기아 중고차 판매 28일 결판난다, "1Q 러시아 판매 25% 감소…러 시장 수익성 방어할 것"-현대차 컨..., 현대차·기아 중고차 판매 28일 결판난다, 현대차 1분기 영업익 1조9289억...판매 줄었지만 이익은 늘어, 현대차, 1Q 영업익 1.9조원…전년비 16.4%↑, "반도체 수급난에도"…현대차, 1분기 실적 선방(상보), 현대차, 1분기 영업익 1조9289억…전년비 16.4% ↑, 현대차, 1분기 매출 30조2986억원…전년比 10.6%↑, 현대차, 1분기 영업익 1조9289억원‥전년比 16.4%↑, 현대자동차, 1분기 영업익 1.9조...전년比 16.4%↑, 현대차 1분기 매출 20조2986억-영업익 1조9289억, "3월 말 기준 국내 미출고 물량 52.2만대…대기 수요 이어져"-현대..., "원자재 가격 상승 반영 3개월~1년…영향 최소화"-현대차 컨콜, '주춤하던' 현대차, 깜짝 실적 발표에 반등…1% 넘게 올라, 현대차, 반도체 공급난에도 영업익 1.9조원…고부가가치 제품 판매 증..., 현대차, 전망치 상회하는 1분기 실적에 주가 '상승세'로 반전</t>
+  </si>
+  <si>
+    <t>불확실한 시장의 확실한 대안, 년도년도 2분기 1분기 , 대외 불확실성 확장 우려를 불식시킨 호실적 기록, 년도년도 2분기 1분기 실적 개선 요인, 년도년도 2분기 2분기 에 더욱 강화, 1분기 어닝 서프라이즈... 현대차·기아 동반 상승, 현대차 UAM 법인 '슈퍼널', 英에 첫 수직이착륙장 건립, '현대차 UAM 법인' 슈퍼널, 英에 첫 수직이착륙장 세웠다, 다시 가시권에 들어온 영업이익 8조원, 연결 매출 30조원(전년 대비 증감율+11%), 영업이익 1.9조원(+16%), OPM 6.4%, 차량사업 매출 24조원(전년 대비 증감율+11%), 영업이익 1.3조원(+13%), OPM 5.6%, 금융 매출 4.4조원(전년 대비 증감율+2%), 영업이익 540십억원(+4%), OPM 12.6%, 다시 가시권에 들어온 연간 영업이익 8조원, 현대차·기아, 어닝 서프라이즈에 동반 상승..기관 매수세 몰려, 가슴이 웅장해지는 실적, 22년도 1분기 영업이익 1.9조원(+16.4%)으로 시장 기대치 +17% 상회, 우려(생산 차질, 원가, 보틀넥)를 이기는 수요, 목표주가 260,000원, 투자의견 매수 유지, 영업이익 +17% 서프. 관건은 지속성, 투자의견 매수, 목표주가 210,000원 유지, 22년도 1분기 매출 30.3조원(전년 대비 증감율 +11%), OP 1.9조원(+16%), OPM 6.4% 시현, 2022년 매출 128.7조원(+9.4%), OP 7.7조원(+15.4%), OPM 5.1% 전망, 년도년도 2분기 1분기 Review: 돌아왔다, 년도년도 2분기 1분기 현대차 실적 Review 및 투자의견 재점검, 아이고, 깜짝이야. 기분 좋은 서프라이즈, 1분기 실적 서프라이즈 기록, 현대차 22년도 1분기 Review: 영업이익률 6.4% 기록, 컨퍼런스 콜의 주요 내용: 영업이익률 가이던스 5.5%~6.5% 유지, 모든 우려를 불식시킨 실적, 1분기 영업이익 1.93조원, 당사 추정 및 시장 기대치 상회, 모든 우려를 불식시킨 실적, 자동차 부문이 견인한 호실적, 22년도 1분기 Review: 예상보다 컸던 우호적 환율 효과, 22년도 2분기 Preview: 원재료비 상승의 본격 반영, 그래도 수익성 개선세는 지속, 투자의견 Buy, 목표주가 280,000원 유지, Back to Earnings, 22년도 1분기 , Surpise, 비용도 내려갈 전망, 본질로 돌아가자, 22년도 1분기 Review: 슈퍼 파워를 갖추어 가는 현대차, 1분기 실적 서프라이즈, 2년간 극심한 공급망 대란의 결과, 부가가치 확장의 시기, 년도년도 2분기 1분기 Review: 부진한 Q를 넘어선 P효과, 년도년도 2분기 1분기 (P): 매출액 30조 2,990억원, 영업이익 1조 9,290억원, 2022년 판매대수 전망 하향, 환율과 Mix 개선이 이익 방어, 하반기부터 제조원가 부담은 커질 전망, 낮아진 기대도 리콜이 되나요, 투자포인트 및 결론, 주요이슈 및 실적전망, 주가전망 및 Valuation, 제품 Mix 개선의 힘, 년도년도 2분기 1분기 Review: 시장 기대치 상회, 투자의견 ‘Buy’, 목표주가 230,000원 유지, 하반기 공급 안정성 회복 기대, 2022년 자동차부문 매출액 100조원 상회 전망, 1분기 Review: 가격변수 개선 &gt; 물량감소 우려, 다시 가시권에 들어온 영업이익 8조원, 연결 매출 30조원(전년 대비 증감율+11%), 영업이익 1.9조원(+16%), OPM 6.4%, 차량사업 매출 24조원(전년 대비 증감율+11%), 영업이익 1.3조원(+13%), OPM 5.6%, 금융 매출 4.4조원(전년 대비 증감율+2%), 영업이익 540십억원(+4%), OPM 12.6%, 다시 가시권에 들어온 연간 영업이익 8조원, ‘깜짝 실적’ 현대차, 영업익 8조 시대 9년만에 다시 여나, 다시 가시권에 들어온 영업이익 8조원, 연결 매출 30조원(전년 대비 증감율+11%), 영업이익 1.9조원(+16%), OPM 6.4%, 차량사업 매출 24조원(전년 대비 증감율+11%), 영업이익 1.3조원(+13%), OPM 5.6%, 금융 매출 4.4조원(전년 대비 증감율+2%), 영업이익 540십억원(+4%), OPM 12.6%, 다시 가시권에 들어온 연간 영업이익 8조원, 1분기 어닝서프라이즈 낸 현대차·기아, 드디어 날았다, 현대차·기아, 1분기 호실적에 나란히 '강세'...3%대 상승, 현대차, 연간 영업이익 '8조원' 회복한다…목표가 25만원 -신영證, 하나금투 “현대차, 1분기 ‘깜짝’ 호실적…2분기 이후에도 견조한 실적..., 현대차, 1분기 깜짝 실적…향후 견조한 실적 전망-하나금투, '깜짝 실적' 현대차, "주가 너무 싸다"…목표가 26만원 -신한, "현대차, 우려 이기는 수요…2분기 실적도 양호 예상"-신한, 현대차, 반도체 공급 정상화 지연에도 가격 변수에 양호한 수익성-NH, 현대차, 하반기 공급안정성 회복…중장기 실적개선 유효 -NH, 현대차, 1Q 실적 개선에…성수기 2Q 기대 커진다-신한, '깜짝 실적' 현대차, "주가 너무 싸다"…목표가 26만원 -신한, "현대차, 우려 이기는 수요…2분기 실적도 양호 예상"-신한, 현대차, 반도체 공급 정상화 지연에도 가격 변수에 양호한 수익성-NH, 현대차, 하반기 공급안정성 회복…중장기 실적개선 유효 -NH, 현대차, 1Q 실적 개선에…성수기 2Q 기대 커진다-신한, 현대차, 인플레이션 방어력+공급망 관리력 입증-삼성證, 현대차, 1분기 판매 대수 감소에도 'SUV·제네시스'덕에 매출액 증가..., 현대차, 우려보다 견조한 실적 이어질 것-하나금융투자, "현대차, 1Q '깜짝' 실적…우려보다 견조한 실적 ..., 1분기 어닝서프라이즈 낸 현대차·기아, 드디어 날았다, 1분기 호실적·중장기 성장 전망에 현대차·기아 강세, '어닝서프라이즈'에 현대차·기아 강세, 현대차·기아, 1분기 ‘깜짝’ 호실적에 동반 상승, 코스피·코스닥 상승 출발, 1분기 호실적에 현대차·기아 강세 [개장시황..., 현대차·기아 깜짝실적…주가도 속도낼까, 현대차 이어 삼성도 RE100 만지작…"원전 아닌 재생에너지 필요", 현대차그룹 UAM社…英에 세계 첫 이착륙장, "실적 좋으면 뭐하나요"…성토 쏟아낸 삼전·현대차 개미들, 제네시스 생산 라인 헛돌린다…현대차에도 닥친 중국發 '공포', 폭스바겐·BMW 등 판매량 급감했는데…유럽서 '나홀로 성장' 현대차, 악재 딛고 '깜짝 실적'…현대차 주가 상승, 이것에 달렸다, 현대차·기아, 1분기 ‘깜짝 실적’에도 주가 전망은 ‘박스권’ 왜?, 폭스바겐·BMW 등 판매량 급감했는데…유럽서 '나홀로 성장' 현대차, 년도년도 2분기 1분기 Review: 올해 영업이익 전망치 9조원으로 상향 조정, 년도년도 2분기 1분기 Review: 실적 서프라이즈, 사업 부문별 실적 요약, 2022년 연간 영업이익 추정치 9조원으로 상향 조정, 악재 딛고 '깜짝 실적'…현대차 주가 상승, 이것에 달렸다, 현대차·기아, 호실적에 주가도 화답…5%대 ↑, 현대차·기아, 어닝 서프라이즈에 동반 상승..기관 매수세 몰려, 쏠라이트 인디고 레이싱, 2022 시즌 출정식 진행…현대성우그룹 임직원..., "원자재 관리 강화"…현대차·기아, 최대실적에도 고삐 더 죄는 배경은, 다올투자증권 “현대차, 돌아왔다”, 오토앤, 현대차·기아 중고차 진출 조정안 논의 소식에 오름세, 오토앤, 현대 기아차 '중고차사업' 본격 진출 소식에 강세, 코스피·코스닥 상승 출발, 1분기 호실적에 현대차·기아 강세 [개장시황..., 오토앤, 현대 기아차 '중고차사업' 본격 진출 소식에 강세, (영상)현대차·기아 1분기 '깜짝실적'...고수익차 판매증가 등, 실적 질주한 현대차 기아…주가 '깜짝 반등', '호실적' 현대차·기아 내달렸다, '호실적' 현대차·기아 내달렸다, ‘깜짝 실적’ 현대차, 영업익 8조 시대 9년만에 다시 여나, 현대차·기아, 어닝 서프라이즈에 동반 상승..기관 매수세 몰려, 1분기 어닝 서프라이즈... 현대차·기아 동반 상승</t>
+  </si>
+  <si>
+    <t>현대차 제치고 SK…'업비트 운영' 두나무, 대기업 반열에[2022 대..., “2024년 유럽 출시 목표”…현대차, 경형 전기 SUV 개발 중, SK, 현대車 제치고 자산 2위…두나무, 대기업 지정, "저탄소·디지털 전환" 현대차 등 14곳, 올해 재직자 5000명 직무..., 반도체 호황 후광효과…SK, 현대차 제치고 재계 서열 2위 등극, SK, 현대차 제치고 ‘재계 2위’…올해도 쿠팡 총수는 ‘쿠팡’, “2024년 유럽 출시 목표”…현대차, 경형 전기 SUV 개발 중, 현대차 등 14곳 5372명 직무전환 훈련, "저탄소·디지털 전환" 현대차 등 14곳, 올해 재직자 5000명 직..., 반도체 호황 후광효과…SK, 현대차 제치고 재계 서열 2위 등극, 역시 반도체의 힘…현대차 제치고 재계 2위 된 SK, SK, 현대차 제치고 사상 첫 재계 2위…업비트도 '대기업', 전기차로 뜨는 현대차·기아 “이번엔 인도”, 생산차질을 이겨낸 믹스, 1분기 컨센서스 상회, SUV와 제네시스 중심의 믹스 개선, 전기차 전환 모멘텀 지속 전망, 투자의견 매수, 목표주가 300,000원, 현대두산인프라, 中 위축에도 선방..1Q 영업익 1049억원, 현대차 UAM 법인 ‘슈퍼널’, 영국에 첫 수직이착륙장 세웠다, 친환경 캠핑 브랜드 '디어디어'…더현대서울에 '팝업스토어' 오픈, 범 삼성·현대家 혼맥… 한솔 장남·현대종합금속 장녀 결혼</t>
   </si>
   <si>
     <t>현대차 역대 4번째 '판매거장'…상용차 2500대 판 강병철 부장, 대기업 중고차 진출 1년 유예…현대차·기아 “아쉬운 결과”, 중고차업계 반발에 결국 내년으로…현대차·기아 중고차 판매, 1년 뒤 ..., 현대차·기아, 내년 5월 중고차 판매 '결론'…1~4월 시범사업 [종합..., 중기부 “현대차·기아, 내년 5월 중고차 시장 진출” 권고, 대기업 중고차 진출 1년 유예…현대차·기아 “아쉬운 결과”, 중고차업계 반발에 결국 내년으로…현대차·기아 중고차 판매, 1년 뒤 ..., 현대차·기아, 내년 5월 중고차 판매 '결론'…1~4월 시범사업 [종합..., 현대·기아, 지능제어 공동연구실 설립... "전동화 선도할 초격차 기..., 중기부 “현대차·기아, 내년 5월 중고차 시장 진출” 권고, 현대차·기아, 내년 5월부터 중고차 시장 진출한다, 현대차·기아 중고차 판매 오늘 결론…중고차업계 '단식투쟁', 매출 비슷한 현대차, 시총은 테슬라의 3.6%…차이는 뭘까, 현대차·기아 중고차 사업 언제 시작?…오늘 결론, 두산퓨얼셀, 수소차 연료전지 시장 진출…현대차와 ‘맞짱’, 현대차그룹, 서울·연세·광운대와 협력…'전기차 제어 SW' 개발, "미래 전기차 제어기술 확보"…현대차·기아, 지능 제어 공동연구실 설..., 현대·기아차 '중고차 판매' 오늘 결론…업계는 '단식투쟁'(종합), '3년 연기'vs현대·기아 '수용 불가'…중고차 사업조정 오늘 결정, "AI 전기차 만들자"…현대차·기아, 국내 대학과 맞손, 현대차그룹, 서울·연세·광운대와 협력…'전기차 제어 SW' 개발, "미래 전기차 제어기술 확보"…현대차·기아, 지능 제어 공동연구실 설..., 현대·기아차 '중고차 판매' 오늘 결론…업계는 '단식투쟁'(종합), 현대차·기아 ‘지능 제어’ 공동연구실 설립, "역대 네번째"…현대차, 강병철 영업부장 '상용차 판매거장' 선정, 상용차만 2500대 판매...현대차 강병철 영업부장 '판매거장'에, '3년 연기'vs현대·기아 '수용 불가'…중고차 사업조정 오늘 결정, 중고차 단체, 현대·기아차 시장 진출 예고에 오늘부터 '단식투쟁', 두나무·크래프톤 대기업 됐다…현대차 제친 'SK' 재계 2위 우뚝, 외국인이 사랑한 그룹주는 SK·현대차…삼성·LG·카카오 외면, 매출 비슷한 현대차, 시총은 테슬라의 3.6%…차이는 뭘까, 중고차 단체, 현대·기아차 시장 진출 예고에 오늘부터 '단식투쟁', 두나무·크래프톤 대기업 됐다…현대차 제친 'SK' 재계 2위 우뚝, 외국인이 사랑한 그룹주는 SK·현대차…삼성·LG·카카오 외면, 현대차·기아 중고차 시장 진출 1년 연기…내년 5월부터 판매 가능, "현대차·기아, 러시아서 차량 생산중" 보도에…현대차 "사실 아냐", 현대차 강병철 영업부장, 역대 4번째 상용차 판매거장, 자동차산업협회 "현대차·기아 중고차 시장 진출 유예 유감", HD현대, 정유 부문 호조로 영업익 8050억.. 전년 대비 50.7..., 현대차·기아 ‘지능 제어’ 공동연구실 설립, 현대·기아, 지능제어 공동연구실 설립... "전동화 선도할 초격차 기..., 현대차·기아 중고차 사업 언제 시작?…오늘 결론, 두산퓨얼셀, 수소차 연료전지 시장 진출…현대차와 ‘맞짱’, 타스, 韓 현대·기아차, 중국 업체 러시아서 계속 생산, ‘정유가 살렸다’…HD현대, 1분기 영업이익 8050억원, HD현대, 조선 적자에도 '효자' 정유에 웃었다…1분기 영업익 805..., “상용차만 2500대 팔아” 현대차 강병철씨 ‘판매거장’에, 강병철 현대차 부장 '판매거장', HD현대, 유가 상승·인프라 수요 확대에 매출 전분기比 33% 증가, HD현대, 정유 부문 호조로 영업익 8050억.. 전년 대비 50.7..., 현대차·기아 중고차 판매 오늘 결론…중고차업계 '단식투쟁', '3년 연기'vs현대·기아 '수용 불가'…중고차 사업조정 오늘 결정, 현대차·기아 ‘지능 제어’ 공동연구실 설립, 현대·기아, 지능제어 공동연구실 설립... "전동화 선도할 초격차 기..., 현대차·기아 중고차 사업 언제 시작?…오늘 결론, 두산퓨얼셀, 수소차 연료전지 시장 진출…현대차와 ‘맞짱’, 현대차그룹, 서울·연세·광운대와 협력…'전기차 제어 SW' 개발, HD현대, 유가 상승·인프라 수요 확대에 매출 전분기比 33% 증가, 강병철 현대차 부장 '판매거장', “상용차만 2500대 팔아” 현대차 강병철씨 ‘판매거장’에, HD현대, 조선 적자에도 '효자' 정유에 웃었다…1분기 영업익 805..., 중기부 “현대차·기아, 내년 5월 중고차 시장 진출” 권고, 현대차·기아 중고차 진출 1년 유예…내년 5월 가능, ‘정유가 살렸다’…HD현대, 1분기 영업이익 8050억원, HD현대, 조선 적자에도 '효자' 정유에 웃었다…1분기 영업익 805..., “상용차만 2500대 팔아” 현대차 강병철씨 ‘판매거장’에, 강병철 현대차 부장 '판매거장', HD현대, 유가 상승·인프라 수요 확대에 매출 전분기比 33% 증가, HD현대, 정유 부문 호조로 영업익 8050억.. 전년 대비 50.7..., 현대차·기아 ‘지능 제어’ 공동연구실 설립, "미래 전기차 제어기술 확보"…현대차·기아, 지능 제어 공동연구실 설..., 러 장관 "현대·기아 러에서 차량 생산 중"…현대차 "사실무근", 현대차·기아, 내년 5월부터 개시…인증중고차 판매 단계적 확대, 현대·기아차 '중고차 판매' 오늘 결론…업계는 '단식투쟁'(종합), 현대차·기아, 중고차 사업 1년 연기, '3년 연기'vs현대·기아 '수용 불가'…중고차 사업조정 오늘 결정, 중기부 “현대차·기아, 내년 5월 중고차 시장 진출” 권고, 현대차·기아 중고차 진출 1년 유예…내년 5월 가능, 러 장관 "현대·기아 러에서 차량 생산 중"…현대차 "사실무근", 러시아 산업부 장관 "현대차·기아 계속 생산 중"…현대차 "사실 아냐..., ‘정유가 살렸다’…HD현대, 1분기 영업이익 8050억원, 현대·기아, 지능제어 공동연구실 설립... "전동화 선도할 초격차 기..., 현대·기아차 '중고차 판매' 오늘 결론…업계는 '단식투쟁'(종합), HD현대, 1분기 매출 11조3000억…정유·조선 훈풍, '3년 연기'vs현대·기아 '수용 불가'…중고차 사업조정 오늘 결정, 현대차·기아, 중고차 사업 1년 연기, HD현대 1분기 영업이익 8050억원…전년 동기比 50.7%↑, 자동차산업협회 "현대차·기아 중고차 시장 진출 유예 유감", 러 장관 "현대·기아 러에서 차량 생산 중"…현대차 "사실무근", "현대차·기아, 러시아서 차량 생산중" 보도에…현대차 "사실 아냐", 현대차·기아, 중고차 사업 1년 연기, 현대·기아차 중고차 시장 진출 내년 5월부터…판매규모 제한(종합), 현대차·기아 중고차 시장 진출 1년 연기…내년 5월부터 판매 가능, 현대차그룹 "중고차 시장 진출 1년 유예…아쉬운 결과", 현대차·기아, 중고차 사업진출 내년 5월로 연기…"아쉽지만 수용"</t>
@@ -7909,7 +7909,7 @@
     <t>코스피 주간 기관 순매수 1위 ‘현대차’, 현대차 아이오닉5, 印尼서 일주일만에 사전계약 1600대, 토요타·혼다 게섯거라…현대차, 日 텃밭 인도네시아서 돌풍, 일본 차 텃밭 인도네시아에서…현대차 아이오닉5 대박, 현대차·기아만 '씽씽'…르쌍쉐, 돌파구 있나, "정년연장에 내가 왜 손해보나"…현대차 MZ, 노조에 뿔났다, 전동화 가속페달 현대차…9년만에 8조 클럽 정조준, 토요타·혼다 게섯거라…현대차, 日 텃밭 인도네시아서 돌풍, 현대차, 인도네시아서 첫 판매 톱10… 일본차 독주 깬다, 현대차·기아, 1분기 친환경차 수출 10만대 넘었다</t>
   </si>
   <si>
-    <t>SK, 현대차 제치고 2위…두나무·크래프톤도 대기업, 현대차-NDR 후기: 올해 대장주 예약, 1분기 호실적 확인, 호황이 지속될 수 있는가?, 2가지 핵심 변수 점검, 원가 상승 vs. 가격 인상과 환율로 방어, 전동화 on track, 현대차, 지난달 글로벌 판매 30만8788대... 전년 대비 11.6%..., 지지부진 삼성전자·현대차, 그룹주 ETF는 '순항', 지지부진 삼성전자·현대차, 그룹주 ETF는 '순항', SK케미칼, 현대차가 점찍은 친환경 시트용 국산 바이오 폴리올 양산, SK케미칼, 바이오 신소재 ‘에코트리온’ 양산…현대차 친환경 내장재로 ..., 현대차그룹, 모든 차량 디지털키 지원한다…현대모비스, '브링앤티' 출시, 완성차업계 임단협 시작된다...3일 르노·10일 현대차 '스타트', '반도체 쇼크' 현대차 4월 30만8788대 판매...11.6% 감소, 현대차 30만8788대 판매…반도체난에 주춤, '부품난 계속' 현대차, 4월 30만8788대 판매…전년비 11.6% ..., 기아, 1년만에 4월 내수 판매 5만대 돌파…현대차는 10%대 급락(종..., '부품 수급난 장기화' …현대차·기아, 4월도 마이너스 성적표, 현대차, 4월 판매 전년比 11.6% 급감…반도체 수급난 여파, ‘끝모를 반도체 수급난’… 현대차 4월 판매 11.6% 줄었다 [현대차..., 현대차, 동호회 아마추어 레이싱팀 6년 연속 후원, 현대차, 아마추어 레이싱팀 TEAM HMC 6년째 후원, 지지부진 삼성전자·현대차, 그룹주 ETF는 '순항', 현대차·기아 4월 실적 부진…러시아·中서 판매량 급락, 현대차, 4월 30만 8788대 판매…전년比 11.6% 감소, 현대차, 4월 판매 전년比 11.6% 급감…반도체 수급난 여파, 완성차업계 임단협 시작된다...3일 르노·10일 현대차 '스타트', 현대차 MZ세대, ‘기득권 ’ 노조에 뿔났다, 현대차 ‘아이오닉5’ 인니서 돌풍…작년 판매량의 2배 계약, 현대차, 공급 정상화 전망에 올해 대장주 넘본다-신한, SK케미칼, 친환경 바이오 소재 양산 본격화…현대차 내장재 채택, 현대차, 아마추어 동호회 레이싱팀 'TEAM HMC' 6년 연속 후원, 현대차, 아마추어 동호회 레이싱팀 ‘TEAM HMC’ 6년 연속 후원, 현대차 MZ세대, ‘기득권 ’ 노조에 뿔났다, 현대차 ‘아이오닉5’ 인니서 돌풍…작년 판매량의 2배 계약, 현대차, 공급 정상화 전망에 올해 대장주 넘본다-신한, 현대차, 양상국·정동하 있는 아마추어 레이싱팀 올해도 후원, SK케미칼, 현대차가 점찍은 친환경 시트용 국산 바이오 폴리올 양산, SK케미칼, 바이오 신소재 ‘에코트리온’ 양산…현대차 친환경 내장재로 ..., 현대차, 아마추어 레이싱팀 'TEAM HMC' 6년연속 후원, 현대차, 동호회 아마추어 레이싱팀 6년 연속 후원, 현대차그룹, 모든 차량 디지털키 지원한다…현대모비스, '브링앤티' 출시, 현대차, 4월 판매 전년比 11.6% 급감…반도체 수급난 여파, 현대차 30만8788대 판매…반도체난에 주춤, ‘끝모를 반도체 수급난’… 현대차 4월 판매 11.6% 줄었다 [현대차..., 현대차, 아마추어 레이싱팀 TEAM HMC 6년째 후원, 현대차, 동호회 아마추어 레이싱팀 6년 연속 후원, SK, 현대차 제치고 2위…두나무·크래프톤도 대기업, 현대차, 아마추어 동호회 레이싱팀 ‘TEAM HMC’ 6년 연속 후원, 현대차 30만8788대 판매…반도체난에 주춤, 현대차, 지난달 글로벌 판매 30만8788대... 전년 대비 11.6%...</t>
+    <t>SK, 현대차 제치고 2위…두나무·크래프톤도 대기업, NDR 후기: 올해 대장주 예약, 1분기 호실적 확인, 호황이 지속될 수 있는가?, 2가지 핵심 변수 점검, 원가 상승 vs. 가격 인상과 환율로 방어, 전동화 on track, 현대차, 지난달 글로벌 판매 30만8788대... 전년 대비 11.6%..., 지지부진 삼성전자·현대차, 그룹주 ETF는 '순항', 지지부진 삼성전자·현대차, 그룹주 ETF는 '순항', SK케미칼, 현대차가 점찍은 친환경 시트용 국산 바이오 폴리올 양산, SK케미칼, 바이오 신소재 ‘에코트리온’ 양산…현대차 친환경 내장재로 ..., 현대차그룹, 모든 차량 디지털키 지원한다…현대모비스, '브링앤티' 출시, 완성차업계 임단협 시작된다...3일 르노·10일 현대차 '스타트', '반도체 쇼크' 현대차 4월 30만8788대 판매...11.6% 감소, 현대차 30만8788대 판매…반도체난에 주춤, '부품난 계속' 현대차, 4월 30만8788대 판매…전년비 11.6% ..., 기아, 1년만에 4월 내수 판매 5만대 돌파…현대차는 10%대 급락(종..., '부품 수급난 장기화' …현대차·기아, 4월도 마이너스 성적표, 현대차, 4월 판매 전년比 11.6% 급감…반도체 수급난 여파, ‘끝모를 반도체 수급난’… 현대차 4월 판매 11.6% 줄었다 [현대차..., 현대차, 동호회 아마추어 레이싱팀 6년 연속 후원, 현대차, 아마추어 레이싱팀 TEAM HMC 6년째 후원, 지지부진 삼성전자·현대차, 그룹주 ETF는 '순항', 현대차·기아 4월 실적 부진…러시아·中서 판매량 급락, 현대차, 4월 30만 8788대 판매…전년比 11.6% 감소, 현대차, 4월 판매 전년比 11.6% 급감…반도체 수급난 여파, 완성차업계 임단협 시작된다...3일 르노·10일 현대차 '스타트', 현대차 MZ세대, ‘기득권 ’ 노조에 뿔났다, 현대차 ‘아이오닉5’ 인니서 돌풍…작년 판매량의 2배 계약, 현대차, 공급 정상화 전망에 올해 대장주 넘본다-신한, SK케미칼, 친환경 바이오 소재 양산 본격화…현대차 내장재 채택, 현대차, 아마추어 동호회 레이싱팀 'TEAM HMC' 6년 연속 후원, 현대차, 아마추어 동호회 레이싱팀 ‘TEAM HMC’ 6년 연속 후원, 현대차 MZ세대, ‘기득권 ’ 노조에 뿔났다, 현대차 ‘아이오닉5’ 인니서 돌풍…작년 판매량의 2배 계약, 현대차, 공급 정상화 전망에 올해 대장주 넘본다-신한, 현대차, 양상국·정동하 있는 아마추어 레이싱팀 올해도 후원, SK케미칼, 현대차가 점찍은 친환경 시트용 국산 바이오 폴리올 양산, SK케미칼, 바이오 신소재 ‘에코트리온’ 양산…현대차 친환경 내장재로 ..., 현대차, 아마추어 레이싱팀 'TEAM HMC' 6년연속 후원, 현대차, 동호회 아마추어 레이싱팀 6년 연속 후원, 현대차그룹, 모든 차량 디지털키 지원한다…현대모비스, '브링앤티' 출시, 현대차, 4월 판매 전년比 11.6% 급감…반도체 수급난 여파, 현대차 30만8788대 판매…반도체난에 주춤, ‘끝모를 반도체 수급난’… 현대차 4월 판매 11.6% 줄었다 [현대차..., 현대차, 아마추어 레이싱팀 TEAM HMC 6년째 후원, 현대차, 동호회 아마추어 레이싱팀 6년 연속 후원, SK, 현대차 제치고 2위…두나무·크래프톤도 대기업, 현대차, 아마추어 동호회 레이싱팀 ‘TEAM HMC’ 6년 연속 후원, 현대차 30만8788대 판매…반도체난에 주춤, 현대차, 지난달 글로벌 판매 30만8788대... 전년 대비 11.6%...</t>
   </si>
   <si>
     <t>‘현대 N 페스티벌’ 6일 본격 질주…3년만에 유관중 개최, "3년 만에 관중받는다" 현대 N 페스티벌 6일 개막, "3년 만에 관중받는다" 현대 N 페스티벌 6일 개막, ‘현대 N 페스티벌’ 6일 본격 질주…3년만에 유관중 개최, '현대 N 페스티벌' 6일 개막...'아반떼 N컵' 신설, "북미 넘어 세계시장 챙긴다"…현대차 美 법인장, 본사 이사회 합류, "어린이도 즐기는 현대N" 칠드런스데이 준비한 현대차, 현대차, 피치스 도원서 ‘칠드런스 데이’ 행사, "시공간을 넘나드는 이동경험" 현대차, 별똥별 NFT 판매, 현대차, 이더리움 기반 ‘별똥별’ NFT 판매, 현대차, 9일~10일 메타모빌리티 NFT 1만개 판매, 현대차, 이더리움 기반 '별똥별 NFT' 1만개 판매, 현대차, '넥쏘' 판매량 감소에도 1분기 세계 수소차시장 1위 수성, 1분기 세계 수소차 판매 4000대 하회…현대차 1위 수성, 1분기 세계 수소차 판매 4000대 하회…현대차 1위 수성, 현대자동차·기아, 매년 협력사와 'R&amp;D 테크데이' 행사…기술정보 공유..., "북미 넘어 세계시장 챙긴다"…현대차 美 법인장, 본사 이사회 합류, 호세 무뇨스 사장, 현대차 이사회 합류…“글로벌 경쟁력 높인다”, 비테스코 테크놀로지스, 현대차그룹에 전동화 구동 시스템 공급…“2조60..., 현대차, 이더리움 기반 '별똥별 NFT' 1만개 판매, 현대차, 이더리움 기반 별똥별 NFT 1만개 판매, 현대차, 피치스 도원서 ‘칠드런스 데이’ 행사, 현대차 “우리 아이도 N브랜드카 드라이버”, "N 브랜드 즐기세요" 현대차, 어린이날 행사 개최, 현대차, N 브랜드 체험할 수 있는 어린이날 행사 개최, 현대차, 9일~10일 메타모빌리티 NFT 1만개 판매, 현대차, ‘별똥별’ NFT 판매…메타모빌리티 비전 담다, 현대차, 메타모빌리티 비전 담은 별똥별 NFT 판매 시작, 현대차, '넥쏘' 판매량 감소에도 1분기 세계 수소차시장 1위 수성, 현대차·기아, 반도체 공급난 뚫고 '깜짝 실적'</t>
@@ -7927,10 +7927,10 @@
     <t>현대차, 대규모 LNG 발전소 짓는다…"전력 직접 생산", 현대차, LNG발전소 직접 짓는다…울산공장 전력량 70% 조달, 현대차, LNG발전소 직접 짓는다…울산공장 전력량 70% 조달, 현대차, 대규모 LNG 발전소 짓는다…"전력 직접 생산", 현대차, 전기차 판매 하이브리드카 추월… 전기차 대중화 속도, 전기차 시장 현대기아·테슬라만 있냐…'가성비' 대항마 풀린다, 현대차, LNG발전소 지어 전력 직접 생산, 현대차, 전기차 판매 하이브리드카 추월… 전기차 대중화 속도, 전기차 공장은 '에너지 하마'…현대차, 탄소배출 줄이고 전력 ..., 전기차 시장 현대기아·테슬라만 있냐…'가성비' 대항마 풀린다, 전기차 시장 현대기아·테슬라만 있냐…'가성비' 대항마 풀린다, 현대차, 전기차 판매 하이브리드카 추월… 전기차 대중화 속도</t>
   </si>
   <si>
-    <t>현대차, 고객 아이디어로 상품 개발한다, "어떻게 하면 20~30대가 현대차 좋아할까요?"…아이디어 공모전 개최, 현대차, 울산에 LNG 발전소 직접 짓는다, 거꾸로 가는 현대차 노조, (영상)현대차, 울산에 LNG 발전소 건설 추진..."전력 직접 생산", 현대이지웰, 1분기 영업익 80억…전년비 13.5% ↑, 현대차, ‘제 2회 H-ear 커스터마이징 아이디어 공모전’ 개최, "현대·기아차 전용 전기차 잘 나가네"…내수 5만대 수출 10만대 돌파, 거꾸로 가는 현대차 노조, 현대차-미국 증설, 감출 수 없는 흥분, 미국 턴어라운드 본격 및 전기차 전용공장 신설로 장기 성장동력 확대 가능성 점검, 현대차-일시적인 판매 부진보다 M/S 상승에 주목, 22년도 1분기 , Surpise, 실적 개선, 이제 시작일 뿐, 판매량 반등이 주가 견인, 현대차, 고객 아이디어로 상품 개발한다, 현대차, 고객 아이디어로 상품 개발한다, 현대자동차 H-ear 커스터마이징 아이디어 공모전, 현대차, 울산공장에 LNG 열병합발전소 짓는다…“전력 자체 조달”, 현대이지웰, 1분기 영업익 80억…전년비 13.5% ↑, "현대·기아차 전용 전기차 잘 나가네"…내수 5만대 수출 10만대 돌..., 현대차, 고객 아이디어로 상품 개발한다, 현대자동차 H-ear 커스터마이징 아이디어 공모전, 현대차, 고객 아이디어로 상품 개발한다, "어떻게 하면 20~30대가 현대차 좋아할까요?"…아이디어 공모전 개최, "고객 의견 받아 상품·서비스 개발"…현대차, 아이디어 공모전 개최, 현대차, 美조지아주에 전기차 전용 공장 신설 추진, 로이터 "현대차, 美 조지아에 전기차 공장 설립", 현대차·기아, 전용 전기차 내수 5만대·수출 10만대 돌파, 현대차·기아, 전용 전기차 내수 5만대·수출 10만대 돌파, "현대차, 美조지아에 전기차공장 건설 협의", "현대·기아차 전용 전기차 잘 나가네"…내수 5만대 수출 10만대 돌..., 현대차·기아, 전용 전기차 내수 5만대·수출 10만대 돌파, 현대차, 울산에 LNG 발전소 직접 짓는다, 현대이지웰, 1분기 영업익 80억…전년비 13.5% ↑, 현대자동차 H-ear 커스터마이징 아이디어 공모전, 현대차, 고객 아이디어로 상품 개발한다, (영상)현대차, 울산에 LNG 발전소 건설 추진..."전력 직접 생산", "현대·기아차 전용 전기차 잘 나가네"…내수 5만대 수출 10만대 돌..., 로이터 "현대차, 美 조지아에 전기차 공장 설립", "어떻게 하면 20~30대가 현대차 좋아할까요?"…아이디어 공모전 개최, 현대차, 美조지아주에 전기차 전용 공장 신설 추진</t>
-  </si>
-  <si>
-    <t>현대차, E-GMP 전기차 해외생산 본격화…美조지아 공장신설 논의, (영상)현대차, 임단협 가시밭길 '예고'...노조 리스크 커진다, 현대차 노사, 임단협 상견례…'정년연장' 놓고 충돌 예고, "반도체 공급난에도 수요 여전…현대차·기아 실적엔 긍정적", 현대百 1분기 매출·영업익 37%↑ 전망치 상회, 트루윈, 현대차그룹 전기차 3종에 'SLS' 공급…실적 기대감, 트루윈, 현대차그룹 전기차 3종에 SLS 공급, 현대차, 북미 친환경 상용차 시장 공략한다, 현대차, ‘ACT 엑스포 2022’ 참가…"북미 친환경 상용차 시장 ..., 트루윈, 현대차그룹 전기차 3종에 'SLS' 공급…실적 기대감, 트루윈, 현대차그룹 전기차 3종에 SLS 공급, 현대차, E-GMP 전기차 해외생산 본격화…美조지아 공장신설 논의, "현대차, 美조지아에 전기차공장 설립…조단위 혜택 예상", “현대차, 美 조지아 주에 새 전기차 공장 설립 논의 중”, 현대차 ‘ACT 엑스포’ 참가…북미 친환경 상용차 시장 공략한다, 현대차, ‘ACT 엑스포 2022’ 참가…"북미 친환경 상용차 시장 공..., 트루윈, 현대자동차 그룹 전기차 3종에 ‘SLS’ 공급, 현대차, 북미 최대 청정 운송수단 박람회서 수소 전기트럭 선봬, 현대차, 'ACT 엑스포 2022' 첫 참가…엑시언트 수소트럭 전시, 현대차, 북미 친환경 상용차 시장 공략한다, 현대차, ‘ACT 엑스포 2022’ 참가…"북미 친환경 상용차 시장 ..., 현대차, 북미 친환경 상용차 시장 공략, 현대百, 1분기 매출·영업익 껑충…'패션·스포츠' 효자 등극, 현대차 "수소트럭 앞세워 북미 공략", "북미 친환경트럭 시장 공략" 현대차, 박람회서 수소트럭 선봬, 현대차-수익성은 제네시스, 미래는 수소 상용차, 투자의견 BUY, 목표주가 240,000 원으로 커버리지 개시, 개선될 실적에 날개를 달아줄 제네시스, 두드러지는 믹스 개선, BEV 성장은 기본, 수소 상용차는 특장점으로, 43조 '글로벌 수소 동맹' 뜬다…현대차·SK·블랙스톤 총출동, 현대차, 올해 임금협상 시작…험난한 가시밭길 예고, 현대차, 美 조지아주 전기차 공장 짓나...외신 "당국과 협의 중", SK·한화·현대…석탄 버리고 LNG발전 전환, 현대에버다임, 1분기 영업익 45억원…전년비 1955.5% 증가, 현대百 1분기 영업익 37% 증가, 현대차, 美 조지아주 전기차 공장 짓나...외신 "당국과 협의 중", 현대차, 美 조지아주에 전기차 전용 공장 검토, 현대百, 최대 3000억 규모 공모채 발행…"단기 CP 상환 ..., (영상)현대차, 임단협 가시밭길 '예고'...노조 리스크 커진다, 이동석 "올해 현대차 임단협 교섭 최대 변곡점…노사 함께 노력해야", 尹대통령, 취임 첫날 삼성·SK·현대차 등 5대그룹 총수와 이례적 만찬, 尹대통령, 취임 첫날 삼성·SK·현대차 등 5대그룹 총수와 이례적 만찬, 이동석 "올해 현대차 임단협 교섭 최대 변곡점…노사 함께 노력해야", (영상)현대차, 임단협 가시밭길 '예고'...노조 리스크 커진다</t>
+    <t>현대차, 고객 아이디어로 상품 개발한다, "어떻게 하면 20~30대가 현대차 좋아할까요?"…아이디어 공모전 개최, 현대차, 울산에 LNG 발전소 직접 짓는다, 거꾸로 가는 현대차 노조, (영상)현대차, 울산에 LNG 발전소 건설 추진..."전력 직접 생산", 현대이지웰, 1분기 영업익 80억…전년비 13.5% ↑, 현대차, ‘제 2회 H-ear 커스터마이징 아이디어 공모전’ 개최, "현대·기아차 전용 전기차 잘 나가네"…내수 5만대 수출 10만대 돌파, 거꾸로 가는 현대차 노조, 미국 증설, 감출 수 없는 흥분, 미국 턴어라운드 본격 및 전기차 전용공장 신설로 장기 성장동력 확대 가능성 점검, 일시적인 판매 부진보다 M/S 상승에 주목, 22년도 1분기 , Surpise, 실적 개선, 이제 시작일 뿐, 판매량 반등이 주가 견인, 현대차, 고객 아이디어로 상품 개발한다, 현대차, 고객 아이디어로 상품 개발한다, 현대자동차 H-ear 커스터마이징 아이디어 공모전, 현대차, 울산공장에 LNG 열병합발전소 짓는다…“전력 자체 조달”, 현대이지웰, 1분기 영업익 80억…전년비 13.5% ↑, "현대·기아차 전용 전기차 잘 나가네"…내수 5만대 수출 10만대 돌..., 현대차, 고객 아이디어로 상품 개발한다, 현대자동차 H-ear 커스터마이징 아이디어 공모전, 현대차, 고객 아이디어로 상품 개발한다, "어떻게 하면 20~30대가 현대차 좋아할까요?"…아이디어 공모전 개최, "고객 의견 받아 상품·서비스 개발"…현대차, 아이디어 공모전 개최, 현대차, 美조지아주에 전기차 전용 공장 신설 추진, 로이터 "현대차, 美 조지아에 전기차 공장 설립", 현대차·기아, 전용 전기차 내수 5만대·수출 10만대 돌파, 현대차·기아, 전용 전기차 내수 5만대·수출 10만대 돌파, "현대차, 美조지아에 전기차공장 건설 협의", "현대·기아차 전용 전기차 잘 나가네"…내수 5만대 수출 10만대 돌..., 현대차·기아, 전용 전기차 내수 5만대·수출 10만대 돌파, 현대차, 울산에 LNG 발전소 직접 짓는다, 현대이지웰, 1분기 영업익 80억…전년비 13.5% ↑, 현대자동차 H-ear 커스터마이징 아이디어 공모전, 현대차, 고객 아이디어로 상품 개발한다, (영상)현대차, 울산에 LNG 발전소 건설 추진..."전력 직접 생산", "현대·기아차 전용 전기차 잘 나가네"…내수 5만대 수출 10만대 돌..., 로이터 "현대차, 美 조지아에 전기차 공장 설립", "어떻게 하면 20~30대가 현대차 좋아할까요?"…아이디어 공모전 개최, 현대차, 美조지아주에 전기차 전용 공장 신설 추진</t>
+  </si>
+  <si>
+    <t>현대차, E-GMP 전기차 해외생산 본격화…美조지아 공장신설 논의, (영상)현대차, 임단협 가시밭길 '예고'...노조 리스크 커진다, 현대차 노사, 임단협 상견례…'정년연장' 놓고 충돌 예고, "반도체 공급난에도 수요 여전…현대차·기아 실적엔 긍정적", 현대百 1분기 매출·영업익 37%↑ 전망치 상회, 트루윈, 현대차그룹 전기차 3종에 'SLS' 공급…실적 기대감, 트루윈, 현대차그룹 전기차 3종에 SLS 공급, 현대차, 북미 친환경 상용차 시장 공략한다, 현대차, ‘ACT 엑스포 2022’ 참가…"북미 친환경 상용차 시장 ..., 트루윈, 현대차그룹 전기차 3종에 'SLS' 공급…실적 기대감, 트루윈, 현대차그룹 전기차 3종에 SLS 공급, 현대차, E-GMP 전기차 해외생산 본격화…美조지아 공장신설 논의, "현대차, 美조지아에 전기차공장 설립…조단위 혜택 예상", “현대차, 美 조지아 주에 새 전기차 공장 설립 논의 중”, 현대차 ‘ACT 엑스포’ 참가…북미 친환경 상용차 시장 공략한다, 현대차, ‘ACT 엑스포 2022’ 참가…"북미 친환경 상용차 시장 공..., 트루윈, 현대자동차 그룹 전기차 3종에 ‘SLS’ 공급, 현대차, 북미 최대 청정 운송수단 박람회서 수소 전기트럭 선봬, 현대차, 'ACT 엑스포 2022' 첫 참가…엑시언트 수소트럭 전시, 현대차, 북미 친환경 상용차 시장 공략한다, 현대차, ‘ACT 엑스포 2022’ 참가…"북미 친환경 상용차 시장 ..., 현대차, 북미 친환경 상용차 시장 공략, 현대百, 1분기 매출·영업익 껑충…'패션·스포츠' 효자 등극, 현대차 "수소트럭 앞세워 북미 공략", "북미 친환경트럭 시장 공략" 현대차, 박람회서 수소트럭 선봬, 수익성은 제네시스, 미래는 수소 상용차, 투자의견 BUY, 목표주가 240,000 원으로 커버리지 개시, 개선될 실적에 날개를 달아줄 제네시스, 두드러지는 믹스 개선, BEV 성장은 기본, 수소 상용차는 특장점으로, 43조 '글로벌 수소 동맹' 뜬다…현대차·SK·블랙스톤 총출동, 현대차, 올해 임금협상 시작…험난한 가시밭길 예고, 현대차, 美 조지아주 전기차 공장 짓나...외신 "당국과 협의 중", SK·한화·현대…석탄 버리고 LNG발전 전환, 현대에버다임, 1분기 영업익 45억원…전년비 1955.5% 증가, 현대百 1분기 영업익 37% 증가, 현대차, 美 조지아주 전기차 공장 짓나...외신 "당국과 협의 중", 현대차, 美 조지아주에 전기차 전용 공장 검토, 현대百, 최대 3000억 규모 공모채 발행…"단기 CP 상환 ..., (영상)현대차, 임단협 가시밭길 '예고'...노조 리스크 커진다, 이동석 "올해 현대차 임단협 교섭 최대 변곡점…노사 함께 노력해야", 尹대통령, 취임 첫날 삼성·SK·현대차 등 5대그룹 총수와 이례적 만찬, 尹대통령, 취임 첫날 삼성·SK·현대차 등 5대그룹 총수와 이례적 만찬, 이동석 "올해 현대차 임단협 교섭 최대 변곡점…노사 함께 노력해야", (영상)현대차, 임단협 가시밭길 '예고'...노조 리스크 커진다</t>
   </si>
   <si>
     <t>현대에버다임, 1분기 호실적 발표 ‘강세’, 현대백화점, "더현대' 약진으로 실적 개선 전망…목표가 25%↑-IBK, 현대차 노조 "번 만큼 받아야…성과금 2340→4680만원 두 배가 적..., 현대차, 상품성 강화한 ‘2022 그랜저’ 출시…3392만원부터, 현대백화점, "더현대' 약진으로 실적 개선 전망…목표가 25%↑-IBK, 현대차그룹 '오토카 어워즈' 5개 부문 수상, 현대차, ‘2022 그랜저’ 출시…"3392만원부터 시작", 현대차그룹, ‘2022 오토카 어워즈’ 5개 부문 수상, 현대차그룹, 英 전문매체 시상식서 5개부문 수상, 현대차, '자율주행 레벨 4' 글로벌 캠페인 영상공개, 현대차그룹, 英 오토카 어워즈서 5개 부문 수상, 英이 사랑하는 현대차그룹…EV6·싼타페·i20 N 오토카 어워즈 수상, 현대차, 연식변경 '2022 그랜저' 출시... "선호 사양 기본화", 현대차 노조 "번 만큼 받아야…성과금 2340→4680만원 두 배가 적..., 현대차그룹, 英 오토카 어워즈서 5개 부문 수상, 英이 사랑하는 현대차그룹…EV6·싼타페·i20 N 오토카 어워즈 수상, 로봇이야 자동차야…현대차 '궁극의 모빌리티' 정체는, 현대차그룹 ‘오토카 어워즈’ 5개부문 수상, 동양피스톤, 현대차·SK 등 43조 ‘글로벌 수소 동맹’ 속 ..., 현대차그룹, 英 전문매체 시상식서 5개부문 수상, "사람을 닮은 자율주행" 현대차가 공개한 레벨4 기술비전, 현대차, 기본 옵션 대폭 확충한 2022 그랜저 출시, 현대차 '2022 그랜저' 출시...3392만원부터, "사람을 닮은 자율주행" 현대차가 공개한 레벨4 기술비전, 현대차, 기본 옵션 대폭 확충한 2022 그랜저 출시, 현대차 '2022 그랜저' 출시...3392만원부터, 英이 사랑하는 현대차그룹…EV6·싼타페·i20 N 오토카 어워즈 수상, 현대차, 영상 통해 ‘레벨 4’ 자율주행 세계 선보인다, 현대차의 레벨 4 수준 자율주행 미리보기…캠페인 영상 공개, 현대차, 연식변경 '2022 그랜저' 출시... "선호 사양 기본화"</t>
@@ -7948,7 +7948,7 @@
     <t>"온돌방車에 누워서 출퇴근"…현대차가 꿈꾸는 자율 주행차, 현대차, 美에 전기차 첫 전용공장 이유…테슬라 안방서 정면승부, 삼성, 4세 경영승계 포기…SK·현대차·LG, 이사회 주도 ESG 강화, 이재용도 선택한 현대 팰리세이드...새 얼굴로 다음주 출격, "이게 차라고?"...현대차그룹, '모빌리티 온돌' 콘셉트 공개, 현대차, 자율車에 온돌 깐다…모빌리티 콘셉트 특허 출원, 현대차, 美에 전기차 첫 전용공장 이유…테슬라 안방서 정면승부, 현대차, 자율車에 온돌 깐다…모빌리티 콘셉트 특허 출원, 이재용도 선택한 현대 팰리세이드...새 얼굴로 다음주 출격, "이게 차라고?"...현대차그룹, '모빌리티 온돌' 콘셉트 공개</t>
   </si>
   <si>
-    <t>구독하면 충전료 186만원 깎인다…현대차, 럭키패스 H 출시, 아모센스, 수소센서 핵심부품 현대차 국책과제 공동개발 부각↑, 아모센스, 수소센서 핵심부품 현대차 국책과제 공동개발 부각↑, "충전요금 최대 50%할인"…현대차, 구독형 전기차 충전 요금제 출시, 구독하면 충전료 186만원 깎인다…현대차, 럭키패스 H 출시, "충전요금 최대 50%할인"…현대차, 구독형 전기차 충전 요금제 출시, 현대차, 구독형 전기차 충전 요금제 선보여, 현대차, 구독형 전기차 충전요금제 출시, 현대차-쏘나타 단종, 대표 선수 제네시스로 교체, 중형 세단 쏘나타, 역사 속으로, 경쟁사 대비 빠른 대응, 제네시스, 쏘나타보다 더 파는 모델, 전기차 충전도 구독시대…현대차, 최대 50% 할인, 현대차, 구독형 전기차 충전요금제 출시, "현대차는 유연하다…전동화 시대 퍼스트무버될 것", 현대차, 구독형 전기차 충전요금제 상품 출시, 현대차, 구독형 전기차 충전 요금제 선보여, 현대차, 구독형 전기차 충전요금제 상품 출시, 전기차 충전도 구독시대…현대차, 최대 50% 할인, 전기차 수출 3배 뛰었지만…웃지 못하는 현대·기아, 구독하면 충전료 186만원 깎인다…현대차, 럭키패스 H 출시, 전기차 충전비 부담 줄인다…현대차, 구독형 상품 '럭키패스 H' 출시, "충전요금 최대 50%할인"…현대차, 구독형 전기차 충전 요금제 출시, 현대차, 구독형 전기차 충전 요금제 출시…“할인·적립 동시에”, 현대차, 구독형 전기차 충전요금제 출시...최대 50% 할인, "현대차는 유연하다…전동화 시대 퍼스트무버될 것"</t>
+    <t>구독하면 충전료 186만원 깎인다…현대차, 럭키패스 H 출시, 아모센스, 수소센서 핵심부품 현대차 국책과제 공동개발 부각↑, 아모센스, 수소센서 핵심부품 현대차 국책과제 공동개발 부각↑, "충전요금 최대 50%할인"…현대차, 구독형 전기차 충전 요금제 출시, 구독하면 충전료 186만원 깎인다…현대차, 럭키패스 H 출시, "충전요금 최대 50%할인"…현대차, 구독형 전기차 충전 요금제 출시, 현대차, 구독형 전기차 충전 요금제 선보여, 현대차, 구독형 전기차 충전요금제 출시, 쏘나타 단종, 대표 선수 제네시스로 교체, 중형 세단 쏘나타, 역사 속으로, 경쟁사 대비 빠른 대응, 제네시스, 쏘나타보다 더 파는 모델, 전기차 충전도 구독시대…현대차, 최대 50% 할인, 현대차, 구독형 전기차 충전요금제 출시, "현대차는 유연하다…전동화 시대 퍼스트무버될 것", 현대차, 구독형 전기차 충전요금제 상품 출시, 현대차, 구독형 전기차 충전 요금제 선보여, 현대차, 구독형 전기차 충전요금제 상품 출시, 전기차 충전도 구독시대…현대차, 최대 50% 할인, 전기차 수출 3배 뛰었지만…웃지 못하는 현대·기아, 구독하면 충전료 186만원 깎인다…현대차, 럭키패스 H 출시, 전기차 충전비 부담 줄인다…현대차, 구독형 상품 '럭키패스 H' 출시, "충전요금 최대 50%할인"…현대차, 구독형 전기차 충전 요금제 출시, 현대차, 구독형 전기차 충전 요금제 출시…“할인·적립 동시에”, 현대차, 구독형 전기차 충전요금제 출시...최대 50% 할인, "현대차는 유연하다…전동화 시대 퍼스트무버될 것"</t>
   </si>
   <si>
     <t>현대차, RV 평균가격 작년보다 290만원 올라, 모셔널, 현대차 아이오닉 5로 우버이츠 자율주행 배송 ‘시동’, 모셔널, 현대차 아이오닉5로 자율주행 '우버이츠' 시작, 엘엠에스, 현대차 모바일로봇 라이다 개발 기대감에 고공행진, 삼성전자 팔고 SK하이닉스, 현대차 대신 기아...2등주 사는 외국인, 현대차 노조 "美 전기차 공장 설립 추진은 단협 위반…강력 대응할 것", "차를 넘어 모빌리티 혁명"…현대차그룹, 모바일 로봇 생태계 구축, 현대차, 모바일 로봇 개발 박차…에스오에스랩과 라이다 공동개발, 모바일 로봇 개발 가속…현대차, 에스오에스랩과 라이다 공동 개발, 현대차 “모바일 로봇용 라이다 개발”…센서업체 에스오에스랩과 업무협약, 엘엠에스, 현대차 모바일로봇 라이다 개발 기대감에 고공행진, 엘엠에스, 현대차-에스오에스랩 모바일 로봇용 라이다 공동개발..., "차를 넘어 모빌리티 혁명"…현대차그룹, 모바일 로봇 생태계 구축, 현대차, 모바일 로봇 개발 박차…에스오에스랩과 라이다 공동개발, 애플 타격에 LGD도 눈물, 현대기아 공장은 빈 벨트만…야속한 ‘中 봉..., 모셔널, 현대차 아이오닉5로 자율주행 '우버이츠' 시작, 모셔널, 현대차 아이오닉 5로 우버이츠 자율주행 배송 ‘시동’, 애플 타격에 LGD도 눈물, 현대기아 공장은 빈 벨트만…야속한 ‘中 봉..., 현대차그룹, 에스오에스랩과 모바일 로봇용 라이다 공동 개발, 현대차그룹-에스오에스랩, 모바일 로봇 라이다 공동 연구개발키로, 현대차 ‘모바일 로봇용 라이다’ 개발한다</t>
@@ -7957,7 +7957,7 @@
     <t>'무공해차 전환' 국정과제 발맞춰… 투자 보따리 푼 현대차 [尹정부의..., 현대차그룹, 2030년 국내서 전기차 144만대 만든다, "국내서 年144만대 생산"…현대차·기아 '전기차'에 21조원 붓는다, 유진로봇, LG·현대와 ‘자율주행로봇’ 공동사업 출범 소식에..., 현대차·기아 21조 투자에...정부, 민간주도 모빌리티 혁명 지원, 현대차의 로봇개 스폿, 포스코 광양제철소에서 안전관리한다, “日전기차 충전성능, 현대차 등 경쟁사에 크게 뒤떨어져", "현대차의 절반 수준…이러다 다 잃는다" 다급해진 日 [정영효의 일본..., 현대차·기아, 21조 투자 국내서 전기차 144만대 만든다, 현대차그룹, 2030년 국내서 전기차 144만대 만든다, 현대차·기아 21조 투자에...정부, 민간주도 모빌리티 혁명 지원, 현대차의 로봇개 스폿, 포스코 광양제철소에서 안전관리한다, 현대차·기아, 2030년까지 국내 전기차에 21조원 투자, “日전기차 충전성능, 현대차 등 경쟁사에 크게 뒤떨어져", 로봇이 서빙하고 잔디깎고 배송하고…삼성·LG·현대차 로봇사업 확대중, '대형 SUV 최강자' 현대차 더 뉴 펠리세이드 출시…가격 3867만 ..., 현대차 ‘더 뉴 팰리세이드’ 출시…3867만원부터, 러시아 생산차질 누적 3만대…현대차 신흥국 전략 ‘무게 이동’? [비즈..., 현대차 '더 뉴 팰리세이드' 출시...3867만원부터, '가성비 대명사' 현대차 더 뉴 팰리세이드 출시…3867만원부터, 현대차證 "코스맥스, 중국 락다운 타격 불가피…목표주가 8만 원으로 ↓..., '가성비 대명사' 현대차 더 뉴 팰리세이드 출시…3867만원부터, 현대차證 "코스맥스, 중국 락다운 타격 불가피…목표주가 8만 원으로 ↓..., "현대차의 절반 수준…이러다 다 잃는다" 다급해진 日 [정영효의 일본산..., 현대차 노사 임단협 첫 교섭…"정년연장 등 고용 안정 관건", "현대차의 절반 수준…이러다 다 잃는다" 다급해진 日 [정영효의 일본..., 현대차·기아, 국내 전기차 생산 年144만대로 늘린다 [속도내는 전기차..., '자동차산업 분수령'…현대차·기아, 전기차에 21조 쏟아붓는다, 이재용이 낙점한 '로봇 사업' 판 커진다…삼성·LG·현대차 출사표(종합..., "테슬라 잡아라"...현대차그룹, 2030년까지 21조원 투자, 현대차 ‘더 뉴 팰리세이드'출시… 3867만원부터, 현대차 '더 뉴 팰리세이드' 출시...3867만원부터, 현대百 회사채에 1조 뭉칫돈…회사채 시장 풀리나, 현대차·기아, 국내 전기차 생산 年144만대로 늘린다 [속도내는 전기차..., '무공해차 전환' 국정과제 발맞춰… 투자 보따리 푼 현대차 [尹정부의..., 현대차 ‘더 뉴 팰리세이드'출시… 3867만원부터, 현대차 '더 뉴 팰리세이드' 출시...3867만원부터, 현대차·기아 "2030년 전기차 절반 한국서 생산", 현대차·기아, 국내 전기차에 21兆 베팅, 현대百 회사채에 1조 뭉칫돈…회사채 시장 풀리나, 로봇이 서빙하고 잔디깎고 배송하고…삼성·LG·현대차 로봇사업 확대중, 대우조선, 대금 미지급에 러 계약 해지…현대·삼성重도 번지나, 현대차·기아, 4월 유럽판매 13.2％↑…점유율 10％ 돌파, 이재용이 낙점한 '로봇 사업' 판 커진다…삼성·LG·현대차 출사표(종합..., 로봇이 서빙하고 잔디깎고 배송하고…삼성·LG·현대차 로봇사업 확대중, '자동차산업 분수령'…현대차·기아, 전기차에 21조 쏟아붓는다, "국내서 年144만대 생산"…현대차·기아 '전기차'에 21조원 붓는다, 유진로봇, LG·현대와 ‘자율주행로봇’ 공동사업 출범 소식에..., 현대차·기아, 4월 유럽판매 13.2％↑…점유율 10％ 돌파, 현대차·기아, 4월 유럽판매 13.2% 늘었다…점유율 10.7% 껑충, 현대차그룹, 국내 전기차 21조 투자 "144만대 생산", 현대차·기아, 2030년까지 국내에 21兆 투입…전기차 144만대 생..., 현대차그룹, 유럽 토종 브랜드 주춤할동안…4월 판매 '나홀로 성장', 현대차·기아 "韓 전기차 허브로…年144만대 생산"</t>
   </si>
   <si>
-    <t>현대차-견조한 실적 유지. 전기차 모멘텀 기대, 하반기에도 견조한 실적 흐름 유지, 전기차 판매비중은 추가 상승, 글로벌 업종평균 대비 Valuation 낮은 편, "공장 안돌아" 현대차·기아 車값↑…'승용차' 평균가는 떨어진 이유, 현대차 선행생산기술센터, 정부인증 연구소 전환 추진, 현대자동차·기아, 2022 '발명의 날' 행사 개최, 현대차·기아 ‘발명의 날’ 우수특허 9건 선정·포상, 인플레 공포 '성큼'?…증권가 "삼전·현대차 등 '대형수출주' 기회", 현대·기아 이어 GM까지...NFT 시장 뛰어든다, 현대·벤츠·포르쉐·아우디 등 차량 6만4754대, 제작결함에 리콜, 현대차 1분기 원재료 구매비 1조 증가… 車값 또 오르나, 현대차·기아 ‘발명의 날’ 우수특허 9건 선정·포상, "로보틱스부터 AI까지"…현대차·기아, '2022발명의 날' 행사 개최, "공장 안돌아" 현대차·기아 車값↑…'승용차' 평균가는 떨어진 이유, 현대·기아 이어 GM까지...NFT 시장 뛰어든다, 인플레 공포 '성큼'?…증권가 "삼전·현대차 등 '대형수출주' 기회", 우수AMS, 현대車 21조 투자...범현대家 등 업고 전기차 ..., 현대차 1분기 원재료 구매비 1조 증가… 車값 또 오르나, 더현대서울, 초고속 손익분기점 달성, 현대차 1분기 원재료 구매비 1조 증가… 車값 또 오르나, 현대차·기아 ‘발명의 날’ 우수특허 9건 선정·포상, "로보틱스부터 AI까지"…현대차·기아, '2022발명의 날' 행사 개최, "주차 중 P단 해제"...국토부, 현대차 아이오닉 5 등 리콜, 美 조지아주, 20일에 현대차 전기차공장 유치 발표할 듯, 더현대서울, 초고속 손익분기점 달성, 더현대서울, 13개월만에 손익분기 넘겼다…초고속 비결은?, "주차 중 P단 해제"...국토부, 현대차 아이오닉 5 등 리콜, 美 조지아주, 20일에 현대차 전기차공장 유치 발표할 듯, 대우조선, ‘대금 미지급’ 러 계약 해지…현대·삼성重도 피해 우려[뒷북..., 현대차·기아, 국내 전기차 분야 21조원 투자…“韓 전기차 허브로”[뒷..., 경사로 주차중 'P단' 풀려…현대차, 아이오닉5 등 5.8만대 무상 업..., 더현대서울, 13개월만에 손익분기 넘겼다…초고속 비결은?, 현대차 선행생산기술센터, 정부인증 연구소 전환 추진</t>
+    <t>견조한 실적 유지. 전기차 모멘텀 기대, 하반기에도 견조한 실적 흐름 유지, 전기차 판매비중은 추가 상승, 글로벌 업종평균 대비 Valuation 낮은 편, "공장 안돌아" 현대차·기아 車값↑…'승용차' 평균가는 떨어진 이유, 현대차 선행생산기술센터, 정부인증 연구소 전환 추진, 현대자동차·기아, 2022 '발명의 날' 행사 개최, 현대차·기아 ‘발명의 날’ 우수특허 9건 선정·포상, 인플레 공포 '성큼'?…증권가 "삼전·현대차 등 '대형수출주' 기회", 현대·기아 이어 GM까지...NFT 시장 뛰어든다, 현대·벤츠·포르쉐·아우디 등 차량 6만4754대, 제작결함에 리콜, 현대차 1분기 원재료 구매비 1조 증가… 車값 또 오르나, 현대차·기아 ‘발명의 날’ 우수특허 9건 선정·포상, "로보틱스부터 AI까지"…현대차·기아, '2022발명의 날' 행사 개최, "공장 안돌아" 현대차·기아 車값↑…'승용차' 평균가는 떨어진 이유, 현대·기아 이어 GM까지...NFT 시장 뛰어든다, 인플레 공포 '성큼'?…증권가 "삼전·현대차 등 '대형수출주' 기회", 우수AMS, 현대車 21조 투자...범현대家 등 업고 전기차 ..., 현대차 1분기 원재료 구매비 1조 증가… 車값 또 오르나, 더현대서울, 초고속 손익분기점 달성, 현대차 1분기 원재료 구매비 1조 증가… 車값 또 오르나, 현대차·기아 ‘발명의 날’ 우수특허 9건 선정·포상, "로보틱스부터 AI까지"…현대차·기아, '2022발명의 날' 행사 개최, "주차 중 P단 해제"...국토부, 현대차 아이오닉 5 등 리콜, 美 조지아주, 20일에 현대차 전기차공장 유치 발표할 듯, 더현대서울, 초고속 손익분기점 달성, 더현대서울, 13개월만에 손익분기 넘겼다…초고속 비결은?, "주차 중 P단 해제"...국토부, 현대차 아이오닉 5 등 리콜, 美 조지아주, 20일에 현대차 전기차공장 유치 발표할 듯, 대우조선, ‘대금 미지급’ 러 계약 해지…현대·삼성重도 피해 우려[뒷북..., 현대차·기아, 국내 전기차 분야 21조원 투자…“韓 전기차 허브로”[뒷..., 경사로 주차중 'P단' 풀려…현대차, 아이오닉5 등 5.8만대 무상 업..., 더현대서울, 13개월만에 손익분기 넘겼다…초고속 비결은?, 현대차 선행생산기술센터, 정부인증 연구소 전환 추진</t>
   </si>
   <si>
     <t>현대차, 바이든 '그린뉴딜' 맞춰 美 전기차 점유율 11%로, 바이든, 22일 정의선 만난다…"현대차 조지아주 투자에 감사", 바이든, 정의선 면담 소식에 현대차·기아 강세, 바이든-정의선 면담 소식에 현대차·기아 '훨훨', 바이든, 22일 정의선 만난다…현대차는 수조원대 美 투자 발표, 현대차, 미국 조지아 주에 전기차 공장 신설 추진, 가성비 버리고 고급화·전동화…현대차, 中心 잡는다, 바이든, 22일 정의선 만난다…"현대차 조지아주 투자에 감사", 바이든, 정의선 면담 소식에 현대차·기아 강세, 바이든-정의선 면담 소식에 현대차·기아 '훨훨', 현대차, 미국 조지아 주에 전기차 공장 신설 추진, 현대차, 바이든 '그린뉴딜' 맞춰 美 전기차 점유율 11%로, 바이든-정의선 면담 소식에 현대차·기아 '훨훨', 가성비 버리고 고급화·전동화…현대차, 中心 잡는다, 바이든, 22일 정의선 만난다…"현대차 조지아주 투자에 감사", 가성비 버리고 고급화·전동화…현대차, 中心 잡는다, 바이든, 정의선 면담 소식에 현대차·기아 강세, 현대차, 미국 조지아 주에 전기차 공장 신설 추진</t>
@@ -7969,10 +7969,10 @@
     <t>"美에 총105억달러 투자" 정의선 어깨에 손얹은 바이든 "현대차 실망..., "6.3조에 6.3조 추가"…현대차그룹 정의선, 美 바이든에 '통큰 투..., 현대차, 모빌리티 꿈나무 양성…‘미래 자동차’ 참가 학교 모집, '모빌리티 인재' 육성…현대차, 초중생 대상 '미래차 학교' 연다, 바이든, 정의선과 50분 독대…"현대차 투자에 보답하겠다" [현대차 "..., 정의선 ‘통큰 선물’에 바이든 활짝 “현대차 실망시키지 않겠다”, 美에 미래산업 생태계 구축…바이든 “현대차 실망시키지..., 현대차 '퍼스트 무버' 승부수…미국서 전기차·UAM 판 키운다, 정의선 ‘통큰 선물’에 바이든 활짝 “현대차 실망시키지 않겠다”, "美에 총105억달러 투자" 정의선 어깨에 손얹은 바이든 "현대차 실망..., 삼성·SK·현대차 등 74개 기업 '새로운 기업가정신' 선포, 50억弗 추가…현대차, 美에 105억弗 통큰 투자, 바이든, 정의선과 50분 만남…"현대차 절대 실망시키지 않겠다", 50억弗 추가…현대차, 美에 105억弗 통큰 투자, 현대차 '퍼스트 무버' 승부수…미국서 전기차·UAM 판 키운다, 삼성·SK·현대차 등 74개 기업 '새로운 기업가정신' 선포, '모빌리티 인재' 육성…현대차, 초중생 대상 '미래차 학교' 연다, 美에 미래산업 생태계 구축…바이든 “현대차 실망시키지..., 현대차, 모빌리티 꿈나무 양성…‘미래 자동차’ 참가 학교 모집</t>
   </si>
   <si>
-    <t>현대차그룹 美에 105억달러 '통 큰 투자'..."미국 정부 세제 혜택..., 하나금투 “현대차, 목표 주가 26만원…북미 전기차 투자 확대로 주가 ..., 현대차 북미 전기차 투자 확대, 주가 상승 요인 될 것-하나금투, 현대차, 쏘나타 단종으로 수익성 향상…목표가↑-삼성, 하나금투 “현대차, 목표 주가 26만원…북미 전기차 투자 확대로 주가 ..., 바이든 방한 약발 끝? 삼성전자·현대차 소폭 상승, 현대차-북미 전기차 공장 확정 등 총 13조원 투자, 미국 조지아주에 연산 30만대 규모로 2025년 가동, 급성장 중인 북미 전기차 시장에 대한 대응력을 높여주는 계기, Valuation 상향 요인으로 작용할 것, 현대차-2022년 하반기 전망: Simple is the best, 저수익 모델 단종으로 수익성 향상 예상, 중형 세단 쏘나타, 역사 속으로, 제네시스, 쏘나타보다 더 파는 모델, 현대차, 쏘나타 단종으로 수익성 향상…목표가↑-삼성, 현대차, 美조지아에 전기차 전용 공장 건설, 바이든 “생큐, 현대차”…정의선, 美에 13조 ‘통큰 투자’ 보따리 [..., 현대차, ‘더 뉴 팰리세이드’ 출시 본격 판매 돌입, 현대차 북미 전기차 투자 확대, 주가 상승 요인 될 것-하나금투, 현대차, 저수익 모델 단종…전기차로 성장 모멘텀↑-삼성, 현대차그룹, 韓전기차 연간 투자금액 美'6배', 美 통큰 투자로 전기차 날개단 현대차…하반기도 '쌩쌩', 현대차그룹 'UAM' 투자 계획에…네온테크, 상한가, 네온테크, 바이든 만난 현대차 정의선 UAM 투자 계획에 오..., 현대차그룹 대규모 투자 소식에 UAM 관련주 '들썩', 우량 회사채 ‘온기’…현대百 이어 SK에너지도 흥행, 로봇株, 현대차 대규모 미국 투자 소식에 '강세', 현대차그룹 “美와 함께 생산 확대”…국내 투자는 어떻게?, 현대차그룹 “美와 함께 생산 확대”…국내 투자는 어떻게? [비즈360..., 전기차 전환 가속…현대차·기아 국내공장도 체질 바꾼다, 하나금투 “현대차, 목표 주가 26만원…북미 전기차 투자 확대로 주가..., 현대차 105억달러 ‘통 큰 투자’ 발표에 UAM, 로봇주 ‘활짝’, '현대차 50억달러 투자' 들썩이는 로봇株.…어떤 종목 담을까, 현대차, 美조지아에 전기차 전용 공장 건설, 현대차, 美 조지아주와 전기차 공장 건설 투자협약, "두달새 16% 오른 건 성 안차"…현대차 美 통큰 투자 주가 동력될까, 현대차, '수입차 무덤' 日 공략 개시…"전기차 상당히 앞서" 현지 호..., "美 선점" 치고 나가는 현대차…GM·폭스바겐 '긴장', 현대차는 협력사 '美 동반진출·선순환' 기대, "코스피 2400까지 밀릴 수도"…삼성전자·현대차 유망, 삼성·현대차가 韓 최고 전략자산…한미 공급망 동맹 중심축됐다, 현대차 싱가포르혁신센터 완공 속도낸다, 세계 '가스올림픽' 내일 대구서 개막···SK·현대차·두산 등 韓 수소..., 美에 13조원 투자하는 현대차... 국내 車산업 성장 선순환 이끄나, "코스피 2400까지 밀릴 수도"…삼성전자·현대차 유망, 현대차 싱가포르혁신센터 완공 속도낸다, 현대차그룹, 전기차 투자 美에만 선물? 국내와 비교해봤더니…, 美 통큰 투자로 전기차 날개단 현대차…하반기도 '쌩쌩', 세계 '가스올림픽' 내일 대구서 개막···SK·현대차·두산 등 韓 수소..., 현대차, '수입차 무덤' 日 공략 개시…"전기차 상당히 앞서" 현지 호...</t>
-  </si>
-  <si>
-    <t>현대차, 가상현실로 배터리 수명 예측, 현대차 ‘디지털 트윈’ 기술로 배터리 성능 관리, 삼성 450兆, 현대차 63조…尹 ‘민간주도성장’에 답했다, NFT 계정 해킹 공격에 현대차도 구매자도 애꿎은 피해, 삼성 450兆, 현대차 63조…尹 ‘민간주도성장’에 답했다, 또 빼앗길까 노심초사…현대차 美 투자 '막전막후', 현대차그룹 전기차공장, 美조지아주 간 사연, 삼성 450兆, 현대차 63兆…尹 ‘민간주도성..., 현대차-매력적인 EV 성장 스토리와 신차 싸이클, EV 성장 스토리 재점화, 미국 EV 신공장 증설 계획 발표, 국내 공장 가동률 회복, 매력적인 신차 싸이클, 삼성전자·현대차 등 "新기업가정신은 혁신의 길", NFT 계정 해킹 공격에 현대차도 구매자도 애꿎은 피해, 삼성 360조·현대차 63조…국내투자 쏟아낸다, 삼성전자·현대차 주가 '뚝뚝'…'역대급' 투자 발표도 안 통했다, 이유..., 삼성·현대차·롯데·한화, 600조원 투자 보따리 풀었다, 현대차그룹, 2025년까지 국내에 63조원 투자, 성창오토텍, 현대차그룹 국내 63조 투자...1차 협력업체 부..., 현대차그룹, 2025년까지 국내에 63조원 투자, 현대차?기아?모비스, 63조 국내 투자..."한국을 미래사업 허브로", "미래사업 허브"…현대차·기아·모비스, 2025년까지 국내에 63조 투..., 현대차·기아·모비스, 2025년까지 국내 63조 투자, 현대차그룹, 2025년까지 국내에 63조 투자, 현대차·기아·모비스 4년간 국내에 63조원 투자 결정, 현대차?기아?모비스 국내 63조원 투자…"한국 미래 사업 허브", 현대차그룹, 국내에 63조 투자…"한국을 미래사업 허브로", 현대차그룹, 국내에 63조원 투자…"한국을 미래사업 허브로", '美 중간선거 앞둔' 바이든, 현대차·삼성 띄운 이유 있었네, 세아메카닉스, 전기차·2차전지 부품 연 5천억 증설…현대차 투..., 현대차·기아·모비스, 2025년까지 국내 63조 투자, 현대차·기아·모비스 "2025년까지 국내 63조원 투자…미래車..., &lt;속보&gt;현대차?기아?모비스, 2025년까지 국내에 63조 투자, '美 중간선거 앞둔' 바이든, 현대차·삼성 띄운 이유 있었네, 세아메카닉스, 전기차·2차전지 부품 연 5천억 증설…현대차 투..., 현대차그룹 “배터리 성능 더 정확하게 예측”, 현대차그룹 '디지털 트윈'으로 전기차 배터리 관리 시험도입, 바이브, 현대차그룹-MS, 전기차 배터리 관리에 '디지털 트윈..., 가상의 쌍둥이 전기차로 배터리 성능 관리…현대차, '디지털 트윈' 기..., 유일로보틱스, 삼성·현대차 고민 '해결사'…비싼임금에도 미국 ..., 한국마이크로소프트, 현대차그룹 전기차 배터리 자산관리 플랫폼 기술 검증, 자동차株, 실적 개선 비해 주가 상승력↓…현대차 '톱픽' -신한금융투자, 현대차, 성장스토리 재점화…하반기 업종 최선호주-유진, 현대차그룹 '디지털 트윈'으로 전기차 배터리 관리 시험도입, 디지털 세계에서 배터리 수명 예측하는 현대차...마이크로소프트와 협업, 자동차株, 실적 개선 비해 주가 상승력↓…현대차 '톱픽' -신한금융투자, 현대차, 성장스토리 재점화…하반기 업종 최선호주-유진, 현대차그룹, 국내에 63조원 투자…"한국을 미래사업 허브로", '450조' 삼성에 현대차·롯데·한화까지…역대급 돈보따리 푼 재계 [..., 성창오토텍, 현대차그룹 국내 63조 투자...1차 협력업체 부..., 현대차 63조 투자 발표에 자동차 부품株 '급등', 전기차 16조 쏟는 현대차…"한국이 車산업 대전환 주도", 현대차?기아?현대모비스, 2025년까지 국내에 63조원 투자, 현대차그룹, 친환경차 16조, 로보틱스·UAM 9조…"韓을 미래사업 허..., 미국 13조, 한국 63조…'통큰 결단' 정의선, 현대차그룹 '글로벌..., 현대차그룹 전기차공장, 美조지아주 간 사연, 국내에 63조 투자하는 현대차그룹…"한국을 미래사업 허브로", 현대차 미국 전기차 공장 설립에…‘서배너 효과’ 기대감 커진다, 국내에 63조 투자하는 현대차그룹…"한국을 미래사업 허브로", 현대차 미국 전기차 공장 설립에…‘서배너 효과’ 기대감 커진다, 삼성 현대차부터 쿠팡 컬리까지…76개 기업 한자리에 모인 이유는, 현대차그룹 전기차 투자계획 보니…거점지역 보인다, '450조' 삼성에 현대차·롯데·한화까지…역대급 돈보따리 푼 재계 [종..., 尹에 화답한 재계…삼성·현대차·롯데·한화, '역대급' 투자 보따리(종..., 현대차, 현대차증권으로부터 450억원 규모 유가증권 매수, 대유에이텍, 현대차그룹 국내 63조 투자...친환경 모빌리티 ..., '현대차-JKL-캠코', 5000억 미래모빌리티 '합승'…어디까지 달릴..., 현대차?기아?현대모비스, 2025년까지 국내에 63조원 투자, 현대차그룹, 2025년까지 국내에 63조 투자, 현대차 그룹 63조 투자 소식에 자동차 부품株 급상승, 현대차그룹 "2025년까지 전동화에 16.2조원·내연차에 38조원 국내..., "韓, 미래車 사업 허브로 키운다"…4년간 63조원 국내에 쏟아붓는 ..., 현대차, '5000억 미래모빌리티' 탑승…캠코합류 JKL펀드 투..., 현대차 그룹 63조 투자 소식에 자동차 부품株 급상승, 현대차?기아?현대모비스, 2025년까지 국내에 63조원 투자, 현대차그룹, 2025년까지 국내에 63조 투자, 현대차그룹 "2025년까지 전동화에 16.2조원·내연차에 38조원 국내..., "韓, 미래車 사업 허브로 키운다"…4년간 63조원 국내에 쏟아붓는 ..., 미국 13조, 한국 63조…'통큰 결단' 정의선, 현대차그룹 '글로벌 ..., 현대차그룹, 2025년까지 국내 63兆 투자…“한국을 미래차 허브로”, 현대차 63조 투자 소식에 에스피시스템스 상한가, 현대차, '5000억 미래모빌리티' 탑승…캠코합류 JKL펀드 ..., 현대차·기아·모비스 "2025년까지 국내 63조원 투자…미래車...</t>
+    <t>현대차그룹 美에 105억달러 '통 큰 투자'..."미국 정부 세제 혜택..., 하나금투 “현대차, 목표 주가 26만원…북미 전기차 투자 확대로 주가 ..., 현대차 북미 전기차 투자 확대, 주가 상승 요인 될 것-하나금투, 현대차, 쏘나타 단종으로 수익성 향상…목표가↑-삼성, 하나금투 “현대차, 목표 주가 26만원…북미 전기차 투자 확대로 주가 ..., 바이든 방한 약발 끝? 삼성전자·현대차 소폭 상승, 북미 전기차 공장 확정 등 총 13조원 투자, 미국 조지아주에 연산 30만대 규모로 2025년 가동, 급성장 중인 북미 전기차 시장에 대한 대응력을 높여주는 계기, Valuation 상향 요인으로 작용할 것, 2022년 하반기 전망: Simple is the best, 저수익 모델 단종으로 수익성 향상 예상, 중형 세단 쏘나타, 역사 속으로, 제네시스, 쏘나타보다 더 파는 모델, 현대차, 쏘나타 단종으로 수익성 향상…목표가↑-삼성, 현대차, 美조지아에 전기차 전용 공장 건설, 바이든 “생큐, 현대차”…정의선, 美에 13조 ‘통큰 투자’ 보따리 [..., 현대차, ‘더 뉴 팰리세이드’ 출시 본격 판매 돌입, 현대차 북미 전기차 투자 확대, 주가 상승 요인 될 것-하나금투, 현대차, 저수익 모델 단종…전기차로 성장 모멘텀↑-삼성, 현대차그룹, 韓전기차 연간 투자금액 美'6배', 美 통큰 투자로 전기차 날개단 현대차…하반기도 '쌩쌩', 현대차그룹 'UAM' 투자 계획에…네온테크, 상한가, 네온테크, 바이든 만난 현대차 정의선 UAM 투자 계획에 오..., 현대차그룹 대규모 투자 소식에 UAM 관련주 '들썩', 우량 회사채 ‘온기’…현대百 이어 SK에너지도 흥행, 로봇株, 현대차 대규모 미국 투자 소식에 '강세', 현대차그룹 “美와 함께 생산 확대”…국내 투자는 어떻게?, 현대차그룹 “美와 함께 생산 확대”…국내 투자는 어떻게? [비즈360..., 전기차 전환 가속…현대차·기아 국내공장도 체질 바꾼다, 하나금투 “현대차, 목표 주가 26만원…북미 전기차 투자 확대로 주가..., 현대차 105억달러 ‘통 큰 투자’ 발표에 UAM, 로봇주 ‘활짝’, '현대차 50억달러 투자' 들썩이는 로봇株.…어떤 종목 담을까, 현대차, 美조지아에 전기차 전용 공장 건설, 현대차, 美 조지아주와 전기차 공장 건설 투자협약, "두달새 16% 오른 건 성 안차"…현대차 美 통큰 투자 주가 동력될까, 현대차, '수입차 무덤' 日 공략 개시…"전기차 상당히 앞서" 현지 호..., "美 선점" 치고 나가는 현대차…GM·폭스바겐 '긴장', 현대차는 협력사 '美 동반진출·선순환' 기대, "코스피 2400까지 밀릴 수도"…삼성전자·현대차 유망, 삼성·현대차가 韓 최고 전략자산…한미 공급망 동맹 중심축됐다, 현대차 싱가포르혁신센터 완공 속도낸다, 세계 '가스올림픽' 내일 대구서 개막···SK·현대차·두산 등 韓 수소..., 美에 13조원 투자하는 현대차... 국내 車산업 성장 선순환 이끄나, "코스피 2400까지 밀릴 수도"…삼성전자·현대차 유망, 현대차 싱가포르혁신센터 완공 속도낸다, 현대차그룹, 전기차 투자 美에만 선물? 국내와 비교해봤더니…, 美 통큰 투자로 전기차 날개단 현대차…하반기도 '쌩쌩', 세계 '가스올림픽' 내일 대구서 개막···SK·현대차·두산 등 韓 수소..., 현대차, '수입차 무덤' 日 공략 개시…"전기차 상당히 앞서" 현지 호...</t>
+  </si>
+  <si>
+    <t>현대차, 가상현실로 배터리 수명 예측, 현대차 ‘디지털 트윈’ 기술로 배터리 성능 관리, 삼성 450兆, 현대차 63조…尹 ‘민간주도성장’에 답했다, NFT 계정 해킹 공격에 현대차도 구매자도 애꿎은 피해, 삼성 450兆, 현대차 63조…尹 ‘민간주도성장’에 답했다, 또 빼앗길까 노심초사…현대차 美 투자 '막전막후', 현대차그룹 전기차공장, 美조지아주 간 사연, 삼성 450兆, 현대차 63兆…尹 ‘민간주도성..., 매력적인 EV 성장 스토리와 신차 싸이클, EV 성장 스토리 재점화, 미국 EV 신공장 증설 계획 발표, 국내 공장 가동률 회복, 매력적인 신차 싸이클, 삼성전자·현대차 등 "新기업가정신은 혁신의 길", NFT 계정 해킹 공격에 현대차도 구매자도 애꿎은 피해, 삼성 360조·현대차 63조…국내투자 쏟아낸다, 삼성전자·현대차 주가 '뚝뚝'…'역대급' 투자 발표도 안 통했다, 이유..., 삼성·현대차·롯데·한화, 600조원 투자 보따리 풀었다, 현대차그룹, 2025년까지 국내에 63조원 투자, 성창오토텍, 현대차그룹 국내 63조 투자...1차 협력업체 부..., 현대차그룹, 2025년까지 국내에 63조원 투자, 현대차?기아?모비스, 63조 국내 투자..."한국을 미래사업 허브로", "미래사업 허브"…현대차·기아·모비스, 2025년까지 국내에 63조 투..., 현대차·기아·모비스, 2025년까지 국내 63조 투자, 현대차그룹, 2025년까지 국내에 63조 투자, 현대차·기아·모비스 4년간 국내에 63조원 투자 결정, 현대차?기아?모비스 국내 63조원 투자…"한국 미래 사업 허브", 현대차그룹, 국내에 63조 투자…"한국을 미래사업 허브로", 현대차그룹, 국내에 63조원 투자…"한국을 미래사업 허브로", '美 중간선거 앞둔' 바이든, 현대차·삼성 띄운 이유 있었네, 세아메카닉스, 전기차·2차전지 부품 연 5천억 증설…현대차 투..., 현대차·기아·모비스, 2025년까지 국내 63조 투자, 현대차·기아·모비스 "2025년까지 국내 63조원 투자…미래車..., &lt;속보&gt;현대차?기아?모비스, 2025년까지 국내에 63조 투자, '美 중간선거 앞둔' 바이든, 현대차·삼성 띄운 이유 있었네, 세아메카닉스, 전기차·2차전지 부품 연 5천억 증설…현대차 투..., 현대차그룹 “배터리 성능 더 정확하게 예측”, 현대차그룹 '디지털 트윈'으로 전기차 배터리 관리 시험도입, 바이브, 현대차그룹-MS, 전기차 배터리 관리에 '디지털 트윈..., 가상의 쌍둥이 전기차로 배터리 성능 관리…현대차, '디지털 트윈' 기..., 유일로보틱스, 삼성·현대차 고민 '해결사'…비싼임금에도 미국 ..., 한국마이크로소프트, 현대차그룹 전기차 배터리 자산관리 플랫폼 기술 검증, 자동차株, 실적 개선 비해 주가 상승력↓…현대차 '톱픽' -신한금융투자, 현대차, 성장스토리 재점화…하반기 업종 최선호주-유진, 현대차그룹 '디지털 트윈'으로 전기차 배터리 관리 시험도입, 디지털 세계에서 배터리 수명 예측하는 현대차...마이크로소프트와 협업, 자동차株, 실적 개선 비해 주가 상승력↓…현대차 '톱픽' -신한금융투자, 현대차, 성장스토리 재점화…하반기 업종 최선호주-유진, 현대차그룹, 국내에 63조원 투자…"한국을 미래사업 허브로", '450조' 삼성에 현대차·롯데·한화까지…역대급 돈보따리 푼 재계 [..., 성창오토텍, 현대차그룹 국내 63조 투자...1차 협력업체 부..., 현대차 63조 투자 발표에 자동차 부품株 '급등', 전기차 16조 쏟는 현대차…"한국이 車산업 대전환 주도", 현대차?기아?현대모비스, 2025년까지 국내에 63조원 투자, 현대차그룹, 친환경차 16조, 로보틱스·UAM 9조…"韓을 미래사업 허..., 미국 13조, 한국 63조…'통큰 결단' 정의선, 현대차그룹 '글로벌..., 현대차그룹 전기차공장, 美조지아주 간 사연, 국내에 63조 투자하는 현대차그룹…"한국을 미래사업 허브로", 현대차 미국 전기차 공장 설립에…‘서배너 효과’ 기대감 커진다, 국내에 63조 투자하는 현대차그룹…"한국을 미래사업 허브로", 현대차 미국 전기차 공장 설립에…‘서배너 효과’ 기대감 커진다, 삼성 현대차부터 쿠팡 컬리까지…76개 기업 한자리에 모인 이유는, 현대차그룹 전기차 투자계획 보니…거점지역 보인다, '450조' 삼성에 현대차·롯데·한화까지…역대급 돈보따리 푼 재계 [종..., 尹에 화답한 재계…삼성·현대차·롯데·한화, '역대급' 투자 보따리(종..., 현대차, 현대차증권으로부터 450억원 규모 유가증권 매수, 대유에이텍, 현대차그룹 국내 63조 투자...친환경 모빌리티 ..., '현대차-JKL-캠코', 5000억 미래모빌리티 '합승'…어디까지 달릴..., 현대차?기아?현대모비스, 2025년까지 국내에 63조원 투자, 현대차그룹, 2025년까지 국내에 63조 투자, 현대차 그룹 63조 투자 소식에 자동차 부품株 급상승, 현대차그룹 "2025년까지 전동화에 16.2조원·내연차에 38조원 국내..., "韓, 미래車 사업 허브로 키운다"…4년간 63조원 국내에 쏟아붓는 ..., 현대차, '5000억 미래모빌리티' 탑승…캠코합류 JKL펀드 투..., 현대차 그룹 63조 투자 소식에 자동차 부품株 급상승, 현대차?기아?현대모비스, 2025년까지 국내에 63조원 투자, 현대차그룹, 2025년까지 국내에 63조 투자, 현대차그룹 "2025년까지 전동화에 16.2조원·내연차에 38조원 국내..., "韓, 미래車 사업 허브로 키운다"…4년간 63조원 국내에 쏟아붓는 ..., 미국 13조, 한국 63조…'통큰 결단' 정의선, 현대차그룹 '글로벌 ..., 현대차그룹, 2025년까지 국내 63兆 투자…“한국을 미래차 허브로”, 현대차 63조 투자 소식에 에스피시스템스 상한가, 현대차, '5000억 미래모빌리티' 탑승…캠코합류 JKL펀드 ..., 현대차·기아·모비스 "2025년까지 국내 63조원 투자…미래車...</t>
   </si>
   <si>
     <t>정의선 현대차 회장, 대우家와 사돈 맺는다, 삼성·현대차·롯데·한화, 청년 고용 책임진다…5년간 588조 투자 [뒷..., 전기차 본고장 유럽 접수하는 현대차·기아…'도장 깨기' 성공적 [박한신..., 현대무벡스, LG화학 자동화솔루션 공급 ‘2차전지 스마트물류 첫 발’, 현대무벡스, LG화학에 자동화 솔루션 공급, 정의선 현대차 회장, 대우家와 사돈 맺는다, 정의선 현대차그룹 회장 장녀, 내달 결혼…대우家와 사돈, "납득할 수 있는 말을 해라"... 국내 투자 63조원에 분노한 현대차..., "이르면 2024년 中에 현대 순수 전기차 첫 판매", 현대차그룹, 멀티콥터 드론 ‘프로젝트N’ 첫선, 미래 항공 모빌리티 비전 소개한 현대차그룹…수소 드론 최초 공개, 현대무벡스, LG화학에 자동화 솔루션 공급, 현대무벡스 2차전지 스마트물류사업 개시..LG화학 맞손, 4년간 63조 투자 현대차 그룹…부품주 함께 달릴까, 삼성·현대차·롯데·한화, 청년 고용 책임진다…5년간 588조 투자 [뒷..., 세계 최대 LG 양극재공장에 현대무벡스 물류시스템 쓴다, 현대무벡스, LG화학에 자동화 솔루션 공급…“2차전지 스마트 물류 탄력..., 코스피 2600선에서 등락 반복…'대규모 투자'에도 삼전·현대차 ↓, 엠에스오토텍, 현대차그룹 국내 63조 투자…전기차 생산 최대 ..., 현대차그룹, 멀티콥터 드론 ‘프로젝트N’ 첫선…AAM 미래 제시하다, “미국에만 투자한다고?” 삼성·현대차·롯데·한화 국내에 보따리 푼 이유..., “尹대통령이 업어줄만 하네” 삼성·현대차·롯데·한화 국내에 ‘480조’..., 현대차그룹, 항공 연구인력 품는다…'AAM 테크데이 2022' 개최, (영상)삼성·현대 등 대기업 4곳 총 600조 투자 계획, 코스피 2600선에서 등락 반복…'대규모 투자'에도 삼전·현대차 ↓, 엠에스오토텍, 현대차그룹 국내 63조 투자…전기차 생산 최대 ..., 현대차그룹, 멀티콥터 드론 '프로젝트N' 기체 공개, 현대차그룹, 멀티콥터 드론 ‘프로젝트N’ 첫선, UAM은 알겠는데…RAM까지 개척한다는 현대차그룹, 코오롱글로벌-현대기아차, 집-차 연결 서비스 선보인다, 현대차 2024년 中서 '첫 순수 전기차' 시동, "이르면 2024년 中에 현대 순수 전기차 첫 판매", 현대차그룹, 항공 연구인력 품는다…'AAM 테크데이 2022' 개최, 현대차 2024년 中서 '첫 순수 전기차' 시동, "이르면 2024년 中에 현대 순수 전기차 첫 판매", 현대차, 국내 첫 수소연료 드론 ‘프로젝트N’ 공개, 현대차 ‘수소·배터리 동시 사용’ 멀티콥터 드론 첫 공개, 정의선 현대차 회장, 대우家와 사돈 맺는다, 엠에스오토텍, 현대차그룹 국내 63조 투자…전기차 생산 최대..., 코오롱글로벌, 현대기아차와 맞손…집과 자동차 경계 허문다, 엠에스오토텍, 현대차그룹 국내 63조 투자…전기차 생산 최대..., 현대차그룹 63조 투자 수혜 기대... 엠에스오토텍 주가 4% 이상 급..., 현대차그룹, UAM서 AAM으로 하늘 영역 확대, 4년간 63조 투자 현대차 그룹…부품주 함께 달릴까, 코오롱글로벌-현대기아차, 집-차 연결 서비스 선보인다, 코오롱글로벌, 현대기아차와 맞손…집과 자동차 경계 허문다, 현대차그룹 63조 투자 수혜 기대... 엠에스오토텍 주가 4% 이상 급...</t>

</xml_diff>